<commit_message>
Modified Technical Documentation + LogBook + MLD ( spell check)
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{0E675FB9-10CD-43EE-A7E4-0C8EBD63A034}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C88D6C38-99C9-4871-9537-E2E331135C41}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{0E675FB9-10CD-43EE-A7E4-0C8EBD63A034}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{D9DF084B-4FCA-422C-8AB0-15C708B0A634}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Documentation</t>
   </si>
@@ -136,7 +136,16 @@
     <t>Anayse du critère 1</t>
   </si>
   <si>
-    <t>Implémentation</t>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Implémentation Creation de compte</t>
+  </si>
+  <si>
+    <t>Implémentation barre de navigation</t>
+  </si>
+  <si>
+    <t>Implémentation Connexion</t>
   </si>
 </sst>
 </file>
@@ -456,17 +465,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -571,6 +582,9 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" s="2">
@@ -773,7 +787,28 @@
         <v>0.3263888888888889</v>
       </c>
       <c r="C33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modfied logbook + documentation
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
   <si>
     <t>Documentation</t>
   </si>
@@ -202,23 +202,67 @@
     <t>Mot de passe (nombre caractère min. + min. 1 chiffre)</t>
   </si>
   <si>
-    <t>Question ajouter au joural de bord</t>
-  </si>
-  <si>
     <t>Analyse du critère 2</t>
   </si>
   <si>
     <t>Implémentation des information personnel</t>
+  </si>
+  <si>
+    <t>Implémentation Histoire</t>
+  </si>
+  <si>
+    <t>https://www.sitepoint.com/community/t/check-whether-string-contains-numbers/5953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erreur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mot de passe </t>
+  </si>
+  <si>
+    <t>https://mdbootstrap.com/docs/jquery/forms/file-input/</t>
+  </si>
+  <si>
+    <t>Implémentation Fonction DB</t>
+  </si>
+  <si>
+    <t>File input Bosstrap</t>
+  </si>
+  <si>
+    <t>Planning Effectif</t>
+  </si>
+  <si>
+    <t>Mail Experts</t>
+  </si>
+  <si>
+    <t>Utiliser ~ pour REGEX en PHP</t>
+  </si>
+  <si>
+    <t>Clément Christensen explication TRIM</t>
+  </si>
+  <si>
+    <t>Question ajouter au journal de bord</t>
+  </si>
+  <si>
+    <t>requête SQL avec comme filtre le nouvelle email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,15 +285,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -528,18 +575,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="90.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
@@ -881,7 +928,7 @@
         <v>0.67361111111111116</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -900,7 +947,7 @@
         <v>0.3125</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,14 +955,128 @@
         <v>0.34722222222222227</v>
       </c>
       <c r="C43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43561</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="C46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+      <c r="C49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="2"/>
+      <c r="C50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C51" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+      <c r="C53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="2">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="2"/>
+      <c r="C55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C56" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="C57" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D52" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -924,7 +1085,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Spell check on Logbook
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_855E4D0B644ABABC04741A84EC131E4EDBD04195" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0657C44A-AE9B-4688-96F4-E8D4A34777A0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal De Bord" sheetId="1" r:id="rId1"/>
@@ -58,21 +59,12 @@
     <t>Mail Planification</t>
   </si>
   <si>
-    <t>Lecture de l'énoncé</t>
-  </si>
-  <si>
     <t xml:space="preserve"> création de V 0.1 passage de V0.1 aV0.2</t>
   </si>
   <si>
     <t>Création GitHub</t>
   </si>
   <si>
-    <t xml:space="preserve"> réponse Q1</t>
-  </si>
-  <si>
-    <t>Modification de la planification initial</t>
-  </si>
-  <si>
     <t>MLD</t>
   </si>
   <si>
@@ -94,39 +86,21 @@
     <t xml:space="preserve">Aide par Clément Christensen </t>
   </si>
   <si>
-    <t>Réponse Q4</t>
-  </si>
-  <si>
     <t>V0.2 a V0.3</t>
   </si>
   <si>
-    <t xml:space="preserve"> réponse Q2,Q3,Q5,Q6</t>
-  </si>
-  <si>
     <t>Question</t>
   </si>
   <si>
     <t>Réponse</t>
   </si>
   <si>
-    <t>Mail à Mme. Mota Stroppolo</t>
-  </si>
-  <si>
-    <t>Contact avec Mme. Mota Stroppolo</t>
-  </si>
-  <si>
     <t>Q7</t>
   </si>
   <si>
-    <t>Implémentation barre de navigation</t>
-  </si>
-  <si>
     <t>Implémentation Connexion</t>
   </si>
   <si>
-    <t>pour sécuriser le dossier les information de la DB</t>
-  </si>
-  <si>
     <t>N°</t>
   </si>
   <si>
@@ -136,12 +110,6 @@
     <t>Pas d’importance mais ne pas mélanger les deux.</t>
   </si>
   <si>
-    <t>RDV. avec M. Folomietow</t>
-  </si>
-  <si>
-    <t>RDV. avec Mme. Mota Stroppolo</t>
-  </si>
-  <si>
     <t>Q8</t>
   </si>
   <si>
@@ -184,18 +152,12 @@
     <t>Création BD</t>
   </si>
   <si>
-    <t>Création données</t>
-  </si>
-  <si>
     <t>Analyse du critère 1</t>
   </si>
   <si>
     <t>Implémentation Création de compte</t>
   </si>
   <si>
-    <t>Q1 (voir feuille "question")</t>
-  </si>
-  <si>
     <t>Vérification du mail (REGEX)</t>
   </si>
   <si>
@@ -205,9 +167,6 @@
     <t>Analyse du critère 2</t>
   </si>
   <si>
-    <t>Implémentation des information personnel</t>
-  </si>
-  <si>
     <t>Implémentation Histoire</t>
   </si>
   <si>
@@ -226,12 +185,6 @@
     <t>Implémentation Fonction DB</t>
   </si>
   <si>
-    <t>File input Bosstrap</t>
-  </si>
-  <si>
-    <t>Planning Effectif</t>
-  </si>
-  <si>
     <t>Mail Experts</t>
   </si>
   <si>
@@ -245,12 +198,60 @@
   </si>
   <si>
     <t>requête SQL avec comme filtre le nouvelle email</t>
+  </si>
+  <si>
+    <t>Contact avec Mme Mota Stroppolo</t>
+  </si>
+  <si>
+    <t>Mail à Mme Mota Stroppolo</t>
+  </si>
+  <si>
+    <t>Modification de la planification initiale</t>
+  </si>
+  <si>
+    <t>Création donnée</t>
+  </si>
+  <si>
+    <t>rdv avec Mme Mota Stroppolo</t>
+  </si>
+  <si>
+    <t>Implémentation Barre de navigation</t>
+  </si>
+  <si>
+    <t>Implémentation des informations personnelles</t>
+  </si>
+  <si>
+    <t>Planning effectif</t>
+  </si>
+  <si>
+    <t>Lecture de l’énoncé</t>
+  </si>
+  <si>
+    <t>Q1 (voir feuille « question »)</t>
+  </si>
+  <si>
+    <t>pour sécuriser le dossier les informations de la base de données</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> réponse Q1</t>
+  </si>
+  <si>
+    <t>Réponse Q4</t>
+  </si>
+  <si>
+    <t>rdv avec M. Folomietow</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> réponse Q2, Q3, Q5, Q6</t>
+  </si>
+  <si>
+    <t>File input bootstrap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -574,25 +575,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="90.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -603,7 +604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>43557</v>
       </c>
@@ -611,23 +612,23 @@
         <v>0.3125</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>0.3263888888888889</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2">
         <v>0.36805555555555558</v>
       </c>
@@ -635,40 +636,40 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="2">
         <v>0.4548611111111111</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="2">
         <v>0.46527777777777773</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="2">
         <v>0.47222222222222227</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="2">
         <v>0.52777777777777779</v>
       </c>
@@ -679,17 +680,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" s="2">
         <v>0.59027777777777779</v>
       </c>
@@ -697,31 +698,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" s="2">
         <v>0.66319444444444442</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" s="2">
         <v>0.66666666666666663</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B16" s="2">
         <v>0.68402777777777779</v>
       </c>
@@ -729,7 +730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B17" s="2">
         <v>0.6875</v>
       </c>
@@ -737,7 +738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>43558</v>
       </c>
@@ -745,47 +746,47 @@
         <v>0.3125</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B19" s="2">
         <v>0.33333333333333331</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B21" s="2">
         <v>0.3611111111111111</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B22" s="2">
         <v>0.375</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B23" s="2">
         <v>0.4201388888888889</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B24" s="2">
         <v>0.52777777777777779</v>
       </c>
@@ -793,51 +794,51 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B25" s="2">
         <v>0.55208333333333337</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B26" s="2"/>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B28" s="2">
         <v>0.59375</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B29" s="2">
         <v>0.61458333333333337</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B30" s="2">
         <v>0.66666666666666663</v>
       </c>
@@ -845,15 +846,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B31" s="2">
         <v>0.69444444444444453</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>43559</v>
       </c>
@@ -861,50 +862,50 @@
         <v>0.3125</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B33" s="2">
         <v>0.3263888888888889</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B35" s="2">
         <v>0.41666666666666669</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B36" s="2">
         <v>0.44097222222222227</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B37" s="2">
         <v>0.52777777777777779</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B38" s="2">
         <v>0.54166666666666663</v>
       </c>
@@ -912,34 +913,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B39" s="2">
         <v>0.5625</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B40" s="2">
         <v>0.67361111111111116</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B41" s="2">
         <v>0.69444444444444453</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>43560</v>
       </c>
@@ -947,34 +948,34 @@
         <v>0.3125</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B43" s="2">
         <v>0.34722222222222227</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B44" s="2">
         <v>0.39583333333333331</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B45" s="2">
         <v>0.47916666666666669</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>43561</v>
       </c>
@@ -982,80 +983,80 @@
         <v>0.3125</v>
       </c>
       <c r="C46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B47" s="2">
         <v>0.31944444444444448</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B48" s="2">
         <v>0.375</v>
       </c>
       <c r="C48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B49" s="2"/>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B50" s="2"/>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B51" s="2">
         <v>0.52777777777777779</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C52" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B53" s="2"/>
       <c r="C53" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B54" s="2">
         <v>0.61805555555555558</v>
       </c>
       <c r="C54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B55" s="2"/>
       <c r="C55" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B56" s="2">
         <v>0.66666666666666663</v>
       </c>
@@ -1063,17 +1064,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B57" s="2">
         <v>0.68055555555555547</v>
       </c>
       <c r="C57" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D52" r:id="rId1"/>
+    <hyperlink ref="D52" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1081,107 +1082,107 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="125.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="125.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed File location from root to Vue folder
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Journal De Bord" sheetId="1" r:id="rId1"/>
     <sheet name="Question" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
   <si>
     <t>Documentation</t>
   </si>
@@ -238,9 +239,6 @@
     <t>Q9</t>
   </si>
   <si>
-    <t>Backlog user stories M court</t>
-  </si>
-  <si>
     <t>Analyse critère 4</t>
   </si>
   <si>
@@ -275,18 +273,6 @@
   </si>
   <si>
     <t>Mcd : ai-je bien implémenté la partie Evaluation-Critere-Note ?</t>
-  </si>
-  <si>
-    <t>Pas de !!!</t>
-  </si>
-  <si>
-    <t>Faudrait-il tableau des à la place des images pour le dictionnaire de données ?</t>
-  </si>
-  <si>
-    <t>Méthode en 6 étapes</t>
-  </si>
-  <si>
-    <t>Faudrait-il tableau faire un "dossier" vu alors que je n’en ai pas ?</t>
   </si>
   <si>
     <r>
@@ -311,9 +297,6 @@
     <t>rendez-vous avec M. Folomietow</t>
   </si>
   <si>
-    <t>RENDEZ-VOUS M.Court</t>
-  </si>
-  <si>
     <t>Implémentation barre de navigation</t>
   </si>
   <si>
@@ -327,6 +310,33 @@
   </si>
   <si>
     <t>Requête SQL finie</t>
+  </si>
+  <si>
+    <t>Annalyse critère 4 et 5</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>Pas d'image</t>
+  </si>
+  <si>
+    <t>Faudrait-it mettre des image pour le dictionnaire de données</t>
+  </si>
+  <si>
+    <t>rendez-vous M.Court</t>
+  </si>
+  <si>
+    <t>Performance rquete SQL , Changer affichage index.php / compte.php</t>
+  </si>
+  <si>
+    <t>Journal de bords a imprimer le jours de la défense</t>
+  </si>
+  <si>
+    <t>réponse Q11</t>
+  </si>
+  <si>
+    <t>Réponse q11</t>
   </si>
 </sst>
 </file>
@@ -379,7 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -401,6 +411,11 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -683,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +999,7 @@
         <v>0.59375</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>55</v>
@@ -1058,7 +1073,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D35" s="2"/>
     </row>
@@ -1098,7 +1113,7 @@
         <v>0.5625</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>35</v>
@@ -1212,7 +1227,7 @@
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>60</v>
@@ -1252,7 +1267,7 @@
         <v>0.61805555555555558</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D54" s="2"/>
     </row>
@@ -1273,7 +1288,7 @@
         <v>42</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1312,7 +1327,7 @@
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>64</v>
@@ -1354,7 +1369,7 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D64" s="2"/>
     </row>
@@ -1362,7 +1377,7 @@
       <c r="A65" s="6"/>
       <c r="B65" s="4"/>
       <c r="C65" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D65" s="2"/>
     </row>
@@ -1372,7 +1387,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>66</v>
@@ -1416,7 +1431,7 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D70" s="2"/>
     </row>
@@ -1470,27 +1485,93 @@
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
-      <c r="B77" s="6"/>
+      <c r="B77" s="7">
+        <v>0.6875</v>
+      </c>
       <c r="C77" s="2" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="7">
-        <v>0.6875</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>49</v>
+      <c r="A78" s="8">
+        <v>43566</v>
+      </c>
+      <c r="B78" s="9">
+        <v>0.3125</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B80" s="9">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="9">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B83" s="9">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="9">
+        <v>0.625</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="9">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1504,15 +1585,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="49.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="49.42578125" style="1"/>
@@ -1520,7 +1601,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
@@ -1534,7 +1615,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -1545,7 +1626,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>69</v>
@@ -1556,7 +1637,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>70</v>
@@ -1567,7 +1648,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>29</v>
@@ -1578,7 +1659,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -1589,7 +1670,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>26</v>
@@ -1600,7 +1681,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1608,51 +1692,63 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Documentation, logbook, planning
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="548" documentId="14_{9F97C56A-0847-4B13-96CB-9482C5495C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0D5468C6-F240-4EBD-A5D0-C6E37A451C5E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal De Bord" sheetId="1" r:id="rId1"/>
     <sheet name="Question" sheetId="2" r:id="rId2"/>
+    <sheet name="Dessin" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="118">
   <si>
     <t>Documentation</t>
   </si>
@@ -311,18 +318,12 @@
     <t>Requête SQL finie</t>
   </si>
   <si>
-    <t>Annalyse critère 4 et 5</t>
-  </si>
-  <si>
     <t>oui</t>
   </si>
   <si>
     <t>Pas d'image</t>
   </si>
   <si>
-    <t>Faudrait-it mettre des image pour le dictionnaire de données</t>
-  </si>
-  <si>
     <t>rendez-vous M.Court</t>
   </si>
   <si>
@@ -336,12 +337,69 @@
   </si>
   <si>
     <t>Réponse q11</t>
+  </si>
+  <si>
+    <t>Faudrait-it mettre des image pour le dictionnaire de données ?</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Annalyse critère 5 et 6</t>
+  </si>
+  <si>
+    <t>Implémentation critère 5</t>
+  </si>
+  <si>
+    <t>Implémentation critère 6</t>
+  </si>
+  <si>
+    <t>Alanyse Critère 7</t>
+  </si>
+  <si>
+    <t>Implémentation Critère 7</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Logiciel pour recuperer tout le code et le transformer en PDF ?</t>
+  </si>
+  <si>
+    <t>Added IMG</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Legende, annalyse des principales fonctionnalités, effectif, Demander a Mme. Travjank pour la Q12</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>Critère 2 B6 ?</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>Manuel utilisateur ?</t>
+  </si>
+  <si>
+    <t>Ne pas en faire un.</t>
+  </si>
+  <si>
+    <t>Rendre 2 fichier séparées</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -411,10 +469,11 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -432,6 +491,2109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>241290</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23707</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4220370</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>153517</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="193" name="Encre 192">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B2D20B9-5F89-4659-A2EE-0C7C9304FE5D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="241290" y="1109557"/>
+            <a:ext cx="3979080" cy="491760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="193" name="Encre 192">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B2D20B9-5F89-4659-A2EE-0C7C9304FE5D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="232650" y="1100557"/>
+              <a:ext cx="3996720" cy="509400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>184140</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>157057</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4163220</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>105892</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="287" name="Encre 286">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB6C3BA5-EA21-4912-A723-075484CD364A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="184140" y="2147782"/>
+            <a:ext cx="3979080" cy="491760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="287" name="Encre 286">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB6C3BA5-EA21-4912-A723-075484CD364A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="175500" y="2138782"/>
+              <a:ext cx="3996720" cy="509400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1572856</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>110415</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>59183</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>13995</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="288" name="Encre 287">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51240D98-072C-4DBF-A3AE-2DB65F89521C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1572856" y="2101140"/>
+            <a:ext cx="6625440" cy="627480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="288" name="Encre 287">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51240D98-072C-4DBF-A3AE-2DB65F89521C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1562091" y="2092262"/>
+              <a:ext cx="6646539" cy="644880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2472840</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>158835</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4275360</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>140430</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="317" name="Encre 316">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BEFFB02-AC14-44E1-B242-7EEDE2FBB5F3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2472840" y="2149560"/>
+            <a:ext cx="1802520" cy="524520"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="317" name="Encre 316">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BEFFB02-AC14-44E1-B242-7EEDE2FBB5F3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2463840" y="2140920"/>
+              <a:ext cx="1820160" cy="542160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>231766</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>210653</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>61620</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="324" name="Encre 323">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4BCD857-ADD8-4531-9408-E924E2776FC2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="231766" y="266595"/>
+            <a:ext cx="8118000" cy="1423800"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="324" name="Encre 323">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4BCD857-ADD8-4531-9408-E924E2776FC2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="221362" y="257762"/>
+              <a:ext cx="8138392" cy="1441112"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4541400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>374647</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>124230</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="380" name="Encre 379">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E40997C-F5A5-4709-BA9A-B0822D813E73}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4541400" y="1859760"/>
+            <a:ext cx="7020360" cy="798120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="380" name="Encre 379">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E40997C-F5A5-4709-BA9A-B0822D813E73}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4532760" y="1851120"/>
+              <a:ext cx="7038000" cy="815760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7263720</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>113580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7273440</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>48165</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="39" name="Encre 38">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{615AA352-5FE0-4663-BE5B-298F94A72F3C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7263720" y="2285280"/>
+            <a:ext cx="9720" cy="115560"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="39" name="Encre 38">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{615AA352-5FE0-4663-BE5B-298F94A72F3C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7254720" y="2276280"/>
+              <a:ext cx="27360" cy="133200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7254000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>29700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7264800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>34740</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="40" name="Encre 39">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D895D8F-1ABA-465C-AABA-D12F04F45B16}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7254000" y="2201400"/>
+            <a:ext cx="10800" cy="5040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="40" name="Encre 39">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D895D8F-1ABA-465C-AABA-D12F04F45B16}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7245360" y="2192400"/>
+              <a:ext cx="28440" cy="22680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7317360</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>169470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7320240</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>108375</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="41" name="Encre 40">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2F82B54-2B4A-4B98-86A9-471D5194E3A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7317360" y="1255320"/>
+            <a:ext cx="2880" cy="119880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="41" name="Encre 40">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2F82B54-2B4A-4B98-86A9-471D5194E3A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7308720" y="1246680"/>
+              <a:ext cx="20520" cy="137520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7293240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>67230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7293600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>71190</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="42" name="Encre 41">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16306A78-0D93-48BD-8A1F-0BC45D441CED}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7293240" y="1153080"/>
+            <a:ext cx="360" cy="3960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="42" name="Encre 41">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16306A78-0D93-48BD-8A1F-0BC45D441CED}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7284240" y="1144440"/>
+              <a:ext cx="18000" cy="21600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4528800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4727160</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>18015</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="212" name="Encre 211">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BF5A875-D754-443D-BEA1-BA5D3DD2B0D1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4528800" y="1432950"/>
+            <a:ext cx="198360" cy="213840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="212" name="Encre 211">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BF5A875-D754-443D-BEA1-BA5D3DD2B0D1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4519800" y="1423950"/>
+              <a:ext cx="216000" cy="231480"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>71047</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>148935</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85087</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180255</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="873" name="Encre 872">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02EAA8FF-B876-4C49-8CFE-799EE954F204}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10496160" y="8654760"/>
+            <a:ext cx="14040" cy="31320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="873" name="Encre 872">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02EAA8FF-B876-4C49-8CFE-799EE954F204}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10487160" y="8646120"/>
+              <a:ext cx="31680" cy="48960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>192607</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>31470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>662047</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="877" name="Encre 876">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C282A44-981F-4FA1-9560-3D758BAC1F74}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9855720" y="8356320"/>
+            <a:ext cx="469440" cy="410760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="877" name="Encre 876">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C282A44-981F-4FA1-9560-3D758BAC1F74}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9846713" y="8347680"/>
+              <a:ext cx="487094" cy="428400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190207</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>170790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>328087</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="880" name="Encre 879">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AD6A9ED-BC2E-4CA1-ACC2-A2A74A8826A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10615320" y="8495640"/>
+            <a:ext cx="137880" cy="338760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="880" name="Encre 879">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AD6A9ED-BC2E-4CA1-ACC2-A2A74A8826A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10606680" y="8486640"/>
+              <a:ext cx="155520" cy="356400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>595207</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>170790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>712207</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>88560</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="885" name="Encre 884">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C24168CF-AD9B-43EB-984D-5AEF459B8382}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11020320" y="8495640"/>
+            <a:ext cx="117000" cy="279720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="885" name="Encre 884">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C24168CF-AD9B-43EB-984D-5AEF459B8382}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11011320" y="8486652"/>
+              <a:ext cx="134640" cy="297337"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>379567</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>90150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504487</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>23040</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="886" name="Encre 885">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B24F0E86-F098-4B3C-B6EC-E22FC65E2A6C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10804680" y="8415000"/>
+            <a:ext cx="124920" cy="294840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="886" name="Encre 885">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B24F0E86-F098-4B3C-B6EC-E22FC65E2A6C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10795680" y="8406000"/>
+              <a:ext cx="142560" cy="312480"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>87840</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>69750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>69487</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>69615</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="914" name="Encre 913">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB01FEEE-C149-4180-A41E-BC534B0CDCC4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="87840" y="2965350"/>
+            <a:ext cx="9644760" cy="5972040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="914" name="Encre 913">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB01FEEE-C149-4180-A41E-BC534B0CDCC4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="78097" y="2956518"/>
+              <a:ext cx="9664651" cy="5989351"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-14T20:40:14.150"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">247 705 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">640 722 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-9 10039 0 0,4 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1036 664 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1384 746 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,4-23-839 0 0,-7 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 79 971 0 0,13-78-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,3-28 325 0 0,-7 43 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 35 365 0 0,9-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-43 40 0 0,-1 48 757 0 0,-8 6-562 0 0,-2 1-34 0 0,14 15 96 0 0,-24 51 294 0 0,10-64 48 0 0,0-2-24 0 0,-12 10 14 0 0,11-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-12 0 0,-1-2-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,16-18-798 0 0,-5 23 705 0 0,11 17 39 0 0,-21-13 64 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 2-10 0 0,2-5 84 0 0,-5 17 237 0 0,-20-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 11-3207 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">1678 463 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 57 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,1 17 113 0 0,-2-14-1404 0 0,-1 51 981 0 0,-4-2-1688 0 0,1-59-1417 0 0,-2-32 962 0 0,-7-28-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">1614 598 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-32 2722 0 0,-14 31-3180 0 0,15-15 1008 0 0,23-24 674 0 0,-35 36-2057 0 0,1 2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 19 1009 0 0,-52 14 55 0 0,-5-18-600 0 0,22 47 1448 0 0,-23 2-2113 0 0,-15-60 230 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 22 399 0 0,1-11-337 0 0,7-8-104 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 37 0 0,-35-1 653 0 0,-7-25-4978 0 0,34 19 2334 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">3006 428 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 48 1154 0 0,-12 24 2052 0 0,-3 33 1755 0 0,3 52-2463 0 0,4-54-962 0 0,-3 32-1172 0 0,7-140-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-3 13-2556 0 0,2-23 1622 0 0,1-1-894 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">3024 486 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-4 772 0 0,-14 10-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,3 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 2-1 0 0,0-2 1 0 0,1 1-1 0 0,-2 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-4-1-4 0 0,-53-44-4198 0 0,55 42-3651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">2230 124 3680 0 0,'-6'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,8 16-23 0 0,2-13-297 0 0,6 3-1604 0 0,-9 95 2 0 0,7-77 200 0 0,1-18-716 0 0,2-41-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">2155 695 1376 0 0,'5'-20'2159'0'0,"2"0"4223"0"0,7-6-3735 0 0,-3 6-1523 0 0,12-17 1153 0 0,4 12 523 0 0,-4 3-1591 0 0,22-17 135 0 0,-44 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 7-27 0 0,10 30 368 0 0,29 120 1443 0 0,-19-124-1634 0 0,0-14-84 0 0,-14-23-77 0 0,-5-2-29 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 13 0 0,40-28-350 0 0,19-12-3834 0 0,-54 36 2533 0 0,3 3-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">1 302 6448 0 0,'7'21'6309'0'0,"-7"-18"-6682"0"0,4 54 3514 0 0,8 85-847 0 0,-2-44-690 0 0,-5-10-929 0 0,13 132 737 0 0,-29 32 57 0 0,6-176-1337 0 0,-1-48-256 0 0,5-13-955 0 0,1-11-4480 0 0,0-4-582 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">12 333 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,18-38 6274 0 0,-18 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,12-3 291 0 0,71-18 828 0 0,-38 5-729 0 0,13-5 96 0 0,50 12 370 0 0,-61 8-222 0 0,43 2-1079 0 0,-22-6 16 0 0,38-20 451 0 0,-31 15 1144 0 0,61 1-1448 0 0,5 19 224 0 0,-54-19-645 0 0,-30-1 1538 0 0,6 0-1123 0 0,-36 8-292 0 0,52 0 264 0 0,-25-6 20 0 0,54-26 70 0 0,10 18-205 0 0,14 9 34 0 0,-67-4 219 0 0,22-5-424 0 0,-4 12 192 0 0,-11 5 584 0 0,45 1-1352 0 0,-8 9 736 0 0,1 6 1017 0 0,-32-10-298 0 0,-11 0-1239 0 0,25-4 520 0 0,15 3 64 0 0,12 29 75 0 0,-60-11-166 0 0,14 1 523 0 0,-3-9-840 0 0,-22-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,74-9-197 0 0,-22 19 0 0 0,-41-15-20 0 0,-44-2 0 0 0,-13-5 0 0 0,25 17 0 0 0,-38-3 0 0 0,6 6 0 0 0,12 23 64 0 0,-5 28 0 0 0,-8 23-64 0 0,-5 32-8 0 0,1-51 125 0 0,-4 32-203 0 0,-8 34 295 0 0,8 44-190 0 0,-17-84 82 0 0,-1-41-13 0 0,6-44 96 0 0,6-12-234 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 2 51 0 0,0-3 114 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0-114 0 0,-14 0 158 0 0,-97 8-218 0 0,81-3 59 0 0,0-1-1 0 0,0-2 1 0 0,0-1 0 0 0,-1-2-1 0 0,1-1 1 0 0,-22-6 1 0 0,4-4-9 0 0,-1 3 0 0 0,0 3 0 0 0,0 2 0 0 0,-23 2 9 0 0,-110 0 332 0 0,138 4-330 0 0,0-1-1 0 0,0-3 1 0 0,-1-2-1 0 0,1-1 1 0 0,-8-7-2 0 0,23 9-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-20 4 18 0 0,-144 30 64 0 0,-2-12-136 0 0,-49-9 152 0 0,173-13-80 0 0,-93 0 11 0 0,-32-17 42 0 0,100 17-53 0 0,-22-13 80 0 0,22-11-176 0 0,-86-18 224 0 0,58 22-196 0 0,62 6 192 0 0,-62-3-124 0 0,50 11 0 0 0,46 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">6713 897 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,22-14-8855 0 0,-18 9 1888 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">7088 941 10592 0 0,'-13'-13'818'0'0,"10"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">7435 851 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,5 0-232 0 0,-2 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">7798 941 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-38 1231 0 0,1 45-2463 0 0,0 1 0 0 0,2 1 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,-1 3-113 0 0,3-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-16-143 0 0,-13 33-62 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-2-43 0 0,3 2 32 0 0,1 10 23 0 0,-10 18 200 0 0,3-27-96 0 0,-7 4-695 0 0,14-7-611 0 0,7-10-5710 0 0,-6 6 446 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">8082 572 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 22-45 0 0,-12-25-3788 0 0,3 8 1039 0 0,3 83 1637 0 0,7 83-1221 0 0,-14-86-1606 0 0,0-79-341 0 0,-2-4-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">8383 613 2760 0 0,'4'8'1828'0'0,"4"20"4892"0"0,5 25-3444 0 0,1 103 1947 0 0,-11-80-3937 0 0,-6-37-4508 0 0,3-36 1701 0 0,-4 6-229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">8436 941 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,9-39 5734 0 0,3-11-521 0 0,-16 20-3279 0 0,11 10-1202 0 0,8-37 1 0 0,-14 56-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,3 0-93 0 0,2-2 95 0 0,-4 3-21 0 0,26 0-60 0 0,1 14-14 0 0,-4 7 0 0 0,-21-12 0 0 0,10 23 0 0 0,19 74 514 0 0,-19-52 356 0 0,6-19-278 0 0,-20-34-517 0 0,7 3 98 0 0,-5-1-141 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-29-4233 0 0,-22 32 2840 0 0,0 1-164 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">9223 669 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-39-6 1747 0 0,43 9-1667 0 0,4-2 170 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 42-483 0 0,18 2 618 0 0,16 12 378 0 0,10 4-513 0 0,15-4 1899 0 0,26-11-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 0 0 0 0,-22-9 0 0 0,-2 2 0 0 0,0-5-64 0 0,30-22-5497 0 0,-31 16 3530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">9488 1002 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-17 649 0 0,-9 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 20 784 0 0,-16 13 56 0 0,6-32-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">9760 661 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 73 1352 0 0,-5-54-2105 0 0,-9 63 686 0 0,-2-6-314 0 0,3 68-530 0 0,6-113-273 0 0,-3-10 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-3-14-1557 0 0,2-1 195 0 0,-3-2-70 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">9725 664 1376 0 0,'4'6'367'0'0,"-3"-5"1002"0"0,-1-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,10-7 51 0 0,32-23 1588 0 0,-29 24-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,2 2 108 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 2 0 0 0,1-2 1 0 0,0 6-108 0 0,9 27 435 0 0,0 58 787 0 0,-11-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-56 0 0,-44 35 929 0 0,43-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-5 0 0 0,4-15-5381 0 0,0 15-2125 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">10202 395 0 0 0,'-12'12'0'0'0,"6"-15"140"0"0,4 3 2586 0 0,2 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 30 3000 0 0,-14 31-1947 0 0,1 50 181 0 0,4 1 624 0 0,-7-41-881 0 0,11 38-1316 0 0,-12-26-173 0 0,8-43 0 0 0,14 3-2476 0 0,-12-41 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">10184 825 4376 0 0,'0'0'199'0'0,"10"-11"1918"0"0,-6-2 1016 0 0,11-10 683 0 0,-6-13-1297 0 0,-2-1-472 0 0,5 29-1272 0 0,-10 7-743 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 22 598 0 0,-25-17-674 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 6-227 0 0,6 92 608 0 0,-7-65-165 0 0,-1-12 997 0 0,27-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,13-10-60 0 0,-20 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27">10811 698 2760 0 0,'0'1'207'0'0,"0"45"6763"0"0,0-45-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 13-344 0 0,-2 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 9-1278 0 0,-12 63 616 0 0,0-18 973 0 0,13 39-2158 0 0,3-87 962 0 0,-3-26-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28">10875 691 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,58-25 1867 0 0,-55 27-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,2 0-156 0 0,-1 0 96 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1-95 0 0,-1-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 5-94 0 0,-43 58 1952 0 0,47-67-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink10.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:15:50.401"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 10136 0 0,'0'0'224'0'0,"0"0"40"0"0,0 0 16 0 0,0 0 8 0 0,0 0-288 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 672 0 0,0 0 88 0 0,0 9 8 0 0,0-9 8 0 0,0 0-424 0 0,0 0-80 0 0,0 0-16 0 0,0 0-8 0 0,0 0-1016 0 0,0 0-208 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:16:37.954"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">170 594 2760 0 0,'-22'-8'3128'0'0,"16"0"-821"0"0,-31-60 5175 0 0,-4-46-4528 0 0,19 34-2212 0 0,-1 5-684 0 0,12 36 1037 0 0,3 9-46 0 0,8-11-1018 0 0,16 27 738 0 0,31-2 95 0 0,18-8-285 0 0,21 11 18 0 0,41-7 553 0 0,-102 10-836 0 0,25-13-4 0 0,8 12-300 0 0,11 18-3179 0 0,-62-7 1586 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:54:15.670"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">38 1 16096 0 0,'0'0'365'0'0,"0"0"56"0"0,-7 12 546 0 0,0-3 6082 0 0,3-1-4429 0 0,-3 13-3843 0 0,6-18 1887 0 0,-10 29-320 0 0,10-31-280 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-22 0 0,0 0-119 0 0,0-8-220 0 0,2-18-184 0 0,0 13-1091 0 0,-2 0-4490 0 0,0 13-914 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:54:13.355"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">139 52 9728 0 0,'-3'28'446'0'0,"2"-22"-10"0"0,1-6-110 0 0,-7 21 5217 0 0,-4 37-376 0 0,-11 67-1014 0 0,-9 212-706 0 0,15-146-2342 0 0,10-95-825 0 0,-9 101-24 0 0,11-169-383 0 0,3-27-26 0 0,1-1-8 0 0,0 0-161 0 0,0 0-650 0 0,1-24-9059 0 0,3 5 1774 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="639.092">110 189 11776 0 0,'6'-17'1280'0'0,"0"-2"2430"0"0,2 1 2588 0 0,2 8-5875 0 0,-3 4 86 0 0,1-2-282 0 0,0 2 0 0 0,0-1 0 0 0,0 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 2 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,9-2-228 0 0,42 10 628 0 0,-56-3-593 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 2-36 0 0,10 9 14 0 0,30 34 450 0 0,-14 3 1116 0 0,-2 58-1568 0 0,-28-98 95 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-7 8-106 0 0,7-11 49 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,-3 2-50 0 0,-52 12 153 0 0,56-16-165 0 0,63-8 9 0 0,-45 7 6 0 0,-5-1-28 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,3 2 25 0 0,-1 0-62 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 3 62 0 0,5 54 641 0 0,-9-58-617 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,-2 3-24 0 0,-6 8 0 0 0,-1 0 0 0 0,0-1 0 0 0,-2-1 0 0 0,1 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,-13 8 0 0 0,8-8 0 0 0,-1-2 0 0 0,-1 0 0 0 0,0-1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0-1 0 0 0,-8 0 0 0 0,-74 23-80 0 0,17-7-16 0 0,86-24 358 0 0,-7 1-2469 0 0,5-10-7469 0 0,4 0 1106 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1210.204">893 1 14456 0 0,'0'0'330'0'0,"0"0"45"0"0,0 0 18 0 0,0 0-42 0 0,0 1-75 0 0,-3 72 6166 0 0,-5-9-4114 0 0,-18 141 1352 0 0,-4 59-2060 0 0,-11 14-805 0 0,7-75-674 0 0,26-176-350 0 0,8-26 82 0 0,-11-12-1918 0 0,6-8-4504 0 0,5 15 4273 0 0,-2-8-6349 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1636.656">935 115 1376 0 0,'7'-36'68'0'0,"7"3"5954"0"0,-5 12 1686 0 0,-8 20-7576 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-132 0 0,0 0 58 0 0,0 1 33 0 0,0-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,2 0-91 0 0,2 0 102 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,2 3-103 0 0,6 13 174 0 0,-10-14-111 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,3 1-63 0 0,34 21 581 0 0,7 34 291 0 0,-42-31-651 0 0,-1-1-1 0 0,-2 2 0 0 0,0-1 1 0 0,-2 0-1 0 0,-2 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,-1 0-1 0 0,-8 28-220 0 0,6-21 236 0 0,-2 1 0 0 0,-1-2 0 0 0,-1 1 0 0 0,-5 5-236 0 0,-23 55 424 0 0,30-82-365 0 0,1 3 31 0 0,-1 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,-9 8-90 0 0,14-15 26 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,-8 2-26 0 0,-115 9 33 0 0,-7-28-1057 0 0,71-9-4105 0 0,60 16 3206 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:54:24.955"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">100 9 3224 0 0,'0'0'457'0'0,"0"0"711"0"0,0 0 311 0 0,0 0 66 0 0,0 0-146 0 0,0 0-671 0 0,0 0-295 0 0,0 0-60 0 0,0 0 9 0 0,0 0 83 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,0 0 102 0 0,0 0 22 0 0,0 14 1235 0 0,-10 56 4955 0 0,4 25-4234 0 0,17 7-97 0 0,-9-47-1040 0 0,-3-28-1012 0 0,0 47-267 0 0,-5 173 1877 0 0,1-157-1879 0 0,6-81-48 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-4 6 0 0 0,-11 12-801 0 0,-7-12-6747 0 0,18-17-982 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="412.915">107 87 2304 0 0,'0'-2'167'0'0,"8"-15"2093"0"0,18-20 9580 0 0,0 22-10365 0 0,-22 12-1240 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,3 2-235 0 0,-2-1 218 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,3 5-217 0 0,5 9 528 0 0,-7-11-392 0 0,1 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0 3-135 0 0,-3 105 1604 0 0,-35-42-855 0 0,31-71-713 0 0,-1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1-35 0 0,1-1-135 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-4-5 136 0 0,6 5-520 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 521 0 0,-5-25-2538 0 0,5 6-19 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:54:27.595"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">67 100 10592 0 0,'0'0'818'0'0,"-3"11"2010"0"0,-12 32 2029 0 0,4 26-1721 0 0,0 16-649 0 0,-5 116 1221 0 0,12-81-2576 0 0,4 10-475 0 0,-3-113-1193 0 0,2-16-68 0 0,1-1-32 0 0,0 0-79 0 0,0 0-314 0 0,-2-14-8176 0 0,1 8 1651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="332.093">71 90 11520 0 0,'5'-10'1224'0'0,"26"-25"6290"0"0,34 0-4470 0 0,-62 33-2967 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 2-77 0 0,4 15 316 0 0,0-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-1 0-1 0 0,-1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-2 4-316 0 0,2-13 99 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,-3 5-100 0 0,5-11 18 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-18 0 0,-2-1-59 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-7-4 59 0 0,-47-32-3704 0 0,55 30 957 0 0,5-1-5943 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:54:26.707"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">142 9 3224 0 0,'-2'-8'1623'0'0,"2"7"4003"0"0,-1 1 5780 0 0,-3 42-9766 0 0,-7 14-232 0 0,-4 46-776 0 0,7 16-182 0 0,-7 69 1156 0 0,16-172-1404 0 0,-2 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,-1-1 1 0 0,-5 14-202 0 0,9 64 272 0 0,-1-85-248 0 0,1-6-103 0 0,0-1-12 0 0,0 0-71 0 0,0 0-341 0 0,-19-3-7577 0 0,14-4 457 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="423.109">0 598 2304 0 0,'0'0'101'0'0,"6"-12"5654"0"0,-2 1-935 0 0,1-12-218 0 0,24-24-1523 0 0,28-17-965 0 0,0 8-1362 0 0,-55 54-723 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,2 2-29 0 0,3 1 86 0 0,0 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-2 0-1 0 0,3 8-85 0 0,-8 81 1468 0 0,-2-79-1328 0 0,-4 13 188 0 0,1 0 0 0 0,2 1 1 0 0,1 0-1 0 0,2 0 0 0 0,1 18-328 0 0,17-52-374 0 0,15-38-3517 0 0,-22 27 1623 0 0,-1 3-436 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink17.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:26:17.165"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+    <inkml:brush xml:id="br1">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">21037 6597 0 0 0,'0'0'580'0'0,"0"0"-64"0"0,0 0 47 0 0,0 0-35 0 0,0 0-254 0 0,0 0-107 0 0,0 0-27 0 0,0 0 51 0 0,0 0 229 0 0,0 0 100 0 0,0 2 21 0 0,3 14 472 0 0,-3-14-554 0 0,0-2-3 0 0,0 0-54 0 0,0 0-223 0 0,0 0-98 0 0,0 0 51 0 0,0 0 272 0 0,0 0 95 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 0 0 0,0 6 0 0 0,0-7 0 0 0,0-1 0 0 0,0 0 36 0 0,0 0 150 0 0,0 0 66 0 0,0 0 18 0 0,0 0-29 0 0,0 7 436 0 0,2 51 2189 0 0,-4 65-643 0 0,-8-38-852 0 0,-6 69-1718 0 0,15-52-165 0 0,0-94 90 0 0,0 2-403 0 0,1 7-2730 0 0,-4-28-1033 0 0,0 1-2741 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="208.461">21033 6655 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,7-3-112 0 0,0 0 125 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 0-346 0 0,43 70 1246 0 0,-46-66-1102 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,-1-1-1 0 0,0 2-143 0 0,2-4 57 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-57 0 0,-84-6-816 0 0,57-14-3738 0 0,26 11 2908 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66203E6">22394 15965 456 0 0,'21'-42'0'0'0,"-7"27"2824"0"0,-6 4 664 0 0,-7 11-2678 0 0,-1 0 44 0 0,0 0 11 0 0,0 0 6 0 0,0 0 21 0 0,0 0 85 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,3-21 2411 0 0,-16 1-1851 0 0,12 18-1397 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-2 1-117 0 0,-3 2 139 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-3 7-139 0 0,-18 35 224 0 0,-4 47 448 0 0,28 4 696 0 0,2-95-1368 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0 0 0 0,-2-1 16 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,0 0-16 0 0,3 0-124 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 125 0 0,11-6-613 0 0,17-16-2912 0 0,-17 11 1494 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66247E6">22712 15647 5984 0 0,'2'-42'472'0'0,"0"1"5162"0"0,-2 39-3819 0 0,0 2-663 0 0,0 0-288 0 0,0 0-58 0 0,0 0-20 0 0,0 0-61 0 0,0 0-21 0 0,0 0-7 0 0,-8 5 1975 0 0,-15 110 1356 0 0,-26 212-3264 0 0,27-143-640 0 0,7-30-1060 0 0,14-138-1236 0 0,1-11-5747 0 0,0-5 911 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66269E6">22661 15829 9216 0 0,'0'0'706'0'0,"0"0"-114"0"0,4-5 3675 0 0,17-11 1993 0 0,15 6-3644 0 0,11-5-1858 0 0,5 19-1979 0 0,-47 6-2143 0 0,-2-2 1389 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.65162E6">21472 15394 6304 0 0,'13'-2'822'0'0,"-13"1"-83"0"0,0 1 249 0 0,0 0 48 0 0,0 0-31 0 0,0 0-170 0 0,0 0-71 0 0,0 0-17 0 0,0 0-27 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0 48 0 0,0 0 202 0 0,0 0 87 0 0,0 0 20 0 0,0 0-70 0 0,0 0-308 0 0,-1-1-137 0 0,-45-66 1234 0 0,-27 2 383 0 0,68 62-1902 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0 1 1 0 0,-4 2-14 0 0,-28 32 373 0 0,8 3-682 0 0,-12 57 985 0 0,25-17-666 0 0,-1 47 460 0 0,16 8-108 0 0,11-13-298 0 0,18 17-7518 0 0,-25-133 13 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.65193E6">21050 15795 11976 0 0,'0'0'546'0'0,"4"-11"204"0"0,13 4 2195 0 0,33-7 2019 0 0,23-3-3091 0 0,-34 19-1743 0 0,0 2 0 0 0,0 1 1 0 0,24 8-131 0 0,-19 1-3223 0 0,-31-10 2016 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.65267E6">21518 16009 920 0 0,'1'-3'80'0'0,"-1"2"-114"0"0,8-20 1775 0 0,19-25 8599 0 0,-13 35-9435 0 0,-2 3-70 0 0,-10 6-714 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 2-121 0 0,28 31 1528 0 0,-17 30 812 0 0,-16-55-2114 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1-226 0 0,0-4 108 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-5 1-108 0 0,6-3-56 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-2 56 0 0,1-35-2485 0 0,3 21 635 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66074E6">21836 15825 9616 0 0,'0'0'216'0'0,"0"0"32"0"0,1-2 12 0 0,8-23 16 0 0,8-32 4156 0 0,-17 55-3764 0 0,0 2 151 0 0,0 0 69 0 0,0 0 10 0 0,0 0-48 0 0,0 0-216 0 0,0 0-98 0 0,0 0-22 0 0,-7 62 3070 0 0,3-7-2456 0 0,-11 163 920 0 0,15-149-2048 0 0,-1-22-64 0 0,1-46-273 0 0,0-1-138 0 0,0 0-33 0 0,0 0-217 0 0,0-8-2919 0 0,1-5 1541 0 0,2 0-9 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66115E6">21783 15975 10136 0 0,'0'0'42'0'0,"0"1"-1"0"0,0-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-42 0 0,27-34 4246 0 0,11 4-1699 0 0,-34 26-2345 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,3 0-202 0 0,26 18 1351 0 0,-29-11-1230 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 5-121 0 0,23 82 144 0 0,-16 1-545 0 0,-17-79-269 0 0,4-12-1904 0 0,0-3-3466 0 0,0 0-762 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67256E6">22983 16006 456 0 0,'10'-3'13004'0'0,"-6"12"-6955"0"0,-7 21-4332 0 0,1-15-273 0 0,6 101-283 0 0,-2-75-2968 0 0,0 0-3416 0 0,-2-41-2002 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67278E6">23059 15640 5984 0 0,'0'0'273'0'0,"0"0"-5"0"0,0 0 121 0 0,0 0 1143 0 0,0 0 514 0 0,0 0 104 0 0,0 0-119 0 0,0 0-596 0 0,0 0-261 0 0,0 0-49 0 0,0 0-98 0 0,0 0-392 0 0,0 0-171 0 0,0 0-31 0 0,0 0-64 0 0,0 0-1670 0 0,0 0-5837 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67316E6">23190 16279 11232 0 0,'0'-4'1016'0'0,"-17"-78"3747"0"0,27 11-109 0 0,-8 63-4545 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0 0 0 0 0,3-2-109 0 0,-6 4 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,14 41 10 0 0,-16-33 52 0 0,-5 50 1898 0 0,-33 28-1744 0 0,34-85-173 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-3-1-43 0 0,2-1-36 0 0,-1 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0-2 36 0 0,5-35-2989 0 0,1 25 1539 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67411E6">23565 16057 456 0 0,'0'0'83'0'0,"0"0"42"0"0,0 0 131 0 0,0 0 32 0 0,0 0 0 0 0,0 0 49 0 0,0 0 209 0 0,0 0 94 0 0,0 0 21 0 0,0 0-5 0 0,0 0-33 0 0,0 0-14 0 0,0 0-1 0 0,0 0-74 0 0,0 0-307 0 0,0 0-135 0 0,0-1-36 0 0,9-36 684 0 0,-2-6 547 0 0,-4 18-691 0 0,-3-25 2561 0 0,0 49-2790 0 0,0 1 1 0 0,0 0 0 0 0,0 7 8134 0 0,-3 27-7718 0 0,-10 123 1476 0 0,0-85-2207 0 0,13-63-53 0 0,0-3-32 0 0,0-4-137 0 0,0-2-71 0 0,0 0-16 0 0,0 0-147 0 0,0 0-589 0 0,0 0-257 0 0,0 0-51 0 0,0 0-35 0 0,0 0-102 0 0,2 14-5517 0 0,-2-14 5738 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67441E6">23571 16099 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,0 0-140 0 0,0 0 368 0 0,0 0 187 0 0,0 0 42 0 0,-6-6 963 0 0,5 1-1582 0 0,1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,3-2-240 0 0,-5 5 154 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1-153 0 0,7 3 222 0 0,16 17-38 0 0,-4 7-184 0 0,-18-24 130 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2 5-130 0 0,3 32 130 0 0,3-17-130 0 0,0-20-97 0 0,20-10-2811 0 0,-17 1 1087 0 0,0-2-377 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1576.986">20599 6498 4608 0 0,'0'0'353'0'0,"5"11"155"0"0,-3-7 2425 0 0,8 26 3145 0 0,-8-6-3733 0 0,-11 20 1085 0 0,1 16-1742 0 0,3-7-736 0 0,9 42-312 0 0,-7-15-640 0 0,6-23 0 0 0,-14-10 0 0 0,11-42-9 0 0,0 0-146 0 0,0-1-4162 0 0,0-4-2729 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-759.689">20586 6796 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,4-3 272 0 0,0 1 2425 0 0,8-14-1132 0 0,6 6-314 0 0,-17 10-1141 0 0,9-10 879 0 0,24-21 835 0 0,9 14-867 0 0,-42 17-985 0 0,7-2 305 0 0,36 14-1282 0 0,-35-5 625 0 0,-6 27 186 0 0,-7 3 15 0 0,1-9 170 0 0,-4 11-74 0 0,6-37-411 0 0,1-2-12 0 0,0 0 37 0 0,2 10 308 0 0,15 9-12 0 0,-16-18-372 0 0,6 16-262 0 0,-1 10-1153 0 0,-5-26 785 0 0,-1-1-831 0 0,0 0-363 0 0,0 0-70 0 0,0 0-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2740.811">20168 6625 2304 0 0,'2'0'473'0'0,"3"-1"1939"0"0,-5 6 6695 0 0,-1 1-5123 0 0,2 1-5610 0 0,-4 32 3901 0 0,5 2 62 0 0,4 56-84 0 0,6 4-1147 0 0,-3-10 156 0 0,-9 11-32 0 0,-9 11-700 0 0,11-100-583 0 0,-2-12-216 0 0,0-1-65 0 0,0-2-2 0 0,2-34-3313 0 0,-6 23 1834 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2395.417">20188 6649 6912 0 0,'-11'-8'528'0'0,"27"-1"-128"0"0,6-10 4668 0 0,32 17 409 0 0,-51 2-5324 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 2-153 0 0,32 70 2062 0 0,-22 6-1603 0 0,-13-2 1130 0 0,-1-72-1534 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0-55 0 0,-24 5 67 0 0,28-10-206 0 0,-2 0-58 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-2-1 198 0 0,-4-4-5692 0 0,-5-2-1767 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.36359E6">3097 14549 7488 0 0,'0'2'340'0'0,"-6"99"3520"0"0,12 112 4791 0 0,-5 31-4784 0 0,5-61-3019 0 0,4-73-648 0 0,1-67-288 0 0,-11-41-387 0 0,0-2-33 0 0,0 0-192 0 0,0 0-790 0 0,0-5-352 0 0,2-20-70 0 0,-2-4-7 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.36416E6">3141 14647 8288 0 0,'-3'16'381'0'0,"2"-13"-6"0"0,8-34-227 0 0,-6 15 279 0 0,1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,5-6-427 0 0,-8 13 230 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 1 0 0 0,2-1-230 0 0,49-1 1008 0 0,-53 5-919 0 0,1 1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,4 4-89 0 0,1 4 277 0 0,-2-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 7-277 0 0,8 88 608 0 0,-8-97-471 0 0,-2 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,-1 3-136 0 0,0-7 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-3 0 0 0 0,-10 7 0 0 0,-25 1 0 0 0,38-13-8 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-2-1 8 0 0,-24-49-411 0 0,30 56 334 0 0,2 1 10 0 0,0 0 3 0 0,0 0 0 0 0,11 5-105 0 0,-6-1 109 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 2 60 0 0,15 22-246 0 0,39 55 1336 0 0,-36-52-896 0 0,1-2 0 0 0,1-1 1 0 0,2-1-1 0 0,7 6-194 0 0,-14-15-3 0 0,68 45-2666 0 0,-73-57 1330 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.37444E6">3876 15198 920 0 0,'0'0'327'0'0,"0"0"1035"0"0,0 9 2340 0 0,-1-6-656 0 0,0 23 2742 0 0,5-12-4840 0 0,-2-12-526 0 0,-2-2-26 0 0,0 0 12 0 0,0 0 68 0 0,0 0 32 0 0,1 1 4 0 0,41 6 1536 0 0,-5-3-1138 0 0,17-63-236 0 0,26-34 437 0 0,-44 22-618 0 0,-16 6-757 0 0,-20 63 329 0 0,1 0-31 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1-34 0 0,-4 0 41 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,-2 1-40 0 0,-20 12 98 0 0,21-13-115 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 3 17 0 0,-16 41 618 0 0,13 24-194 0 0,25 34-1082 0 0,-13-101 704 0 0,1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1-2 1 0 0,3 1-47 0 0,36-5-792 0 0,-46 4 622 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-2 170 0 0,12-9-5654 0 0,-2 7-1513 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.37552E6">4652 14839 1376 0 0,'0'0'65'0'0,"0"0"287"0"0,0 0 1184 0 0,0 0 522 0 0,0 0 100 0 0,0 0-171 0 0,0-15 1609 0 0,16-86 4054 0 0,-9 72-6749 0 0,-7 26-797 0 0,0-4-41 0 0,0 6-160 0 0,0 1-19 0 0,0 0 92 0 0,0 0 344 0 0,0 0 154 0 0,0 0 34 0 0,0 0-97 0 0,0 0-403 0 0,0 0-59 0 0,0 0 127 0 0,0 0 15 0 0,0 0 21 0 0,0 0 128 0 0,0 1 59 0 0,-7 71 675 0 0,-13 52-478 0 0,8-31-496 0 0,2 80 642 0 0,9 81-1033 0 0,-2-174 1100 0 0,-4-19-1141 0 0,7-59 208 0 0,-6 0-1960 0 0,5-1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.37579E6">4636 14955 12696 0 0,'10'-14'1376'0'0,"36"8"1778"0"0,12-5 1363 0 0,1 2-3125 0 0,4 23-1540 0 0,-42-7-2470 0 0,-15-2-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.49339E6">5661 15296 8288 0 0,'13'-33'1072'0'0,"24"-2"4316"0"0,-33 34-5186 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 3-203 0 0,3 4 280 0 0,-1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 6-281 0 0,-1-10 347 0 0,2-5-303 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1 1-44 0 0,1-1 8 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-2 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-8 0 0,-4-3-53 0 0,1 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-2-4 53 0 0,4 9-246 0 0,0-2 1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-2 245 0 0,10-27-3579 0 0,-5 19-2927 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.49221E6">5110 15065 3224 0 0,'0'-2'240'0'0,"0"-2"25"0"0,0 3 855 0 0,0 1 359 0 0,0 0 66 0 0,0 0-81 0 0,0 0-397 0 0,0 0-178 0 0,0 0-32 0 0,0 0-13 0 0,0 0-24 0 0,0 0-10 0 0,0 0-2 0 0,0 0-18 0 0,0 0-74 0 0,4 31 1869 0 0,-11 146 1427 0 0,-4 4-2668 0 0,5-90-1106 0 0,6-90-198 0 0,1 20-364 0 0,-1-21 191 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 134 0 0,3-14-2091 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.49258E6">5124 15201 8288 0 0,'3'9'2948'0'0,"4"-25"1960"0"0,-3 7-5020 0 0,29-40 3418 0 0,17-5-299 0 0,-48 52-2908 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1-99 0 0,19 30 274 0 0,18 33 16 0 0,-2-8-146 0 0,-11-21 0 0 0,-23-25-597 0 0,-4-10-3304 0 0,-1-2 2223 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35574.03">17513 6632 11888 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 14 0 0,1 10 69 0 0,-2 75 4760 0 0,-5-16-2346 0 0,6-30-2146 0 0,-1-35-594 0 0,-3 29-145 0 0,2-22-10 0 0,1-9-188 0 0,1-2-789 0 0,0 0-344 0 0,0 0-65 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35139.521">17760 6635 2304 0 0,'-3'1'3435'0'0,"8"5"13324"0"0,-3-4-18570 0 0,11 96 5563 0 0,0 28-2624 0 0,-5-51-1128 0 0,-6-66-133 0 0,-1-8-563 0 0,-1-1-257 0 0,0 0-922 0 0,0 0-3642 0 0,0 0-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-34747.75">17777 6762 1840 0 0,'0'0'83'0'0,"0"0"373"0"0,0 0 1526 0 0,0 0 670 0 0,0 0 131 0 0,2-1 950 0 0,9-6-2192 0 0,7-23 2196 0 0,-3 10-2845 0 0,-13 15-638 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,4-2-254 0 0,19 15 16 0 0,-23-6-15 0 0,43 50 773 0 0,-43-47-785 0 0,-4-7-105 0 0,12 4-2683 0 0,-13-5 751 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44644.387">16898 6448 3224 0 0,'-1'0'2310'0'0,"-1"1"10093"0"0,1 0-11285 0 0,1 2-3278 0 0,-13 169 7048 0 0,-10 34-3120 0 0,19-147-1645 0 0,5 48-583 0 0,2-100 325 0 0,-3-7-3458 0 0,0 0 1850 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44417.264">16835 6523 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,2 0-220 0 0,52 3 3130 0 0,50 25-834 0 0,-52-21-4427 0 0,-50-7-69 0 0,4 0-4147 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36024.581">17142 6868 2304 0 0,'0'0'348'0'0,"0"0"620"0"0,-8-5 2737 0 0,3-54-382 0 0,5 58-2754 0 0,-7-16 2487 0 0,2-43 2906 0 0,6 54-5754 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,1-1-207 0 0,-3 3-36 0 0,1-1 14 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,2 0 23 0 0,-2 0 21 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 2 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0-21 0 0,1 4 5 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 5-5 0 0,2-4 151 0 0,-1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,-2 3-151 0 0,5-8 28 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1-27 0 0,-3-3-27 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1 27 0 0,-5-55-3584 0 0,10 57 2142 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33796.383">18099 6861 456 0 0,'0'0'2349'0'0,"0"0"293"0"0,0 0 128 0 0,0 0-221 0 0,0 0-1013 0 0,0 0-448 0 0,0 0-89 0 0,0 0-30 0 0,4 8 1768 0 0,-1-5-2425 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0-312 0 0,52-6 2120 0 0,3-22-1296 0 0,-4-15-672 0 0,-21-2 656 0 0,-15-24-516 0 0,-33 14-160 0 0,12 52-153 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-2 1 22 0 0,-3 4 44 0 0,0 2 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-4 9-44 0 0,0-2 32 0 0,1 2-32 0 0,0 1 0 0 0,1 0 0 0 0,1-1 0 0 0,0 2 0 0 0,2-1 0 0 0,-1 9 0 0 0,3-22 8 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,3 7-8 0 0,10 5 88 0 0,39-11-2149 0 0,-19-14-6089 0 0,-22 3 1076 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33464.079">18542 6858 13824 0 0,'0'0'314'0'0,"-7"8"872"0"0,2 10-891 0 0,4-12 1764 0 0,-1-4 3765 0 0,7-3-5807 0 0,9-6-1723 0 0,-7 1-236 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-28557.543">17554 6394 4144 0 0,'0'0'319'0'0,"0"0"295"0"0,0 0 2022 0 0,0 0 904 0 0,0 0 185 0 0,0 0-408 0 0,0 0-1846 0 0,0 0-815 0 0,0 0-161 0 0,0 0-25 0 0,0 0 16 0 0,0 0 8 0 0,0 0 2 0 0,0 0-64 0 0,0 0-1313 0 0,0 0-4508 0 0,0 0-1916 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19052.719">18787 6598 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 6 160 0 0,3-3 8708 0 0,19 86-4943 0 0,-16 7-3675 0 0,-12-11-98 0 0,9-78-623 0 0,0-6-63 0 0,0-1-165 0 0,0 0-726 0 0,0 0-316 0 0,0 0-65 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-9426.741">19041 6482 920 0 0,'1'-1'67'0'0,"0"-4"143"0"0,0 4 814 0 0,-1 1 355 0 0,0 0 70 0 0,0 1 5373 0 0,0 3-3378 0 0,0 18-2234 0 0,11 164 4151 0 0,-9-31-3309 0 0,2-105-1683 0 0,-2-32-1984 0 0,0 0-3835 0 0,-2-18 3608 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-8994.302">19041 6649 3224 0 0,'0'6'527'0'0,"9"-31"8375"0"0,7-1-6343 0 0,-14 23-2627 0 0,0-1 178 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0-110 0 0,18 30 453 0 0,0 11 891 0 0,-17-24-1051 0 0,1 57 781 0 0,7 7 131 0 0,-4-38-1044 0 0,8-12-3885 0 0,-17-31 1631 0 0,-1-2-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7909.834">19600 6584 2760 0 0,'0'0'395'0'0,"0"0"617"0"0,0 0 274 0 0,0 0 53 0 0,0 0-86 0 0,0 0-380 0 0,0 0-163 0 0,0 0-36 0 0,0 0-28 0 0,0 0-85 0 0,5 0 260 0 0,-4-1 2703 0 0,-1 0-3426 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-98 0 0,-9 0 483 0 0,-28 6 677 0 0,-1 20-16 0 0,37-24-1069 0 0,-1 1-1 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,2 4-74 0 0,26 85 784 0 0,-17-66-634 0 0,-10-21-112 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1-38 0 0,-2-1-114 0 0,0 0 0 0 0,0-1 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,2-1 114 0 0,4-1-2547 0 0,0-4-5195 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7043.896">19830 6919 7112 0 0,'14'0'324'0'0,"-11"0"-4"0"0,-3 0-94 0 0,0 0 380 0 0,0 0 186 0 0,0 0 37 0 0,0 0 35 0 0,0 0 107 0 0,0 0 42 0 0,0 0 10 0 0,0 0-26 0 0,0 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-58 0 0,0 0-240 0 0,0 0-102 0 0,0 0-17 0 0,0 0-25 0 0,0 0-82 0 0,0 0-40 0 0,0 0-5 0 0,0 0-26 0 0,0 0-108 0 0,0 0-42 0 0,1-18-240 0 0,14 0 132 0 0,-15 17-8 0 0,0 1 88 0 0,0 0 35 0 0,0 0-18 0 0,-1 1-1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0-67 0 0,1 1-279 0 0,-1-2-186 0 0,0 0-42 0 0,0 0-209 0 0,0 0-857 0 0,0 0-379 0 0,0 0-80 0 0,0 0-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2101.423">18793 6250 13304 0 0,'0'0'605'0'0,"0"0"-9"0"0,0-1-381 0 0,-2-3-42 0 0,1 2 600 0 0,1 2 260 0 0,0 0 45 0 0,0 0-26 0 0,0 0-144 0 0,0 0-63 0 0,-3 20 1994 0 0,12-13-5523 0 0,-8-7-4821 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-307399.761">3589 799 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-120 0 0,0 0 193 0 0,-4-7 582 0 0,-43-24 3117 0 0,23 18-1623 0 0,-46-17-841 0 0,60 27-1311 0 0,1 1-1 0 0,-1 1 0 0 0,-1-1 1 0 0,1 2-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 1-1 0 0,1 1 0 0 0,-9 5-284 0 0,14-8 41 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 0-1 0 0,-1 2-40 0 0,5 8 100 0 0,1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0-100 0 0,-7-6 32 0 0,65 83-590 0 0,-58-70 602 0 0,0 2 1 0 0,-2-1-1 0 0,0 2 1 0 0,-1-1 0 0 0,0 1-1 0 0,-1 1 1 0 0,-1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-3 21-45 0 0,1-28 91 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 2-91 0 0,6-9 67 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,-5-3-68 0 0,6 1 4 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-2-5-4 0 0,0 1-603 0 0,0-1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-3 603 0 0,-4-11-1535 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-307011.559">3489 530 13680 0 0,'0'0'306'0'0,"-5"7"421"0"0,-1 6-534 0 0,-1 1-1 0 0,2 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 13-193 0 0,0-6 459 0 0,-9 65 963 0 0,3 1 0 0 0,4 0 0 0 0,3 0 0 0 0,5 56-1422 0 0,-10 68 1773 0 0,-6-14-700 0 0,0 109-1515 0 0,16-246-1557 0 0,-1-33 952 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-286862.719">3909 1565 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 0 0 0 0,0 0 200 0 0,0 0 24 0 0,-3-7 8 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-244252.177">4046 1922 1376 0 0,'0'0'65'0'0,"0"0"321"0"0,0 0 1322 0 0,0 0 578 0 0,0 0 119 0 0,-2 2 764 0 0,-6 7-2143 0 0,7-9-849 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1-177 0 0,-10-12 1364 0 0,-1-25 743 0 0,14 4-644 0 0,-11-28-661 0 0,11 41-733 0 0,0 0-1 0 0,1 0 1 0 0,1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,2 0 1 0 0,0 1-1 0 0,1 0 1 0 0,7-11-69 0 0,-6 9-213 0 0,23-24 417 0 0,-32 43-216 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,0 0 11 0 0,24 12-403 0 0,-12-11 372 0 0,1 10 529 0 0,-3-2 172 0 0,-9-6-605 0 0,1 0-1 0 0,-1-1 0 0 0,0 2 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 3-64 0 0,11 25-60 0 0,1 50 132 0 0,-7-47-67 0 0,-5-31 15 0 0,1 1 1 0 0,-1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 5-20 0 0,-5 17 568 0 0,7-28-650 0 0,-3 7-326 0 0,3-8 412 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-4 0 0,-1-27 743 0 0,14-38-633 0 0,-2 27-110 0 0,13-30 0 0 0,20-17-320 0 0,-14 45-430 0 0,-1 9 1668 0 0,11 3-918 0 0,-35 26-7 0 0,-2 1-32 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 38 0 0,-1-2 222 0 0,13 18 286 0 0,0 11-904 0 0,-2 22 920 0 0,-2 12-181 0 0,-6-25 197 0 0,-4 37-687 0 0,0-40 334 0 0,23 38-102 0 0,6-12-74 0 0,-27-58 31 0 0,1 1-20 0 0,27-6 135 0 0,-13-11 0 0 0,6-12-434 0 0,4-16 434 0 0,-18 23-314 0 0,2-1 685 0 0,5-11-776 0 0,-15 29 365 0 0,-1 1-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0 39 0 0,0 0 168 0 0,4-13-278 0 0,-3 10-5968 0 0,0 2-1741 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-243361.782">5063 1677 11288 0 0,'0'0'514'0'0,"-10"-10"196"0"0,8 8-539 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-171 0 0,36-47 2046 0 0,-27 41-1874 0 0,-7 6-154 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0-18 0 0,-1 1 60 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 1-60 0 0,-1 2 134 0 0,9 74 1428 0 0,-12-55-1106 0 0,-13 40 934 0 0,13-61-1313 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-5 2-77 0 0,-25-4 728 0 0,19-4-305 0 0,13 4-401 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-2-22 0 0,0-2-121 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 121 0 0,22-46-8730 0 0,-12 30 1471 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-234308.981">5554 1397 456 0 0,'-6'20'336'0'0,"0"0"10502"0"0,5-16-10470 0 0,1 54 5149 0 0,0 21-1998 0 0,10 55-1146 0 0,7-61-2293 0 0,13-24 752 0 0,-3-10-288 0 0,-20-32-468 0 0,2-6 16 0 0,29-4 116 0 0,8-22 32 0 0,-3-34-153 0 0,-15 14-38 0 0,-2 5-49 0 0,-6 14 0 0 0,14-38 64 0 0,-11 28-74 0 0,-14 26-44 0 0,2-20 54 0 0,-1 19 28 0 0,-4-8-2 0 0,3-4-69 0 0,-8 22 96 0 0,-3 19-9 0 0,-9 60-144 0 0,7-7 100 0 0,2-40 0 0 0,2 18 0 0 0,-8 45 254 0 0,-10-1-28 0 0,-10 29 293 0 0,6-57 286 0 0,15-40-797 0 0,-1 1 0 0 0,-1-2 1 0 0,-1 1-1 0 0,-1-2 0 0 0,-1 0 0 0 0,-7 10-8 0 0,9-18 52 0 0,0-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,0-1-1 0 0,-1 0 0 0 0,-4 2-51 0 0,11-8 15 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2-1-14 0 0,7 1-35 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-3 34 0 0,-1-2 20 0 0,10-79-2121 0 0,-9 53-659 0 0,0 19 1197 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-233142.626">6149 1779 1840 0 0,'1'-1'138'0'0,"-1"0"0"0"0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1-138 0 0,13 0 3296 0 0,36-8 1940 0 0,-32 1-4448 0 0,55-29 1921 0 0,-13-17-1408 0 0,-52 39-1068 0 0,-6 10-211 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 0-21 0 0,-1 0 9 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-4-1-9 0 0,-4-4-199 0 0,10 6 228 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0 1-1 0 0,-3-1-28 0 0,-13 5 307 0 0,15-5-243 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-2 3-64 0 0,0 3 118 0 0,-3 2 3 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1 0 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,0 7-121 0 0,1-10 43 0 0,1-1-1 0 0,0 0 1 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,3 4-43 0 0,2 0 29 0 0,26 22 88 0 0,-27-30-139 0 0,1-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,3-1 23 0 0,51-5-3801 0 0,-43 6 2362 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-231376.003">6705 1431 4832 0 0,'2'65'3666'0'0,"1"-43"-222"0"0,-2-21-2786 0 0,-2 34 2622 0 0,2 73 551 0 0,-1-43-3103 0 0,0 46 110 0 0,0-38-4281 0 0,0-72-1079 0 0,0-1-1230 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-230982.797">6695 1701 3680 0 0,'0'0'284'0'0,"0"-1"-187"0"0,0-2 155 0 0,2-12 5681 0 0,7-11-2141 0 0,-4 13-2532 0 0,-4 9-1000 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,0 0-260 0 0,28-20 850 0 0,-29 22-780 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 1-70 0 0,30 32 293 0 0,30 47 1327 0 0,-64-81-1617 0 0,3 3 19 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 2-22 0 0,10 56 581 0 0,-18-34-1430 0 0,6-21-1922 0 0,-2 0 1115 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-220476.757">7259 1444 6880 0 0,'0'0'314'0'0,"0"0"-6"0"0,0 0-77 0 0,0 0 409 0 0,0 0 199 0 0,0 0 38 0 0,0 0-32 0 0,0 0-173 0 0,0 0-80 0 0,0 0-14 0 0,0 0-2 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 6 0 0,0 0 30 0 0,7 14 2401 0 0,9 31-517 0 0,-15 36-102 0 0,-8-15-1028 0 0,4-53-1323 0 0,1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,0-1 1 0 0,2 6-35 0 0,1 56 86 0 0,0-18-106 0 0,-2-51 540 0 0,-2-5-4113 0 0,1 1-6903 0 0,0-2 5190 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-220015.405">7275 1646 1840 0 0,'0'0'403'0'0,"0"0"1018"0"0,0-5 1680 0 0,1 3 1760 0 0,27-60 991 0 0,-23 55-5592 0 0,0 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,2 0 1 0 0,1-1-260 0 0,-5 5 92 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 1-1 0 0,1 1-92 0 0,29 52 1184 0 0,-17-13-1184 0 0,-5 51 0 0 0,-7-47 848 0 0,-4-47-637 0 0,0-1-324 0 0,0 0-141 0 0,0 0-30 0 0,0 0-132 0 0,-5 8-4129 0 0,2-6-2469 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-218714.051">7763 1691 6304 0 0,'0'0'289'0'0,"0"0"-8"0"0,0 0-50 0 0,0 0 462 0 0,0 0 218 0 0,0 0 45 0 0,0 0-8 0 0,0 0-77 0 0,2 1-37 0 0,8 4 1041 0 0,-9-4-1679 0 0,1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1-197 0 0,61-48 1877 0 0,-7-8-1229 0 0,-48 43-648 0 0,-10 11 43 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,-3 1-43 0 0,2 0 15 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 2-15 0 0,-1 2 78 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0 7-78 0 0,0-7 84 0 0,0 4-20 0 0,1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1 0 0 0 0,1 0 0 0 0,1 4-64 0 0,30 101 743 0 0,-31-115-717 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,4-1-26 0 0,2-3-217 0 0,0-1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,4-8 217 0 0,23-19-3383 0 0,-22 24 1685 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-217159.938">8212 1886 1376 0 0,'0'0'65'0'0,"0"0"286"0"0,0 0 1176 0 0,0 0 510 0 0,0 0 105 0 0,0 0-140 0 0,0 0-688 0 0,0 0-303 0 0,0 0-62 0 0,0 0-31 0 0,0 0-86 0 0,10-8 1503 0 0,24-87 2243 0 0,-1 6-2552 0 0,36-61-1672 0 0,32-14 444 0 0,-47 72 85 0 0,-42 69-1159 0 0,-11 22 177 0 0,-1 1 151 0 0,0 0 68 0 0,0 0 10 0 0,6 10-109 0 0,4 75 56 0 0,-13-3-233 0 0,3 120 500 0 0,4 120-424 0 0,2-252-61 0 0,-6-69-590 0 0,0-1-241 0 0,-1-1-1406 0 0,-4-5-5471 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-216555.754">8279 1745 6448 0 0,'0'0'498'0'0,"4"-4"32"0"0,0 0 484 0 0,-3 3-660 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-354 0 0,55-13 3164 0 0,36 29-2595 0 0,-78-14-475 0 0,-3 0-1562 0 0,-3-1-3055 0 0,-1-1-2147 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-215887.433">8824 1619 920 0 0,'0'0'295'0'0,"0"0"901"0"0,-4-15 3639 0 0,2 13-5213 0 0,-3-1 8750 0 0,3 3-7138 0 0,1 0-721 0 0,-6 4 1698 0 0,-12 26-994 0 0,0 21-137 0 0,11 7 52 0 0,21 23 127 0 0,-12-77-1227 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,2 1-32 0 0,-2-1 21 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1-2-20 0 0,51-50-20 0 0,-12-29-456 0 0,-33 43-464 0 0,-22 7-1392 0 0,11 34-2925 0 0,1 0-1661 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-215158.946">9255 1298 2304 0 0,'0'1'167'0'0,"3"24"1727"0"0,-8-7 5773 0 0,-3 118 1948 0 0,5-16-6975 0 0,6-38-2192 0 0,1 76-376 0 0,2-76-72 0 0,4-2-3116 0 0,-10-79 1546 0 0,0-1-280 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-214871.79">9241 1531 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,1-2-344 0 0,25-21 826 0 0,7 17 3479 0 0,2-2-2907 0 0,11 2-1414 0 0,-23 9-2102 0 0,-13 0-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213551.059">9666 1714 10136 0 0,'8'12'230'0'0,"-6"-10"30"0"0,-2-2 19 0 0,0 0 104 0 0,-3 20 7879 0 0,4-19-7647 0 0,-1-1-21 0 0,1 1-38 0 0,9-1-436 0 0,-1 1-1 0 0,0-2 0 0 0,1 1 1 0 0,-1-2-1 0 0,0 1 0 0 0,1-1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-2 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-2 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2-1-1 0 0,3-4-119 0 0,7-49 69 0 0,-14 60-69 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-3 0 0 0 0,1 1 61 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1-61 0 0,-48 58-543 0 0,45-53 613 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 7-70 0 0,2-8 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,5 4 0 0 0,-7-8-56 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 56 0 0,8-4-1098 0 0,1-2-56 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213242.538">10188 1541 4608 0 0,'-17'14'3105'0'0,"0"1"6005"0"0,10 0-7943 0 0,-4 9 1032 0 0,9 16-1221 0 0,-3 46 1209 0 0,4-78-2095 0 0,1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,2 1-92 0 0,2-3 0 0 0,-6-5 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,17-30 0 0 0,-3 0 0 0 0,0-1 0 0 0,-2-1 0 0 0,-1-2 0 0 0,-7 12 0 0 0,-14 8-1384 0 0,7 18 600 0 0,1 1-1144 0 0,0 0-496 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212663.88">10669 1482 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0 88 0 0,0 0 1067 0 0,0 0 483 0 0,0 0 98 0 0,0 0-138 0 0,0 0-670 0 0,0 0-295 0 0,0 0-60 0 0,0 0-101 0 0,0 0-377 0 0,0 0-167 0 0,0 0-31 0 0,-3 9 1448 0 0,0 92 1023 0 0,9-9-2584 0 0,-2-31 1296 0 0,2 92-752 0 0,-3-140-818 0 0,-2-12-854 0 0,-1-1-382 0 0,0 0-76 0 0,0 0-20 0 0,0 0-2 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212449.687">10689 1697 456 0 0,'-5'-9'365'0'0,"4"8"1529"0"0,1-6 6369 0 0,3-6-4715 0 0,16-27-181 0 0,-11 21-2471 0 0,-2 10-747 0 0,-5 7-63 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-85 0 0,-2 1 239 0 0,9 5 186 0 0,-6-3-373 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 4-52 0 0,6 6 0 0 0,-9-13-55 0 0,-1-1-16 0 0,5 5-460 0 0,-4-3-2608 0 0,-1-2-3526 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-206308.339">2652 2649 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,0 2-294 0 0,-5 8 6808 0 0,0-7-3282 0 0,-8-20-2050 0 0,13 16-1469 0 0,-10-98 2153 0 0,10-139-1048 0 0,-4 0-752 0 0,-6-56-24 0 0,-3 51-128 0 0,3-99-168 0 0,6 165 559 0 0,-8-52-726 0 0,8 94-532 0 0,-2 21 446 0 0,2 39-11 0 0,0 17 64 0 0,1 2 0 0 0,7-110 128 0 0,3 130-128 0 0,9 13 0 0 0,-9 20-4 0 0,0-1 1 0 0,0 2-1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,7 4 4 0 0,30 10 0 0 0,-22-8 79 0 0,1 0 0 0 0,-1-2-1 0 0,1-1 1 0 0,0-1-1 0 0,1-1-78 0 0,31-2-104 0 0,1-3 0 0 0,-1-3-1 0 0,1-3 1 0 0,51-15 104 0 0,348-68 0 0 0,-349 81 0 0 0,0 5 0 0 0,0 6 0 0 0,33 8 0 0 0,16-1 0 0 0,4-6 99 0 0,0-7-1 0 0,75-17-98 0 0,-99 9 64 0 0,95 6-64 0 0,-148 11 41 0 0,1 4-1 0 0,33 11-40 0 0,7 1 143 0 0,68 3 11 0 0,2-9-1 0 0,147-13-153 0 0,33-22 125 0 0,-265 16-98 0 0,141 4 106 0 0,162 32 123 0 0,-64-1-170 0 0,316-33 188 0 0,-287 23 29 0 0,-166-6-190 0 0,-55-3-38 0 0,141-12-75 0 0,31-13 0 0 0,-154 6 128 0 0,36 10-128 0 0,294 41 0 0 0,-423-42 0 0 0,32-18 64 0 0,54-20-160 0 0,-118 33 85 0 0,19 0-42 0 0,22-27 429 0 0,-58 29-376 0 0,-15 8 0 0 0,-2 4 0 0 0,9 17 0 0 0,-12 1 0 0 0,18 64 0 0 0,-11 4-189 0 0,-5 0-1 0 0,4 95 190 0 0,-8 12 307 0 0,5 187-618 0 0,-10 113 606 0 0,1-147-200 0 0,5-4-14 0 0,-6-153-6 0 0,-4-180-59 0 0,0-1 1 0 0,-1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,-3 9-17 0 0,5-23 9 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1-9 0 0,-43-2 22 0 0,1-3 0 0 0,0-1-1 0 0,1-4 1 0 0,-10-4-22 0 0,-82-17 52 0 0,-103 10-87 0 0,26 29 35 0 0,-324 9 0 0 0,-18-17 0 0 0,276 18 70 0 0,-13 17-70 0 0,-62 6 47 0 0,267-32-39 0 0,-363 18-5 0 0,-320-20-3 0 0,-313 30 240 0 0,583-43-256 0 0,106-15-48 0 0,20-7 64 0 0,-72 7 11 0 0,190 10 114 0 0,-68-27-85 0 0,-40-28-40 0 0,232 46 0 0 0,-14 7 0 0 0,-1 28 0 0 0,-35-12 0 0 0,76-8-100 0 0,99 4 7 0 0,7 3-64 0 0,0-1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1 156 0 0,1-10-10012 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202306.829">6824 2965 3224 0 0,'0'2'240'0'0,"17"57"4562"0"0,-7-10 530 0 0,-4-24-2824 0 0,-2 9-572 0 0,6 46 269 0 0,4 27-781 0 0,-1 49 0 0 0,4 111 552 0 0,-1-124-1272 0 0,8 153 568 0 0,-16-38-696 0 0,1-123-389 0 0,-2 41 722 0 0,-7-54-581 0 0,-3-2-93 0 0,6-5-91 0 0,-6 40-19 0 0,3-99-61 0 0,-4 85 0 0 0,0-107-64 0 0,4-28-67 0 0,0-5-281 0 0,0-1-129 0 0,0 0-31 0 0,0 0-72 0 0,-4-17-3152 0 0,1 2-2356 0 0,0-4-1623 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201855.109">6521 4734 12264 0 0,'0'0'273'0'0,"-5"14"786"0"0,5-4-595 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,3 5-464 0 0,-5-10 43 0 0,46 112 3185 0 0,26 119 95 0 0,-57-169-2734 0 0,3-1 0 0 0,23 57-589 0 0,18 11 416 0 0,-3-53-72 0 0,-47-71-248 0 0,0 0-1 0 0,0-1 0 0 0,1 0 1 0 0,0-1-1 0 0,0-1 1 0 0,12 7-96 0 0,-19-12 39 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-39 0 0,56-64 528 0 0,17-74-224 0 0,64-284-391 0 0,-129 389-257 0 0,22-56-4278 0 0,-29 83 2515 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186308.475">12549 1257 1840 0 0,'0'0'83'0'0,"0"1"-6"0"0,0 4 363 0 0,0-4 1761 0 0,0-1 766 0 0,1 19 5666 0 0,1-1-5371 0 0,1 18-970 0 0,-3-25-1727 0 0,-10 107 2961 0 0,-23 79-2557 0 0,36-156-1425 0 0,-3-41 48 0 0,0 0-940 0 0,0 0-410 0 0,1 0-88 0 0,4-5-10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-185850.611">12876 1257 13040 0 0,'0'0'597'0'0,"0"0"-9"0"0,0 0-220 0 0,0 0 481 0 0,0 0 250 0 0,0-5 715 0 0,-1 4 3304 0 0,-4 3-5002 0 0,0 1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 3-116 0 0,0 2 121 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,3 4-120 0 0,43 111 0 0 0,-44-95 0 0 0,-7-24 0 0 0,0-5 60 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,-1-2-60 0 0,-4-4-110 0 0,7 7-9 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 119 0 0,1-7-1959 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-187118.879">11947 926 13184 0 0,'0'0'604'0'0,"0"0"-14"0"0,0 0-252 0 0,0 0 326 0 0,0 0 185 0 0,0 0 41 0 0,2 0-12 0 0,-1-1-747 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0-131 0 0,6 17 493 0 0,-2 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-2 0 1 0 0,1 18-493 0 0,-3-33 76 0 0,-2 91 1295 0 0,1 20-942 0 0,-5-17-247 0 0,-2 118-43 0 0,11-173-247 0 0,-2-43-448 0 0,-1-1-176 0 0,0 0-32 0 0,3-21-3836 0 0,-2 1 2544 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186774.862">12014 1320 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-79 0 0,0 0-421 0 0,0 0-180 0 0,0 0-37 0 0,0-14 1908 0 0,1 9-2997 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-346 0 0,12-9 712 0 0,-14 10-708 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,2 0-4 0 0,-1 0 90 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 1-1 0 0,1 0-89 0 0,47 202 1931 0 0,-45-182-1912 0 0,-1 1 1 0 0,0-1-1 0 0,-2 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,-2 3-19 0 0,0 6-4294 0 0,2-35-4235 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184500.212">13244 1138 11976 0 0,'-3'2'1082'0'0,"-17"95"550"0"0,2 54 3297 0 0,12 52-1046 0 0,9-100-3866 0 0,4-75-17 0 0,-7-26-850 0 0,0 3 2050 0 0,0-2-4324 0 0,0 4-3781 0 0,0-7 913 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184054.319">13301 1182 3224 0 0,'0'0'143'0'0,"1"1"-3"0"0,3 4 390 0 0,12 11 9462 0 0,3-2-5178 0 0,-15-11-4675 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0-138 0 0,31 3-1260 0 0,-20-7 497 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-183416.48">13187 1271 5960 0 0,'-3'-8'266'0'0,"3"7"1"0"0,0-22 1002 0 0,9-17 3955 0 0,11-5-2882 0 0,-10-5-311 0 0,-8 47-2036 0 0,-6-14-175 0 0,0 13-433 0 0,4 4-2775 0 0,0 0 1855 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-182333.102">13541 1568 0 0 0,'0'0'2721'0'0,"0"0"-302"0"0,0 0 223 0 0,1-1-119 0 0,8-8-671 0 0,-8 7-1682 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0-170 0 0,5 2 296 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,2 8-296 0 0,7 44 792 0 0,-11-56-721 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,-2 2-71 0 0,4-4 2 0 0,-1 1 15 0 0,-1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,-1-1-18 0 0,0 1 49 0 0,-1-1 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1-1-1 0 0,1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0-2-49 0 0,2 3-126 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,2-4 126 0 0,12-34-3998 0 0,-2 22-3873 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-175901.286">13952 1537 4144 0 0,'0'0'191'0'0,"0"0"375"0"0,-4-9 14804 0 0,9 56-13610 0 0,2 19 8 0 0,3 26 351 0 0,-9-75-1781 0 0,7 22-3577 0 0,-8-38 1789 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172641.548">14618 1695 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,1 1-72 0 0,14 38 5565 0 0,-10-25-3129 0 0,0-12-2556 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-2-1 0 0,-1 1 0 0 0,4-4-209 0 0,59-64 153 0 0,-47 35-213 0 0,-19 35 61 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 0 0 0,0-1 2 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-3 1-2 0 0,-14 8 0 0 0,15-8 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-3 5 0 0 0,-4 11 27 0 0,5-11 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 2-27 0 0,1-5-27 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,4 5 28 0 0,14-1 0 0 0,20-20-1385 0 0,-29 3-166 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172385.72">15083 1719 11832 0 0,'-34'14'7253'0'0,"31"-12"-6259"0"0,3-1-12 0 0,0-1-29 0 0,0 0-122 0 0,0 0-482 0 0,0 0-205 0 0,0 0-44 0 0,0 0-7 0 0,0 0 17 0 0,0 0 8 0 0,0 0 2 0 0,0 0-237 0 0,0 0-996 0 0,0 0-434 0 0,1 0-86 0 0,4 0-21 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170574.713">15822 1121 2760 0 0,'0'0'589'0'0,"0"0"1434"0"0,0 0 626 0 0,0 0 126 0 0,0 0-214 0 0,0 8 88 0 0,0 171 4329 0 0,0 91-4387 0 0,-1-167-2591 0 0,-3 26 0 0 0,4-63 0 0 0,-3-3-134 0 0,3-62-570 0 0,0-1-263 0 0,0 0-916 0 0,0-1-3632 0 0,-2-5-1553 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170137.543">15788 1582 5064 0 0,'0'0'389'0'0,"2"-3"794"0"0,0 1 3071 0 0,24-31 3094 0 0,7-4-4244 0 0,18-4-1223 0 0,-46 40-1852 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 1-29 0 0,5 16 310 0 0,-2 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,-1 10-310 0 0,-7 90 1048 0 0,7-92-908 0 0,5-1-148 0 0,10-34-432 0 0,3-13-1437 0 0,2 1-5762 0 0,-8 5 145 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172102.041">15380 1364 9760 0 0,'3'-26'2366'0'0,"-3"25"-894"0"0,0 1 68 0 0,0 0-60 0 0,0 0-321 0 0,0 0-139 0 0,0 0-27 0 0,0 0-34 0 0,0 0-114 0 0,-2 6 736 0 0,-8 73 997 0 0,2 35-801 0 0,-6 76-1676 0 0,8-115-101 0 0,3 23 0 0 0,2-85 704 0 0,-1-2-2693 0 0,1 3-6478 0 0,1-14 756 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-171739.932">15410 1364 16064 0 0,'4'-14'1715'0'0,"-2"10"-1471"0"0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,3 0-244 0 0,-3 0 90 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,3 2-90 0 0,-2 7 116 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,-1 0 1 0 0,-4 9-116 0 0,-40 68 1297 0 0,47-86-1274 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1-22 0 0,-1-1-128 0 0,2 1 21 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,1 0 106 0 0,-1-10-1478 0 0,-2 2-66 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174133.091">14303 1415 4144 0 0,'0'0'319'0'0,"0"0"-7"0"0,0 0 751 0 0,0 0 355 0 0,0 0 71 0 0,0 0-42 0 0,0 0-234 0 0,0 0-101 0 0,0 0-21 0 0,0 19 3966 0 0,-9 4-3283 0 0,8-21-1264 0 0,1-2-29 0 0,0 2-8 0 0,-3 249 2166 0 0,-9-135-2099 0 0,7-62 33 0 0,-1 21-3333 0 0,7-76 56 0 0,1-8-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173508.196">14267 1653 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,1-1 491 0 0,25-52 6288 0 0,-24 50-6862 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,1 1-157 0 0,0 0 54 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,1 1-53 0 0,0-6-149 0 0,4 18-2358 0 0,-4-9 487 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-169732.621">16337 1391 18287 0 0,'0'0'414'0'0,"0"0"56"0"0,0 1 32 0 0,0 84 1564 0 0,-11 58 154 0 0,1 10-612 0 0,4-20 14 0 0,-2-52-1333 0 0,8-80-974 0 0,0-1-274 0 0,0 0-53 0 0,0 0-215 0 0,0 0-858 0 0,0 0-379 0 0,1-2-80 0 0,2-13-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168923.508">16394 1507 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,3-7-322 0 0,3-4-3 0 0,-3 5 250 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1-1 0 0,1-1-460 0 0,-2 1 236 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 2-1 0 0,0-1 1 0 0,0 0-236 0 0,1 2 105 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,3 5-105 0 0,11 84 177 0 0,-26 79 1151 0 0,-10-109-745 0 0,17-62-571 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-2 0 0 0,1 1 0 0 0,-2-1-12 0 0,-3-2-508 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,-5-8 508 0 0,1 1-1504 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-130876.917">2833 6188 6448 0 0,'23'-2'672'0'0,"-20"1"-608"0"0,1 3 3996 0 0,-2 5-3602 0 0,-2-3 96 0 0,1-3 14 0 0,-3 12 453 0 0,8 165 2956 0 0,-11 72-1512 0 0,9-98-1338 0 0,3-73-1094 0 0,-4-70-94 0 0,-3-7-264 0 0,4-17-6236 0 0,-1 2 317 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-124973.04">2852 6239 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 0-79 0 0,0 0 561 0 0,0 0 272 0 0,-3 7 1195 0 0,-3-4 2766 0 0,7-10-4160 0 0,8-13-1197 0 0,-7 13 345 0 0,2 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,4 0-78 0 0,-6 2-15 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 15 0 0,20 116 716 0 0,-22-117-672 0 0,2 2 51 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-95 0 0,-33 27 236 0 0,30-30-233 0 0,-3 2 17 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-2 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,-9 0-20 0 0,-25-5-116 0 0,41 0 127 0 0,3 2 42 0 0,9 13-2 0 0,35 49-118 0 0,63 112 1347 0 0,-62-104-1908 0 0,-28-56-2350 0 0,-9-6-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123928.98">3297 6776 3224 0 0,'0'0'143'0'0,"0"0"315"0"0,0 0 1222 0 0,0 0 531 0 0,0 0 106 0 0,0 0-213 0 0,0 0-968 0 0,0 0-428 0 0,5 10 1069 0 0,0-8-1546 0 0,1 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,3-2-231 0 0,-7 3-25 0 0,10-4 212 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1-1 1 0 0,-1 1-1 0 0,0-2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-2-186 0 0,-6 7 3 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-4-3 0 0,0 7 35 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-35 0 0,0-1 16 0 0,-1 1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1-16 0 0,-48 120 249 0 0,34-10-267 0 0,17-106 28 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,4 3-9 0 0,-5-6 6 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,5-1-6 0 0,-5 0 57 0 0,24-6-1613 0 0,-10 1-3577 0 0,-2-5-2072 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123239.429">3865 6319 920 0 0,'0'0'279'0'0,"0"0"833"0"0,0 0 362 0 0,0 0 78 0 0,0 0-63 0 0,0 0-322 0 0,0 0-140 0 0,0 0-31 0 0,0 0-26 0 0,0 0-88 0 0,0 0-40 0 0,0 0-8 0 0,0 0-34 0 0,0 0-136 0 0,0 0-66 0 0,0 0-12 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0-42 0 0,0 7-12 0 0,-9 47 1334 0 0,2 14-600 0 0,0 50 252 0 0,8 96-1210 0 0,2-96-216 0 0,7-13 642 0 0,-4-91-1088 0 0,-5-12-25 0 0,-1-2-998 0 0,0 0-429 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122817.09">3839 6537 12176 0 0,'0'0'561'0'0,"0"0"-17"0"0,2 1-217 0 0,77 9 5294 0 0,-10 9-5284 0 0,-10 9-2062 0 0,-57-28 475 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122538.437">4257 6834 2304 0 0,'-11'-8'3825'0'0,"9"5"-3248"0"0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-5-578 0 0,1 4 116 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0-116 0 0,-2 1 36 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 2-36 0 0,50 60 1232 0 0,-48-52-822 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,-1-1-1 0 0,0 2 1 0 0,0-1-1 0 0,-2 0 1 0 0,1 1 0 0 0,-1 9-410 0 0,-13 37 100 0 0,11-57-42 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 1-58 0 0,-2-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-4-3 0 0 0,-30-45-1424 0 0,29 25-5473 0 0,4 13-533 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121496.511">4622 6625 15176 0 0,'0'0'340'0'0,"0"0"50"0"0,-2 1 26 0 0,-13 19 101 0 0,12-16-271 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0-245 0 0,3 57-21 0 0,42 58 1584 0 0,-42-115-1524 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,2 0-39 0 0,-1-3-10 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,1-2 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-2 10 0 0,2-4 49 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-2 0-1 0 0,1 0 1 0 0,-2-13-49 0 0,1 12-17 0 0,0 17 17 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 0 0 0,-12 36-209 0 0,12 91 192 0 0,11-91-2918 0 0,-10-23 1407 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-118100.252">5082 6571 4608 0 0,'22'-33'2473'0'0,"-14"18"4749"0"0,-3 19-1038 0 0,-1 7-5674 0 0,1-1-1 0 0,-1 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 2-509 0 0,6 35 445 0 0,-1 22-52 0 0,5 70-233 0 0,-8-77-380 0 0,6 3-218 0 0,-10-65 32 0 0,0-2-1020 0 0,0 0-4245 0 0,0 0-1815 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-117537.033">5129 6674 1376 0 0,'0'0'448'0'0,"0"0"1344"0"0,0 0 588 0 0,0 0 116 0 0,0 0-136 0 0,0 0-684 0 0,0 0-299 0 0,0 0-58 0 0,0 0-107 0 0,0 0-419 0 0,0 0-179 0 0,0 0-35 0 0,0 0-40 0 0,10-4 578 0 0,48-64 1084 0 0,-55 67-2155 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0-45 0 0,39 32 240 0 0,-10 33 664 0 0,-32-66-973 0 0,-1-1-608 0 0,0 0-262 0 0,0 0-1349 0 0,0 0-5210 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116084.978">5615 6722 920 0 0,'0'17'0'0'0,"0"-17"80"0"0,0 0-80 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 352 0 0,0 0 64 0 0,0 0 0 0 0,0 0 8 0 0,0 6-424 0 0,0-6 0 0 0,0 0 0 0 0,2 11-96 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115526.386">5637 6516 7856 0 0,'0'0'174'0'0,"0"0"29"0"0,0 0 13 0 0,0 9 2112 0 0,7 28 1209 0 0,-6-10-1555 0 0,4 68 1712 0 0,-1 27-2229 0 0,0-46-1465 0 0,-3-32 69 0 0,-2-25-2628 0 0,1-14 952 0 0,0-5-279 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115183.311">5637 6773 11832 0 0,'0'-17'1285'0'0,"22"-59"4317"0"0,17 32-3283 0 0,-36 43-2299 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1-20 0 0,18 39 831 0 0,16 53 83 0 0,-26-45-684 0 0,-6 8 68 0 0,-7-26-874 0 0,3-32 150 0 0,0-1-988 0 0,-1 1-436 0 0,-1 4-92 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-114236.626">6072 6790 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0 0 43 0 0,0 0 159 0 0,0 0 70 0 0,0 0 14 0 0,0 0 69 0 0,0 0 285 0 0,0 0 126 0 0,0 0 29 0 0,0 0-15 0 0,0 0-77 0 0,0 0-31 0 0,0 0-8 0 0,0 0-33 0 0,0 0-134 0 0,2 1-61 0 0,43 6 2321 0 0,-29-8-2644 0 0,32-21 394 0 0,-45 20-751 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-4 19 0 0,-7-6 0 0 0,6 11 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,-1 1 76 0 0,0 1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,1 3-75 0 0,38 54 0 0 0,-39-61 25 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,2-1-25 0 0,43-22-3889 0 0,-40 15-4253 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-106495.084">6591 6608 2760 0 0,'-32'-29'1211'0'0,"31"28"-702"0"0,-13-6 1981 0 0,-3 8-1483 0 0,10 5-408 0 0,-26 17 451 0 0,14-22 2469 0 0,7-5 2535 0 0,17-3-4219 0 0,42-13 338 0 0,36 21-421 0 0,-77 2-1693 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 2-59 0 0,43 34-101 0 0,-15-40 802 0 0,-33-2-571 0 0,-1 1 4 0 0,0 0-4 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-2 0 0,0 0-6 0 0,-17 28 213 0 0,-26 3-28 0 0,12-10-202 0 0,-35 16-64 0 0,-25 24 212 0 0,48-16-359 0 0,20-17 389 0 0,19-19-217 0 0,1-3 36 0 0,4-5-46 0 0,-1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-14 0 0,45-13 417 0 0,143-23 582 0 0,-139 39-919 0 0,-12 12-3590 0 0,-38-16 1676 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101751.894">6981 6933 3680 0 0,'-6'17'1721'0'0,"5"-12"9907"0"0,13-11-8856 0 0,14-14-2535 0 0,48-89 2026 0 0,2-45-1063 0 0,48-118-374 0 0,12 13-1554 0 0,-112 233 728 0 0,-9 0 0 0 0,-15 27 24 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1-23 0 0,-1 23 138 0 0,-1-1 0 0 0,-1 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,-6 18-138 0 0,-6 29 173 0 0,-10 75-35 0 0,20-44 4 0 0,7-84-93 0 0,-1 0 0 0 0,2-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,1 6-50 0 0,1 2 36 0 0,8 20 71 0 0,10 1 53 0 0,-15-50 10 0 0,56-159 270 0 0,-2 19-376 0 0,49-141-64 0 0,-67 188 0 0 0,-32 79 0 0 0,-12 20-2 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 2 0 0,0 0-1 0 0,7 59-63 0 0,-3 43 64 0 0,-8 37 203 0 0,-6 4 7 0 0,-5 36-63 0 0,-4-60-94 0 0,6-24-185 0 0,7-62-625 0 0,6-32-572 0 0,0-1-410 0 0,0 0-1290 0 0,0 0-4861 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101158">8022 6810 11232 0 0,'0'0'256'0'0,"0"0"34"0"0,0 0 20 0 0,-2 0-40 0 0,-26-3 1829 0 0,27 3-1367 0 0,1-2 59 0 0,8-47 2427 0 0,-6 41-3131 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,2 0-86 0 0,-4 2 36 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-36 0 0,3 7 185 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,-2 7-185 0 0,4-16 57 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-3-57 0 0,-3 0-194 0 0,1 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-2-4 194 0 0,-5-36-3540 0 0,6 26-4246 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-100410.518">8580 6574 8496 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 10 0 0,0 0 112 0 0,-1 1 406 0 0,-34 76 4453 0 0,11-35-3370 0 0,12 0-456 0 0,10-17-994 0 0,-8 31 976 0 0,10-52-1274 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-2-1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-81 0 0,5 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,4-7 0 0 0,49-99 0 0 0,-26 20 1046 0 0,-26 53-920 0 0,-6 39-27 0 0,-1 1-10 0 0,0 0 6 0 0,0 0 29 0 0,7 1 281 0 0,-1 12-392 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 1 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,-1 6-13 0 0,-14 102 1090 0 0,2-78-947 0 0,-2-1 1 0 0,-1-1 0 0 0,-2-1 0 0 0,-1 0-1 0 0,-2-2 1 0 0,-9 11-144 0 0,20-34 225 0 0,-2 0 0 0 0,0-2 0 0 0,0 1 0 0 0,-1-2 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1-2 0 0 0,0 0 0 0 0,-14 8-225 0 0,26-18-3 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-2 3 0 0,1-6-150 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,2 0 150 0 0,4-14-1149 0 0,2-3-679 0 0,-1 5-278 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-99222.683">9139 6831 10136 0 0,'2'14'230'0'0,"-2"-11"30"0"0,0-3 19 0 0,0 0 105 0 0,0 0 411 0 0,0 0 182 0 0,9 7 1891 0 0,-5-4-2546 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,2 0-322 0 0,3-2 206 0 0,0 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,3-3-206 0 0,39-72 696 0 0,-47 74-668 0 0,0-1-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,-1-6-28 0 0,3 12 5 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1-5 0 0,-4 6 19 0 0,1 1 1 0 0,-1-1 0 0 0,1 2 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,1 1 0 0 0,0 1-20 0 0,-1 0 77 0 0,1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,1 1 1 0 0,0 1-77 0 0,-2-7 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,33-17-1473 0 0,-23 4 614 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95784.389">9646 6578 4608 0 0,'0'0'353'0'0,"0"0"35"0"0,0 0 1008 0 0,0 0 461 0 0,0 0 95 0 0,0 0-104 0 0,0 0-522 0 0,0 0-228 0 0,0 0-46 0 0,1 2-59 0 0,10 17 2469 0 0,5 32-1092 0 0,-10 40-307 0 0,0 15-686 0 0,-9 8-869 0 0,3-112-577 0 0,0-2-52 0 0,0 0-21 0 0,0 0-198 0 0,0 0-824 0 0,0 0-362 0 0,0-1-1274 0 0,-3-4-4833 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94862.106">9690 6800 10016 0 0,'0'0'462'0'0,"0"0"-12"0"0,0 0-148 0 0,1-4 1464 0 0,45-67 3773 0 0,4 10-3387 0 0,-27 50-1432 0 0,-22 10-464 0 0,6 5 586 0 0,-3 1-782 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 2-60 0 0,3 9 248 0 0,12 69 841 0 0,-1 6-628 0 0,-21-70-366 0 0,4-22-174 0 0,1-1-11 0 0,0 0-178 0 0,0 0-783 0 0,0 0-344 0 0,0 0-69 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93718.359">10181 6520 3224 0 0,'0'12'2345'0'0,"0"32"5493"0"0,-1 2-4114 0 0,-1 50-712 0 0,5 9 343 0 0,-6-86-3334 0 0,1-11-891 0 0,-9 3-7476 0 0,6-8 8097 0 0,3-2-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93135.977">10152 6800 456 0 0,'0'0'1763'0'0,"3"-15"5211"0"0,6-44-1110 0 0,12 41-1851 0 0,23-7-1678 0 0,-37 26-2203 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 1 0 0 0,2 6-132 0 0,19 39 1090 0 0,-23-42-1055 0 0,-1-1 0 0 0,0 1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,-1-1-34 0 0,1 11-14 0 0,1-19-184 0 0,0-1-536 0 0,0 0-236 0 0,0 0-888 0 0,0 0-3561 0 0,0 0-1523 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-90762.018">10576 6831 8288 0 0,'-3'9'5575'0'0,"14"2"-3896"0"0,-10-11-1688 0 0,2 2 148 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-2 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,3-4-139 0 0,22-46 514 0 0,-19 27-481 0 0,-6 23-28 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-4-4 0 0,1 6 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-55-10 0 0 0,52 10-6 0 0,0 0 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 2 1 0 0,0-1 0 0 0,-1 2 6 0 0,0 0 50 0 0,0 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,3 6-51 0 0,-2-7 64 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,3 0-64 0 0,33 0-544 0 0,-22-10-5374 0 0,-4 1-1399 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88936.296">11061 6226 3224 0 0,'-3'18'4649'0'0,"-17"29"2676"0"0,2 38-3229 0 0,3 62-1931 0 0,16-131-1939 0 0,17 122 1016 0 0,12-36-627 0 0,-4-40 597 0 0,-24-60-1196 0 0,-1-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1-16 0 0,24-29 176 0 0,10-57-176 0 0,-13 2 0 0 0,-9-12 0 0 0,-4 17 0 0 0,-7-30 0 0 0,-3 5 43 0 0,0 105-266 0 0,0 1-29 0 0,0 0-4 0 0,0 0-141 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1251 0 0,0 0-4804 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87751.59">11526 6370 2304 0 0,'-4'14'3512'0'0,"4"-14"-3295"0"0,1 31 9139 0 0,8 16-4914 0 0,-7-37-4052 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,-2 4-389 0 0,0 29-162 0 0,2 44 39 0 0,6 34 299 0 0,-4-109 129 0 0,-1-1-2806 0 0,-1-12 1101 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87470.909">11532 6469 7832 0 0,'0'0'602'0'0,"1"1"-134"0"0,8 1 1838 0 0,28 8 3878 0 0,20-10-2721 0 0,10-9-2874 0 0,-38 8-6863 0 0,-22 1-248 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86426.787">11890 6632 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-128 0 0,1 2-606 0 0,8 96 6111 0 0,-9-24-5043 0 0,-3-7-2402 0 0,2-60 17 0 0,1-5-6835 0 0,0-2 4521 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86230.545">12180 6455 4144 0 0,'0'0'191'0'0,"-4"2"22"0"0,2 0 5833 0 0,-6 20 354 0 0,-7 11-4079 0 0,9 10-269 0 0,7-12-1028 0 0,-4-10-798 0 0,0 0 0 0 0,2 0-1 0 0,0 0 1 0 0,1 0-1 0 0,2 20-225 0 0,1 66 0 0 0,-9-39 0 0 0,4-57 13 0 0,1-2-3106 0 0,1-9 1973 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85578.149">12345 6683 3224 0 0,'0'15'553'0'0,"6"8"6334"0"0,-12 65 1088 0 0,2-9-6591 0 0,4-64-1121 0 0,0-2-3991 0 0,0-13-2374 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85386.832">12392 6526 17503 0 0,'0'0'776'0'0,"0"0"160"0"0,0 0-744 0 0,0 0-192 0 0,0 0 0 0 0,0 0 0 0 0,0 0 448 0 0,0 0 48 0 0,0 0 16 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1568 0 0,2 11-304 0 0,-2-11-64 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85026.437">11873 6428 18455 0 0,'0'0'408'0'0,"0"0"80"0"0,0 0 24 0 0,0 0 0 0 0,0 0-408 0 0,0 0-104 0 0,0 0 0 0 0,0 0 0 0 0,0 0 224 0 0,-6 0 16 0 0,6 0 8 0 0,0 0 0 0 0,0 0-992 0 0,0 0-200 0 0,0 0-40 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-83816.66">12676 6533 9584 0 0,'0'0'216'0'0,"-8"5"521"0"0,-44 35 3704 0 0,28-13-975 0 0,20-23-3254 0 0,0-1 1 0 0,0 2-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 4-213 0 0,2-4 22 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,4 4-22 0 0,33 44 54 0 0,-17-36 918 0 0,-20-15-642 0 0,-2-1-115 0 0,7 3 109 0 0,0 10-171 0 0,-7-11-153 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-2 1 0 0 0,0 0-4 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 5 0 0,-4-18-2397 0 0,8 8 122 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-79727.133">12869 6773 4632 0 0,'0'0'209'0'0,"1"-2"-5"0"0,28-61 6992 0 0,-28 63-6393 0 0,-1 0-31 0 0,19-8 2699 0 0,61 9 1055 0 0,-19-4-2917 0 0,-45 15-1448 0 0,-6 9-150 0 0,-11-21-7 0 0,1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-4 0 0,-10-7 202 0 0,9 6-204 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-2 0 1 0 0,-28 18 268 0 0,26-15-199 0 0,1 2-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1 0 0 0,1 1-69 0 0,0-4 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,50-5-132 0 0,-47-2 154 0 0,-1-1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,2-3-22 0 0,39-62-80 0 0,-34 26 64 0 0,-5-1 16 0 0,1 165 0 0 0,-7-72 0 0 0,4 5 0 0 0,9 11 0 0 0,-3-4-2782 0 0,-7-47 64 0 0,-3 1-4789 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76952.167">13785 6841 2304 0 0,'0'0'464'0'0,"-1"1"2357"0"0,-4 6-1769 0 0,5-5 3151 0 0,0-1 4184 0 0,26 15-5739 0 0,-21-15-2588 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 0-1 0 0,3-3-59 0 0,4-7-111 0 0,-6 10 95 0 0,0-2 0 0 0,0 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-2 16 0 0,-2 4-53 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-2-2 54 0 0,3 4-6 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 7 0 0,-4 7 93 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,5 11-93 0 0,-6-18 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,3 0 0 0 0,-3-1-22 0 0,10-6-6424 0 0,-9-2-869 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77950.243">13427 6360 1840 0 0,'0'0'307'0'0,"0"-2"615"0"0,-2-30 3370 0 0,2 32-4103 0 0,0 0-1 0 0,0 0 44 0 0,0 0 22 0 0,0 0 2 0 0,0 0 74 0 0,0 0 316 0 0,0 0 142 0 0,0 1 32 0 0,6 62 3244 0 0,-6 77 861 0 0,0 71-1667 0 0,4-84-1971 0 0,5 64-363 0 0,-8-147-963 0 0,-2-26-3502 0 0,1-18 1678 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77348.9">13421 6509 13504 0 0,'0'0'620'0'0,"0"0"-16"0"0,4-6-364 0 0,16-5 1491 0 0,-16 8-1438 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1-293 0 0,76 5 662 0 0,-39 9-2436 0 0,-18-8-4491 0 0,-13 0 465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76210.45">14301 6578 1840 0 0,'0'0'583'0'0,"-1"1"2720"0"0,-6 1-1116 0 0,-22 24 7260 0 0,25-18-9058 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 9-389 0 0,-3 51 2048 0 0,11 43-1440 0 0,-6-105-566 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,2 2-42 0 0,-4-6 48 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 0-48 0 0,6-6 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,3-9 0 0 0,19-47 0 0 0,-1-11 0 0 0,-24 56 0 0 0,-3 15 0 0 0,-6 1-177 0 0,-8 13-4614 0 0,9-6-2832 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-72325.515">14732 6564 3224 0 0,'0'0'143'0'0,"0"0"-3"0"0,6 0 2973 0 0,-5-1 7737 0 0,-5 4-3072 0 0,3 3-10123 0 0,2 28 3033 0 0,-2-6 1192 0 0,1-27-1368 0 0,0 1 0 0 0,-15 79 715 0 0,6-16-1010 0 0,4-11-308 0 0,21 76-94 0 0,-13-93 185 0 0,-5-31-139 0 0,2-5-580 0 0,0-1-251 0 0,0-1-1544 0 0,2-8-6015 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45518.414">16319 6605 8288 0 0,'0'139'4740'0'0,"0"-122"-3699"0"0,0 14 42 0 0,0 1 0 0 0,1-1 0 0 0,2 0 1 0 0,1 0-1 0 0,6 22-1083 0 0,2-11-70 0 0,-6-27-1026 0 0,-4-14-85 0 0,-2-1-45 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45023.887">16670 6581 1376 0 0,'0'0'299'0'0,"0"0"715"0"0,0 0 313 0 0,0 0 66 0 0,-10-7 1242 0 0,7 6-2367 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,-1 1-268 0 0,-44 91 3206 0 0,45-88-3121 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1-85 0 0,68 38 528 0 0,-72-44-518 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1-9 0 0,-1 2-25 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 25 0 0,-9-14-3267 0 0,9 6-3203 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22924.697">14732 6769 920 0 0,'-4'10'80'0'0,"-5"7"5114"0"0,8-16-3500 0 0,1-1-770 0 0,0 0-336 0 0,0 0-68 0 0,0 0-20 0 0,0 0-51 0 0,0 0-22 0 0,0 0-3 0 0,0 0 25 0 0,0 0 107 0 0,0 0 48 0 0,0 0 11 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,6-22 5642 0 0,26-28-4223 0 0,11 15-1739 0 0,-39 34-286 0 0,3 2 1 0 0,4 10 96 0 0,-7-4-97 0 0,-4-6-115 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 105 0 0,9 2-1084 0 0,13-1-5055 0 0,-19-1 4517 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23746.448">15220 6475 1376 0 0,'0'0'331'0'0,"0"0"853"0"0,0 0 380 0 0,0 0 71 0 0,0 0-79 0 0,0 0-405 0 0,0 0-178 0 0,0 0-39 0 0,0 0-42 0 0,0 0-151 0 0,0 0-65 0 0,0 0-17 0 0,0 0 26 0 0,0 0 124 0 0,0 0 58 0 0,0 0 11 0 0,0 0-43 0 0,0 0-192 0 0,0 0-89 0 0,-14-3 1062 0 0,-26 17 904 0 0,-10 37-429 0 0,6 34-1643 0 0,24-37-267 0 0,4 48 275 0 0,12 20 391 0 0,9-83-660 0 0,-5-25-158 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,3 1-29 0 0,20 26 0 0 0,-18-29-4 0 0,-6-4-118 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-2 122 0 0,22-17-6775 0 0,-19 11 184 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24081.144">15314 6652 456 0 0,'12'-36'1833'0'0,"5"16"8000"0"0,-4 3-4338 0 0,-12 16-4746 0 0,-1 1-12 0 0,8 1 2655 0 0,-4 4-3184 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 5-208 0 0,0-4 187 0 0,1 171 1174 0 0,-8-103-1017 0 0,-6-7-212 0 0,10-60-136 0 0,2-3 10 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1-5 0 0,-8 6-315 0 0,-26 22-6531 0 0,28-26 5010 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28120.561">15440 6056 4608 0 0,'3'-4'886'0'0,"0"-3"-1808"0"0,-2 2 5374 0 0,-1-3 4827 0 0,15 9-6424 0 0,-8 3-2408 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,2 3-447 0 0,10 27 1006 0 0,14 73 508 0 0,-20-24-882 0 0,4 239 416 0 0,-14-51-535 0 0,-11-44 14 0 0,-2 6-74 0 0,0-142-389 0 0,0-25 75 0 0,12-63-128 0 0,-18-2 223 0 0,-103-34-95 0 0,82 27-75 0 0,-6 7 28 0 0,-1-2 1 0 0,1-2-1 0 0,-19-4-92 0 0,-37-13 67 0 0,-146-71-67 0 0,219 81-114 0 0,-1 2 1 0 0,1 1-1 0 0,-1 2 0 0 0,0 1 0 0 0,1 2 1 0 0,-1 1-1 0 0,-14 4 114 0 0,-504 86 796 0 0,80-34-796 0 0,12 1 0 0 0,189-19 0 0 0,-11-9 0 0 0,-189-10 0 0 0,-359-19 0 0 0,534 6 0 0 0,-252-33 0 0 0,-64-19 0 0 0,139 27-457 0 0,-193-4 202 0 0,234-3-1 0 0,-133 19 256 0 0,284 4 172 0 0,-64 0 164 0 0,26-15-196 0 0,57 16 180 0 0,78 1-722 0 0,-27 1 8 0 0,-172-5 478 0 0,129-5 308 0 0,23-9-72 0 0,-224-16-1032 0 0,293 19 852 0 0,-64-10 432 0 0,-122-6-572 0 0,153 13 0 0 0,-35 20 0 0 0,-50-8 0 0 0,72-4 0 0 0,-78 33 0 0 0,20 14 0 0 0,111-49 0 0 0,13 18 0 0 0,50 0 0 0 0,84-6-20 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1-1 20 0 0,-26-46-115 0 0,-8-66 687 0 0,-13-89-572 0 0,-16-91 0 0 0,42 48 0 0 0,-4 80 0 0 0,-2-19 0 0 0,19 73-796 0 0,9 24 1592 0 0,12 20-796 0 0,25-26 0 0 0,-31 85 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,7-7 0 0 0,65-39 0 0 0,73-25 0 0 0,-129 70 0 0 0,0 1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1 2 0 0 0,0 1 0 0 0,8 1 0 0 0,-32 1 0 0 0,111 0 0 0 0,0-5 0 0 0,25-9 0 0 0,21-13-712 0 0,78-21 1413 0 0,-142 32-697 0 0,0 4-1 0 0,1 6 1 0 0,56 5-4 0 0,254 19 0 0 0,-105-2 0 0 0,-239-12-72 0 0,1 2 1 0 0,-1 4-1 0 0,43 14 72 0 0,71 7-105 0 0,-58-20 425 0 0,53 12-320 0 0,-44 2 0 0 0,56 16 0 0 0,68 2 0 0 0,48 22 0 0 0,-158-27 0 0 0,46-1 0 0 0,39 1-796 0 0,-78-3 1592 0 0,4-12-831 0 0,7-27-250 0 0,-29 4 605 0 0,51 11-320 0 0,-84-8 0 0 0,76-20 0 0 0,-34-2 0 0 0,119 14 0 0 0,-168 5 0 0 0,0-5 0 0 0,62-13 0 0 0,45-4 0 0 0,118 6 0 0 0,-35-7 0 0 0,-127 5 0 0 0,197 1 0 0 0,-89 15 0 0 0,91-20 0 0 0,74-12 0 0 0,-289 27 0 0 0,15-1 0 0 0,227 3 0 0 0,-124 15 0 0 0,-50-3 0 0 0,104-21 0 0 0,9 21 0 0 0,-186 0 0 0 0,6-11 0 0 0,-11-3 0 0 0,-15 7 0 0 0,9 4 0 0 0,27-11 0 0 0,51 14 0 0 0,-64 9 0 0 0,-71-19 0 0 0,146-4 0 0 0,-57 24 0 0 0,-75-7 0 0 0,43-2 0 0 0,-37 2 0 0 0,131 14 0 0 0,-53-8 0 0 0,-61-2 0 0 0,58 4 0 0 0,-68-16 0 0 0,30-5 0 0 0,-33 26-4336 0 0,-33-5-1782 0 0,-38-14-3483 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29020.976">15120 5809 1376 0 0,'0'0'591'0'0,"0"0"1942"0"0,0 0 851 0 0,0 0 174 0 0,0 0-327 0 0,-11 8 6223 0 0,14-5-9289 0 0,1 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,1-1-165 0 0,0 2 87 0 0,97 18 1139 0 0,-6 19-943 0 0,-53-21-166 0 0,5-27 11 0 0,-18 7-64 0 0,-15 20-64 0 0,-9 16 13 0 0,-6 5 198 0 0,-2 60 157 0 0,3-7-616 0 0,0-31-3854 0 0,1-36-5107 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.15371E6">7867 7688 1376 0 0,'0'0'65'0'0,"0"0"189"0"0,0 0 767 0 0,0 0 335 0 0,0 0 69 0 0,0 0-94 0 0,0 8 1469 0 0,-2 72 3116 0 0,4-14-3609 0 0,-14 102-383 0 0,11-29-438 0 0,1-60-917 0 0,-2-1 598 0 0,1 106-205 0 0,-6 4-322 0 0,11 98-40 0 0,-1-188-336 0 0,-3 21 8 0 0,9 119 323 0 0,5-5 583 0 0,-3-60-1855 0 0,-6 84 952 0 0,0-53-94 0 0,-4-145-117 0 0,4-3-2277 0 0,-2-78-5567 0 0,-3 8 286 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.15425E6">7393 9856 5528 0 0,'0'0'422'0'0,"0"0"-88"0"0,0 0 656 0 0,0 17 2881 0 0,10 38-2527 0 0,7 40 2164 0 0,20-9-466 0 0,69 129 109 0 0,-71-150-2761 0 0,-26-45-296 0 0,1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,1-1-1 0 0,1 0 1 0 0,0-1-1 0 0,12 10-94 0 0,56 24 544 0 0,-78-47-475 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,3-2-69 0 0,28-40 176 0 0,81-237 1624 0 0,-34 86-1872 0 0,-40 74-576 0 0,-26 68-2737 0 0,-10 39 1634 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16329E6">3054 10697 13128 0 0,'0'-16'633'0'0,"0"15"-277"0"0,0 8 83 0 0,13 222 3164 0 0,17-12-1187 0 0,-7-2-1552 0 0,-25-125-897 0 0,-13-32-3046 0 0,12-49 1239 0 0,-4-5-71 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16383E6">2980 10685 7056 0 0,'-2'-5'116'0'0,"1"0"0"0"0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,2-3-117 0 0,0-6 1073 0 0,-2 12-878 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,3-1-195 0 0,-1 1 85 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,2 2-85 0 0,42 48 670 0 0,-22-21 265 0 0,20 39 175 0 0,-42-59-1010 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,-3 7-100 0 0,2-10 186 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0-1-1 0 0,0 1 1 0 0,-3 0-186 0 0,7-4 12 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1-1-11 0 0,-39 6 164 0 0,43-5-225 0 0,16 13-71 0 0,34 31 57 0 0,-29-19 68 0 0,52 78 132 0 0,0 46-125 0 0,-37-69-5360 0 0,-31-61 3443 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16516E6">3718 11368 6912 0 0,'0'0'528'0'0,"0"0"-219"0"0,0 0 347 0 0,0 2 192 0 0,12 9 3088 0 0,43-14-2645 0 0,19-34-467 0 0,-27 7 415 0 0,-44 27-1110 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1-128 0 0,-26-40 870 0 0,22 42-830 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 2 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,-1 3-41 0 0,1 0 30 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 2-30 0 0,18 104 84 0 0,-16-107-98 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 0 0 0 0,1 0 14 0 0,7 0-1085 0 0,-1-1-349 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16566E6">4230 10979 920 0 0,'1'2'67'0'0,"5"16"218"0"0,-6-16 1126 0 0,0-2 485 0 0,0 0 95 0 0,0 0-144 0 0,0 0-698 0 0,0 0-306 0 0,3 14 5156 0 0,4 70-3006 0 0,-1 145-2907 0 0,15-68 348 0 0,-8-98-1540 0 0,-9-56-81 0 0,-1-4-3107 0 0,-3-2-1448 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16596E6">4230 11064 5984 0 0,'0'0'464'0'0,"0"0"-82"0"0,10 12 5502 0 0,34-2-3006 0 0,29-10-1919 0 0,-23-4-2545 0 0,-39 4-3811 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29091E6">7353 10942 1840 0 0,'0'0'83'0'0,"0"7"10"0"0,-3-2 194 0 0,-4 6 6325 0 0,0 3-4677 0 0,4-8-1065 0 0,-3 26 3503 0 0,8 49-1185 0 0,2 49-2006 0 0,0-58-326 0 0,4-42-586 0 0,20 43 628 0 0,-26-71-870 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2-1-28 0 0,4-5 21 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,3-9-21 0 0,21-42 0 0 0,-9-13 1099 0 0,1-24-934 0 0,-15 6-165 0 0,-3 62 0 0 0,-6-38 0 0 0,2 22-283 0 0,2 27-8605 0 0,-1 19 2172 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29171E6">7871 10880 8288 0 0,'-9'70'3321'0'0,"8"21"1356"0"0,2-6-2700 0 0,1-30-1241 0 0,1 132 440 0 0,-3-171-966 0 0,7 43-294 0 0,-6-58-163 0 0,-1-1-857 0 0,0-2-3536 0 0,0-6-1518 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.2919E6">7855 10979 8288 0 0,'0'0'638'0'0,"7"-3"2018"0"0,17-3 1429 0 0,15 17-2828 0 0,-24-6-864 0 0,29 23-411 0 0,-38-23-355 0 0,14 19-3587 0 0,-12-12 2594 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29212E6">8218 11195 3680 0 0,'0'0'284'0'0,"3"8"797"0"0,-2-4 4784 0 0,1 30-1677 0 0,0 5-3145 0 0,-3 37-251 0 0,5-14-1216 0 0,-4-46-1299 0 0,0-6-3631 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29254E6">8483 10979 920 0 0,'-3'-14'343'0'0,"3"11"1102"0"0,0 3 482 0 0,0 0 96 0 0,0 0-124 0 0,0 0-614 0 0,0 0-269 0 0,0 0-50 0 0,0 0-57 0 0,0 0-212 0 0,0 0-90 0 0,0 2-20 0 0,-1 36 1508 0 0,-5 36-993 0 0,-4 83 402 0 0,6-56-494 0 0,11 56-140 0 0,3-75-1121 0 0,-10-81-772 0 0,0-1-333 0 0,0 0-68 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29304E6">8751 11290 456 0 0,'-5'20'0'0'0,"5"-19"651"0"0,-2 0 4741 0 0,-1 2 3820 0 0,3 1-9813 0 0,2 172 4824 0 0,2-124-4491 0 0,-4-47-754 0 0,0-4-326 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29369E6">9051 11263 10136 0 0,'0'0'464'0'0,"-2"0"-10"0"0,-4 0-222 0 0,-11 14 3123 0 0,15-13-3266 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1-89 0 0,22 51-256 0 0,-14-29 538 0 0,33 28 412 0 0,-12 3-275 0 0,-26-21-94 0 0,-18 6 1227 0 0,3-25-785 0 0,-13 5 957 0 0,13-18-1575 0 0,-9-2-133 0 0,-4-17-2201 0 0,21 11-250 0 0,2 4-4568 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29508E6">9302 11512 10136 0 0,'6'17'230'0'0,"-5"-13"30"0"0,-1-4 19 0 0,2-8 478 0 0,5-33 763 0 0,-6 39-1014 0 0,0-1-2 0 0,7-26 334 0 0,-7 23-761 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,2 0-78 0 0,-4 4 167 0 0,26-16 1024 0 0,-25 16-1129 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0-61 0 0,25 30 1857 0 0,-25-31-1723 0 0,-1-1-46 0 0,0 0-22 0 0,0 0-2 0 0,0 0 2 0 0,0 0 4 0 0,-21 0 2 0 0,17 0-87 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-2 1 16 0 0,-22 15-85 0 0,25-18 77 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 2 8 0 0,10 30-54 0 0,-10-32 57 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-3 0 0,44 5 163 0 0,-40-9-205 0 0,-1 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,-1-4 43 0 0,7-69-556 0 0,-7 79 622 0 0,0 1 34 0 0,0 0 10 0 0,-1 3-16 0 0,0 11 66 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,3 10-160 0 0,1 26 76 0 0,14 26 0 0 0,-11-36-1057 0 0,-8-38-90 0 0,5 7-37 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29562E6">9847 11082 456 0 0,'0'-22'204'0'0,"0"8"5674"0"0,-3 14 1245 0 0,-5 26-4666 0 0,-1 52-110 0 0,9 97-830 0 0,-4 70-628 0 0,13-184-907 0 0,-8-54 2 0 0,-1-7-2564 0 0,0 0 1298 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29586E6">9813 11229 8752 0 0,'5'8'936'0'0,"11"-23"1798"0"0,38 15 2614 0 0,31 4-4455 0 0,-48 12-4124 0 0,-30-12 2047 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29642E6">10205 11581 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,2 1-40 0 0,36-7 2129 0 0,-16-1-968 0 0,-19 6-1318 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1-82 0 0,6-10 268 0 0,-5 10-243 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-3-4-25 0 0,5 6 20 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-20 0 0,-5 10 226 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 4-225 0 0,0-13 37 0 0,1 2 31 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,1 0-67 0 0,-1-2 33 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,3 0-33 0 0,40 8-313 0 0,-11-15-1742 0 0,-27 5 191 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29693E6">10646 11363 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,-10 3 2224 0 0,1 9-1481 0 0,8-10-561 0 0,1-2 0 0 0,-1 1 0 0 0,-29 38 1128 0 0,28-36-1631 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-9 0 0,0 18 74 0 0,-1-17-14 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1-59 0 0,55 33 164 0 0,-55-36-163 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1-1 0 0 0,23-40 0 0 0,0-26 0 0 0,-21 39 0 0 0,-5-43 0 0 0,0 65 0 0 0,0 10-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 2 0 0,-1 2-86 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 5 86 0 0,10 44-6882 0 0,-5-42 1085 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.2974E6">11181 11219 3224 0 0,'3'17'240'0'0,"-16"13"5162"0"0,-7 23 1702 0 0,1 32-4883 0 0,10-45-1389 0 0,6 22 96 0 0,-3-22-476 0 0,6 22 178 0 0,-4 6-648 0 0,1-57 50 0 0,0-5-3037 0 0,3-6 1818 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29771E6">11130 11444 10136 0 0,'2'9'1085'0'0,"43"-45"1390"0"0,-42 33-2239 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,3-1-236 0 0,28-14 608 0 0,-10 30 520 0 0,-9 4-434 0 0,-14-17-580 0 0,15 13-10 0 0,-16-11-96 0 0,12 22-8 0 0,-12-20-92 0 0,-1-3-390 0 0,0 7-1954 0 0,3-1-3569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.30092E6">11702 11093 2304 0 0,'0'0'101'0'0,"1"-2"1"0"0,1-4-3003 0 0,-1 1 4359 0 0,-6-3 14711 0 0,-3 14-13468 0 0,5-3-2385 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 4-316 0 0,-1 99 1202 0 0,2-97-965 0 0,3 41-228 0 0,1 0 0 0 0,2 0 1 0 0,2-1-1 0 0,2 0 0 0 0,8 20-9 0 0,-10-39 0 0 0,-2-22 0 0 0,17 1-1058 0 0,11-29-4850 0 0,-24 9 3794 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.30128E6">12030 11003 1376 0 0,'0'0'65'0'0,"0"0"454"0"0,0 0 1882 0 0,5 0 5023 0 0,3 0-3511 0 0,-6 2-3615 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 3-297 0 0,26 51 2384 0 0,-5-9-1738 0 0,-14-33-400 0 0,-1 1 0 0 0,0 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-2 1-1 0 0,0 1-245 0 0,13 118 608 0 0,-14 68 104 0 0,-11-64-61 0 0,0-95-3304 0 0,-3-2-3362 0 0,7-32-807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.30531E6">12605 12454 3224 0 0,'0'0'143'0'0,"0"0"327"0"0,0 0 1271 0 0,0 0 550 0 0,0 0 114 0 0,0-3 988 0 0,1-12-1052 0 0,0-52 2752 0 0,7-3-2899 0 0,9-98-927 0 0,5-50-315 0 0,-9 76 489 0 0,-4-103-1441 0 0,-7 153 170 0 0,1 8 86 0 0,3 0-1 0 0,8-37-255 0 0,4-24 592 0 0,-5 22-253 0 0,-10 24 96 0 0,5 48-99 0 0,4-14-403 0 0,-1 37 67 0 0,-5 11 13 0 0,-3 0 79 0 0,-6 7 139 0 0,-6-10-231 0 0,8 18 5 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-5 0 0,-113 3 320 0 0,59 1-256 0 0,-57 5 61 0 0,-220 12 207 0 0,40 3-320 0 0,13 14 52 0 0,25 17-64 0 0,-256 57 128 0 0,327-88-117 0 0,73-14 98 0 0,-1-5 0 0 0,-32-7-109 0 0,19 0-2 0 0,-69-5 367 0 0,-82 2-133 0 0,-23-7-541 0 0,95-2 706 0 0,-12 0-710 0 0,51 4 634 0 0,-171 0-321 0 0,184-3-16 0 0,-35 1-155 0 0,-34-11 182 0 0,-102-10 65 0 0,188 22-88 0 0,-23 4 12 0 0,-45 4 64 0 0,17 0-64 0 0,-53-8 0 0 0,-289-30 64 0 0,361 27-64 0 0,-258-10 0 0 0,373 25 0 0 0,-139-11 0 0 0,66-4 0 0 0,-37-6 0 0 0,-23-2 0 0 0,-96 16 0 0 0,188 8 0 0 0,-48-15 0 0 0,28-5 0 0 0,79 14 0 0 0,0 1 0 0 0,-1 2 0 0 0,-32 4 0 0 0,-10 0 0 0 0,-221 7-11 0 0,111-35 22 0 0,-82-18-11 0 0,-44 39-64 0 0,239-6 128 0 0,50 9-64 0 0,0 0 0 0 0,1-2 0 0 0,-1-1 0 0 0,-21-7 0 0 0,29 6 0 0 0,5 0 0 0 0,0 2 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,-4 1 0 0 0,4 1 0 0 0,7-3 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 2 0 0 0,-14 72-244 0 0,40 143 168 0 0,-3-63 299 0 0,30 231-446 0 0,-6-30 520 0 0,2-178-530 0 0,-22-88 233 0 0,17 53 0 0 0,12-7 0 0 0,-43-120 0 0 0,53 78 0 0 0,-47-83 4 0 0,0-1 0 0 0,1-1 0 0 0,0-1 0 0 0,1-1-1 0 0,0-1 1 0 0,0 0 0 0 0,0-2 0 0 0,1 0 0 0 0,5 0-4 0 0,26 11 140 0 0,77 16-242 0 0,-13-11 207 0 0,86 4-105 0 0,-76-11-23 0 0,70 3-132 0 0,6-8 155 0 0,446 20 0 0 0,-127-7 0 0 0,-55 0 0 0 0,76-19 53 0 0,-62-41-42 0 0,-142-15-11 0 0,42 10 0 0 0,-164 25 12 0 0,-10 11 112 0 0,87-8-204 0 0,46 20 149 0 0,13-8-58 0 0,-4-10-107 0 0,9 1 96 0 0,-156 3 96 0 0,101 12-192 0 0,-211 14 96 0 0,41-2 0 0 0,31 0 144 0 0,-48-19-240 0 0,3-2 192 0 0,-80 6-96 0 0,0-1 0 0 0,1-3 0 0 0,-1-1 0 0 0,30-8 0 0 0,25-3-96 0 0,32 7 96 0 0,98 3 0 0 0,-108-9 80 0 0,-32 2-160 0 0,90-5 80 0 0,-71 19 11 0 0,80-17 42 0 0,-85-3-141 0 0,-15-8 94 0 0,1 4 0 0 0,55-5-6 0 0,-37 13 60 0 0,-1 12-60 0 0,38 36 0 0 0,-48-18 0 0 0,-77-15 0 0 0,18 13 0 0 0,-23-8 59 0 0,-5-6-111 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 52 0 0,-4 4-1004 0 0,4-4-3898 0 0,1-1 2712 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.31424E6">15845 6350 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0-11 1147 0 0,0 7-3619 0 0,1-4 9257 0 0,0 5 2091 0 0,-1 8-7632 0 0,12 193 1589 0 0,-16-103-2526 0 0,-4-7-90 0 0,3-5-182 0 0,14 6-118 0 0,-2-42-2244 0 0,-6-46 1548 0 0,-1-1-185 0 0,0 0-84 0 0,0 0-21 0 0,2 3-3895 0 0,-2-3 2635 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.31517E6">15868 6780 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0 0-22 0 0,0-15 2511 0 0,14-70 5565 0 0,-4 59-6834 0 0,10 1-281 0 0,-5 9-550 0 0,-14 15-517 0 0,-1 1-6 0 0,2 0 3 0 0,20 7 472 0 0,-2 13 14 0 0,10 53 396 0 0,7 63-438 0 0,-27-83-450 0 0,-10-26-1627 0 0,0-12-6318 0 0,0-5 1470 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.32608E6">13264 11283 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,3-9 1867 0 0,-2 8-1852 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1-240 0 0,-4-4 274 0 0,-1 1-1 0 0,1 0 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-2 2-273 0 0,-9 5 0 0 0,11-1 0 0 0,-25 34 0 0 0,23-25 150 0 0,0 1 1 0 0,1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 1 0 0,1-1-1 0 0,1 1 0 0 0,0 5-150 0 0,-1-2 104 0 0,-14 207-482 0 0,9-119 567 0 0,8-13-136 0 0,-1-96-229 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0 176 0 0,7-3-1901 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.32649E6">12960 11591 5984 0 0,'0'0'464'0'0,"0"0"-100"0"0,0 0 717 0 0,0 0 346 0 0,0 0 69 0 0,0 0-71 0 0,0 0-330 0 0,0 0-146 0 0,6 13 1624 0 0,-3-9-2296 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,4-1-277 0 0,14 8 296 0 0,18 1 73 0 0,-33-7-712 0 0,19 11-175 0 0,-12 4-5552 0 0,-8-5-166 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.3268E6">13237 11939 6624 0 0,'0'0'298'0'0,"0"0"-3"0"0,0-2-188 0 0,24-54 3721 0 0,-17 43-2931 0 0,-6 11-725 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-173 0 0,-1 2 83 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 1-83 0 0,3 4 241 0 0,0 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 7-241 0 0,-5 51 1376 0 0,-2-47-782 0 0,6-18-550 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1-44 0 0,-2-2-23 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1-1 1 0 0,2 0-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-2 24 0 0,-12-41-1750 0 0,9 20 132 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.32804E6">13625 11915 4608 0 0,'0'0'101'0'0,"-3"-4"150"0"0,2-1-50 0 0,1 4 308 0 0,0 1 135 0 0,0-2 27 0 0,-2-36 1126 0 0,2 37-1534 0 0,0 1-330 0 0,0 0-71 0 0,0 0 38 0 0,0 0 152 0 0,0 0 68 0 0,0 0 9 0 0,0 1-17 0 0,2 1-16 0 0,-2-1 280 0 0,0-1 113 0 0,0 0 21 0 0,0 0-68 0 0,0 0-262 0 0,0 0-9 0 0,-1 6 712 0 0,0-6-575 0 0,1 0 4 0 0,0 0 26 0 0,0 0 113 0 0,0 0 49 0 0,0 0 11 0 0,0 0-57 0 0,0 0-239 0 0,0 0-102 0 0,0 0-17 0 0,0 0 18 0 0,0 0 99 0 0,0 0 47 0 0,0 0 11 0 0,0 0 0 0 0,0 0 1 0 0,0 0 0 0 0,2 7 268 0 0,9 26 656 0 0,-8 17 132 0 0,9 17 242 0 0,-7-33 28 0 0,-5 34-1582 0 0,-4-23-16 0 0,4-35 0 0 0,1-86 1117 0 0,-2 36-1650 0 0,5-51 37 0 0,-7-2 27 0 0,13 63 834 0 0,-7 23-365 0 0,22-7-1090 0 0,-24 14 1590 0 0,0 1-59 0 0,48 46-276 0 0,-19-2-165 0 0,-10-1 0 0 0,1 10 0 0 0,-12-10 0 0 0,-8-26 72 0 0,5 4-112 0 0,-6-20-81 0 0,0-2-30 0 0,12 6-660 0 0,9-4-2647 0 0,-17-10 2023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33006E6">14079 11874 6448 0 0,'27'-50'4184'0'0,"-26"49"-3679"0"0,-1 1 6 0 0,0 0 1 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 0 0 0,0 0-24 0 0,0 0-100 0 0,0 0-42 0 0,0 0-8 0 0,0 0-20 0 0,0 0-74 0 0,0 0-39 0 0,0 0-5 0 0,0 0 26 0 0,0 0 104 0 0,0 0 44 0 0,0 0 8 0 0,0 0-31 0 0,13 3 130 0 0,-13-2-345 0 0,-18 8 299 0 0,-2 5-94 0 0,-29 30 589 0 0,15-9 20 0 0,21 11-70 0 0,13-44-729 0 0,0 0-40 0 0,-1 14 5 0 0,1-13-81 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,2 0-27 0 0,0 1 24 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,3 0-23 0 0,25 6-16 0 0,2-12-321 0 0,0-17-1384 0 0,-17 18-2498 0 0,-7-1-2527 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33103E6">14417 11587 456 0 0,'0'0'1877'0'0,"0"0"225"0"0,0 0 96 0 0,0 0-174 0 0,0 0-800 0 0,0 0-352 0 0,0 2-68 0 0,-3 81 5406 0 0,0-9-3788 0 0,-4 7-533 0 0,0 109-938 0 0,8-93-994 0 0,-1-94-228 0 0,2 9 239 0 0,-1-4-2836 0 0,-1-14 836 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33125E6">14367 11725 10592 0 0,'0'0'818'0'0,"0"0"-382"0"0,0 0 375 0 0,2 0 224 0 0,46 12 3870 0 0,-11 5-4655 0 0,-15-10-2639 0 0,-21-6 1115 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33171E6">14651 11925 920 0 0,'0'-6'1780'0'0,"-7"-31"5181"0"0,7 36-6117 0 0,0 1-63 0 0,3-5 1525 0 0,-1 2 782 0 0,6 22-961 0 0,-15 41 414 0 0,-1-12-2418 0 0,14-6-123 0 0,7 31-266 0 0,-13-71-1124 0 0,0-2-490 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33205E6">14875 11956 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,-6-14-276 0 0,6 10-201 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0-59 0 0,-1 1 59 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-61 0 0,12 48 1489 0 0,-13-40-1068 0 0,1 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,-1 1-420 0 0,2-11 47 0 0,-17 57 2134 0 0,-23 17-2086 0 0,40-74-50 0 0,-1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-2-46 0 0,-33-49 76 0 0,18 3-2636 0 0,11 14-3921 0 0,2 10-600 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34044E6">15193 11735 2760 0 0,'2'6'3463'0'0,"-1"-1"5440"0"0,-9 22-3399 0 0,8 21-2728 0 0,-2 12-1732 0 0,-6 24 73 0 0,10 41-1117 0 0,1-98-2100 0 0,-3-29 527 0 0,3-4-370 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34087E6">15183 11936 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0 0 240 0 0,0-8 1066 0 0,13-32 2918 0 0,30 3-1475 0 0,-28 29-2427 0 0,21-2-98 0 0,-28 12-954 0 0,40 19 0 0 0,13 47 242 0 0,-27 32 636 0 0,-25-62-878 0 0,-6-21 0 0 0,-6 7-49 0 0,3-23-207 0 0,0-1-87 0 0,0 0-917 0 0,0 0-3813 0 0,0 0-1633 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34281E6">15771 11448 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,0 17 1877 0 0,7 82 4244 0 0,-5-24-3972 0 0,-7 45-624 0 0,1-24-1860 0 0,3 87 1890 0 0,2-5-1730 0 0,2-164-88 0 0,0 2-289 0 0,-2 2-5727 0 0,-4-34 687 0 0,0 1 3586 0 0,6 1-135 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34372E6">15781 11495 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,3-7-177 0 0,-3 5 136 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1-247 0 0,10-6 1678 0 0,39-8 1057 0 0,21 26-286 0 0,-56-7-2099 0 0,-4-1-94 0 0,0 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,3 7-256 0 0,12 29 768 0 0,7 36 88 0 0,-25-15-68 0 0,-10-16 336 0 0,-16-12-1124 0 0,15-32 144 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,-4 1-143 0 0,-37 16 238 0 0,45-19-196 0 0,-1-1-31 0 0,0 2-27 0 0,56-29-776 0 0,13 17-152 0 0,-3 28-54 0 0,-17 17 92 0 0,-12 13 866 0 0,-25-27 40 0 0,-5-16 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 3 0 0 0,-23 33 1352 0 0,-11 0-736 0 0,23-33-497 0 0,-1 0-1 0 0,1-2 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1-2-1 0 0,0 0 1 0 0,-1 0-1 0 0,0-2 1 0 0,0 0 0 0 0,0-1-1 0 0,-5-1-118 0 0,-56 7 387 0 0,26 10-334 0 0,25-16-53 0 0,-5-18-801 0 0,21 9-282 0 0,2 1-2237 0 0,2 1-3262 0 0,-1-1-1015 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34474E6">16523 11465 14800 0 0,'0'0'332'0'0,"0"0"50"0"0,0 0 25 0 0,0 0-47 0 0,0 0-106 0 0,0 0 417 0 0,0 2 206 0 0,-8 54 3904 0 0,6-25-4120 0 0,-15 139 1824 0 0,-2-30-880 0 0,6-34-165 0 0,-11 135-832 0 0,23-234-672 0 0,1-6-273 0 0,0-1-138 0 0,0 3-1216 0 0,-1 5 3621 0 0,0-3-4753 0 0,1 0-9564 0 0,0-5 10339 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34497E6">16531 11519 920 0 0,'0'-6'1157'0'0,"1"3"5384"0"0,16-13-1079 0 0,28 8 55 0 0,21 14-2419 0 0,-2 11-1830 0 0,-10 14 320 0 0,16 44-1572 0 0,-17 13 2016 0 0,-48-75-1886 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,-1 8-146 0 0,1-2 8 0 0,-1 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-2-2 0 0 0,0 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-3 2-8 0 0,10-10 173 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,-3 0-174 0 0,-111-3-286 0 0,94-4-191 0 0,20 5 329 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-5-5 148 0 0,5 3-710 0 0,4 7-8073 0 0,3 0 434 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34598E6">17182 12104 7368 0 0,'0'0'333'0'0,"0"0"0"0"0,-8 4 14776 0 0,6-4-14374 0 0,2-2-710 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,1 0-25 0 0,-3 2 94 0 0,0 0 9 0 0,0 0 29 0 0,0 0 17 0 0,0 0 3 0 0,0 0 11 0 0,0 0 44 0 0,0 0 17 0 0,0 0 6 0 0,0 0 4 0 0,0 0 4 0 0,0 0 2 0 0,0 0 0 0 0,0 0-16 0 0,0 0-66 0 0,0 0-29 0 0,0 0-8 0 0,0 0-9 0 0,0 0-33 0 0,-1 0-25 0 0,-18 29-43 0 0,13-9 74 0 0,5-18-19 0 0,1-2 6 0 0,1-2-18 0 0,8-16-135 0 0,5 10 5 0 0,7 14-588 0 0,-16 2 664 0 0,2 17 16 0 0,-7-24 62 0 0,-4 8 297 0 0,-7-1-725 0 0,10-8 151 0 0,-8 8-801 0 0,1-8-2062 0 0,8 0 1532 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34684E6">17509 11649 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-3 420 0 0,0 3 3077 0 0,0 1 3963 0 0,-6 140-3072 0 0,-4-26-2600 0 0,-7 65-1021 0 0,7-68-304 0 0,4 24-619 0 0,6-135-213 0 0,0-1-69 0 0,0 0-12 0 0,0 0-139 0 0,0-56-6135 0 0,0 33 4451 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34718E6">17483 11689 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,1-1 21 0 0,2-2-256 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,2 0-170 0 0,4 4 318 0 0,-1 0 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 2 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1-318 0 0,18 16-106 0 0,-22-21 167 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 3-62 0 0,2 17 844 0 0,-3-17-830 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,-2 3-14 0 0,1-2 119 0 0,1-1-1 0 0,-1 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-2 1 0 0,0 1-1 0 0,-1-1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,0-1-1 0 0,-4 2-118 0 0,-7 5 128 0 0,17-8-128 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,-12-22-1234 0 0,12 3-3424 0 0,5 5-3433 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34835E6">17934 11397 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-270 0 0,1 1 131 0 0,11 73 4572 0 0,-15-13-1957 0 0,3 5-1459 0 0,3 29-1321 0 0,-6 20-232 0 0,-3 73 0 0 0,-5-82 962 0 0,-11 13-720 0 0,22-118-750 0 0,0-1-89 0 0,0 0-360 0 0,0 0-163 0 0,-4-11-5760 0 0,0 1 563 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34856E6">17931 11908 1376 0 0,'0'0'65'0'0,"0"-2"389"0"0,24-33 11411 0 0,9-15-8036 0 0,3 19-1988 0 0,-34 30-1803 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-38 0 0,6 5 156 0 0,30 77 888 0 0,-32-75-884 0 0,1 1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 6-159 0 0,-8 89 1127 0 0,4-98-1133 0 0,1-8-6257 0 0,0-1-578 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34932E6">18442 11713 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 2 21 0 0,-7 45 177 0 0,-9 35 3194 0 0,6 30-1553 0 0,-4 93-172 0 0,-1-91-257 0 0,9-100-2469 0 0,4-13-3087 0 0,2 0-3929 0 0,0-1 1033 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34952E6">18416 11713 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,13-6-181 0 0,-10 4-54 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 2 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 2 1 0 0,1-1-1 0 0,-1 0 0 0 0,3 2-301 0 0,0 0 145 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 1 0 0 0,0 4-144 0 0,6 63 1883 0 0,-23 16-1742 0 0,12-88-123 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,-3 0-18 0 0,-46 3 1171 0 0,-2 14-2729 0 0,51-18 1668 0 0,-16-3-935 0 0,1-8-3444 0 0,12 5 2477 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.3524E6">14718 11567 3224 0 0,'0'-1'240'0'0,"0"-1"165"0"0,0 1 1443 0 0,0 1 616 0 0,0 0 116 0 0,0-1 259 0 0,0-3-1698 0 0,1 2 2411 0 0,11-14-2439 0 0,-11 10-1053 0 0,-1-5 606 0 0,0 7-4232 0 0,0 4 2520 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.47889E6">5066 11499 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,3-8 314 0 0,17-68 850 0 0,-17 63-996 0 0,1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-1 0 1 0 0,2 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,2 1 1 0 0,7-8-478 0 0,-15 16 40 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-40 0 0,23 53 1331 0 0,-23-52-1287 0 0,2 11 148 0 0,-1 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,-1 4-192 0 0,5-15 21 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-22 0 0,-2-2-60 0 0,0 1-1 0 0,0-2 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-7 60 0 0,-6-53-3591 0 0,8 43 1933 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48055E6">6444 11389 4144 0 0,'0'0'319'0'0,"-9"2"1818"0"0,8-1 2461 0 0,1 0 4419 0 0,6 0-8694 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0-323 0 0,92-55 185 0 0,-67 20-185 0 0,-28 36 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-29-38 0 0 0,28 38 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-4 1 0 0 0,-36 17 0 0 0,35-11 47 0 0,1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 8-47 0 0,1-12 52 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,3 4-52 0 0,-4-6 15 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0-15 0 0,44-6-958 0 0,-33 0-1726 0 0,-2-1-3307 0 0,-5 0-1687 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48192E6">6928 11115 10304 0 0,'0'-4'934'0'0,"0"-10"-627"0"0,0 12 320 0 0,0-3 712 0 0,-1 3 3325 0 0,0 3-4568 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 2-95 0 0,-2 5 224 0 0,1 32 664 0 0,-6 118 1598 0 0,11-75-1828 0 0,-4-41-734 0 0,-2-35-364 0 0,1 8-1982 0 0,-2-11-5617 0 0,2-5 5673 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48237E6">6844 11215 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,1-2-294 0 0,1-2 74 0 0,-1 3 886 0 0,12-9 3459 0 0,-9 8-4230 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-348 0 0,31 4 963 0 0,-17-6-540 0 0,-14 0-358 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1 1-64 0 0,48 64 377 0 0,-49-57-1065 0 0,-4 2-3411 0 0,-1-9 774 0 0,1-2-4194 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48542E6">4739 11256 456 0 0,'0'-16'1413'0'0,"0"15"159"0"0,0-1 76 0 0,0-43 2855 0 0,0 44-3991 0 0,0 1 0 0 0,0 0-24 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0 47 0 0,0 0 207 0 0,0 0 89 0 0,0 0 21 0 0,0 0-24 0 0,-10 5 931 0 0,8-3-1418 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1-182 0 0,5 90 3864 0 0,1 21-3175 0 0,-11-60 34 0 0,4 17-176 0 0,1-69-729 0 0,-4 6 3 0 0,2-6-7687 0 0,1-2-336 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48563E6">4732 11351 11976 0 0,'0'-4'180'0'0,"1"-1"0"0"0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,1-2-180 0 0,6-4 1628 0 0,-6 5-1094 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,4-1-535 0 0,-6 1 86 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,2 3-86 0 0,20 35 302 0 0,16 38 108 0 0,-28-49-1847 0 0,-8-23-150 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.5473E6">5467 11225 456 0 0,'-2'29'10790'0'0,"-5"-3"-6142"0"0,-14 83 1001 0 0,19-102-5360 0 0,-1 2-52 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 6-237 0 0,7 22 1589 0 0,-1-30-1573 0 0,-5-6-16 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2-3 0 0 0,46-82 357 0 0,-49 87-357 0 0,50-132 184 0 0,-47 90-184 0 0,-5 36-21 0 0,-5 2 2 0 0,2 4-2431 0 0,4 0 1260 0 0,-7 0-578 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.5481E6">5819 11185 2304 0 0,'0'0'428'0'0,"0"0"959"0"0,0 0 422 0 0,0 0 81 0 0,0 0-74 0 0,0 0-388 0 0,0 0-168 0 0,0 0-38 0 0,0 0-52 0 0,0 0-190 0 0,0 0-85 0 0,0 0-21 0 0,-4 13 2869 0 0,8 30-896 0 0,6 19-821 0 0,-4 32-482 0 0,14 22-8 0 0,-17-108-1420 0 0,-3-6-17 0 0,4 5 78 0 0,12 26 298 0 0,-16-32-578 0 0,0-1-4 0 0,1 1 26 0 0,4 3 65 0 0,-1 7 16 0 0,3-15 203 0 0,27-94 1554 0 0,-14 17-2314 0 0,-3 30 1122 0 0,18-34-626 0 0,-21 61-1899 0 0,-1 6 396 0 0,-8 14-8315 0 0,-5 4 2000 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55012E6">6163 15251 1376 0 0,'0'0'65'0'0,"0"0"298"0"0,0 0 1226 0 0,-4-11 8887 0 0,2 2-10689 0 0,2 8 20 0 0,0-13-1355 0 0,0 5-2483 0 0,0 6 619 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55029E6">6160 15221 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 10 0 0 0,-3 3 1224 0 0,3-13 232 0 0,0 0 48 0 0,0 0 0 0 0,0 0-1128 0 0,0 0-232 0 0,0 0-48 0 0,0-6 0 0 0,0 2-96 0 0,0 4-128 0 0,0 0 32 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55124E6">6153 15200 2760 0 0,'0'0'125'0'0,"0"-12"2231"0"0,-1 1 3939 0 0,-14 48-2743 0 0,7 58-695 0 0,16 32 396 0 0,15-20-1214 0 0,10-62-933 0 0,-30-44-1072 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-3-34 0 0,96-166 703 0 0,-72 114-639 0 0,-9-32-572 0 0,-17 77 468 0 0,0 10-31 0 0,-6-22-455 0 0,0 11-3508 0 0,5 10-3672 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59771E6">9359 15275 11952 0 0,'0'-1'67'0'0,"0"0"0"0"0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-67 0 0,-34-9 5146 0 0,36 8-5069 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 2-77 0 0,-10 8 763 0 0,6-6-634 0 0,0 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 3-128 0 0,0 1 108 0 0,-3 11 172 0 0,0 0 0 0 0,2 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,2 0-280 0 0,2 61 688 0 0,19-37-159 0 0,-7-32-346 0 0,-13-12-174 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0-9 0 0,9-8 35 0 0,-1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,1-1 0 0 0,-2 1-1 0 0,6-12-34 0 0,27-40 89 0 0,-3 7-100 0 0,-17 20-55 0 0,-21 35-4 0 0,-1-1-103 0 0,1 2-332 0 0,1 1-119 0 0,0 0-16 0 0,-2 0-596 0 0,-1 1 165 0 0,2-2-2477 0 0,1 1 1724 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59826E6">9798 14961 12064 0 0,'0'0'553'0'0,"0"0"-16"0"0,-8 14-151 0 0,-4 33 4878 0 0,4 28-1596 0 0,2-22-2083 0 0,-7 73 353 0 0,-1 17 194 0 0,1 140-900 0 0,12-189-1248 0 0,1-92-72 0 0,0-2-51 0 0,0 0-18 0 0,0 0-158 0 0,-3-25-4130 0 0,2 8-1692 0 0,-1-2-1669 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59851E6">9720 15241 2304 0 0,'18'-58'224'0'0,"-10"36"1777"0"0,16 3 11624 0 0,9 21-9044 0 0,8 22-2754 0 0,0 22-1302 0 0,-8-25-2042 0 0,-26-15-78 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55168E6">6645 15101 10136 0 0,'-10'50'1272'0'0,"8"-44"-735"0"0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,2 3-538 0 0,6 27 1513 0 0,18 70 1825 0 0,8 12-1726 0 0,10-8-228 0 0,-23-68-629 0 0,-2-14-113 0 0,-18-12-556 0 0,5-23-22 0 0,11-37 0 0 0,12-47 53 0 0,15 8-396 0 0,-9 31 158 0 0,-16-11 121 0 0,-5 11 0 0 0,4-6 0 0 0,-14 45-97 0 0,-6 12-406 0 0,0 1-165 0 0,7-8-841 0 0,-2 1-1411 0 0,-2 6-6017 0 0,2 2 8141 0 0,-4 0 11 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55301E6">7252 15446 1840 0 0,'1'4'465'0'0,"-1"3"-969"0"0,-3-2 8499 0 0,3-4-5413 0 0,0-1-959 0 0,-3 15 3293 0 0,5-13-4747 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0-168 0 0,6-3 150 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,3-5-150 0 0,6-9 74 0 0,-1-1 1 0 0,-1 0-1 0 0,-1-2 1 0 0,0 1-1 0 0,-2-2 1 0 0,8-21-75 0 0,-17 44 4 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-4 0 0,-6 3 35 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,1 2-34 0 0,0-9 18 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 1 0 0,1 0-18 0 0,4 1-63 0 0,1 1 0 0 0,0-2 0 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,10-2 63 0 0,-8 1-520 0 0,13-4-1481 0 0,-8 1-3720 0 0,0 1-1868 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55402E6">7724 14971 6624 0 0,'3'19'-4'0'0,"-2"-6"534"0"0,-1 4 5466 0 0,0-17-4969 0 0,0 0-16 0 0,-7 44 3846 0 0,1 31-3228 0 0,2 1 0 0 0,4 42-1629 0 0,0-65 228 0 0,4 11-228 0 0,-4 44-16 0 0,-4-65-2758 0 0,4-30-1657 0 0,0-11 1925 0 0,0-1-3470 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55438E6">7687 15333 10136 0 0,'20'-72'1056'0'0,"11"-13"3846"0"0,-29 80-4603 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,4-1-299 0 0,-5 3 72 0 0,1-1-1 0 0,0 1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 2 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,3 2-71 0 0,25 23 580 0 0,9 42 1278 0 0,-28-1-3924 0 0,-11-48-2692 0 0,-2-15 3016 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59644E6">8400 14770 5872 0 0,'0'0'266'0'0,"0"0"1"0"0,-3-11 1056 0 0,3 9 7600 0 0,-8 81-5279 0 0,8-26-2198 0 0,1 28 275 0 0,-4 0-1 0 0,-5 31-1720 0 0,-11 187 1691 0 0,15-172-981 0 0,5-114-1358 0 0,-2-20-2345 0 0,-5-53-991 0 0,2 19 1937 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59675E6">8199 14780 8752 0 0,'0'0'673'0'0,"10"7"4424"0"0,12 7-302 0 0,17-11-2564 0 0,-29-3-1654 0 0,54 1 445 0 0,-44-3-776 0 0,0 1 0 0 0,0 1 0 0 0,0 1-1 0 0,0 1 1 0 0,0 1 0 0 0,9 3-246 0 0,-19-3 75 0 0,0 1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-75 0 0,33 48-3176 0 0,-37-45 1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59726E6">8767 15518 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 0-276 0 0,-27 2 2318 0 0,12-7 1927 0 0,2-23-2183 0 0,16 23-2093 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,2-2-146 0 0,6-21 178 0 0,-7 19-156 0 0,1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,2 1 0 0 0,1-3-22 0 0,-5 7 22 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,2 0-22 0 0,-1 0 73 0 0,-1 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 1 0 0 0,-2-1 0 0 0,1 1-1 0 0,0 0 1 0 0,1 2-73 0 0,10 73 976 0 0,-13-62-728 0 0,0 2 22 0 0,-2 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,0-1 1 0 0,-2 6-271 0 0,2-8 132 0 0,2-12-108 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,-2 0-24 0 0,1-2 9 0 0,0 1-1 0 0,0-2 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-2-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,-3-2-8 0 0,4 2-63 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-4 63 0 0,1 5-278 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,2-4 278 0 0,4-8-2146 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60188E6">10874 15382 3680 0 0,'0'0'284'0'0,"0"0"17"0"0,3-6 3845 0 0,4-1 6650 0 0,-21 234-6730 0 0,16-198-3860 0 0,0 0-3590 0 0,-2-29 1760 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60243E6">11191 15268 920 0 0,'-3'11'76'0'0,"-21"26"272"0"0,-6-6 6376 0 0,5-9-722 0 0,23-21-4979 0 0,-4 7 987 0 0,2 17 528 0 0,5-7-1218 0 0,4-12-1123 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,5 2-198 0 0,20 11 384 0 0,-27-14-322 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-62 0 0,-2 2 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,3-2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-3 0 0 0,0 1-326 0 0,-13-19-857 0 0,14 1-6482 0 0,3 12 584 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.6007E6">10305 14882 10824 0 0,'0'0'241'0'0,"0"7"331"0"0,-6 109 4121 0 0,-1 8-200 0 0,1-18-2317 0 0,-4 60-880 0 0,10 66-5334 0 0,0-231-1053 0 0,0-1-1451 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60107E6">10619 14899 2760 0 0,'-16'-16'247'0'0,"13"15"193"0"0,2 1 1710 0 0,-1 3 4946 0 0,-3 8-4369 0 0,3-4-1946 0 0,-24 37 1201 0 0,32-2-671 0 0,-26 125 670 0 0,-21 99 167 0 0,8-127-2609 0 0,27-124-2025 0 0,2-7-2648 0 0,0 1-1568 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60129E6">10249 15292 9672 0 0,'0'0'748'0'0,"1"1"-492"0"0,2 3-231 0 0,-2-2 331 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0-356 0 0,98 17 3649 0 0,-95-16-4114 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,4 4 465 0 0,8 8-1693 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60753E6">12482 15244 1840 0 0,'0'2'133'0'0,"0"7"1371"0"0,-7 15 9957 0 0,2-12-10918 0 0,1 10 2807 0 0,3-13-2599 0 0,1-8-23 0 0,0-1-45 0 0,0 3-163 0 0,-6 42 1090 0 0,-8 102 530 0 0,11-19-1604 0 0,6-91-486 0 0,-3-35-216 0 0,0-2-402 0 0,0 0-174 0 0,5-17-2600 0 0,-3 6 1430 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60794E6">12459 15428 4144 0 0,'0'0'319'0'0,"0"0"75"0"0,-2-4 5801 0 0,0-1-4842 0 0,2-5-34 0 0,9-37 4642 0 0,6 34-3827 0 0,24-1-548 0 0,-6 20-1696 0 0,-29-6 128 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 1-18 0 0,31 8 0 0 0,-22-7 0 0 0,-7-1 0 0 0,6 11 0 0 0,-2 11-870 0 0,-12-22 616 0 0,1-2-383 0 0,0 1-179 0 0,-12 34-4440 0 0,11-32 3346 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.6059E6">11589 14930 3224 0 0,'0'0'143'0'0,"0"2"-3"0"0,-1-2 1084 0 0,-4 10-2538 0 0,3-8 6295 0 0,0-2 6252 0 0,3 17-9469 0 0,8 56 352 0 0,-22 137-1892 0 0,9-122 559 0 0,1-61-682 0 0,2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,1 0 0 0 0,1 2-101 0 0,3 27-450 0 0,-10-48-56 0 0,2-6-6442 0 0,2-2 4901 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60615E6">11573 15101 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 0 21 0 0,2 0-42 0 0,96-20 3931 0 0,-39 9-2346 0 0,-35 15-4175 0 0,-17 3 964 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60651E6">11900 15494 7744 0 0,'0'0'356'0'0,"0"0"-8"0"0,0 0-63 0 0,0 0 571 0 0,-3 9 4563 0 0,-13-48-211 0 0,22-30-2906 0 0,24 40-1872 0 0,-13 16-315 0 0,-14 12-110 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 2-4 0 0,-1 0 59 0 0,1 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 1-59 0 0,1-4 22 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1-1-23 0 0,-30 7 210 0 0,2-37-185 0 0,14 8-523 0 0,11-7-2557 0 0,7 18 1503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60693E6">12232 15278 8288 0 0,'1'16'273'0'0,"0"-32"1643"0"0,-1 16-472 0 0,0 0 76 0 0,0 0-55 0 0,0 0-287 0 0,0 2-123 0 0,-6 44 4957 0 0,-7-1-5210 0 0,12 95 812 0 0,5-41-1951 0 0,-4-93-1422 0 0,0-5-625 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60843E6">12124 15037 8752 0 0,'20'16'1346'0'0,"-20"-14"-166"0"0,2-2-1575 0 0,2-4 4378 0 0,3-4 4520 0 0,3 1-11521 0 0,-6 3 1866 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61118E6">12923 15514 6912 0 0,'70'11'8898'0'0,"-65"-10"-8618"0"0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,2-4-280 0 0,31-51 1321 0 0,-35 52-1321 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0-2-1 0 0,-17-34-90 0 0,14 39 124 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-34 0 0,-50 23 664 0 0,47-18-600 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 3-64 0 0,2-1 41 0 0,0 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,3 8-41 0 0,-3-11 98 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,5 6-98 0 0,-6-11 5 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-5 0 0,1-1-54 0 0,98-32-5788 0 0,-58 8 1619 0 0,-21 11 2079 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61533E6">14274 15358 1840 0 0,'0'0'83'0'0,"0"0"169"0"0,0 0 668 0 0,0 0 288 0 0,0 0 58 0 0,0 0-22 0 0,0 0-144 0 0,0 0-63 0 0,0 0-11 0 0,0 0-2 0 0,0 8 2048 0 0,-3 19-266 0 0,2-2-362 0 0,1 78 1520 0 0,-2-32-3723 0 0,1 18-415 0 0,2-81 488 0 0,4 6-6100 0 0,0-7-783 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61567E6">14278 15514 10136 0 0,'19'-57'5082'0'0,"8"11"-1747"0"0,-4 27-1698 0 0,-21 16-1500 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,1 0-137 0 0,0 1 60 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 3-60 0 0,15 17 54 0 0,-6-15-897 0 0,-9-7-100 0 0,-1-2-37 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61341E6">13529 14750 2304 0 0,'0'0'101'0'0,"0"0"294"0"0,0 0 1149 0 0,0 0 506 0 0,0 2 1554 0 0,0 9-1838 0 0,2 148 6571 0 0,-2 118-5024 0 0,-13-9-1402 0 0,10-164-1693 0 0,-6-29-376 0 0,8-74-114 0 0,1-1-766 0 0,-4-11-2968 0 0,-3-2-3447 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61375E6">13505 14951 920 0 0,'0'-1'67'0'0,"-3"-7"403"0"0,4 0 4358 0 0,4-6-1924 0 0,-4 11-1691 0 0,17-32 4007 0 0,23-5-3052 0 0,6 8-888 0 0,-28 24-1087 0 0,-17 7-85 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1-108 0 0,0 0 199 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,3 4-199 0 0,27 61 460 0 0,-25-41-231 0 0,0 2 1 0 0,-2-1-1 0 0,-1 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,-2 27-229 0 0,0-48 147 0 0,-1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-3 3-146 0 0,3-7 10 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 0 0 0,-4-2-10 0 0,-3-3-494 0 0,0 0-1 0 0,1-1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-3-6 495 0 0,3 1-5994 0 0,3-5-1719 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61458E6">13882 15514 8288 0 0,'0'0'190'0'0,"4"-6"253"0"0,9-6-212 0 0,26 0 5159 0 0,2 7-1205 0 0,-16 13-2607 0 0,-3-2 202 0 0,-14-4-715 0 0,-15-5-592 0 0,-34 8 113 0 0,-36 16 500 0 0,73-19-1076 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 2-10 0 0,-2 6 2 0 0,1-6-2 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,3 5 0 0 0,11 14 0 0 0,-15-25 1 0 0,2 2 37 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,2-1-39 0 0,43-29 241 0 0,-36 16-275 0 0,-1 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,0-2 34 0 0,12-69-964 0 0,-14 34 382 0 0,-16 90 634 0 0,9-24-10 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,2-1-1 0 0,0 1 1 0 0,3 7-42 0 0,14 45 54 0 0,-8-42-1794 0 0,-7-22 730 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61927E6">14869 14865 3224 0 0,'0'0'143'0'0,"0"0"279"0"0,0 0 1073 0 0,0 0 470 0 0,0 0 92 0 0,0 0-154 0 0,0 0-730 0 0,0 0-315 0 0,0 7 684 0 0,-3 1-898 0 0,3-6-48 0 0,0 7 1051 0 0,-7 47 1551 0 0,-33 303 1366 0 0,37-333-4246 0 0,2 0 0 0 0,0 0-1 0 0,2 0 1 0 0,0 1 0 0 0,2-1-1 0 0,0-1 1 0 0,1 1-1 0 0,6 18-317 0 0,20 15 208 0 0,-28-54-186 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-2 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,3 0-22 0 0,-4-2 31 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1-30 0 0,-2 5 3 0 0,9-17 55 0 0,-2 0 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,3-17-58 0 0,5-18 41 0 0,21-98-41 0 0,14-148-432 0 0,-44 262-57 0 0,-1 7-2509 0 0,-2 9-4848 0 0,0 12 100 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62065E6">15902 15394 2304 0 0,'0'0'101'0'0,"0"17"22"0"0,-7 6 6125 0 0,-3 17 4249 0 0,8-9-9080 0 0,-2 87 316 0 0,0-84-1477 0 0,1-21-426 0 0,2-12-721 0 0,1-1-329 0 0,0 0-75 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62116E6">16132 14930 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 2-242 0 0,4 71 6774 0 0,-8 3-1144 0 0,-8 43-2340 0 0,2 49-2718 0 0,6-9-705 0 0,0 16-1521 0 0,4-164 244 0 0,0-9-61 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62155E6">16367 15360 10136 0 0,'0'0'777'0'0,"-1"2"-505"0"0,-3 43 4407 0 0,3-12-457 0 0,3 79-789 0 0,-4-104-3589 0 0,2 0-1781 0 0,0-7 758 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62214E6">16751 15348 1376 0 0,'1'-2'299'0'0,"11"-58"5252"0"0,-14 43-5059 0 0,1 13-375 0 0,1 3 35 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,1-1-152 0 0,-3 1 283 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-285 0 0,-7 12 754 0 0,-42 66 501 0 0,31-7-220 0 0,21-68-992 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,4 3-41 0 0,1 6 59 0 0,7 9 178 0 0,-12-20-112 0 0,0 0 0 0 0,0 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-125 0 0,-12 16 28 0 0,8-19-9 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-2 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1-19 0 0,-34 2-215 0 0,6 22-3705 0 0,29-16-4023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62285E6">17055 15446 3680 0 0,'0'0'284'0'0,"0"0"109"0"0,2-1 1154 0 0,27-18 5762 0 0,31 18-2771 0 0,-31 12-2764 0 0,-16-1 1490 0 0,-56-16-3312 0 0,39 4 32 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-3 3 16 0 0,1-1 34 0 0,-1 0-1 0 0,1 1 0 0 0,0 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 3-33 0 0,3-7 57 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 2-56 0 0,-1-4 45 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1-45 0 0,91-156-3426 0 0,-93 160 3373 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 53 0 0,-2 20 337 0 0,-15 82 1575 0 0,10 6-1206 0 0,14-63-7272 0 0,-4-35-749 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61995E6">15614 14814 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 2 76 0 0,-5 11 2311 0 0,-6 38 3900 0 0,-3 115-3759 0 0,-16 87 806 0 0,4 41-2464 0 0,19-203-1627 0 0,7-90-756 0 0,-3-6-2095 0 0,3-4 1602 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62019E6">15538 15095 11232 0 0,'-4'-29'1016'0'0,"5"29"-836"0"0,12-29 2777 0 0,60 24 2000 0 0,15 19-1797 0 0,-49 7-4345 0 0,-32-17-189 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62446E6">17905 15521 15664 0 0,'13'5'1187'0'0,"-11"-4"-976"0"0,1-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-2-210 0 0,7-13-211 0 0,-4 9-129 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-10 340 0 0,-7-34-1540 0 0,3 51 1562 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-22 0 0,-19 17 1568 0 0,17-13-1383 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,0 1-185 0 0,-6 32 308 0 0,4-27-103 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,1 0 0 0 0,0 3-205 0 0,14 19 1394 0 0,-16-34-1436 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1 42 0 0,0 0-47 0 0,85-59-5723 0 0,-74 51 4417 0 0,-3 0-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.6237E6">17517 15193 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0-6 199 0 0,3-21 284 0 0,-3 26 22 0 0,0 1 21 0 0,0 0 53 0 0,0 0 198 0 0,0 0 86 0 0,0 0 21 0 0,0 0-28 0 0,0 1-122 0 0,-9 88 4045 0 0,2-22-3014 0 0,-20 182 836 0 0,13-109-2456 0 0,12-124-5049 0 0,1-15-3688 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62393E6">17497 15313 19351 0 0,'0'0'439'0'0,"0"0"62"0"0,0 0 33 0 0,0 0-65 0 0,7-3-292 0 0,86-18 2799 0 0,-37 10-2385 0 0,-21 8-4619 0 0,-33 3 2335 0 0,-2 0-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62896E6">18258 15404 920 0 0,'0'0'115'0'0,"0"0"146"0"0,0 0 68 0 0,2-1 14 0 0,10-26-975 0 0,1 13 771 0 0,-12 12 195 0 0,-1 2 149 0 0,0 0 590 0 0,0 0-1059 0 0,6-7 9846 0 0,-2 4-8006 0 0,-3 1-1530 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1-1-324 0 0,1-1 1337 0 0,0 4-893 0 0,-9 8-200 0 0,-28 59 2244 0 0,12 5-1504 0 0,23-16-648 0 0,2-55-335 0 0,1 7 28 0 0,0-1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,1 1-28 0 0,-1-3 14 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,4-1-13 0 0,31-21 64 0 0,-3-47 8 0 0,-14-11-72 0 0,-16 42-89 0 0,2-53-263 0 0,-9 93 324 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 29 0 0,-3 9-8024 0 0,1 0 350 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62952E6">18714 15275 2304 0 0,'0'0'101'0'0,"0"0"363"0"0,0 0 1439 0 0,0 0 626 0 0,0 0 126 0 0,0 0-194 0 0,3-14 1239 0 0,-1 23 4485 0 0,0 48-5205 0 0,-6 21-1571 0 0,1 35-565 0 0,-4-51-599 0 0,8 98 126 0 0,5-102-812 0 0,6-132-3199 0 0,-11 24-1172 0 0,-1 37 2865 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62976E6">18721 15419 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-150 0 0,-7-5 3377 0 0,16-32 352 0 0,32-14-1964 0 0,-35 48-2182 0 0,-3 1 153 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,3 1-123 0 0,33 13 165 0 0,-8 20-245 0 0,-9 22-3497 0 0,-21-54-1940 0 0,-1-2-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.63177E6">19319 15244 9416 0 0,'-2'-4'852'0'0,"-22"-10"284"0"0,14 12 6835 0 0,-10 31-4820 0 0,16-20-2774 0 0,-46 128 2838 0 0,22-39-1934 0 0,20-71-1118 0 0,2 0 0 0 0,1 1-1 0 0,0 0 1 0 0,2 0 0 0 0,1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,3 6-163 0 0,-2-16-6 0 0,13 117-229 0 0,4-77-1218 0 0,-1-37-2030 0 0,-10-15-2522 0 0,-5-5-1562 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.63203E6">19640 15197 11520 0 0,'0'0'886'0'0,"1"-1"-582"0"0,15 6 5156 0 0,-12-1-5008 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 5-452 0 0,5 13 803 0 0,6 61 1048 0 0,-10-35-1193 0 0,-4 50 394 0 0,-5 10-300 0 0,-10 5-403 0 0,-12 46-253 0 0,1-47-2616 0 0,-8-4-4080 0 0,18-61-2023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.63734E6">2265 13773 2760 0 0,'-20'-11'247'0'0,"9"-2"39"0"0,10 13 290 0 0,-3-1-375 0 0,1-4 6201 0 0,2-1-5440 0 0,13 4 7229 0 0,-7 2-9038 0 0,92 45 4699 0 0,-28-9-2217 0 0,48-15-519 0 0,45 0-182 0 0,-19 27-394 0 0,-118-36-455 0 0,-4 0-32 0 0,1-1 0 0 0,0-1-1 0 0,0-2 1 0 0,1-1-1 0 0,0 0 1 0 0,0-2-1 0 0,1-1 1 0 0,-1-2-1 0 0,1 0 1 0 0,6-2-53 0 0,140-29 1189 0 0,90-38-261 0 0,-93 44-928 0 0,-140 21 0 0 0,280-2 0 0 0,-23 32 15 0 0,24-11 250 0 0,13 13-174 0 0,-116-13 135 0 0,-9 4-42 0 0,116 20-48 0 0,-211-30-125 0 0,78 13 42 0 0,188 33 22 0 0,116 2 393 0 0,-197-19-403 0 0,334 59 135 0 0,-253-57-200 0 0,-47 1-61 0 0,-51-2 141 0 0,8 4-80 0 0,-97-24 0 0 0,75-1 0 0 0,152 7 0 0 0,-170-6 0 0 0,69-8 0 0 0,178-23 0 0 0,-283 11 0 0 0,-32 5 0 0 0,294-2 0 0 0,-254-14 0 0 0,388-11-9 0 0,-304 1 914 0 0,-18-9-1376 0 0,63 5 966 0 0,-78 29-599 0 0,-6 4-152 0 0,-127 2 112 0 0,-3 6 239 0 0,3-3 314 0 0,54 6-541 0 0,29-16-88 0 0,3-7 252 0 0,-109-4-160 0 0,188-28 128 0 0,-62 1 0 0 0,-42 5 11 0 0,8 0-22 0 0,112 5 11 0 0,-31 4 80 0 0,108 6-133 0 0,-148 17 42 0 0,184-16 11 0 0,-123 9 0 0 0,40 0 0 0 0,300 26 139 0 0,-127-30-86 0 0,-306 23 75 0 0,-17-3-128 0 0,-81-19 0 0 0,-8-9 148 0 0,25-12-132 0 0,-40 16-28 0 0,64 15 12 0 0,-48 6-96 0 0,-93-8 80 0 0,-9 3 5 0 0,-12 12-319 0 0,19-2 154 0 0,9 7-187 0 0,-8 3 347 0 0,0 61 16 0 0,-5 86 15 0 0,13 162 28 0 0,-1-117-101 0 0,17 27 233 0 0,-4-5-91 0 0,-5 21-20 0 0,-25-46 106 0 0,-5-63-95 0 0,0-20-75 0 0,0 17 0 0 0,0-28 224 0 0,-6-29-160 0 0,13-84-64 0 0,1-2 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-2 1 0 0 0,-16 8 0 0 0,4-9 0 0 0,-287 7 96 0 0,105-13-96 0 0,-219 3 0 0 0,52 3 71 0 0,-112 7-86 0 0,-140-20 71 0 0,40 0-136 0 0,53 3 80 0 0,84 0 0 0 0,-343-11 0 0 0,144 1 68 0 0,179 8 268 0 0,256 9-440 0 0,-543-18 204 0 0,252-19-164 0 0,102 6 77 0 0,-352-3 78 0 0,305 14-91 0 0,-3-17 0 0 0,23 5 0 0 0,86 15 0 0 0,71 10 0 0 0,-207 7 0 0 0,203 4 0 0 0,-775-1 0 0 0,268-46 0 0 0,286 8 0 0 0,-119-10 0 0 0,402 23 0 0 0,1-10 0 0 0,-67-10 0 0 0,163 31 0 0 0,0 5 0 0 0,-101 10 0 0 0,29 9 0 0 0,14 0 0 0 0,-35-9 0 0 0,21-14 0 0 0,-20 3 0 0 0,-160-3 0 0 0,170 17 0 0 0,-30-14 0 0 0,58 4 0 0 0,144 4 0 0 0,-116 7 0 0 0,-61-7 0 0 0,101-8 0 0 0,-48-10 0 0 0,56 10 0 0 0,-80 4 0 0 0,107-4 0 0 0,-71 0 0 0 0,44-5 0 0 0,82 11-60 0 0,4 1-252 0 0,1 0-111 0 0,0 0-1358 0 0,0 0-5615 0 0,0 0-2407 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.64323E6">2259 13660 1376 0 0,'0'0'65'0'0,"0"1"-6"0"0,0 17 154 0 0,0-16 831 0 0,0-2 358 0 0,0 0 65 0 0,0 0-83 0 0,0 0-422 0 0,0 0-186 0 0,0 0-38 0 0,0 0-28 0 0,0 0-88 0 0,0 0-40 0 0,0 0-6 0 0,0 0 2 0 0,0 0 12 0 0,0 0 2 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0-1 0 0,0 9 1801 0 0,6 105 2520 0 0,1-8-2608 0 0,3 115-760 0 0,-10-2-472 0 0,34 57-113 0 0,-28-238-854 0 0,20 102-208 0 0,-1 69 1907 0 0,-12-83-2238 0 0,16 175 898 0 0,-33-185-286 0 0,-47 142-20 0 0,45-159-169 0 0,6-49-56 0 0,-3 10 374 0 0,-13 49-182 0 0,15-23-546 0 0,8-12 992 0 0,4-2-446 0 0,-9-66-106 0 0,-1-5-17 0 0,-1-1-234 0 0,-6-18-3530 0 0,6 9 2303 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.86899E6">2341 7605 4144 0 0,'0'0'319'0'0,"-5"1"252"0"0,5-2 2376 0 0,22-31-2360 0 0,-26 13 5029 0 0,4 18-5505 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-112 0 0,-49 23 1284 0 0,15 1-659 0 0,-29 36 50 0 0,18-11-590 0 0,-89 126 107 0 0,45-43-21 0 0,5 2 334 0 0,13-5-252 0 0,-15 47-182 0 0,-52 145 566 0 0,126-284-548 0 0,-55 176 254 0 0,2 101-151 0 0,35-58 504 0 0,13-108-216 0 0,8 106 134 0 0,8-137-457 0 0,-2 110 104 0 0,12-113-187 0 0,5-1-1 0 0,15 60-73 0 0,4-10 269 0 0,25 66-269 0 0,-6-40 164 0 0,17 66 46 0 0,-15-74 888 0 0,60 138-1098 0 0,15 34 320 0 0,-89-236-133 0 0,21 45 186 0 0,-2-46 46 0 0,16 57-249 0 0,-13-25-191 0 0,-19-56 21 0 0,22 54 139 0 0,-33-59-22 0 0,-27-79-141 0 0,-3-7-107 0 0,0-2-69 0 0,0 0-21 0 0,0-3-260 0 0,0-9-1082 0 0,-3-4-465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.86969E6">1686 13345 13824 0 0,'-49'24'1677'0'0,"47"-23"-740"0"0,27-3 3060 0 0,5 0-4365 0 0,70 37 323 0 0,0 33 373 0 0,-10 8 165 0 0,110 105 1071 0 0,-176-164-1495 0 0,-1-2-1 0 0,2-1 0 0 0,-1-1 0 0 0,2-1 1 0 0,20 5-69 0 0,64 13 245 0 0,-49-23 458 0 0,-48-18 147 0 0,-12 9-799 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-2-51 0 0,0-5 176 0 0,-19-113 411 0 0,-19-86-1189 0 0,0 67-4384 0 0,20 87 2801 0 0,-4 9-21 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.87098E6">2532 13727 2760 0 0,'-7'-3'248'0'0,"-33"-31"6865"0"0,23 4-6498 0 0,-13-19 774 0 0,-3-6 1367 0 0,2-27 825 0 0,7 5-1573 0 0,17 19-676 0 0,-1-14-560 0 0,11-76 1085 0 0,17 5-1137 0 0,-11 93-1006 0 0,-12 5-1132 0 0,1 8-1456 0 0,3 35 1591 0 0,4 0-48 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87216E6">4602 10374 14976 0 0,'-24'21'1597'0'0,"-12"-7"-1817"0"0,35-14 85 0 0,1 0-121 0 0,-8-1-614 0 0,-3-22 1632 0 0,3-15 143 0 0,-8-55 2063 0 0,-1-15-936 0 0,1-84-705 0 0,12-23-328 0 0,0 21-897 0 0,2-166 234 0 0,1-27 12 0 0,8 202-193 0 0,-1-125-36 0 0,-8 155-1315 0 0,27 90-2477 0 0,-17 52 2086 0 0,1-15-2513 0 0,-8 24 1999 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87257E6">3956 8288 18887 0 0,'0'0'863'0'0,"-1"-1"-14"0"0,1-12-806 0 0,-1 1-1 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,2-1-42 0 0,-2 0-42 0 0,119-204-129 0 0,-59 112 171 0 0,27-2 0 0 0,-82 95 2 0 0,-1 1-1 0 0,1 0 0 0 0,0 1 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 2-1 0 0,1-1 0 0 0,5 0-1 0 0,-10 5 48 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 2 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 2-47 0 0,70 216 1312 0 0,-19-36-1200 0 0,-27-64-32 0 0,-1-30-402 0 0,4-42-2524 0 0,-21-46 814 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87403E6">2174 15272 13040 0 0,'-3'7'1185'0'0,"-23"29"-737"0"0,2-28 563 0 0,-30-22 2664 0 0,24-3-2667 0 0,-37-18 867 0 0,34 16-1425 0 0,0-1 0 0 0,2-2 0 0 0,0-2-1 0 0,2-1 1 0 0,-14-15-450 0 0,-162-174 1230 0 0,175 178-981 0 0,-28-30-91 0 0,3-4 0 0 0,3-2 1 0 0,-3-10-159 0 0,-125-221 786 0 0,-85-179 150 0 0,174 267-915 0 0,9-4 1 0 0,8-5-1 0 0,-6-58-21 0 0,-61-201 160 0 0,65 179-160 0 0,-46-195-216 0 0,73 261 184 0 0,9-3 0 0 0,3-65 32 0 0,3-72-64 0 0,8 70 0 0 0,15 186 64 0 0,5 0 0 0 0,6-110 0 0 0,3 166 0 0 0,5-74 0 0 0,18-97 0 0 0,27-111-80 0 0,51-149-171 0 0,-6 153-223 0 0,-16 98 455 0 0,-45 154 70 0 0,4 2 0 0 0,3 3-1 0 0,8-6-50 0 0,-22 41 25 0 0,78-115 30 0 0,41-1-129 0 0,8 30-44 0 0,33-36-58 0 0,-146 130 134 0 0,78-63-842 0 0,-122 107 868 0 0,24-14-1611 0 0,-13 11-5936 0 0,-10 3 272 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87445E6">1365 6048 11976 0 0,'0'0'922'0'0,"-1"-2"-600"0"0,-7-9-54 0 0,7 10 932 0 0,-1-8 2652 0 0,1-6-2353 0 0,4 11-1499 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,2 0 1 0 0,17-11-106 0 0,88-31-209 0 0,-101 40 308 0 0,0 0-1 0 0,0 2 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 2-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,7 5 8 0 0,-7-2 12 0 0,0 0 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 2-1 0 0,0-1 1 0 0,5 11-12 0 0,-4-4 37 0 0,0 1 0 0 0,-1 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,-2 0 1 0 0,3 17-38 0 0,-4 88 434 0 0,-27-12 5 0 0,13-77-354 0 0,-46 122 75 0 0,-60 119-1810 0 0,106-249 551 0 0,-2-2-48 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87588E6">8232 5839 13360 0 0,'-4'-1'271'0'0,"1"0"1"0"0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-272 0 0,0-3 27 0 0,0 1 0 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1-4-27 0 0,-1-8 302 0 0,-10-128 1863 0 0,-6-5-421 0 0,-5-149 624 0 0,5 54-1161 0 0,-12-355-614 0 0,22 347-593 0 0,-1 78-104 0 0,7 170 61 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0-1 43 0 0,2 8-62 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 62 0 0,-7 16-1775 0 0,1 4-289 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87619E6">7550 3518 22607 0 0,'0'0'514'0'0,"-1"-2"71"0"0,-1 0-530 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1-55 0 0,11-18-19 0 0,0 0-1 0 0,0 2 0 0 0,2-1 1 0 0,0 2-1 0 0,0 0 1 0 0,2 1-1 0 0,-1 1 0 0 0,2 1 1 0 0,0 0-1 0 0,3 0 20 0 0,21-20-44 0 0,-34 27-32 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 76 0 0,-5 2-16 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,1 0 16 0 0,49 140 542 0 0,-28-90-361 0 0,1-1 0 0 0,3-1 1 0 0,16 24-182 0 0,39 48-220 0 0,-45-66-1394 0 0,-19-35-78 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-14T20:43:56.589"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">247 705 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">640 722 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-9 10039 0 0,4 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1036 664 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1384 746 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,4-23-839 0 0,-7 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 79 971 0 0,13-78-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,3-28 325 0 0,-7 43 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 35 365 0 0,9-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-43 40 0 0,-1 48 757 0 0,-8 6-562 0 0,-2 1-34 0 0,14 15 96 0 0,-24 51 294 0 0,10-64 48 0 0,0-2-24 0 0,-12 10 14 0 0,11-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-12 0 0,-1-2-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,16-18-798 0 0,-5 23 705 0 0,11 17 39 0 0,-21-13 64 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 2-10 0 0,2-5 84 0 0,-5 17 237 0 0,-20-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 11-3207 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">1679 463 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 57 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,1 17 113 0 0,-2-14-1404 0 0,-1 51 981 0 0,-4-2-1688 0 0,1-59-1417 0 0,-2-32 962 0 0,-7-28-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">1615 598 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-32 2722 0 0,-14 31-3180 0 0,15-15 1008 0 0,23-24 674 0 0,-35 36-2057 0 0,1 2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 19 1009 0 0,-52 14 55 0 0,-4-18-600 0 0,21 47 1448 0 0,-23 2-2113 0 0,-15-60 230 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 22 399 0 0,1-11-337 0 0,7-8-104 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 37 0 0,-35-1 653 0 0,-7-25-4978 0 0,34 19 2334 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">3007 428 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 48 1154 0 0,-12 24 2052 0 0,-3 33 1755 0 0,3 52-2463 0 0,4-54-962 0 0,-3 32-1172 0 0,7-140-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-3 13-2556 0 0,2-23 1622 0 0,1-1-894 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">3025 486 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-4 772 0 0,-14 10-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 1 1 0 0,2 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 2-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-4-1-4 0 0,-53-44-4198 0 0,55 42-3651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">2231 124 3680 0 0,'-6'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,8 16-23 0 0,2-13-297 0 0,6 3-1604 0 0,-9 95 2 0 0,7-77 200 0 0,1-18-716 0 0,2-41-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">2155 695 1376 0 0,'5'-20'2159'0'0,"2"0"4223"0"0,7-6-3735 0 0,-2 6-1523 0 0,11-17 1153 0 0,4 12 523 0 0,-4 3-1591 0 0,22-17 135 0 0,-44 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 7-27 0 0,10 30 368 0 0,29 120 1443 0 0,-20-124-1634 0 0,1-14-84 0 0,-13-23-77 0 0,-6-2-29 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 13 0 0,40-28-350 0 0,19-12-3834 0 0,-54 36 2533 0 0,3 3-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">1 302 6448 0 0,'7'21'6309'0'0,"-7"-18"-6682"0"0,4 54 3514 0 0,8 85-847 0 0,-2-44-690 0 0,-5-10-929 0 0,13 132 737 0 0,-29 32 57 0 0,6-176-1337 0 0,-1-48-256 0 0,5-13-955 0 0,1-11-4480 0 0,0-4-582 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">12 333 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,18-38 6274 0 0,-18 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,12-3 291 0 0,71-18 828 0 0,-37 5-729 0 0,11-5 96 0 0,51 12 370 0 0,-61 8-222 0 0,43 2-1079 0 0,-21-6 16 0 0,36-20 451 0 0,-30 15 1144 0 0,62 1-1448 0 0,3 19 224 0 0,-53-19-645 0 0,-30-1 1538 0 0,7 0-1123 0 0,-37 8-292 0 0,52 0 264 0 0,-26-6 20 0 0,55-26 70 0 0,11 18-205 0 0,12 9 34 0 0,-66-4 219 0 0,23-5-424 0 0,-5 12 192 0 0,-11 5 584 0 0,44 1-1352 0 0,-6 9 736 0 0,0 6 1017 0 0,-32-10-298 0 0,-12 0-1239 0 0,27-4 520 0 0,14 3 64 0 0,12 29 75 0 0,-60-11-166 0 0,14 1 523 0 0,-3-9-840 0 0,-22-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,74-9-197 0 0,-22 19 0 0 0,-41-15-20 0 0,-43-2 0 0 0,-14-5 0 0 0,25 17 0 0 0,-38-3 0 0 0,5 6 0 0 0,13 23 64 0 0,-5 28 0 0 0,-8 23-64 0 0,-5 32-8 0 0,1-51 125 0 0,-4 32-203 0 0,-8 34 295 0 0,8 44-190 0 0,-17-84 82 0 0,-1-41-13 0 0,6-44 96 0 0,6-12-234 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 2 51 0 0,0-3 114 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0-114 0 0,-14 0 158 0 0,-98 8-218 0 0,82-3 59 0 0,0-1-1 0 0,0-2 1 0 0,0-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-23-6 1 0 0,5-4-9 0 0,-1 3 0 0 0,0 3 0 0 0,0 2 0 0 0,-22 2 9 0 0,-112 0 332 0 0,139 4-330 0 0,0-1-1 0 0,-1-3 1 0 0,1-2-1 0 0,0-1 1 0 0,-8-7-2 0 0,23 9-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-21 4 18 0 0,-142 30 64 0 0,-4-12-136 0 0,-48-9 152 0 0,173-13-80 0 0,-92 0 11 0 0,-34-17 42 0 0,102 17-53 0 0,-24-13 80 0 0,23-11-176 0 0,-85-18 224 0 0,56 22-196 0 0,63 6 192 0 0,-62-3-124 0 0,50 11 0 0 0,46 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12">6715 897 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,22-14-8855 0 0,-18 9 1888 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13">7090 941 10592 0 0,'-13'-13'818'0'0,"10"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">7438 851 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,5 0-232 0 0,-2 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">7801 941 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-38 1231 0 0,1 45-2463 0 0,0 1 0 0 0,2 1 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,-1 3-113 0 0,3-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-16-143 0 0,-13 33-62 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-2-43 0 0,3 2 32 0 0,1 10 23 0 0,-10 18 200 0 0,3-27-96 0 0,-7 4-695 0 0,14-7-611 0 0,7-10-5710 0 0,-6 6 446 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">8085 572 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 22-45 0 0,-12-25-3788 0 0,3 8 1039 0 0,3 83 1637 0 0,7 83-1221 0 0,-14-86-1606 0 0,0-79-341 0 0,-2-4-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">8386 613 2760 0 0,'4'8'1828'0'0,"4"20"4892"0"0,5 25-3444 0 0,1 103 1947 0 0,-11-80-3937 0 0,-6-37-4508 0 0,3-36 1701 0 0,-4 6-229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">8439 941 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,9-39 5734 0 0,3-11-521 0 0,-16 20-3279 0 0,11 10-1202 0 0,8-37 1 0 0,-14 56-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,3 0-93 0 0,2-2 95 0 0,-4 3-21 0 0,26 0-60 0 0,2 14-14 0 0,-6 7 0 0 0,-20-12 0 0 0,10 23 0 0 0,19 74 514 0 0,-19-52 356 0 0,6-19-278 0 0,-20-34-517 0 0,7 3 98 0 0,-5-1-141 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-29-4233 0 0,-22 32 2840 0 0,0 1-164 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">9226 669 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-39-6 1747 0 0,43 9-1667 0 0,4-2 170 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 42-483 0 0,18 2 618 0 0,16 12 378 0 0,10 4-513 0 0,15-4 1899 0 0,26-11-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 0 0 0 0,-22-9 0 0 0,-2 2 0 0 0,0-5-64 0 0,31-22-5497 0 0,-32 16 3530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">9491 1002 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-17 649 0 0,-9 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 20 784 0 0,-16 13 56 0 0,6-32-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">9763 661 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 73 1352 0 0,-5-54-2105 0 0,-9 63 686 0 0,-2-6-314 0 0,3 68-530 0 0,6-113-273 0 0,-3-10 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-3-14-1557 0 0,2-1 195 0 0,-3-2-70 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">9729 664 1376 0 0,'4'6'367'0'0,"-3"-5"1002"0"0,-1-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,9-7 51 0 0,33-23 1588 0 0,-29 24-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,2 2 108 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 2 0 0 0,1-2 1 0 0,0 6-108 0 0,10 27 435 0 0,-1 58 787 0 0,-11-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-3 0 0 0 0,2 0 0 0 0,0 0-56 0 0,-44 35 929 0 0,43-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-5 0 0 0,4-15-5381 0 0,0 15-2125 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">10205 395 0 0 0,'-12'12'0'0'0,"6"-15"140"0"0,4 3 2586 0 0,2 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 30 3000 0 0,-14 31-1947 0 0,1 50 181 0 0,4 1 624 0 0,-7-41-881 0 0,11 38-1316 0 0,-12-26-173 0 0,8-43 0 0 0,14 3-2476 0 0,-12-41 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">10187 825 4376 0 0,'0'0'199'0'0,"10"-11"1918"0"0,-6-2 1016 0 0,11-10 683 0 0,-6-13-1297 0 0,-2-1-472 0 0,5 29-1272 0 0,-10 7-743 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 22 598 0 0,-25-17-674 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 6-227 0 0,6 92 608 0 0,-7-65-165 0 0,-1-12 997 0 0,27-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,12-10-60 0 0,-19 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">10815 698 2760 0 0,'0'1'207'0'0,"0"45"6763"0"0,0-45-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 13-344 0 0,-2 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 9-1278 0 0,-12 63 616 0 0,0-18 973 0 0,13 39-2158 0 0,3-87 962 0 0,-3-26-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">10879 691 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,58-25 1867 0 0,-55 27-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,2 0-156 0 0,-1 0 96 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1-95 0 0,-1-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 5-94 0 0,-43 58 1952 0 0,47-67-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-14T20:43:56.649"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+    <inkml:brush xml:id="br1">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">5678 3769 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-8 0 710 0 0,-57 11 2232 0 0,-87-9 113 0 0,65-16-2111 0 0,82 11-1711 0 0,2 1 0 0 0,0 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0-7 0 0,0 0 3 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,-2-1-3 0 0,-4-1 53 0 0,-47 16 746 0 0,-3-34-422 0 0,-40 20 95 0 0,18 18-267 0 0,-2-27 255 0 0,17 6-262 0 0,-8-5 515 0 0,23 24-785 0 0,-7-11 316 0 0,59-3-237 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 1 0 0 0,0-2 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,1 5-384 0 0,-1 0-2483 0 0,0-5 1589 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">4643 3507 12384 0 0,'-12'-11'1277'0'0,"-1"9"-438"0"0,-12 9 3998 0 0,7 3-3431 0 0,-18 14 690 0 0,-43 37-1014 0 0,22-27 402 0 0,6 18-1322 0 0,28-24-154 0 0,-8 14 872 0 0,29-39-855 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,2-1-1 0 0,0 2 1 0 0,0-2 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-2-1 0 0,3 3-23 0 0,31 38 389 0 0,-24-33-394 0 0,-1-2 1 0 0,2 0-1 0 0,0-1 0 0 0,0-1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1-2 0 0 0,1 0 0 0 0,-1-1 1 0 0,1-1-1 0 0,4 0 4 0 0,-4 0-173 0 0,87 19-1371 0 0,-36 1-4118 0 0,-48-15-1845 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="2">3938 2858 2760 0 0,'7'14'125'0'0,"-19"-7"1798"0"0,-5 10-59 0 0,13-10 428 0 0,-20 6 4862 0 0,24-13-6578 0 0,0 0-15 0 0,0 0-34 0 0,-2 2 119 0 0,1-1-159 0 0,1-1 2989 0 0,47-16-1901 0 0,9 9-396 0 0,17 3-749 0 0,-18 1 156 0 0,34-1 469 0 0,18-5-497 0 0,-3-2-454 0 0,46-3 952 0 0,-44 8-543 0 0,-43-4-402 0 0,45-9 402 0 0,-58 7-745 0 0,4 12 112 0 0,-30-6 120 0 0,14 4 0 0 0,6-13 444 0 0,-21 4-280 0 0,11 0-164 0 0,-21 3 0 0 0,-4 7 0 0 0,15 7-1208 0 0,-23-5 877 0 0,5 3-1583 0 0,8 12-3659 0 0,-8-10 3847 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="3">5204 2402 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,8 22 9129 0 0,19-4-7935 0 0,-14-13-2328 0 0,51 29 1337 0 0,-51-23-2420 0 0,-5-5 346 0 0,1 0 1 0 0,-1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,3 9-255 0 0,6 66 1080 0 0,-23-5-224 0 0,-9-28-856 0 0,-24-2 327 0 0,-24-10 1242 0 0,8-16-2553 0 0,31-23-3117 0 0,21-1 2058 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="4">10723 2919 8288 0 0,'9'-47'864'0'0,"-10"44"-720"0"0,2-9 1811 0 0,1 9 5703 0 0,52-2-3242 0 0,-20 5-4222 0 0,66 2 1838 0 0,5 8-1085 0 0,231-13 1101 0 0,-146-1-1030 0 0,-64 8-540 0 0,34-1-45 0 0,11-13 803 0 0,-40-21-1236 0 0,-127 29-64 0 0,-4 2-273 0 0,20-11-2694 0 0,-18 11 2502 0 0,6 0-15 0 0,-3 5-3511 0 0,-2 1-4432 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="5">12221 2484 8288 0 0,'0'0'638'0'0,"-1"1"-414"0"0,-1 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,6 6 488 0 0,57 15 2067 0 0,-34-13-2223 0 0,43 21 954 0 0,-46-9-1577 0 0,36 39 370 0 0,-15 1-375 0 0,25 32 240 0 0,-69-89-712 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 2-23 0 0,-2 3 44 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1-1 0 0 0,1 0-44 0 0,-23 11 59 0 0,0-3-1 0 0,0 0 1 0 0,-1-2 0 0 0,0-3-1 0 0,0-1 1 0 0,-15 0-59 0 0,25-5-59 0 0,-63-10-1395 0 0,76 4-1171 0 0,8 5 1267 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="6">13160 2603 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-10 7 790 0 0,-11 10 150 0 0,-42 21 1099 0 0,5-4-1196 0 0,56-32-1165 0 0,-12 9 158 0 0,1 0 0 0 0,0 1-1 0 0,1 1 1 0 0,0 1 0 0 0,1-1 0 0 0,0 2 0 0 0,1 0 0 0 0,0 1-1 0 0,-5 11-202 0 0,13-22 65 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1-1 0 0,1 1 1 0 0,1-1-1 0 0,-1 2 1 0 0,1-1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1-64 0 0,1 2 108 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,0-1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,8 2-107 0 0,-4-1 42 0 0,-1-2-1 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 0 0 0,6-3-41 0 0,20-17-4007 0 0,-30 14-3607 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="7">13318 2943 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-4-9 655 0 0,4 3-930 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,2-1-345 0 0,-4 2 74 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-2 0 0 0,0 2 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0-1 0 0,1 2 1 0 0,1-2 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 2-73 0 0,1 5 95 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 9-95 0 0,-11 70 1049 0 0,11-81-938 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-111 0 0,2-3 23 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,2-1 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,1 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,-1-1-24 0 0,-1-1-63 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,3 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0-5 63 0 0,5-23-2404 0 0,-2 17 1056 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8">13746 2617 0 0 0,'-3'-6'-1709'0'0,"1"-5"9298"0"0,3 9 1867 0 0,-1 14-7849 0 0,4 100 2619 0 0,-7-23-3124 0 0,6 9 60 0 0,-7 39-1060 0 0,12-67-102 0 0,-6-64-68 0 0,-1-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="9">13727 2835 2304 0 0,'0'0'464'0'0,"4"-8"3648"0"0,-4 5 1786 0 0,25-41-750 0 0,9 4-2447 0 0,4 12-1313 0 0,-20 32-788 0 0,-16-4-482 0 0,-1 1-42 0 0,3 2-30 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 2-1 0 0,0-2 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-2 0 1 0 0,2 0-1 0 0,-1 1-46 0 0,19 88 1079 0 0,-11-66-711 0 0,-8-14-53 0 0,16 64 642 0 0,0-36-721 0 0,10-30-183 0 0,33-40-1154 0 0,-25-3-4448 0 0,-26 23 3543 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="10">14370 2437 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,7 2 583 0 0,-5-7-849 0 0,-2 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 17-2962 0 0,1 58 539 0 0,-5 69 472 0 0,-5 14 1084 0 0,7 78-784 0 0,9-190-592 0 0,1-26-84 0 0,11-17 3 0 0,-13-9-156 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1-3-35 0 0,42-41 80 0 0,-36 36-172 0 0,-7 8-92 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-3 184 0 0,1 0-1288 0 0,2-8-6336 0 0,-6 10 565 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="11">14374 2658 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,52-5 2910 0 0,-37 4-3513 0 0,5 0-489 0 0,-8 4-4783 0 0,-4 1-1037 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="12">14802 2682 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,4 5 4769 0 0,-1 0-4077 0 0,0-1-1648 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 3-394 0 0,-5 181 4855 0 0,0-66-3199 0 0,1-93-1224 0 0,5-9-3265 0 0,-1-14 1400 0 0,0-7-5540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="13">14834 2916 456 0 0,'2'-11'295'0'0,"-1"9"1230"0"0,5-14 4652 0 0,-6 15-4821 0 0,8-16 3233 0 0,-3 7-3731 0 0,17-34 2412 0 0,-21 42-3133 0 0,0-2-1 0 0,1 1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,2 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-137 0 0,33 1 1322 0 0,-33 1-1262 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 3-59 0 0,19 18 91 0 0,-7 1-240 0 0,-14-24-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="14">15243 2980 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,0-1 0 0 0,1-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,3-4-329 0 0,9-25 1366 0 0,18-4-185 0 0,-29 35-1119 0 0,-1 1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,2 2-62 0 0,38 64 531 0 0,-37-53-291 0 0,0-1-1 0 0,-2 1 1 0 0,2 1 0 0 0,-3 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,-2 10-239 0 0,-6 41 0 0 0,-10-24 1095 0 0,0-44-406 0 0,12 1-606 0 0,1 1-72 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,2 0 1 0 0,0 0 0 0 0,-3-2-11 0 0,2 0-209 0 0,0 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-6 209 0 0,0-20-4042 0 0,2 16-3529 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="15">15669 2358 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,3 8 590 0 0,9 66 2596 0 0,-17 147-2669 0 0,-2-75 14 0 0,7 85-1117 0 0,3-180 0 0 0,0-46-165 0 0,-2-4-698 0 0,-1-1-315 0 0,0-1-1352 0 0,3-5-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="16">15919 2893 3568 0 0,'18'-11'1553'0'0,"-5"-5"1718"0"0,-2 11-2487 0 0,35-32 3450 0 0,-22 9-3218 0 0,30-43-474 0 0,-45 48-542 0 0,-6 15 0 0 0,-6-1 0 0 0,2 6-7 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,-4 0 6 0 0,0 2 11 0 0,-1-1 1 0 0,1 2-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-3 5-12 0 0,-13 25 272 0 0,-5 55 161 0 0,24-85-291 0 0,0 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 2 0 0 0,1-2-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-2-1-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,2-1-142 0 0,-1-1 13 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,3 0-13 0 0,56-24-2033 0 0,-51 16 586 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="17">16312 2610 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-1 1-172 0 0,-13 53 5027 0 0,7-27-3083 0 0,-6 32 478 0 0,11-49-2198 0 0,0 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,0 5-320 0 0,1 26 797 0 0,-2-36-713 0 0,1-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,3 3-83 0 0,-5-7 16 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-2 0 0 0 0,2 1 1 0 0,-1-1-1 0 0,0-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0-2-15 0 0,6-4 20 0 0,16-33 87 0 0,10-39-97 0 0,-30 73-49 0 0,1 0 0 0 0,-2 0-1 0 0,1-2 1 0 0,-1 2 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-6 39 0 0,-3-22-1383 0 0,3 36 837 0 0,-1 0-1200 0 0,-5-5-4721 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="18">15169 2437 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,1-1-292 0 0,5-4-365 0 0,1-2-1 0 0,-1 1 1 0 0,-1-1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-2-363 0 0,41-75 852 0 0,-32 68-781 0 0,-2 15-61 0 0,-8 6 2 0 0,-2 0 0 0 0,2 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 2-11 0 0,1 2-4 0 0,6 26 57 0 0,2-5-53 0 0,4 0-1856 0 0,-8-23-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="19">7370 2668 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-10-2-24 0 0,6 2 8851 0 0,2 5-9133 0 0,-8 15-17 0 0,6-17-769 0 0,3-2-3236 0 0,1-1-1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="20">18030 2977 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-6 0-423 0 0,1-2-329 0 0,3 2-272 0 0,0-3-398 0 0,0-1-3749 0 0,-2-9 2451 0 0,3 11-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="21">17794 2702 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-12-3 2088 0 0,-5-4-821 0 0,17 7-1285 0 0,-13 3 543 0 0,-28 27 578 0 0,-3 49-1009 0 0,43-70-646 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1-74 0 0,21 24 398 0 0,-24-30-397 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,0-1-1 0 0,8 1-134 0 0,-8-1-167 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-2-1 0 0,0 1 1 0 0,-1 0 301 0 0,-3 2-105 0 0,12-9-1239 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="22">18209 2743 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,5 8 1656 0 0,-4-5-2461 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 1-229 0 0,1 73 2716 0 0,15 160 1049 0 0,-24-73-3749 0 0,-1-93-16 0 0,-1 20 0 0 0,10-87-64 0 0,1-3-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="23">18234 2818 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,4-7 616 0 0,18-28 2026 0 0,-4 18-2035 0 0,-16 16-1214 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,1-1 0 0 0,-2 2 0 0 0,2-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-84 0 0,2 5 138 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,-1 6-137 0 0,3-12 22 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-2 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0-21 0 0,-30 9 162 0 0,29-10-192 0 0,2 0 1 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,2-1-1 0 0,-4-2 30 0 0,-13-30-3512 0 0,16 21 1769 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="24">18629 2559 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="25">18612 2535 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="26">18600 2641 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="27">18572 2448 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,4 11 2392 0 0,11 80 1583 0 0,-15 34-1639 0 0,9 45-192 0 0,10-22-2656 0 0,-21-130 0 0 0,-2-3-337 0 0,3-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="28">18603 2871 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-1-17 3737 0 0,3-5 4077 0 0,7-20-4186 0 0,7 0-1366 0 0,-1 21-2142 0 0,-8 18-211 0 0,-7 8 222 0 0,17-9 1281 0 0,7 11-1444 0 0,-21 1-105 0 0,38 32-8 0 0,-19-4 744 0 0,-10-2-56 0 0,7 33-96 0 0,-13-20-16 0 0,4 13 191 0 0,-1-20-526 0 0,-1-3-59 0 0,-1-16-12 0 0,-5-14-90 0 0,13 3 16 0 0,16-2-96 0 0,-6-4-141 0 0,-25 2-596 0 0,25-10-4249 0 0,-14 3 1073 0 0,-6 3 1923 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="29">19111 2668 1376 0 0,'-14'6'65'0'0,"12"-5"277"0"0,2-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-5 12 5285 0 0,10 44-3424 0 0,-9-9-2068 0 0,1 48 541 0 0,-5-53-877 0 0,4 2-432 0 0,5 23-1088 0 0,8 8 915 0 0,-5-3-416 0 0,-3-60-545 0 0,-1 19 164 0 0,-5-12-45 0 0,5-18-557 0 0,0-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-5 0-797 0 0,4 0-5332 0 0,1 0 728 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="30">19073 2718 456 0 0,'28'-10'12581'0'0,"-19"4"-11549"0"0,16 5 3076 0 0,-4-5-1928 0 0,26 39 262 0 0,-16 2-1426 0 0,-9 17-48 0 0,-8-18-336 0 0,-13-30-440 0 0,-4 28-53 0 0,-6-11-60 0 0,-6-7 791 0 0,14-12-867 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-2 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1-3 0 0,-31-21-1713 0 0,11-2-2008 0 0,20 16 1827 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="31">16653 2634 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,2 14 1120 0 0,1 37 395 0 0,0 69 75 0 0,4-40-2940 0 0,3 8-252 0 0,-4-14-192 0 0,1-37-12 0 0,-7-35-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="32">16665 2796 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,4-14 2209 0 0,9-3-1077 0 0,27-23 345 0 0,-16 33-1146 0 0,-4 21-314 0 0,-16-11-177 0 0,0 2 0 0 0,0-1-1 0 0,-1 1 1 0 0,2-1 0 0 0,-2 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-37 0 0,-1-4 176 0 0,7 12 413 0 0,-7-13-998 0 0,9 6-4069 0 0,-10-7 3075 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="33">16939 3100 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,5-4 224 0 0,-3 3 3136 0 0,8-10-3493 0 0,-8 8-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="37">17276 2743 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 13 8138 0 0,-3 35-5693 0 0,3-50-1919 0 0,-3 17 1214 0 0,0 78 988 0 0,3-95-2320 0 0,0-2-72 0 0,0 7 75 0 0,-3 27-43 0 0,-3 44-122 0 0,6-75-45 0 0,0 1-235 0 0,0-1-3512 0 0,0-3-1706 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="38">17264 2886 5296 0 0,'3'7'472'0'0,"-3"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-23 1372 0 0,0 21-1542 0 0,0 0-40 0 0,5-28 954 0 0,-4 29-1144 0 0,11-28 1755 0 0,3 10-1413 0 0,-14 18-538 0 0,-1 1 0 0 0,0 0-6 0 0,13-2 374 0 0,-7 3-368 0 0,-5-1-159 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-2 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 2 0 0 0,0-2-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 1-24 0 0,13 60 908 0 0,-10-26-544 0 0,-4-13-78 0 0,1-22-204 0 0,0 22 170 0 0,1-20-204 0 0,2 5-36 0 0,0 0-1 0 0,0 0 42 0 0,3-4 13 0 0,-3-3-58 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,3-3-9 0 0,28-23-3222 0 0,-28 22-430 0 0,-3 5 1775 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-14T20:45:26.850"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">76 216 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0 0 240 0 0,0 0 43 0 0,0 0-73 0 0,0 0-345 0 0,0 0-150 0 0,0 0-28 0 0,0 0 21 0 0,0 0 115 0 0,7 3 1247 0 0,-5-2-1608 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-193 0 0,4 18 1030 0 0,-3-19-673 0 0,-5 5 279 0 0,-3 67 1076 0 0,-4 32-280 0 0,7-28-400 0 0,-11 43 496 0 0,-3 45-1568 0 0,14-85 184 0 0,7 2-144 0 0,0-21 0 0 0,-3-57 130 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 2-1 0 0,0-2-129 0 0,-10 45-329 0 0,20 5-50 0 0,-8-33-4669 0 0,-8-50-385 0 0,8 12 3507 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1970.78">91 130 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-129 0 0,0 0 200 0 0,0 0 108 0 0,0 0 24 0 0,9 0 2199 0 0,29 0-1100 0 0,-36 0-1400 0 0,-2 0 18 0 0,7-1 404 0 0,107-18 2883 0 0,-15 18-2302 0 0,-36 2-385 0 0,31-30 289 0 0,-78 25-961 0 0,1 0 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 2 1 0 0,0 0 0 0 0,-1 0-1 0 0,12 2-147 0 0,10 4-51 0 0,87 7 245 0 0,-76-12 432 0 0,30 0 101 0 0,-2 11-519 0 0,29-2-51 0 0,5-14 91 0 0,1-20 123 0 0,73-3 48 0 0,8 22-113 0 0,12-19 369 0 0,-127 16-555 0 0,-5 6-351 0 0,-21 6 134 0 0,87 14 97 0 0,-54-6 53 0 0,9-22 230 0 0,-22 11-283 0 0,36 5 0 0 0,0 25-96 0 0,-64-21 96 0 0,47 8 16 0 0,-23-9-16 0 0,15 1 64 0 0,35 16-48 0 0,21 8-16 0 0,-80-26-96 0 0,118-13 96 0 0,-23 18 53 0 0,-71-8-42 0 0,49-4-11 0 0,-9-7-19 0 0,-117 7 21 0 0,33-1 0 0 0,0 2 1 0 0,0 2-1 0 0,-1 1 0 0 0,35 9-2 0 0,-60-11-4 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-2 1 0 0,1 0 0 0 0,-1-3-1 0 0,0 2 1 0 0,3-2 4 0 0,52-3-32 0 0,15 2 19 0 0,8 4 93 0 0,-16 4-80 0 0,29-11 64 0 0,60-3-1144 0 0,-163 10 588 0 0,-1 0-421 0 0,0 0-189 0 0,0 0-1663 0 0,0 0-6530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2876.335">5022 167 11488 0 0,'0'0'528'0'0,"0"0"-16"0"0,0 1-326 0 0,-10 30 3021 0 0,8 61 849 0 0,-27 143 1534 0 0,21-140-5590 0 0,4 56 1815 0 0,-11-5-1045 0 0,8-51 113 0 0,3-44-550 0 0,-3-4-190 0 0,10-29-15 0 0,-3-2-205 0 0,1-13 119 0 0,-5 37-31 0 0,3-30-11 0 0,-2-1 11 0 0,3-7-103 0 0,0-2-600 0 0,0 0-268 0 0,0 0-1097 0 0,0 0-4403 0 0,0 0-1889 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4565.136">0 1294 5528 0 0,'0'0'422'0'0,"0"0"-34"0"0,0 0 887 0 0,0 0 416 0 0,0 0 79 0 0,0 17 2778 0 0,3 7-429 0 0,13-18-2249 0 0,48-19-14 0 0,31 6 228 0 0,-39 11-2068 0 0,13 12 56 0 0,24 13 1888 0 0,-21-1-1944 0 0,39-6-16 0 0,-40-14 0 0 0,57 11 0 0 0,-43-4 0 0 0,179 7 952 0 0,-249-23-877 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,0-1-1 0 0,0-1 0 0 0,7-4-75 0 0,66-14 289 0 0,19 9-114 0 0,0 5-1 0 0,48 5-174 0 0,-109 1 103 0 0,57 7-95 0 0,-20 24-140 0 0,230-11 1020 0 0,-60-14-517 0 0,-124-2-155 0 0,166 4 61 0 0,-79-14 534 0 0,28 1-910 0 0,-109 1 187 0 0,51 0 104 0 0,-100 5-192 0 0,0 3 0 0 0,24 7 0 0 0,42-22 256 0 0,-12 4-200 0 0,-12 9-123 0 0,-60-8-10 0 0,5 3 88 0 0,9 12 122 0 0,-36-11-133 0 0,-12 10 0 0 0,-12-13 0 0 0,16-6 0 0 0,4-3 0 0 0,-7 4-113 0 0,-27 10 27 0 0,-5 1 12 0 0,-2 2-5 0 0,26-7-753 0 0,-20 7 648 0 0,11-1 96 0 0,-9 3 88 0 0,3 8-17 0 0,-11-8-67 0 0,-1-2-6 0 0,0 0 9 0 0,0 0-139 0 0,0 0-588 0 0,0 0-257 0 0,0 0-1738 0 0,0 0-6757 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-14T20:38:25.554"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+    <inkml:brush xml:id="br1">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">213 659 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="310.099">552 676 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-2-9 10039 0 0,3 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="684.255">894 617 11976 0 0,'-1'5'296'0'0,"-4"5"4551"0"0,3-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1921.293">1194 700 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,1-6-6507 0 0,4-23-839 0 0,-6 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-12 79 971 0 0,11-78-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,2-28 325 0 0,-6 43 218 0 0,0 1 13 0 0,6-5-260 0 0,-1 9-230 0 0,-3 1 347 0 0,-11 35 365 0 0,8-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-9-12-214 0 0,18-43 40 0 0,0 48 757 0 0,-7 6-562 0 0,-2 1-34 0 0,12 15 96 0 0,-21 51 294 0 0,9-64 48 0 0,0-2-24 0 0,-10 10 14 0 0,9-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0-12 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,14-18-798 0 0,-5 23 705 0 0,10 17 39 0 0,-18-13 64 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 2-10 0 0,1-5 84 0 0,-5 17 237 0 0,-16-9-89 0 0,20-9-144 0 0,1 0 0 0 0,-6-10-1050 0 0,3-10-3857 0 0,2 11-3207 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8390.611">1448 417 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,7 57 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,2 17 113 0 0,-3-14-1404 0 0,0 51 981 0 0,-4-2-1688 0 0,1-59-1417 0 0,-2-32 962 0 0,-6-28-2248 0 0,3-5-5035 0 0,5-10 5419 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8997.239">1393 552 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,11-32 2722 0 0,-12 31-3180 0 0,13-15 1008 0 0,20-24 674 0 0,-31 36-2057 0 0,2 2 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,2-1 1 0 0,-2 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1-137 0 0,58 19 1009 0 0,-45 14 55 0 0,-4-18-600 0 0,19 47 1448 0 0,-20 2-2113 0 0,-13-61 230 0 0,0 1 0 0 0,-1-2 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-2 1-29 0 0,3-3 5 0 0,-8 22 399 0 0,1-11-337 0 0,7-8-104 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,-1 1 37 0 0,-29-1 653 0 0,-7-25-4978 0 0,29 19 2334 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11709.08">2594 382 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,3 48 1154 0 0,-10 24 2052 0 0,-2 33 1755 0 0,2 52-2463 0 0,3-54-962 0 0,-2 32-1172 0 0,6-140-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-2 13-2556 0 0,1-23 1622 0 0,1-1-894 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12315.019">2609 440 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,11-7 8 0 0,2-4 772 0 0,-12 10-801 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-250 0 0,8 4 395 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-2 1 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 1 1 0 0,4 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 2-1 0 0,-1-2 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,0 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,2 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 2-79 0 0,-1 0 4 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-3-1-4 0 0,-47-44-4198 0 0,48 42-3651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10346.212">1924 78 3680 0 0,'-5'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,7 16-23 0 0,3-13-297 0 0,4 3-1604 0 0,-8 95 2 0 0,7-77 200 0 0,0-18-716 0 0,3-41-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10997.838">1859 649 1376 0 0,'4'-20'2159'0'0,"3"0"4223"0"0,5-6-3735 0 0,-3 5-1523 0 0,11-15 1153 0 0,3 11 523 0 0,-3 3-1591 0 0,19-17 135 0 0,-38 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 1-1 0 0,2-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 1 0 0,1 1-51 0 0,2 3 27 0 0,2 1 1 0 0,-2 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,-2 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 7-27 0 0,8 30 368 0 0,26 120 1443 0 0,-18-124-1634 0 0,1-14-84 0 0,-12-24-77 0 0,-4-1-29 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,1 2 0 0 0,-2-2 0 0 0,1-2 0 0 0,-1 2-1 0 0,1 0 1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 13 0 0,34-28-350 0 0,16-12-3834 0 0,-46 36 2533 0 0,3 3-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32289.342">1 256 6448 0 0,'6'21'6309'0'0,"-6"-18"-6682"0"0,4 54 3514 0 0,6 85-847 0 0,-1-44-690 0 0,-5-10-929 0 0,11 131 737 0 0,-24 34 57 0 0,5-177-1337 0 0,-2-48-256 0 0,6-13-955 0 0,0-12-4480 0 0,0-3-582 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35199.426">11 287 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,15-38 6274 0 0,-15 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,10-3 291 0 0,62-18 828 0 0,-33 5-729 0 0,11-5 96 0 0,43 12 370 0 0,-52 8-222 0 0,36 2-1079 0 0,-18-6 16 0 0,32-20 451 0 0,-26 15 1144 0 0,53 1-1448 0 0,3 19 224 0 0,-46-19-645 0 0,-26-1 1538 0 0,6 0-1123 0 0,-32 8-292 0 0,45 0 264 0 0,-22-6 20 0 0,48-26 70 0 0,8 18-205 0 0,11 9 34 0 0,-57-4 219 0 0,20-5-424 0 0,-5 12 192 0 0,-8 5 584 0 0,37 1-1352 0 0,-6 9 736 0 0,2 6 1017 0 0,-29-10-298 0 0,-10 0-1239 0 0,23-4 520 0 0,12 3 64 0 0,11 29 75 0 0,-53-11-166 0 0,14 1 523 0 0,-4-9-840 0 0,-18-6 749 0 0,-6-3-675 0 0,21 6 487 0 0,63-10-197 0 0,-18 21 0 0 0,-35-16-20 0 0,-39-2 0 0 0,-10-5 0 0 0,21 17 0 0 0,-33-3 0 0 0,4 6 0 0 0,12 23 64 0 0,-5 28 0 0 0,-7 23-64 0 0,-3 31-8 0 0,-1-49 125 0 0,-2 31-203 0 0,-8 34 295 0 0,8 44-190 0 0,-15-84 82 0 0,-1-41-13 0 0,5-44 96 0 0,5-13-234 0 0,0 2-1 0 0,0-2 1 0 0,1 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,-2 1 51 0 0,1-2 114 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 0-114 0 0,-12 0 158 0 0,-84 8-218 0 0,70-3 59 0 0,-1-1-1 0 0,1-2 1 0 0,0-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-19-6 1 0 0,3-4-9 0 0,-1 3 0 0 0,1 3 0 0 0,-1 2 0 0 0,-18 2 9 0 0,-97 0 332 0 0,120 4-330 0 0,0-1-1 0 0,-1-3 1 0 0,1-2-1 0 0,0-1 1 0 0,-7-7-2 0 0,19 9-18 0 0,0 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-18 4 18 0 0,-123 30 64 0 0,-3-12-136 0 0,-41-9 152 0 0,149-13-80 0 0,-80 0 11 0 0,-29-17 42 0 0,88 17-53 0 0,-20-13 80 0 0,19-11-176 0 0,-74-18 224 0 0,50 21-196 0 0,53 8 192 0 0,-53-4-124 0 0,43 11 0 0 0,40 13-499 0 0,28-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="78758.085">3259 863 13560 0 0,'0'0'306'0'0,"-11"-2"752"0"0,-20-5-12 0 0,30 7-11 0 0,-6-6 1119 0 0,7 5 2052 0 0,56 4-3188 0 0,26-6 262 0 0,139 30 512 0 0,-118-20-1336 0 0,134 27-663 0 0,-43 7 353 0 0,-4-7 891 0 0,-108-31-445 0 0,-66-3-541 0 0,0-1 0 0 0,0 0 0 0 0,0-2 1 0 0,0 0-1 0 0,0-1 0 0 0,8-4-51 0 0,63-36-278 0 0,-85 43 89 0 0,-2 1-156 0 0,3 0-611 0 0,-1 1-1432 0 0,-1-2-4991 0 0,-1 1-504 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="79175.854">4641 574 6448 0 0,'0'0'498'0'0,"1"-1"-28"0"0,26-3 10100 0 0,20 23-6654 0 0,-28-10-3356 0 0,1 1 0 0 0,-1 2 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,4 8-560 0 0,52 53 264 0 0,-67-64-125 0 0,-1 1-1 0 0,0 1 1 0 0,0 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 1 1 0 0,2 11-139 0 0,-5-12 187 0 0,0 0 1 0 0,0 2-1 0 0,0-2 1 0 0,-2 1-1 0 0,0-1 1 0 0,0 2 0 0 0,0-2-1 0 0,-2 1 1 0 0,1-1-1 0 0,-2 2 1 0 0,1-2-1 0 0,-1 0 1 0 0,0 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,-4 6-188 0 0,-21 30 165 0 0,-29-8 587 0 0,-77-23 352 0 0,107-18-1542 0 0,-19 5-2761 0 0,40 0 2491 0 0,-24 12-2399 0 0,14-3-3298 0 0,4 0-1217 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37346.914">5792 851 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,2 2 218 0 0,1-1 5134 0 0,18-14-8855 0 0,-14 9 1888 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37618.204">6115 895 10592 0 0,'-11'-13'818'0'0,"8"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,11-3-8082 0 0,-4 4-1569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37903.659">6415 805 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,4 0-232 0 0,-1 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38875.93">6729 895 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-38 1231 0 0,1 45-2463 0 0,-1 1 0 0 0,2 1 52 0 0,-4 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,6 8 88 0 0,-5-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,0 3-113 0 0,2-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-7-17 194 0 0,21-16-143 0 0,-11 33-62 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 11 0 0,1-1-43 0 0,2 1 32 0 0,1 10 23 0 0,-9 18 200 0 0,3-27-96 0 0,-6 4-695 0 0,12-7-611 0 0,7-10-5710 0 0,-6 6 446 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="44618.988">6973 526 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,9 21-45 0 0,-10-24-3788 0 0,2 9 1039 0 0,3 82 1637 0 0,6 83-1221 0 0,-12-86-1606 0 0,0-80-341 0 0,-1-2-56 0 0,0-6-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53832.509">7233 567 2760 0 0,'3'8'1828'0'0,"4"20"4892"0"0,4 25-3444 0 0,2 103 1947 0 0,-11-80-3937 0 0,-4-37-4508 0 0,2-36 1701 0 0,-4 5-229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54557.219">7279 895 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,7-39 5734 0 0,4-11-521 0 0,-15 20-3279 0 0,10 10-1202 0 0,7-37 1 0 0,-12 56-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-2 2 0 0 0,2-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,3 0-93 0 0,1-2 95 0 0,-4 3-21 0 0,23 0-60 0 0,1 14-14 0 0,-4 7 0 0 0,-18-12 0 0 0,9 23 0 0 0,17 74 514 0 0,-17-52 356 0 0,5-19-278 0 0,-17-34-517 0 0,5 3 98 0 0,-3-2-141 0 0,0-1 0 0 0,-1 2-1 0 0,1-2 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,2-1 0 0 0,-1 1-1 0 0,-1-1 1 0 0,2 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-32 0 0,21-4-185 0 0,-5-27-4233 0 0,-19 31 2840 0 0,0 1-164 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56701.452">7958 623 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-9-2-143 0 0,-34-6 1747 0 0,36 9-1667 0 0,5-2 170 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0-107 0 0,-30 42-483 0 0,15 1 618 0 0,15 14 378 0 0,8 3-513 0 0,13-4 1899 0 0,22-11-1734 0 0,-10-18-165 0 0,-16-20 0 0 0,13 2 0 0 0,-20-10 0 0 0,-1 2 0 0 0,0-5-64 0 0,26-22-5497 0 0,-27 16 3530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57367.528">8186 956 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,10-17 649 0 0,-7 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,8 19 784 0 0,-13 15 56 0 0,5-33-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="64361.857">8421 615 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,6 17 886 0 0,4 73 1352 0 0,-4-54-2105 0 0,-8 63 686 0 0,-1-6-314 0 0,2 68-530 0 0,5-113-273 0 0,-2-10 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-2-14-1557 0 0,1-2 195 0 0,-2 0-70 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="69762.645">8391 617 1376 0 0,'4'7'367'0'0,"-4"-6"1002"0"0,0-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,8-7 51 0 0,28-23 1588 0 0,-24 24-1245 0 0,-11 4-294 0 0,1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 1-100 0 0,2 2 108 0 0,1 1-1 0 0,-1 0 0 0 0,0-1 0 0 0,-1 2 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,0 2 0 0 0,1-2 1 0 0,0 6-108 0 0,7 27 435 0 0,1 58 787 0 0,-10-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-56 0 0,-38 35 929 0 0,38-35-879 0 0,0-1-45 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0 0 0 0,0-1-1 0 0,1 2 1 0 0,0-1 0 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 1-5 0 0,-2-1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-2-3 0 0 0,4-16-5381 0 0,0 15-2125 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70961.788">8802 348 0 0 0,'-10'13'0'0'0,"5"-16"140"0"0,3 3 2586 0 0,2 0 5496 0 0,13 20-7158 0 0,-12-19-552 0 0,6 30 3000 0 0,-11 31-1947 0 0,1 50 181 0 0,3 1 624 0 0,-6-41-881 0 0,9 38-1316 0 0,-10-26-173 0 0,7-43 0 0 0,12 2-2476 0 0,-10-39 2128 0 0,-2-3 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,0-1-2221 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="71766.961">8787 778 4376 0 0,'0'0'199'0'0,"8"-10"1918"0"0,-4-3 1016 0 0,9-10 683 0 0,-6-13-1297 0 0,-1-1-472 0 0,5 29-1272 0 0,-9 7-743 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,1 1-33 0 0,5 0 304 0 0,18 22 598 0 0,-22-17-674 0 0,2 0-1 0 0,-2 0 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,1 6-227 0 0,6 92 608 0 0,-7-65-165 0 0,0-12 997 0 0,23-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,10-10-60 0 0,-16 1-2985 0 0,-15 8-1180 0 0,-6 1 2595 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73476.329">9328 652 2760 0 0,'0'1'207'0'0,"0"45"6763"0"0,0-45-5925 0 0,0-1-21 0 0,2 8 598 0 0,1 13-344 0 0,-1 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 9-1278 0 0,-10 63 616 0 0,0-18 973 0 0,12 39-2158 0 0,1-87 962 0 0,-1-26-377 0 0,1-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="74025.376">9383 645 3224 0 0,'-1'-5'1144'0'0,"3"-6"9068"0"0,-1 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,49-25 1867 0 0,-47 27-2559 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-2 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,2 2-156 0 0,-1-1 96 0 0,2 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1-95 0 0,-1-1 94 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,-3 5-94 0 0,-37 57 1952 0 0,40-65-2012 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0-2 0 0 0,0 2 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-7-6-2618 0 0,5-2 1170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128695.154">5097 1481 4144 0 0,'0'0'319'0'0,"-6"7"1871"0"0,2-2 3495 0 0,-24-2-688 0 0,1-4-2621 0 0,2-15 488 0 0,-15 7-1852 0 0,-6-1 1272 0 0,-22-14-812 0 0,3 4-939 0 0,0 3 998 0 0,-4 0-1171 0 0,-8 11-360 0 0,-100 12 1824 0 0,95 7-1887 0 0,33-8 230 0 0,-29-9-256 0 0,7-6 82 0 0,12 7 87 0 0,20 3-80 0 0,-65-14 0 0 0,44-2 0 0 0,-7 7 0 0 0,43 2 0 0 0,11 5-60 0 0,9 2-440 0 0,5 5-11674 0 0,-1-4 3997 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129337.391">3822 1149 8288 0 0,'0'2'227'0'0,"-1"-1"0"0"0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,0 1-227 0 0,-17 1 2894 0 0,12 2-2512 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 2 0 0 0,-5 4-381 0 0,-3 3 422 0 0,-13 14 408 0 0,-33 33 222 0 0,15-4-867 0 0,42-32 92 0 0,1-22-266 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 2-1 0 0,0-2 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2-1-1 0 0,2 1 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-11 0 0,22 11 26 0 0,84 21-304 0 0,-43-10-3852 0 0,-17 7-1623 0 0,-34-16 3707 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="133691.162">5216 3772 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-8 0 710 0 0,-60 11 2232 0 0,-88-9 113 0 0,65-16-2111 0 0,87 12-1711 0 0,0 0 0 0 0,1 1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-1 0 0,-2-1 1 0 0,2 1 0 0 0,-2 0-1 0 0,1 0-7 0 0,0 0 3 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 0 0 0 0,-4-1-3 0 0,-3-1 53 0 0,-49 15 746 0 0,-4-32-422 0 0,-40 19 95 0 0,19 18-267 0 0,-4-27 255 0 0,18 6-262 0 0,-6-5 515 0 0,21 24-785 0 0,-6-11 316 0 0,61-3-237 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,1 0 0 0 0,-1 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,0 5-384 0 0,1 0-2483 0 0,-1-5 1589 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="134078.302">4145 3509 12384 0 0,'-12'-11'1277'0'0,"-1"9"-438"0"0,-13 9 3998 0 0,7 3-3431 0 0,-19 15 690 0 0,-43 36-1014 0 0,22-27 402 0 0,6 19-1322 0 0,29-26-154 0 0,-8 16 872 0 0,30-40-855 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1-2-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-2-1 0 0,2 3-23 0 0,31 39 389 0 0,-23-35-394 0 0,-1-1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 0 0 0,0-2 1 0 0,1 1-1 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,0-1-1 0 0,5 0 4 0 0,-5 0-173 0 0,90 18-1371 0 0,-36 3-4118 0 0,-51-16-1845 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136187.119">3415 2857 2760 0 0,'8'14'125'0'0,"-20"-6"1798"0"0,-6 8-59 0 0,14-9 428 0 0,-22 6 4862 0 0,26-13-6578 0 0,0 0-15 0 0,0 0-34 0 0,-1 2 119 0 0,0-1-159 0 0,1-1 2989 0 0,48-16-1901 0 0,10 9-396 0 0,18 3-749 0 0,-19 1 156 0 0,35-1 469 0 0,19-4-497 0 0,-4-4-454 0 0,48-2 952 0 0,-45 8-543 0 0,-44-4-402 0 0,45-10 402 0 0,-59 9-745 0 0,3 11 112 0 0,-29-6 120 0 0,13 4 0 0 0,6-13 444 0 0,-21 4-280 0 0,11-1-164 0 0,-21 4 0 0 0,-5 7 0 0 0,16 7-1208 0 0,-24-5 877 0 0,6 3-1583 0 0,6 13-3659 0 0,-7-11 3847 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136591.973">4726 2399 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,8 22 9129 0 0,20-4-7935 0 0,-15-13-2328 0 0,53 29 1337 0 0,-52-22-2420 0 0,-6-7 346 0 0,1 1 1 0 0,0 0-1 0 0,-1 1 1 0 0,-1 0-1 0 0,0 2 1 0 0,1-1-1 0 0,-2 0 1 0 0,1 1-1 0 0,3 8-255 0 0,7 68 1080 0 0,-24-5-224 0 0,-10-30-856 0 0,-24 0 327 0 0,-25-11 1242 0 0,7-15-2553 0 0,34-24-3117 0 0,21-1 2058 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="139663.33">10436 2918 8288 0 0,'10'-47'864'0'0,"-12"44"-720"0"0,4-9 1811 0 0,-1 9 5703 0 0,56-2-3242 0 0,-23 5-4222 0 0,70 2 1838 0 0,4 8-1085 0 0,240-13 1101 0 0,-152-1-1030 0 0,-65 8-540 0 0,35-1-45 0 0,10-13 803 0 0,-40-22-1236 0 0,-131 30-64 0 0,-5 2-273 0 0,20-10-2694 0 0,-18 10 2502 0 0,7 0-15 0 0,-5 4-3511 0 0,0 2-4432 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="140326.574">11985 2481 8288 0 0,'0'0'638'0'0,"0"1"-414"0"0,-2 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,6 6 488 0 0,60 16 2067 0 0,-37-15-2223 0 0,45 22 954 0 0,-47-8-1577 0 0,38 38 370 0 0,-16 1-375 0 0,25 33 240 0 0,-71-90-712 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1-23 0 0,-4 4 44 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-2 1 0 0,0 1-1 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1-1 0 0 0,0 0-44 0 0,-23 11 59 0 0,0-3-1 0 0,0 0 1 0 0,-1-2 0 0 0,0-3-1 0 0,0-1 1 0 0,-16 0-59 0 0,27-5-59 0 0,-66-10-1395 0 0,78 4-1171 0 0,9 5 1267 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151416.768">12958 2600 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-11 8 790 0 0,-11 9 150 0 0,-43 21 1099 0 0,5-4-1196 0 0,58-32-1165 0 0,-12 9 158 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,1 2 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-6 13-202 0 0,14-23 65 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1-64 0 0,0 1 108 0 0,2 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0-1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-2 0 0 0,-1 0-1 0 0,8 2-107 0 0,-3-2 42 0 0,-2-1-1 0 0,1-1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 0 0 0,7-2-41 0 0,20-19-4007 0 0,-31 15-3607 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="152065.555">13120 2943 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-3-9 655 0 0,3 2-930 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-2 0 0 0,-1 2 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,2-2-345 0 0,-3 3 74 0 0,-1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,0-1 1 0 0,-2 1 0 0 0,2 1-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,1 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 2-73 0 0,1 5 95 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 10-95 0 0,-11 69 1049 0 0,10-82-938 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-2-111 0 0,2-3 23 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,-2-1-24 0 0,1-2-63 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-2-1-1 0 0,2 1 1 0 0,-2-1-1 0 0,2 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1-2-1 0 0,1 2 1 0 0,-1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-2-1 0 0,0-4 63 0 0,6-22-2404 0 0,-4 15 1056 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153048.506">13564 2615 0 0 0,'-3'-6'-1709'0'0,"1"-6"9298"0"0,3 10 1867 0 0,-1 15-7849 0 0,3 100 2619 0 0,-5-25-3124 0 0,5 11 60 0 0,-7 39-1060 0 0,12-68-102 0 0,-6-64-68 0 0,-1-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153375.191">13544 2834 2304 0 0,'0'0'464'0'0,"4"-8"3648"0"0,-3 5 1786 0 0,24-41-750 0 0,10 3-2447 0 0,4 13-1313 0 0,-20 33-788 0 0,-17-5-482 0 0,0 1-42 0 0,2 2-30 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 2 1 0 0,-1-2-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1-46 0 0,20 88 1079 0 0,-11-66-711 0 0,-10-13-53 0 0,18 63 642 0 0,0-36-721 0 0,10-30-183 0 0,33-40-1154 0 0,-24-3-4448 0 0,-27 23 3543 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160253.303">14210 2434 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,6 2 583 0 0,-3-7-849 0 0,-3 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 17-2962 0 0,1 58 539 0 0,-5 70 472 0 0,-6 14 1084 0 0,8 79-784 0 0,9-192-592 0 0,2-26-84 0 0,10-17 3 0 0,-13-9-156 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,2-4-35 0 0,42-39 80 0 0,-37 34-172 0 0,-7 9-92 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-3 184 0 0,2 0-1288 0 0,0-8-6336 0 0,-5 9 565 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160816.746">14214 2656 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,53-5 2910 0 0,-37 4-3513 0 0,4 0-489 0 0,-7 4-4783 0 0,-4 1-1037 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="165875.957">14657 2680 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,3 5 4769 0 0,1 0-4077 0 0,-2-1-1648 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 3-394 0 0,-5 183 4855 0 0,0-68-3199 0 0,1-92-1224 0 0,5-11-3265 0 0,-1-13 1400 0 0,0-7-5540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="166400.987">14690 2915 456 0 0,'1'-11'295'0'0,"0"9"1230"0"0,5-14 4652 0 0,-5 15-4821 0 0,7-16 3233 0 0,-3 7-3731 0 0,18-35 2412 0 0,-22 43-3133 0 0,0-1-1 0 0,1 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-137 0 0,34 1 1322 0 0,-33 1-1262 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,2 2-59 0 0,18 20 91 0 0,-6 0-240 0 0,-15-24-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167273.982">15113 2979 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,2-3-329 0 0,9-27 1366 0 0,19-4-185 0 0,-30 37-1119 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,2 2-62 0 0,39 65 531 0 0,-38-54-291 0 0,1-1-1 0 0,-3 2 1 0 0,2 0 0 0 0,-2-1-1 0 0,-1 0 1 0 0,0 2 0 0 0,0-2-1 0 0,-2 10-239 0 0,-6 42 0 0 0,-11-26 1095 0 0,1-43-406 0 0,12 1-606 0 0,0 1-72 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,2-1 1 0 0,-1 0 0 0 0,-2-3-11 0 0,2 1-209 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0-2 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-6 209 0 0,0-20-4042 0 0,2 16-3529 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167927.933">15554 2355 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,2 8 590 0 0,11 66 2596 0 0,-19 148-2669 0 0,-1-75 14 0 0,7 85-1117 0 0,4-181 0 0 0,-2-45-165 0 0,-1-5-698 0 0,-1-1-315 0 0,1-1-1352 0 0,2-6-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="189572.02">15812 2892 3568 0 0,'19'-10'1553'0'0,"-6"-7"1718"0"0,-1 12-2487 0 0,35-32 3450 0 0,-22 9-3218 0 0,31-43-474 0 0,-47 47-542 0 0,-6 16 0 0 0,-6-1 0 0 0,2 6-7 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,2 1 1 0 0,-4 0 6 0 0,0 2 11 0 0,-1-1 1 0 0,1 2-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-4 5-12 0 0,-12 25 272 0 0,-6 56 161 0 0,25-86-291 0 0,0 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,1-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,1-1 0 0 0,-2-1-1 0 0,2 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,1-1-142 0 0,-1-1 13 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,3 0-13 0 0,59-24-2033 0 0,-54 16 586 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190134.967">16219 2608 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-1 1-172 0 0,-14 53 5027 0 0,8-27-3083 0 0,-6 32 478 0 0,10-49-2198 0 0,1 2 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 1 0 0 0,1 0 0 0 0,1 5-320 0 0,-1 26 797 0 0,-1-36-713 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 2 1 0 0,-1-2 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,5 3-83 0 0,-6-7 16 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,1-2-15 0 0,5-4 20 0 0,16-33 87 0 0,12-39-97 0 0,-32 73-49 0 0,1 0 0 0 0,-2-1-1 0 0,1 0 1 0 0,0 1 0 0 0,-2-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-6 39 0 0,-4-22-1383 0 0,4 36 837 0 0,-1 0-1200 0 0,-5-5-4721 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192408.343">15036 2434 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,1-1-292 0 0,5-4-365 0 0,1-2-1 0 0,-1 1 1 0 0,0-1 0 0 0,1-1-1 0 0,-2 1 1 0 0,0-2 0 0 0,0 1-1 0 0,-1 0 1 0 0,2-1-363 0 0,42-77 852 0 0,-34 69-781 0 0,-1 15-61 0 0,-10 6 2 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 2-11 0 0,2 2-4 0 0,5 26 57 0 0,2-4-53 0 0,5-1-1856 0 0,-9-23-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="211829.387">6966 2666 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-10-2-24 0 0,7 2 8851 0 0,0 5-9133 0 0,-7 15-17 0 0,5-17-769 0 0,4-2-3236 0 0,1-1-1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-211952.654">17997 2976 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-7 0-423 0 0,2-2-329 0 0,3 2-272 0 0,-1-3-398 0 0,2-1-3749 0 0,-4-8 2451 0 0,4 10-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212149.586">17752 2700 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-12-3 2088 0 0,-5-4-821 0 0,16 7-1285 0 0,-12 3 543 0 0,-30 28 578 0 0,-3 48-1009 0 0,46-71-646 0 0,-2 0 0 0 0,1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 2-74 0 0,22 25 398 0 0,-24-31-397 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,2-1-1 0 0,7 1-134 0 0,-8-1-167 0 0,0 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,2-1 1 0 0,-2 0-1 0 0,1 1 1 0 0,0-2-1 0 0,-1 1 1 0 0,1 0 301 0 0,-4 2-105 0 0,13-10-1239 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205932.193">18182 2741 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,5 8 1656 0 0,-4-5-2461 0 0,1 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2 0 1 0 0,-2 1-1 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 2-229 0 0,2 74 2716 0 0,17 160 1049 0 0,-27-73-3749 0 0,0-93-16 0 0,-2 19 0 0 0,11-86-64 0 0,1-4-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205389.214">18208 2816 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,3-7 616 0 0,20-27 2026 0 0,-4 16-2035 0 0,-17 17-1214 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,0-1-84 0 0,2 5 138 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-2 2 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-3 1 0 0 0,2-2 0 0 0,-1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 2 1 0 0,0-1-1 0 0,0 0 0 0 0,0-1 0 0 0,-3 7-137 0 0,4-12 22 0 0,0 2-1 0 0,-1-2 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 1-1 0 0,1-2 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0-21 0 0,-32 9 162 0 0,31-10-192 0 0,2 0 1 0 0,-2-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,2 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,2-2-1 0 0,-5 0 30 0 0,-12-31-3512 0 0,16 20 1769 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-204187.105">18616 2557 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203902.979">18599 2532 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203901.979">18586 2639 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203439.752">18557 2444 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,4 12 2392 0 0,11 79 1583 0 0,-14 35-1639 0 0,8 45-192 0 0,11-22-2656 0 0,-23-131 0 0 0,0-3-337 0 0,2-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202468.889">18589 2870 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-1-17 3737 0 0,3-5 4077 0 0,8-21-4186 0 0,6 1-1366 0 0,0 21-2142 0 0,-9 18-211 0 0,-7 8 222 0 0,17-9 1281 0 0,8 11-1444 0 0,-22 1-105 0 0,40 32-8 0 0,-21-3 744 0 0,-9-4-56 0 0,6 34-96 0 0,-12-19-16 0 0,3 12 191 0 0,-1-19-526 0 0,0-5-59 0 0,-2-14-12 0 0,-5-15-90 0 0,14 3 16 0 0,16-2-96 0 0,-7-4-141 0 0,-24 2-596 0 0,24-10-4249 0 0,-13 3 1073 0 0,-7 2 1923 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201801.05">19115 2666 1376 0 0,'-14'6'65'0'0,"11"-5"277"0"0,3-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-5 12 5285 0 0,10 44-3424 0 0,-8-8-2068 0 0,-1 47 541 0 0,-5-53-877 0 0,6 2-432 0 0,4 24-1088 0 0,7 7 915 0 0,-3-3-416 0 0,-3-59-545 0 0,-3 18 164 0 0,-4-12-45 0 0,4-18-557 0 0,1-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-4 0-797 0 0,2 0-5332 0 0,2 0 728 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201246.613">19075 2717 456 0 0,'29'-11'12581'0'0,"-19"5"-11549"0"0,15 5 3076 0 0,-3-5-1928 0 0,27 40 262 0 0,-17 0-1426 0 0,-9 18-48 0 0,-8-17-336 0 0,-15-31-440 0 0,-3 28-53 0 0,-6-11-60 0 0,-7-7 791 0 0,15-12-867 0 0,0-1 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,2-1 0 0 0,-2 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-3 1-3 0 0,-31-22-1713 0 0,11-1-2008 0 0,21 16 1827 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190828.747">16571 2632 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,3 14 1120 0 0,-1 37 395 0 0,2 69 75 0 0,3-39-2940 0 0,3 8-252 0 0,-3-15-192 0 0,0-36-12 0 0,-7-36-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="191215.919">16584 2795 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,4-14 2209 0 0,9-4-1077 0 0,29-21 345 0 0,-17 32-1146 0 0,-4 21-314 0 0,-17-11-177 0 0,0 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-37 0 0,-1-4 176 0 0,7 11 413 0 0,-7-12-998 0 0,10 7-4069 0 0,-11-8 3075 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="199554.903">16867 3101 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,6-4 224 0 0,-4 3 3136 0 0,8-11-3493 0 0,-8 9-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174270.903">17216 2741 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 13 8138 0 0,-3 35-5693 0 0,3-50-1919 0 0,-3 18 1214 0 0,0 78 988 0 0,3-96-2320 0 0,0-2-72 0 0,0 7 75 0 0,-4 26-43 0 0,-2 46-122 0 0,6-76-45 0 0,0 1-235 0 0,0-1-3512 0 0,0-3-1706 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173620.241">17203 2885 5296 0 0,'4'7'472'0'0,"-4"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-22 1372 0 0,0 19-1542 0 0,0 1-40 0 0,5-28 954 0 0,-4 29-1144 0 0,11-29 1755 0 0,4 12-1413 0 0,-15 17-538 0 0,-1 1 0 0 0,0 0-6 0 0,13-2 374 0 0,-7 3-368 0 0,-4-1-159 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-2 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1-24 0 0,12 62 908 0 0,-9-29-544 0 0,-5-11-78 0 0,1-23-204 0 0,0 21 170 0 0,1-19-204 0 0,1 5-36 0 0,2 1-1 0 0,-1-1 42 0 0,3-4 13 0 0,-3-3-58 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,2 1 0 0 0,0-1 0 0 0,-2-2 0 0 0,2 2 0 0 0,-1 0-1 0 0,-1 0 1 0 0,3-3-9 0 0,30-22-3222 0 0,-30 21-430 0 0,-3 5 1775 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="-165827.57">12107 3608 920 0 0,'0'0'411'0'0,"0"0"1389"0"0,0 0 609 0 0,0 0 119 0 0,0 0-215 0 0,0 0-1014 0 0,0 0-445 0 0,0 0-87 0 0,0 0-46 0 0,0 0-109 0 0,0 0-48 0 0,0 0-10 0 0,0 0 0 0 0,0 0 11 0 0,-13-2 1750 0 0,-6-2-885 0 0,-1 1-1 0 0,1 2 1 0 0,-1 0-1 0 0,1 1 1 0 0,-12 2-1430 0 0,-35 10 1057 0 0,-22-11-2 0 0,27-4-630 0 0,-73 0 196 0 0,30-8-298 0 0,33-8 8 0 0,59 14-305 0 0,0 2-1 0 0,0 0 1 0 0,0 1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 2 0 0 0,1 0 0 0 0,0 0-1 0 0,-4 2-25 0 0,-40 13 22 0 0,11-7 31 0 0,9-13 11 0 0,-68-2 64 0 0,50 27-128 0 0,-20 2 0 0 0,41-22 0 0 0,-9-5 0 0 0,-20 7 0 0 0,33 4 0 0 0,-11-14 0 0 0,-2-24 0 0 0,-6 29 0 0 0,3-3 0 0 0,30 3-632 0 0,13 1 769 0 0,0 1-984 0 0,2 0-6440 0 0,5-2 5260 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-62540.216">5345 243 9240 0 0,'0'0'208'0'0,"0"0"33"0"0,0 0 14 0 0,0 0 69 0 0,0 0 284 0 0,0 0 120 0 0,0 0 28 0 0,0 0-30 0 0,0 0-139 0 0,0 0-62 0 0,0 16 1654 0 0,-6 124 2954 0 0,-2 16-3081 0 0,7 59-343 0 0,8 152 170 0 0,1-204-1465 0 0,-8-131-531 0 0,0-30-556 0 0,0-4-270 0 0,-3-26-3089 0 0,0 17 1904 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-50190.827">5317 279 3224 0 0,'0'0'387'0'0,"0"0"414"0"0,0 0 183 0 0,0 0 37 0 0,-11-2 2900 0 0,4 0 1482 0 0,3 5 686 0 0,19 7-5649 0 0,73-9 731 0 0,-29-11-391 0 0,59 6-160 0 0,44-6-302 0 0,-61-2-104 0 0,23 7 148 0 0,-6 3 150 0 0,-10 2-320 0 0,21 3-48 0 0,-24 4 171 0 0,57 16 58 0 0,-52-10 92 0 0,7-8 14 0 0,-7-13-479 0 0,-41 3 68 0 0,-53 2-39 0 0,1 2-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 1-1 0 0,0 1 1 0 0,9 2-29 0 0,33 5 0 0 0,27-4 0 0 0,-11-1 0 0 0,-7-1 0 0 0,-32 7 0 0 0,41-4 0 0 0,44-8 0 0 0,-86-1 0 0 0,39 5 0 0 0,-62 1 5 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,4-1-5 0 0,57-5 19 0 0,83 21-8 0 0,-92-7 95 0 0,18-6-31 0 0,-16-10-11 0 0,84 1 0 0 0,-71 2 0 0 0,7 1-64 0 0,-40-3 53 0 0,33 0-42 0 0,-40 9-11 0 0,52-4 0 0 0,17 0 0 0 0,-30 16 0 0 0,179-10 0 0 0,-113-19 0 0 0,-75 10 0 0 0,36 0 0 0 0,-25 11 0 0 0,-30 3 0 0 0,25-6 64 0 0,-4-6 128 0 0,53 5-192 0 0,-94 4 0 0 0,-1-1 0 0 0,-22-3 0 0 0,-2 0-12 0 0,-4 0-53 0 0,-1 0-170 0 0,0 0-576 0 0,0 0-247 0 0,0 0-49 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-49193.598">10117 195 5928 0 0,'0'0'266'0'0,"0"0"1"0"0,0 1-171 0 0,0 4 92 0 0,0-4 732 0 0,-2 15 4758 0 0,4 14-1191 0 0,7 35 169 0 0,-12-10-3447 0 0,-3 119 1305 0 0,2-61-2021 0 0,-1-7-60 0 0,4 51 591 0 0,7-35-728 0 0,-3-90-284 0 0,-2 1 204 0 0,-1-32-157 0 0,0-1 6 0 0,0 0-26 0 0,0 0-98 0 0,0 0-9 0 0,0 0 4 0 0,0 0 0 0 0,0 0-43 0 0,0 0-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0-98 0 0,0 0-410 0 0,0 0-182 0 0,0 0-42 0 0,0 0-73 0 0,0 0-285 0 0,0 0-126 0 0,0 0-983 0 0,0 0-3823 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-48911.614">10104 1101 456 0 0,'0'0'1737'0'0,"0"0"207"0"0,0 0 88 0 0,0 0-76 0 0,0 0-381 0 0,0 0-174 0 0,0 0-32 0 0,0 0-62 0 0,0 0-231 0 0,0 3-99 0 0,0 75 4474 0 0,4-45-4150 0 0,1 16 250 0 0,-4 2-1349 0 0,-2-22-20 0 0,1-21-172 0 0,0 5 904 0 0,0-13-2338 0 0,0 3-8055 0 0,0-3 3197 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-46458.211">10126 1337 3224 0 0,'-10'8'2653'0'0,"-37"20"4634"0"0,46-28-6665 0 0,-1 0 33 0 0,-41-7 3329 0 0,-32 1 217 0 0,48 7-3372 0 0,-71-2 683 0 0,42-21 54 0 0,27 12-1308 0 0,13 5-82 0 0,1 1 1 0 0,-1 0-1 0 0,1 2 0 0 0,-1 0 0 0 0,0 2 0 0 0,0 0 1 0 0,-10 2-177 0 0,-13-1 177 0 0,-36-8 419 0 0,12-3-51 0 0,-54 6 350 0 0,23 11-662 0 0,13 3-169 0 0,11-2-64 0 0,-14-16 140 0 0,-53 7 320 0 0,42 2-460 0 0,6-13 83 0 0,15 0-30 0 0,28 6-53 0 0,-35 0 0 0 0,-55 6 0 0 0,-18-4 0 0 0,69 1 0 0 0,0 5 0 0 0,-41-4 0 0 0,8-6 0 0 0,-127 8 0 0 0,171 5 0 0 0,-32-10 117 0 0,8-7 118 0 0,43 8-410 0 0,-94 8 326 0 0,90-8-162 0 0,-76-1 37 0 0,3 9-289 0 0,7 5 263 0 0,-31-1 208 0 0,57 0-413 0 0,-44-5 194 0 0,32-6 11 0 0,-33 22 344 0 0,67-5-608 0 0,-58 4 160 0 0,67-15 104 0 0,-33-3 968 0 0,13-11-1140 0 0,11 11-113 0 0,21 10 214 0 0,-36-5 71 0 0,63-6-97 0 0,22 2 121 0 0,4-1-4216 0 0,3 0-5767 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-41895.864">5460 2561 5264 0 0,'3'0'1129'0'0,"6"0"-2200"0"0,-6 0 4901 0 0,-2 1 4833 0 0,6 41-6741 0 0,-7 54 512 0 0,-7 20-998 0 0,14 103 1044 0 0,6-75-1600 0 0,-3-46-128 0 0,3 49-792 0 0,-7-71 515 0 0,-6-35 182 0 0,-4-16 138 0 0,0-14-1692 0 0,4-11-2271 0 0,1-8 1285 0 0,0-1-408 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-39644.648">5427 2564 456 0 0,'0'0'1548'0'0,"0"0"185"0"0,0 0 82 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-42 0 0,0 0-140 0 0,0 0-57 0 0,0 0-16 0 0,0 0-1 0 0,0 0 12 0 0,0 0 2 0 0,0 0-1 0 0,0 0-47 0 0,0 0-202 0 0,0 0-92 0 0,2 0-11 0 0,45-7 2042 0 0,42 1 147 0 0,61 5-222 0 0,-21 11-1432 0 0,-17-16-175 0 0,125-12 402 0 0,-106-6-820 0 0,-48 7 18 0 0,-49 10-382 0 0,2 2 1 0 0,-1 2-1 0 0,28 1 7 0 0,57 2 256 0 0,-80 0-256 0 0,38 0 181 0 0,-19 10-106 0 0,6-4 1 0 0,-3-2 68 0 0,50 0-1 0 0,-71-1-90 0 0,74-4 144 0 0,166-8-122 0 0,-224 12-75 0 0,39 8 0 0 0,18-8 0 0 0,-59 5 0 0 0,-3-3 0 0 0,50-5 0 0 0,14 0 0 0 0,-57 11 0 0 0,-20-4 64 0 0,57-18 0 0 0,-35 1-64 0 0,47-3-67 0 0,38 24 54 0 0,-84-12 13 0 0,-38-3 11 0 0,2 2-1 0 0,-2 1 1 0 0,0 1 0 0 0,0 1-1 0 0,23 5-10 0 0,8-3 11 0 0,69-6-74 0 0,-45-3 30 0 0,42 19 33 0 0,13-3 152 0 0,-80-3-152 0 0,-20-6-172 0 0,39 4 160 0 0,10-5 12 0 0,-24 0 0 0 0,-7-3 0 0 0,-21 3 0 0 0,2 0-16 0 0,-32 0-61 0 0,-1 0-6 0 0,0 0-138 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1739 0 0,0 0-6757 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-38736.343">9765 2513 1376 0 0,'0'0'65'0'0,"0"0"341"0"0,0 0 1404 0 0,0 0 611 0 0,8 0 3921 0 0,-6 1-6029 0 0,0 0 0 0 0,1-1-1 0 0,-2 1 1 0 0,1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 3-313 0 0,5 61 2731 0 0,17 121-151 0 0,-13-101-1558 0 0,-14 40 98 0 0,13 24 148 0 0,-4-78-785 0 0,-3-29-243 0 0,-2 26 129 0 0,1 22 111 0 0,-1-56-253 0 0,0-34-205 0 0,0-1-106 0 0,0 0-8 0 0,-17 20-828 0 0,17-20 767 0 0,-9 16-1455 0 0,8-15 1350 0 0,1-1-81 0 0,0 0-40 0 0,0 0-5 0 0,0 0-101 0 0,0 0-426 0 0,0 0-185 0 0,0 0-37 0 0,0 0-102 0 0,0 0-386 0 0,0 0-166 0 0,0 0-32 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36969.387">9836 3547 3224 0 0,'-6'11'5642'0'0,"-7"14"-878"0"0,13-23-3930 0 0,-1-1-138 0 0,-29 28 3385 0 0,-31-14 128 0 0,32-13-2861 0 0,-118 22 765 0 0,99-14-1621 0 0,-90-3 1168 0 0,18-23-712 0 0,-119 2-243 0 0,132 17-482 0 0,-27 1 141 0 0,44-5-364 0 0,-162 8 0 0 0,157 3 0 0 0,-253-7 0 0 0,192 1 228 0 0,-51-31 541 0 0,114 17-750 0 0,-55-4-19 0 0,103 7 0 0 0,24 6 0 0 0,0-2 0 0 0,0-1 0 0 0,0-1 0 0 0,1 0 0 0 0,-7-5 0 0 0,17 7 0 0 0,-34-14 0 0 0,-2 4 0 0 0,1 2 0 0 0,-1 3 0 0 0,0 1 0 0 0,-13 3 0 0 0,-24 7 0 0 0,25 3 0 0 0,-76-8 0 0 0,76-2 0 0 0,-67 7 0 0 0,44 10-21 0 0,2-3-5 0 0,-28 0-287 0 0,75-4 334 0 0,-11-1 286 0 0,-67-12-307 0 0,28-7-103 0 0,3 11-9 0 0,47 6 23 0 0,-4-3 89 0 0,-9 13 0 0 0,-50 6 73 0 0,46-10-143 0 0,3-2 403 0 0,4-9-333 0 0,16 4 0 0 0,-14-4-32 0 0,41 2-137 0 0,-2 9-3011 0 0,2-6 1857 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1488.941">12517 2225 3224 0 0,'0'0'389'0'0,"0"0"426"0"0,0 0 185 0 0,0 0 37 0 0,0 0-41 0 0,0 0-211 0 0,7 15 2921 0 0,1 0-2586 0 0,-7-14-544 0 0,-1 0 0 0 0,13 148 6159 0 0,-20 6-3759 0 0,5-42-1768 0 0,4 60 608 0 0,2 45-811 0 0,19 106 755 0 0,-10-183-1237 0 0,-7 21-2562 0 0,-6-171-744 0 0,0-8-6530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="854.454">12511 2182 3224 0 0,'-3'-1'-2321'0'0,"0"-2"3355"0"0,-4-5 11775 0 0,9 6-10726 0 0,-1 1-1175 0 0,-1 1-164 0 0,10-2 590 0 0,105 15 3826 0 0,119-6-1952 0 0,0 0-2760 0 0,-67-11 16 0 0,-39-10 16 0 0,41-9 88 0 0,-23 6-187 0 0,37 1-162 0 0,-29 5-75 0 0,31-4 144 0 0,-5 2-149 0 0,-41 2-22 0 0,58-6-205 0 0,-5 11 211 0 0,49 5 714 0 0,-26 8-953 0 0,36 10-59 0 0,-146-3 482 0 0,5-11-635 0 0,-9 1 267 0 0,74 19 74 0 0,-27-1-13 0 0,19-2-88 0 0,15-10 152 0 0,11-10-64 0 0,-68-3 0 0 0,-38-4 0 0 0,148-3 0 0 0,-102 7 0 0 0,66 2 0 0 0,-124 11 0 0 0,63-3 0 0 0,-9 0 0 0 0,-53 8 0 0 0,51 5 0 0 0,-77-8 0 0 0,50-1 0 0 0,33 1 0 0 0,8 1 0 0 0,-65-7 400 0 0,-6 1-480 0 0,65-11 133 0 0,-11 1-106 0 0,-93 3 53 0 0,52-1-64 0 0,-19-4 64 0 0,-18 2 11 0 0,65 1 375 0 0,-58-15-452 0 0,-25 11 108 0 0,32-4-95 0 0,-36 10 53 0 0,-24 19-245 0 0,-2-15 238 0 0,2-4 7 0 0,-1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,10 61 0 0 0,-1-27 0 0 0,-10 4 0 0 0,16 3 0 0 0,-20 3 0 0 0,7-27 0 0 0,-1-9 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 5 0 0 0,-9 82-11 0 0,-7-3-42 0 0,15-3 53 0 0,8 36 0 0 0,0-59 0 0 0,-3-8 12 0 0,0-52 4 0 0,-1 40 108 0 0,-29 62-44 0 0,18-59-80 0 0,4-38 0 0 0,-2 21 0 0 0,6 34 0 0 0,11-32 0 0 0,-7 3 0 0 0,-6-26 0 0 0,3 1 0 0 0,-2 29 99 0 0,1-29 95 0 0,-7 13-174 0 0,3-7 27 0 0,7-8-47 0 0,5-2 0 0 0,1-1 0 0 0,-6-1 0 0 0,5-3-20 0 0,-4-2-73 0 0,-2-1 7 0 0,-2 0-3 0 0,1 0-9 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 98 0 0,4-6-6888 0 0,-3 1-1987 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6517.426">12583 3720 7688 0 0,'0'0'349'0'0,"0"0"-2"0"0,0 0-90 0 0,0 0 455 0 0,0 0 227 0 0,0 0 42 0 0,13 5 4082 0 0,49-12-625 0 0,2 6-2566 0 0,-13 4-1407 0 0,110-3 623 0 0,-13 5-464 0 0,-41 12 788 0 0,23-6-770 0 0,155-36 656 0 0,-179 25-914 0 0,-56 3-169 0 0,117-13 21 0 0,-19-2-119 0 0,-85 21-53 0 0,9 4 128 0 0,-27-6-192 0 0,43 4-8 0 0,47-1 144 0 0,-55 3-136 0 0,10 0 32 0 0,-61-9 64 0 0,10-4-335 0 0,9 4 142 0 0,17 7 97 0 0,-3-8 168 0 0,71-14-96 0 0,-70 5-8 0 0,8-5-240 0 0,-12 17 64 0 0,32-15 96 0 0,-6-1 167 0 0,27-3-62 0 0,-63 13-25 0 0,97-18-57 0 0,-87 8-318 0 0,94 5 639 0 0,36-2-696 0 0,-25 21 1344 0 0,-54-5-976 0 0,-14-3 0 0 0,-6-3 0 0 0,15 7 200 0 0,-52 3-40 0 0,181 4-64 0 0,-25-9 203 0 0,-144-11-246 0 0,62 13 139 0 0,117-7-128 0 0,-132-6 428 0 0,-1-5 0 0 0,2-8-492 0 0,28-1 0 0 0,136-24-11 0 0,-160 24-42 0 0,13 1 53 0 0,-42 11 0 0 0,-69 3 0 0 0,0 2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 3 0 0 0,17 3 0 0 0,63 6 0 0 0,14-3 0 0 0,51 0 0 0 0,-94-9 0 0 0,-41-6 0 0 0,8-1 0 0 0,33-7 0 0 0,-18 6 0 0 0,-41 7 0 0 0,-5 0 0 0 0,5 0-16 0 0,-10 0-68 0 0,-1 0-32 0 0,14 3-689 0 0,-18 1-1817 0 0,-7 5-1623 0 0,-23 7 1843 0 0,-6-4-20 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-14T20:45:42.705"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+    <inkml:brush xml:id="br1">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2006 764 2760 0 0,'0'0'531'0'0,"0"0"1186"0"0,0 0 519 0 0,0 0 106 0 0,0 0-166 0 0,0 0-792 0 0,0 0-346 0 0,0 0-70 0 0,0 0-47 0 0,0 0-163 0 0,0 0-71 0 0,0 0-14 0 0,0 0 10 0 0,0 0 42 0 0,0 0 13 0 0,0 9 699 0 0,-5 116 2364 0 0,10 24-1865 0 0,5 117-247 0 0,3-21-814 0 0,-10-50-319 0 0,-16-69 500 0 0,19-96-2539 0 0,-6-29 905 0 0,0-1-60 0 0,0 0-15 0 0,0 0-116 0 0,0 0-476 0 0,0 0-209 0 0,2 0-39 0 0,6-2-10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2597.859">1857 679 4144 0 0,'0'0'319'0'0,"0"0"23"0"0,0 0 881 0 0,4-5 1496 0 0,0 3 846 0 0,42-24 2209 0 0,15 21-278 0 0,110-4-967 0 0,-100-1-3873 0 0,5-1-272 0 0,97-9 368 0 0,-40 17-373 0 0,-130 3-377 0 0,51 0 316 0 0,0-2-1 0 0,48-11-317 0 0,27-6 240 0 0,36-9-96 0 0,-46 18-73 0 0,-39 6 277 0 0,24 2-231 0 0,71-12 51 0 0,-32 4-88 0 0,-32 17-27 0 0,-51-1-42 0 0,-39-3 14 0 0,-2-2 0 0 0,1 0-1 0 0,1-2 1 0 0,-2 0 0 0 0,18-4-25 0 0,46-3 73 0 0,16 5 130 0 0,-63 3-371 0 0,49-10 88 0 0,45-23 197 0 0,-50 15-106 0 0,-32 12 42 0 0,104 8-170 0 0,-79-2 117 0 0,-22 5 64 0 0,77-3-64 0 0,40 5 0 0 0,-50-1 0 0 0,52-9 0 0 0,-50 10-64 0 0,3 0 75 0 0,-40 1 31 0 0,50-2-95 0 0,40 4 53 0 0,-31 10-160 0 0,-53-14 107 0 0,0-2-22 0 0,-9 7 11 0 0,34-9 53 0 0,-51 5-42 0 0,78-6-339 0 0,-16 6 280 0 0,32-3 32 0 0,-111-3 80 0 0,103 4 0 0 0,-27-15 177 0 0,-1-3-378 0 0,-17 15 201 0 0,-21-12 0 0 0,-39 2 46 0 0,1 1 0 0 0,0 4-1 0 0,11 1-45 0 0,68-2-5 0 0,19 1-127 0 0,-34-6 284 0 0,88-8-13 0 0,51 9-422 0 0,-129-1 407 0 0,10-3 201 0 0,-102 18-371 0 0,-25-5-57 0 0,7 0-101 0 0,-3 1 124 0 0,26 8 64 0 0,-7-1 16 0 0,-8 10 0 0 0,-7-2 0 0 0,2 23 0 0 0,-6 5 0 0 0,-9 6 0 0 0,-3 10 257 0 0,-1-14-154 0 0,7 20 193 0 0,-9 33-376 0 0,0-11-72 0 0,-4-5 152 0 0,-1 49 64 0 0,3-29-64 0 0,4-12 64 0 0,9-28-53 0 0,-5-3 42 0 0,1-3-53 0 0,-4 26 75 0 0,0-36 31 0 0,2-12-84 0 0,1-28 20 0 0,6-1-31 0 0,0 0-11 0 0,0 11-21 0 0,-3-16-85 0 0,0-2-15 0 0,0 0 1 0 0,-2 1-73 0 0,-4 4-309 0 0,4-4-135 0 0,2-1-31 0 0,-3 3-3225 0 0,3-3 2170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4154.481">8975 1816 456 0 0,'0'0'1935'0'0,"0"0"230"0"0,0 0 105 0 0,6 0 2569 0 0,-14 0 1235 0 0,7 0-5318 0 0,-6 0 604 0 0,-34 0 319 0 0,-3 3 418 0 0,5 4-841 0 0,-2-1-398 0 0,-116-19 1481 0 0,-3 0-1024 0 0,52 19-770 0 0,47 5-530 0 0,-130 23 160 0 0,39-26 530 0 0,-102-4-273 0 0,30 7-305 0 0,17-8 282 0 0,73-17-409 0 0,-57 12 0 0 0,-399 82 0 0 0,539-73 12 0 0,1-4 1 0 0,-1-2-1 0 0,0-3 1 0 0,1-4-1 0 0,-1-1 1 0 0,-37-12-13 0 0,-137-32 117 0 0,56 21-117 0 0,46 17 89 0 0,-79 6-89 0 0,-154-10-97 0 0,229 30 97 0 0,-161-30 0 0 0,63-8 0 0 0,127 13 11 0 0,-70 5 138 0 0,-88 7-149 0 0,171 3 0 0 0,-27-10 0 0 0,-50 7 45 0 0,67 4-26 0 0,0 6-322 0 0,-169 15 758 0 0,189-19-455 0 0,-114-5 344 0 0,17 8-365 0 0,95-3-99 0 0,-26 5 109 0 0,43-15 11 0 0,34-1 0 0 0,-23 1 0 0 0,-50 10-368 0 0,48 4-707 0 0,36-6-1382 0 0,14-4 988 0 0,1 0-298 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8166.184">1641 1826 2760 0 0,'6'32'2136'0'0,"-6"-31"-1553"0"0,0-1-342 0 0,0 0-148 0 0,30 15 2680 0 0,-29-15-2055 0 0,-1 0 30 0 0,0 0 117 0 0,0 0 51 0 0,0 0 11 0 0,0 0-21 0 0,0 0-87 0 0,0 0-34 0 0,0 0-7 0 0,0 0-4 0 0,0 0-6 0 0,0 0-7 0 0,0 0-1 0 0,0 0-33 0 0,0 0-140 0 0,0 0-62 0 0,-12 6 796 0 0,-31 1 55 0 0,-15 10 107 0 0,-24-10 121 0 0,-53 7-11 0 0,31 2-921 0 0,36-16-416 0 0,20-4-63 0 0,-59-16 422 0 0,81 14-425 0 0,-1 1-1 0 0,1 2 0 0 0,-1 0 1 0 0,0 3-1 0 0,-3 1-189 0 0,12-1 26 0 0,-56-1-15 0 0,-56 41-11 0 0,63-37 0 0 0,-23-2 0 0 0,63-5 0 0 0,8-5-11 0 0,0-1-554 0 0,18 9 409 0 0,-9-10-997 0 0,6-3-1235 0 0,-1-3-4013 0 0,4 15 1126 0 0,-2-5-1271 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8769.491">422 1697 4144 0 0,'-3'0'371'0'0,"-32"10"5674"0"0,9-4 1575 0 0,8 1-6482 0 0,-46 24 2093 0 0,-51 54-822 0 0,18 27-2088 0 0,39-17 366 0 0,57-91-645 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,2 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,1 0-42 0 0,8 8 113 0 0,1-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-2 0 0 0,13 2-113 0 0,35 7 53 0 0,29-4-769 0 0,-90-9-139 0 0,-1 0-1079 0 0,2 1-4291 0 0,4 2-1841 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11563.093">9347 621 1376 0 0,'0'0'65'0'0,"0"0"-6"0"0,-2 2 265 0 0,2 0 1296 0 0,-9 5 9233 0 0,6-5-11305 0 0,-2 2 8571 0 0,9-3-7501 0 0,-2-1-153 0 0,-2 0-1 0 0,0 0-25 0 0,8-1 177 0 0,122-26 2488 0 0,158-23-951 0 0,-131 25-1665 0 0,-88 16-280 0 0,56 5-144 0 0,-58 7 3 0 0,9 1 63 0 0,66 2 73 0 0,-96-15-234 0 0,-44 4 49 0 0,-1 3-3067 0 0,-1 2-3310 0 0,0 0 4316 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12290.505">10534 204 13104 0 0,'0'0'297'0'0,"0"0"39"0"0,0 0 19 0 0,0 0-34 0 0,0 0-126 0 0,0 0 250 0 0,0 0 130 0 0,0 0 29 0 0,0 0-13 0 0,8 6 913 0 0,38 15 1575 0 0,33 14-91 0 0,-70-31-2871 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,3 3-117 0 0,16 48 400 0 0,-19-14-62 0 0,1-7 43 0 0,-1 10 309 0 0,-28 11 92 0 0,10-40-673 0 0,-1-2 0 0 0,1 0 0 0 0,-2-1 0 0 0,1-1 0 0 0,-16 14-109 0 0,16-19 53 0 0,1-1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-2-1 1 0 0,1-1-1 0 0,-13 6-53 0 0,-10-12-351 0 0,32-4-332 0 0,1-1-1543 0 0,2 3-4239 0 0,-1 1-1953 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="90996.656">11571 1191 920 0 0,'0'0'304'0'0,"0"0"941"0"0,0 0 414 0 0,0-1 1565 0 0,5-8-1987 0 0,32-69 3794 0 0,-34 71-4715 0 0,0 1 1 0 0,2 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0-316 0 0,-3 4 87 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,2 1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0-86 0 0,7 24 477 0 0,-1-1 0 0 0,-1 0 0 0 0,-1 2 0 0 0,0-1-1 0 0,-1 28-476 0 0,-8 54 1538 0 0,4-107-1494 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-2 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-45 0 0,-2 1 47 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,-1-2-47 0 0,-2-3-7 0 0,2 0-1 0 0,-2-1 0 0 0,1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-3 0 0 0,1 2 1 0 0,0-1-1 0 0,1 0 1 0 0,1 0-1 0 0,-4-11 8 0 0,5 15-502 0 0,2 0 0 0 0,-1-2 0 0 0,0 2 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 502 0 0,5-10-7366 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="91897.027">12041 897 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-132 0 0,0 0-646 0 0,0 0-278 0 0,1-1-58 0 0,10-8 2229 0 0,-10 9-2573 0 0,-1 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-13 0 0,0 0-49 0 0,8 5 828 0 0,-6-1-1148 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 1 0 0,-1-2-140 0 0,-1 25 426 0 0,-14 195 876 0 0,16-147-1182 0 0,0-76-384 0 0,0 4 981 0 0,0 1-1983 0 0,0 6-3464 0 0,0-12 2540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="92647.981">12063 1097 920 0 0,'0'1'67'0'0,"0"3"290"0"0,0-3 1430 0 0,0-1 622 0 0,0 0 119 0 0,0 0-204 0 0,0 0-970 0 0,0 0-423 0 0,0 0-88 0 0,4-22 1733 0 0,-4 21-2071 0 0,1-1-229 0 0,9-15 61 0 0,-8 15-136 0 0,3-4 690 0 0,24-29 1892 0 0,5 12-882 0 0,-29 22-1876 0 0,-2 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1-25 0 0,16 33 1472 0 0,-2 11-864 0 0,-15-18-608 0 0,8 11 0 0 0,-7-3 72 0 0,-3-34 299 0 0,0-2 117 0 0,17 14 597 0 0,4-2-1750 0 0,-20-11 404 0 0,15-8-493 0 0,11-20-1947 0 0,-16 1-3478 0 0,-9 18-300 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="93989.379">12764 962 456 0 0,'0'0'1413'0'0,"0"0"159"0"0,0 0 76 0 0,0 0-140 0 0,0 0-647 0 0,0 0-278 0 0,0 0-58 0 0,0-7 1476 0 0,-1 6 4407 0 0,-7 1-5892 0 0,0 0-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,2 0 0 0 0,-7 5-515 0 0,-5 5 424 0 0,13-12-374 0 0,2 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 3-50 0 0,-11 43 264 0 0,12 1-125 0 0,3-41-85 0 0,0 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,2 2 1 0 0,0-2-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,6 8-54 0 0,-8-13-18 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,3 0 18 0 0,31-6-3249 0 0,-32 2 1306 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95267.643">13094 510 920 0 0,'0'0'341'0'0,"0"0"1098"0"0,0 0 480 0 0,0 0 96 0 0,0 0-104 0 0,0 0-531 0 0,0 0-237 0 0,1 2-45 0 0,2 14 790 0 0,-3-15-1129 0 0,0-1-20 0 0,0 2-30 0 0,0 129 4843 0 0,-4-36-3927 0 0,-2 119 184 0 0,3-54-1385 0 0,3-133-472 0 0,0 5-118 0 0,0-9-6313 0 0,0-23 4748 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95643.07">13107 648 920 0 0,'10'-7'6425'0'0,"11"-16"3843"0"0,19 3-5971 0 0,-33 17-3958 0 0,-2 1 0 0 0,2 0-1 0 0,0 0 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 2 1 0 0,6 0-339 0 0,29 11 773 0 0,-11-1-4595 0 0,-23-11-1695 0 0,-1 0-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98550.722">13464 865 920 0 0,'0'0'241'0'0,"0"0"678"0"0,0 0 296 0 0,0 0 58 0 0,0 0-53 0 0,0 0-254 0 0,0 0-114 0 0,0 0-20 0 0,0 0-22 0 0,0 0-70 0 0,0 0-32 0 0,0 26 3129 0 0,-10 230 4156 0 0,12-97-6298 0 0,2-95-1707 0 0,-4-63-70 0 0,0-1-160 0 0,0 0-685 0 0,0-7-2761 0 0,0-3-3454 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98832.077">13486 607 7976 0 0,'0'14'364'0'0,"0"-10"-8"0"0,0 3-212 0 0,0-1-7 0 0,0-5 574 0 0,0-1 238 0 0,0 11 1235 0 0,0-10 2609 0 0,1-1-5097 0 0,1-9-870 0 0,1 6-3805 0 0,-3 3 790 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="100011.114">13794 1184 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-6 6 0 0,-5-42 6095 0 0,12 11-2868 0 0,25-8-2391 0 0,-11 28 397 0 0,-18 17-1428 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 3-36 0 0,9 80 216 0 0,-19 14 176 0 0,-5-61 1491 0 0,14-38-1877 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0-6 0 0,-13-9 9 0 0,-28-33 46 0 0,24-18-327 0 0,18 56 112 0 0,0-1-1 0 0,1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 1 0 0,1-1 160 0 0,20-36-6577 0 0,-14 32 179 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="112707.469">11396 862 6192 0 0,'0'0'133'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 66 0 0,0 0 226 0 0,1-22 6285 0 0,-2-21-2539 0 0,-8 24-3101 0 0,-34-45-120 0 0,-13 22-726 0 0,37 36-73 0 0,-17 9 54 0 0,-17 21-89 0 0,21 31-88 0 0,10 8-64 0 0,12 26 80 0 0,7-63 60 0 0,2 1 0 0 0,1 0 0 0 0,0 0 0 0 0,2-1 0 0 0,1 1 0 0 0,3 10-140 0 0,6 89 1072 0 0,-3-56-1705 0 0,3 4-463 0 0,-11-62-34 0 0,-1-9-5836 0 0,0-3 1152 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="113106.261">11112 1036 11952 0 0,'0'0'546'0'0,"0"0"-10"0"0,5-5-322 0 0,1 1 384 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1 1-1 0 0,2-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 1-599 0 0,14-4 579 0 0,16 8 986 0 0,1-1-980 0 0,-15 0-2039 0 0,-7-2-3511 0 0,-3-1-1716 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119095.651">14207 972 920 0 0,'0'0'215'0'0,"0"0"565"0"0,0 0 246 0 0,0 0 50 0 0,0 0-38 0 0,0 0-207 0 0,0 0-88 0 0,-9-18 1465 0 0,9 18-2144 0 0,-4-8 120 0 0,4 3-161 0 0,0 4 46 0 0,0 1 50 0 0,0 0 7 0 0,0 0-4 0 0,-1-6-39 0 0,0 6 8497 0 0,-10 47-6476 0 0,6 52 348 0 0,2-28-1794 0 0,8 71 1307 0 0,-5-54-1940 0 0,1-75 372 0 0,-1 1-4686 0 0,0-14 2473 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119948.343">14189 1191 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-112 0 0,0 0 219 0 0,6-5 2204 0 0,11-20-38 0 0,-16 24-2011 0 0,-1-21 3079 0 0,2 8-2359 0 0,12-37 1842 0 0,8 21-1982 0 0,7 5 8 0 0,-23 24-1121 0 0,-4 2 6 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1 0 0 0,-2 0-1 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 3-22 0 0,10 9-263 0 0,-10-10 258 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 1 5 0 0,5 19 825 0 0,7 57 291 0 0,-2-48-1116 0 0,0-12 562 0 0,10-21 72 0 0,-17-2-761 0 0,1-1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,1-1 0 0 0,0 1 0 0 0,-1-2 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-2 1-1 0 0,3-2 127 0 0,2-1-1228 0 0,16-13-4345 0 0,-21 17 3808 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121219.819">14777 503 3224 0 0,'-3'12'2653'0'0,"0"28"1684"0"0,-7-1-951 0 0,6 30-459 0 0,-2 41-127 0 0,5 44-152 0 0,0-92-2024 0 0,3 2 194 0 0,-2-3 190 0 0,-9 26-96 0 0,0 83-482 0 0,4-149-526 0 0,3-19 68 0 0,2-2-108 0 0,0 0-10 0 0,0 0 8 0 0,0 0-167 0 0,0 0-710 0 0,-1-10-2894 0 0,-1-3-3509 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121883.773">14777 551 11024 0 0,'0'0'248'0'0,"0"0"34"0"0,0 0 22 0 0,0 0-29 0 0,1 1-54 0 0,41 5 5667 0 0,-3 9-4316 0 0,3 7 205 0 0,2 19-391 0 0,-15-4-436 0 0,-10-6-482 0 0,25 67 576 0 0,-24-42-556 0 0,1 40 243 0 0,-20-77-582 0 0,0-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-3-1 1 0 0,1 0-1 0 0,-2 3-149 0 0,-13 98 744 0 0,-1-15 79 0 0,11-81-656 0 0,4-15-103 0 0,2 1 0 0 0,-2 0 0 0 0,1-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,0-1 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,-5 6-64 0 0,4-8 14 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 0-14 0 0,-34-13-1612 0 0,35 10 372 0 0,2 2 9 0 0,1-6-3128 0 0,-1-6 2299 0 0,4 11-11 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122684.061">15346 510 6968 0 0,'0'0'316'0'0,"0"0"-3"0"0,0 0-49 0 0,0 0 543 0 0,0 0 258 0 0,0 0 50 0 0,3 11 2997 0 0,-3 30-882 0 0,-3 12-957 0 0,-23 120 1538 0 0,-1 74-1086 0 0,17-111-1413 0 0,6-17-1045 0 0,4-61-214 0 0,0-50-2118 0 0,-2-6-5266 0 0,1-2 4284 0 0,4-10-3949 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="123499.345">15400 527 1376 0 0,'0'0'455'0'0,"0"0"1373"0"0,0 0 605 0 0,0 0 119 0 0,0 0-232 0 0,0 0-1087 0 0,0 0-473 0 0,0 0-96 0 0,0 0-7 0 0,0 0 58 0 0,0 0 21 0 0,0 0 7 0 0,0 0-22 0 0,2 0-96 0 0,31-7 3303 0 0,-31 7-3725 0 0,2-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,2 1-203 0 0,1 1 237 0 0,69 38 1652 0 0,-67-34-1701 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 1 0 0 0,3 5-188 0 0,-7-11 45 0 0,23 89 375 0 0,-25-88-406 0 0,0-1 0 0 0,0 1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 1 0 0,-1-1-1 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,0 2-14 0 0,-2-1 56 0 0,0 2 0 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,-3 1-56 0 0,-14 6 176 0 0,13-11-196 0 0,36 13-457 0 0,-19-11 473 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 4 4 0 0,-17 89 137 0 0,11-82 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-4 7-137 0 0,-10 12 332 0 0,-31 38 176 0 0,28-51-504 0 0,-8-41-3300 0 0,31 16 1814 0 0,-1-2-56 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="126421.51">10864 1874 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-2 10-158 0 0,1-10 318 0 0,1 0 203 0 0,-3-17 4327 0 0,9-85 858 0 0,7-11-4362 0 0,-9-52-443 0 0,-5 32-346 0 0,12-67-590 0 0,-6 45 735 0 0,2-20-741 0 0,-5-31-100 0 0,17-20 802 0 0,14 48-1204 0 0,-8 60 526 0 0,-16 95-375 0 0,12-25 96 0 0,-9 34 0 0 0,-7 11 11 0 0,2-3 42 0 0,6 5-120 0 0,133 32 118 0 0,-66-21-51 0 0,19 1 0 0 0,79 28 0 0 0,-33-11 13 0 0,-50-7 12 0 0,2-6 1 0 0,81-1-26 0 0,320-33 619 0 0,-219-3-286 0 0,178-2 704 0 0,-107 2-1079 0 0,305 34 539 0 0,-111-24-461 0 0,-336-3-36 0 0,-36 6 0 0 0,-23 0-89 0 0,199 1 178 0 0,34 58-89 0 0,-137-19-53 0 0,-165-27 106 0 0,-68 13-53 0 0,-10-12 0 0 0,0 1 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 5 0 0 0,-3 26 0 0 0,-11 134 0 0 0,-14 51 0 0 0,-9 74 0 0 0,-6 64 0 0 0,14-181 0 0 0,17-107 0 0 0,-30 107 0 0 0,21-89 0 0 0,-1 10 0 0 0,14-49 0 0 0,-10 31 0 0 0,-10-22 0 0 0,24-52 0 0 0,-15 9 0 0 0,-2-1 0 0 0,-52 12 0 0 0,19-22-89 0 0,-244-1 178 0 0,115 1-89 0 0,-113-18 0 0 0,26-3 0 0 0,-311 8-364 0 0,303 23 728 0 0,-61-30-364 0 0,103 7-488 0 0,133 6 351 0 0,-222 9-206 0 0,233-2 409 0 0,-1-6 0 0 0,-53-9-66 0 0,-83-18 67 0 0,-46-1 57 0 0,82 20-596 0 0,-17-13 472 0 0,145 14 141 0 0,-146-19 66 0 0,94 7-414 0 0,-188-35 751 0 0,205 45-712 0 0,56 2-1600 0 0,25 7-7788 0 0,14 0 569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128916.561">10598 1626 1376 0 0,'1'0'379'0'0,"1"0"-255"0"0,2-1 1065 0 0,17-35 2596 0 0,-17 28-3929 0 0,-1-24 6888 0 0,-3 31-6157 0 0,-13 1 1265 0 0,-35 24 2723 0 0,-92 15-187 0 0,70-26-3294 0 0,-1-5 0 0 0,-1-4 0 0 0,1-3 0 0 0,-1-5-1094 0 0,-33-3 693 0 0,-172-34-271 0 0,205 28-246 0 0,-5 6 42 0 0,-21-2-111 0 0,66 27-215 0 0,31-17-45 0 0,-6-3-2 0 0,5 1-5493 0 0,2 1 3616 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129317.678">9656 1385 12496 0 0,'0'0'572'0'0,"-7"4"186"0"0,-90 25 4653 0 0,-32 34-21 0 0,-1 45-3631 0 0,90-44-1578 0 0,28-15 21 0 0,11-48-198 0 0,0 2 21 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-26 0 0,28 54 343 0 0,15-18 88 0 0,20-2-135 0 0,94 33-1529 0 0,-139-64-94 0 0,-2-4-65 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:15:44.344"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">27 6 1208 0 0,'-4'-6'289'0'0,"3"6"8094"0"0,-2 14-7238 0 0,2-13-680 0 0,1 17 1541 0 0,-4 22-206 0 0,4-15-1476 0 0,-1 29 1078 0 0,-6 27 73 0 0,1 5-627 0 0,6-84-1179 0 0,0-2-137 0 0,0 0-767 0 0,0 0-3063 0 0,0 0-1315 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:15:44.664"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 3 3224 0 0,'14'10'573'0'0,"-13"-10"782"0"0,-1 0 461 0 0,0 0 82 0 0,11-3 3130 0 0,-10-1-4221 0 0,1-2-3150 0 0,-2 6 1465 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-04-15T12:15:50.085"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2 1 920 0 0,'0'0'295'0'0,"0"0"901"0"0,0 0 393 0 0,0 0 77 0 0,0 0-131 0 0,0 0-630 0 0,0 0-274 0 0,0 0-58 0 0,0 0-19 0 0,0 0-34 0 0,0 0-10 0 0,0 0-4 0 0,0 0-4 0 0,0 0-4 0 0,0 0-2 0 0,0 0 0 0 0,0 0-12 0 0,0 0-50 0 0,0 0-18 0 0,0 9 390 0 0,-1 36 705 0 0,5 33-228 0 0,-1-5-566 0 0,-5 27-297 0 0,-2-75-370 0 0,4-24-120 0 0,0-1 2 0 0,0 0-58 0 0,0 0-264 0 0,0 0-111 0 0,0-1-1130 0 0,0-7-4448 0 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,25 +2858,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="90.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.73046875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="3" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -728,7 +2891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>43557</v>
       </c>
@@ -738,17 +2901,15 @@
       <c r="C2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="4">
         <v>0.3263888888888889</v>
@@ -756,9 +2917,8 @@
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="4">
         <v>0.36805555555555558</v>
@@ -770,7 +2930,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="4">
         <v>0.4548611111111111</v>
@@ -778,9 +2938,8 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="4">
         <v>0.46527777777777773</v>
@@ -792,7 +2951,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="4">
         <v>0.47222222222222227</v>
@@ -804,7 +2963,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="B9" s="4">
         <v>0.52777777777777779</v>
@@ -816,23 +2975,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
       <c r="B12" s="4">
         <v>0.59027777777777779</v>
@@ -840,17 +2997,15 @@
       <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
       <c r="B14" s="4">
         <v>0.66319444444444442</v>
@@ -862,7 +3017,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="4">
         <v>0.66666666666666663</v>
@@ -870,9 +3025,8 @@
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
       <c r="B16" s="4">
         <v>0.68402777777777779</v>
@@ -880,9 +3034,8 @@
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="4">
         <v>0.6875</v>
@@ -890,9 +3043,8 @@
       <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>43558</v>
       </c>
@@ -902,9 +3054,8 @@
       <c r="C18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
       <c r="B19" s="4">
         <v>0.33333333333333331</v>
@@ -912,17 +3063,15 @@
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="4">
         <v>0.3611111111111111</v>
@@ -930,9 +3079,8 @@
       <c r="C21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="4">
         <v>0.375</v>
@@ -940,9 +3088,8 @@
       <c r="C22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
       <c r="B23" s="4">
         <v>0.4201388888888889</v>
@@ -950,9 +3097,8 @@
       <c r="C23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="4">
         <v>0.52777777777777779</v>
@@ -964,7 +3110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
       <c r="B25" s="4">
         <v>0.55208333333333337</v>
@@ -972,9 +3118,8 @@
       <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="2" t="s">
@@ -984,15 +3129,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="4">
         <v>0.59375</v>
@@ -1004,7 +3148,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
       <c r="B29" s="4">
         <v>0.61458333333333337</v>
@@ -1012,9 +3156,8 @@
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" s="4">
         <v>0.66666666666666663</v>
@@ -1022,9 +3165,8 @@
       <c r="C30" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
       <c r="B31" s="4">
         <v>0.69444444444444453</v>
@@ -1032,9 +3174,8 @@
       <c r="C31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="3">
         <v>43559</v>
       </c>
@@ -1044,9 +3185,8 @@
       <c r="C32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="2"/>
       <c r="B33" s="4">
         <v>0.3263888888888889</v>
@@ -1058,15 +3198,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="2"/>
       <c r="B35" s="4">
         <v>0.41666666666666669</v>
@@ -1074,9 +3213,8 @@
       <c r="C35" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="2"/>
       <c r="B36" s="4">
         <v>0.44097222222222227</v>
@@ -1084,9 +3222,8 @@
       <c r="C36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="2"/>
       <c r="B37" s="4">
         <v>0.52777777777777779</v>
@@ -1094,9 +3231,8 @@
       <c r="C37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="2"/>
       <c r="B38" s="4">
         <v>0.54166666666666663</v>
@@ -1104,9 +3240,8 @@
       <c r="C38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="2"/>
       <c r="B39" s="4">
         <v>0.5625</v>
@@ -1118,7 +3253,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A40" s="2"/>
       <c r="B40" s="4">
         <v>0.67361111111111116</v>
@@ -1126,9 +3261,8 @@
       <c r="C40" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="2"/>
       <c r="B41" s="4">
         <v>0.69444444444444453</v>
@@ -1136,9 +3270,8 @@
       <c r="C41" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="3">
         <v>43560</v>
       </c>
@@ -1148,9 +3281,8 @@
       <c r="C42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="2"/>
       <c r="B43" s="4">
         <v>0.34722222222222227</v>
@@ -1158,9 +3290,8 @@
       <c r="C43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="2"/>
       <c r="B44" s="4">
         <v>0.39583333333333331</v>
@@ -1168,9 +3299,8 @@
       <c r="C44" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="2"/>
       <c r="B45" s="4">
         <v>0.47916666666666669</v>
@@ -1178,9 +3308,8 @@
       <c r="C45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="3">
         <v>43563</v>
       </c>
@@ -1190,9 +3319,8 @@
       <c r="C46" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A47" s="2"/>
       <c r="B47" s="4">
         <v>0.31944444444444448</v>
@@ -1200,9 +3328,8 @@
       <c r="C47" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="2"/>
       <c r="B48" s="4">
         <v>0.375</v>
@@ -1210,9 +3337,8 @@
       <c r="C48" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A49" s="2"/>
       <c r="B49" s="4"/>
       <c r="C49" s="2" t="s">
@@ -1222,7 +3348,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
@@ -1232,7 +3358,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="2"/>
       <c r="B51" s="4">
         <v>0.52777777777777779</v>
@@ -1240,9 +3366,8 @@
       <c r="C51" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
@@ -1252,15 +3377,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="2"/>
       <c r="B53" s="4"/>
       <c r="C53" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A54" s="2"/>
       <c r="B54" s="4">
         <v>0.61805555555555558</v>
@@ -1268,9 +3392,8 @@
       <c r="C54" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
@@ -1280,7 +3403,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A56" s="2"/>
       <c r="B56" s="4"/>
       <c r="C56" s="2" t="s">
@@ -1290,7 +3413,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="2"/>
       <c r="B57" s="4">
         <v>0.66666666666666663</v>
@@ -1298,9 +3421,8 @@
       <c r="C57" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="2"/>
       <c r="B58" s="4">
         <v>0.68055555555555547</v>
@@ -1308,9 +3430,8 @@
       <c r="C58" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="3">
         <v>43564</v>
       </c>
@@ -1320,9 +3441,8 @@
       <c r="C59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
@@ -1332,7 +3452,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="2"/>
       <c r="B61" s="4">
         <v>0.34375</v>
@@ -1340,9 +3460,8 @@
       <c r="C61" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="2"/>
       <c r="B62" s="4">
         <v>0.4201388888888889</v>
@@ -1350,9 +3469,8 @@
       <c r="C62" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="2"/>
       <c r="B63" s="4">
         <v>0.45833333333333331</v>
@@ -1360,49 +3478,41 @@
       <c r="C63" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
+    </row>
+    <row r="64" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B64" s="4">
         <v>0.52777777777777779</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B65" s="4"/>
       <c r="C65" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B66" s="7">
         <v>0.66666666666666663</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B67" s="7">
         <v>0.6875</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="3"/>
       <c r="B68" s="7">
         <v>0.70138888888888884</v>
@@ -1410,9 +3520,8 @@
       <c r="C68" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="3">
         <v>43565</v>
       </c>
@@ -1422,159 +3531,240 @@
       <c r="C69" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B70" s="7">
         <v>0.3611111111111111</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B71" s="7">
         <v>0.375</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B72" s="7">
         <v>0.43402777777777773</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B73" s="7">
         <v>0.4513888888888889</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C74" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C75" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="6"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C76" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B77" s="7">
         <v>0.6875</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
+      <c r="C77" s="2" t="str">
+        <f>+C87</f>
+        <v>Alanyse Critère 7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A78" s="9">
         <v>43566</v>
       </c>
-      <c r="B78" s="9">
+      <c r="B78" s="7">
         <v>0.3125</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="9">
+      <c r="C78" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B79" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B80" s="9">
+      <c r="C79" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B80" s="7">
         <v>0.35416666666666669</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="9">
+      <c r="D80" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B81" s="7">
         <v>0.54166666666666663</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="1" t="s">
+      <c r="D81" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C82" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B83" s="9">
+    <row r="83" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B83" s="7">
         <v>0.56944444444444442</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="9">
+      <c r="D83" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B84" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B85" s="7">
         <v>0.625</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C85" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="9">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B86" s="7">
         <v>0.65277777777777779</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87" s="9">
+        <v>43567</v>
+      </c>
+      <c r="B87" s="7">
+        <v>0.3125</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B88" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B89" s="7">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90" s="9">
+        <v>43568</v>
+      </c>
+      <c r="B90" s="7">
+        <v>0.3125</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C91" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B92" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B93" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B94" s="7">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B95" s="7">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C96" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C97" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C98" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D52" r:id="rId1"/>
+    <hyperlink ref="D52" r:id="rId1" xr:uid="{3ABE7781-7A63-49E3-B7D9-7A926D777280}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1583,159 +3773,217 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C13" sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="49.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="49.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="49.42578125" style="1"/>
+    <col min="1" max="1" width="5.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1328125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="49.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="B12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405881BC-250B-44EF-9833-781DFFD746B9}">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="103.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified logook and documentation
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="548" documentId="14_{9F97C56A-0847-4B13-96CB-9482C5495C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0D5468C6-F240-4EBD-A5D0-C6E37A451C5E}"/>
+  <xr:revisionPtr revIDLastSave="581" documentId="14_{9F97C56A-0847-4B13-96CB-9482C5495C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7D68FEF2-323C-4779-8FC8-A381F2E88FFB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal De Bord" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="122">
   <si>
     <t>Documentation</t>
   </si>
@@ -394,6 +394,18 @@
   </si>
   <si>
     <t>Rendre 2 fichier séparées</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>PhpStorm génère automatiquement les PDF</t>
+  </si>
+  <si>
+    <t>Discution avec Mme Travjnak</t>
+  </si>
+  <si>
+    <t>Admin dans DB ?</t>
   </si>
 </sst>
 </file>
@@ -469,11 +481,11 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -638,8 +650,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>13995</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="288" name="Encre 287">
@@ -658,7 +670,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="288" name="Encre 287">
@@ -768,8 +780,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>61620</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="324" name="Encre 323">
@@ -788,7 +800,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="324" name="Encre 323">
@@ -898,8 +910,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>48165</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="39" name="Encre 38">
@@ -918,7 +930,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="39" name="Encre 38">
@@ -963,8 +975,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>34740</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="40" name="Encre 39">
@@ -983,7 +995,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="40" name="Encre 39">
@@ -1028,8 +1040,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>108375</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="41" name="Encre 40">
@@ -1048,7 +1060,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="41" name="Encre 40">
@@ -1093,8 +1105,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>71190</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="42" name="Encre 41">
@@ -1113,7 +1125,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="42" name="Encre 41">
@@ -1158,8 +1170,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>18015</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="212" name="Encre 211">
@@ -1178,7 +1190,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="212" name="Encre 211">
@@ -1223,8 +1235,8 @@
       <xdr:row>47</xdr:row>
       <xdr:rowOff>180255</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="873" name="Encre 872">
@@ -1243,7 +1255,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="873" name="Encre 872">
@@ -1288,8 +1300,8 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="877" name="Encre 876">
@@ -1308,7 +1320,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="877" name="Encre 876">
@@ -1353,8 +1365,8 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="880" name="Encre 879">
@@ -1373,7 +1385,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="880" name="Encre 879">
@@ -1418,8 +1430,8 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>88560</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="885" name="Encre 884">
@@ -1438,7 +1450,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="885" name="Encre 884">
@@ -1483,8 +1495,8 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="886" name="Encre 885">
@@ -1503,7 +1515,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="886" name="Encre 885">
@@ -1548,8 +1560,8 @@
       <xdr:row>49</xdr:row>
       <xdr:rowOff>69615</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="914" name="Encre 913">
@@ -1568,7 +1580,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="914" name="Encre 913">
@@ -1816,7 +1828,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">100 9 3224 0 0,'0'0'457'0'0,"0"0"711"0"0,0 0 311 0 0,0 0 66 0 0,0 0-146 0 0,0 0-671 0 0,0 0-295 0 0,0 0-60 0 0,0 0 9 0 0,0 0 83 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,0 0 102 0 0,0 0 22 0 0,0 14 1235 0 0,-10 56 4955 0 0,4 25-4234 0 0,17 7-97 0 0,-9-47-1040 0 0,-3-28-1012 0 0,0 47-267 0 0,-5 173 1877 0 0,1-157-1879 0 0,6-81-48 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-4 6 0 0 0,-11 12-801 0 0,-7-12-6747 0 0,18-17-982 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="412.915">107 87 2304 0 0,'0'-2'167'0'0,"8"-15"2093"0"0,18-20 9580 0 0,0 22-10365 0 0,-22 12-1240 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,3 2-235 0 0,-2-1 218 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,3 5-217 0 0,5 9 528 0 0,-7-11-392 0 0,1 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0 3-135 0 0,-3 105 1604 0 0,-35-42-855 0 0,31-71-713 0 0,-1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1-35 0 0,1-1-135 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-4-5 136 0 0,6 5-520 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 521 0 0,-5-25-2538 0 0,5 6-19 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="412.914">107 87 2304 0 0,'0'-2'167'0'0,"8"-15"2093"0"0,18-20 9580 0 0,0 22-10365 0 0,-22 12-1240 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,3 2-235 0 0,-2-1 218 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,3 5-217 0 0,5 9 528 0 0,-7-11-392 0 0,1 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0 3-135 0 0,-3 105 1604 0 0,-35-42-855 0 0,31-71-713 0 0,-1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1-35 0 0,1-1-135 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-4-5 136 0 0,6 5-520 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 521 0 0,-5-25-2538 0 0,5 6-19 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1848,7 +1860,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">67 100 10592 0 0,'0'0'818'0'0,"-3"11"2010"0"0,-12 32 2029 0 0,4 26-1721 0 0,0 16-649 0 0,-5 116 1221 0 0,12-81-2576 0 0,4 10-475 0 0,-3-113-1193 0 0,2-16-68 0 0,1-1-32 0 0,0 0-79 0 0,0 0-314 0 0,-2-14-8176 0 0,1 8 1651 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="332.093">71 90 11520 0 0,'5'-10'1224'0'0,"26"-25"6290"0"0,34 0-4470 0 0,-62 33-2967 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 2-77 0 0,4 15 316 0 0,0-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-1 0-1 0 0,-1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-2 4-316 0 0,2-13 99 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,-3 5-100 0 0,5-11 18 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-18 0 0,-2-1-59 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-7-4 59 0 0,-47-32-3704 0 0,55 30 957 0 0,5-1-5943 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="332.092">71 90 11520 0 0,'5'-10'1224'0'0,"26"-25"6290"0"0,34 0-4470 0 0,-62 33-2967 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 2-77 0 0,4 15 316 0 0,0-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-1 0-1 0 0,-1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-2 4-316 0 0,2-13 99 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,-3 5-100 0 0,5-11 18 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-18 0 0,-2-1-59 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-7-4 59 0 0,-47-32-3704 0 0,55 30 957 0 0,5-1-5943 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1916,251 +1928,251 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">21037 6597 0 0 0,'0'0'580'0'0,"0"0"-64"0"0,0 0 47 0 0,0 0-35 0 0,0 0-254 0 0,0 0-107 0 0,0 0-27 0 0,0 0 51 0 0,0 0 229 0 0,0 0 100 0 0,0 2 21 0 0,3 14 472 0 0,-3-14-554 0 0,0-2-3 0 0,0 0-54 0 0,0 0-223 0 0,0 0-98 0 0,0 0 51 0 0,0 0 272 0 0,0 0 95 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 0 0 0,0 6 0 0 0,0-7 0 0 0,0-1 0 0 0,0 0 36 0 0,0 0 150 0 0,0 0 66 0 0,0 0 18 0 0,0 0-29 0 0,0 7 436 0 0,2 51 2189 0 0,-4 65-643 0 0,-8-38-852 0 0,-6 69-1718 0 0,15-52-165 0 0,0-94 90 0 0,0 2-403 0 0,1 7-2730 0 0,-4-28-1033 0 0,0 1-2741 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="208.461">21033 6655 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,7-3-112 0 0,0 0 125 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 0-346 0 0,43 70 1246 0 0,-46-66-1102 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,-1-1-1 0 0,0 2-143 0 0,2-4 57 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-57 0 0,-84-6-816 0 0,57-14-3738 0 0,26 11 2908 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66203E6">22394 15965 456 0 0,'21'-42'0'0'0,"-7"27"2824"0"0,-6 4 664 0 0,-7 11-2678 0 0,-1 0 44 0 0,0 0 11 0 0,0 0 6 0 0,0 0 21 0 0,0 0 85 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,3-21 2411 0 0,-16 1-1851 0 0,12 18-1397 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-2 1-117 0 0,-3 2 139 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-3 7-139 0 0,-18 35 224 0 0,-4 47 448 0 0,28 4 696 0 0,2-95-1368 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0 0 0 0,-2-1 16 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,0 0-16 0 0,3 0-124 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 125 0 0,11-6-613 0 0,17-16-2912 0 0,-17 11 1494 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66247E6">22712 15647 5984 0 0,'2'-42'472'0'0,"0"1"5162"0"0,-2 39-3819 0 0,0 2-663 0 0,0 0-288 0 0,0 0-58 0 0,0 0-20 0 0,0 0-61 0 0,0 0-21 0 0,0 0-7 0 0,-8 5 1975 0 0,-15 110 1356 0 0,-26 212-3264 0 0,27-143-640 0 0,7-30-1060 0 0,14-138-1236 0 0,1-11-5747 0 0,0-5 911 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66269E6">22661 15829 9216 0 0,'0'0'706'0'0,"0"0"-114"0"0,4-5 3675 0 0,17-11 1993 0 0,15 6-3644 0 0,11-5-1858 0 0,5 19-1979 0 0,-47 6-2143 0 0,-2-2 1389 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.65162E6">21472 15394 6304 0 0,'13'-2'822'0'0,"-13"1"-83"0"0,0 1 249 0 0,0 0 48 0 0,0 0-31 0 0,0 0-170 0 0,0 0-71 0 0,0 0-17 0 0,0 0-27 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0 48 0 0,0 0 202 0 0,0 0 87 0 0,0 0 20 0 0,0 0-70 0 0,0 0-308 0 0,-1-1-137 0 0,-45-66 1234 0 0,-27 2 383 0 0,68 62-1902 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0 1 1 0 0,-4 2-14 0 0,-28 32 373 0 0,8 3-682 0 0,-12 57 985 0 0,25-17-666 0 0,-1 47 460 0 0,16 8-108 0 0,11-13-298 0 0,18 17-7518 0 0,-25-133 13 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.65193E6">21050 15795 11976 0 0,'0'0'546'0'0,"4"-11"204"0"0,13 4 2195 0 0,33-7 2019 0 0,23-3-3091 0 0,-34 19-1743 0 0,0 2 0 0 0,0 1 1 0 0,24 8-131 0 0,-19 1-3223 0 0,-31-10 2016 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.65267E6">21518 16009 920 0 0,'1'-3'80'0'0,"-1"2"-114"0"0,8-20 1775 0 0,19-25 8599 0 0,-13 35-9435 0 0,-2 3-70 0 0,-10 6-714 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 2-121 0 0,28 31 1528 0 0,-17 30 812 0 0,-16-55-2114 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1-226 0 0,0-4 108 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-5 1-108 0 0,6-3-56 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-2 56 0 0,1-35-2485 0 0,3 21 635 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66074E6">21836 15825 9616 0 0,'0'0'216'0'0,"0"0"32"0"0,1-2 12 0 0,8-23 16 0 0,8-32 4156 0 0,-17 55-3764 0 0,0 2 151 0 0,0 0 69 0 0,0 0 10 0 0,0 0-48 0 0,0 0-216 0 0,0 0-98 0 0,0 0-22 0 0,-7 62 3070 0 0,3-7-2456 0 0,-11 163 920 0 0,15-149-2048 0 0,-1-22-64 0 0,1-46-273 0 0,0-1-138 0 0,0 0-33 0 0,0 0-217 0 0,0-8-2919 0 0,1-5 1541 0 0,2 0-9 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.66115E6">21783 15975 10136 0 0,'0'0'42'0'0,"0"1"-1"0"0,0-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-42 0 0,27-34 4246 0 0,11 4-1699 0 0,-34 26-2345 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,3 0-202 0 0,26 18 1351 0 0,-29-11-1230 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 5-121 0 0,23 82 144 0 0,-16 1-545 0 0,-17-79-269 0 0,4-12-1904 0 0,0-3-3466 0 0,0 0-762 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67256E6">22983 16006 456 0 0,'10'-3'13004'0'0,"-6"12"-6955"0"0,-7 21-4332 0 0,1-15-273 0 0,6 101-283 0 0,-2-75-2968 0 0,0 0-3416 0 0,-2-41-2002 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67278E6">23059 15640 5984 0 0,'0'0'273'0'0,"0"0"-5"0"0,0 0 121 0 0,0 0 1143 0 0,0 0 514 0 0,0 0 104 0 0,0 0-119 0 0,0 0-596 0 0,0 0-261 0 0,0 0-49 0 0,0 0-98 0 0,0 0-392 0 0,0 0-171 0 0,0 0-31 0 0,0 0-64 0 0,0 0-1670 0 0,0 0-5837 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67316E6">23190 16279 11232 0 0,'0'-4'1016'0'0,"-17"-78"3747"0"0,27 11-109 0 0,-8 63-4545 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0 0 0 0 0,3-2-109 0 0,-6 4 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,14 41 10 0 0,-16-33 52 0 0,-5 50 1898 0 0,-33 28-1744 0 0,34-85-173 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-3-1-43 0 0,2-1-36 0 0,-1 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0-2 36 0 0,5-35-2989 0 0,1 25 1539 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67411E6">23565 16057 456 0 0,'0'0'83'0'0,"0"0"42"0"0,0 0 131 0 0,0 0 32 0 0,0 0 0 0 0,0 0 49 0 0,0 0 209 0 0,0 0 94 0 0,0 0 21 0 0,0 0-5 0 0,0 0-33 0 0,0 0-14 0 0,0 0-1 0 0,0 0-74 0 0,0 0-307 0 0,0 0-135 0 0,0-1-36 0 0,9-36 684 0 0,-2-6 547 0 0,-4 18-691 0 0,-3-25 2561 0 0,0 49-2790 0 0,0 1 1 0 0,0 0 0 0 0,0 7 8134 0 0,-3 27-7718 0 0,-10 123 1476 0 0,0-85-2207 0 0,13-63-53 0 0,0-3-32 0 0,0-4-137 0 0,0-2-71 0 0,0 0-16 0 0,0 0-147 0 0,0 0-589 0 0,0 0-257 0 0,0 0-51 0 0,0 0-35 0 0,0 0-102 0 0,2 14-5517 0 0,-2-14 5738 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.67441E6">23571 16099 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,0 0-140 0 0,0 0 368 0 0,0 0 187 0 0,0 0 42 0 0,-6-6 963 0 0,5 1-1582 0 0,1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,3-2-240 0 0,-5 5 154 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1-153 0 0,7 3 222 0 0,16 17-38 0 0,-4 7-184 0 0,-18-24 130 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2 5-130 0 0,3 32 130 0 0,3-17-130 0 0,0-20-97 0 0,20-10-2811 0 0,-17 1 1087 0 0,0-2-377 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1576.986">20599 6498 4608 0 0,'0'0'353'0'0,"5"11"155"0"0,-3-7 2425 0 0,8 26 3145 0 0,-8-6-3733 0 0,-11 20 1085 0 0,1 16-1742 0 0,3-7-736 0 0,9 42-312 0 0,-7-15-640 0 0,6-23 0 0 0,-14-10 0 0 0,11-42-9 0 0,0 0-146 0 0,0-1-4162 0 0,0-4-2729 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-759.689">20586 6796 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,4-3 272 0 0,0 1 2425 0 0,8-14-1132 0 0,6 6-314 0 0,-17 10-1141 0 0,9-10 879 0 0,24-21 835 0 0,9 14-867 0 0,-42 17-985 0 0,7-2 305 0 0,36 14-1282 0 0,-35-5 625 0 0,-6 27 186 0 0,-7 3 15 0 0,1-9 170 0 0,-4 11-74 0 0,6-37-411 0 0,1-2-12 0 0,0 0 37 0 0,2 10 308 0 0,15 9-12 0 0,-16-18-372 0 0,6 16-262 0 0,-1 10-1153 0 0,-5-26 785 0 0,-1-1-831 0 0,0 0-363 0 0,0 0-70 0 0,0 0-17 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2740.811">20168 6625 2304 0 0,'2'0'473'0'0,"3"-1"1939"0"0,-5 6 6695 0 0,-1 1-5123 0 0,2 1-5610 0 0,-4 32 3901 0 0,5 2 62 0 0,4 56-84 0 0,6 4-1147 0 0,-3-10 156 0 0,-9 11-32 0 0,-9 11-700 0 0,11-100-583 0 0,-2-12-216 0 0,0-1-65 0 0,0-2-2 0 0,2-34-3313 0 0,-6 23 1834 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2395.417">20188 6649 6912 0 0,'-11'-8'528'0'0,"27"-1"-128"0"0,6-10 4668 0 0,32 17 409 0 0,-51 2-5324 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 2-153 0 0,32 70 2062 0 0,-22 6-1603 0 0,-13-2 1130 0 0,-1-72-1534 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0-55 0 0,-24 5 67 0 0,28-10-206 0 0,-2 0-58 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-2-1 198 0 0,-4-4-5692 0 0,-5-2-1767 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.36359E6">3097 14549 7488 0 0,'0'2'340'0'0,"-6"99"3520"0"0,12 112 4791 0 0,-5 31-4784 0 0,5-61-3019 0 0,4-73-648 0 0,1-67-288 0 0,-11-41-387 0 0,0-2-33 0 0,0 0-192 0 0,0 0-790 0 0,0-5-352 0 0,2-20-70 0 0,-2-4-7 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.36416E6">3141 14647 8288 0 0,'-3'16'381'0'0,"2"-13"-6"0"0,8-34-227 0 0,-6 15 279 0 0,1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,5-6-427 0 0,-8 13 230 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 1 0 0 0,2-1-230 0 0,49-1 1008 0 0,-53 5-919 0 0,1 1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,4 4-89 0 0,1 4 277 0 0,-2-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 7-277 0 0,8 88 608 0 0,-8-97-471 0 0,-2 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,-1 3-136 0 0,0-7 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-3 0 0 0 0,-10 7 0 0 0,-25 1 0 0 0,38-13-8 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-2-1 8 0 0,-24-49-411 0 0,30 56 334 0 0,2 1 10 0 0,0 0 3 0 0,0 0 0 0 0,11 5-105 0 0,-6-1 109 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 2 60 0 0,15 22-246 0 0,39 55 1336 0 0,-36-52-896 0 0,1-2 0 0 0,1-1 1 0 0,2-1-1 0 0,7 6-194 0 0,-14-15-3 0 0,68 45-2666 0 0,-73-57 1330 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.37444E6">3876 15198 920 0 0,'0'0'327'0'0,"0"0"1035"0"0,0 9 2340 0 0,-1-6-656 0 0,0 23 2742 0 0,5-12-4840 0 0,-2-12-526 0 0,-2-2-26 0 0,0 0 12 0 0,0 0 68 0 0,0 0 32 0 0,1 1 4 0 0,41 6 1536 0 0,-5-3-1138 0 0,17-63-236 0 0,26-34 437 0 0,-44 22-618 0 0,-16 6-757 0 0,-20 63 329 0 0,1 0-31 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1-34 0 0,-4 0 41 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,-2 1-40 0 0,-20 12 98 0 0,21-13-115 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 3 17 0 0,-16 41 618 0 0,13 24-194 0 0,25 34-1082 0 0,-13-101 704 0 0,1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1-2 1 0 0,3 1-47 0 0,36-5-792 0 0,-46 4 622 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-2 170 0 0,12-9-5654 0 0,-2 7-1513 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.37552E6">4652 14839 1376 0 0,'0'0'65'0'0,"0"0"287"0"0,0 0 1184 0 0,0 0 522 0 0,0 0 100 0 0,0 0-171 0 0,0-15 1609 0 0,16-86 4054 0 0,-9 72-6749 0 0,-7 26-797 0 0,0-4-41 0 0,0 6-160 0 0,0 1-19 0 0,0 0 92 0 0,0 0 344 0 0,0 0 154 0 0,0 0 34 0 0,0 0-97 0 0,0 0-403 0 0,0 0-59 0 0,0 0 127 0 0,0 0 15 0 0,0 0 21 0 0,0 0 128 0 0,0 1 59 0 0,-7 71 675 0 0,-13 52-478 0 0,8-31-496 0 0,2 80 642 0 0,9 81-1033 0 0,-2-174 1100 0 0,-4-19-1141 0 0,7-59 208 0 0,-6 0-1960 0 0,5-1 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.37579E6">4636 14955 12696 0 0,'10'-14'1376'0'0,"36"8"1778"0"0,12-5 1363 0 0,1 2-3125 0 0,4 23-1540 0 0,-42-7-2470 0 0,-15-2-4791 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.49339E6">5661 15296 8288 0 0,'13'-33'1072'0'0,"24"-2"4316"0"0,-33 34-5186 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 3-203 0 0,3 4 280 0 0,-1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 6-281 0 0,-1-10 347 0 0,2-5-303 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1 1-44 0 0,1-1 8 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-2 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-8 0 0,-4-3-53 0 0,1 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-2-4 53 0 0,4 9-246 0 0,0-2 1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-2 245 0 0,10-27-3579 0 0,-5 19-2927 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.49221E6">5110 15065 3224 0 0,'0'-2'240'0'0,"0"-2"25"0"0,0 3 855 0 0,0 1 359 0 0,0 0 66 0 0,0 0-81 0 0,0 0-397 0 0,0 0-178 0 0,0 0-32 0 0,0 0-13 0 0,0 0-24 0 0,0 0-10 0 0,0 0-2 0 0,0 0-18 0 0,0 0-74 0 0,4 31 1869 0 0,-11 146 1427 0 0,-4 4-2668 0 0,5-90-1106 0 0,6-90-198 0 0,1 20-364 0 0,-1-21 191 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 134 0 0,3-14-2091 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.49258E6">5124 15201 8288 0 0,'3'9'2948'0'0,"4"-25"1960"0"0,-3 7-5020 0 0,29-40 3418 0 0,17-5-299 0 0,-48 52-2908 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1-99 0 0,19 30 274 0 0,18 33 16 0 0,-2-8-146 0 0,-11-21 0 0 0,-23-25-597 0 0,-4-10-3304 0 0,-1-2 2223 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35574.03">17513 6632 11888 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 14 0 0,1 10 69 0 0,-2 75 4760 0 0,-5-16-2346 0 0,6-30-2146 0 0,-1-35-594 0 0,-3 29-145 0 0,2-22-10 0 0,1-9-188 0 0,1-2-789 0 0,0 0-344 0 0,0 0-65 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35139.521">17760 6635 2304 0 0,'-3'1'3435'0'0,"8"5"13324"0"0,-3-4-18570 0 0,11 96 5563 0 0,0 28-2624 0 0,-5-51-1128 0 0,-6-66-133 0 0,-1-8-563 0 0,-1-1-257 0 0,0 0-922 0 0,0 0-3642 0 0,0 0-1564 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-34747.75">17777 6762 1840 0 0,'0'0'83'0'0,"0"0"373"0"0,0 0 1526 0 0,0 0 670 0 0,0 0 131 0 0,2-1 950 0 0,9-6-2192 0 0,7-23 2196 0 0,-3 10-2845 0 0,-13 15-638 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,4-2-254 0 0,19 15 16 0 0,-23-6-15 0 0,43 50 773 0 0,-43-47-785 0 0,-4-7-105 0 0,12 4-2683 0 0,-13-5 751 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44644.387">16898 6448 3224 0 0,'-1'0'2310'0'0,"-1"1"10093"0"0,1 0-11285 0 0,1 2-3278 0 0,-13 169 7048 0 0,-10 34-3120 0 0,19-147-1645 0 0,5 48-583 0 0,2-100 325 0 0,-3-7-3458 0 0,0 0 1850 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44417.264">16835 6523 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,2 0-220 0 0,52 3 3130 0 0,50 25-834 0 0,-52-21-4427 0 0,-50-7-69 0 0,4 0-4147 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36024.581">17142 6868 2304 0 0,'0'0'348'0'0,"0"0"620"0"0,-8-5 2737 0 0,3-54-382 0 0,5 58-2754 0 0,-7-16 2487 0 0,2-43 2906 0 0,6 54-5754 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,1-1-207 0 0,-3 3-36 0 0,1-1 14 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,2 0 23 0 0,-2 0 21 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 2 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0-21 0 0,1 4 5 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 5-5 0 0,2-4 151 0 0,-1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,-2 3-151 0 0,5-8 28 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1-27 0 0,-3-3-27 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1 27 0 0,-5-55-3584 0 0,10 57 2142 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33796.383">18099 6861 456 0 0,'0'0'2349'0'0,"0"0"293"0"0,0 0 128 0 0,0 0-221 0 0,0 0-1013 0 0,0 0-448 0 0,0 0-89 0 0,0 0-30 0 0,4 8 1768 0 0,-1-5-2425 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0-312 0 0,52-6 2120 0 0,3-22-1296 0 0,-4-15-672 0 0,-21-2 656 0 0,-15-24-516 0 0,-33 14-160 0 0,12 52-153 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-2 1 22 0 0,-3 4 44 0 0,0 2 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-4 9-44 0 0,0-2 32 0 0,1 2-32 0 0,0 1 0 0 0,1 0 0 0 0,1-1 0 0 0,0 2 0 0 0,2-1 0 0 0,-1 9 0 0 0,3-22 8 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,3 7-8 0 0,10 5 88 0 0,39-11-2149 0 0,-19-14-6089 0 0,-22 3 1076 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33464.079">18542 6858 13824 0 0,'0'0'314'0'0,"-7"8"872"0"0,2 10-891 0 0,4-12 1764 0 0,-1-4 3765 0 0,7-3-5807 0 0,9-6-1723 0 0,-7 1-236 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-28557.543">17554 6394 4144 0 0,'0'0'319'0'0,"0"0"295"0"0,0 0 2022 0 0,0 0 904 0 0,0 0 185 0 0,0 0-408 0 0,0 0-1846 0 0,0 0-815 0 0,0 0-161 0 0,0 0-25 0 0,0 0 16 0 0,0 0 8 0 0,0 0 2 0 0,0 0-64 0 0,0 0-1313 0 0,0 0-4508 0 0,0 0-1916 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19052.719">18787 6598 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 6 160 0 0,3-3 8708 0 0,19 86-4943 0 0,-16 7-3675 0 0,-12-11-98 0 0,9-78-623 0 0,0-6-63 0 0,0-1-165 0 0,0 0-726 0 0,0 0-316 0 0,0 0-65 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-9426.741">19041 6482 920 0 0,'1'-1'67'0'0,"0"-4"143"0"0,0 4 814 0 0,-1 1 355 0 0,0 0 70 0 0,0 1 5373 0 0,0 3-3378 0 0,0 18-2234 0 0,11 164 4151 0 0,-9-31-3309 0 0,2-105-1683 0 0,-2-32-1984 0 0,0 0-3835 0 0,-2-18 3608 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-8994.302">19041 6649 3224 0 0,'0'6'527'0'0,"9"-31"8375"0"0,7-1-6343 0 0,-14 23-2627 0 0,0-1 178 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0-110 0 0,18 30 453 0 0,0 11 891 0 0,-17-24-1051 0 0,1 57 781 0 0,7 7 131 0 0,-4-38-1044 0 0,8-12-3885 0 0,-17-31 1631 0 0,-1-2-17 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7909.834">19600 6584 2760 0 0,'0'0'395'0'0,"0"0"617"0"0,0 0 274 0 0,0 0 53 0 0,0 0-86 0 0,0 0-380 0 0,0 0-163 0 0,0 0-36 0 0,0 0-28 0 0,0 0-85 0 0,5 0 260 0 0,-4-1 2703 0 0,-1 0-3426 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-98 0 0,-9 0 483 0 0,-28 6 677 0 0,-1 20-16 0 0,37-24-1069 0 0,-1 1-1 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,2 4-74 0 0,26 85 784 0 0,-17-66-634 0 0,-10-21-112 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1-38 0 0,-2-1-114 0 0,0 0 0 0 0,0-1 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,2-1 114 0 0,4-1-2547 0 0,0-4-5195 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7043.896">19830 6919 7112 0 0,'14'0'324'0'0,"-11"0"-4"0"0,-3 0-94 0 0,0 0 380 0 0,0 0 186 0 0,0 0 37 0 0,0 0 35 0 0,0 0 107 0 0,0 0 42 0 0,0 0 10 0 0,0 0-26 0 0,0 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-58 0 0,0 0-240 0 0,0 0-102 0 0,0 0-17 0 0,0 0-25 0 0,0 0-82 0 0,0 0-40 0 0,0 0-5 0 0,0 0-26 0 0,0 0-108 0 0,0 0-42 0 0,1-18-240 0 0,14 0 132 0 0,-15 17-8 0 0,0 1 88 0 0,0 0 35 0 0,0 0-18 0 0,-1 1-1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0-67 0 0,1 1-279 0 0,-1-2-186 0 0,0 0-42 0 0,0 0-209 0 0,0 0-857 0 0,0 0-379 0 0,0 0-80 0 0,0 0-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2101.423">18793 6250 13304 0 0,'0'0'605'0'0,"0"0"-9"0"0,0-1-381 0 0,-2-3-42 0 0,1 2 600 0 0,1 2 260 0 0,0 0 45 0 0,0 0-26 0 0,0 0-144 0 0,0 0-63 0 0,-3 20 1994 0 0,12-13-5523 0 0,-8-7-4821 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-307399.761">3589 799 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-120 0 0,0 0 193 0 0,-4-7 582 0 0,-43-24 3117 0 0,23 18-1623 0 0,-46-17-841 0 0,60 27-1311 0 0,1 1-1 0 0,-1 1 0 0 0,-1-1 1 0 0,1 2-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 1-1 0 0,1 1 0 0 0,-9 5-284 0 0,14-8 41 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 0-1 0 0,-1 2-40 0 0,5 8 100 0 0,1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0-100 0 0,-7-6 32 0 0,65 83-590 0 0,-58-70 602 0 0,0 2 1 0 0,-2-1-1 0 0,0 2 1 0 0,-1-1 0 0 0,0 1-1 0 0,-1 1 1 0 0,-1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-3 21-45 0 0,1-28 91 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 2-91 0 0,6-9 67 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,-5-3-68 0 0,6 1 4 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-2-5-4 0 0,0 1-603 0 0,0-1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-3 603 0 0,-4-11-1535 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-307011.559">3489 530 13680 0 0,'0'0'306'0'0,"-5"7"421"0"0,-1 6-534 0 0,-1 1-1 0 0,2 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 13-193 0 0,0-6 459 0 0,-9 65 963 0 0,3 1 0 0 0,4 0 0 0 0,3 0 0 0 0,5 56-1422 0 0,-10 68 1773 0 0,-6-14-700 0 0,0 109-1515 0 0,16-246-1557 0 0,-1-33 952 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-286862.719">3909 1565 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 0 0 0 0,0 0 200 0 0,0 0 24 0 0,-3-7 8 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-244252.177">4046 1922 1376 0 0,'0'0'65'0'0,"0"0"321"0"0,0 0 1322 0 0,0 0 578 0 0,0 0 119 0 0,-2 2 764 0 0,-6 7-2143 0 0,7-9-849 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1-177 0 0,-10-12 1364 0 0,-1-25 743 0 0,14 4-644 0 0,-11-28-661 0 0,11 41-733 0 0,0 0-1 0 0,1 0 1 0 0,1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,2 0 1 0 0,0 1-1 0 0,1 0 1 0 0,7-11-69 0 0,-6 9-213 0 0,23-24 417 0 0,-32 43-216 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,0 0 11 0 0,24 12-403 0 0,-12-11 372 0 0,1 10 529 0 0,-3-2 172 0 0,-9-6-605 0 0,1 0-1 0 0,-1-1 0 0 0,0 2 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 3-64 0 0,11 25-60 0 0,1 50 132 0 0,-7-47-67 0 0,-5-31 15 0 0,1 1 1 0 0,-1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 5-20 0 0,-5 17 568 0 0,7-28-650 0 0,-3 7-326 0 0,3-8 412 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-4 0 0,-1-27 743 0 0,14-38-633 0 0,-2 27-110 0 0,13-30 0 0 0,20-17-320 0 0,-14 45-430 0 0,-1 9 1668 0 0,11 3-918 0 0,-35 26-7 0 0,-2 1-32 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 38 0 0,-1-2 222 0 0,13 18 286 0 0,0 11-904 0 0,-2 22 920 0 0,-2 12-181 0 0,-6-25 197 0 0,-4 37-687 0 0,0-40 334 0 0,23 38-102 0 0,6-12-74 0 0,-27-58 31 0 0,1 1-20 0 0,27-6 135 0 0,-13-11 0 0 0,6-12-434 0 0,4-16 434 0 0,-18 23-314 0 0,2-1 685 0 0,5-11-776 0 0,-15 29 365 0 0,-1 1-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0 39 0 0,0 0 168 0 0,4-13-278 0 0,-3 10-5968 0 0,0 2-1741 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-243361.782">5063 1677 11288 0 0,'0'0'514'0'0,"-10"-10"196"0"0,8 8-539 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-171 0 0,36-47 2046 0 0,-27 41-1874 0 0,-7 6-154 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0-18 0 0,-1 1 60 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 1-60 0 0,-1 2 134 0 0,9 74 1428 0 0,-12-55-1106 0 0,-13 40 934 0 0,13-61-1313 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-5 2-77 0 0,-25-4 728 0 0,19-4-305 0 0,13 4-401 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-2-22 0 0,0-2-121 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 121 0 0,22-46-8730 0 0,-12 30 1471 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-234308.981">5554 1397 456 0 0,'-6'20'336'0'0,"0"0"10502"0"0,5-16-10470 0 0,1 54 5149 0 0,0 21-1998 0 0,10 55-1146 0 0,7-61-2293 0 0,13-24 752 0 0,-3-10-288 0 0,-20-32-468 0 0,2-6 16 0 0,29-4 116 0 0,8-22 32 0 0,-3-34-153 0 0,-15 14-38 0 0,-2 5-49 0 0,-6 14 0 0 0,14-38 64 0 0,-11 28-74 0 0,-14 26-44 0 0,2-20 54 0 0,-1 19 28 0 0,-4-8-2 0 0,3-4-69 0 0,-8 22 96 0 0,-3 19-9 0 0,-9 60-144 0 0,7-7 100 0 0,2-40 0 0 0,2 18 0 0 0,-8 45 254 0 0,-10-1-28 0 0,-10 29 293 0 0,6-57 286 0 0,15-40-797 0 0,-1 1 0 0 0,-1-2 1 0 0,-1 1-1 0 0,-1-2 0 0 0,-1 0 0 0 0,-7 10-8 0 0,9-18 52 0 0,0-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,0-1-1 0 0,-1 0 0 0 0,-4 2-51 0 0,11-8 15 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2-1-14 0 0,7 1-35 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-3 34 0 0,-1-2 20 0 0,10-79-2121 0 0,-9 53-659 0 0,0 19 1197 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-233142.626">6149 1779 1840 0 0,'1'-1'138'0'0,"-1"0"0"0"0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1-138 0 0,13 0 3296 0 0,36-8 1940 0 0,-32 1-4448 0 0,55-29 1921 0 0,-13-17-1408 0 0,-52 39-1068 0 0,-6 10-211 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 0-21 0 0,-1 0 9 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-4-1-9 0 0,-4-4-199 0 0,10 6 228 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0 1-1 0 0,-3-1-28 0 0,-13 5 307 0 0,15-5-243 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-2 3-64 0 0,0 3 118 0 0,-3 2 3 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1 0 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,0 7-121 0 0,1-10 43 0 0,1-1-1 0 0,0 0 1 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,3 4-43 0 0,2 0 29 0 0,26 22 88 0 0,-27-30-139 0 0,1-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,3-1 23 0 0,51-5-3801 0 0,-43 6 2362 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-231376.003">6705 1431 4832 0 0,'2'65'3666'0'0,"1"-43"-222"0"0,-2-21-2786 0 0,-2 34 2622 0 0,2 73 551 0 0,-1-43-3103 0 0,0 46 110 0 0,0-38-4281 0 0,0-72-1079 0 0,0-1-1230 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-230982.797">6695 1701 3680 0 0,'0'0'284'0'0,"0"-1"-187"0"0,0-2 155 0 0,2-12 5681 0 0,7-11-2141 0 0,-4 13-2532 0 0,-4 9-1000 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,0 0-260 0 0,28-20 850 0 0,-29 22-780 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 1-70 0 0,30 32 293 0 0,30 47 1327 0 0,-64-81-1617 0 0,3 3 19 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 2-22 0 0,10 56 581 0 0,-18-34-1430 0 0,6-21-1922 0 0,-2 0 1115 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-220476.757">7259 1444 6880 0 0,'0'0'314'0'0,"0"0"-6"0"0,0 0-77 0 0,0 0 409 0 0,0 0 199 0 0,0 0 38 0 0,0 0-32 0 0,0 0-173 0 0,0 0-80 0 0,0 0-14 0 0,0 0-2 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 6 0 0,0 0 30 0 0,7 14 2401 0 0,9 31-517 0 0,-15 36-102 0 0,-8-15-1028 0 0,4-53-1323 0 0,1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,0-1 1 0 0,2 6-35 0 0,1 56 86 0 0,0-18-106 0 0,-2-51 540 0 0,-2-5-4113 0 0,1 1-6903 0 0,0-2 5190 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-220015.405">7275 1646 1840 0 0,'0'0'403'0'0,"0"0"1018"0"0,0-5 1680 0 0,1 3 1760 0 0,27-60 991 0 0,-23 55-5592 0 0,0 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,2 0 1 0 0,1-1-260 0 0,-5 5 92 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 1-1 0 0,1 1-92 0 0,29 52 1184 0 0,-17-13-1184 0 0,-5 51 0 0 0,-7-47 848 0 0,-4-47-637 0 0,0-1-324 0 0,0 0-141 0 0,0 0-30 0 0,0 0-132 0 0,-5 8-4129 0 0,2-6-2469 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-218714.051">7763 1691 6304 0 0,'0'0'289'0'0,"0"0"-8"0"0,0 0-50 0 0,0 0 462 0 0,0 0 218 0 0,0 0 45 0 0,0 0-8 0 0,0 0-77 0 0,2 1-37 0 0,8 4 1041 0 0,-9-4-1679 0 0,1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1-197 0 0,61-48 1877 0 0,-7-8-1229 0 0,-48 43-648 0 0,-10 11 43 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,-3 1-43 0 0,2 0 15 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 2-15 0 0,-1 2 78 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0 7-78 0 0,0-7 84 0 0,0 4-20 0 0,1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1 0 0 0 0,1 0 0 0 0,1 4-64 0 0,30 101 743 0 0,-31-115-717 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,4-1-26 0 0,2-3-217 0 0,0-1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,4-8 217 0 0,23-19-3383 0 0,-22 24 1685 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-217159.938">8212 1886 1376 0 0,'0'0'65'0'0,"0"0"286"0"0,0 0 1176 0 0,0 0 510 0 0,0 0 105 0 0,0 0-140 0 0,0 0-688 0 0,0 0-303 0 0,0 0-62 0 0,0 0-31 0 0,0 0-86 0 0,10-8 1503 0 0,24-87 2243 0 0,-1 6-2552 0 0,36-61-1672 0 0,32-14 444 0 0,-47 72 85 0 0,-42 69-1159 0 0,-11 22 177 0 0,-1 1 151 0 0,0 0 68 0 0,0 0 10 0 0,6 10-109 0 0,4 75 56 0 0,-13-3-233 0 0,3 120 500 0 0,4 120-424 0 0,2-252-61 0 0,-6-69-590 0 0,0-1-241 0 0,-1-1-1406 0 0,-4-5-5471 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-216555.754">8279 1745 6448 0 0,'0'0'498'0'0,"4"-4"32"0"0,0 0 484 0 0,-3 3-660 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-354 0 0,55-13 3164 0 0,36 29-2595 0 0,-78-14-475 0 0,-3 0-1562 0 0,-3-1-3055 0 0,-1-1-2147 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-215887.433">8824 1619 920 0 0,'0'0'295'0'0,"0"0"901"0"0,-4-15 3639 0 0,2 13-5213 0 0,-3-1 8750 0 0,3 3-7138 0 0,1 0-721 0 0,-6 4 1698 0 0,-12 26-994 0 0,0 21-137 0 0,11 7 52 0 0,21 23 127 0 0,-12-77-1227 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,2 1-32 0 0,-2-1 21 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1-2-20 0 0,51-50-20 0 0,-12-29-456 0 0,-33 43-464 0 0,-22 7-1392 0 0,11 34-2925 0 0,1 0-1661 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-215158.946">9255 1298 2304 0 0,'0'1'167'0'0,"3"24"1727"0"0,-8-7 5773 0 0,-3 118 1948 0 0,5-16-6975 0 0,6-38-2192 0 0,1 76-376 0 0,2-76-72 0 0,4-2-3116 0 0,-10-79 1546 0 0,0-1-280 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-214871.79">9241 1531 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,1-2-344 0 0,25-21 826 0 0,7 17 3479 0 0,2-2-2907 0 0,11 2-1414 0 0,-23 9-2102 0 0,-13 0-4791 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213551.059">9666 1714 10136 0 0,'8'12'230'0'0,"-6"-10"30"0"0,-2-2 19 0 0,0 0 104 0 0,-3 20 7879 0 0,4-19-7647 0 0,-1-1-21 0 0,1 1-38 0 0,9-1-436 0 0,-1 1-1 0 0,0-2 0 0 0,1 1 1 0 0,-1-2-1 0 0,0 1 0 0 0,1-1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-2 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-2 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2-1-1 0 0,3-4-119 0 0,7-49 69 0 0,-14 60-69 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-3 0 0 0 0,1 1 61 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1-61 0 0,-48 58-543 0 0,45-53 613 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 7-70 0 0,2-8 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,5 4 0 0 0,-7-8-56 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 56 0 0,8-4-1098 0 0,1-2-56 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213242.538">10188 1541 4608 0 0,'-17'14'3105'0'0,"0"1"6005"0"0,10 0-7943 0 0,-4 9 1032 0 0,9 16-1221 0 0,-3 46 1209 0 0,4-78-2095 0 0,1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,2 1-92 0 0,2-3 0 0 0,-6-5 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,17-30 0 0 0,-3 0 0 0 0,0-1 0 0 0,-2-1 0 0 0,-1-2 0 0 0,-7 12 0 0 0,-14 8-1384 0 0,7 18 600 0 0,1 1-1144 0 0,0 0-496 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212663.88">10669 1482 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0 88 0 0,0 0 1067 0 0,0 0 483 0 0,0 0 98 0 0,0 0-138 0 0,0 0-670 0 0,0 0-295 0 0,0 0-60 0 0,0 0-101 0 0,0 0-377 0 0,0 0-167 0 0,0 0-31 0 0,-3 9 1448 0 0,0 92 1023 0 0,9-9-2584 0 0,-2-31 1296 0 0,2 92-752 0 0,-3-140-818 0 0,-2-12-854 0 0,-1-1-382 0 0,0 0-76 0 0,0 0-20 0 0,0 0-2 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212449.687">10689 1697 456 0 0,'-5'-9'365'0'0,"4"8"1529"0"0,1-6 6369 0 0,3-6-4715 0 0,16-27-181 0 0,-11 21-2471 0 0,-2 10-747 0 0,-5 7-63 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-85 0 0,-2 1 239 0 0,9 5 186 0 0,-6-3-373 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 4-52 0 0,6 6 0 0 0,-9-13-55 0 0,-1-1-16 0 0,5 5-460 0 0,-4-3-2608 0 0,-1-2-3526 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-206308.339">2652 2649 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,0 2-294 0 0,-5 8 6808 0 0,0-7-3282 0 0,-8-20-2050 0 0,13 16-1469 0 0,-10-98 2153 0 0,10-139-1048 0 0,-4 0-752 0 0,-6-56-24 0 0,-3 51-128 0 0,3-99-168 0 0,6 165 559 0 0,-8-52-726 0 0,8 94-532 0 0,-2 21 446 0 0,2 39-11 0 0,0 17 64 0 0,1 2 0 0 0,7-110 128 0 0,3 130-128 0 0,9 13 0 0 0,-9 20-4 0 0,0-1 1 0 0,0 2-1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,7 4 4 0 0,30 10 0 0 0,-22-8 79 0 0,1 0 0 0 0,-1-2-1 0 0,1-1 1 0 0,0-1-1 0 0,1-1-78 0 0,31-2-104 0 0,1-3 0 0 0,-1-3-1 0 0,1-3 1 0 0,51-15 104 0 0,348-68 0 0 0,-349 81 0 0 0,0 5 0 0 0,0 6 0 0 0,33 8 0 0 0,16-1 0 0 0,4-6 99 0 0,0-7-1 0 0,75-17-98 0 0,-99 9 64 0 0,95 6-64 0 0,-148 11 41 0 0,1 4-1 0 0,33 11-40 0 0,7 1 143 0 0,68 3 11 0 0,2-9-1 0 0,147-13-153 0 0,33-22 125 0 0,-265 16-98 0 0,141 4 106 0 0,162 32 123 0 0,-64-1-170 0 0,316-33 188 0 0,-287 23 29 0 0,-166-6-190 0 0,-55-3-38 0 0,141-12-75 0 0,31-13 0 0 0,-154 6 128 0 0,36 10-128 0 0,294 41 0 0 0,-423-42 0 0 0,32-18 64 0 0,54-20-160 0 0,-118 33 85 0 0,19 0-42 0 0,22-27 429 0 0,-58 29-376 0 0,-15 8 0 0 0,-2 4 0 0 0,9 17 0 0 0,-12 1 0 0 0,18 64 0 0 0,-11 4-189 0 0,-5 0-1 0 0,4 95 190 0 0,-8 12 307 0 0,5 187-618 0 0,-10 113 606 0 0,1-147-200 0 0,5-4-14 0 0,-6-153-6 0 0,-4-180-59 0 0,0-1 1 0 0,-1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,-3 9-17 0 0,5-23 9 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1-9 0 0,-43-2 22 0 0,1-3 0 0 0,0-1-1 0 0,1-4 1 0 0,-10-4-22 0 0,-82-17 52 0 0,-103 10-87 0 0,26 29 35 0 0,-324 9 0 0 0,-18-17 0 0 0,276 18 70 0 0,-13 17-70 0 0,-62 6 47 0 0,267-32-39 0 0,-363 18-5 0 0,-320-20-3 0 0,-313 30 240 0 0,583-43-256 0 0,106-15-48 0 0,20-7 64 0 0,-72 7 11 0 0,190 10 114 0 0,-68-27-85 0 0,-40-28-40 0 0,232 46 0 0 0,-14 7 0 0 0,-1 28 0 0 0,-35-12 0 0 0,76-8-100 0 0,99 4 7 0 0,7 3-64 0 0,0-1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1 156 0 0,1-10-10012 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202306.829">6824 2965 3224 0 0,'0'2'240'0'0,"17"57"4562"0"0,-7-10 530 0 0,-4-24-2824 0 0,-2 9-572 0 0,6 46 269 0 0,4 27-781 0 0,-1 49 0 0 0,4 111 552 0 0,-1-124-1272 0 0,8 153 568 0 0,-16-38-696 0 0,1-123-389 0 0,-2 41 722 0 0,-7-54-581 0 0,-3-2-93 0 0,6-5-91 0 0,-6 40-19 0 0,3-99-61 0 0,-4 85 0 0 0,0-107-64 0 0,4-28-67 0 0,0-5-281 0 0,0-1-129 0 0,0 0-31 0 0,0 0-72 0 0,-4-17-3152 0 0,1 2-2356 0 0,0-4-1623 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201855.109">6521 4734 12264 0 0,'0'0'273'0'0,"-5"14"786"0"0,5-4-595 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,3 5-464 0 0,-5-10 43 0 0,46 112 3185 0 0,26 119 95 0 0,-57-169-2734 0 0,3-1 0 0 0,23 57-589 0 0,18 11 416 0 0,-3-53-72 0 0,-47-71-248 0 0,0 0-1 0 0,0-1 0 0 0,1 0 1 0 0,0-1-1 0 0,0-1 1 0 0,12 7-96 0 0,-19-12 39 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-39 0 0,56-64 528 0 0,17-74-224 0 0,64-284-391 0 0,-129 389-257 0 0,22-56-4278 0 0,-29 83 2515 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186308.475">12549 1257 1840 0 0,'0'0'83'0'0,"0"1"-6"0"0,0 4 363 0 0,0-4 1761 0 0,0-1 766 0 0,1 19 5666 0 0,1-1-5371 0 0,1 18-970 0 0,-3-25-1727 0 0,-10 107 2961 0 0,-23 79-2557 0 0,36-156-1425 0 0,-3-41 48 0 0,0 0-940 0 0,0 0-410 0 0,1 0-88 0 0,4-5-10 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-185850.611">12876 1257 13040 0 0,'0'0'597'0'0,"0"0"-9"0"0,0 0-220 0 0,0 0 481 0 0,0 0 250 0 0,0-5 715 0 0,-1 4 3304 0 0,-4 3-5002 0 0,0 1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 3-116 0 0,0 2 121 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,3 4-120 0 0,43 111 0 0 0,-44-95 0 0 0,-7-24 0 0 0,0-5 60 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,-1-2-60 0 0,-4-4-110 0 0,7 7-9 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 119 0 0,1-7-1959 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-187118.879">11947 926 13184 0 0,'0'0'604'0'0,"0"0"-14"0"0,0 0-252 0 0,0 0 326 0 0,0 0 185 0 0,0 0 41 0 0,2 0-12 0 0,-1-1-747 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0-131 0 0,6 17 493 0 0,-2 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-2 0 1 0 0,1 18-493 0 0,-3-33 76 0 0,-2 91 1295 0 0,1 20-942 0 0,-5-17-247 0 0,-2 118-43 0 0,11-173-247 0 0,-2-43-448 0 0,-1-1-176 0 0,0 0-32 0 0,3-21-3836 0 0,-2 1 2544 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186774.862">12014 1320 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-79 0 0,0 0-421 0 0,0 0-180 0 0,0 0-37 0 0,0-14 1908 0 0,1 9-2997 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-346 0 0,12-9 712 0 0,-14 10-708 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,2 0-4 0 0,-1 0 90 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0 1-1 0 0,1 0-89 0 0,47 202 1931 0 0,-45-182-1912 0 0,-1 1 1 0 0,0-1-1 0 0,-2 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,-2 3-19 0 0,0 6-4294 0 0,2-35-4235 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184500.212">13244 1138 11976 0 0,'-3'2'1082'0'0,"-17"95"550"0"0,2 54 3297 0 0,12 52-1046 0 0,9-100-3866 0 0,4-75-17 0 0,-7-26-850 0 0,0 3 2050 0 0,0-2-4324 0 0,0 4-3781 0 0,0-7 913 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184054.319">13301 1182 3224 0 0,'0'0'143'0'0,"1"1"-3"0"0,3 4 390 0 0,12 11 9462 0 0,3-2-5178 0 0,-15-11-4675 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0-138 0 0,31 3-1260 0 0,-20-7 497 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-183416.48">13187 1271 5960 0 0,'-3'-8'266'0'0,"3"7"1"0"0,0-22 1002 0 0,9-17 3955 0 0,11-5-2882 0 0,-10-5-311 0 0,-8 47-2036 0 0,-6-14-175 0 0,0 13-433 0 0,4 4-2775 0 0,0 0 1855 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-182333.102">13541 1568 0 0 0,'0'0'2721'0'0,"0"0"-302"0"0,0 0 223 0 0,1-1-119 0 0,8-8-671 0 0,-8 7-1682 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0-170 0 0,5 2 296 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,2 8-296 0 0,7 44 792 0 0,-11-56-721 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,-2 2-71 0 0,4-4 2 0 0,-1 1 15 0 0,-1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,-1-1-18 0 0,0 1 49 0 0,-1-1 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1-1-1 0 0,1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0-2-49 0 0,2 3-126 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,2-4 126 0 0,12-34-3998 0 0,-2 22-3873 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-175901.286">13952 1537 4144 0 0,'0'0'191'0'0,"0"0"375"0"0,-4-9 14804 0 0,9 56-13610 0 0,2 19 8 0 0,3 26 351 0 0,-9-75-1781 0 0,7 22-3577 0 0,-8-38 1789 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172641.548">14618 1695 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,1 1-72 0 0,14 38 5565 0 0,-10-25-3129 0 0,0-12-2556 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-2-1 0 0,-1 1 0 0 0,4-4-209 0 0,59-64 153 0 0,-47 35-213 0 0,-19 35 61 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 0 0 0,0-1 2 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-3 1-2 0 0,-14 8 0 0 0,15-8 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-3 5 0 0 0,-4 11 27 0 0,5-11 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 2-27 0 0,1-5-27 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,4 5 28 0 0,14-1 0 0 0,20-20-1385 0 0,-29 3-166 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172385.72">15083 1719 11832 0 0,'-34'14'7253'0'0,"31"-12"-6259"0"0,3-1-12 0 0,0-1-29 0 0,0 0-122 0 0,0 0-482 0 0,0 0-205 0 0,0 0-44 0 0,0 0-7 0 0,0 0 17 0 0,0 0 8 0 0,0 0 2 0 0,0 0-237 0 0,0 0-996 0 0,0 0-434 0 0,1 0-86 0 0,4 0-21 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170574.713">15822 1121 2760 0 0,'0'0'589'0'0,"0"0"1434"0"0,0 0 626 0 0,0 0 126 0 0,0 0-214 0 0,0 8 88 0 0,0 171 4329 0 0,0 91-4387 0 0,-1-167-2591 0 0,-3 26 0 0 0,4-63 0 0 0,-3-3-134 0 0,3-62-570 0 0,0-1-263 0 0,0 0-916 0 0,0-1-3632 0 0,-2-5-1553 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170137.543">15788 1582 5064 0 0,'0'0'389'0'0,"2"-3"794"0"0,0 1 3071 0 0,24-31 3094 0 0,7-4-4244 0 0,18-4-1223 0 0,-46 40-1852 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 1-29 0 0,5 16 310 0 0,-2 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,-1 10-310 0 0,-7 90 1048 0 0,7-92-908 0 0,5-1-148 0 0,10-34-432 0 0,3-13-1437 0 0,2 1-5762 0 0,-8 5 145 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172102.041">15380 1364 9760 0 0,'3'-26'2366'0'0,"-3"25"-894"0"0,0 1 68 0 0,0 0-60 0 0,0 0-321 0 0,0 0-139 0 0,0 0-27 0 0,0 0-34 0 0,0 0-114 0 0,-2 6 736 0 0,-8 73 997 0 0,2 35-801 0 0,-6 76-1676 0 0,8-115-101 0 0,3 23 0 0 0,2-85 704 0 0,-1-2-2693 0 0,1 3-6478 0 0,1-14 756 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-171739.932">15410 1364 16064 0 0,'4'-14'1715'0'0,"-2"10"-1471"0"0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,3 0-244 0 0,-3 0 90 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,3 2-90 0 0,-2 7 116 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,-1 0 1 0 0,-4 9-116 0 0,-40 68 1297 0 0,47-86-1274 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1-22 0 0,-1-1-128 0 0,2 1 21 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,1 0 106 0 0,-1-10-1478 0 0,-2 2-66 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174133.091">14303 1415 4144 0 0,'0'0'319'0'0,"0"0"-7"0"0,0 0 751 0 0,0 0 355 0 0,0 0 71 0 0,0 0-42 0 0,0 0-234 0 0,0 0-101 0 0,0 0-21 0 0,0 19 3966 0 0,-9 4-3283 0 0,8-21-1264 0 0,1-2-29 0 0,0 2-8 0 0,-3 249 2166 0 0,-9-135-2099 0 0,7-62 33 0 0,-1 21-3333 0 0,7-76 56 0 0,1-8-4807 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173508.196">14267 1653 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,1-1 491 0 0,25-52 6288 0 0,-24 50-6862 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,1 1-157 0 0,0 0 54 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,1 1-53 0 0,0-6-149 0 0,4 18-2358 0 0,-4-9 487 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-169732.621">16337 1391 18287 0 0,'0'0'414'0'0,"0"0"56"0"0,0 1 32 0 0,0 84 1564 0 0,-11 58 154 0 0,1 10-612 0 0,4-20 14 0 0,-2-52-1333 0 0,8-80-974 0 0,0-1-274 0 0,0 0-53 0 0,0 0-215 0 0,0 0-858 0 0,0 0-379 0 0,1-2-80 0 0,2-13-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168923.508">16394 1507 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,3-7-322 0 0,3-4-3 0 0,-3 5 250 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1-1 0 0,1-1-460 0 0,-2 1 236 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 2-1 0 0,0-1 1 0 0,0 0-236 0 0,1 2 105 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,3 5-105 0 0,11 84 177 0 0,-26 79 1151 0 0,-10-109-745 0 0,17-62-571 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-2 0 0 0,1 1 0 0 0,-2-1-12 0 0,-3-2-508 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,-5-8 508 0 0,1 1-1504 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-130876.917">2833 6188 6448 0 0,'23'-2'672'0'0,"-20"1"-608"0"0,1 3 3996 0 0,-2 5-3602 0 0,-2-3 96 0 0,1-3 14 0 0,-3 12 453 0 0,8 165 2956 0 0,-11 72-1512 0 0,9-98-1338 0 0,3-73-1094 0 0,-4-70-94 0 0,-3-7-264 0 0,4-17-6236 0 0,-1 2 317 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-124973.04">2852 6239 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 0-79 0 0,0 0 561 0 0,0 0 272 0 0,-3 7 1195 0 0,-3-4 2766 0 0,7-10-4160 0 0,8-13-1197 0 0,-7 13 345 0 0,2 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,4 0-78 0 0,-6 2-15 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 15 0 0,20 116 716 0 0,-22-117-672 0 0,2 2 51 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-95 0 0,-33 27 236 0 0,30-30-233 0 0,-3 2 17 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-2 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,-9 0-20 0 0,-25-5-116 0 0,41 0 127 0 0,3 2 42 0 0,9 13-2 0 0,35 49-118 0 0,63 112 1347 0 0,-62-104-1908 0 0,-28-56-2350 0 0,-9-6-4791 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123928.98">3297 6776 3224 0 0,'0'0'143'0'0,"0"0"315"0"0,0 0 1222 0 0,0 0 531 0 0,0 0 106 0 0,0 0-213 0 0,0 0-968 0 0,0 0-428 0 0,5 10 1069 0 0,0-8-1546 0 0,1 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,3-2-231 0 0,-7 3-25 0 0,10-4 212 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1-1 1 0 0,-1 1-1 0 0,0-2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-2-186 0 0,-6 7 3 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-4-3 0 0,0 7 35 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-35 0 0,0-1 16 0 0,-1 1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1-16 0 0,-48 120 249 0 0,34-10-267 0 0,17-106 28 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,4 3-9 0 0,-5-6 6 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,5-1-6 0 0,-5 0 57 0 0,24-6-1613 0 0,-10 1-3577 0 0,-2-5-2072 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123239.429">3865 6319 920 0 0,'0'0'279'0'0,"0"0"833"0"0,0 0 362 0 0,0 0 78 0 0,0 0-63 0 0,0 0-322 0 0,0 0-140 0 0,0 0-31 0 0,0 0-26 0 0,0 0-88 0 0,0 0-40 0 0,0 0-8 0 0,0 0-34 0 0,0 0-136 0 0,0 0-66 0 0,0 0-12 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0-42 0 0,0 7-12 0 0,-9 47 1334 0 0,2 14-600 0 0,0 50 252 0 0,8 96-1210 0 0,2-96-216 0 0,7-13 642 0 0,-4-91-1088 0 0,-5-12-25 0 0,-1-2-998 0 0,0 0-429 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122817.09">3839 6537 12176 0 0,'0'0'561'0'0,"0"0"-17"0"0,2 1-217 0 0,77 9 5294 0 0,-10 9-5284 0 0,-10 9-2062 0 0,-57-28 475 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122538.437">4257 6834 2304 0 0,'-11'-8'3825'0'0,"9"5"-3248"0"0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-5-578 0 0,1 4 116 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0-116 0 0,-2 1 36 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 2-36 0 0,50 60 1232 0 0,-48-52-822 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,-1-1-1 0 0,0 2 1 0 0,0-1-1 0 0,-2 0 1 0 0,1 1 0 0 0,-1 9-410 0 0,-13 37 100 0 0,11-57-42 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 1-58 0 0,-2-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-4-3 0 0 0,-30-45-1424 0 0,29 25-5473 0 0,4 13-533 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121496.511">4622 6625 15176 0 0,'0'0'340'0'0,"0"0"50"0"0,-2 1 26 0 0,-13 19 101 0 0,12-16-271 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0-245 0 0,3 57-21 0 0,42 58 1584 0 0,-42-115-1524 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,2 0-39 0 0,-1-3-10 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,1-2 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-2 10 0 0,2-4 49 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-2 0-1 0 0,1 0 1 0 0,-2-13-49 0 0,1 12-17 0 0,0 17 17 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 0 0 0,-12 36-209 0 0,12 91 192 0 0,11-91-2918 0 0,-10-23 1407 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-118100.252">5082 6571 4608 0 0,'22'-33'2473'0'0,"-14"18"4749"0"0,-3 19-1038 0 0,-1 7-5674 0 0,1-1-1 0 0,-1 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 2-509 0 0,6 35 445 0 0,-1 22-52 0 0,5 70-233 0 0,-8-77-380 0 0,6 3-218 0 0,-10-65 32 0 0,0-2-1020 0 0,0 0-4245 0 0,0 0-1815 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-117537.033">5129 6674 1376 0 0,'0'0'448'0'0,"0"0"1344"0"0,0 0 588 0 0,0 0 116 0 0,0 0-136 0 0,0 0-684 0 0,0 0-299 0 0,0 0-58 0 0,0 0-107 0 0,0 0-419 0 0,0 0-179 0 0,0 0-35 0 0,0 0-40 0 0,10-4 578 0 0,48-64 1084 0 0,-55 67-2155 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0-45 0 0,39 32 240 0 0,-10 33 664 0 0,-32-66-973 0 0,-1-1-608 0 0,0 0-262 0 0,0 0-1349 0 0,0 0-5210 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116084.978">5615 6722 920 0 0,'0'17'0'0'0,"0"-17"80"0"0,0 0-80 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 352 0 0,0 0 64 0 0,0 0 0 0 0,0 0 8 0 0,0 6-424 0 0,0-6 0 0 0,0 0 0 0 0,2 11-96 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115526.386">5637 6516 7856 0 0,'0'0'174'0'0,"0"0"29"0"0,0 0 13 0 0,0 9 2112 0 0,7 28 1209 0 0,-6-10-1555 0 0,4 68 1712 0 0,-1 27-2229 0 0,0-46-1465 0 0,-3-32 69 0 0,-2-25-2628 0 0,1-14 952 0 0,0-5-279 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115183.311">5637 6773 11832 0 0,'0'-17'1285'0'0,"22"-59"4317"0"0,17 32-3283 0 0,-36 43-2299 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1-20 0 0,18 39 831 0 0,16 53 83 0 0,-26-45-684 0 0,-6 8 68 0 0,-7-26-874 0 0,3-32 150 0 0,0-1-988 0 0,-1 1-436 0 0,-1 4-92 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-114236.626">6072 6790 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0 0 43 0 0,0 0 159 0 0,0 0 70 0 0,0 0 14 0 0,0 0 69 0 0,0 0 285 0 0,0 0 126 0 0,0 0 29 0 0,0 0-15 0 0,0 0-77 0 0,0 0-31 0 0,0 0-8 0 0,0 0-33 0 0,0 0-134 0 0,2 1-61 0 0,43 6 2321 0 0,-29-8-2644 0 0,32-21 394 0 0,-45 20-751 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-4 19 0 0,-7-6 0 0 0,6 11 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,-1 1 76 0 0,0 1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,1 3-75 0 0,38 54 0 0 0,-39-61 25 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,2-1-25 0 0,43-22-3889 0 0,-40 15-4253 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-106495.084">6591 6608 2760 0 0,'-32'-29'1211'0'0,"31"28"-702"0"0,-13-6 1981 0 0,-3 8-1483 0 0,10 5-408 0 0,-26 17 451 0 0,14-22 2469 0 0,7-5 2535 0 0,17-3-4219 0 0,42-13 338 0 0,36 21-421 0 0,-77 2-1693 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 2-59 0 0,43 34-101 0 0,-15-40 802 0 0,-33-2-571 0 0,-1 1 4 0 0,0 0-4 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-2 0 0,0 0-6 0 0,-17 28 213 0 0,-26 3-28 0 0,12-10-202 0 0,-35 16-64 0 0,-25 24 212 0 0,48-16-359 0 0,20-17 389 0 0,19-19-217 0 0,1-3 36 0 0,4-5-46 0 0,-1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-14 0 0,45-13 417 0 0,143-23 582 0 0,-139 39-919 0 0,-12 12-3590 0 0,-38-16 1676 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101751.894">6981 6933 3680 0 0,'-6'17'1721'0'0,"5"-12"9907"0"0,13-11-8856 0 0,14-14-2535 0 0,48-89 2026 0 0,2-45-1063 0 0,48-118-374 0 0,12 13-1554 0 0,-112 233 728 0 0,-9 0 0 0 0,-15 27 24 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1-23 0 0,-1 23 138 0 0,-1-1 0 0 0,-1 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,-6 18-138 0 0,-6 29 173 0 0,-10 75-35 0 0,20-44 4 0 0,7-84-93 0 0,-1 0 0 0 0,2-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,1 6-50 0 0,1 2 36 0 0,8 20 71 0 0,10 1 53 0 0,-15-50 10 0 0,56-159 270 0 0,-2 19-376 0 0,49-141-64 0 0,-67 188 0 0 0,-32 79 0 0 0,-12 20-2 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 2 0 0,0 0-1 0 0,7 59-63 0 0,-3 43 64 0 0,-8 37 203 0 0,-6 4 7 0 0,-5 36-63 0 0,-4-60-94 0 0,6-24-185 0 0,7-62-625 0 0,6-32-572 0 0,0-1-410 0 0,0 0-1290 0 0,0 0-4861 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101158">8022 6810 11232 0 0,'0'0'256'0'0,"0"0"34"0"0,0 0 20 0 0,-2 0-40 0 0,-26-3 1829 0 0,27 3-1367 0 0,1-2 59 0 0,8-47 2427 0 0,-6 41-3131 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,2 0-86 0 0,-4 2 36 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-36 0 0,3 7 185 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,-2 7-185 0 0,4-16 57 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-3-57 0 0,-3 0-194 0 0,1 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-2-4 194 0 0,-5-36-3540 0 0,6 26-4246 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-100410.518">8580 6574 8496 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 10 0 0,0 0 112 0 0,-1 1 406 0 0,-34 76 4453 0 0,11-35-3370 0 0,12 0-456 0 0,10-17-994 0 0,-8 31 976 0 0,10-52-1274 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-2-1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-81 0 0,5 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,4-7 0 0 0,49-99 0 0 0,-26 20 1046 0 0,-26 53-920 0 0,-6 39-27 0 0,-1 1-10 0 0,0 0 6 0 0,0 0 29 0 0,7 1 281 0 0,-1 12-392 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 1 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,-1 6-13 0 0,-14 102 1090 0 0,2-78-947 0 0,-2-1 1 0 0,-1-1 0 0 0,-2-1 0 0 0,-1 0-1 0 0,-2-2 1 0 0,-9 11-144 0 0,20-34 225 0 0,-2 0 0 0 0,0-2 0 0 0,0 1 0 0 0,-1-2 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1-2 0 0 0,0 0 0 0 0,-14 8-225 0 0,26-18-3 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-2 3 0 0,1-6-150 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,2 0 150 0 0,4-14-1149 0 0,2-3-679 0 0,-1 5-278 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-99222.683">9139 6831 10136 0 0,'2'14'230'0'0,"-2"-11"30"0"0,0-3 19 0 0,0 0 105 0 0,0 0 411 0 0,0 0 182 0 0,9 7 1891 0 0,-5-4-2546 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,2 0-322 0 0,3-2 206 0 0,0 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,3-3-206 0 0,39-72 696 0 0,-47 74-668 0 0,0-1-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,-1-6-28 0 0,3 12 5 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1-5 0 0,-4 6 19 0 0,1 1 1 0 0,-1-1 0 0 0,1 2 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,1 1 0 0 0,0 1-20 0 0,-1 0 77 0 0,1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,1 1 1 0 0,0 1-77 0 0,-2-7 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,33-17-1473 0 0,-23 4 614 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95784.389">9646 6578 4608 0 0,'0'0'353'0'0,"0"0"35"0"0,0 0 1008 0 0,0 0 461 0 0,0 0 95 0 0,0 0-104 0 0,0 0-522 0 0,0 0-228 0 0,0 0-46 0 0,1 2-59 0 0,10 17 2469 0 0,5 32-1092 0 0,-10 40-307 0 0,0 15-686 0 0,-9 8-869 0 0,3-112-577 0 0,0-2-52 0 0,0 0-21 0 0,0 0-198 0 0,0 0-824 0 0,0 0-362 0 0,0-1-1274 0 0,-3-4-4833 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94862.106">9690 6800 10016 0 0,'0'0'462'0'0,"0"0"-12"0"0,0 0-148 0 0,1-4 1464 0 0,45-67 3773 0 0,4 10-3387 0 0,-27 50-1432 0 0,-22 10-464 0 0,6 5 586 0 0,-3 1-782 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 2-60 0 0,3 9 248 0 0,12 69 841 0 0,-1 6-628 0 0,-21-70-366 0 0,4-22-174 0 0,1-1-11 0 0,0 0-178 0 0,0 0-783 0 0,0 0-344 0 0,0 0-69 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93718.359">10181 6520 3224 0 0,'0'12'2345'0'0,"0"32"5493"0"0,-1 2-4114 0 0,-1 50-712 0 0,5 9 343 0 0,-6-86-3334 0 0,1-11-891 0 0,-9 3-7476 0 0,6-8 8097 0 0,3-2-5157 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93135.977">10152 6800 456 0 0,'0'0'1763'0'0,"3"-15"5211"0"0,6-44-1110 0 0,12 41-1851 0 0,23-7-1678 0 0,-37 26-2203 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 1 0 0 0,2 6-132 0 0,19 39 1090 0 0,-23-42-1055 0 0,-1-1 0 0 0,0 1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,-1-1-34 0 0,1 11-14 0 0,1-19-184 0 0,0-1-536 0 0,0 0-236 0 0,0 0-888 0 0,0 0-3561 0 0,0 0-1523 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-90762.018">10576 6831 8288 0 0,'-3'9'5575'0'0,"14"2"-3896"0"0,-10-11-1688 0 0,2 2 148 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-2 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,3-4-139 0 0,22-46 514 0 0,-19 27-481 0 0,-6 23-28 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-4-4 0 0,1 6 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-55-10 0 0 0,52 10-6 0 0,0 0 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 2 1 0 0,0-1 0 0 0,-1 2 6 0 0,0 0 50 0 0,0 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,3 6-51 0 0,-2-7 64 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,3 0-64 0 0,33 0-544 0 0,-22-10-5374 0 0,-4 1-1399 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88936.296">11061 6226 3224 0 0,'-3'18'4649'0'0,"-17"29"2676"0"0,2 38-3229 0 0,3 62-1931 0 0,16-131-1939 0 0,17 122 1016 0 0,12-36-627 0 0,-4-40 597 0 0,-24-60-1196 0 0,-1-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1-16 0 0,24-29 176 0 0,10-57-176 0 0,-13 2 0 0 0,-9-12 0 0 0,-4 17 0 0 0,-7-30 0 0 0,-3 5 43 0 0,0 105-266 0 0,0 1-29 0 0,0 0-4 0 0,0 0-141 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1251 0 0,0 0-4804 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87751.59">11526 6370 2304 0 0,'-4'14'3512'0'0,"4"-14"-3295"0"0,1 31 9139 0 0,8 16-4914 0 0,-7-37-4052 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,-2 4-389 0 0,0 29-162 0 0,2 44 39 0 0,6 34 299 0 0,-4-109 129 0 0,-1-1-2806 0 0,-1-12 1101 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87470.909">11532 6469 7832 0 0,'0'0'602'0'0,"1"1"-134"0"0,8 1 1838 0 0,28 8 3878 0 0,20-10-2721 0 0,10-9-2874 0 0,-38 8-6863 0 0,-22 1-248 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86426.787">11890 6632 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-128 0 0,1 2-606 0 0,8 96 6111 0 0,-9-24-5043 0 0,-3-7-2402 0 0,2-60 17 0 0,1-5-6835 0 0,0-2 4521 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86230.545">12180 6455 4144 0 0,'0'0'191'0'0,"-4"2"22"0"0,2 0 5833 0 0,-6 20 354 0 0,-7 11-4079 0 0,9 10-269 0 0,7-12-1028 0 0,-4-10-798 0 0,0 0 0 0 0,2 0-1 0 0,0 0 1 0 0,1 0-1 0 0,2 20-225 0 0,1 66 0 0 0,-9-39 0 0 0,4-57 13 0 0,1-2-3106 0 0,1-9 1973 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85578.149">12345 6683 3224 0 0,'0'15'553'0'0,"6"8"6334"0"0,-12 65 1088 0 0,2-9-6591 0 0,4-64-1121 0 0,0-2-3991 0 0,0-13-2374 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85386.832">12392 6526 17503 0 0,'0'0'776'0'0,"0"0"160"0"0,0 0-744 0 0,0 0-192 0 0,0 0 0 0 0,0 0 0 0 0,0 0 448 0 0,0 0 48 0 0,0 0 16 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1568 0 0,2 11-304 0 0,-2-11-64 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85026.437">11873 6428 18455 0 0,'0'0'408'0'0,"0"0"80"0"0,0 0 24 0 0,0 0 0 0 0,0 0-408 0 0,0 0-104 0 0,0 0 0 0 0,0 0 0 0 0,0 0 224 0 0,-6 0 16 0 0,6 0 8 0 0,0 0 0 0 0,0 0-992 0 0,0 0-200 0 0,0 0-40 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-83816.66">12676 6533 9584 0 0,'0'0'216'0'0,"-8"5"521"0"0,-44 35 3704 0 0,28-13-975 0 0,20-23-3254 0 0,0-1 1 0 0,0 2-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 4-213 0 0,2-4 22 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,4 4-22 0 0,33 44 54 0 0,-17-36 918 0 0,-20-15-642 0 0,-2-1-115 0 0,7 3 109 0 0,0 10-171 0 0,-7-11-153 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-2 1 0 0 0,0 0-4 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 5 0 0,-4-18-2397 0 0,8 8 122 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-79727.133">12869 6773 4632 0 0,'0'0'209'0'0,"1"-2"-5"0"0,28-61 6992 0 0,-28 63-6393 0 0,-1 0-31 0 0,19-8 2699 0 0,61 9 1055 0 0,-19-4-2917 0 0,-45 15-1448 0 0,-6 9-150 0 0,-11-21-7 0 0,1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-4 0 0,-10-7 202 0 0,9 6-204 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-2 0 1 0 0,-28 18 268 0 0,26-15-199 0 0,1 2-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1 0 0 0,1 1-69 0 0,0-4 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,50-5-132 0 0,-47-2 154 0 0,-1-1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,2-3-22 0 0,39-62-80 0 0,-34 26 64 0 0,-5-1 16 0 0,1 165 0 0 0,-7-72 0 0 0,4 5 0 0 0,9 11 0 0 0,-3-4-2782 0 0,-7-47 64 0 0,-3 1-4789 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76952.167">13785 6841 2304 0 0,'0'0'464'0'0,"-1"1"2357"0"0,-4 6-1769 0 0,5-5 3151 0 0,0-1 4184 0 0,26 15-5739 0 0,-21-15-2588 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 0-1 0 0,3-3-59 0 0,4-7-111 0 0,-6 10 95 0 0,0-2 0 0 0,0 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-2 16 0 0,-2 4-53 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-2-2 54 0 0,3 4-6 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 7 0 0,-4 7 93 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,5 11-93 0 0,-6-18 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,3 0 0 0 0,-3-1-22 0 0,10-6-6424 0 0,-9-2-869 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77950.243">13427 6360 1840 0 0,'0'0'307'0'0,"0"-2"615"0"0,-2-30 3370 0 0,2 32-4103 0 0,0 0-1 0 0,0 0 44 0 0,0 0 22 0 0,0 0 2 0 0,0 0 74 0 0,0 0 316 0 0,0 0 142 0 0,0 1 32 0 0,6 62 3244 0 0,-6 77 861 0 0,0 71-1667 0 0,4-84-1971 0 0,5 64-363 0 0,-8-147-963 0 0,-2-26-3502 0 0,1-18 1678 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77348.9">13421 6509 13504 0 0,'0'0'620'0'0,"0"0"-16"0"0,4-6-364 0 0,16-5 1491 0 0,-16 8-1438 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1-293 0 0,76 5 662 0 0,-39 9-2436 0 0,-18-8-4491 0 0,-13 0 465 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76210.45">14301 6578 1840 0 0,'0'0'583'0'0,"-1"1"2720"0"0,-6 1-1116 0 0,-22 24 7260 0 0,25-18-9058 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 9-389 0 0,-3 51 2048 0 0,11 43-1440 0 0,-6-105-566 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,2 2-42 0 0,-4-6 48 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 0-48 0 0,6-6 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,3-9 0 0 0,19-47 0 0 0,-1-11 0 0 0,-24 56 0 0 0,-3 15 0 0 0,-6 1-177 0 0,-8 13-4614 0 0,9-6-2832 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-72325.515">14732 6564 3224 0 0,'0'0'143'0'0,"0"0"-3"0"0,6 0 2973 0 0,-5-1 7737 0 0,-5 4-3072 0 0,3 3-10123 0 0,2 28 3033 0 0,-2-6 1192 0 0,1-27-1368 0 0,0 1 0 0 0,-15 79 715 0 0,6-16-1010 0 0,4-11-308 0 0,21 76-94 0 0,-13-93 185 0 0,-5-31-139 0 0,2-5-580 0 0,0-1-251 0 0,0-1-1544 0 0,2-8-6015 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45518.414">16319 6605 8288 0 0,'0'139'4740'0'0,"0"-122"-3699"0"0,0 14 42 0 0,0 1 0 0 0,1-1 0 0 0,2 0 1 0 0,1 0-1 0 0,6 22-1083 0 0,2-11-70 0 0,-6-27-1026 0 0,-4-14-85 0 0,-2-1-45 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45023.887">16670 6581 1376 0 0,'0'0'299'0'0,"0"0"715"0"0,0 0 313 0 0,0 0 66 0 0,-10-7 1242 0 0,7 6-2367 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,-1 1-268 0 0,-44 91 3206 0 0,45-88-3121 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1-85 0 0,68 38 528 0 0,-72-44-518 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1-9 0 0,-1 2-25 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 25 0 0,-9-14-3267 0 0,9 6-3203 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22924.697">14732 6769 920 0 0,'-4'10'80'0'0,"-5"7"5114"0"0,8-16-3500 0 0,1-1-770 0 0,0 0-336 0 0,0 0-68 0 0,0 0-20 0 0,0 0-51 0 0,0 0-22 0 0,0 0-3 0 0,0 0 25 0 0,0 0 107 0 0,0 0 48 0 0,0 0 11 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,6-22 5642 0 0,26-28-4223 0 0,11 15-1739 0 0,-39 34-286 0 0,3 2 1 0 0,4 10 96 0 0,-7-4-97 0 0,-4-6-115 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 105 0 0,9 2-1084 0 0,13-1-5055 0 0,-19-1 4517 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23746.448">15220 6475 1376 0 0,'0'0'331'0'0,"0"0"853"0"0,0 0 380 0 0,0 0 71 0 0,0 0-79 0 0,0 0-405 0 0,0 0-178 0 0,0 0-39 0 0,0 0-42 0 0,0 0-151 0 0,0 0-65 0 0,0 0-17 0 0,0 0 26 0 0,0 0 124 0 0,0 0 58 0 0,0 0 11 0 0,0 0-43 0 0,0 0-192 0 0,0 0-89 0 0,-14-3 1062 0 0,-26 17 904 0 0,-10 37-429 0 0,6 34-1643 0 0,24-37-267 0 0,4 48 275 0 0,12 20 391 0 0,9-83-660 0 0,-5-25-158 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,3 1-29 0 0,20 26 0 0 0,-18-29-4 0 0,-6-4-118 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-2 122 0 0,22-17-6775 0 0,-19 11 184 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24081.144">15314 6652 456 0 0,'12'-36'1833'0'0,"5"16"8000"0"0,-4 3-4338 0 0,-12 16-4746 0 0,-1 1-12 0 0,8 1 2655 0 0,-4 4-3184 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 5-208 0 0,0-4 187 0 0,1 171 1174 0 0,-8-103-1017 0 0,-6-7-212 0 0,10-60-136 0 0,2-3 10 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1-5 0 0,-8 6-315 0 0,-26 22-6531 0 0,28-26 5010 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28120.561">15440 6056 4608 0 0,'3'-4'886'0'0,"0"-3"-1808"0"0,-2 2 5374 0 0,-1-3 4827 0 0,15 9-6424 0 0,-8 3-2408 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,2 3-447 0 0,10 27 1006 0 0,14 73 508 0 0,-20-24-882 0 0,4 239 416 0 0,-14-51-535 0 0,-11-44 14 0 0,-2 6-74 0 0,0-142-389 0 0,0-25 75 0 0,12-63-128 0 0,-18-2 223 0 0,-103-34-95 0 0,82 27-75 0 0,-6 7 28 0 0,-1-2 1 0 0,1-2-1 0 0,-19-4-92 0 0,-37-13 67 0 0,-146-71-67 0 0,219 81-114 0 0,-1 2 1 0 0,1 1-1 0 0,-1 2 0 0 0,0 1 0 0 0,1 2 1 0 0,-1 1-1 0 0,-14 4 114 0 0,-504 86 796 0 0,80-34-796 0 0,12 1 0 0 0,189-19 0 0 0,-11-9 0 0 0,-189-10 0 0 0,-359-19 0 0 0,534 6 0 0 0,-252-33 0 0 0,-64-19 0 0 0,139 27-457 0 0,-193-4 202 0 0,234-3-1 0 0,-133 19 256 0 0,284 4 172 0 0,-64 0 164 0 0,26-15-196 0 0,57 16 180 0 0,78 1-722 0 0,-27 1 8 0 0,-172-5 478 0 0,129-5 308 0 0,23-9-72 0 0,-224-16-1032 0 0,293 19 852 0 0,-64-10 432 0 0,-122-6-572 0 0,153 13 0 0 0,-35 20 0 0 0,-50-8 0 0 0,72-4 0 0 0,-78 33 0 0 0,20 14 0 0 0,111-49 0 0 0,13 18 0 0 0,50 0 0 0 0,84-6-20 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1-1 20 0 0,-26-46-115 0 0,-8-66 687 0 0,-13-89-572 0 0,-16-91 0 0 0,42 48 0 0 0,-4 80 0 0 0,-2-19 0 0 0,19 73-796 0 0,9 24 1592 0 0,12 20-796 0 0,25-26 0 0 0,-31 85 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,7-7 0 0 0,65-39 0 0 0,73-25 0 0 0,-129 70 0 0 0,0 1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1 2 0 0 0,0 1 0 0 0,8 1 0 0 0,-32 1 0 0 0,111 0 0 0 0,0-5 0 0 0,25-9 0 0 0,21-13-712 0 0,78-21 1413 0 0,-142 32-697 0 0,0 4-1 0 0,1 6 1 0 0,56 5-4 0 0,254 19 0 0 0,-105-2 0 0 0,-239-12-72 0 0,1 2 1 0 0,-1 4-1 0 0,43 14 72 0 0,71 7-105 0 0,-58-20 425 0 0,53 12-320 0 0,-44 2 0 0 0,56 16 0 0 0,68 2 0 0 0,48 22 0 0 0,-158-27 0 0 0,46-1 0 0 0,39 1-796 0 0,-78-3 1592 0 0,4-12-831 0 0,7-27-250 0 0,-29 4 605 0 0,51 11-320 0 0,-84-8 0 0 0,76-20 0 0 0,-34-2 0 0 0,119 14 0 0 0,-168 5 0 0 0,0-5 0 0 0,62-13 0 0 0,45-4 0 0 0,118 6 0 0 0,-35-7 0 0 0,-127 5 0 0 0,197 1 0 0 0,-89 15 0 0 0,91-20 0 0 0,74-12 0 0 0,-289 27 0 0 0,15-1 0 0 0,227 3 0 0 0,-124 15 0 0 0,-50-3 0 0 0,104-21 0 0 0,9 21 0 0 0,-186 0 0 0 0,6-11 0 0 0,-11-3 0 0 0,-15 7 0 0 0,9 4 0 0 0,27-11 0 0 0,51 14 0 0 0,-64 9 0 0 0,-71-19 0 0 0,146-4 0 0 0,-57 24 0 0 0,-75-7 0 0 0,43-2 0 0 0,-37 2 0 0 0,131 14 0 0 0,-53-8 0 0 0,-61-2 0 0 0,58 4 0 0 0,-68-16 0 0 0,30-5 0 0 0,-33 26-4336 0 0,-33-5-1782 0 0,-38-14-3483 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29020.976">15120 5809 1376 0 0,'0'0'591'0'0,"0"0"1942"0"0,0 0 851 0 0,0 0 174 0 0,0 0-327 0 0,-11 8 6223 0 0,14-5-9289 0 0,1 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,1-1-165 0 0,0 2 87 0 0,97 18 1139 0 0,-6 19-943 0 0,-53-21-166 0 0,5-27 11 0 0,-18 7-64 0 0,-15 20-64 0 0,-9 16 13 0 0,-6 5 198 0 0,-2 60 157 0 0,3-7-616 0 0,0-31-3854 0 0,1-36-5107 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.15371E6">7867 7688 1376 0 0,'0'0'65'0'0,"0"0"189"0"0,0 0 767 0 0,0 0 335 0 0,0 0 69 0 0,0 0-94 0 0,0 8 1469 0 0,-2 72 3116 0 0,4-14-3609 0 0,-14 102-383 0 0,11-29-438 0 0,1-60-917 0 0,-2-1 598 0 0,1 106-205 0 0,-6 4-322 0 0,11 98-40 0 0,-1-188-336 0 0,-3 21 8 0 0,9 119 323 0 0,5-5 583 0 0,-3-60-1855 0 0,-6 84 952 0 0,0-53-94 0 0,-4-145-117 0 0,4-3-2277 0 0,-2-78-5567 0 0,-3 8 286 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.15425E6">7393 9856 5528 0 0,'0'0'422'0'0,"0"0"-88"0"0,0 0 656 0 0,0 17 2881 0 0,10 38-2527 0 0,7 40 2164 0 0,20-9-466 0 0,69 129 109 0 0,-71-150-2761 0 0,-26-45-296 0 0,1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,1-1-1 0 0,1 0 1 0 0,0-1-1 0 0,12 10-94 0 0,56 24 544 0 0,-78-47-475 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,3-2-69 0 0,28-40 176 0 0,81-237 1624 0 0,-34 86-1872 0 0,-40 74-576 0 0,-26 68-2737 0 0,-10 39 1634 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16329E6">3054 10697 13128 0 0,'0'-16'633'0'0,"0"15"-277"0"0,0 8 83 0 0,13 222 3164 0 0,17-12-1187 0 0,-7-2-1552 0 0,-25-125-897 0 0,-13-32-3046 0 0,12-49 1239 0 0,-4-5-71 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16383E6">2980 10685 7056 0 0,'-2'-5'116'0'0,"1"0"0"0"0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,2-3-117 0 0,0-6 1073 0 0,-2 12-878 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,3-1-195 0 0,-1 1 85 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,2 2-85 0 0,42 48 670 0 0,-22-21 265 0 0,20 39 175 0 0,-42-59-1010 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,-3 7-100 0 0,2-10 186 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0-1-1 0 0,0 1 1 0 0,-3 0-186 0 0,7-4 12 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1-1-11 0 0,-39 6 164 0 0,43-5-225 0 0,16 13-71 0 0,34 31 57 0 0,-29-19 68 0 0,52 78 132 0 0,0 46-125 0 0,-37-69-5360 0 0,-31-61 3443 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16516E6">3718 11368 6912 0 0,'0'0'528'0'0,"0"0"-219"0"0,0 0 347 0 0,0 2 192 0 0,12 9 3088 0 0,43-14-2645 0 0,19-34-467 0 0,-27 7 415 0 0,-44 27-1110 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1-128 0 0,-26-40 870 0 0,22 42-830 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 2 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,-1 3-41 0 0,1 0 30 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 2-30 0 0,18 104 84 0 0,-16-107-98 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 0 0 0 0,1 0 14 0 0,7 0-1085 0 0,-1-1-349 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16566E6">4230 10979 920 0 0,'1'2'67'0'0,"5"16"218"0"0,-6-16 1126 0 0,0-2 485 0 0,0 0 95 0 0,0 0-144 0 0,0 0-698 0 0,0 0-306 0 0,3 14 5156 0 0,4 70-3006 0 0,-1 145-2907 0 0,15-68 348 0 0,-8-98-1540 0 0,-9-56-81 0 0,-1-4-3107 0 0,-3-2-1448 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.16596E6">4230 11064 5984 0 0,'0'0'464'0'0,"0"0"-82"0"0,10 12 5502 0 0,34-2-3006 0 0,29-10-1919 0 0,-23-4-2545 0 0,-39 4-3811 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29091E6">7353 10942 1840 0 0,'0'0'83'0'0,"0"7"10"0"0,-3-2 194 0 0,-4 6 6325 0 0,0 3-4677 0 0,4-8-1065 0 0,-3 26 3503 0 0,8 49-1185 0 0,2 49-2006 0 0,0-58-326 0 0,4-42-586 0 0,20 43 628 0 0,-26-71-870 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2-1-28 0 0,4-5 21 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,3-9-21 0 0,21-42 0 0 0,-9-13 1099 0 0,1-24-934 0 0,-15 6-165 0 0,-3 62 0 0 0,-6-38 0 0 0,2 22-283 0 0,2 27-8605 0 0,-1 19 2172 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29171E6">7871 10880 8288 0 0,'-9'70'3321'0'0,"8"21"1356"0"0,2-6-2700 0 0,1-30-1241 0 0,1 132 440 0 0,-3-171-966 0 0,7 43-294 0 0,-6-58-163 0 0,-1-1-857 0 0,0-2-3536 0 0,0-6-1518 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.2919E6">7855 10979 8288 0 0,'0'0'638'0'0,"7"-3"2018"0"0,17-3 1429 0 0,15 17-2828 0 0,-24-6-864 0 0,29 23-411 0 0,-38-23-355 0 0,14 19-3587 0 0,-12-12 2594 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29212E6">8218 11195 3680 0 0,'0'0'284'0'0,"3"8"797"0"0,-2-4 4784 0 0,1 30-1677 0 0,0 5-3145 0 0,-3 37-251 0 0,5-14-1216 0 0,-4-46-1299 0 0,0-6-3631 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29254E6">8483 10979 920 0 0,'-3'-14'343'0'0,"3"11"1102"0"0,0 3 482 0 0,0 0 96 0 0,0 0-124 0 0,0 0-614 0 0,0 0-269 0 0,0 0-50 0 0,0 0-57 0 0,0 0-212 0 0,0 0-90 0 0,0 2-20 0 0,-1 36 1508 0 0,-5 36-993 0 0,-4 83 402 0 0,6-56-494 0 0,11 56-140 0 0,3-75-1121 0 0,-10-81-772 0 0,0-1-333 0 0,0 0-68 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29304E6">8751 11290 456 0 0,'-5'20'0'0'0,"5"-19"651"0"0,-2 0 4741 0 0,-1 2 3820 0 0,3 1-9813 0 0,2 172 4824 0 0,2-124-4491 0 0,-4-47-754 0 0,0-4-326 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29369E6">9051 11263 10136 0 0,'0'0'464'0'0,"-2"0"-10"0"0,-4 0-222 0 0,-11 14 3123 0 0,15-13-3266 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1-89 0 0,22 51-256 0 0,-14-29 538 0 0,33 28 412 0 0,-12 3-275 0 0,-26-21-94 0 0,-18 6 1227 0 0,3-25-785 0 0,-13 5 957 0 0,13-18-1575 0 0,-9-2-133 0 0,-4-17-2201 0 0,21 11-250 0 0,2 4-4568 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29508E6">9302 11512 10136 0 0,'6'17'230'0'0,"-5"-13"30"0"0,-1-4 19 0 0,2-8 478 0 0,5-33 763 0 0,-6 39-1014 0 0,0-1-2 0 0,7-26 334 0 0,-7 23-761 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,2 0-78 0 0,-4 4 167 0 0,26-16 1024 0 0,-25 16-1129 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0-61 0 0,25 30 1857 0 0,-25-31-1723 0 0,-1-1-46 0 0,0 0-22 0 0,0 0-2 0 0,0 0 2 0 0,0 0 4 0 0,-21 0 2 0 0,17 0-87 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-2 1 16 0 0,-22 15-85 0 0,25-18 77 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 2 8 0 0,10 30-54 0 0,-10-32 57 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-3 0 0,44 5 163 0 0,-40-9-205 0 0,-1 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,-1-4 43 0 0,7-69-556 0 0,-7 79 622 0 0,0 1 34 0 0,0 0 10 0 0,-1 3-16 0 0,0 11 66 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,3 10-160 0 0,1 26 76 0 0,14 26 0 0 0,-11-36-1057 0 0,-8-38-90 0 0,5 7-37 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29562E6">9847 11082 456 0 0,'0'-22'204'0'0,"0"8"5674"0"0,-3 14 1245 0 0,-5 26-4666 0 0,-1 52-110 0 0,9 97-830 0 0,-4 70-628 0 0,13-184-907 0 0,-8-54 2 0 0,-1-7-2564 0 0,0 0 1298 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29586E6">9813 11229 8752 0 0,'5'8'936'0'0,"11"-23"1798"0"0,38 15 2614 0 0,31 4-4455 0 0,-48 12-4124 0 0,-30-12 2047 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29642E6">10205 11581 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,2 1-40 0 0,36-7 2129 0 0,-16-1-968 0 0,-19 6-1318 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1-82 0 0,6-10 268 0 0,-5 10-243 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-3-4-25 0 0,5 6 20 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-20 0 0,-5 10 226 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 4-225 0 0,0-13 37 0 0,1 2 31 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,1 0-67 0 0,-1-2 33 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,3 0-33 0 0,40 8-313 0 0,-11-15-1742 0 0,-27 5 191 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29693E6">10646 11363 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,-10 3 2224 0 0,1 9-1481 0 0,8-10-561 0 0,1-2 0 0 0,-1 1 0 0 0,-29 38 1128 0 0,28-36-1631 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-9 0 0,0 18 74 0 0,-1-17-14 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1-59 0 0,55 33 164 0 0,-55-36-163 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1-1 0 0 0,23-40 0 0 0,0-26 0 0 0,-21 39 0 0 0,-5-43 0 0 0,0 65 0 0 0,0 10-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 2 0 0,-1 2-86 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 5 86 0 0,10 44-6882 0 0,-5-42 1085 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.2974E6">11181 11219 3224 0 0,'3'17'240'0'0,"-16"13"5162"0"0,-7 23 1702 0 0,1 32-4883 0 0,10-45-1389 0 0,6 22 96 0 0,-3-22-476 0 0,6 22 178 0 0,-4 6-648 0 0,1-57 50 0 0,0-5-3037 0 0,3-6 1818 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.29771E6">11130 11444 10136 0 0,'2'9'1085'0'0,"43"-45"1390"0"0,-42 33-2239 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,3-1-236 0 0,28-14 608 0 0,-10 30 520 0 0,-9 4-434 0 0,-14-17-580 0 0,15 13-10 0 0,-16-11-96 0 0,12 22-8 0 0,-12-20-92 0 0,-1-3-390 0 0,0 7-1954 0 0,3-1-3569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.30092E6">11702 11093 2304 0 0,'0'0'101'0'0,"1"-2"1"0"0,1-4-3003 0 0,-1 1 4359 0 0,-6-3 14711 0 0,-3 14-13468 0 0,5-3-2385 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 4-316 0 0,-1 99 1202 0 0,2-97-965 0 0,3 41-228 0 0,1 0 0 0 0,2 0 1 0 0,2-1-1 0 0,2 0 0 0 0,8 20-9 0 0,-10-39 0 0 0,-2-22 0 0 0,17 1-1058 0 0,11-29-4850 0 0,-24 9 3794 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.30128E6">12030 11003 1376 0 0,'0'0'65'0'0,"0"0"454"0"0,0 0 1882 0 0,5 0 5023 0 0,3 0-3511 0 0,-6 2-3615 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 3-297 0 0,26 51 2384 0 0,-5-9-1738 0 0,-14-33-400 0 0,-1 1 0 0 0,0 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-2 1-1 0 0,0 1-245 0 0,13 118 608 0 0,-14 68 104 0 0,-11-64-61 0 0,0-95-3304 0 0,-3-2-3362 0 0,7-32-807 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.30531E6">12605 12454 3224 0 0,'0'0'143'0'0,"0"0"327"0"0,0 0 1271 0 0,0 0 550 0 0,0 0 114 0 0,0-3 988 0 0,1-12-1052 0 0,0-52 2752 0 0,7-3-2899 0 0,9-98-927 0 0,5-50-315 0 0,-9 76 489 0 0,-4-103-1441 0 0,-7 153 170 0 0,1 8 86 0 0,3 0-1 0 0,8-37-255 0 0,4-24 592 0 0,-5 22-253 0 0,-10 24 96 0 0,5 48-99 0 0,4-14-403 0 0,-1 37 67 0 0,-5 11 13 0 0,-3 0 79 0 0,-6 7 139 0 0,-6-10-231 0 0,8 18 5 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-5 0 0,-113 3 320 0 0,59 1-256 0 0,-57 5 61 0 0,-220 12 207 0 0,40 3-320 0 0,13 14 52 0 0,25 17-64 0 0,-256 57 128 0 0,327-88-117 0 0,73-14 98 0 0,-1-5 0 0 0,-32-7-109 0 0,19 0-2 0 0,-69-5 367 0 0,-82 2-133 0 0,-23-7-541 0 0,95-2 706 0 0,-12 0-710 0 0,51 4 634 0 0,-171 0-321 0 0,184-3-16 0 0,-35 1-155 0 0,-34-11 182 0 0,-102-10 65 0 0,188 22-88 0 0,-23 4 12 0 0,-45 4 64 0 0,17 0-64 0 0,-53-8 0 0 0,-289-30 64 0 0,361 27-64 0 0,-258-10 0 0 0,373 25 0 0 0,-139-11 0 0 0,66-4 0 0 0,-37-6 0 0 0,-23-2 0 0 0,-96 16 0 0 0,188 8 0 0 0,-48-15 0 0 0,28-5 0 0 0,79 14 0 0 0,0 1 0 0 0,-1 2 0 0 0,-32 4 0 0 0,-10 0 0 0 0,-221 7-11 0 0,111-35 22 0 0,-82-18-11 0 0,-44 39-64 0 0,239-6 128 0 0,50 9-64 0 0,0 0 0 0 0,1-2 0 0 0,-1-1 0 0 0,-21-7 0 0 0,29 6 0 0 0,5 0 0 0 0,0 2 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,-4 1 0 0 0,4 1 0 0 0,7-3 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 2 0 0 0,-14 72-244 0 0,40 143 168 0 0,-3-63 299 0 0,30 231-446 0 0,-6-30 520 0 0,2-178-530 0 0,-22-88 233 0 0,17 53 0 0 0,12-7 0 0 0,-43-120 0 0 0,53 78 0 0 0,-47-83 4 0 0,0-1 0 0 0,1-1 0 0 0,0-1 0 0 0,1-1-1 0 0,0-1 1 0 0,0 0 0 0 0,0-2 0 0 0,1 0 0 0 0,5 0-4 0 0,26 11 140 0 0,77 16-242 0 0,-13-11 207 0 0,86 4-105 0 0,-76-11-23 0 0,70 3-132 0 0,6-8 155 0 0,446 20 0 0 0,-127-7 0 0 0,-55 0 0 0 0,76-19 53 0 0,-62-41-42 0 0,-142-15-11 0 0,42 10 0 0 0,-164 25 12 0 0,-10 11 112 0 0,87-8-204 0 0,46 20 149 0 0,13-8-58 0 0,-4-10-107 0 0,9 1 96 0 0,-156 3 96 0 0,101 12-192 0 0,-211 14 96 0 0,41-2 0 0 0,31 0 144 0 0,-48-19-240 0 0,3-2 192 0 0,-80 6-96 0 0,0-1 0 0 0,1-3 0 0 0,-1-1 0 0 0,30-8 0 0 0,25-3-96 0 0,32 7 96 0 0,98 3 0 0 0,-108-9 80 0 0,-32 2-160 0 0,90-5 80 0 0,-71 19 11 0 0,80-17 42 0 0,-85-3-141 0 0,-15-8 94 0 0,1 4 0 0 0,55-5-6 0 0,-37 13 60 0 0,-1 12-60 0 0,38 36 0 0 0,-48-18 0 0 0,-77-15 0 0 0,18 13 0 0 0,-23-8 59 0 0,-5-6-111 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 52 0 0,-4 4-1004 0 0,4-4-3898 0 0,1-1 2712 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.31424E6">15845 6350 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0-11 1147 0 0,0 7-3619 0 0,1-4 9257 0 0,0 5 2091 0 0,-1 8-7632 0 0,12 193 1589 0 0,-16-103-2526 0 0,-4-7-90 0 0,3-5-182 0 0,14 6-118 0 0,-2-42-2244 0 0,-6-46 1548 0 0,-1-1-185 0 0,0 0-84 0 0,0 0-21 0 0,2 3-3895 0 0,-2-3 2635 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.31517E6">15868 6780 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0 0-22 0 0,0-15 2511 0 0,14-70 5565 0 0,-4 59-6834 0 0,10 1-281 0 0,-5 9-550 0 0,-14 15-517 0 0,-1 1-6 0 0,2 0 3 0 0,20 7 472 0 0,-2 13 14 0 0,10 53 396 0 0,7 63-438 0 0,-27-83-450 0 0,-10-26-1627 0 0,0-12-6318 0 0,0-5 1470 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.32608E6">13264 11283 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,3-9 1867 0 0,-2 8-1852 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1-240 0 0,-4-4 274 0 0,-1 1-1 0 0,1 0 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-2 2-273 0 0,-9 5 0 0 0,11-1 0 0 0,-25 34 0 0 0,23-25 150 0 0,0 1 1 0 0,1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 1 0 0,1-1-1 0 0,1 1 0 0 0,0 5-150 0 0,-1-2 104 0 0,-14 207-482 0 0,9-119 567 0 0,8-13-136 0 0,-1-96-229 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0 176 0 0,7-3-1901 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.32649E6">12960 11591 5984 0 0,'0'0'464'0'0,"0"0"-100"0"0,0 0 717 0 0,0 0 346 0 0,0 0 69 0 0,0 0-71 0 0,0 0-330 0 0,0 0-146 0 0,6 13 1624 0 0,-3-9-2296 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,4-1-277 0 0,14 8 296 0 0,18 1 73 0 0,-33-7-712 0 0,19 11-175 0 0,-12 4-5552 0 0,-8-5-166 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.3268E6">13237 11939 6624 0 0,'0'0'298'0'0,"0"0"-3"0"0,0-2-188 0 0,24-54 3721 0 0,-17 43-2931 0 0,-6 11-725 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-173 0 0,-1 2 83 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 1-83 0 0,3 4 241 0 0,0 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 7-241 0 0,-5 51 1376 0 0,-2-47-782 0 0,6-18-550 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1-44 0 0,-2-2-23 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1-1 1 0 0,2 0-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-2 24 0 0,-12-41-1750 0 0,9 20 132 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.32804E6">13625 11915 4608 0 0,'0'0'101'0'0,"-3"-4"150"0"0,2-1-50 0 0,1 4 308 0 0,0 1 135 0 0,0-2 27 0 0,-2-36 1126 0 0,2 37-1534 0 0,0 1-330 0 0,0 0-71 0 0,0 0 38 0 0,0 0 152 0 0,0 0 68 0 0,0 0 9 0 0,0 1-17 0 0,2 1-16 0 0,-2-1 280 0 0,0-1 113 0 0,0 0 21 0 0,0 0-68 0 0,0 0-262 0 0,0 0-9 0 0,-1 6 712 0 0,0-6-575 0 0,1 0 4 0 0,0 0 26 0 0,0 0 113 0 0,0 0 49 0 0,0 0 11 0 0,0 0-57 0 0,0 0-239 0 0,0 0-102 0 0,0 0-17 0 0,0 0 18 0 0,0 0 99 0 0,0 0 47 0 0,0 0 11 0 0,0 0 0 0 0,0 0 1 0 0,0 0 0 0 0,2 7 268 0 0,9 26 656 0 0,-8 17 132 0 0,9 17 242 0 0,-7-33 28 0 0,-5 34-1582 0 0,-4-23-16 0 0,4-35 0 0 0,1-86 1117 0 0,-2 36-1650 0 0,5-51 37 0 0,-7-2 27 0 0,13 63 834 0 0,-7 23-365 0 0,22-7-1090 0 0,-24 14 1590 0 0,0 1-59 0 0,48 46-276 0 0,-19-2-165 0 0,-10-1 0 0 0,1 10 0 0 0,-12-10 0 0 0,-8-26 72 0 0,5 4-112 0 0,-6-20-81 0 0,0-2-30 0 0,12 6-660 0 0,9-4-2647 0 0,-17-10 2023 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33006E6">14079 11874 6448 0 0,'27'-50'4184'0'0,"-26"49"-3679"0"0,-1 1 6 0 0,0 0 1 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 0 0 0,0 0-24 0 0,0 0-100 0 0,0 0-42 0 0,0 0-8 0 0,0 0-20 0 0,0 0-74 0 0,0 0-39 0 0,0 0-5 0 0,0 0 26 0 0,0 0 104 0 0,0 0 44 0 0,0 0 8 0 0,0 0-31 0 0,13 3 130 0 0,-13-2-345 0 0,-18 8 299 0 0,-2 5-94 0 0,-29 30 589 0 0,15-9 20 0 0,21 11-70 0 0,13-44-729 0 0,0 0-40 0 0,-1 14 5 0 0,1-13-81 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,2 0-27 0 0,0 1 24 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,3 0-23 0 0,25 6-16 0 0,2-12-321 0 0,0-17-1384 0 0,-17 18-2498 0 0,-7-1-2527 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33103E6">14417 11587 456 0 0,'0'0'1877'0'0,"0"0"225"0"0,0 0 96 0 0,0 0-174 0 0,0 0-800 0 0,0 0-352 0 0,0 2-68 0 0,-3 81 5406 0 0,0-9-3788 0 0,-4 7-533 0 0,0 109-938 0 0,8-93-994 0 0,-1-94-228 0 0,2 9 239 0 0,-1-4-2836 0 0,-1-14 836 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33125E6">14367 11725 10592 0 0,'0'0'818'0'0,"0"0"-382"0"0,0 0 375 0 0,2 0 224 0 0,46 12 3870 0 0,-11 5-4655 0 0,-15-10-2639 0 0,-21-6 1115 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33171E6">14651 11925 920 0 0,'0'-6'1780'0'0,"-7"-31"5181"0"0,7 36-6117 0 0,0 1-63 0 0,3-5 1525 0 0,-1 2 782 0 0,6 22-961 0 0,-15 41 414 0 0,-1-12-2418 0 0,14-6-123 0 0,7 31-266 0 0,-13-71-1124 0 0,0-2-490 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.33205E6">14875 11956 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,-6-14-276 0 0,6 10-201 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0-59 0 0,-1 1 59 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-61 0 0,12 48 1489 0 0,-13-40-1068 0 0,1 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,-1 1-420 0 0,2-11 47 0 0,-17 57 2134 0 0,-23 17-2086 0 0,40-74-50 0 0,-1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-2-46 0 0,-33-49 76 0 0,18 3-2636 0 0,11 14-3921 0 0,2 10-600 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34044E6">15193 11735 2760 0 0,'2'6'3463'0'0,"-1"-1"5440"0"0,-9 22-3399 0 0,8 21-2728 0 0,-2 12-1732 0 0,-6 24 73 0 0,10 41-1117 0 0,1-98-2100 0 0,-3-29 527 0 0,3-4-370 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34087E6">15183 11936 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0 0 240 0 0,0-8 1066 0 0,13-32 2918 0 0,30 3-1475 0 0,-28 29-2427 0 0,21-2-98 0 0,-28 12-954 0 0,40 19 0 0 0,13 47 242 0 0,-27 32 636 0 0,-25-62-878 0 0,-6-21 0 0 0,-6 7-49 0 0,3-23-207 0 0,0-1-87 0 0,0 0-917 0 0,0 0-3813 0 0,0 0-1633 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34281E6">15771 11448 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,0 17 1877 0 0,7 82 4244 0 0,-5-24-3972 0 0,-7 45-624 0 0,1-24-1860 0 0,3 87 1890 0 0,2-5-1730 0 0,2-164-88 0 0,0 2-289 0 0,-2 2-5727 0 0,-4-34 687 0 0,0 1 3586 0 0,6 1-135 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34372E6">15781 11495 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,3-7-177 0 0,-3 5 136 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1-247 0 0,10-6 1678 0 0,39-8 1057 0 0,21 26-286 0 0,-56-7-2099 0 0,-4-1-94 0 0,0 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,3 7-256 0 0,12 29 768 0 0,7 36 88 0 0,-25-15-68 0 0,-10-16 336 0 0,-16-12-1124 0 0,15-32 144 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,-4 1-143 0 0,-37 16 238 0 0,45-19-196 0 0,-1-1-31 0 0,0 2-27 0 0,56-29-776 0 0,13 17-152 0 0,-3 28-54 0 0,-17 17 92 0 0,-12 13 866 0 0,-25-27 40 0 0,-5-16 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 3 0 0 0,-23 33 1352 0 0,-11 0-736 0 0,23-33-497 0 0,-1 0-1 0 0,1-2 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1-2-1 0 0,0 0 1 0 0,-1 0-1 0 0,0-2 1 0 0,0 0 0 0 0,0-1-1 0 0,-5-1-118 0 0,-56 7 387 0 0,26 10-334 0 0,25-16-53 0 0,-5-18-801 0 0,21 9-282 0 0,2 1-2237 0 0,2 1-3262 0 0,-1-1-1015 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34474E6">16523 11465 14800 0 0,'0'0'332'0'0,"0"0"50"0"0,0 0 25 0 0,0 0-47 0 0,0 0-106 0 0,0 0 417 0 0,0 2 206 0 0,-8 54 3904 0 0,6-25-4120 0 0,-15 139 1824 0 0,-2-30-880 0 0,6-34-165 0 0,-11 135-832 0 0,23-234-672 0 0,1-6-273 0 0,0-1-138 0 0,0 3-1216 0 0,-1 5 3621 0 0,0-3-4753 0 0,1 0-9564 0 0,0-5 10339 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34497E6">16531 11519 920 0 0,'0'-6'1157'0'0,"1"3"5384"0"0,16-13-1079 0 0,28 8 55 0 0,21 14-2419 0 0,-2 11-1830 0 0,-10 14 320 0 0,16 44-1572 0 0,-17 13 2016 0 0,-48-75-1886 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,-1 8-146 0 0,1-2 8 0 0,-1 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-2-2 0 0 0,0 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-3 2-8 0 0,10-10 173 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,-3 0-174 0 0,-111-3-286 0 0,94-4-191 0 0,20 5 329 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-5-5 148 0 0,5 3-710 0 0,4 7-8073 0 0,3 0 434 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34598E6">17182 12104 7368 0 0,'0'0'333'0'0,"0"0"0"0"0,-8 4 14776 0 0,6-4-14374 0 0,2-2-710 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,1 0-25 0 0,-3 2 94 0 0,0 0 9 0 0,0 0 29 0 0,0 0 17 0 0,0 0 3 0 0,0 0 11 0 0,0 0 44 0 0,0 0 17 0 0,0 0 6 0 0,0 0 4 0 0,0 0 4 0 0,0 0 2 0 0,0 0 0 0 0,0 0-16 0 0,0 0-66 0 0,0 0-29 0 0,0 0-8 0 0,0 0-9 0 0,0 0-33 0 0,-1 0-25 0 0,-18 29-43 0 0,13-9 74 0 0,5-18-19 0 0,1-2 6 0 0,1-2-18 0 0,8-16-135 0 0,5 10 5 0 0,7 14-588 0 0,-16 2 664 0 0,2 17 16 0 0,-7-24 62 0 0,-4 8 297 0 0,-7-1-725 0 0,10-8 151 0 0,-8 8-801 0 0,1-8-2062 0 0,8 0 1532 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34684E6">17509 11649 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-3 420 0 0,0 3 3077 0 0,0 1 3963 0 0,-6 140-3072 0 0,-4-26-2600 0 0,-7 65-1021 0 0,7-68-304 0 0,4 24-619 0 0,6-135-213 0 0,0-1-69 0 0,0 0-12 0 0,0 0-139 0 0,0-56-6135 0 0,0 33 4451 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34718E6">17483 11689 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,1-1 21 0 0,2-2-256 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,2 0-170 0 0,4 4 318 0 0,-1 0 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 2 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1-318 0 0,18 16-106 0 0,-22-21 167 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 3-62 0 0,2 17 844 0 0,-3-17-830 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,-2 3-14 0 0,1-2 119 0 0,1-1-1 0 0,-1 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-2 1 0 0,0 1-1 0 0,-1-1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,0-1-1 0 0,-4 2-118 0 0,-7 5 128 0 0,17-8-128 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,-12-22-1234 0 0,12 3-3424 0 0,5 5-3433 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34835E6">17934 11397 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-270 0 0,1 1 131 0 0,11 73 4572 0 0,-15-13-1957 0 0,3 5-1459 0 0,3 29-1321 0 0,-6 20-232 0 0,-3 73 0 0 0,-5-82 962 0 0,-11 13-720 0 0,22-118-750 0 0,0-1-89 0 0,0 0-360 0 0,0 0-163 0 0,-4-11-5760 0 0,0 1 563 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34856E6">17931 11908 1376 0 0,'0'0'65'0'0,"0"-2"389"0"0,24-33 11411 0 0,9-15-8036 0 0,3 19-1988 0 0,-34 30-1803 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-38 0 0,6 5 156 0 0,30 77 888 0 0,-32-75-884 0 0,1 1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 6-159 0 0,-8 89 1127 0 0,4-98-1133 0 0,1-8-6257 0 0,0-1-578 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34932E6">18442 11713 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 2 21 0 0,-7 45 177 0 0,-9 35 3194 0 0,6 30-1553 0 0,-4 93-172 0 0,-1-91-257 0 0,9-100-2469 0 0,4-13-3087 0 0,2 0-3929 0 0,0-1 1033 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.34952E6">18416 11713 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,13-6-181 0 0,-10 4-54 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 2 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 2 1 0 0,1-1-1 0 0,-1 0 0 0 0,3 2-301 0 0,0 0 145 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 1 0 0 0,0 4-144 0 0,6 63 1883 0 0,-23 16-1742 0 0,12-88-123 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,-3 0-18 0 0,-46 3 1171 0 0,-2 14-2729 0 0,51-18 1668 0 0,-16-3-935 0 0,1-8-3444 0 0,12 5 2477 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.3524E6">14718 11567 3224 0 0,'0'-1'240'0'0,"0"-1"165"0"0,0 1 1443 0 0,0 1 616 0 0,0 0 116 0 0,0-1 259 0 0,0-3-1698 0 0,1 2 2411 0 0,11-14-2439 0 0,-11 10-1053 0 0,-1-5 606 0 0,0 7-4232 0 0,0 4 2520 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.47889E6">5066 11499 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,3-8 314 0 0,17-68 850 0 0,-17 63-996 0 0,1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-1 0 1 0 0,2 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,2 1 1 0 0,7-8-478 0 0,-15 16 40 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-40 0 0,23 53 1331 0 0,-23-52-1287 0 0,2 11 148 0 0,-1 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,-1 4-192 0 0,5-15 21 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-22 0 0,-2-2-60 0 0,0 1-1 0 0,0-2 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-7 60 0 0,-6-53-3591 0 0,8 43 1933 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48055E6">6444 11389 4144 0 0,'0'0'319'0'0,"-9"2"1818"0"0,8-1 2461 0 0,1 0 4419 0 0,6 0-8694 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0-323 0 0,92-55 185 0 0,-67 20-185 0 0,-28 36 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-29-38 0 0 0,28 38 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-4 1 0 0 0,-36 17 0 0 0,35-11 47 0 0,1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 8-47 0 0,1-12 52 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,3 4-52 0 0,-4-6 15 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0-15 0 0,44-6-958 0 0,-33 0-1726 0 0,-2-1-3307 0 0,-5 0-1687 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48192E6">6928 11115 10304 0 0,'0'-4'934'0'0,"0"-10"-627"0"0,0 12 320 0 0,0-3 712 0 0,-1 3 3325 0 0,0 3-4568 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 2-95 0 0,-2 5 224 0 0,1 32 664 0 0,-6 118 1598 0 0,11-75-1828 0 0,-4-41-734 0 0,-2-35-364 0 0,1 8-1982 0 0,-2-11-5617 0 0,2-5 5673 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48237E6">6844 11215 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,1-2-294 0 0,1-2 74 0 0,-1 3 886 0 0,12-9 3459 0 0,-9 8-4230 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-348 0 0,31 4 963 0 0,-17-6-540 0 0,-14 0-358 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1 1-64 0 0,48 64 377 0 0,-49-57-1065 0 0,-4 2-3411 0 0,-1-9 774 0 0,1-2-4194 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48542E6">4739 11256 456 0 0,'0'-16'1413'0'0,"0"15"159"0"0,0-1 76 0 0,0-43 2855 0 0,0 44-3991 0 0,0 1 0 0 0,0 0-24 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0 47 0 0,0 0 207 0 0,0 0 89 0 0,0 0 21 0 0,0 0-24 0 0,-10 5 931 0 0,8-3-1418 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1-182 0 0,5 90 3864 0 0,1 21-3175 0 0,-11-60 34 0 0,4 17-176 0 0,1-69-729 0 0,-4 6 3 0 0,2-6-7687 0 0,1-2-336 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.48563E6">4732 11351 11976 0 0,'0'-4'180'0'0,"1"-1"0"0"0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,1-2-180 0 0,6-4 1628 0 0,-6 5-1094 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,4-1-535 0 0,-6 1 86 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,2 3-86 0 0,20 35 302 0 0,16 38 108 0 0,-28-49-1847 0 0,-8-23-150 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.5473E6">5467 11225 456 0 0,'-2'29'10790'0'0,"-5"-3"-6142"0"0,-14 83 1001 0 0,19-102-5360 0 0,-1 2-52 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 6-237 0 0,7 22 1589 0 0,-1-30-1573 0 0,-5-6-16 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2-3 0 0 0,46-82 357 0 0,-49 87-357 0 0,50-132 184 0 0,-47 90-184 0 0,-5 36-21 0 0,-5 2 2 0 0,2 4-2431 0 0,4 0 1260 0 0,-7 0-578 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.5481E6">5819 11185 2304 0 0,'0'0'428'0'0,"0"0"959"0"0,0 0 422 0 0,0 0 81 0 0,0 0-74 0 0,0 0-388 0 0,0 0-168 0 0,0 0-38 0 0,0 0-52 0 0,0 0-190 0 0,0 0-85 0 0,0 0-21 0 0,-4 13 2869 0 0,8 30-896 0 0,6 19-821 0 0,-4 32-482 0 0,14 22-8 0 0,-17-108-1420 0 0,-3-6-17 0 0,4 5 78 0 0,12 26 298 0 0,-16-32-578 0 0,0-1-4 0 0,1 1 26 0 0,4 3 65 0 0,-1 7 16 0 0,3-15 203 0 0,27-94 1554 0 0,-14 17-2314 0 0,-3 30 1122 0 0,18-34-626 0 0,-21 61-1899 0 0,-1 6 396 0 0,-8 14-8315 0 0,-5 4 2000 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55012E6">6163 15251 1376 0 0,'0'0'65'0'0,"0"0"298"0"0,0 0 1226 0 0,-4-11 8887 0 0,2 2-10689 0 0,2 8 20 0 0,0-13-1355 0 0,0 5-2483 0 0,0 6 619 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55029E6">6160 15221 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 10 0 0 0,-3 3 1224 0 0,3-13 232 0 0,0 0 48 0 0,0 0 0 0 0,0 0-1128 0 0,0 0-232 0 0,0 0-48 0 0,0-6 0 0 0,0 2-96 0 0,0 4-128 0 0,0 0 32 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55124E6">6153 15200 2760 0 0,'0'0'125'0'0,"0"-12"2231"0"0,-1 1 3939 0 0,-14 48-2743 0 0,7 58-695 0 0,16 32 396 0 0,15-20-1214 0 0,10-62-933 0 0,-30-44-1072 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-3-34 0 0,96-166 703 0 0,-72 114-639 0 0,-9-32-572 0 0,-17 77 468 0 0,0 10-31 0 0,-6-22-455 0 0,0 11-3508 0 0,5 10-3672 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59771E6">9359 15275 11952 0 0,'0'-1'67'0'0,"0"0"0"0"0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-67 0 0,-34-9 5146 0 0,36 8-5069 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 2-77 0 0,-10 8 763 0 0,6-6-634 0 0,0 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 3-128 0 0,0 1 108 0 0,-3 11 172 0 0,0 0 0 0 0,2 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,2 0-280 0 0,2 61 688 0 0,19-37-159 0 0,-7-32-346 0 0,-13-12-174 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0-9 0 0,9-8 35 0 0,-1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,1-1 0 0 0,-2 1-1 0 0,6-12-34 0 0,27-40 89 0 0,-3 7-100 0 0,-17 20-55 0 0,-21 35-4 0 0,-1-1-103 0 0,1 2-332 0 0,1 1-119 0 0,0 0-16 0 0,-2 0-596 0 0,-1 1 165 0 0,2-2-2477 0 0,1 1 1724 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59826E6">9798 14961 12064 0 0,'0'0'553'0'0,"0"0"-16"0"0,-8 14-151 0 0,-4 33 4878 0 0,4 28-1596 0 0,2-22-2083 0 0,-7 73 353 0 0,-1 17 194 0 0,1 140-900 0 0,12-189-1248 0 0,1-92-72 0 0,0-2-51 0 0,0 0-18 0 0,0 0-158 0 0,-3-25-4130 0 0,2 8-1692 0 0,-1-2-1669 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59851E6">9720 15241 2304 0 0,'18'-58'224'0'0,"-10"36"1777"0"0,16 3 11624 0 0,9 21-9044 0 0,8 22-2754 0 0,0 22-1302 0 0,-8-25-2042 0 0,-26-15-78 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55168E6">6645 15101 10136 0 0,'-10'50'1272'0'0,"8"-44"-735"0"0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,2 3-538 0 0,6 27 1513 0 0,18 70 1825 0 0,8 12-1726 0 0,10-8-228 0 0,-23-68-629 0 0,-2-14-113 0 0,-18-12-556 0 0,5-23-22 0 0,11-37 0 0 0,12-47 53 0 0,15 8-396 0 0,-9 31 158 0 0,-16-11 121 0 0,-5 11 0 0 0,4-6 0 0 0,-14 45-97 0 0,-6 12-406 0 0,0 1-165 0 0,7-8-841 0 0,-2 1-1411 0 0,-2 6-6017 0 0,2 2 8141 0 0,-4 0 11 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55301E6">7252 15446 1840 0 0,'1'4'465'0'0,"-1"3"-969"0"0,-3-2 8499 0 0,3-4-5413 0 0,0-1-959 0 0,-3 15 3293 0 0,5-13-4747 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0-168 0 0,6-3 150 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,3-5-150 0 0,6-9 74 0 0,-1-1 1 0 0,-1 0-1 0 0,-1-2 1 0 0,0 1-1 0 0,-2-2 1 0 0,8-21-75 0 0,-17 44 4 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-4 0 0,-6 3 35 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,1 2-34 0 0,0-9 18 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 1 0 0,1 0-18 0 0,4 1-63 0 0,1 1 0 0 0,0-2 0 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,10-2 63 0 0,-8 1-520 0 0,13-4-1481 0 0,-8 1-3720 0 0,0 1-1868 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55402E6">7724 14971 6624 0 0,'3'19'-4'0'0,"-2"-6"534"0"0,-1 4 5466 0 0,0-17-4969 0 0,0 0-16 0 0,-7 44 3846 0 0,1 31-3228 0 0,2 1 0 0 0,4 42-1629 0 0,0-65 228 0 0,4 11-228 0 0,-4 44-16 0 0,-4-65-2758 0 0,4-30-1657 0 0,0-11 1925 0 0,0-1-3470 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.55438E6">7687 15333 10136 0 0,'20'-72'1056'0'0,"11"-13"3846"0"0,-29 80-4603 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,4-1-299 0 0,-5 3 72 0 0,1-1-1 0 0,0 1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 2 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,3 2-71 0 0,25 23 580 0 0,9 42 1278 0 0,-28-1-3924 0 0,-11-48-2692 0 0,-2-15 3016 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59644E6">8400 14770 5872 0 0,'0'0'266'0'0,"0"0"1"0"0,-3-11 1056 0 0,3 9 7600 0 0,-8 81-5279 0 0,8-26-2198 0 0,1 28 275 0 0,-4 0-1 0 0,-5 31-1720 0 0,-11 187 1691 0 0,15-172-981 0 0,5-114-1358 0 0,-2-20-2345 0 0,-5-53-991 0 0,2 19 1937 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59675E6">8199 14780 8752 0 0,'0'0'673'0'0,"10"7"4424"0"0,12 7-302 0 0,17-11-2564 0 0,-29-3-1654 0 0,54 1 445 0 0,-44-3-776 0 0,0 1 0 0 0,0 1 0 0 0,0 1-1 0 0,0 1 1 0 0,0 1 0 0 0,9 3-246 0 0,-19-3 75 0 0,0 1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-75 0 0,33 48-3176 0 0,-37-45 1404 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.59726E6">8767 15518 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 0-276 0 0,-27 2 2318 0 0,12-7 1927 0 0,2-23-2183 0 0,16 23-2093 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,2-2-146 0 0,6-21 178 0 0,-7 19-156 0 0,1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,2 1 0 0 0,1-3-22 0 0,-5 7 22 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,2 0-22 0 0,-1 0 73 0 0,-1 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 1 0 0 0,-2-1 0 0 0,1 1-1 0 0,0 0 1 0 0,1 2-73 0 0,10 73 976 0 0,-13-62-728 0 0,0 2 22 0 0,-2 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,0-1 1 0 0,-2 6-271 0 0,2-8 132 0 0,2-12-108 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,-2 0-24 0 0,1-2 9 0 0,0 1-1 0 0,0-2 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-2-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,-3-2-8 0 0,4 2-63 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-4 63 0 0,1 5-278 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,2-4 278 0 0,4-8-2146 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60188E6">10874 15382 3680 0 0,'0'0'284'0'0,"0"0"17"0"0,3-6 3845 0 0,4-1 6650 0 0,-21 234-6730 0 0,16-198-3860 0 0,0 0-3590 0 0,-2-29 1760 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60243E6">11191 15268 920 0 0,'-3'11'76'0'0,"-21"26"272"0"0,-6-6 6376 0 0,5-9-722 0 0,23-21-4979 0 0,-4 7 987 0 0,2 17 528 0 0,5-7-1218 0 0,4-12-1123 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,5 2-198 0 0,20 11 384 0 0,-27-14-322 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-62 0 0,-2 2 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,3-2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-3 0 0 0,0 1-326 0 0,-13-19-857 0 0,14 1-6482 0 0,3 12 584 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.6007E6">10305 14882 10824 0 0,'0'0'241'0'0,"0"7"331"0"0,-6 109 4121 0 0,-1 8-200 0 0,1-18-2317 0 0,-4 60-880 0 0,10 66-5334 0 0,0-231-1053 0 0,0-1-1451 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60107E6">10619 14899 2760 0 0,'-16'-16'247'0'0,"13"15"193"0"0,2 1 1710 0 0,-1 3 4946 0 0,-3 8-4369 0 0,3-4-1946 0 0,-24 37 1201 0 0,32-2-671 0 0,-26 125 670 0 0,-21 99 167 0 0,8-127-2609 0 0,27-124-2025 0 0,2-7-2648 0 0,0 1-1568 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60129E6">10249 15292 9672 0 0,'0'0'748'0'0,"1"1"-492"0"0,2 3-231 0 0,-2-2 331 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0-356 0 0,98 17 3649 0 0,-95-16-4114 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,4 4 465 0 0,8 8-1693 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60753E6">12482 15244 1840 0 0,'0'2'133'0'0,"0"7"1371"0"0,-7 15 9957 0 0,2-12-10918 0 0,1 10 2807 0 0,3-13-2599 0 0,1-8-23 0 0,0-1-45 0 0,0 3-163 0 0,-6 42 1090 0 0,-8 102 530 0 0,11-19-1604 0 0,6-91-486 0 0,-3-35-216 0 0,0-2-402 0 0,0 0-174 0 0,5-17-2600 0 0,-3 6 1430 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60794E6">12459 15428 4144 0 0,'0'0'319'0'0,"0"0"75"0"0,-2-4 5801 0 0,0-1-4842 0 0,2-5-34 0 0,9-37 4642 0 0,6 34-3827 0 0,24-1-548 0 0,-6 20-1696 0 0,-29-6 128 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 1-18 0 0,31 8 0 0 0,-22-7 0 0 0,-7-1 0 0 0,6 11 0 0 0,-2 11-870 0 0,-12-22 616 0 0,1-2-383 0 0,0 1-179 0 0,-12 34-4440 0 0,11-32 3346 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.6059E6">11589 14930 3224 0 0,'0'0'143'0'0,"0"2"-3"0"0,-1-2 1084 0 0,-4 10-2538 0 0,3-8 6295 0 0,0-2 6252 0 0,3 17-9469 0 0,8 56 352 0 0,-22 137-1892 0 0,9-122 559 0 0,1-61-682 0 0,2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,1 0 0 0 0,1 2-101 0 0,3 27-450 0 0,-10-48-56 0 0,2-6-6442 0 0,2-2 4901 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60615E6">11573 15101 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 0 21 0 0,2 0-42 0 0,96-20 3931 0 0,-39 9-2346 0 0,-35 15-4175 0 0,-17 3 964 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60651E6">11900 15494 7744 0 0,'0'0'356'0'0,"0"0"-8"0"0,0 0-63 0 0,0 0 571 0 0,-3 9 4563 0 0,-13-48-211 0 0,22-30-2906 0 0,24 40-1872 0 0,-13 16-315 0 0,-14 12-110 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 2-4 0 0,-1 0 59 0 0,1 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 1-59 0 0,1-4 22 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1-1-23 0 0,-30 7 210 0 0,2-37-185 0 0,14 8-523 0 0,11-7-2557 0 0,7 18 1503 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60693E6">12232 15278 8288 0 0,'1'16'273'0'0,"0"-32"1643"0"0,-1 16-472 0 0,0 0 76 0 0,0 0-55 0 0,0 0-287 0 0,0 2-123 0 0,-6 44 4957 0 0,-7-1-5210 0 0,12 95 812 0 0,5-41-1951 0 0,-4-93-1422 0 0,0-5-625 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.60843E6">12124 15037 8752 0 0,'20'16'1346'0'0,"-20"-14"-166"0"0,2-2-1575 0 0,2-4 4378 0 0,3-4 4520 0 0,3 1-11521 0 0,-6 3 1866 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61118E6">12923 15514 6912 0 0,'70'11'8898'0'0,"-65"-10"-8618"0"0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,2-4-280 0 0,31-51 1321 0 0,-35 52-1321 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0-2-1 0 0,-17-34-90 0 0,14 39 124 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-34 0 0,-50 23 664 0 0,47-18-600 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 3-64 0 0,2-1 41 0 0,0 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,3 8-41 0 0,-3-11 98 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,5 6-98 0 0,-6-11 5 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-5 0 0,1-1-54 0 0,98-32-5788 0 0,-58 8 1619 0 0,-21 11 2079 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61533E6">14274 15358 1840 0 0,'0'0'83'0'0,"0"0"169"0"0,0 0 668 0 0,0 0 288 0 0,0 0 58 0 0,0 0-22 0 0,0 0-144 0 0,0 0-63 0 0,0 0-11 0 0,0 0-2 0 0,0 8 2048 0 0,-3 19-266 0 0,2-2-362 0 0,1 78 1520 0 0,-2-32-3723 0 0,1 18-415 0 0,2-81 488 0 0,4 6-6100 0 0,0-7-783 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61567E6">14278 15514 10136 0 0,'19'-57'5082'0'0,"8"11"-1747"0"0,-4 27-1698 0 0,-21 16-1500 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,1 0-137 0 0,0 1 60 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 3-60 0 0,15 17 54 0 0,-6-15-897 0 0,-9-7-100 0 0,-1-2-37 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61341E6">13529 14750 2304 0 0,'0'0'101'0'0,"0"0"294"0"0,0 0 1149 0 0,0 0 506 0 0,0 2 1554 0 0,0 9-1838 0 0,2 148 6571 0 0,-2 118-5024 0 0,-13-9-1402 0 0,10-164-1693 0 0,-6-29-376 0 0,8-74-114 0 0,1-1-766 0 0,-4-11-2968 0 0,-3-2-3447 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61375E6">13505 14951 920 0 0,'0'-1'67'0'0,"-3"-7"403"0"0,4 0 4358 0 0,4-6-1924 0 0,-4 11-1691 0 0,17-32 4007 0 0,23-5-3052 0 0,6 8-888 0 0,-28 24-1087 0 0,-17 7-85 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1-108 0 0,0 0 199 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,3 4-199 0 0,27 61 460 0 0,-25-41-231 0 0,0 2 1 0 0,-2-1-1 0 0,-1 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,-2 27-229 0 0,0-48 147 0 0,-1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-3 3-146 0 0,3-7 10 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 0 0 0,-4-2-10 0 0,-3-3-494 0 0,0 0-1 0 0,1-1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-3-6 495 0 0,3 1-5994 0 0,3-5-1719 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61458E6">13882 15514 8288 0 0,'0'0'190'0'0,"4"-6"253"0"0,9-6-212 0 0,26 0 5159 0 0,2 7-1205 0 0,-16 13-2607 0 0,-3-2 202 0 0,-14-4-715 0 0,-15-5-592 0 0,-34 8 113 0 0,-36 16 500 0 0,73-19-1076 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 2-10 0 0,-2 6 2 0 0,1-6-2 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,3 5 0 0 0,11 14 0 0 0,-15-25 1 0 0,2 2 37 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,2-1-39 0 0,43-29 241 0 0,-36 16-275 0 0,-1 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,0-2 34 0 0,12-69-964 0 0,-14 34 382 0 0,-16 90 634 0 0,9-24-10 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,2-1-1 0 0,0 1 1 0 0,3 7-42 0 0,14 45 54 0 0,-8-42-1794 0 0,-7-22 730 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61927E6">14869 14865 3224 0 0,'0'0'143'0'0,"0"0"279"0"0,0 0 1073 0 0,0 0 470 0 0,0 0 92 0 0,0 0-154 0 0,0 0-730 0 0,0 0-315 0 0,0 7 684 0 0,-3 1-898 0 0,3-6-48 0 0,0 7 1051 0 0,-7 47 1551 0 0,-33 303 1366 0 0,37-333-4246 0 0,2 0 0 0 0,0 0-1 0 0,2 0 1 0 0,0 1 0 0 0,2-1-1 0 0,0-1 1 0 0,1 1-1 0 0,6 18-317 0 0,20 15 208 0 0,-28-54-186 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-2 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,3 0-22 0 0,-4-2 31 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1-30 0 0,-2 5 3 0 0,9-17 55 0 0,-2 0 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,3-17-58 0 0,5-18 41 0 0,21-98-41 0 0,14-148-432 0 0,-44 262-57 0 0,-1 7-2509 0 0,-2 9-4848 0 0,0 12 100 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62065E6">15902 15394 2304 0 0,'0'0'101'0'0,"0"17"22"0"0,-7 6 6125 0 0,-3 17 4249 0 0,8-9-9080 0 0,-2 87 316 0 0,0-84-1477 0 0,1-21-426 0 0,2-12-721 0 0,1-1-329 0 0,0 0-75 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62116E6">16132 14930 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 2-242 0 0,4 71 6774 0 0,-8 3-1144 0 0,-8 43-2340 0 0,2 49-2718 0 0,6-9-705 0 0,0 16-1521 0 0,4-164 244 0 0,0-9-61 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62155E6">16367 15360 10136 0 0,'0'0'777'0'0,"-1"2"-505"0"0,-3 43 4407 0 0,3-12-457 0 0,3 79-789 0 0,-4-104-3589 0 0,2 0-1781 0 0,0-7 758 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62214E6">16751 15348 1376 0 0,'1'-2'299'0'0,"11"-58"5252"0"0,-14 43-5059 0 0,1 13-375 0 0,1 3 35 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,1-1-152 0 0,-3 1 283 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-285 0 0,-7 12 754 0 0,-42 66 501 0 0,31-7-220 0 0,21-68-992 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,4 3-41 0 0,1 6 59 0 0,7 9 178 0 0,-12-20-112 0 0,0 0 0 0 0,0 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-125 0 0,-12 16 28 0 0,8-19-9 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-2 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1-19 0 0,-34 2-215 0 0,6 22-3705 0 0,29-16-4023 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62285E6">17055 15446 3680 0 0,'0'0'284'0'0,"0"0"109"0"0,2-1 1154 0 0,27-18 5762 0 0,31 18-2771 0 0,-31 12-2764 0 0,-16-1 1490 0 0,-56-16-3312 0 0,39 4 32 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-3 3 16 0 0,1-1 34 0 0,-1 0-1 0 0,1 1 0 0 0,0 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 3-33 0 0,3-7 57 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 2-56 0 0,-1-4 45 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1-45 0 0,91-156-3426 0 0,-93 160 3373 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 53 0 0,-2 20 337 0 0,-15 82 1575 0 0,10 6-1206 0 0,14-63-7272 0 0,-4-35-749 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.61995E6">15614 14814 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 2 76 0 0,-5 11 2311 0 0,-6 38 3900 0 0,-3 115-3759 0 0,-16 87 806 0 0,4 41-2464 0 0,19-203-1627 0 0,7-90-756 0 0,-3-6-2095 0 0,3-4 1602 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62019E6">15538 15095 11232 0 0,'-4'-29'1016'0'0,"5"29"-836"0"0,12-29 2777 0 0,60 24 2000 0 0,15 19-1797 0 0,-49 7-4345 0 0,-32-17-189 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62446E6">17905 15521 15664 0 0,'13'5'1187'0'0,"-11"-4"-976"0"0,1-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-2-210 0 0,7-13-211 0 0,-4 9-129 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-10 340 0 0,-7-34-1540 0 0,3 51 1562 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-22 0 0,-19 17 1568 0 0,17-13-1383 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,0 1-185 0 0,-6 32 308 0 0,4-27-103 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,1 0 0 0 0,0 3-205 0 0,14 19 1394 0 0,-16-34-1436 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1 42 0 0,0 0-47 0 0,85-59-5723 0 0,-74 51 4417 0 0,-3 0-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.6237E6">17517 15193 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0-6 199 0 0,3-21 284 0 0,-3 26 22 0 0,0 1 21 0 0,0 0 53 0 0,0 0 198 0 0,0 0 86 0 0,0 0 21 0 0,0 0-28 0 0,0 1-122 0 0,-9 88 4045 0 0,2-22-3014 0 0,-20 182 836 0 0,13-109-2456 0 0,12-124-5049 0 0,1-15-3688 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62393E6">17497 15313 19351 0 0,'0'0'439'0'0,"0"0"62"0"0,0 0 33 0 0,0 0-65 0 0,7-3-292 0 0,86-18 2799 0 0,-37 10-2385 0 0,-21 8-4619 0 0,-33 3 2335 0 0,-2 0-17 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62896E6">18258 15404 920 0 0,'0'0'115'0'0,"0"0"146"0"0,0 0 68 0 0,2-1 14 0 0,10-26-975 0 0,1 13 771 0 0,-12 12 195 0 0,-1 2 149 0 0,0 0 590 0 0,0 0-1059 0 0,6-7 9846 0 0,-2 4-8006 0 0,-3 1-1530 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1-1-324 0 0,1-1 1337 0 0,0 4-893 0 0,-9 8-200 0 0,-28 59 2244 0 0,12 5-1504 0 0,23-16-648 0 0,2-55-335 0 0,1 7 28 0 0,0-1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,1 1-28 0 0,-1-3 14 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,4-1-13 0 0,31-21 64 0 0,-3-47 8 0 0,-14-11-72 0 0,-16 42-89 0 0,2-53-263 0 0,-9 93 324 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 29 0 0,-3 9-8024 0 0,1 0 350 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62952E6">18714 15275 2304 0 0,'0'0'101'0'0,"0"0"363"0"0,0 0 1439 0 0,0 0 626 0 0,0 0 126 0 0,0 0-194 0 0,3-14 1239 0 0,-1 23 4485 0 0,0 48-5205 0 0,-6 21-1571 0 0,1 35-565 0 0,-4-51-599 0 0,8 98 126 0 0,5-102-812 0 0,6-132-3199 0 0,-11 24-1172 0 0,-1 37 2865 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.62976E6">18721 15419 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-150 0 0,-7-5 3377 0 0,16-32 352 0 0,32-14-1964 0 0,-35 48-2182 0 0,-3 1 153 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,3 1-123 0 0,33 13 165 0 0,-8 20-245 0 0,-9 22-3497 0 0,-21-54-1940 0 0,-1-2-1564 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.63177E6">19319 15244 9416 0 0,'-2'-4'852'0'0,"-22"-10"284"0"0,14 12 6835 0 0,-10 31-4820 0 0,16-20-2774 0 0,-46 128 2838 0 0,22-39-1934 0 0,20-71-1118 0 0,2 0 0 0 0,1 1-1 0 0,0 0 1 0 0,2 0 0 0 0,1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,3 6-163 0 0,-2-16-6 0 0,13 117-229 0 0,4-77-1218 0 0,-1-37-2030 0 0,-10-15-2522 0 0,-5-5-1562 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.63203E6">19640 15197 11520 0 0,'0'0'886'0'0,"1"-1"-582"0"0,15 6 5156 0 0,-12-1-5008 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 5-452 0 0,5 13 803 0 0,6 61 1048 0 0,-10-35-1193 0 0,-4 50 394 0 0,-5 10-300 0 0,-10 5-403 0 0,-12 46-253 0 0,1-47-2616 0 0,-8-4-4080 0 0,18-61-2023 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.63734E6">2265 13773 2760 0 0,'-20'-11'247'0'0,"9"-2"39"0"0,10 13 290 0 0,-3-1-375 0 0,1-4 6201 0 0,2-1-5440 0 0,13 4 7229 0 0,-7 2-9038 0 0,92 45 4699 0 0,-28-9-2217 0 0,48-15-519 0 0,45 0-182 0 0,-19 27-394 0 0,-118-36-455 0 0,-4 0-32 0 0,1-1 0 0 0,0-1-1 0 0,0-2 1 0 0,1-1-1 0 0,0 0 1 0 0,0-2-1 0 0,1-1 1 0 0,-1-2-1 0 0,1 0 1 0 0,6-2-53 0 0,140-29 1189 0 0,90-38-261 0 0,-93 44-928 0 0,-140 21 0 0 0,280-2 0 0 0,-23 32 15 0 0,24-11 250 0 0,13 13-174 0 0,-116-13 135 0 0,-9 4-42 0 0,116 20-48 0 0,-211-30-125 0 0,78 13 42 0 0,188 33 22 0 0,116 2 393 0 0,-197-19-403 0 0,334 59 135 0 0,-253-57-200 0 0,-47 1-61 0 0,-51-2 141 0 0,8 4-80 0 0,-97-24 0 0 0,75-1 0 0 0,152 7 0 0 0,-170-6 0 0 0,69-8 0 0 0,178-23 0 0 0,-283 11 0 0 0,-32 5 0 0 0,294-2 0 0 0,-254-14 0 0 0,388-11-9 0 0,-304 1 914 0 0,-18-9-1376 0 0,63 5 966 0 0,-78 29-599 0 0,-6 4-152 0 0,-127 2 112 0 0,-3 6 239 0 0,3-3 314 0 0,54 6-541 0 0,29-16-88 0 0,3-7 252 0 0,-109-4-160 0 0,188-28 128 0 0,-62 1 0 0 0,-42 5 11 0 0,8 0-22 0 0,112 5 11 0 0,-31 4 80 0 0,108 6-133 0 0,-148 17 42 0 0,184-16 11 0 0,-123 9 0 0 0,40 0 0 0 0,300 26 139 0 0,-127-30-86 0 0,-306 23 75 0 0,-17-3-128 0 0,-81-19 0 0 0,-8-9 148 0 0,25-12-132 0 0,-40 16-28 0 0,64 15 12 0 0,-48 6-96 0 0,-93-8 80 0 0,-9 3 5 0 0,-12 12-319 0 0,19-2 154 0 0,9 7-187 0 0,-8 3 347 0 0,0 61 16 0 0,-5 86 15 0 0,13 162 28 0 0,-1-117-101 0 0,17 27 233 0 0,-4-5-91 0 0,-5 21-20 0 0,-25-46 106 0 0,-5-63-95 0 0,0-20-75 0 0,0 17 0 0 0,0-28 224 0 0,-6-29-160 0 0,13-84-64 0 0,1-2 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-2 1 0 0 0,-16 8 0 0 0,4-9 0 0 0,-287 7 96 0 0,105-13-96 0 0,-219 3 0 0 0,52 3 71 0 0,-112 7-86 0 0,-140-20 71 0 0,40 0-136 0 0,53 3 80 0 0,84 0 0 0 0,-343-11 0 0 0,144 1 68 0 0,179 8 268 0 0,256 9-440 0 0,-543-18 204 0 0,252-19-164 0 0,102 6 77 0 0,-352-3 78 0 0,305 14-91 0 0,-3-17 0 0 0,23 5 0 0 0,86 15 0 0 0,71 10 0 0 0,-207 7 0 0 0,203 4 0 0 0,-775-1 0 0 0,268-46 0 0 0,286 8 0 0 0,-119-10 0 0 0,402 23 0 0 0,1-10 0 0 0,-67-10 0 0 0,163 31 0 0 0,0 5 0 0 0,-101 10 0 0 0,29 9 0 0 0,14 0 0 0 0,-35-9 0 0 0,21-14 0 0 0,-20 3 0 0 0,-160-3 0 0 0,170 17 0 0 0,-30-14 0 0 0,58 4 0 0 0,144 4 0 0 0,-116 7 0 0 0,-61-7 0 0 0,101-8 0 0 0,-48-10 0 0 0,56 10 0 0 0,-80 4 0 0 0,107-4 0 0 0,-71 0 0 0 0,44-5 0 0 0,82 11-60 0 0,4 1-252 0 0,1 0-111 0 0,0 0-1358 0 0,0 0-5615 0 0,0 0-2407 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.64323E6">2259 13660 1376 0 0,'0'0'65'0'0,"0"1"-6"0"0,0 17 154 0 0,0-16 831 0 0,0-2 358 0 0,0 0 65 0 0,0 0-83 0 0,0 0-422 0 0,0 0-186 0 0,0 0-38 0 0,0 0-28 0 0,0 0-88 0 0,0 0-40 0 0,0 0-6 0 0,0 0 2 0 0,0 0 12 0 0,0 0 2 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0-1 0 0,0 9 1801 0 0,6 105 2520 0 0,1-8-2608 0 0,3 115-760 0 0,-10-2-472 0 0,34 57-113 0 0,-28-238-854 0 0,20 102-208 0 0,-1 69 1907 0 0,-12-83-2238 0 0,16 175 898 0 0,-33-185-286 0 0,-47 142-20 0 0,45-159-169 0 0,6-49-56 0 0,-3 10 374 0 0,-13 49-182 0 0,15-23-546 0 0,8-12 992 0 0,4-2-446 0 0,-9-66-106 0 0,-1-5-17 0 0,-1-1-234 0 0,-6-18-3530 0 0,6 9 2303 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.86899E6">2341 7605 4144 0 0,'0'0'319'0'0,"-5"1"252"0"0,5-2 2376 0 0,22-31-2360 0 0,-26 13 5029 0 0,4 18-5505 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-112 0 0,-49 23 1284 0 0,15 1-659 0 0,-29 36 50 0 0,18-11-590 0 0,-89 126 107 0 0,45-43-21 0 0,5 2 334 0 0,13-5-252 0 0,-15 47-182 0 0,-52 145 566 0 0,126-284-548 0 0,-55 176 254 0 0,2 101-151 0 0,35-58 504 0 0,13-108-216 0 0,8 106 134 0 0,8-137-457 0 0,-2 110 104 0 0,12-113-187 0 0,5-1-1 0 0,15 60-73 0 0,4-10 269 0 0,25 66-269 0 0,-6-40 164 0 0,17 66 46 0 0,-15-74 888 0 0,60 138-1098 0 0,15 34 320 0 0,-89-236-133 0 0,21 45 186 0 0,-2-46 46 0 0,16 57-249 0 0,-13-25-191 0 0,-19-56 21 0 0,22 54 139 0 0,-33-59-22 0 0,-27-79-141 0 0,-3-7-107 0 0,0-2-69 0 0,0 0-21 0 0,0-3-260 0 0,0-9-1082 0 0,-3-4-465 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.86969E6">1686 13345 13824 0 0,'-49'24'1677'0'0,"47"-23"-740"0"0,27-3 3060 0 0,5 0-4365 0 0,70 37 323 0 0,0 33 373 0 0,-10 8 165 0 0,110 105 1071 0 0,-176-164-1495 0 0,-1-2-1 0 0,2-1 0 0 0,-1-1 0 0 0,2-1 1 0 0,20 5-69 0 0,64 13 245 0 0,-49-23 458 0 0,-48-18 147 0 0,-12 9-799 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-2-51 0 0,0-5 176 0 0,-19-113 411 0 0,-19-86-1189 0 0,0 67-4384 0 0,20 87 2801 0 0,-4 9-21 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1.87098E6">2532 13727 2760 0 0,'-7'-3'248'0'0,"-33"-31"6865"0"0,23 4-6498 0 0,-13-19 774 0 0,-3-6 1367 0 0,2-27 825 0 0,7 5-1573 0 0,17 19-676 0 0,-1-14-560 0 0,11-76 1085 0 0,17 5-1137 0 0,-11 93-1006 0 0,-12 5-1132 0 0,1 8-1456 0 0,3 35 1591 0 0,4 0-48 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87216E6">4602 10374 14976 0 0,'-24'21'1597'0'0,"-12"-7"-1817"0"0,35-14 85 0 0,1 0-121 0 0,-8-1-614 0 0,-3-22 1632 0 0,3-15 143 0 0,-8-55 2063 0 0,-1-15-936 0 0,1-84-705 0 0,12-23-328 0 0,0 21-897 0 0,2-166 234 0 0,1-27 12 0 0,8 202-193 0 0,-1-125-36 0 0,-8 155-1315 0 0,27 90-2477 0 0,-17 52 2086 0 0,1-15-2513 0 0,-8 24 1999 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87257E6">3956 8288 18887 0 0,'0'0'863'0'0,"-1"-1"-14"0"0,1-12-806 0 0,-1 1-1 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,2-1-42 0 0,-2 0-42 0 0,119-204-129 0 0,-59 112 171 0 0,27-2 0 0 0,-82 95 2 0 0,-1 1-1 0 0,1 0 0 0 0,0 1 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 2-1 0 0,1-1 0 0 0,5 0-1 0 0,-10 5 48 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 2 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 2-47 0 0,70 216 1312 0 0,-19-36-1200 0 0,-27-64-32 0 0,-1-30-402 0 0,4-42-2524 0 0,-21-46 814 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87403E6">2174 15272 13040 0 0,'-3'7'1185'0'0,"-23"29"-737"0"0,2-28 563 0 0,-30-22 2664 0 0,24-3-2667 0 0,-37-18 867 0 0,34 16-1425 0 0,0-1 0 0 0,2-2 0 0 0,0-2-1 0 0,2-1 1 0 0,-14-15-450 0 0,-162-174 1230 0 0,175 178-981 0 0,-28-30-91 0 0,3-4 0 0 0,3-2 1 0 0,-3-10-159 0 0,-125-221 786 0 0,-85-179 150 0 0,174 267-915 0 0,9-4 1 0 0,8-5-1 0 0,-6-58-21 0 0,-61-201 160 0 0,65 179-160 0 0,-46-195-216 0 0,73 261 184 0 0,9-3 0 0 0,3-65 32 0 0,3-72-64 0 0,8 70 0 0 0,15 186 64 0 0,5 0 0 0 0,6-110 0 0 0,3 166 0 0 0,5-74 0 0 0,18-97 0 0 0,27-111-80 0 0,51-149-171 0 0,-6 153-223 0 0,-16 98 455 0 0,-45 154 70 0 0,4 2 0 0 0,3 3-1 0 0,8-6-50 0 0,-22 41 25 0 0,78-115 30 0 0,41-1-129 0 0,8 30-44 0 0,33-36-58 0 0,-146 130 134 0 0,78-63-842 0 0,-122 107 868 0 0,24-14-1611 0 0,-13 11-5936 0 0,-10 3 272 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87445E6">1365 6048 11976 0 0,'0'0'922'0'0,"-1"-2"-600"0"0,-7-9-54 0 0,7 10 932 0 0,-1-8 2652 0 0,1-6-2353 0 0,4 11-1499 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,2 0 1 0 0,17-11-106 0 0,88-31-209 0 0,-101 40 308 0 0,0 0-1 0 0,0 2 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 2-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,7 5 8 0 0,-7-2 12 0 0,0 0 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 2-1 0 0,0-1 1 0 0,5 11-12 0 0,-4-4 37 0 0,0 1 0 0 0,-1 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,-2 0 1 0 0,3 17-38 0 0,-4 88 434 0 0,-27-12 5 0 0,13-77-354 0 0,-46 122 75 0 0,-60 119-1810 0 0,106-249 551 0 0,-2-2-48 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87588E6">8232 5839 13360 0 0,'-4'-1'271'0'0,"1"0"1"0"0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-272 0 0,0-3 27 0 0,0 1 0 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1-4-27 0 0,-1-8 302 0 0,-10-128 1863 0 0,-6-5-421 0 0,-5-149 624 0 0,5 54-1161 0 0,-12-355-614 0 0,22 347-593 0 0,-1 78-104 0 0,7 170 61 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0-1 43 0 0,2 8-62 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 62 0 0,-7 16-1775 0 0,1 4-289 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="1.87619E6">7550 3518 22607 0 0,'0'0'514'0'0,"-1"-2"71"0"0,-1 0-530 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1-55 0 0,11-18-19 0 0,0 0-1 0 0,0 2 0 0 0,2-1 1 0 0,0 2-1 0 0,0 0 1 0 0,2 1-1 0 0,-1 1 0 0 0,2 1 1 0 0,0 0-1 0 0,3 0 20 0 0,21-20-44 0 0,-34 27-32 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 76 0 0,-5 2-16 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,1 0 16 0 0,49 140 542 0 0,-28-90-361 0 0,1-1 0 0 0,3-1 1 0 0,16 24-182 0 0,39 48-220 0 0,-45-66-1394 0 0,-19-35-78 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">23709 6389 0 0 0,'0'0'580'0'0,"0"0"-64"0"0,0 0 47 0 0,0 0-35 0 0,0 0-254 0 0,0 0-107 0 0,0 0-27 0 0,0 0 51 0 0,0 0 229 0 0,0 0 100 0 0,0 2 21 0 0,3 13 472 0 0,-3-13-554 0 0,0-2-3 0 0,0 0-54 0 0,0 0-223 0 0,0 0-98 0 0,0 0 51 0 0,0 0 272 0 0,0 0 95 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 0 0 0,0 6 0 0 0,0-7 0 0 0,0-1 0 0 0,0 0 36 0 0,0 0 150 0 0,0 0 66 0 0,0 0 18 0 0,0 0-29 0 0,0 6 436 0 0,2 51 2189 0 0,-4 62-643 0 0,-9-37-852 0 0,-7 67-1718 0 0,16-50-165 0 0,1-91 90 0 0,0 1-403 0 0,1 8-2730 0 0,-4-28-1033 0 0,-1 2-2741 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="208.461">23704 6445 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,8-3-112 0 0,0 0 125 0 0,-1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-2 1 0 0 0,1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1-346 0 0,48 68 1246 0 0,-52-64-1102 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-2 0 0 0,0 1-1 0 0,-2 1 1 0 0,0-1-1 0 0,0 2-143 0 0,2-4 57 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0-57 0 0,-96-6-816 0 0,65-14-3738 0 0,29 12 2908 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55956.919">25238 15461 456 0 0,'23'-41'0'0'0,"-7"27"2824"0"0,-7 3 664 0 0,-8 11-2678 0 0,-1 0 44 0 0,0 0 11 0 0,0 0 6 0 0,0 0 21 0 0,0 0 85 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,4-21 2411 0 0,-19 3-1851 0 0,14 16-1397 0 0,-1-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 1-117 0 0,-4 2 139 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-3 7-139 0 0,-20 33 224 0 0,-5 46 448 0 0,32 4 696 0 0,2-92-1368 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,2 0 1 0 0,-1 0 0 0 0,-2-1 16 0 0,1-1 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1-1 1 0 0,-1 2-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0-16 0 0,4 0-124 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 0 125 0 0,12-6-613 0 0,19-15-2912 0 0,-19 11 1494 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55516.919">25596 15153 5984 0 0,'3'-41'472'0'0,"-1"1"5162"0"0,-2 38-3819 0 0,0 2-663 0 0,0 0-288 0 0,0 0-58 0 0,0 0-20 0 0,0 0-61 0 0,0 0-21 0 0,0 0-7 0 0,-9 5 1975 0 0,-17 107 1356 0 0,-29 205-3264 0 0,30-140-640 0 0,8-28-1060 0 0,16-133-1236 0 0,1-11-5747 0 0,0-5 911 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55296.919">25539 15329 9216 0 0,'0'0'706'0'0,"0"0"-114"0"0,4-5 3675 0 0,20-10 1993 0 0,17 5-3644 0 0,12-5-1858 0 0,5 19-1979 0 0,-52 6-2143 0 0,-3-2 1389 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-66366.92">24199 14907 6304 0 0,'15'-1'822'0'0,"-15"0"-83"0"0,0 1 249 0 0,0 0 48 0 0,0 0-31 0 0,0 0-170 0 0,0 0-71 0 0,0 0-17 0 0,0 0-27 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0 48 0 0,0 0 202 0 0,0 0 87 0 0,0 0 20 0 0,0 0-70 0 0,0 0-308 0 0,-1-1-137 0 0,-51-64 1234 0 0,-31 2 383 0 0,78 60-1902 0 0,-2 0 0 0 0,1 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-6 2-14 0 0,-30 31 373 0 0,8 2-682 0 0,-13 56 985 0 0,28-16-666 0 0,-1 44 460 0 0,17 9-108 0 0,14-12-298 0 0,19 15-7518 0 0,-27-128 13 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-66056.919">23723 15296 11976 0 0,'0'0'546'0'0,"5"-11"204"0"0,14 5 2195 0 0,37-8 2019 0 0,27-2-3091 0 0,-39 18-1743 0 0,0 2 0 0 0,-1 0 1 0 0,29 9-131 0 0,-23 0-3223 0 0,-34-9 2016 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-65316.919">24251 15504 920 0 0,'1'-3'80'0'0,"-1"2"-114"0"0,9-20 1775 0 0,21-24 8599 0 0,-15 35-9435 0 0,-1 2-70 0 0,-12 6-714 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,1 2-121 0 0,32 29 1528 0 0,-19 31 812 0 0,-18-55-2114 0 0,0-1 0 0 0,-1 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,1 0-226 0 0,-1-3 108 0 0,2 1 0 0 0,-2-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,2-1 0 0 0,-2 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,-5 1-108 0 0,6-3-56 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 0 1 0 0,-1 1 0 0 0,1-2-1 0 0,0 1 1 0 0,0-2 56 0 0,1-34-2485 0 0,3 21 635 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-57246.919">24609 15325 9616 0 0,'0'0'216'0'0,"0"0"32"0"0,1-2 12 0 0,9-22 16 0 0,9-31 4156 0 0,-19 53-3764 0 0,0 2 151 0 0,0 0 69 0 0,0 0 10 0 0,0 0-48 0 0,0 0-216 0 0,0 0-98 0 0,0 0-22 0 0,-8 60 3070 0 0,4-6-2456 0 0,-13 157 920 0 0,17-145-2048 0 0,-1-21-64 0 0,1-44-273 0 0,0-1-138 0 0,0 0-33 0 0,0 0-217 0 0,0-8-2919 0 0,1-4 1541 0 0,2 0-9 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-56836.919">24549 15470 10136 0 0,'0'0'42'0'0,"0"1"-1"0"0,0-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,2 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-42 0 0,31-33 4246 0 0,12 4-1699 0 0,-39 25-2345 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,3 0-202 0 0,29 18 1351 0 0,-32-11-1230 0 0,-2 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2 4-121 0 0,25 80 144 0 0,-18 1-545 0 0,-19-77-269 0 0,5-11-1904 0 0,0-3-3466 0 0,-1 0-762 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45426.919">25902 15501 456 0 0,'11'-3'13004'0'0,"-6"12"-6955"0"0,-9 19-4332 0 0,2-13-273 0 0,7 97-283 0 0,-3-72-2968 0 0,0-1-3416 0 0,-2-39-2002 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45206.919">25987 15146 5984 0 0,'0'0'273'0'0,"0"0"-5"0"0,0 0 121 0 0,0 0 1143 0 0,0 0 514 0 0,0 0 104 0 0,0 0-119 0 0,0 0-596 0 0,0 0-261 0 0,0 0-49 0 0,0 0-98 0 0,0 0-392 0 0,0 0-171 0 0,0 0-31 0 0,0 0-64 0 0,0 0-1670 0 0,0 0-5837 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44826.919">26134 15765 11232 0 0,'0'-4'1016'0'0,"-19"-76"3747"0"0,30 12-109 0 0,-8 60-4545 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 2 0 0 0,2-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 2 0 0 0,1-1 0 0 0,3-1-109 0 0,-6 3 0 0 0,-1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,2 0 0 0 0,15 39 10 0 0,-17-31 52 0 0,-7 48 1898 0 0,-36 27-1744 0 0,37-82-173 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-2-1 1 0 0,2 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-2 0 0 0,-1 2-1 0 0,2-1 1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-4-1-43 0 0,3-1-36 0 0,-2 1 0 0 0,0-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,0-2 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-3 36 0 0,5-34-2989 0 0,1 24 1539 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-43876.919">26557 15550 456 0 0,'0'0'83'0'0,"0"0"42"0"0,0 0 131 0 0,0 0 32 0 0,0 0 0 0 0,0 0 49 0 0,0 0 209 0 0,0 0 94 0 0,0 0 21 0 0,0 0-5 0 0,0 0-33 0 0,0 0-14 0 0,0 0-1 0 0,0 0-74 0 0,0 0-307 0 0,0 0-135 0 0,0-1-36 0 0,10-35 684 0 0,-2-6 547 0 0,-4 18-691 0 0,-4-24 2561 0 0,0 47-2790 0 0,0 1 1 0 0,0 0 0 0 0,0 7 8134 0 0,-4 25-7718 0 0,-10 120 1476 0 0,-1-82-2207 0 0,15-61-53 0 0,0-4-32 0 0,0-3-137 0 0,0-2-71 0 0,0 0-16 0 0,0 0-147 0 0,0 0-589 0 0,0 0-257 0 0,0 0-51 0 0,0 0-35 0 0,0 0-102 0 0,2 14-5517 0 0,-2-14 5738 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-43576.919">26564 15590 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,0 0-140 0 0,0 0 368 0 0,0 0 187 0 0,0 0 42 0 0,-7-6 963 0 0,6 2-1582 0 0,1-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-2 0 0 0,0 1 1 0 0,0 2-1 0 0,1-2 0 0 0,-1 0 0 0 0,4-2-240 0 0,-6 5 154 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,-1-1-153 0 0,8 3 222 0 0,18 15-38 0 0,-4 9-184 0 0,-21-24 130 0 0,0 1-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2 4-130 0 0,3 32 130 0 0,4-17-130 0 0,-1-19-97 0 0,23-10-2811 0 0,-19 1 1087 0 0,0-2-377 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1576.986">23215 6293 4608 0 0,'0'0'353'0'0,"5"10"155"0"0,-3-6 2425 0 0,10 26 3145 0 0,-10-8-3733 0 0,-12 21 1085 0 0,1 15-1742 0 0,3-7-736 0 0,11 42-312 0 0,-9-16-640 0 0,8-22 0 0 0,-17-9 0 0 0,13-41-9 0 0,0 0-146 0 0,0-1-4162 0 0,0-4-2729 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-759.69">23200 6581 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,4-3 272 0 0,1 1 2425 0 0,8-13-1132 0 0,8 6-314 0 0,-20 9-1141 0 0,10-10 879 0 0,28-21 835 0 0,9 16-867 0 0,-47 15-985 0 0,8-2 305 0 0,41 12-1282 0 0,-40-3 625 0 0,-7 27 186 0 0,-7 1 15 0 0,0-8 170 0 0,-3 12-74 0 0,5-38-411 0 0,2-1-12 0 0,0 0 37 0 0,3 10 308 0 0,16 8-12 0 0,-18-17-372 0 0,7 16-262 0 0,-1 9-1153 0 0,-6-25 785 0 0,-1-1-831 0 0,0 0-363 0 0,0 0-70 0 0,0 0-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2740.813">22729 6416 2304 0 0,'2'0'473'0'0,"3"-1"1939"0"0,-5 6 6695 0 0,-1 0-5123 0 0,2 2-5610 0 0,-4 31 3901 0 0,5 1 62 0 0,5 56-84 0 0,7 3-1147 0 0,-4-10 156 0 0,-10 10-32 0 0,-10 12-700 0 0,12-97-583 0 0,-2-12-216 0 0,0-1-65 0 0,0-2-2 0 0,2-34-3313 0 0,-6 24 1834 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2395.418">22751 6439 6912 0 0,'-12'-8'528'0'0,"30"-1"-128"0"0,7-9 4668 0 0,35 16 409 0 0,-56 2-5324 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0 0 0 0,1 2-153 0 0,35 67 2062 0 0,-24 7-1603 0 0,-15-3 1130 0 0,-1-69-1534 0 0,-2 0 1 0 0,2-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,-2-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1-55 0 0,-27 5 67 0 0,32-10-206 0 0,-2 0-58 0 0,-2 0-1 0 0,2-1 1 0 0,-2 1 0 0 0,2-1-1 0 0,0 0 1 0 0,-2 0-1 0 0,2-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-2-1 0 0,0 1 1 0 0,0-1-1 0 0,-1-1 198 0 0,-5-4-5692 0 0,-6-2-1767 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="75099.81">3490 14089 7488 0 0,'0'2'340'0'0,"-7"96"3520"0"0,14 108 4791 0 0,-6 31-4784 0 0,6-60-3019 0 0,4-71-648 0 0,2-64-288 0 0,-13-40-387 0 0,0-2-33 0 0,0 0-192 0 0,0 0-790 0 0,0-5-352 0 0,2-19-70 0 0,-2-4-7 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="75669.811">3540 14184 8288 0 0,'-4'16'381'0'0,"3"-13"-6"0"0,9-34-227 0 0,-7 16 279 0 0,2 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 1 0 0 0,6-6-427 0 0,-10 12 230 0 0,2-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 1 0 0 0,2 0-230 0 0,56-2 1008 0 0,-60 5-919 0 0,1 1 0 0 0,-2 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 2 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0-1 0 0,-2 1 1 0 0,5 3-89 0 0,1 5 277 0 0,-2-1 1 0 0,0 1-1 0 0,0-2 0 0 0,-1 3 0 0 0,0 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 8-277 0 0,10 84 608 0 0,-10-93-471 0 0,-2-1-1 0 0,1 1 1 0 0,-2 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-2 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,-2-3 1 0 0,1 2-1 0 0,-1 0 1 0 0,-1 0-1 0 0,0-2 1 0 0,-1 1-1 0 0,-1 2-136 0 0,0-6 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,-4 0 0 0 0,-11 7 0 0 0,-28 1 0 0 0,43-13-8 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,0 0 1 0 0,2-1-1 0 0,-3-1 8 0 0,-27-47-411 0 0,33 54 334 0 0,3 1 10 0 0,0 0 3 0 0,0 0 0 0 0,13 5-105 0 0,-8-1 109 0 0,2 0 0 0 0,-1-1 0 0 0,-1 2 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1 2 60 0 0,18 20-246 0 0,43 55 1336 0 0,-40-51-896 0 0,1-3 0 0 0,1 1 1 0 0,2-2-1 0 0,9 6-194 0 0,-17-15-3 0 0,77 44-2666 0 0,-82-55 1330 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="85949.811">4368 14718 920 0 0,'0'0'327'0'0,"0"0"1035"0"0,0 9 2340 0 0,-1-6-656 0 0,-1 22 2742 0 0,7-12-4840 0 0,-3-11-526 0 0,-2-2-26 0 0,0 0 12 0 0,0 0 68 0 0,0 0 32 0 0,1 1 4 0 0,47 6 1536 0 0,-7-3-1138 0 0,20-61-236 0 0,30-33 437 0 0,-51 21-618 0 0,-17 6-757 0 0,-23 61 329 0 0,1 0-31 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 1-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1-34 0 0,-5 0 41 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 1 0 0 0,2 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,-2 0-40 0 0,-23 13 98 0 0,24-13-115 0 0,-1-1 0 0 0,0 2 0 0 0,1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-2 0 0 0,-2 5 17 0 0,-18 40 618 0 0,15 23-194 0 0,28 32-1082 0 0,-15-97 704 0 0,1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,2 1 1 0 0,1-1 0 0 0,-2 0 0 0 0,2-2-1 0 0,-1 2 1 0 0,1-2 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 1 1 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0-2 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1-2 1 0 0,3 1-47 0 0,41-5-792 0 0,-52 4 622 0 0,2 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,1-1-1 0 0,-2 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-2 170 0 0,14-9-5654 0 0,-3 7-1513 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="87029.81">5243 14371 1376 0 0,'0'0'65'0'0,"0"0"287"0"0,0 0 1184 0 0,0 0 522 0 0,0 0 100 0 0,0 0-171 0 0,0-15 1609 0 0,18-83 4054 0 0,-10 70-6749 0 0,-8 25-797 0 0,0-3-41 0 0,0 5-160 0 0,0 1-19 0 0,0 0 92 0 0,0 0 344 0 0,0 0 154 0 0,0 0 34 0 0,0 0-97 0 0,0 0-403 0 0,0 0-59 0 0,0 0 127 0 0,0 0 15 0 0,0 0 21 0 0,0 0 128 0 0,0 1 59 0 0,-8 68 675 0 0,-15 51-478 0 0,10-30-496 0 0,1 78 642 0 0,11 77-1033 0 0,-2-167 1100 0 0,-5-19-1141 0 0,8-57 208 0 0,-7 0-1960 0 0,6-1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="87299.81">5225 14482 12696 0 0,'11'-13'1376'0'0,"41"7"1778"0"0,13-4 1363 0 0,2 1-3125 0 0,4 22-1540 0 0,-47-6-2470 0 0,-18-2-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="204899.81">6380 14813 8288 0 0,'14'-32'1072'0'0,"28"-2"4316"0"0,-38 33-5186 0 0,2 0 1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,-1 2 1 0 0,2-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-2 1 0 0 0,1 3-203 0 0,4 3 280 0 0,-2 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,-1 2 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 7-281 0 0,-1-10 347 0 0,2-5-303 0 0,-1-1 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1-44 0 0,1-1 8 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-2 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2-1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-2-2-8 0 0,-4-3-53 0 0,1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,1 2 0 0 0,0-2 0 0 0,1-1 0 0 0,-3-4 53 0 0,5 10-246 0 0,-1-3 1 0 0,2 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1 1-1 0 0,-1-2 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-2 245 0 0,11-25-3579 0 0,-5 17-2927 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="203719.811">5759 14589 3224 0 0,'0'-2'240'0'0,"0"-1"25"0"0,0 2 855 0 0,0 1 359 0 0,0 0 66 0 0,0 0-81 0 0,0 0-397 0 0,0 0-178 0 0,0 0-32 0 0,0 0-13 0 0,0 0-24 0 0,0 0-10 0 0,0 0-2 0 0,0 0-18 0 0,0 0-74 0 0,5 29 1869 0 0,-13 143 1427 0 0,-5 3-2668 0 0,7-86-1106 0 0,6-88-198 0 0,1 18-364 0 0,-1-19 191 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 134 0 0,3-13-2091 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="204089.811">5775 14721 8288 0 0,'3'9'2948'0'0,"5"-25"1960"0"0,-3 7-5020 0 0,32-38 3418 0 0,18-5-299 0 0,-52 50-2908 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-99 0 0,22 30 274 0 0,20 32 16 0 0,-2-8-146 0 0,-12-20 0 0 0,-27-24-597 0 0,-3-10-3304 0 0,-2-2 2223 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35574.03">19737 6422 11888 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 14 0 0,1 10 69 0 0,-2 72 4760 0 0,-6-15-2346 0 0,7-29-2146 0 0,-1-34-594 0 0,-4 28-145 0 0,3-22-10 0 0,1-8-188 0 0,1-2-789 0 0,0 0-344 0 0,0 0-65 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35139.521">20015 6425 2304 0 0,'-3'1'3435'0'0,"8"5"13324"0"0,-2-4-18570 0 0,11 93 5563 0 0,1 27-2624 0 0,-6-50-1128 0 0,-7-63-133 0 0,-1-8-563 0 0,-1-1-257 0 0,0 0-922 0 0,0 0-3642 0 0,0 0-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-34747.75">20034 6549 1840 0 0,'0'0'83'0'0,"0"0"373"0"0,0 0 1526 0 0,0 0 670 0 0,0 0 131 0 0,3-1 950 0 0,9-6-2192 0 0,8-23 2196 0 0,-3 12-2845 0 0,-15 13-638 0 0,2 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,5-2-254 0 0,22 15 16 0 0,-26-7-15 0 0,48 49 773 0 0,-49-45-785 0 0,-4-7-105 0 0,14 4-2683 0 0,-15-5 751 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44644.387">19044 6244 3224 0 0,'-1'0'2310'0'0,"-1"1"10093"0"0,1 0-11285 0 0,1 2-3278 0 0,-15 164 7048 0 0,-11 32-3120 0 0,21-142-1645 0 0,7 47-583 0 0,1-97 325 0 0,-3-7-3458 0 0,0 0 1850 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44417.264">18973 6317 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,2 0-220 0 0,59 3 3130 0 0,56 23-834 0 0,-58-19-4427 0 0,-57-7-69 0 0,5 0-4147 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36024.581">19318 6651 2304 0 0,'0'0'348'0'0,"0"0"620"0"0,-9-5 2737 0 0,4-52-382 0 0,5 56-2754 0 0,-8-16 2487 0 0,2-41 2906 0 0,7 52-5754 0 0,0 1-1 0 0,2 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,2-1-207 0 0,-4 3-36 0 0,2-1 14 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,2 1 0 0 0,-2 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,3 0 23 0 0,-3 0 21 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-2 2 0 0 0,2-1 1 0 0,-1 0-1 0 0,-1 1 0 0 0,2 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,2 1-1 0 0,-2 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2 1 0 0 0,1-2 1 0 0,-1 1-1 0 0,-1 1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 0-21 0 0,0 4 5 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 4-5 0 0,2-3 151 0 0,-1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0-1 1 0 0,1 2-1 0 0,-2-1 1 0 0,0 0-1 0 0,0-2 1 0 0,-1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,-3 3-151 0 0,6-8 28 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1-27 0 0,-4-2-27 0 0,0-2-1 0 0,2 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,1-1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0-1 27 0 0,-4-53-3584 0 0,10 56 2142 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33796.383">20397 6645 456 0 0,'0'0'2349'0'0,"0"0"293"0"0,0 0 128 0 0,0 0-221 0 0,0 0-1013 0 0,0 0-448 0 0,0 0-89 0 0,0 0-30 0 0,5 7 1768 0 0,-2-4-2425 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,1 0-312 0 0,58-6 2120 0 0,4-20-1296 0 0,-5-16-672 0 0,-24-1 656 0 0,-16-24-516 0 0,-38 13-160 0 0,14 51-153 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 2-1 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,-3 2 22 0 0,-3 4 44 0 0,1 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1 0 0 0,-5 8-44 0 0,0-2 32 0 0,1 3-32 0 0,0 1 0 0 0,1-2 0 0 0,2 1 0 0 0,-1 1 0 0 0,3 0 0 0 0,-2 7 0 0 0,4-20 8 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0-1-1 0 0,2 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,4 7-8 0 0,11 4 88 0 0,44-10-2149 0 0,-22-14-6089 0 0,-24 3 1076 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33464.079">20897 6642 13824 0 0,'0'0'314'0'0,"-8"7"872"0"0,2 10-891 0 0,5-11 1764 0 0,-1-4 3765 0 0,8-3-5807 0 0,9-6-1723 0 0,-7 1-236 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-28557.543">19783 6192 4144 0 0,'0'0'319'0'0,"0"0"295"0"0,0 0 2022 0 0,0 0 904 0 0,0 0 185 0 0,0 0-408 0 0,0 0-1846 0 0,0 0-815 0 0,0 0-161 0 0,0 0-25 0 0,0 0 16 0 0,0 0 8 0 0,0 0 2 0 0,0 0-64 0 0,0 0-1313 0 0,0 0-4508 0 0,0 0-1916 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19052.719">21172 6390 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 6 160 0 0,3-4 8708 0 0,21 85-4943 0 0,-17 5-3675 0 0,-14-10-98 0 0,10-75-623 0 0,0-6-63 0 0,0-1-165 0 0,0 0-726 0 0,0 0-316 0 0,0 0-65 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-9426.743">21459 6277 920 0 0,'1'-1'67'0'0,"0"-4"143"0"0,0 5 814 0 0,-1 0 355 0 0,0 0 70 0 0,0 0 5373 0 0,0 4-3378 0 0,0 17-2234 0 0,12 160 4151 0 0,-9-31-3309 0 0,1-102-1683 0 0,-1-30-1984 0 0,-1-1-3835 0 0,-2-17 3608 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-8994.302">21459 6439 3224 0 0,'0'6'527'0'0,"10"-30"8375"0"0,8-1-6343 0 0,-16 22-2627 0 0,0-1 178 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-2 1 0 0 0,1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 0-110 0 0,21 31 453 0 0,0 10 891 0 0,-19-24-1051 0 0,1 55 781 0 0,8 8 131 0 0,-5-37-1044 0 0,9-13-3885 0 0,-19-29 1631 0 0,-1-2-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7909.834">22089 6376 2760 0 0,'0'0'395'0'0,"0"0"617"0"0,0 0 274 0 0,0 0 53 0 0,0 0-86 0 0,0 0-380 0 0,0 0-163 0 0,0 0-36 0 0,0 0-28 0 0,0 0-85 0 0,6 0 260 0 0,-5-1 2703 0 0,-1 0-3426 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-98 0 0,-11 0 483 0 0,-31 6 677 0 0,-1 20-16 0 0,42-24-1069 0 0,-2 1-1 0 0,2-2 0 0 0,1 2 0 0 0,-2 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,2 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,3 4-74 0 0,28 82 784 0 0,-18-63-634 0 0,-12-21-112 0 0,2-1 0 0 0,-2 0 1 0 0,1 1-1 0 0,1-2 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,1-1-38 0 0,-3-1-114 0 0,0 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,1-1-1 0 0,-2 1 1 0 0,2-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,3-1 114 0 0,4-1-2547 0 0,1-3-5195 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7043.897">22348 6701 7112 0 0,'16'0'324'0'0,"-12"0"-4"0"0,-4 0-94 0 0,0 0 380 0 0,0 0 186 0 0,0 0 37 0 0,0 0 35 0 0,0 0 107 0 0,0 0 42 0 0,0 0 10 0 0,0 0-26 0 0,0 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-58 0 0,0 0-240 0 0,0 0-102 0 0,0 0-17 0 0,0 0-25 0 0,0 0-82 0 0,0 0-40 0 0,0 0-5 0 0,0 0-26 0 0,0 0-108 0 0,0 0-42 0 0,1-18-240 0 0,16 0 132 0 0,-17 17-8 0 0,0 1 88 0 0,0 0 35 0 0,0 0-18 0 0,-1 1-1 0 0,-1 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,2-1 0 0 0,-2 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0-67 0 0,1 1-279 0 0,-1-2-186 0 0,0 0-42 0 0,0 0-209 0 0,0 0-857 0 0,0 0-379 0 0,0 0-80 0 0,0 0-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2101.423">21179 6052 13304 0 0,'0'0'605'0'0,"0"0"-9"0"0,0-1-381 0 0,-2-3-42 0 0,1 2 600 0 0,1 2 260 0 0,0 0 45 0 0,0 0-26 0 0,0 0-144 0 0,0 0-63 0 0,-4 20 1994 0 0,14-13-5523 0 0,-8-7-4821 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122096.968">4045 774 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-120 0 0,0 0 193 0 0,-4-7 582 0 0,-49-23 3117 0 0,25 17-1623 0 0,-50-15-841 0 0,66 25-1311 0 0,2 1-1 0 0,-1 1 0 0 0,-2-1 1 0 0,2 2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 2-1 0 0,1 1 0 0 0,-11 4-284 0 0,17-7 41 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-2 0 0 0 0,2 1-1 0 0,0-1 1 0 0,1-1-1 0 0,-1 2 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 2-40 0 0,6 8 100 0 0,0 0 0 0 0,2-1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,3 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0-100 0 0,-7-6 32 0 0,72 80-590 0 0,-64-67 602 0 0,-1 1 1 0 0,-2 0-1 0 0,1 1 1 0 0,-2 0 0 0 0,0-1-1 0 0,-1 3 1 0 0,-2 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-2 2 1 0 0,-1-2 0 0 0,0 2-1 0 0,-2-2 1 0 0,0 2-1 0 0,-1 0 1 0 0,-3 19-45 0 0,0-26 91 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-2-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,0-2 1 0 0,-1 0-1 0 0,-2 3-91 0 0,7-9 67 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-2 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 1 0 0,-2 1-1 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,-7-2-68 0 0,8 0 4 0 0,-2 0 0 0 0,0 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1-5-4 0 0,-1 1-603 0 0,0 0 1 0 0,1 0-1 0 0,1-2 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-3 603 0 0,-4-12-1535 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122485.17">3932 513 13680 0 0,'0'0'306'0'0,"-5"7"421"0"0,-2 6-534 0 0,-1 0-1 0 0,2 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,2 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-2 11-193 0 0,1-4 459 0 0,-11 62 963 0 0,4 2 0 0 0,4-1 0 0 0,4-1 0 0 0,5 57-1422 0 0,-11 64 1773 0 0,-7-14-700 0 0,0 106-1515 0 0,19-237-1557 0 0,-2-33 952 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="142634.009">4405 1516 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 0 0 0 0,0 0 200 0 0,0 0 24 0 0,-3-7 8 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="185244.55">4559 1861 1376 0 0,'0'0'65'0'0,"0"0"321"0"0,0 0 1322 0 0,0 0 578 0 0,0 0 119 0 0,-2 2 764 0 0,-7 7-2143 0 0,8-9-849 0 0,0 1 1 0 0,0 0-1 0 0,-2 0 1 0 0,2-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-2 0 1 0 0,2 0-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-2-1 0 0 0,2 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1-177 0 0,-12-12 1364 0 0,0-23 743 0 0,15 2-644 0 0,-12-25-661 0 0,12 38-733 0 0,0 1-1 0 0,2 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-1 1 0 0 0,2-1-1 0 0,1 1 1 0 0,0 0-1 0 0,2 1 1 0 0,0 1-1 0 0,2-1 1 0 0,7-10-69 0 0,-7 9-213 0 0,26-24 417 0 0,-35 42-216 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,0 0 1 0 0,0 0 11 0 0,28 11-403 0 0,-14-10 372 0 0,0 10 529 0 0,-2-2 172 0 0,-11-7-605 0 0,2 1-1 0 0,-2-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-2 1 0 0 0,0 2-64 0 0,12 25-60 0 0,2 48 132 0 0,-8-44-67 0 0,-6-32 15 0 0,1 1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,-1 5-20 0 0,-6 15 568 0 0,8-26-650 0 0,-3 7-326 0 0,3-8 412 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-4 0 0,-2-25 743 0 0,17-39-633 0 0,-3 28-110 0 0,15-30 0 0 0,23-16-320 0 0,-17 43-430 0 0,0 9 1668 0 0,12 3-918 0 0,-40 25-7 0 0,-1 1-32 0 0,-1 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1 0 38 0 0,-1-2 222 0 0,15 17 286 0 0,0 11-904 0 0,-2 22 920 0 0,-3 11-181 0 0,-7-24 197 0 0,-4 35-687 0 0,0-38 334 0 0,26 36-102 0 0,7-11-74 0 0,-31-56 31 0 0,2 1-20 0 0,29-6 135 0 0,-13-11 0 0 0,6-10-434 0 0,4-17 434 0 0,-20 23-314 0 0,3-2 685 0 0,5-10-776 0 0,-17 28 365 0 0,-1 1-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0 39 0 0,0 0 168 0 0,4-13-278 0 0,-3 10-5968 0 0,0 2-1741 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="186134.947">5706 1624 11288 0 0,'0'0'514'0'0,"-11"-9"196"0"0,9 7-539 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 2 0 0 0,0-2 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-171 0 0,41-45 2046 0 0,-31 39-1874 0 0,-7 6-154 0 0,-2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2 0-18 0 0,-2 0 60 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 1-60 0 0,-1 2 134 0 0,11 71 1428 0 0,-15-53-1106 0 0,-14 39 934 0 0,15-60-1313 0 0,0 1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,2-1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 0 0 0 0,-5 2-77 0 0,-28-4 728 0 0,21-4-305 0 0,14 4-401 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,-2 1 1 0 0,2-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 1 1 0 0,0-2-1 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-2-22 0 0,-1-2-121 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 121 0 0,25-44-8730 0 0,-13 28 1471 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="195187.748">6259 1353 456 0 0,'-7'20'336'0'0,"0"-2"10502"0"0,6-14-10470 0 0,1 53 5149 0 0,0 20-1998 0 0,12 52-1146 0 0,7-58-2293 0 0,15-24 752 0 0,-4-9-288 0 0,-22-31-468 0 0,2-6 16 0 0,33-4 116 0 0,9-22 32 0 0,-4-32-153 0 0,-16 13-38 0 0,-3 6-49 0 0,-6 13 0 0 0,15-37 64 0 0,-12 27-74 0 0,-16 26-44 0 0,3-21 54 0 0,-2 19 28 0 0,-4-7-2 0 0,3-4-69 0 0,-9 21 96 0 0,-3 19-9 0 0,-11 57-144 0 0,9-6 100 0 0,1-40 0 0 0,3 20 0 0 0,-9 41 254 0 0,-11 0-28 0 0,-11 29 293 0 0,6-56 286 0 0,17-40-797 0 0,-1 3 0 0 0,-1-3 1 0 0,-2 1-1 0 0,0-2 0 0 0,-2 1 0 0 0,-7 8-8 0 0,10-16 52 0 0,-1-1-1 0 0,0-1 1 0 0,0 1-1 0 0,-2-1 1 0 0,1-2-1 0 0,-2 0 0 0 0,-4 3-51 0 0,12-8 15 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-2-1 0 0,0 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-2-14 0 0,8 1-35 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0-1 0 0,-2 1 1 0 0,2 0 0 0 0,0-3 34 0 0,-1-1 20 0 0,11-78-2121 0 0,-10 52-659 0 0,0 18 1197 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="196354.103">6930 1723 1840 0 0,'1'-1'138'0'0,"-1"0"0"0"0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,2 0-1 0 0,-2 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,2-1-1 0 0,-2 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1-138 0 0,15 0 3296 0 0,41-8 1940 0 0,-37 1-4448 0 0,63-27 1921 0 0,-16-18-1408 0 0,-57 39-1068 0 0,-8 9-211 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0-1-21 0 0,-1 1 9 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 2 0 0 0,2-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-6-1-9 0 0,-3-4-199 0 0,11 6 228 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-2 1 0 0 0,2 0 0 0 0,0 1-1 0 0,-4-1-28 0 0,-15 4 307 0 0,18-4-243 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-1 4-64 0 0,-1 2 118 0 0,-3 3 3 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,2 0 0 0 0,0 1 0 0 0,0 1 1 0 0,1-2-1 0 0,0 2 0 0 0,2 1 0 0 0,-1-2 1 0 0,2 0-1 0 0,0 8-121 0 0,1-10 43 0 0,1-1-1 0 0,0-1 1 0 0,1 0 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1-1 0 0,0-2 1 0 0,1 1 0 0 0,-1-1 0 0 0,4 5-43 0 0,2 0 29 0 0,30 20 88 0 0,-31-28-139 0 0,1-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 0-1 0 0,0 0 0 0 0,2-1 23 0 0,58-5-3801 0 0,-48 6 2362 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="198120.726">7556 1386 4832 0 0,'2'63'3666'0'0,"1"-42"-222"0"0,-1-20-2786 0 0,-4 33 2622 0 0,4 71 551 0 0,-2-42-3103 0 0,0 44 110 0 0,0-37-4281 0 0,0-69-1079 0 0,0-1-1230 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="198513.93">7545 1647 3680 0 0,'0'0'284'0'0,"0"-1"-187"0"0,0-2 155 0 0,2-11 5681 0 0,8-11-2141 0 0,-4 12-2532 0 0,-5 9-1000 0 0,1-1-1 0 0,-1 2 0 0 0,1-2 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 2 0 0 0,0-1 1 0 0,1 0-260 0 0,31-19 850 0 0,-33 21-780 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1-70 0 0,33 30 293 0 0,34 46 1327 0 0,-72-78-1617 0 0,3 3 19 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1-1 0 0,1-2 1 0 0,-1 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 2-22 0 0,12 54 581 0 0,-21-33-1430 0 0,7-20-1922 0 0,-3 0 1115 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="209019.972">8181 1398 6880 0 0,'0'0'314'0'0,"0"0"-6"0"0,0 0-77 0 0,0 0 409 0 0,0 0 199 0 0,0 0 38 0 0,0 0-32 0 0,0 0-173 0 0,0 0-80 0 0,0 0-14 0 0,0 0-2 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 6 0 0,0 0 30 0 0,7 14 2401 0 0,12 30-517 0 0,-18 34-102 0 0,-9-14-1028 0 0,4-51-1323 0 0,2-1-1 0 0,0 0 1 0 0,1 2-1 0 0,0-1 1 0 0,1 1-1 0 0,0-2 1 0 0,2 6-35 0 0,1 55 86 0 0,1-17-106 0 0,-3-51 540 0 0,-2-5-4113 0 0,1 2-6903 0 0,0-2 5190 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="209481.323">8199 1594 1840 0 0,'0'0'403'0'0,"0"0"1018"0"0,0-5 1680 0 0,1 3 1760 0 0,30-57 991 0 0,-25 52-5592 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-2 0 0 0 0,3 1 1 0 0,2-2-260 0 0,-7 5 92 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 1-1 0 0,2 1-92 0 0,32 50 1184 0 0,-19-12-1184 0 0,-6 49 0 0 0,-7-45 848 0 0,-5-47-637 0 0,0 0-324 0 0,0 0-141 0 0,0 0-30 0 0,0 0-132 0 0,-6 8-4129 0 0,3-6-2469 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="210782.678">8749 1637 6304 0 0,'0'0'289'0'0,"0"0"-8"0"0,0 0-50 0 0,0 0 462 0 0,0 0 218 0 0,0 0 45 0 0,0 0-8 0 0,0 0-77 0 0,2 1-37 0 0,9 4 1041 0 0,-9-4-1679 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,2-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,2-1-197 0 0,68-46 1877 0 0,-8-9-1229 0 0,-54 44-648 0 0,-11 9 43 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-4 1-43 0 0,2 0 15 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 1 0 0 0,2-1 0 0 0,-2 2-15 0 0,0 2 78 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,2 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,0 1-1 0 0,-1 6-78 0 0,1-6 84 0 0,0 3-20 0 0,1 1 0 0 0,1-2 1 0 0,0 2-1 0 0,0 0 0 0 0,1-1 0 0 0,1 0 0 0 0,1 5-64 0 0,35 98 743 0 0,-36-112-717 0 0,0 0 0 0 0,0-2 0 0 0,1 2 0 0 0,-1-1 1 0 0,0 1-1 0 0,2-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,4-1-26 0 0,2-3-217 0 0,0-1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,5-9 217 0 0,26-18-3383 0 0,-26 23 1685 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212336.791">9254 1827 1376 0 0,'0'0'65'0'0,"0"0"286"0"0,0 0 1176 0 0,0 0 510 0 0,0 0 105 0 0,0 0-140 0 0,0 0-688 0 0,0 0-303 0 0,0 0-62 0 0,0 0-31 0 0,0 0-86 0 0,12-8 1503 0 0,26-84 2243 0 0,-1 5-2552 0 0,41-58-1672 0 0,36-14 444 0 0,-53 70 85 0 0,-48 67-1159 0 0,-12 21 177 0 0,-1 1 151 0 0,0 0 68 0 0,0 0 10 0 0,7 10-109 0 0,4 72 56 0 0,-14-3-233 0 0,3 117 500 0 0,4 116-424 0 0,3-244-61 0 0,-7-67-590 0 0,0-1-241 0 0,-1-1-1406 0 0,-5-5-5471 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212940.975">9330 1690 6448 0 0,'0'0'498'0'0,"4"-4"32"0"0,1 1 484 0 0,-4 2-660 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2-1-354 0 0,61-13 3164 0 0,41 29-2595 0 0,-88-14-475 0 0,-4 0-1562 0 0,-3-1-3055 0 0,-1-1-2147 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="213609.296">9944 1568 920 0 0,'0'0'295'0'0,"0"0"901"0"0,-4-15 3639 0 0,2 13-5213 0 0,-4-1 8750 0 0,4 3-7138 0 0,1 0-721 0 0,-7 4 1698 0 0,-14 25-994 0 0,1 21-137 0 0,12 6 52 0 0,23 22 127 0 0,-12-74-1227 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,2 1-32 0 0,-3-1 21 0 0,-1-1-1 0 0,2 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,0-2-20 0 0,58-48-20 0 0,-13-28-456 0 0,-38 41-464 0 0,-25 7-1392 0 0,13 33-2925 0 0,1 0-1661 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="214337.783">10430 1257 2304 0 0,'0'1'167'0'0,"4"23"1727"0"0,-10-6 5773 0 0,-3 113 1948 0 0,6-15-6975 0 0,6-36-2192 0 0,2 73-376 0 0,1-74-72 0 0,6-1-3116 0 0,-12-77 1546 0 0,0-1-280 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="214624.938">10415 1482 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,1-2-344 0 0,28-19 826 0 0,8 15 3479 0 0,3-2-2907 0 0,12 2-1414 0 0,-26 9-2102 0 0,-15 0-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213551.059">10893 1660 10136 0 0,'9'12'230'0'0,"-7"-10"30"0"0,-2-2 19 0 0,0 0 104 0 0,-3 18 7879 0 0,4-17-7647 0 0,-1-1-21 0 0,1 1-38 0 0,10-1-436 0 0,-1 1-1 0 0,1-2 0 0 0,0 1 1 0 0,-1-2-1 0 0,0 1 0 0 0,1 0 1 0 0,0-2-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-2 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-2 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0-1 0 0 0,-2 1 1 0 0,1-2-1 0 0,-1 1 0 0 0,1-1 1 0 0,-3 0-1 0 0,4-5-119 0 0,8-47 69 0 0,-16 58-69 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-4 0 0 0 0,2 1 61 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1-1-61 0 0,-55 56-543 0 0,52-51 613 0 0,0 0 0 0 0,0-1 0 0 0,1 2-1 0 0,-1 0 1 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,-1 7-70 0 0,1-9 0 0 0,1 2 0 0 0,1-2 0 0 0,0 2 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,3-1 0 0 0,-2 0 0 0 0,1 1 0 0 0,0-2 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,7 5 0 0 0,-9-8-56 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,2-1 56 0 0,8-4-1098 0 0,2-2-56 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213242.538">11481 1492 4608 0 0,'-19'14'3105'0'0,"0"1"6005"0"0,11-1-7943 0 0,-4 9 1032 0 0,10 16-1221 0 0,-4 45 1209 0 0,5-77-2095 0 0,1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,2-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 0 0 0,2-2 1 0 0,-1 1-1 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 1 0 0,2-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,1-2 0 0 0,2 3-92 0 0,2-3 0 0 0,-7-5 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,19-28 0 0 0,-3-1 0 0 0,0-2 0 0 0,-2 1 0 0 0,-1-3 0 0 0,-8 12 0 0 0,-16 8-1384 0 0,7 17 600 0 0,2 1-1144 0 0,0 0-496 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212663.88">12024 1435 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0 88 0 0,0 0 1067 0 0,0 0 483 0 0,0 0 98 0 0,0 0-138 0 0,0 0-670 0 0,0 0-295 0 0,0 0-60 0 0,0 0-101 0 0,0 0-377 0 0,0 0-167 0 0,0 0-31 0 0,-3 9 1448 0 0,-1 88 1023 0 0,11-7-2584 0 0,-3-31 1296 0 0,3 90-752 0 0,-3-138-818 0 0,-3-10-854 0 0,-1-1-382 0 0,0 0-76 0 0,0 0-20 0 0,0 0-2 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212449.687">12046 1643 456 0 0,'-5'-9'365'0'0,"4"8"1529"0"0,1-5 6369 0 0,3-6-4715 0 0,18-27-181 0 0,-11 20-2471 0 0,-4 10-747 0 0,-5 7-63 0 0,1-1-1 0 0,0 0 0 0 0,-1 2 0 0 0,1-2 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0-85 0 0,-3 1 239 0 0,10 5 186 0 0,-6-3-373 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,2 4-52 0 0,6 5 0 0 0,-10-12-55 0 0,-1-1-16 0 0,6 5-460 0 0,-5-3-2608 0 0,-1-2-3526 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-206308.339">2988 2565 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,0 2-294 0 0,-5 8 6808 0 0,-1-7-3282 0 0,-9-19-2050 0 0,15 15-1469 0 0,-11-96 2153 0 0,11-133-1048 0 0,-4-1-752 0 0,-8-53-24 0 0,-2 48-128 0 0,2-94-168 0 0,8 158 559 0 0,-10-50-726 0 0,10 92-532 0 0,-3 19 446 0 0,3 38-11 0 0,-1 17 64 0 0,2 2 0 0 0,7-106 128 0 0,4 124-128 0 0,10 14 0 0 0,-10 19-4 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,8 3 4 0 0,33 10 0 0 0,-24-7 79 0 0,1 0 0 0 0,-1-2-1 0 0,1-1 1 0 0,0-1-1 0 0,1-1-78 0 0,35-2-104 0 0,1-3 0 0 0,-1-3-1 0 0,1-3 1 0 0,58-14 104 0 0,392-67 0 0 0,-394 80 0 0 0,0 4 0 0 0,1 6 0 0 0,36 8 0 0 0,19-2 0 0 0,4-5 99 0 0,1-7-1 0 0,84-15-98 0 0,-112 7 64 0 0,106 6-64 0 0,-165 11 41 0 0,0 4-1 0 0,38 10-40 0 0,8 1 143 0 0,76 4 11 0 0,3-10-1 0 0,165-12-153 0 0,37-21 125 0 0,-298 15-98 0 0,158 4 106 0 0,184 31 123 0 0,-73-1-170 0 0,356-32 188 0 0,-323 22 29 0 0,-187-5-190 0 0,-63-3-38 0 0,160-12-75 0 0,34-13 0 0 0,-173 6 128 0 0,41 10-128 0 0,331 41 0 0 0,-477-43 0 0 0,36-16 64 0 0,62-21-160 0 0,-135 34 85 0 0,22-1-42 0 0,26-26 429 0 0,-66 28-376 0 0,-17 8 0 0 0,-3 4 0 0 0,11 15 0 0 0,-13 3 0 0 0,20 61 0 0 0,-13 3-189 0 0,-6 2-1 0 0,6 91 190 0 0,-10 11 307 0 0,6 182-618 0 0,-12 110 606 0 0,2-144-200 0 0,5-3-14 0 0,-6-148-6 0 0,-5-175-59 0 0,0-1 1 0 0,-2 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-1 1-1 0 0,0-2 1 0 0,-4 11-17 0 0,6-23 9 0 0,1 0 0 0 0,-2 1 0 0 0,1-2 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-9 0 0,-48-3 22 0 0,1-3 0 0 0,0-1-1 0 0,2-4 1 0 0,-12-3-22 0 0,-92-17 52 0 0,-116 9-87 0 0,28 29 35 0 0,-364 9 0 0 0,-20-17 0 0 0,310 18 70 0 0,-15 15-70 0 0,-69 7 47 0 0,301-31-39 0 0,-409 17-5 0 0,-361-20-3 0 0,-353 31 240 0 0,658-43-256 0 0,118-15-48 0 0,24-5 64 0 0,-82 5 11 0 0,214 10 114 0 0,-76-25-85 0 0,-45-29-40 0 0,261 47 0 0 0,-15 5 0 0 0,-2 28 0 0 0,-40-12 0 0 0,87-8-100 0 0,111 4 7 0 0,7 3-64 0 0,1-1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1 156 0 0,1-9-10012 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202306.829">7690 2872 3224 0 0,'0'2'240'0'0,"19"54"4562"0"0,-8-8 530 0 0,-4-24-2824 0 0,-2 9-572 0 0,6 45 269 0 0,5 25-781 0 0,-2 48 0 0 0,6 108 552 0 0,-2-121-1272 0 0,9 149 568 0 0,-18-37-696 0 0,1-120-389 0 0,-2 41 722 0 0,-8-53-581 0 0,-4-1-93 0 0,8-7-91 0 0,-8 41-19 0 0,4-97-61 0 0,-4 83 0 0 0,-1-105-64 0 0,5-26-67 0 0,0-5-281 0 0,0-1-129 0 0,0 0-31 0 0,0 0-72 0 0,-4-17-3152 0 0,1 3-2356 0 0,-1-4-1623 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201855.109">7349 4585 12264 0 0,'0'0'273'0'0,"-5"13"786"0"0,5-3-595 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 2 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-2 0 0 0,2 7-464 0 0,-5-10 43 0 0,52 109 3185 0 0,30 114 95 0 0,-65-163-2734 0 0,2-1 0 0 0,28 55-589 0 0,19 11 416 0 0,-3-51-72 0 0,-52-71-248 0 0,-1 2-1 0 0,0-1 0 0 0,2 0 1 0 0,-1-1-1 0 0,1-1 1 0 0,12 6-96 0 0,-20-11 39 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-1-39 0 0,64-62 528 0 0,18-72-224 0 0,73-275-391 0 0,-145 378-257 0 0,24-55-4278 0 0,-33 80 2515 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186308.475">14143 1218 1840 0 0,'0'0'83'0'0,"0"0"-6"0"0,0 5 363 0 0,0-4 1761 0 0,0-1 766 0 0,1 18 5666 0 0,1 0-5371 0 0,2 17-970 0 0,-4-24-1727 0 0,-12 103 2961 0 0,-25 77-2557 0 0,41-152-1425 0 0,-4-39 48 0 0,0 0-940 0 0,0 0-410 0 0,1 0-88 0 0,4-5-10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-185850.611">14511 1218 13040 0 0,'0'0'597'0'0,"0"0"-9"0"0,0 0-220 0 0,0 0 481 0 0,0 0 250 0 0,0-5 715 0 0,-1 4 3304 0 0,-5 3-5002 0 0,0 1 0 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 0 0 0,2 1 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,2-2-1 0 0,-2 2 1 0 0,1-1-1 0 0,1 1 0 0 0,-2 3-116 0 0,1 2 121 0 0,-1-1-1 0 0,2 1 1 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 1 1 0 0,0-2-1 0 0,1 2 1 0 0,0-1-1 0 0,1 0 1 0 0,0 0-1 0 0,2 1 1 0 0,-1-1-1 0 0,1-1 1 0 0,0 0-1 0 0,4 5-120 0 0,48 107 0 0 0,-49-92 0 0 0,-8-23 0 0 0,0-5 60 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 0 0 0 0,2-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,-2-2-60 0 0,-4-4-110 0 0,8 7-9 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 119 0 0,1-6-1959 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-187118.879">13464 897 13184 0 0,'0'0'604'0'0,"0"0"-14"0"0,0 0-252 0 0,0 0 326 0 0,0 0 185 0 0,0 0 41 0 0,2 0-12 0 0,-1-1-747 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2 0-131 0 0,6 17 493 0 0,-1-1 0 0 0,-1 0 0 0 0,1 2-1 0 0,-3-1 1 0 0,1 18-493 0 0,-3-32 76 0 0,-2 88 1295 0 0,1 19-942 0 0,-6-16-247 0 0,-2 114-43 0 0,13-167-247 0 0,-3-42-448 0 0,-1-1-176 0 0,0 0-32 0 0,3-21-3836 0 0,-2 2 2544 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186774.862">13540 1278 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-79 0 0,0 0-421 0 0,0 0-180 0 0,0 0-37 0 0,0-13 1908 0 0,1 8-2997 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0-346 0 0,14-9 712 0 0,-16 10-708 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,3 1-4 0 0,-2-1 90 0 0,2 2-1 0 0,-2-1 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,2 1 0 0 0,-2-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1-2 0 0 0,-1 2 1 0 0,0 1-1 0 0,1 0-89 0 0,54 195 1931 0 0,-52-175-1912 0 0,0-1 1 0 0,-1 1-1 0 0,-2 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,-2 4-19 0 0,0 4-4294 0 0,2-33-4235 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184500.214">14926 1102 11976 0 0,'-4'2'1082'0'0,"-18"92"550"0"0,1 52 3297 0 0,15 50-1046 0 0,9-96-3866 0 0,5-72-17 0 0,-8-26-850 0 0,0 3 2050 0 0,0-2-4324 0 0,0 3-3781 0 0,0-6 913 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184054.319">14990 1145 3224 0 0,'0'0'143'0'0,"1"1"-3"0"0,4 4 390 0 0,13 9 9462 0 0,3 0-5178 0 0,-16-11-4675 0 0,-2-1-1 0 0,1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 0-138 0 0,34 3-1260 0 0,-22-7 497 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-183416.48">14861 1231 5960 0 0,'-3'-8'266'0'0,"3"7"1"0"0,0-21 1002 0 0,10-16 3955 0 0,13-7-2882 0 0,-12-3-311 0 0,-9 45-2036 0 0,-6-13-175 0 0,-1 12-433 0 0,5 4-2775 0 0,0 0 1855 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-182333.102">15261 1519 0 0 0,'0'0'2721'0'0,"0"0"-302"0"0,0 0 223 0 0,1-1-119 0 0,9-8-671 0 0,-9 7-1682 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,2-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,2 0 1 0 0,-2 1-1 0 0,0-1 0 0 0,0 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,0 1-1 0 0,0 0-170 0 0,6 2 296 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-2 1 0 0 0,1-2 0 0 0,0 2 0 0 0,-2-1 0 0 0,2 2 1 0 0,-2-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,3 8-296 0 0,8 42 792 0 0,-13-54-721 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-3 2-71 0 0,5-4 2 0 0,-1 1 15 0 0,-1 1 1 0 0,-2-1-1 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,-2-2-18 0 0,1 1 49 0 0,-2-1 1 0 0,0 0-1 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,-1-1-1 0 0,2 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-2-49 0 0,3 2-126 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,3-3 126 0 0,13-34-3998 0 0,-3 21-3873 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-175901.286">15724 1488 4144 0 0,'0'0'191'0'0,"0"0"375"0"0,-4-9 14804 0 0,9 56-13610 0 0,3 16 8 0 0,3 27 351 0 0,-10-75-1781 0 0,8 24-3577 0 0,-9-38 1789 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172641.548">16474 1641 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,1 1-72 0 0,16 38 5565 0 0,-11-27-3129 0 0,-1-10-2556 0 0,2-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 0 0 0 0,2 1 0 0 0,-1-2 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,-2 1 0 0 0,5-4-209 0 0,67-62 153 0 0,-54 34-213 0 0,-21 34 61 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 0 0 0,-1-1 2 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 1 1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 1-2 0 0,-17 7 0 0 0,17-7 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 4 0 0 0,-6 11 27 0 0,7-10 0 0 0,-1-1-1 0 0,0 0 1 0 0,2 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,0-2 0 0 0,-1 2-1 0 0,2-1 1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,1 2-27 0 0,0-6-27 0 0,-1 0-1 0 0,1 1 1 0 0,0 0 0 0 0,1-2-1 0 0,0 1 1 0 0,-1 1-1 0 0,3-2 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,2 0-1 0 0,4 5 28 0 0,16-3 0 0 0,22-16-1385 0 0,-32 1-166 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172385.72">16998 1665 11832 0 0,'-38'14'7253'0'0,"35"-12"-6259"0"0,3-1-12 0 0,0-1-29 0 0,0 0-122 0 0,0 0-482 0 0,0 0-205 0 0,0 0-44 0 0,0 0-7 0 0,0 0 17 0 0,0 0 8 0 0,0 0 2 0 0,0 0-237 0 0,0 0-996 0 0,0 0-434 0 0,1 0-86 0 0,4 0-21 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170574.714">17831 1086 2760 0 0,'0'0'589'0'0,"0"0"1434"0"0,0 0 626 0 0,0 0 126 0 0,0 0-214 0 0,0 7 88 0 0,0 167 4329 0 0,0 88-4387 0 0,-1-163-2591 0 0,-4 26 0 0 0,5-61 0 0 0,-3-3-134 0 0,3-60-570 0 0,0-1-263 0 0,0 0-916 0 0,0-1-3632 0 0,-3-5-1553 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170137.543">17792 1532 5064 0 0,'0'0'389'0'0,"3"-3"794"0"0,-1 2 3071 0 0,27-32 3094 0 0,8-2-4244 0 0,21-5-1223 0 0,-52 39-1852 0 0,-2 1 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2-2 0 0 0,1 2 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-2-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,-1 1-29 0 0,5 14 310 0 0,-1 3 0 0 0,-1-1 0 0 0,-1 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,-1 8-310 0 0,-8 89 1048 0 0,8-91-908 0 0,6 1-148 0 0,10-34-432 0 0,5-13-1437 0 0,1 1-5762 0 0,-9 7 145 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172102.041">17333 1321 9760 0 0,'4'-25'2366'0'0,"-4"24"-894"0"0,0 1 68 0 0,0 0-60 0 0,0 0-321 0 0,0 0-139 0 0,0 0-27 0 0,0 0-34 0 0,0 0-114 0 0,-3 6 736 0 0,-8 70 997 0 0,2 34-801 0 0,-7 75-1676 0 0,10-113-101 0 0,2 24 0 0 0,3-85 704 0 0,-1 0-2693 0 0,1 3-6478 0 0,1-14 756 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-171739.932">17367 1321 16064 0 0,'5'-13'1715'0'0,"-3"9"-1471"0"0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,4 0-244 0 0,-4 0 90 0 0,2 0 1 0 0,-2 0-1 0 0,2 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-2 0-1 0 0,1 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,2 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,-2 0-1 0 0,4 2-90 0 0,-3 7 116 0 0,0-1 0 0 0,1 0 0 0 0,-2 0-1 0 0,0 1 1 0 0,1 0 0 0 0,-3 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,-2-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-3-2 0 0 0,2 1 0 0 0,-2 0-1 0 0,0 0 1 0 0,-6 9-116 0 0,-44 65 1297 0 0,53-83-1274 0 0,1 1-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 0 1 0 0,2-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 0-22 0 0,-2-2-128 0 0,3 1 21 0 0,0 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,1-2 0 0 0,0 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,1 0 106 0 0,-1-9-1478 0 0,-3 1-66 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174133.091">16119 1371 4144 0 0,'0'0'319'0'0,"0"0"-7"0"0,0 0 751 0 0,0 0 355 0 0,0 0 71 0 0,0 0-42 0 0,0 0-234 0 0,0 0-101 0 0,0 0-21 0 0,0 18 3966 0 0,-10 4-3283 0 0,9-20-1264 0 0,1-2-29 0 0,0 2-8 0 0,-4 241 2166 0 0,-9-131-2099 0 0,7-59 33 0 0,-1 19-3333 0 0,8-73 56 0 0,2-7-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173508.196">16078 1601 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,1-1 491 0 0,29-51 6288 0 0,-28 49-6862 0 0,-1-1 1 0 0,1 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2 0 0 0 0,-2-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,2 1-157 0 0,-1 0 54 0 0,1-1 0 0 0,-2 2 0 0 0,0-2 0 0 0,1 2-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 0-53 0 0,0-5-149 0 0,4 18-2358 0 0,-4-9 487 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-169732.621">18411 1347 18287 0 0,'0'0'414'0'0,"0"0"56"0"0,0 1 32 0 0,0 81 1564 0 0,-12 57 154 0 0,1 9-612 0 0,4-20 14 0 0,-2-49-1333 0 0,9-78-974 0 0,0-1-274 0 0,0 0-53 0 0,0 0-215 0 0,0 0-858 0 0,0 0-379 0 0,1-2-80 0 0,3-12-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168923.508">18476 1460 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,3-7-322 0 0,4-4-3 0 0,-4 5 250 0 0,1 1-1 0 0,-1-1 1 0 0,2 2 0 0 0,-2-1 0 0 0,1 0 0 0 0,1 0-1 0 0,1 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,-2 1-1 0 0,2 0-460 0 0,-3 0 236 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 2-1 0 0,1-1 1 0 0,-1 0-236 0 0,2 1 105 0 0,-2 2 0 0 0,2-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2 5-105 0 0,13 81 177 0 0,-29 76 1151 0 0,-12-105-745 0 0,20-60-571 0 0,1 0 0 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-2 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-2-1 0 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-2 0 0 0,0 1 0 0 0,-1-1-12 0 0,-4-2-508 0 0,0 1 0 0 0,0-2 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 2 0 0 0,0-3 0 0 0,0 1-1 0 0,0-1 1 0 0,-5-7 508 0 0,0 0-1504 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-130876.917">3193 5992 6448 0 0,'25'-2'672'0'0,"-21"1"-608"0"0,0 3 3996 0 0,-1 5-3602 0 0,-3-3 96 0 0,1-3 14 0 0,-4 12 453 0 0,10 160 2956 0 0,-12 68-1512 0 0,9-94-1338 0 0,4-70-1094 0 0,-5-69-94 0 0,-3-6-264 0 0,5-16-6236 0 0,-2 2 317 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-124973.04">3214 6042 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 0-79 0 0,0 0 561 0 0,0 0 272 0 0,-3 6 1195 0 0,-4-3 2766 0 0,8-9-4160 0 0,9-13-1197 0 0,-8 12 345 0 0,3 1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 0 0 0 0,3 0 0 0 0,-2 1 0 0 0,1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,4 0-78 0 0,-7 2-15 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 15 0 0,23 112 716 0 0,-25-113-672 0 0,3 2 51 0 0,-2 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-3 0 0 0,0 3 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1-95 0 0,-38 25 236 0 0,34-28-233 0 0,-3 2 17 0 0,0-1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2-2 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,-9 0-20 0 0,-29-5-116 0 0,47 0 127 0 0,2 2 42 0 0,11 13-2 0 0,40 47-118 0 0,71 108 1347 0 0,-71-100-1908 0 0,-31-54-2350 0 0,-10-7-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123928.98">3716 6562 3224 0 0,'0'0'143'0'0,"0"0"315"0"0,0 0 1222 0 0,0 0 531 0 0,0 0 106 0 0,0 0-213 0 0,0 0-968 0 0,0 0-428 0 0,5 9 1069 0 0,1-7-1546 0 0,1 0-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 0-1 0 0,0 0 1 0 0,-2-1-1 0 0,2 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-2-1 1 0 0,2-1-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,-1-1 1 0 0,3-2-231 0 0,-8 3-25 0 0,11-4 212 0 0,2 0-1 0 0,-2-1 0 0 0,1-1 0 0 0,-2 0 0 0 0,1-1 0 0 0,0-1 1 0 0,-2 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0-2-186 0 0,-6 7 3 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-2-4-3 0 0,1 7 35 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 2-1 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,0-1 0 0 0,-2 1-35 0 0,1-1 16 0 0,-2 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-2 0 0 0,-1 1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-16 0 0,-55 117 249 0 0,39-11-267 0 0,19-103 28 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,2-1-1 0 0,0 0 1 0 0,1-1 0 0 0,-2 0-1 0 0,5 4-9 0 0,-6-6 6 0 0,2-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0-1 1 0 0,1 1 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1-1 0 0 0,-1 1-1 0 0,2-1 1 0 0,-2 1 0 0 0,1-1-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,6-1-6 0 0,-5 0 57 0 0,26-6-1613 0 0,-10 1-3577 0 0,-3-4-2072 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123239.429">4355 6120 920 0 0,'0'0'279'0'0,"0"0"833"0"0,0 0 362 0 0,0 0 78 0 0,0 0-63 0 0,0 0-322 0 0,0 0-140 0 0,0 0-31 0 0,0 0-26 0 0,0 0-88 0 0,0 0-40 0 0,0 0-8 0 0,0 0-34 0 0,0 0-136 0 0,0 0-66 0 0,0 0-12 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0-42 0 0,0 6-12 0 0,-10 47 1334 0 0,2 12-600 0 0,0 49 252 0 0,9 94-1210 0 0,3-94-216 0 0,7-12 642 0 0,-4-88-1088 0 0,-6-13-25 0 0,-1-1-998 0 0,0 0-429 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122817.09">4326 6331 12176 0 0,'0'0'561'0'0,"0"0"-17"0"0,2 1-217 0 0,87 9 5294 0 0,-11 7-5284 0 0,-11 11-2062 0 0,-65-28 475 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122538.437">4797 6618 2304 0 0,'-12'-8'3825'0'0,"10"5"-3248"0"0,-2 1 1 0 0,2-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-2-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-4-578 0 0,1 3 116 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-2 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0-116 0 0,-1 1 36 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-2 0 0 0,0 2 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 2-36 0 0,57 58 1232 0 0,-54-50-822 0 0,0 1 0 0 0,0-1-1 0 0,-2 0 1 0 0,1 2-1 0 0,-2 0 1 0 0,0-2-1 0 0,-1 3 1 0 0,1-1-1 0 0,-3-1 1 0 0,1 1 0 0 0,-1 10-410 0 0,-14 35 100 0 0,11-55-42 0 0,1 1 0 0 0,0-2 1 0 0,0 2-1 0 0,-1-1 0 0 0,1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-2 0-1 0 0,2-2 0 0 0,-1 2 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-2 1-58 0 0,-2-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,1-1 0 0 0,-6-2 0 0 0,-33-45-1424 0 0,33 25-5473 0 0,4 13-533 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121496.511">5209 6416 15176 0 0,'0'0'340'0'0,"0"0"50"0"0,-2 1 26 0 0,-15 18 101 0 0,13-15-271 0 0,1 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,2 1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0-245 0 0,4 55-21 0 0,47 57 1584 0 0,-48-113-1524 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,3 0-39 0 0,-1-3-10 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-2 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,1-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,-1 0 0 0 0,2-1-1 0 0,-2 0 1 0 0,0-2 10 0 0,3-3 49 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1 1 0 0 0,1-2 0 0 0,-3 0-1 0 0,1 0 1 0 0,-2-11-49 0 0,1 10-17 0 0,0 17 17 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 0 0 0,-13 36-209 0 0,13 86 192 0 0,12-86-2918 0 0,-11-24 1407 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-118100.252">5728 6363 4608 0 0,'24'-31'2473'0'0,"-15"16"4749"0"0,-3 19-1038 0 0,-1 7-5674 0 0,0-1-1 0 0,0 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 2-509 0 0,6 35 445 0 0,-1 21-52 0 0,5 67-233 0 0,-8-74-380 0 0,6 3-218 0 0,-11-63 32 0 0,0-2-1020 0 0,0 0-4245 0 0,0 0-1815 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-117537.033">5781 6463 1376 0 0,'0'0'448'0'0,"0"0"1344"0"0,0 0 588 0 0,0 0 116 0 0,0 0-136 0 0,0 0-684 0 0,0 0-299 0 0,0 0-58 0 0,0 0-107 0 0,0 0-419 0 0,0 0-179 0 0,0 0-35 0 0,0 0-40 0 0,11-4 578 0 0,54-61 1084 0 0,-62 64-2155 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,2-1-45 0 0,43 32 240 0 0,-11 32 664 0 0,-36-64-973 0 0,-1-1-608 0 0,0 0-262 0 0,0 0-1349 0 0,0 0-5210 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116084.978">6328 6509 920 0 0,'0'17'0'0'0,"0"-17"80"0"0,0 0-80 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 352 0 0,0 0 64 0 0,0 0 0 0 0,0 0 8 0 0,0 6-424 0 0,0-6 0 0 0,0 0 0 0 0,2 11-96 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115526.386">6353 6310 7856 0 0,'0'0'174'0'0,"0"0"29"0"0,0 0 13 0 0,0 9 2112 0 0,7 26 1209 0 0,-5-8-1555 0 0,3 65 1712 0 0,0 26-2229 0 0,-1-45-1465 0 0,-3-29 69 0 0,-2-27-2628 0 0,1-12 952 0 0,0-5-279 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115183.311">6353 6559 11832 0 0,'0'-16'1285'0'0,"24"-58"4317"0"0,20 31-3283 0 0,-40 42-2299 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 1-1 0 0,2-1 1 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 1-20 0 0,19 37 831 0 0,19 53 83 0 0,-30-45-684 0 0,-7 9 68 0 0,-7-27-874 0 0,3-30 150 0 0,0-1-988 0 0,-1 1-436 0 0,-1 4-92 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-114236.626">6843 6575 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0 0 43 0 0,0 0 159 0 0,0 0 70 0 0,0 0 14 0 0,0 0 69 0 0,0 0 285 0 0,0 0 126 0 0,0 0 29 0 0,0 0-15 0 0,0 0-77 0 0,0 0-31 0 0,0 0-8 0 0,0 0-33 0 0,0 0-134 0 0,2 1-61 0 0,49 6 2321 0 0,-33-8-2644 0 0,36-20 394 0 0,-50 19-751 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,2 1-1 0 0,-3-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-4 19 0 0,-8-6 0 0 0,7 11 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,-2 1 76 0 0,0 1 0 0 0,1 1-1 0 0,-1-1 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,2-1-1 0 0,0 3-75 0 0,44 52 0 0 0,-45-59 25 0 0,0 0 0 0 0,2 0 0 0 0,-1-2 0 0 0,0 1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,3-1-25 0 0,49-22-3889 0 0,-46 16-4253 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-106495.084">7428 6399 2760 0 0,'-36'-28'1211'0'0,"35"27"-702"0"0,-15-6 1981 0 0,-3 8-1483 0 0,11 5-408 0 0,-29 17 451 0 0,16-22 2469 0 0,7-5 2535 0 0,20-3-4219 0 0,47-13 338 0 0,40 21-421 0 0,-86 2-1693 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,0 3-59 0 0,49 33-101 0 0,-17-39 802 0 0,-37-2-571 0 0,-1 1 4 0 0,0 0-4 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-2 0 0,0 0-6 0 0,-19 27 213 0 0,-29 2-28 0 0,13-8-202 0 0,-39 15-64 0 0,-29 23 212 0 0,55-16-359 0 0,22-15 389 0 0,21-19-217 0 0,2-3 36 0 0,4-5-46 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-14 0 0,51-13 417 0 0,162-21 582 0 0,-159 37-919 0 0,-12 12-3590 0 0,-43-16 1676 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101751.894">7867 6714 3680 0 0,'-7'16'1721'0'0,"6"-11"9907"0"0,15-11-8856 0 0,15-13-2535 0 0,54-86 2026 0 0,3-45-1063 0 0,54-113-374 0 0,13 12-1554 0 0,-126 226 728 0 0,-10 0 0 0 0,-17 26 24 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1-23 0 0,-1 23 138 0 0,-1-2 0 0 0,-2 2 0 0 0,0-3-1 0 0,-2 3 1 0 0,-6 17-138 0 0,-7 28 173 0 0,-12 72-35 0 0,23-43 4 0 0,8-80-93 0 0,-1 0 0 0 0,2-1 0 0 0,0 0 1 0 0,2 0-1 0 0,-1 1 0 0 0,1-2 1 0 0,2 7-50 0 0,1 1 36 0 0,8 20 71 0 0,12 0 53 0 0,-17-48 10 0 0,63-153 270 0 0,-2 17-376 0 0,55-136-64 0 0,-75 182 0 0 0,-36 77 0 0 0,-14 19-2 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 2 0 0,0 0-1 0 0,8 57-63 0 0,-4 41 64 0 0,-8 38 203 0 0,-7 2 7 0 0,-6 36-63 0 0,-5-60-94 0 0,8-21-185 0 0,7-62-625 0 0,7-30-572 0 0,0-1-410 0 0,0 0-1290 0 0,0 0-4861 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101158">9041 6595 11232 0 0,'0'0'256'0'0,"0"0"34"0"0,0 0 20 0 0,-2 0-40 0 0,-30-3 1829 0 0,31 3-1367 0 0,1-2 59 0 0,9-45 2427 0 0,-7 39-3131 0 0,1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,0 1 1 0 0,-1 1-1 0 0,2-2 1 0 0,-1 1-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,2 0-86 0 0,-5 2 36 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-2 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-36 0 0,4 7 185 0 0,-1-1 0 0 0,0-1 0 0 0,-1 2 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-2-1-1 0 0,0 2 0 0 0,0-1 0 0 0,-3 7-185 0 0,5-16 57 0 0,-1 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-2 1-1 0 0,2-1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-3-57 0 0,-4 1-194 0 0,2-1 0 0 0,0 0 0 0 0,-1-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,2 0 1 0 0,0-1 0 0 0,-3-4 194 0 0,-5-35-3540 0 0,7 26-4246 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-100410.518">9669 6366 8496 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 10 0 0,0 0 112 0 0,-1 1 406 0 0,-38 74 4453 0 0,12-34-3370 0 0,13-1-456 0 0,12-15-994 0 0,-10 29 976 0 0,12-51-1274 0 0,0 2 0 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-2-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1-81 0 0,7 1 0 0 0,-2 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,4-7 0 0 0,56-96 0 0 0,-30 21 1046 0 0,-29 50-920 0 0,-7 38-27 0 0,-1 1-10 0 0,0 0 6 0 0,0 0 29 0 0,8 1 281 0 0,-2 12-392 0 0,2 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,-3 1 0 0 0,2 0 0 0 0,-3 1 0 0 0,1 0 0 0 0,-1-2 0 0 0,-1 2-1 0 0,-1 0 1 0 0,1 1 0 0 0,-2-2 0 0 0,-2 6-13 0 0,-14 100 1090 0 0,1-77-947 0 0,-2 0 1 0 0,-1-2 0 0 0,-2 0 0 0 0,-2 0-1 0 0,-1-3 1 0 0,-11 12-144 0 0,22-33 225 0 0,-1-2 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-3 0 0 0,-1 1-1 0 0,1-1 1 0 0,-2-1 0 0 0,0-1 0 0 0,-16 9-225 0 0,30-18-3 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-2-2 3 0 0,2-5-150 0 0,1 0 0 0 0,0-1 1 0 0,0 2-1 0 0,1-2 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,2 0 0 0 0,-2 1 1 0 0,1-1-1 0 0,2 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,3 1 150 0 0,4-14-1149 0 0,3-3-679 0 0,-2 4-278 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-99222.683">10300 6615 10136 0 0,'2'14'230'0'0,"-2"-11"30"0"0,0-3 19 0 0,0 0 105 0 0,0 0 411 0 0,0 0 182 0 0,10 7 1891 0 0,-6-4-2546 0 0,2-1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-2-1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,-1-1-1 0 0,3 0-322 0 0,3-2 206 0 0,1 1 0 0 0,-2 0 0 0 0,0-2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,3-4-206 0 0,44-70 696 0 0,-52 72-668 0 0,-1 0-1 0 0,0 0 1 0 0,-1-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 2 0 0 0,-1-2 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,-1-5-28 0 0,3 11 5 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,1-1-1 0 0,-1 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-2 1 1 0 0,2-1-1 0 0,0 1 1 0 0,-2 0-1 0 0,2-1 1 0 0,0 1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-5 0 0,-5 6 19 0 0,1 1 1 0 0,-1-3 0 0 0,2 4 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1 0 0 0,2 2-1 0 0,-1-1 1 0 0,2 0 0 0 0,-1 2-20 0 0,0-1 77 0 0,0 1-1 0 0,2 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 2 1 0 0,2-1 0 0 0,0 0 0 0 0,2 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,2 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,2-1-1 0 0,0 0 1 0 0,1 1-77 0 0,-3-6 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,0 0-1 0 0,-2 0 1 0 0,3 0 0 0 0,37-17-1473 0 0,-26 4 614 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95784.39">10871 6370 4608 0 0,'0'0'353'0'0,"0"0"35"0"0,0 0 1008 0 0,0 0 461 0 0,0 0 95 0 0,0 0-104 0 0,0 0-522 0 0,0 0-228 0 0,0 0-46 0 0,1 2-59 0 0,11 17 2469 0 0,6 30-1092 0 0,-11 39-307 0 0,-1 15-686 0 0,-9 7-869 0 0,3-108-577 0 0,0-2-52 0 0,0 0-21 0 0,0 0-198 0 0,0 0-824 0 0,0 0-362 0 0,0-1-1274 0 0,-3-4-4833 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94862.106">10920 6585 10016 0 0,'0'0'462'0'0,"0"0"-12"0"0,0 0-148 0 0,1-4 1464 0 0,51-65 3773 0 0,4 10-3387 0 0,-30 49-1432 0 0,-25 9-464 0 0,7 5 586 0 0,-3 0-782 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 2-60 0 0,2 8 248 0 0,14 67 841 0 0,-1 6-628 0 0,-23-68-366 0 0,4-21-174 0 0,1-1-11 0 0,0 0-178 0 0,0 0-783 0 0,0 0-344 0 0,0 0-69 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93718.36">11474 6314 3224 0 0,'0'12'2345'0'0,"0"30"5493"0"0,-2 3-4114 0 0,0 47-712 0 0,6 10 343 0 0,-8-83-3334 0 0,2-11-891 0 0,-10 3-7476 0 0,6-9 8097 0 0,4-1-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93135.977">11441 6585 456 0 0,'0'0'1763'0'0,"3"-14"5211"0"0,7-44-1110 0 0,14 41-1851 0 0,26-7-1678 0 0,-42 25-2203 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,3 6-132 0 0,21 37 1090 0 0,-25-40-1055 0 0,-2-2 0 0 0,0 2-1 0 0,1 1 1 0 0,-2-1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,-2-2-34 0 0,2 11-14 0 0,1-18-184 0 0,0-1-536 0 0,0 0-236 0 0,0 0-888 0 0,0 0-3561 0 0,0 0-1523 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-90762.018">11919 6615 8288 0 0,'-3'9'5575'0'0,"15"2"-3896"0"0,-11-11-1688 0 0,3 2 148 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,4-4-139 0 0,24-44 514 0 0,-21 26-481 0 0,-6 22-28 0 0,-2-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-3-4 0 0,1 5 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-63-9 0 0 0,60 9-6 0 0,-1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 1-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 2 1 0 0,-1-2 0 0 0,0 3 6 0 0,-1 0 50 0 0,0 0 1 0 0,2 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,2 0 1 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,2 0-1 0 0,0 1 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-2-1 0 0,0 2 1 0 0,1 0 0 0 0,2 6-51 0 0,-2-7 64 0 0,1-1 0 0 0,-1 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 1 0 0,2 1-1 0 0,-1 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,3 0-64 0 0,37 0-544 0 0,-24-10-5374 0 0,-5 1-1399 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88936.296">12466 6030 3224 0 0,'-3'16'4649'0'0,"-20"30"2676"0"0,3 37-3229 0 0,3 59-1931 0 0,18-126-1939 0 0,19 117 1016 0 0,14-34-627 0 0,-5-39 597 0 0,-26-58-1196 0 0,-2-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,2-1-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-3 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1-16 0 0,27-28 176 0 0,12-56-176 0 0,-15 3 0 0 0,-10-11 0 0 0,-5 15 0 0 0,-8-29 0 0 0,-3 6 43 0 0,0 101-266 0 0,0 1-29 0 0,0 0-4 0 0,0 0-141 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1251 0 0,0 0-4804 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87751.59">12989 6169 2304 0 0,'-4'14'3512'0'0,"4"-14"-3295"0"0,1 29 9139 0 0,9 17-4914 0 0,-8-36-4052 0 0,1-1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,0 2 1 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1-1 0 0 0,-2 6-389 0 0,0 28-162 0 0,2 43 39 0 0,6 31 299 0 0,-3-104 129 0 0,-2-1-2806 0 0,-1-12 1101 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87470.909">12996 6265 7832 0 0,'0'0'602'0'0,"1"1"-134"0"0,9 1 1838 0 0,32 7 3878 0 0,22-9-2721 0 0,12-8-2874 0 0,-43 7-6863 0 0,-25 1-248 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86426.787">13400 6422 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-128 0 0,1 2-606 0 0,9 93 6111 0 0,-10-23-5043 0 0,-3-7-2402 0 0,2-59 17 0 0,1-4-6835 0 0,0-2 4521 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86230.545">13727 6251 4144 0 0,'0'0'191'0'0,"-5"2"22"0"0,3 0 5833 0 0,-7 19 354 0 0,-8 11-4079 0 0,10 9-269 0 0,8-10-1028 0 0,-4-11-798 0 0,0 1 0 0 0,2-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,3 18-225 0 0,0 65 0 0 0,-10-38 0 0 0,5-55 13 0 0,1-3-3106 0 0,1-8 1973 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85578.149">13913 6472 3224 0 0,'0'15'553'0'0,"7"6"6334"0"0,-14 65 1088 0 0,2-10-6591 0 0,5-61-1121 0 0,0-2-3991 0 0,0-13-2374 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85386.832">13966 6320 17503 0 0,'0'0'776'0'0,"0"0"160"0"0,0 0-744 0 0,0 0-192 0 0,0 0 0 0 0,0 0 0 0 0,0 0 448 0 0,0 0 48 0 0,0 0 16 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1568 0 0,2 11-304 0 0,-2-11-64 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85026.437">13381 6225 18455 0 0,'0'0'408'0'0,"0"0"80"0"0,0 0 24 0 0,0 0 0 0 0,0 0-408 0 0,0 0-104 0 0,0 0 0 0 0,0 0 0 0 0,0 0 224 0 0,-7 0 16 0 0,7 0 8 0 0,0 0 0 0 0,0 0-992 0 0,0 0-200 0 0,0 0-40 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-83816.66">14285 6327 9584 0 0,'0'0'216'0'0,"-9"5"521"0"0,-49 33 3704 0 0,31-11-975 0 0,23-24-3254 0 0,-1 0 1 0 0,1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-1 1-1 0 0,1-2 1 0 0,-2 5-213 0 0,3-4 22 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,0-1 0 0 0,5 5-22 0 0,37 42 54 0 0,-20-34 918 0 0,-22-15-642 0 0,-2-1-115 0 0,8 3 109 0 0,0 9-171 0 0,-8-10-153 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,0 1 0 0 0,-2 1 0 0 0,0 0-4 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 5 0 0,-5-18-2397 0 0,9 8 122 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-79727.133">14503 6559 4632 0 0,'0'0'209'0'0,"1"-2"-5"0"0,32-59 6992 0 0,-32 61-6393 0 0,-1 0-31 0 0,21-7 2699 0 0,69 8 1055 0 0,-21-4-2917 0 0,-51 14-1448 0 0,-7 9-150 0 0,-12-20-7 0 0,1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 1 1 0 0,-1-1-4 0 0,-11-7 202 0 0,10 6-204 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 0 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1 1 0 0,-33 19 268 0 0,31-15-199 0 0,0 2-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,3 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,1 1-69 0 0,0-4 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,2 1 0 0 0,56-5-132 0 0,-53-2 154 0 0,-2-1 0 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-1 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,3-3-22 0 0,44-59-80 0 0,-39 25 64 0 0,-5-3 16 0 0,1 162 0 0 0,-8-71 0 0 0,4 6 0 0 0,11 10 0 0 0,-4-4-2782 0 0,-7-45 64 0 0,-4 1-4789 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76952.167">15536 6625 2304 0 0,'0'0'464'0'0,"-1"1"2357"0"0,-5 6-1769 0 0,6-5 3151 0 0,0-1 4184 0 0,29 14-5739 0 0,-23-14-2588 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-2 0-1 0 0,4-3-59 0 0,4-6-111 0 0,-6 9 95 0 0,-1-2 0 0 0,1 1 0 0 0,-2 0 1 0 0,2-1-1 0 0,-2 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,0-2 16 0 0,-2 4-53 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-3-1 0 0 0,2 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-3-2 54 0 0,4 4-6 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 2 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-2 1 0 0 0,2 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-2 0 7 0 0,-3 7 93 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,0-1 0 0 0,1 2 0 0 0,0 0 0 0 0,1-2 0 0 0,-1 2 0 0 0,2 0 0 0 0,0-1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 2 0 0 0,1-1 0 0 0,5 11-93 0 0,-7-19 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,4 0 0 0 0,-3-1-22 0 0,11-6-6424 0 0,-11-2-869 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77950.243">15132 6159 1840 0 0,'0'0'307'0'0,"0"-2"615"0"0,-2-29 3370 0 0,2 31-4103 0 0,0 0-1 0 0,0 0 44 0 0,0 0 22 0 0,0 0 2 0 0,0 0 74 0 0,0 0 316 0 0,0 0 142 0 0,0 1 32 0 0,7 61 3244 0 0,-7 73 861 0 0,0 69-1667 0 0,4-81-1971 0 0,6 62-363 0 0,-9-143-963 0 0,-2-24-3502 0 0,1-18 1678 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77348.9">15125 6303 13504 0 0,'0'0'620'0'0,"0"0"-16"0"0,5-6-364 0 0,17-4 1491 0 0,-17 7-1438 0 0,-1 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,-1 1-293 0 0,85 5 662 0 0,-44 8-2436 0 0,-20-7-4491 0 0,-15 0 465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76210.45">16117 6370 1840 0 0,'0'0'583'0'0,"-2"1"2720"0"0,-5 1-1116 0 0,-26 23 7260 0 0,28-17-9058 0 0,2 1 1 0 0,0-2-1 0 0,-1 2 0 0 0,1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,2 1 0 0 0,0 0 0 0 0,0 9-389 0 0,-4 48 2048 0 0,13 42-1440 0 0,-7-101-566 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,1 2-42 0 0,-3-6 48 0 0,-1-1 1 0 0,-1-1-1 0 0,1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2-1 0 0 0,2 0-48 0 0,8-6 0 0 0,-2 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,3-9 0 0 0,22-45 0 0 0,-2-10 0 0 0,-26 53 0 0 0,-4 15 0 0 0,-7 1-177 0 0,-8 13-4614 0 0,9-6-2832 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-72325.515">16603 6356 3224 0 0,'0'0'143'0'0,"0"0"-3"0"0,6 0 2973 0 0,-5-1 7737 0 0,-5 4-3072 0 0,3 3-10123 0 0,2 28 3033 0 0,-2-8 1192 0 0,1-25-1368 0 0,0 1 0 0 0,-17 76 715 0 0,7-14-1010 0 0,4-12-308 0 0,24 74-94 0 0,-14-90 185 0 0,-7-30-139 0 0,3-5-580 0 0,0-1-251 0 0,0-1-1544 0 0,3-8-6015 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45518.415">18391 6397 8288 0 0,'0'134'4740'0'0,"0"-117"-3699"0"0,0 12 42 0 0,0 2 0 0 0,1 0 0 0 0,3-2 1 0 0,0 2-1 0 0,7 20-1083 0 0,3-10-70 0 0,-7-27-1026 0 0,-5-13-85 0 0,-2-1-45 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45023.887">18787 6373 1376 0 0,'0'0'299'0'0,"0"0"715"0"0,0 0 313 0 0,0 0 66 0 0,-11-7 1242 0 0,7 6-2367 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2-1 1 0 0,0 2-1 0 0,-2 1-268 0 0,-49 87 3206 0 0,51-84-3121 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,0-1-1 0 0,0 1 1 0 0,2 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,2-2 0 0 0,-1 2 0 0 0,1-2-1 0 0,0 1 1 0 0,1 1-85 0 0,76 37 528 0 0,-80-43-518 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1-9 0 0,-1 2-25 0 0,0-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2-1 25 0 0,-9-14-3267 0 0,9 7-3203 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22924.697">16603 6555 920 0 0,'-5'10'80'0'0,"-5"6"5114"0"0,9-15-3500 0 0,1-1-770 0 0,0 0-336 0 0,0 0-68 0 0,0 0-20 0 0,0 0-51 0 0,0 0-22 0 0,0 0-3 0 0,0 0 25 0 0,0 0 107 0 0,0 0 48 0 0,0 0 11 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,7-21 5642 0 0,29-28-4223 0 0,12 16-1739 0 0,-43 32-286 0 0,3 2 1 0 0,4 10 96 0 0,-8-5-97 0 0,-4-5-115 0 0,2 0 1 0 0,-1 1-1 0 0,-1-1 0 0 0,1-1 0 0 0,0 2 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 105 0 0,10 2-1084 0 0,15-1-5055 0 0,-21-1 4517 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23746.448">17153 6271 1376 0 0,'0'0'331'0'0,"0"0"853"0"0,0 0 380 0 0,0 0 71 0 0,0 0-79 0 0,0 0-405 0 0,0 0-178 0 0,0 0-39 0 0,0 0-42 0 0,0 0-151 0 0,0 0-65 0 0,0 0-17 0 0,0 0 26 0 0,0 0 124 0 0,0 0 58 0 0,0 0 11 0 0,0 0-43 0 0,0 0-192 0 0,0 0-89 0 0,-16-3 1062 0 0,-29 16 904 0 0,-11 37-429 0 0,6 32-1643 0 0,27-36-267 0 0,5 48 275 0 0,14 17 391 0 0,10-78-660 0 0,-6-25-158 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,4 1-29 0 0,23 24 0 0 0,-21-27-4 0 0,-7-4-118 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,0 0 0 0 0,2-1-1 0 0,-2 0 1 0 0,0 1 0 0 0,1-2 122 0 0,26-17-6775 0 0,-23 11 184 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24081.144">17259 6442 456 0 0,'13'-35'1833'0'0,"7"16"8000"0"0,-6 2-4338 0 0,-13 16-4746 0 0,-1 1-12 0 0,9 1 2655 0 0,-4 4-3184 0 0,-2-1 0 0 0,2 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,-1 1 0 0 0,2 1-1 0 0,-2-1 1 0 0,0 1 0 0 0,0-2-1 0 0,1 2 1 0 0,-2 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 5-208 0 0,0-4 187 0 0,1 165 1174 0 0,-9-100-1017 0 0,-6-5-212 0 0,10-60-136 0 0,3-2 10 0 0,-1 1 0 0 0,1-2 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-2 1-5 0 0,-8 5-315 0 0,-30 22-6531 0 0,32-25 5010 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28120.561">17401 5865 4608 0 0,'3'-4'886'0'0,"1"-3"-1808"0"0,-3 2 5374 0 0,-1-3 4827 0 0,17 9-6424 0 0,-9 3-2408 0 0,-2 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-2 0 0 0 0,2 0 1 0 0,-1-1-1 0 0,-1 2 0 0 0,0-1 1 0 0,-1 1-1 0 0,3 3-447 0 0,11 26 1006 0 0,16 70 508 0 0,-23-23-882 0 0,4 232 416 0 0,-15-49-535 0 0,-11-43 14 0 0,-4 6-74 0 0,0-139-389 0 0,1-23 75 0 0,13-62-128 0 0,-21-1 223 0 0,-115-32-95 0 0,92 25-75 0 0,-7 7 28 0 0,-1-2 1 0 0,1-2-1 0 0,-22-4-92 0 0,-41-13 67 0 0,-164-68-67 0 0,246 78-114 0 0,-1 2 1 0 0,2 1-1 0 0,-2 2 0 0 0,0 1 0 0 0,1 2 1 0 0,-1 1-1 0 0,-15 4 114 0 0,-568 83 796 0 0,89-33-796 0 0,14 1 0 0 0,213-18 0 0 0,-12-8 0 0 0,-213-12 0 0 0,-406-17 0 0 0,604 6 0 0 0,-286-32 0 0 0,-71-18 0 0 0,157 25-457 0 0,-219-3 202 0 0,265-3-1 0 0,-150 18 256 0 0,320 4 172 0 0,-73 0 164 0 0,30-15-196 0 0,65 16 180 0 0,87 1-722 0 0,-30 1 8 0 0,-195-5 478 0 0,146-5 308 0 0,26-8-72 0 0,-251-16-1032 0 0,329 18 852 0 0,-73-9 432 0 0,-137-6-572 0 0,173 13 0 0 0,-39 19 0 0 0,-57-8 0 0 0,81-4 0 0 0,-88 33 0 0 0,23 12 0 0 0,124-47 0 0 0,16 18 0 0 0,55 0 0 0 0,96-6-20 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-2-1-1 0 0,2 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,2-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,2-1 20 0 0,-30-45-115 0 0,-8-62 687 0 0,-15-88-572 0 0,-19-88 0 0 0,48 48 0 0 0,-4 76 0 0 0,-3-19 0 0 0,22 72-796 0 0,10 23 1592 0 0,13 19-796 0 0,29-25 0 0 0,-36 82 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,1 0 0 0 0,8-7 0 0 0,73-37 0 0 0,82-24 0 0 0,-145 67 0 0 0,0 1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1 2 0 0 0,0 1 0 0 0,10 1 0 0 0,-37 1 0 0 0,125 0 0 0 0,0-4 0 0 0,29-9 0 0 0,23-14-712 0 0,88-19 1413 0 0,-160 30-697 0 0,0 5-1 0 0,1 5 1 0 0,64 5-4 0 0,284 18 0 0 0,-116-1 0 0 0,-271-12-72 0 0,2 2 1 0 0,-1 3-1 0 0,48 14 72 0 0,81 8-105 0 0,-66-21 425 0 0,59 12-320 0 0,-50 3 0 0 0,65 14 0 0 0,76 3 0 0 0,54 21 0 0 0,-179-26 0 0 0,53-2 0 0 0,44 3-796 0 0,-88-5 1592 0 0,3-10-831 0 0,9-27-250 0 0,-32 4 605 0 0,57 10-320 0 0,-95-7 0 0 0,86-19 0 0 0,-39-3 0 0 0,135 14 0 0 0,-189 5 0 0 0,-1-5 0 0 0,69-11 0 0 0,52-6 0 0 0,133 6 0 0 0,-39-6 0 0 0,-144 5 0 0 0,223 0 0 0 0,-102 15 0 0 0,104-19 0 0 0,83-11 0 0 0,-325 25 0 0 0,16-1 0 0 0,255 3 0 0 0,-138 15 0 0 0,-57-3 0 0 0,117-21 0 0 0,10 21 0 0 0,-209 0 0 0 0,7-11 0 0 0,-14-3 0 0 0,-16 7 0 0 0,10 4 0 0 0,31-11 0 0 0,57 14 0 0 0,-72 7 0 0 0,-80-16 0 0 0,165-4 0 0 0,-65 21 0 0 0,-84-5 0 0 0,49-2 0 0 0,-44 2 0 0 0,149 13 0 0 0,-59-8 0 0 0,-69-1 0 0 0,65 3 0 0 0,-77-15 0 0 0,35-5 0 0 0,-38 26-4336 0 0,-37-5-1782 0 0,-43-14-3483 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29020.976">17040 5625 1376 0 0,'0'0'591'0'0,"0"0"1942"0"0,0 0 851 0 0,0 0 174 0 0,0 0-327 0 0,-12 8 6223 0 0,15-5-9289 0 0,2 1 0 0 0,-2-2 0 0 0,0 1 0 0 0,2 0-1 0 0,-2-1 1 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,1-1 1 0 0,0-1-165 0 0,1 2 87 0 0,109 16 1139 0 0,-6 21-943 0 0,-61-22-166 0 0,6-26 11 0 0,-20 8-64 0 0,-17 18-64 0 0,-10 16 13 0 0,-7 5 198 0 0,-2 57 157 0 0,4-6-616 0 0,-1-30-3854 0 0,1-34-5107 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-134780.189">8866 7445 1376 0 0,'0'0'65'0'0,"0"0"189"0"0,0 0 767 0 0,0 0 335 0 0,0 0 69 0 0,0 0-94 0 0,0 8 1469 0 0,-2 70 3116 0 0,4-15-3609 0 0,-15 100-383 0 0,12-28-438 0 0,1-59-917 0 0,-3 0 598 0 0,2 102-205 0 0,-7 4-322 0 0,13 94-40 0 0,-2-180-336 0 0,-3 19 8 0 0,10 116 323 0 0,6-5 583 0 0,-4-60-1855 0 0,-6 84 952 0 0,0-53-94 0 0,-5-139-117 0 0,5-4-2277 0 0,-3-76-5567 0 0,-3 8 286 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-134240.189">8332 9545 5528 0 0,'0'0'422'0'0,"0"0"-88"0"0,0 0 656 0 0,0 16 2881 0 0,11 37-2527 0 0,8 40 2164 0 0,23-10-466 0 0,77 125 109 0 0,-79-145-2761 0 0,-30-44-296 0 0,1 0 0 0 0,2-1 1 0 0,-1 0-1 0 0,2 0 1 0 0,0-1-1 0 0,2-2 1 0 0,0 1-1 0 0,13 10-94 0 0,64 22 544 0 0,-89-45-475 0 0,2-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 1 0 0,0 0-1 0 0,-2 0 0 0 0,2-1 0 0 0,3-2-69 0 0,31-38 176 0 0,92-231 1624 0 0,-38 85-1872 0 0,-47 71-576 0 0,-27 65-2737 0 0,-12 38 1634 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-125200.19">3442 10359 13128 0 0,'0'-16'633'0'0,"0"15"-277"0"0,0 8 83 0 0,14 215 3164 0 0,20-12-1187 0 0,-8-1-1552 0 0,-28-122-897 0 0,-15-31-3046 0 0,14-47 1239 0 0,-5-5-71 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-124660.19">3358 10347 7056 0 0,'-2'-5'116'0'0,"1"0"0"0"0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,2-4-117 0 0,1-6 1073 0 0,-3 12-878 0 0,1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,0 2 1 0 0,-1-2 0 0 0,2 1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0-1 0 0,-2 1 1 0 0,4-1-195 0 0,-2 1 85 0 0,1 1 1 0 0,0 0-1 0 0,-2 0 0 0 0,2 0 0 0 0,-2 1 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,3 3-85 0 0,47 46 670 0 0,-25-19 265 0 0,23 36 175 0 0,-47-56-1010 0 0,-2 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-2-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-2 0 1 0 0,0 1-1 0 0,-2 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,-2 0 0 0 0,1 1 1 0 0,-2-2-1 0 0,-3 8-100 0 0,3-10 186 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-2-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1-1-1 0 0,0 1 1 0 0,-3 0-186 0 0,7-5 12 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0-1-11 0 0,-43 6 164 0 0,48-5-225 0 0,18 13-71 0 0,38 30 57 0 0,-32-19 68 0 0,58 76 132 0 0,0 44-125 0 0,-41-67-5360 0 0,-35-58 3443 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123330.19">4190 11009 6912 0 0,'0'0'528'0'0,"0"0"-219"0"0,0 0 347 0 0,0 1 192 0 0,13 10 3088 0 0,49-14-2645 0 0,22-32-467 0 0,-31 6 415 0 0,-50 26-1110 0 0,-1 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1-128 0 0,-29-38 870 0 0,24 40-830 0 0,1 0 1 0 0,-1 0 0 0 0,-1 0-1 0 0,2 1 1 0 0,-2 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 2 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,2 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,2 1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-2 1 0 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,2 1-1 0 0,-1-2 1 0 0,-2 5-41 0 0,1 0 30 0 0,2 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-30 0 0,20 102 84 0 0,-18-104-98 0 0,2-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,2-2 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0-1 0 0,-2 0 1 0 0,2-1 0 0 0,0 0 0 0 0,1 0 14 0 0,8 0-1085 0 0,-1-1-349 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122830.19">4767 10632 920 0 0,'1'2'67'0'0,"6"15"218"0"0,-7-15 1126 0 0,0-2 485 0 0,0 0 95 0 0,0 0-144 0 0,0 0-698 0 0,0 0-306 0 0,3 14 5156 0 0,5 68-3006 0 0,-1 139-2907 0 0,17-65 348 0 0,-10-95-1540 0 0,-9-54-81 0 0,-2-4-3107 0 0,-3-2-1448 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122530.19">4767 10714 5984 0 0,'0'0'464'0'0,"0"0"-82"0"0,11 12 5502 0 0,39-2-3006 0 0,32-10-1919 0 0,-26-4-2545 0 0,-43 4-3811 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2419.811">8287 10596 1840 0 0,'0'0'83'0'0,"0"7"10"0"0,-4-2 194 0 0,-4 6 6325 0 0,0 2-4677 0 0,5-7-1065 0 0,-4 25 3503 0 0,10 48-1185 0 0,1 46-2006 0 0,1-55-326 0 0,4-41-586 0 0,22 42 628 0 0,-29-69-870 0 0,2 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 0 1 0 0,1 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,2-1-28 0 0,5-5 21 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,0-2-1 0 0,0 1 0 0 0,3-8-21 0 0,23-41 0 0 0,-9-13 1099 0 0,1-23-934 0 0,-18 6-165 0 0,-2 60 0 0 0,-8-37 0 0 0,3 21-283 0 0,2 27-8605 0 0,-1 18 2172 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3219.811">8871 10537 8288 0 0,'-10'67'3321'0'0,"8"22"1356"0"0,4-7-2700 0 0,0-29-1241 0 0,1 128 440 0 0,-3-166-966 0 0,8 42-294 0 0,-7-56-163 0 0,-1-1-857 0 0,0-2-3536 0 0,0-5-1518 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3409.81">8853 10632 8288 0 0,'0'0'638'0'0,"8"-3"2018"0"0,19-2 1429 0 0,17 15-2828 0 0,-27-5-864 0 0,32 22-411 0 0,-42-22-355 0 0,15 19-3587 0 0,-13-14 2594 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3629.811">9261 10842 3680 0 0,'0'0'284'0'0,"3"8"797"0"0,-1-5 4784 0 0,0 30-1677 0 0,0 5-3145 0 0,-3 36-251 0 0,5-14-1216 0 0,-4-45-1299 0 0,0-6-3631 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4049.811">9560 10632 920 0 0,'-4'-13'343'0'0,"4"10"1102"0"0,0 3 482 0 0,0 0 96 0 0,0 0-124 0 0,0 0-614 0 0,0 0-269 0 0,0 0-50 0 0,0 0-57 0 0,0 0-212 0 0,0 0-90 0 0,0 2-20 0 0,-1 34 1508 0 0,-5 36-993 0 0,-6 80 402 0 0,8-54-494 0 0,12 54-140 0 0,3-72-1121 0 0,-11-79-772 0 0,0-1-333 0 0,0 0-68 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4549.811">9862 10933 456 0 0,'-6'20'0'0'0,"6"-19"651"0"0,-2 0 4741 0 0,-1 1 3820 0 0,3 2-9813 0 0,2 167 4824 0 0,3-121-4491 0 0,-5-45-754 0 0,0-4-326 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5199.81">10200 10907 10136 0 0,'0'0'464'0'0,"-2"0"-10"0"0,-5 0-222 0 0,-12 14 3123 0 0,17-13-3266 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1-89 0 0,25 49-256 0 0,-16-28 538 0 0,38 27 412 0 0,-14 3-275 0 0,-30-19-94 0 0,-20 4 1227 0 0,4-23-785 0 0,-15 4 957 0 0,14-17-1575 0 0,-9-2-133 0 0,-5-16-2201 0 0,23 10-250 0 0,3 4-4568 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6589.811">10483 11149 10136 0 0,'7'15'230'0'0,"-6"-11"30"0"0,-1-4 19 0 0,3-7 478 0 0,4-33 763 0 0,-5 38-1014 0 0,-1-1-2 0 0,8-25 334 0 0,-8 22-761 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,3 0-78 0 0,-5 4 167 0 0,29-15 1024 0 0,-28 15-1129 0 0,1 1 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-2 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2-1-1 0 0,1 1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0-61 0 0,27 30 1857 0 0,-28-31-1723 0 0,-1-1-46 0 0,0 0-22 0 0,0 0-2 0 0,0 0 2 0 0,0 0 4 0 0,-24 0 2 0 0,20 0-87 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,2-1 1 0 0,0 1-1 0 0,-3 1 16 0 0,-25 15-85 0 0,29-18 77 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-2 0 0 0,-2 2 0 0 0,2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,0 2 8 0 0,12 29-54 0 0,-12-31 57 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,2 1 0 0 0,-2-2 0 0 0,1 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-3 0 0,50 5 163 0 0,-45-9-205 0 0,-1 0-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-2 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,-1-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 2-1 0 0,-2-5 43 0 0,7-67-556 0 0,-7 77 622 0 0,0 1 34 0 0,0 0 10 0 0,-1 3-16 0 0,0 11 66 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,2 0-1 0 0,-1-1 0 0 0,3 11-160 0 0,2 24 76 0 0,16 26 0 0 0,-13-36-1057 0 0,-9-36-90 0 0,6 7-37 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7129.81">11097 10732 456 0 0,'0'-22'204'0'0,"0"10"5674"0"0,-3 12 1245 0 0,-6 24-4666 0 0,-2 52-110 0 0,11 93-830 0 0,-4 69-628 0 0,14-179-907 0 0,-9-53 2 0 0,-1-6-2564 0 0,0 0 1298 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7369.81">11059 10874 8752 0 0,'5'8'936'0'0,"13"-23"1798"0"0,43 15 2614 0 0,35 4-4455 0 0,-54 12-4124 0 0,-34-12 2047 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7929.811">11501 11216 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,2 1-40 0 0,41-7 2129 0 0,-18-1-968 0 0,-22 6-1318 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2 0-1 0 0,-2 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1-82 0 0,7-9 268 0 0,-5 10-243 0 0,-2-2 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 2 1 0 0,-1-2 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-4-3-25 0 0,6 5 20 0 0,-2 1 0 0 0,2-2-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,0 2-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0-1-20 0 0,-6 11 226 0 0,1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-2 0 0 0,1 1-1 0 0,1 1 1 0 0,0 1 0 0 0,1-2 0 0 0,0 2-1 0 0,1 3-225 0 0,-1-12 37 0 0,2 2 31 0 0,0-1-1 0 0,0 1 0 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 0 1 0 0,0-1-1 0 0,-1 2 0 0 0,2-1 1 0 0,-1 0-1 0 0,2 0-67 0 0,-2-2 33 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,3 0-33 0 0,45 7-313 0 0,-12-14-1742 0 0,-31 5 191 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8439.811">11998 11004 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,-11 3 2224 0 0,1 8-1481 0 0,8-9-561 0 0,2-2 0 0 0,-1 1 0 0 0,-33 38 1128 0 0,32-37-1631 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-9 0 0,0 19 74 0 0,-1-17-14 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,2 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,2 1-59 0 0,61 32 164 0 0,-61-35-163 0 0,-2-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,2 0 1 0 0,-2-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2-1-1 0 0,1-1 0 0 0,27-38 0 0 0,-1-26 0 0 0,-23 38 0 0 0,-6-42 0 0 0,0 63 0 0 0,0 10-1 0 0,0 0 0 0 0,0-1 0 0 0,-2 1-1 0 0,2 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 2 0 0,-2 2-86 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,2 5 86 0 0,10 43-6882 0 0,-5-42 1085 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8909.811">12600 10864 3224 0 0,'4'17'240'0'0,"-19"12"5162"0"0,-8 22 1702 0 0,3 32-4883 0 0,10-45-1389 0 0,6 23 96 0 0,-2-23-476 0 0,6 22 178 0 0,-5 6-648 0 0,2-55 50 0 0,-1-6-3037 0 0,4-5 1818 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9219.811">12544 11082 10136 0 0,'2'9'1085'0'0,"48"-43"1390"0"0,-47 31-2239 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,2 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1 0 0 0 0,3-1-236 0 0,31-14 608 0 0,-11 30 520 0 0,-10 4-434 0 0,-15-17-580 0 0,16 13-10 0 0,-18-11-96 0 0,14 20-8 0 0,-14-18-92 0 0,-1-3-390 0 0,0 7-1954 0 0,3-1-3569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12429.81">13188 10743 2304 0 0,'0'0'101'0'0,"1"-2"1"0"0,1-4-3003 0 0,-1 1 4359 0 0,-6-3 14711 0 0,-4 14-13468 0 0,5-3-2385 0 0,1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,3 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,1 5-316 0 0,-1 96 1202 0 0,2-94-965 0 0,3 39-228 0 0,2 1 0 0 0,1-1 1 0 0,3-1-1 0 0,3 1 0 0 0,8 19-9 0 0,-11-39 0 0 0,-2-20 0 0 0,19 1-1058 0 0,12-29-4850 0 0,-27 9 3794 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12789.811">13558 10655 1376 0 0,'0'0'65'0'0,"0"0"454"0"0,0 0 1882 0 0,5 0 5023 0 0,4 0-3511 0 0,-6 2-3615 0 0,0-1-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,2 3-297 0 0,28 49 2384 0 0,-5-9-1738 0 0,-16-32-400 0 0,-1 2 0 0 0,0 1-1 0 0,-2-2 1 0 0,1 2 0 0 0,-2 1-1 0 0,-1 0-245 0 0,16 115 608 0 0,-17 65 104 0 0,-12-62-61 0 0,0-90-3304 0 0,-3-4-3362 0 0,8-31-807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16819.81">14206 12060 3224 0 0,'0'0'143'0'0,"0"0"327"0"0,0 0 1271 0 0,0 0 550 0 0,0 0 114 0 0,0-3 988 0 0,1-10-1052 0 0,0-53 2752 0 0,8-2-2899 0 0,10-94-927 0 0,5-50-315 0 0,-9 75 489 0 0,-5-100-1441 0 0,-8 148 170 0 0,2 8 86 0 0,3-1-1 0 0,8-35-255 0 0,6-24 592 0 0,-7 23-253 0 0,-10 22 96 0 0,5 46-99 0 0,4-12-403 0 0,0 34 67 0 0,-7 12 13 0 0,-2-1 79 0 0,-8 7 139 0 0,-6-9-231 0 0,9 17 5 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1-5 0 0,-127 3 320 0 0,66 1-256 0 0,-64 5 61 0 0,-249 11 207 0 0,46 3-320 0 0,14 14 52 0 0,28 16-64 0 0,-287 56 128 0 0,368-86-117 0 0,82-14 98 0 0,-2-4 0 0 0,-35-7-109 0 0,21 0-2 0 0,-78-4 367 0 0,-91 1-133 0 0,-27-6-541 0 0,107-3 706 0 0,-14 0-710 0 0,58 5 634 0 0,-193-1-321 0 0,208-3-16 0 0,-39 1-155 0 0,-39-9 182 0 0,-116-12 65 0 0,213 22-88 0 0,-26 5 12 0 0,-51 3 64 0 0,19 0-64 0 0,-58-7 0 0 0,-328-30 64 0 0,408 26-64 0 0,-291-9 0 0 0,420 24 0 0 0,-156-10 0 0 0,75-5 0 0 0,-43-6 0 0 0,-25-1 0 0 0,-109 16 0 0 0,212 7 0 0 0,-54-15 0 0 0,31-5 0 0 0,90 14 0 0 0,0 1 0 0 0,-2 2 0 0 0,-35 4 0 0 0,-12 0 0 0 0,-248 7-11 0 0,124-34 22 0 0,-92-18-11 0 0,-50 38-64 0 0,269-5 128 0 0,57 8-64 0 0,0 0 0 0 0,1-2 0 0 0,-1-1 0 0 0,-24-7 0 0 0,33 6 0 0 0,6 0 0 0 0,0 2 0 0 0,-1-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,1 2 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1 0 0 0,-4 1 0 0 0,5 1 0 0 0,8-3 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-2 2 0 0 0,-15 70-244 0 0,45 138 168 0 0,-3-61 299 0 0,33 223-446 0 0,-6-28 520 0 0,1-173-530 0 0,-24-84 233 0 0,20 50 0 0 0,12-7 0 0 0,-47-115 0 0 0,59 74 0 0 0,-53-79 4 0 0,0-1 0 0 0,1-2 0 0 0,0 0 0 0 0,2-1-1 0 0,-1-2 1 0 0,0 1 0 0 0,0-3 0 0 0,2 1 0 0 0,5 0-4 0 0,29 11 140 0 0,88 14-242 0 0,-16-9 207 0 0,98 3-105 0 0,-87-10-23 0 0,80 2-132 0 0,6-8 155 0 0,503 21 0 0 0,-143-9 0 0 0,-62 2 0 0 0,86-19 53 0 0,-70-39-42 0 0,-161-16-11 0 0,48 10 0 0 0,-185 25 12 0 0,-11 10 112 0 0,98-8-204 0 0,51 20 149 0 0,16-8-58 0 0,-5-10-107 0 0,11 1 96 0 0,-177 3 96 0 0,113 12-192 0 0,-236 14 96 0 0,45-2 0 0 0,36-1 144 0 0,-55-18-240 0 0,4-2 192 0 0,-90 6-96 0 0,-1-1 0 0 0,2-3 0 0 0,-2-1 0 0 0,35-7 0 0 0,28-4-96 0 0,35 7 96 0 0,111 3 0 0 0,-122-9 80 0 0,-36 4-160 0 0,102-7 80 0 0,-80 19 11 0 0,90-17 42 0 0,-96-3-141 0 0,-17-6 94 0 0,1 2 0 0 0,63-4-6 0 0,-43 12 60 0 0,0 12-60 0 0,42 35 0 0 0,-53-17 0 0 0,-88-15 0 0 0,21 12 0 0 0,-27-7 59 0 0,-4-6-111 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 52 0 0,-5 4-1004 0 0,5-4-3898 0 0,1-1 2712 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25749.81">17857 6149 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0-10 1147 0 0,0 6-3619 0 0,1-4 9257 0 0,0 5 2091 0 0,-1 8-7632 0 0,13 187 1589 0 0,-17-100-2526 0 0,-5-7-90 0 0,3-5-182 0 0,16 6-118 0 0,-2-40-2244 0 0,-7-45 1548 0 0,-1-1-185 0 0,0 0-84 0 0,0 0-21 0 0,3 3-3895 0 0,-3-3 2635 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26679.81">17883 6566 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0 0-22 0 0,0-14 2511 0 0,15-69 5565 0 0,-3 58-6834 0 0,10 1-281 0 0,-5 8-550 0 0,-16 15-517 0 0,-1 1-6 0 0,3 0 3 0 0,21 7 472 0 0,-1 12 14 0 0,11 52 396 0 0,7 61-438 0 0,-29-81-450 0 0,-12-25-1627 0 0,0-12-6318 0 0,0-4 1470 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37589.811">14948 10926 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,4-8 1867 0 0,-3 7-1852 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-240 0 0,-5-2 274 0 0,-1-1-1 0 0,1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-2 0 0 0 0,1 0-1 0 0,-3 2-273 0 0,-9 5 0 0 0,12-1 0 0 0,-28 32 0 0 0,26-23 150 0 0,0 0 1 0 0,1 2-1 0 0,0-2 0 0 0,1 2 0 0 0,1 0 0 0 0,0 1 0 0 0,2-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 1 0 0,2-1-1 0 0,1 2 0 0 0,0 4-150 0 0,-1-1 104 0 0,-16 200-482 0 0,10-116 567 0 0,9-12-136 0 0,-1-93-229 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0 176 0 0,8-3-1901 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37999.811">14605 11225 5984 0 0,'0'0'464'0'0,"0"0"-100"0"0,0 0 717 0 0,0 0 346 0 0,0 0 69 0 0,0 0-71 0 0,0 0-330 0 0,0 0-146 0 0,7 12 1624 0 0,-3-8-2296 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1-1-1 0 0,1 1 1 0 0,1-1 0 0 0,-2 1 0 0 0,5-1-277 0 0,16 8 296 0 0,20 1 73 0 0,-37-7-712 0 0,21 10-175 0 0,-13 4-5552 0 0,-9-4-166 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38309.811">14918 11562 6624 0 0,'0'0'298'0'0,"0"0"-3"0"0,0-2-188 0 0,27-52 3721 0 0,-19 41-2931 0 0,-7 11-725 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 1 0 0,1-1-173 0 0,0 2 83 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 1 1 0 0,-1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 1-83 0 0,4 3 241 0 0,0 1 0 0 0,-2 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 6-241 0 0,-5 51 1376 0 0,-3-48-782 0 0,7-16-550 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1-44 0 0,-2-2-23 0 0,-1 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,2-1-1 0 0,-2 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,2 1 0 0 0,-1-1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0-2 24 0 0,-12-40-1750 0 0,9 20 132 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39549.811">15355 11538 4608 0 0,'0'0'101'0'0,"-3"-4"150"0"0,2-1-50 0 0,1 4 308 0 0,0 1 135 0 0,0-1 27 0 0,-2-36 1126 0 0,2 36-1534 0 0,0 1-330 0 0,0 0-71 0 0,0 0 38 0 0,0 0 152 0 0,0 0 68 0 0,0 0 9 0 0,0 1-17 0 0,2 1-16 0 0,-2-1 280 0 0,0-1 113 0 0,0 0 21 0 0,0 0-68 0 0,0 0-262 0 0,0 0-9 0 0,-1 6 712 0 0,0-6-575 0 0,1 0 4 0 0,0 0 26 0 0,0 0 113 0 0,0 0 49 0 0,0 0 11 0 0,0 0-57 0 0,0 0-239 0 0,0 0-102 0 0,0 0-17 0 0,0 0 18 0 0,0 0 99 0 0,0 0 47 0 0,0 0 11 0 0,0 0 0 0 0,0 0 1 0 0,0 0 0 0 0,2 7 268 0 0,10 24 656 0 0,-8 18 132 0 0,9 16 242 0 0,-7-33 28 0 0,-6 35-1582 0 0,-5-24-16 0 0,5-33 0 0 0,1-83 1117 0 0,-2 33-1650 0 0,6-48 37 0 0,-9-1 27 0 0,16 59 834 0 0,-9 23-365 0 0,25-6-1090 0 0,-27 13 1590 0 0,0 1-59 0 0,55 45-276 0 0,-22-3-165 0 0,-12 0 0 0 0,2 9 0 0 0,-14-10 0 0 0,-9-24 72 0 0,6 4-112 0 0,-7-20-81 0 0,0-2-30 0 0,13 5-660 0 0,11-3-2647 0 0,-19-9 2023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41569.811">15867 11499 6448 0 0,'31'-48'4184'0'0,"-30"47"-3679"0"0,-1 1 6 0 0,0 0 1 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 0 0 0,0 0-24 0 0,0 0-100 0 0,0 0-42 0 0,0 0-8 0 0,0 0-20 0 0,0 0-74 0 0,0 0-39 0 0,0 0-5 0 0,0 0 26 0 0,0 0 104 0 0,0 0 44 0 0,0 0 8 0 0,0 0-31 0 0,13 2 130 0 0,-13-1-345 0 0,-19 8 299 0 0,-3 4-94 0 0,-34 31 589 0 0,18-11 20 0 0,23 12-70 0 0,15-43-729 0 0,0 0-40 0 0,-1 13 5 0 0,1-12-81 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,3-1-27 0 0,-1 2 24 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,4 0-23 0 0,28 6-16 0 0,2-12-321 0 0,0-16-1384 0 0,-19 18-2498 0 0,-8-2-2527 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42539.811">16247 11221 456 0 0,'0'0'1877'0'0,"0"0"225"0"0,0 0 96 0 0,0 0-174 0 0,0 0-800 0 0,0 0-352 0 0,0 2-68 0 0,-3 78 5406 0 0,0-8-3788 0 0,-5 6-533 0 0,0 106-938 0 0,9-89-994 0 0,-1-92-228 0 0,2 8 239 0 0,-1-4-2836 0 0,-1-12 836 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42759.811">16191 11355 10592 0 0,'0'0'818'0'0,"0"0"-382"0"0,0 0 375 0 0,2 0 224 0 0,52 12 3870 0 0,-12 3-4655 0 0,-17-8-2639 0 0,-24-6 1115 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="43219.811">16511 11548 920 0 0,'0'-6'1780'0'0,"-8"-29"5181"0"0,8 34-6117 0 0,0 1-63 0 0,4-5 1525 0 0,-2 2 782 0 0,7 22-961 0 0,-17 39 414 0 0,-1-12-2418 0 0,16-5-123 0 0,8 30-266 0 0,-15-69-1124 0 0,0-2-490 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="43559.811">16764 11579 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,-7-14-276 0 0,7 10-201 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 3 0 0 0,1-3 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0-59 0 0,-2 1 59 0 0,-1 1 0 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-61 0 0,14 46 1489 0 0,-15-38-1068 0 0,1 1-1 0 0,-1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,-1 0-420 0 0,2-10 47 0 0,-19 55 2134 0 0,-26 17-2086 0 0,45-72-50 0 0,-2 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-2-2-46 0 0,-36-47 76 0 0,20 3-2636 0 0,12 12-3921 0 0,2 11-600 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51949.811">17122 11365 2760 0 0,'3'6'3463'0'0,"-2"-2"5440"0"0,-10 22-3399 0 0,9 21-2728 0 0,-2 11-1732 0 0,-7 23 73 0 0,11 40-1117 0 0,1-94-2100 0 0,-3-29 527 0 0,4-4-370 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="52379.811">17111 11559 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0 0 240 0 0,0-8 1066 0 0,15-30 2918 0 0,33 1-1475 0 0,-31 30-2427 0 0,24-3-98 0 0,-32 12-954 0 0,45 18 0 0 0,15 46 242 0 0,-31 31 636 0 0,-28-60-878 0 0,-6-21 0 0 0,-8 8-49 0 0,4-23-207 0 0,0-1-87 0 0,0 0-917 0 0,0 0-3813 0 0,0 0-1633 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54319.811">17773 11086 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,0 17 1877 0 0,8 79 4244 0 0,-6-24-3972 0 0,-7 44-624 0 0,0-23-1860 0 0,4 85 1890 0 0,2-6-1730 0 0,3-159-88 0 0,-1 3-289 0 0,-2 2-5727 0 0,-4-34 687 0 0,-1 1 3586 0 0,8 2-135 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55229.81">17785 11132 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,3-7-177 0 0,-3 5 136 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-2 1-247 0 0,11-6 1678 0 0,45-7 1057 0 0,23 24-286 0 0,-63-6-2099 0 0,-5-1-94 0 0,0 1 0 0 0,1 1 0 0 0,-2 0 0 0 0,0-1 1 0 0,1 2-1 0 0,-2 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,4 6-256 0 0,13 29 768 0 0,8 35 88 0 0,-28-15-68 0 0,-12-16 336 0 0,-17-11-1124 0 0,16-32 144 0 0,-1 1 0 0 0,2 0-1 0 0,-2-1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,0-1-1 0 0,-5 1-143 0 0,-41 16 238 0 0,51-19-196 0 0,-2-1-31 0 0,1 2-27 0 0,62-29-776 0 0,16 17-152 0 0,-4 28-54 0 0,-20 15 92 0 0,-12 14 866 0 0,-29-27 40 0 0,-6-15 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,-2 2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 3 0 0 0,-27 31 1352 0 0,-11 1-736 0 0,25-32-497 0 0,-1 0-1 0 0,2-2 1 0 0,-2 0-1 0 0,-1-1 1 0 0,1-1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-2 1 0 0,0 0 0 0 0,0-1-1 0 0,-6-1-118 0 0,-62 7 387 0 0,28 10-334 0 0,29-16-53 0 0,-6-18-801 0 0,24 9-282 0 0,2 1-2237 0 0,2 2-3262 0 0,0-2-1015 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56249.811">18621 11103 14800 0 0,'0'0'332'0'0,"0"0"50"0"0,0 0 25 0 0,0 0-47 0 0,0 0-106 0 0,0 0 417 0 0,0 2 206 0 0,-9 52 3904 0 0,7-24-4120 0 0,-17 135 1824 0 0,-3-30-880 0 0,8-32-165 0 0,-13 131-832 0 0,26-228-672 0 0,1-5-273 0 0,0-1-138 0 0,0 3-1216 0 0,-2 4 3621 0 0,1-2-4753 0 0,1 0-9564 0 0,0-5 10339 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56479.811">18630 11155 920 0 0,'0'-5'1157'0'0,"1"2"5384"0"0,19-13-1079 0 0,30 8 55 0 0,25 14-2419 0 0,-3 11-1830 0 0,-11 12 320 0 0,18 44-1572 0 0,-20 12 2016 0 0,-53-72-1886 0 0,-1 1 0 0 0,-1-2 0 0 0,1 1 0 0 0,-2 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-2 1 0 0 0,0-1 0 0 0,-1 2 0 0 0,0-2-1 0 0,-1 1 1 0 0,-2 0 0 0 0,0 6-146 0 0,1 0 8 0 0,-2 0 0 0 0,1-1 0 0 0,-3-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-3-1 0 0 0,1 1 0 0 0,-1-2 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-2 0 0 0,-4 2-8 0 0,11-9 173 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,-4 0-174 0 0,-124-3-286 0 0,105-4-191 0 0,23 5 329 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-6-4 148 0 0,6 3-710 0 0,5 6-8073 0 0,3 0 434 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57489.811">19363 11722 7368 0 0,'0'0'333'0'0,"0"0"0"0"0,-9 4 14776 0 0,7-4-14374 0 0,2-2-710 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,2 0 1 0 0,-1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,1 0 0 0 0,0 1-25 0 0,-3 1 94 0 0,0 0 9 0 0,0 0 29 0 0,0 0 17 0 0,0 0 3 0 0,0 0 11 0 0,0 0 44 0 0,0 0 17 0 0,0 0 6 0 0,0 0 4 0 0,0 0 4 0 0,0 0 2 0 0,0 0 0 0 0,0 0-16 0 0,0 0-66 0 0,0 0-29 0 0,0 0-8 0 0,0 0-9 0 0,0 0-33 0 0,-1 0-25 0 0,-21 28-43 0 0,16-8 74 0 0,5-18-19 0 0,1-2 6 0 0,1-2-18 0 0,9-16-135 0 0,6 10 5 0 0,7 14-588 0 0,-17 2 664 0 0,2 16 16 0 0,-8-23 62 0 0,-5 8 297 0 0,-7-2-725 0 0,11-7 151 0 0,-9 8-801 0 0,1-8-2062 0 0,9 0 1532 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58349.811">19732 11281 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-3 420 0 0,0 3 3077 0 0,0 1 3963 0 0,-7 136-3072 0 0,-4-26-2600 0 0,-8 63-1021 0 0,8-65-304 0 0,4 23-619 0 0,7-132-213 0 0,0 0-69 0 0,0 0-12 0 0,0 0-139 0 0,0-53-6135 0 0,0 30 4451 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58689.811">19703 11320 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,1-1 21 0 0,2-2-256 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0-1 0 0,-2 1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,2 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,1 0-170 0 0,6 4 318 0 0,-2 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1-318 0 0,21 14-106 0 0,-26-19 167 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 2 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0 3-62 0 0,3 16 844 0 0,-5-16-830 0 0,2 1-1 0 0,-1-1 1 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-3 1 0 0 0,2 0-1 0 0,-2-2 1 0 0,-1 4-14 0 0,0-2 119 0 0,1-2-1 0 0,0 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,0 1-1 0 0,-1-2 1 0 0,0 1-1 0 0,-1-2 1 0 0,0-1-1 0 0,0 2 1 0 0,0-1-1 0 0,1 0 1 0 0,-2-1-1 0 0,0 0 1 0 0,0-1-1 0 0,-5 2-118 0 0,-7 5 128 0 0,18-8-128 0 0,2-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-2 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,2-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,-14-22-1234 0 0,14 3-3424 0 0,6 7-3433 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="59859.811">20211 11037 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-270 0 0,1 1 131 0 0,13 71 4572 0 0,-17-14-1957 0 0,3 6-1459 0 0,3 28-1321 0 0,-6 20-232 0 0,-4 70 0 0 0,-6-79 962 0 0,-11 12-720 0 0,24-114-750 0 0,0-1-89 0 0,0 0-360 0 0,0 0-163 0 0,-5-10-5760 0 0,1 0 563 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60069.811">20208 11531 1376 0 0,'0'0'65'0'0,"0"-2"389"0"0,27-31 11411 0 0,10-15-8036 0 0,4 18-1988 0 0,-39 29-1803 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,2 2 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-38 0 0,7 4 156 0 0,34 75 888 0 0,-37-72-884 0 0,2 1-1 0 0,-1 0 1 0 0,-2 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2 7-159 0 0,-10 85 1127 0 0,5-94-1133 0 0,1-8-6257 0 0,0-1-578 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60829.81">20784 11343 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 2 21 0 0,-8 43 177 0 0,-10 35 3194 0 0,7 29-1553 0 0,-5 89-172 0 0,-1-87-257 0 0,11-98-2469 0 0,3-12-3087 0 0,3 0-3929 0 0,0-1 1033 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61029.81">20755 11343 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,15-6-181 0 0,-12 4-54 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 2 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 2 1 0 0,2-1-1 0 0,-2 0 0 0 0,4 2-301 0 0,0 0 145 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0 1-1 0 0,-2-1 1 0 0,2 1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-3 1-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 2 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,2 2 0 0 0,-1 4-144 0 0,7 61 1883 0 0,-26 14-1742 0 0,14-84-123 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,-3 0-18 0 0,-51 3 1171 0 0,-3 13-2729 0 0,57-16 1668 0 0,-17-4-935 0 0,1-8-3444 0 0,13 5 2477 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63909.811">16587 11202 3224 0 0,'0'-1'240'0'0,"0"-1"165"0"0,0 1 1443 0 0,0 1 616 0 0,0 0 116 0 0,0-1 259 0 0,0-3-1698 0 0,1 2 2411 0 0,12-14-2439 0 0,-11 10-1053 0 0,-2-4 606 0 0,0 6-4232 0 0,0 4 2520 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190399.81">5710 11136 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,3-8 314 0 0,20-65 850 0 0,-20 60-996 0 0,1 1 0 0 0,2-1-1 0 0,-1 2 1 0 0,1 0-1 0 0,0-1 1 0 0,2 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,4 2 1 0 0,7-8-478 0 0,-17 15 40 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-40 0 0,26 51 1331 0 0,-26-50-1287 0 0,3 11 148 0 0,-2 0 0 0 0,1-3 0 0 0,-2 3 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,-1 0 0 0 0,1-2 0 0 0,-3 0 0 0 0,-1 5-192 0 0,6-15 21 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-2 1 1 0 0,2 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0-1-22 0 0,-3-2-60 0 0,1 1-1 0 0,-1-2 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,2 0 1 0 0,-1 0-1 0 0,2-1 1 0 0,-1 2-1 0 0,1-2 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-7 60 0 0,-8-51-3591 0 0,10 42 1933 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192059.811">7263 11029 4144 0 0,'0'0'319'0'0,"-11"2"1818"0"0,10-1 2461 0 0,1 0 4419 0 0,7 0-8694 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 0-323 0 0,104-53 185 0 0,-77 19-185 0 0,-30 36 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,-32-36 0 0 0,32 36 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-5 1 0 0 0,-41 17 0 0 0,40-11 47 0 0,1 0 0 0 0,0 1 1 0 0,2-2-1 0 0,-1 3 0 0 0,0-1 0 0 0,0 1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,2 1-1 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-2 0 0 0,2 10-47 0 0,2-12 52 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-2-1 0 0,0 2 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,4 4-52 0 0,-5-6 15 0 0,-1-2 0 0 0,1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 0-15 0 0,49-5-958 0 0,-37-1-1726 0 0,-3-1-3307 0 0,-5 0-1687 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="193429.81">7807 10764 10304 0 0,'0'-4'934'0'0,"0"-9"-627"0"0,0 11 320 0 0,0-3 712 0 0,-1 3 3325 0 0,0 3-4568 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 2-95 0 0,-2 5 224 0 0,1 31 664 0 0,-7 114 1598 0 0,13-73-1828 0 0,-5-40-734 0 0,-2-33-364 0 0,1 8-1982 0 0,-2-11-5617 0 0,2-5 5673 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="193879.811">7713 10860 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,1-2-294 0 0,1-2 74 0 0,-1 3 886 0 0,14-7 3459 0 0,-11 6-4230 0 0,2 0-1 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,-2 1-1 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-348 0 0,36 4 963 0 0,-20-6-540 0 0,-15 0-358 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,2 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 1 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,2 2-64 0 0,53 63 377 0 0,-54-57-1065 0 0,-5 3-3411 0 0,-1-9 774 0 0,1-2-4194 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="196929.81">5341 10901 456 0 0,'0'-16'1413'0'0,"0"15"159"0"0,0-1 76 0 0,0-41 2855 0 0,0 42-3991 0 0,0 1 0 0 0,0 0-24 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0 47 0 0,0 0 207 0 0,0 0 89 0 0,0 0 21 0 0,0 0-24 0 0,-11 5 931 0 0,8-3-1418 0 0,2 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1-182 0 0,5 87 3864 0 0,2 20-3175 0 0,-12-58 34 0 0,4 17-176 0 0,1-67-729 0 0,-4 5 3 0 0,1-5-7687 0 0,2-2-336 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="197139.81">5333 10993 11976 0 0,'0'-4'180'0'0,"1"-1"0"0"0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,2-2-180 0 0,6-4 1628 0 0,-6 6-1094 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 1 1 0 0,5-1-535 0 0,-6 1 86 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 1 0 0 0,0-1 0 0 0,2 1 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,0 1-1 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 1 0 0 0,3 3-86 0 0,22 34 302 0 0,18 36 108 0 0,-32-47-1847 0 0,-8-22-150 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170686.919">6161 10870 456 0 0,'-2'29'10790'0'0,"-6"-4"-6142"0"0,-16 80 1001 0 0,22-98-5360 0 0,-2 2-52 0 0,2 0 0 0 0,0-1-1 0 0,0 2 1 0 0,-1-2-1 0 0,2 2 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-2 1 0 0,1 7-237 0 0,8 20 1589 0 0,-1-28-1573 0 0,-6-6-16 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1-1-1 0 0,-2 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-3 0 0 0,52-79 357 0 0,-55 84-357 0 0,57-128 184 0 0,-54 88-184 0 0,-5 34-21 0 0,-6 2 2 0 0,2 4-2431 0 0,5 0 1260 0 0,-8 0-578 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-169886.919">6558 10832 2304 0 0,'0'0'428'0'0,"0"0"959"0"0,0 0 422 0 0,0 0 81 0 0,0 0-74 0 0,0 0-388 0 0,0 0-168 0 0,0 0-38 0 0,0 0-52 0 0,0 0-190 0 0,0 0-85 0 0,0 0-21 0 0,-5 13 2869 0 0,10 28-896 0 0,6 19-821 0 0,-4 31-482 0 0,15 22-8 0 0,-18-106-1420 0 0,-4-5-17 0 0,4 4 78 0 0,14 27 298 0 0,-18-32-578 0 0,0-1-4 0 0,1 1 26 0 0,5 3 65 0 0,-1 7 16 0 0,2-15 203 0 0,32-92 1554 0 0,-17 18-2314 0 0,-2 29 1122 0 0,19-33-626 0 0,-23 58-1899 0 0,-2 6 396 0 0,-8 14-8315 0 0,-6 4 2000 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-167866.919">6946 14769 1376 0 0,'0'0'65'0'0,"0"0"298"0"0,0 0 1226 0 0,-5-11 8887 0 0,3 3-10689 0 0,2 7 20 0 0,0-12-1355 0 0,0 4-2483 0 0,0 6 619 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-167696.919">6942 14740 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 10 0 0 0,-3 2 1224 0 0,3-12 232 0 0,0 0 48 0 0,0 0 0 0 0,0 0-1128 0 0,0 0-232 0 0,0 0-48 0 0,0-6 0 0 0,0 3-96 0 0,0 3-128 0 0,0 0 32 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-166746.919">6934 14720 2760 0 0,'0'0'125'0'0,"0"-12"2231"0"0,-1 1 3939 0 0,-16 48-2743 0 0,8 55-695 0 0,18 30 396 0 0,17-18-1214 0 0,11-60-933 0 0,-33-43-1072 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,2-3-34 0 0,107-160 703 0 0,-81 109-639 0 0,-9-30-572 0 0,-20 75 468 0 0,0 9-31 0 0,-7-21-455 0 0,0 10-3508 0 0,6 10-3672 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-120276.919">10548 14792 11952 0 0,'0'-1'67'0'0,"0"1"0"0"0,-1-2 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-67 0 0,-38-9 5146 0 0,40 8-5069 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,2-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 2-77 0 0,-11 8 763 0 0,6-6-634 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,1 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,0 1-1 0 0,-1-2 1 0 0,1 2 0 0 0,1-1 0 0 0,0 0-1 0 0,-1 3-128 0 0,-1 1 108 0 0,-2 11 172 0 0,-1-1 0 0 0,3 1 0 0 0,-1-1 0 0 0,2 2 0 0 0,0-1 0 0 0,2 0-280 0 0,2 60 688 0 0,22-36-159 0 0,-8-32-346 0 0,-15-11-174 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1-9 0 0,11-9 35 0 0,-2-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,1-2 0 0 0,-2 1-1 0 0,6-10-34 0 0,31-40 89 0 0,-3 6-100 0 0,-19 21-55 0 0,-24 33-4 0 0,-2-1-103 0 0,2 2-332 0 0,1 1-119 0 0,0 0-16 0 0,-2 0-596 0 0,-1 1 165 0 0,1-2-2477 0 0,2 1 1724 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-119726.919">11042 14488 12064 0 0,'0'0'553'0'0,"0"0"-16"0"0,-9 14-151 0 0,-5 31 4878 0 0,5 28-1596 0 0,2-21-2083 0 0,-7 69 353 0 0,-2 18 194 0 0,1 135-900 0 0,14-183-1248 0 0,1-89-72 0 0,0-2-51 0 0,0 0-18 0 0,0 0-158 0 0,-3-24-4130 0 0,2 7-1692 0 0,-2-1-1669 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-119476.919">10954 14759 2304 0 0,'20'-56'224'0'0,"-11"35"1777"0"0,18 3 11624 0 0,10 20-9044 0 0,10 20-2754 0 0,-1 24-1302 0 0,-9-26-2042 0 0,-29-15-78 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-166306.919">7489 14624 10136 0 0,'-11'49'1272'0'0,"9"-43"-735"0"0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1-1-1 0 0,0 2 1 0 0,2-1-1 0 0,-2-1 0 0 0,1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,1 3-538 0 0,7 26 1513 0 0,21 67 1825 0 0,8 13-1726 0 0,11-9-228 0 0,-25-65-629 0 0,-2-15-113 0 0,-21-10-556 0 0,6-23-22 0 0,13-35 0 0 0,13-46 53 0 0,17 7-396 0 0,-11 31 158 0 0,-17-11 121 0 0,-6 10 0 0 0,5-4 0 0 0,-17 42-97 0 0,-6 12-406 0 0,0 1-165 0 0,8-8-841 0 0,-2 1-1411 0 0,-3 6-6017 0 0,3 2 8141 0 0,-5 0 11 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-164976.919">8173 14958 1840 0 0,'1'4'465'0'0,"-1"3"-969"0"0,-4-2 8499 0 0,4-4-5413 0 0,0-1-959 0 0,-3 14 3293 0 0,5-12-4747 0 0,1 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0 0 0 0,2-2-1 0 0,-2 1 1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,1 0-1 0 0,0 0-168 0 0,6-2 150 0 0,0-2 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,3-4-150 0 0,7-10 74 0 0,-1 0 1 0 0,-2 0-1 0 0,0-3 1 0 0,-1 2-1 0 0,-1-2 1 0 0,8-21-75 0 0,-19 43 4 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0-4 0 0,-7 2 35 0 0,-2 0-1 0 0,2 2 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,0 0 1 0 0,1 1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2-1 0 0 0,0 2 1 0 0,0-1-1 0 0,0 1 1 0 0,2 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 2-1 0 0,1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,2 1-1 0 0,1 3-34 0 0,0-9 18 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,2 0-1 0 0,-1-2 1 0 0,-1 2-1 0 0,2-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-18 0 0,5 1-63 0 0,2 1 0 0 0,-1-2 0 0 0,0 0 0 0 0,-1 0-1 0 0,2-1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,11-2 63 0 0,-8 1-520 0 0,14-4-1481 0 0,-9 1-3720 0 0,0 1-1868 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-163966.919">8705 14498 6624 0 0,'3'19'-4'0'0,"-2"-6"534"0"0,-1 2 5466 0 0,0-15-4969 0 0,0 0-16 0 0,-7 43 3846 0 0,0 30-3228 0 0,2 1 0 0 0,5 39-1629 0 0,0-61 228 0 0,5 10-228 0 0,-5 42-16 0 0,-5-62-2758 0 0,5-29-1657 0 0,0-11 1925 0 0,0-1-3470 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-163606.919">8663 14848 10136 0 0,'23'-69'1056'0'0,"12"-14"3846"0"0,-33 78-4603 0 0,1 1 0 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,4-1-299 0 0,-5 3 72 0 0,0-1-1 0 0,1 1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 2 0 0 0,2-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,2 2-71 0 0,29 22 580 0 0,10 41 1278 0 0,-31-1-3924 0 0,-13-47-2692 0 0,-2-15 3016 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121546.919">9466 14304 5872 0 0,'0'0'266'0'0,"0"0"1"0"0,-3-11 1056 0 0,3 9 7600 0 0,-9 79-5279 0 0,9-26-2198 0 0,1 27 275 0 0,-4 1-1 0 0,-6 29-1720 0 0,-13 182 1691 0 0,18-167-981 0 0,5-111-1358 0 0,-2-19-2345 0 0,-6-50-991 0 0,2 16 1937 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121236.919">9240 14313 8752 0 0,'0'0'673'0'0,"11"7"4424"0"0,14 6-302 0 0,19-10-2564 0 0,-33-3-1654 0 0,61 1 445 0 0,-49-3-776 0 0,-1 1 0 0 0,1 1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1 1 0 0 0,11 3-246 0 0,-22-3 75 0 0,1 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1 1 1 0 0,-2 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1-75 0 0,38 47-3176 0 0,-43-44 1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-120726.919">9880 15028 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 0-276 0 0,-31 2 2318 0 0,14-7 1927 0 0,2-22-2183 0 0,18 22-2093 0 0,-2 0 0 0 0,1-1 0 0 0,1 2 0 0 0,0-2-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 2-1 0 0,0-1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,2-2-146 0 0,8-19 178 0 0,-9 17-156 0 0,1-1 1 0 0,1 1-1 0 0,1 0 0 0 0,-2 1 1 0 0,2 1-1 0 0,1-2 1 0 0,-2 1-1 0 0,3 1 0 0 0,1-3-22 0 0,-6 7 22 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1 0 0 0,3 0-22 0 0,-1 0 73 0 0,-2 1 0 0 0,2 0-1 0 0,-2 1 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1-1 1 0 0,0 2 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 0 1 0 0,0 1 0 0 0,-2-1 0 0 0,2 1-1 0 0,-1 0 1 0 0,2 1-73 0 0,10 71 976 0 0,-13-59-728 0 0,-1 1 22 0 0,-2 2 1 0 0,-1-2-1 0 0,0 0 0 0 0,0 1 0 0 0,-3 0 0 0 0,1-3 1 0 0,-3 8-271 0 0,3-9 132 0 0,1-11-108 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1-2 1 0 0,0 2-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-2-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,-2 0-24 0 0,1-2 9 0 0,1 1-1 0 0,-1-2 1 0 0,0 1 0 0 0,0-1-1 0 0,2 1 1 0 0,-2-2-1 0 0,1 1 1 0 0,-1-1 0 0 0,2 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,-3-2-8 0 0,4 3-63 0 0,1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 2 1 0 0,0-2-1 0 0,0 0 0 0 0,1 1 0 0 0,-2-4 63 0 0,2 5-278 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 2 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,2-4 278 0 0,5-7-2146 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116106.919">12255 14896 3680 0 0,'0'0'284'0'0,"0"0"17"0"0,3-5 3845 0 0,5-2 6650 0 0,-23 226-6730 0 0,17-190-3860 0 0,0-2-3590 0 0,-2-27 1760 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115556.919">12612 14786 920 0 0,'-4'10'76'0'0,"-23"26"272"0"0,-6-6 6376 0 0,5-8-722 0 0,26-21-4979 0 0,-5 7 987 0 0,3 15 528 0 0,5-5-1218 0 0,4-12-1123 0 0,1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,3 0-1 0 0,-1-1 1 0 0,-1 0 0 0 0,7 1-198 0 0,22 11 384 0 0,-31-13-322 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,0 2 0 0 0,-1-1 0 0 0,2 1 1 0 0,-2 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1-62 0 0,-2 3 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1-2 0 0 0,4 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,0-3 0 0 0,-1 1-326 0 0,-14-19-857 0 0,16 2-6482 0 0,3 11 584 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-117286.919">11613 14412 10824 0 0,'0'0'241'0'0,"0"7"331"0"0,-6 105 4121 0 0,-2 8-200 0 0,1-17-2317 0 0,-4 57-880 0 0,11 65-5334 0 0,0-224-1053 0 0,0-1-1451 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116916.919">11968 14428 2760 0 0,'-19'-15'247'0'0,"16"14"193"0"0,2 1 1710 0 0,-1 3 4946 0 0,-4 8-4369 0 0,4-5-1946 0 0,-28 37 1201 0 0,37-2-671 0 0,-29 121 670 0 0,-25 95 167 0 0,10-123-2609 0 0,30-119-2025 0 0,3-7-2648 0 0,-1 1-1568 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116696.92">11550 14809 9672 0 0,'0'0'748'0'0,"1"1"-492"0"0,3 3-231 0 0,-3-2 331 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 0-356 0 0,110 16 3649 0 0,-108-15-4114 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,4 4 465 0 0,10 8-1693 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-110456.919">14067 14762 1840 0 0,'0'2'133'0'0,"0"7"1371"0"0,-8 14 9957 0 0,3-11-10918 0 0,0 10 2807 0 0,4-14-2599 0 0,1-7-23 0 0,0-1-45 0 0,0 3-163 0 0,-7 41 1090 0 0,-8 98 530 0 0,11-18-1604 0 0,8-88-486 0 0,-4-34-216 0 0,0-2-402 0 0,0 0-174 0 0,5-17-2600 0 0,-2 6 1430 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-110046.919">14041 14941 4144 0 0,'0'0'319'0'0,"0"0"75"0"0,-2-4 5801 0 0,0-1-4842 0 0,2-5-34 0 0,10-35 4642 0 0,7 32-3827 0 0,27-1-548 0 0,-7 20-1696 0 0,-32-6 128 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1-18 0 0,35 8 0 0 0,-24-7 0 0 0,-9-1 0 0 0,8 10 0 0 0,-2 11-870 0 0,-15-21 616 0 0,2-2-383 0 0,0 1-179 0 0,-13 33-4440 0 0,12-31 3346 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-112086.92">13060 14458 3224 0 0,'0'0'143'0'0,"0"2"-3"0"0,-1-2 1084 0 0,-4 10-2538 0 0,2-8 6295 0 0,1-2 6252 0 0,3 16-9469 0 0,9 55 352 0 0,-24 132-1892 0 0,9-118 559 0 0,2-58-682 0 0,2-1 0 0 0,0 0 0 0 0,2 0 0 0 0,1 1 0 0 0,1 0-101 0 0,4 27-450 0 0,-11-46-56 0 0,1-6-6442 0 0,3-2 4901 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111836.919">13042 14624 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 0 21 0 0,3 0-42 0 0,107-19 3931 0 0,-43 8-2346 0 0,-40 15-4175 0 0,-19 3 964 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111476.919">13411 15004 7744 0 0,'0'0'356'0'0,"0"0"-8"0"0,0 0-63 0 0,0 0 571 0 0,-3 9 4563 0 0,-15-46-211 0 0,24-31-2906 0 0,28 41-1872 0 0,-15 14-315 0 0,-15 12-110 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 1-4 0 0,-1 1 59 0 0,2 0-1 0 0,-2 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,-2 0-1 0 0,2 1 1 0 0,-1-1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-2 1-59 0 0,2-4 22 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 0 0 0,2-1 1 0 0,0 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-23 0 0,-34 5 210 0 0,2-34-185 0 0,15 6-523 0 0,13-5-2557 0 0,8 16 1503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111056.919">13785 14795 8288 0 0,'2'16'273'0'0,"-1"-32"1643"0"0,-1 16-472 0 0,0 0 76 0 0,0 0-55 0 0,0 0-287 0 0,0 2-123 0 0,-7 43 4957 0 0,-8-1-5210 0 0,14 91 812 0 0,6-39-1951 0 0,-5-90-1422 0 0,0-5-625 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-109556.919">13664 14562 8752 0 0,'22'16'1346'0'0,"-22"-14"-166"0"0,2-2-1575 0 0,3-4 4378 0 0,3-4 4520 0 0,3 1-11521 0 0,-6 3 1866 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-106806.919">14564 15024 6912 0 0,'79'11'8898'0'0,"-74"-10"-8618"0"0,1-1-1 0 0,0 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 0-1 0 0,-1 1 1 0 0,3-4-280 0 0,35-49 1321 0 0,-40 50-1321 0 0,0 1 1 0 0,1-1-1 0 0,0 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0-2-1 0 0,-19-33-90 0 0,15 38 124 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-34 0 0,-56 23 664 0 0,53-19-600 0 0,0 2 0 0 0,0-1 0 0 0,1 1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,2 1 0 0 0,-1-2 0 0 0,0 2 0 0 0,0 2-64 0 0,1 0 41 0 0,1 1 0 0 0,0-2 0 0 0,1 2 1 0 0,-1 0-1 0 0,2-1 0 0 0,1 2 0 0 0,-1-2 0 0 0,2 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,2 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,4 7-41 0 0,-4-10 98 0 0,2-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,5 6-98 0 0,-6-11 5 0 0,-1 0 0 0 0,2 0 0 0 0,-2-2 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 0-5 0 0,2-1-54 0 0,110-32-5788 0 0,-65 9 1619 0 0,-24 11 2079 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-102656.919">16086 14873 1840 0 0,'0'0'83'0'0,"0"0"169"0"0,0 0 668 0 0,0 0 288 0 0,0 0 58 0 0,0 0-22 0 0,0 0-144 0 0,0 0-63 0 0,0 0-11 0 0,0 0-2 0 0,0 8 2048 0 0,-3 18-266 0 0,2-2-362 0 0,1 76 1520 0 0,-3-31-3723 0 0,2 17-415 0 0,2-78 488 0 0,5 5-6100 0 0,0-7-783 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-102316.919">16091 15024 10136 0 0,'21'-55'5082'0'0,"10"10"-1747"0"0,-6 27-1698 0 0,-22 15-1500 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,2 0 1 0 0,0 0-137 0 0,1 1 60 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 1 0 0,-2-1-1 0 0,1 2 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 1 1 0 0,-1-2-1 0 0,2 2 0 0 0,-2 0 0 0 0,1 3-60 0 0,17 16 54 0 0,-6-14-897 0 0,-11-8-100 0 0,-1-1-37 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-104576.919">15247 14284 2304 0 0,'0'0'101'0'0,"0"0"294"0"0,0 0 1149 0 0,0 0 506 0 0,0 2 1554 0 0,0 9-1838 0 0,2 143 6571 0 0,-2 114-5024 0 0,-14-8-1402 0 0,10-160-1693 0 0,-6-27-376 0 0,9-72-114 0 0,1-1-766 0 0,-5-11-2968 0 0,-2-1-3447 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-104236.919">15220 14479 920 0 0,'0'-1'67'0'0,"-3"-7"403"0"0,4 0 4358 0 0,4-5-1924 0 0,-4 10-1691 0 0,20-31 4007 0 0,25-4-3052 0 0,7 6-888 0 0,-32 24-1087 0 0,-18 7-85 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 1-108 0 0,1 0 199 0 0,-2 1 0 0 0,2-1 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1-1 0 0,2 1 1 0 0,-2-1 0 0 0,4 4-199 0 0,30 58 460 0 0,-28-39-231 0 0,0 2 1 0 0,-2 0-1 0 0,-2-1 0 0 0,0 2 1 0 0,-2-2-1 0 0,0 1 0 0 0,-3 26-229 0 0,0-46 147 0 0,-2 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 1 0 0,-2 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1-1 1 0 0,-1 1-1 0 0,2-1 0 0 0,-4 3-146 0 0,4-7 10 0 0,-2 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-4-2-10 0 0,-4-2-494 0 0,1-1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1-1 1 0 0,2 1-1 0 0,0-2 1 0 0,0 0-1 0 0,-4-5 495 0 0,4 0-5994 0 0,3-4-1719 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-103406.919">15645 15024 8288 0 0,'0'0'190'0'0,"5"-6"253"0"0,9-6-212 0 0,30 1 5159 0 0,2 6-1205 0 0,-17 13-2607 0 0,-5-3 202 0 0,-15-3-715 0 0,-16-5-592 0 0,-40 8 113 0 0,-39 16 500 0 0,81-19-1076 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 0 0 0 0,2 2 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-2 0 0 0,0 3-10 0 0,-2 6 2 0 0,0-6-2 0 0,2 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-2 0 0 0,3 7 0 0 0,13 14 0 0 0,-17-25 1 0 0,2 2 37 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1-2 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,1-1 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,1 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,3-1-39 0 0,48-28 241 0 0,-41 15-275 0 0,-1 2 0 0 0,1-3 0 0 0,-2-1 0 0 0,-1 2 0 0 0,0-3 0 0 0,-1 2 0 0 0,0-2 34 0 0,13-68-964 0 0,-15 34 382 0 0,-19 87 634 0 0,11-24-10 0 0,1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,3-2-1 0 0,-1 2 1 0 0,4 6-42 0 0,15 45 54 0 0,-9-43-1794 0 0,-7-20 730 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-98716.919">16757 14395 3224 0 0,'0'0'143'0'0,"0"0"279"0"0,0 0 1073 0 0,0 0 470 0 0,0 0 92 0 0,0 0-154 0 0,0 0-730 0 0,0 0-315 0 0,0 7 684 0 0,-3 1-898 0 0,3-6-48 0 0,0 7 1051 0 0,-8 45 1551 0 0,-37 294 1366 0 0,41-324-4246 0 0,3 2 0 0 0,0-1-1 0 0,2 0 1 0 0,0 1 0 0 0,3 0-1 0 0,-1-3 1 0 0,2 3-1 0 0,6 16-317 0 0,23 16 208 0 0,-32-53-186 0 0,1-2 0 0 0,1 2 0 0 0,-1-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2-2-1 0 0,1 2 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-2-2 1 0 0,2 1 0 0 0,0-1 0 0 0,-2 1-1 0 0,2-1 1 0 0,3 0-22 0 0,-5-2 31 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-2-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-2-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0-1-30 0 0,-2 5 3 0 0,10-17 55 0 0,-2 1 1 0 0,0-2-1 0 0,0 1 0 0 0,-1 0 0 0 0,3-18-58 0 0,6-16 41 0 0,23-95-41 0 0,16-143-432 0 0,-49 253-57 0 0,-2 7-2509 0 0,-1 9-4848 0 0,-1 11 100 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-97336.919">17921 14907 2304 0 0,'0'0'101'0'0,"0"17"22"0"0,-8 5 6125 0 0,-3 17 4249 0 0,9-9-9080 0 0,-3 85 316 0 0,1-83-1477 0 0,0-19-426 0 0,3-12-721 0 0,1-1-329 0 0,0 0-75 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-96826.919">18180 14458 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 2-242 0 0,5 69 6774 0 0,-10 3-1144 0 0,-8 41-2340 0 0,2 48-2718 0 0,6-9-705 0 0,0 15-1521 0 0,5-159 244 0 0,0-8-61 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-96436.919">18445 14875 10136 0 0,'0'0'777'0'0,"-1"2"-505"0"0,-3 41 4407 0 0,3-11-457 0 0,3 76-789 0 0,-4-100-3589 0 0,2 0-1781 0 0,0-7 758 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95846.919">18878 14863 1376 0 0,'1'-2'299'0'0,"13"-56"5252"0"0,-16 42-5059 0 0,1 12-375 0 0,1 3 35 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,1-1-152 0 0,-4 1 283 0 0,1 0 0 0 0,1 1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-2 1 0 0 0,2-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 1-285 0 0,-9 12 754 0 0,-46 63 501 0 0,34-6-220 0 0,24-66-992 0 0,-1-1-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,2 0 1 0 0,-2 0-1 0 0,5 3-41 0 0,1 6 59 0 0,8 8 178 0 0,-13-19-112 0 0,-1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0-125 0 0,-14 16 28 0 0,10-19-9 0 0,0 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2-2 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1-19 0 0,-39 2-215 0 0,7 20-3705 0 0,33-14-4023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95136.919">19221 14958 3680 0 0,'0'0'284'0'0,"0"0"109"0"0,2-1 1154 0 0,30-17 5762 0 0,36 17-2771 0 0,-36 11-2764 0 0,-17 0 1490 0 0,-63-16-3312 0 0,43 4 32 0 0,1 1 0 0 0,-2 0 1 0 0,0 0-1 0 0,2 1 1 0 0,-2-1-1 0 0,2 1 0 0 0,-2 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 1 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 1 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,-2 3 16 0 0,0-1 34 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 0 0 0,1 2 1 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,-1 3-33 0 0,4-7 57 0 0,1 0-1 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,2 2-56 0 0,-2-4 45 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 1 0 0,2-1-1 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1-45 0 0,103-151-3426 0 0,-105 155 3373 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,2-1 0 0 0,-2 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 53 0 0,-2 20 337 0 0,-17 78 1575 0 0,11 7-1206 0 0,16-62-7272 0 0,-5-33-749 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-98036.919">17596 14346 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 2 76 0 0,-5 11 2311 0 0,-8 36 3900 0 0,-2 112-3759 0 0,-18 84 806 0 0,3 40-2464 0 0,22-197-1627 0 0,8-87-756 0 0,-3-6-2095 0 0,3-4 1602 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-97796.919">17511 14618 11232 0 0,'-4'-28'1016'0'0,"5"28"-836"0"0,14-28 2777 0 0,66 23 2000 0 0,18 19-1797 0 0,-55 6-4345 0 0,-36-16-189 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93526.919">20179 15031 15664 0 0,'14'5'1187'0'0,"-11"-4"-976"0"0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 1 0 0,1 1-1 0 0,-2-1 0 0 0,1 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,2-1 1 0 0,-2 1-1 0 0,1-2-210 0 0,8-12-211 0 0,-4 9-129 0 0,-2-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,0-1 0 0 0,0 2 0 0 0,2-10 340 0 0,-9-34-1540 0 0,4 51 1562 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-2 1 0 0 0,2-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-22 0 0,-22 17 1568 0 0,19-13-1383 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,1-1 0 0 0,0 1-185 0 0,-7 31 308 0 0,5-27-103 0 0,1 2 0 0 0,0-2-1 0 0,0 1 1 0 0,1 1 0 0 0,1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,2 0 0 0 0,-1 2-205 0 0,16 19 1394 0 0,-17-33-1436 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 0 0 0 0,-2 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0 42 0 0,0-1-47 0 0,96-58-5723 0 0,-83 50 4417 0 0,-4 1-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94286.919">19741 14713 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0-6 199 0 0,4-20 284 0 0,-4 26 22 0 0,0 0 21 0 0,0 0 53 0 0,0 0 198 0 0,0 0 86 0 0,0 0 21 0 0,0 0-28 0 0,0 0-122 0 0,-11 86 4045 0 0,3-21-3014 0 0,-22 176 836 0 0,14-106-2456 0 0,14-119-5049 0 0,1-15-3688 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94056.92">19719 14830 19351 0 0,'0'0'439'0'0,"0"0"62"0"0,0 0 33 0 0,0 0-65 0 0,7-3-292 0 0,98-18 2799 0 0,-42 10-2385 0 0,-23 8-4619 0 0,-38 3 2335 0 0,-2 0-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-89026.919">20577 14917 920 0 0,'0'0'115'0'0,"0"0"146"0"0,0 0 68 0 0,2-1 14 0 0,12-24-975 0 0,0 11 771 0 0,-13 12 195 0 0,-1 2 149 0 0,0 0 590 0 0,0 0-1059 0 0,7-7 9846 0 0,-2 4-8006 0 0,-4 1-1530 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1-1-324 0 0,1-1 1337 0 0,0 4-893 0 0,-10 8-200 0 0,-32 57 2244 0 0,14 4-1504 0 0,26-15-648 0 0,2-53-335 0 0,1 7 28 0 0,0-1-1 0 0,1 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,2 0 0 0 0,-2-1-1 0 0,1 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,1 0-1 0 0,1 1-28 0 0,-2-3 14 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-2 0 0 0,4-1-13 0 0,35-21 64 0 0,-3-45 8 0 0,-17-10-72 0 0,-17 41-89 0 0,2-53-263 0 0,-10 91 324 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 29 0 0,-4 9-8024 0 0,2 0 350 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88466.92">21090 14792 2304 0 0,'0'0'101'0'0,"0"0"363"0"0,0 0 1439 0 0,0 0 626 0 0,0 0 126 0 0,0 0-194 0 0,3-13 1239 0 0,0 22 4485 0 0,-1 45-5205 0 0,-7 22-1571 0 0,2 34-565 0 0,-5-50-599 0 0,9 95 126 0 0,6-99-812 0 0,6-128-3199 0 0,-11 24-1172 0 0,-2 35 2865 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88226.92">21098 14932 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-150 0 0,-8-5 3377 0 0,18-30 352 0 0,36-15-1964 0 0,-39 47-2182 0 0,-4 1 153 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,4 1-123 0 0,37 11 165 0 0,-9 22-245 0 0,-10 20-3497 0 0,-24-52-1940 0 0,-1-2-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86216.919">21772 14762 9416 0 0,'-2'-4'852'0'0,"-25"-9"284"0"0,16 11 6835 0 0,-12 30-4820 0 0,19-19-2774 0 0,-53 123 2838 0 0,26-37-1934 0 0,22-68-1118 0 0,2-2 0 0 0,1 3-1 0 0,1-1 1 0 0,1 0 0 0 0,2 0 0 0 0,1 1-1 0 0,0-2 1 0 0,3 8-163 0 0,-2-17-6 0 0,15 114-229 0 0,4-75-1218 0 0,-1-36-2030 0 0,-11-14-2522 0 0,-6-5-1562 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85956.919">22134 14717 11520 0 0,'0'0'886'0'0,"1"-1"-582"0"0,17 6 5156 0 0,-13-1-5008 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 2 1 0 0,0 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 5-452 0 0,6 12 803 0 0,7 60 1048 0 0,-12-35-1193 0 0,-4 49 394 0 0,-5 9-300 0 0,-12 6-403 0 0,-14 44-253 0 0,2-46-2616 0 0,-9-3-4080 0 0,20-60-2023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-80646.919">2552 13338 2760 0 0,'-23'-10'247'0'0,"11"-3"39"0"0,11 13 290 0 0,-4-1-375 0 0,3-4 6201 0 0,1-1-5440 0 0,13 4 7229 0 0,-6 2-9038 0 0,103 43 4699 0 0,-31-7-2217 0 0,54-16-519 0 0,51 0-182 0 0,-22 27-394 0 0,-133-35-455 0 0,-4-1-32 0 0,1-1 0 0 0,0 0-1 0 0,-1-2 1 0 0,2-1-1 0 0,0 0 1 0 0,0-2-1 0 0,1-1 1 0 0,-1-2-1 0 0,1 0 1 0 0,7-2-53 0 0,158-29 1189 0 0,101-36-261 0 0,-105 43-928 0 0,-158 20 0 0 0,316-2 0 0 0,-26 31 15 0 0,28-10 250 0 0,14 11-174 0 0,-131-11 135 0 0,-11 4-42 0 0,132 18-48 0 0,-239-28-125 0 0,89 12 42 0 0,212 32 22 0 0,130 2 393 0 0,-222-18-403 0 0,378 58 135 0 0,-287-57-200 0 0,-53 1-61 0 0,-56-1 141 0 0,8 3-80 0 0,-109-22 0 0 0,84-1 0 0 0,171 5 0 0 0,-190-4 0 0 0,77-9 0 0 0,201-21 0 0 0,-320 10 0 0 0,-36 5 0 0 0,332-3 0 0 0,-286-12 0 0 0,437-12-9 0 0,-344 2 914 0 0,-19-9-1376 0 0,71 4 966 0 0,-87 29-599 0 0,-8 4-152 0 0,-143 2 112 0 0,-4 6 239 0 0,4-4 314 0 0,61 6-541 0 0,33-15-88 0 0,3-7 252 0 0,-122-4-160 0 0,211-26 128 0 0,-70-1 0 0 0,-48 7 11 0 0,10-2-22 0 0,127 6 11 0 0,-36 4 80 0 0,122 6-133 0 0,-167 16 42 0 0,207-16 11 0 0,-138 9 0 0 0,45 0 0 0 0,338 25 139 0 0,-143-28-86 0 0,-345 21 75 0 0,-19-2-128 0 0,-91-19 0 0 0,-9-8 148 0 0,27-13-132 0 0,-45 16-28 0 0,73 15 12 0 0,-54 6-96 0 0,-105-8 80 0 0,-11 3 5 0 0,-12 12-319 0 0,20-3 154 0 0,11 7-187 0 0,-9 4 347 0 0,0 58 16 0 0,-6 84 15 0 0,14 157 28 0 0,0-114-101 0 0,19 26 233 0 0,-5-4-91 0 0,-5 19-20 0 0,-29-44 106 0 0,-5-60-95 0 0,0-20-75 0 0,0 16 0 0 0,0-27 224 0 0,-7-28-160 0 0,15-81-64 0 0,1-2 0 0 0,-1 1 0 0 0,0-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-3 0 0 0 0,-17 8 0 0 0,3-8 0 0 0,-321 7 96 0 0,116-13-96 0 0,-246 3 0 0 0,58 3 71 0 0,-125 7-86 0 0,-159-20 71 0 0,45 0-136 0 0,61 4 80 0 0,94-1 0 0 0,-387-10 0 0 0,163 0 68 0 0,202 8 268 0 0,287 9-440 0 0,-610-17 204 0 0,283-18-164 0 0,114 4 77 0 0,-395-1 78 0 0,343 12-91 0 0,-3-16 0 0 0,25 5 0 0 0,97 15 0 0 0,81 9 0 0 0,-233 7 0 0 0,227 4 0 0 0,-873-1 0 0 0,303-45 0 0 0,322 8 0 0 0,-134-9 0 0 0,453 21 0 0 0,1-9 0 0 0,-76-9 0 0 0,184 29 0 0 0,0 5 0 0 0,-114 10 0 0 0,34 9 0 0 0,15 0 0 0 0,-40-10 0 0 0,24-12 0 0 0,-22 2 0 0 0,-182-3 0 0 0,193 17 0 0 0,-33-14 0 0 0,64 4 0 0 0,163 4 0 0 0,-132 7 0 0 0,-68-7 0 0 0,114-8 0 0 0,-54-10 0 0 0,63 10 0 0 0,-90 4 0 0 0,120-3 0 0 0,-80-1 0 0 0,50-4 0 0 0,92 10-60 0 0,5 1-252 0 0,1 0-111 0 0,0 0-1358 0 0,0 0-5615 0 0,0 0-2407 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-74756.919">2545 13229 1376 0 0,'0'0'65'0'0,"0"1"-6"0"0,0 16 154 0 0,0-15 831 0 0,0-2 358 0 0,0 0 65 0 0,0 0-83 0 0,0 0-422 0 0,0 0-186 0 0,0 0-38 0 0,0 0-28 0 0,0 0-88 0 0,0 0-40 0 0,0 0-6 0 0,0 0 2 0 0,0 0 12 0 0,0 0 2 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0-1 0 0,0 8 1801 0 0,7 103 2520 0 0,1-8-2608 0 0,3 111-760 0 0,-11-2-472 0 0,39 55-113 0 0,-33-230-854 0 0,24 98-208 0 0,-2 67 1907 0 0,-14-79-2238 0 0,19 168 898 0 0,-37-179-286 0 0,-54 138-20 0 0,51-153-169 0 0,7-49-56 0 0,-3 9 374 0 0,-15 49-182 0 0,17-22-546 0 0,9-13 992 0 0,4-1-446 0 0,-10-64-106 0 0,0-5-17 0 0,-2-1-234 0 0,-7-18-3530 0 0,7 9 2303 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151003.08">2638 7365 4144 0 0,'0'0'319'0'0,"-6"1"252"0"0,6-2 2376 0 0,25-31-2360 0 0,-30 15 5029 0 0,5 16-5505 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-2 1 1 0 0,2-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 1 0 0,-2 1-112 0 0,-54 22 1284 0 0,16 1-659 0 0,-31 35 50 0 0,19-10-590 0 0,-100 121 107 0 0,50-41-21 0 0,6 2 334 0 0,15-6-252 0 0,-18 47-182 0 0,-57 140 566 0 0,141-276-548 0 0,-62 172 254 0 0,2 97-151 0 0,40-56 504 0 0,15-105-216 0 0,8 103 134 0 0,10-132-457 0 0,-3 106 104 0 0,14-111-187 0 0,6 1-1 0 0,16 57-73 0 0,5-9 269 0 0,28 64-269 0 0,-6-39 164 0 0,18 64 46 0 0,-16-72 888 0 0,67 134-1098 0 0,17 33 320 0 0,-100-229-133 0 0,24 44 186 0 0,-3-45 46 0 0,18 56-249 0 0,-14-25-191 0 0,-22-54 21 0 0,25 52 139 0 0,-38-56-22 0 0,-29-77-141 0 0,-4-7-107 0 0,0-2-69 0 0,0 0-21 0 0,0-3-260 0 0,0-9-1082 0 0,-4-4-465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151703.08">1900 12924 13824 0 0,'-55'23'1677'0'0,"53"-22"-740"0"0,30-3 3060 0 0,6 0-4365 0 0,78 35 323 0 0,1 33 373 0 0,-11 8 165 0 0,123 101 1071 0 0,-198-158-1495 0 0,-1-2-1 0 0,1-2 0 0 0,0-1 0 0 0,3 0 1 0 0,22 5-69 0 0,72 11 245 0 0,-56-21 458 0 0,-53-17 147 0 0,-14 8-799 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 2-1 0 0,-1-1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-2-51 0 0,0-4 176 0 0,-22-110 411 0 0,-21-83-1189 0 0,0 63-4384 0 0,23 86 2801 0 0,-5 9-21 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="152993.08">2853 13293 2760 0 0,'-8'-3'248'0'0,"-37"-30"6865"0"0,26 5-6498 0 0,-15-20 774 0 0,-3-5 1367 0 0,2-27 825 0 0,8 6-1573 0 0,19 18-676 0 0,-1-14-560 0 0,12-73 1085 0 0,20 4-1137 0 0,-13 90-1006 0 0,-13 6-1132 0 0,0 7-1456 0 0,5 34 1591 0 0,3 0-48 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="154173.08">5186 10046 14976 0 0,'-27'21'1597'0'0,"-13"-8"-1817"0"0,39-13 85 0 0,1 0-121 0 0,-9-1-614 0 0,-4-21 1632 0 0,4-14 143 0 0,-9-55 2063 0 0,-1-14-936 0 0,1-80-705 0 0,13-24-328 0 0,1 22-897 0 0,2-162 234 0 0,0-25 12 0 0,10 194-193 0 0,-1-120-36 0 0,-9 150-1315 0 0,30 87-2477 0 0,-19 50 2086 0 0,1-14-2513 0 0,-9 23 1999 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="154583.08">4458 8026 18887 0 0,'0'0'863'0'0,"-1"-1"-14"0"0,1-12-806 0 0,-1 2-1 0 0,2 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,2-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,1-1 0 0 0,-1 3 1 0 0,1-2-1 0 0,2-1-42 0 0,-2 0-42 0 0,134-197-129 0 0,-67 108 171 0 0,31-2 0 0 0,-92 93 2 0 0,-2 0-1 0 0,1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 0 1 0 0,1 2-1 0 0,0-1 0 0 0,7 0-1 0 0,-12 5 48 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 2 1 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-2 0 1 0 0,1 1 0 0 0,0 0-1 0 0,-2 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-2 1 0 0 0,1-1-1 0 0,-1 2-47 0 0,79 209 1312 0 0,-21-36-1200 0 0,-30-60-32 0 0,-2-31-402 0 0,5-39-2524 0 0,-24-46 814 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="156043.08">2450 14790 13040 0 0,'-3'6'1185'0'0,"-26"30"-737"0"0,2-29 563 0 0,-34-20 2664 0 0,27-4-2667 0 0,-42-17 867 0 0,39 15-1425 0 0,0 1 0 0 0,2-4 0 0 0,0-2-1 0 0,2 1 1 0 0,-15-16-450 0 0,-183-168 1230 0 0,197 171-981 0 0,-32-27-91 0 0,4-5 0 0 0,4-2 1 0 0,-4-9-159 0 0,-141-215 786 0 0,-96-173 150 0 0,196 259-915 0 0,12-4 1 0 0,7-4-1 0 0,-6-58-21 0 0,-69-193 160 0 0,73 173-160 0 0,-51-190-216 0 0,82 253 184 0 0,10-2 0 0 0,3-63 32 0 0,3-70-64 0 0,10 67 0 0 0,17 182 64 0 0,5-2 0 0 0,7-106 0 0 0,3 162 0 0 0,6-73 0 0 0,21-93 0 0 0,29-109-80 0 0,59-143-171 0 0,-8 148-223 0 0,-17 94 455 0 0,-52 150 70 0 0,6 3 0 0 0,2 2-1 0 0,10-7-50 0 0,-25 41 25 0 0,88-112 30 0 0,45-1-129 0 0,10 30-44 0 0,37-36-58 0 0,-164 127 134 0 0,87-62-842 0 0,-137 104 868 0 0,27-14-1611 0 0,-14 11-5936 0 0,-12 3 272 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="156463.08">1538 5857 11976 0 0,'0'0'922'0'0,"-1"-2"-600"0"0,-8-9-54 0 0,8 10 932 0 0,-1-8 2652 0 0,0-5-2353 0 0,6 11-1499 0 0,-1-2-1 0 0,1 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,1 1 0 0 0,2-1 1 0 0,19-11-106 0 0,99-29-209 0 0,-114 38 308 0 0,0 0-1 0 0,1 2 1 0 0,0-1-1 0 0,-1 1 1 0 0,2 1-1 0 0,-1 0 1 0 0,-1 1-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 2-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,2 1-1 0 0,-2 0 1 0 0,0 0-1 0 0,0 0 0 0 0,7 6 8 0 0,-8-3 12 0 0,0 1 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-2 0 0 0,-1 3-1 0 0,0-1 1 0 0,5 10-12 0 0,-4-4 37 0 0,0 2 0 0 0,-1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-3 1 1 0 0,4 16-38 0 0,-4 85 434 0 0,-31-12 5 0 0,14-74-354 0 0,-51 118 75 0 0,-68 116-1810 0 0,119-243 551 0 0,-1 0-48 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="157893.08">9277 5655 13360 0 0,'-5'-1'271'0'0,"2"0"1"0"0,-2 0 0 0 0,1 0-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-2 1 0 0,0 1-272 0 0,-1-3 27 0 0,1 1 0 0 0,0-1 0 0 0,1 2-1 0 0,0-2 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1-4-27 0 0,-1-7 302 0 0,-11-125 1863 0 0,-7-4-421 0 0,-6-144 624 0 0,6 51-1161 0 0,-13-343-614 0 0,24 336-593 0 0,-1 77-104 0 0,8 163 61 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0-1 43 0 0,2 8-62 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 62 0 0,-8 15-1775 0 0,2 4-289 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="158203.08">8509 3407 22607 0 0,'0'0'514'0'0,"-1"-2"71"0"0,-2 0-530 0 0,2 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1-55 0 0,13-16-19 0 0,0-2-1 0 0,-1 3 0 0 0,3-2 1 0 0,0 3-1 0 0,-1 0 1 0 0,3 0-1 0 0,-1 1 0 0 0,3 2 1 0 0,-1 0-1 0 0,3-1 20 0 0,24-19-44 0 0,-38 26-32 0 0,0 1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 2 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0-1 0 0,0 2 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 1 76 0 0,-5 2-16 0 0,-1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-2 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-2 0 0 0 0,1-1-1 0 0,0 2 1 0 0,0 0 16 0 0,56 136 542 0 0,-32-88-361 0 0,1-1 0 0 0,4-1 1 0 0,17 24-182 0 0,44 46-220 0 0,-50-63-1394 0 0,-22-36-78 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2253,42 +2265,42 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">5678 3769 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-8 0 710 0 0,-57 11 2232 0 0,-87-9 113 0 0,65-16-2111 0 0,82 11-1711 0 0,2 1 0 0 0,0 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0-7 0 0,0 0 3 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,-2-1-3 0 0,-4-1 53 0 0,-47 16 746 0 0,-3-34-422 0 0,-40 20 95 0 0,18 18-267 0 0,-2-27 255 0 0,17 6-262 0 0,-8-5 515 0 0,23 24-785 0 0,-7-11 316 0 0,59-3-237 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 1 0 0 0,0-2 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,1 5-384 0 0,-1 0-2483 0 0,0-5 1589 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">4643 3507 12384 0 0,'-12'-11'1277'0'0,"-1"9"-438"0"0,-12 9 3998 0 0,7 3-3431 0 0,-18 14 690 0 0,-43 37-1014 0 0,22-27 402 0 0,6 18-1322 0 0,28-24-154 0 0,-8 14 872 0 0,29-39-855 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,2-1-1 0 0,0 2 1 0 0,0-2 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-2-1 0 0,3 3-23 0 0,31 38 389 0 0,-24-33-394 0 0,-1-2 1 0 0,2 0-1 0 0,0-1 0 0 0,0-1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1-2 0 0 0,1 0 0 0 0,-1-1 1 0 0,1-1-1 0 0,4 0 4 0 0,-4 0-173 0 0,87 19-1371 0 0,-36 1-4118 0 0,-48-15-1845 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="2">3938 2858 2760 0 0,'7'14'125'0'0,"-19"-7"1798"0"0,-5 10-59 0 0,13-10 428 0 0,-20 6 4862 0 0,24-13-6578 0 0,0 0-15 0 0,0 0-34 0 0,-2 2 119 0 0,1-1-159 0 0,1-1 2989 0 0,47-16-1901 0 0,9 9-396 0 0,17 3-749 0 0,-18 1 156 0 0,34-1 469 0 0,18-5-497 0 0,-3-2-454 0 0,46-3 952 0 0,-44 8-543 0 0,-43-4-402 0 0,45-9 402 0 0,-58 7-745 0 0,4 12 112 0 0,-30-6 120 0 0,14 4 0 0 0,6-13 444 0 0,-21 4-280 0 0,11 0-164 0 0,-21 3 0 0 0,-4 7 0 0 0,15 7-1208 0 0,-23-5 877 0 0,5 3-1583 0 0,8 12-3659 0 0,-8-10 3847 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="3">5204 2402 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,8 22 9129 0 0,19-4-7935 0 0,-14-13-2328 0 0,51 29 1337 0 0,-51-23-2420 0 0,-5-5 346 0 0,1 0 1 0 0,-1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,3 9-255 0 0,6 66 1080 0 0,-23-5-224 0 0,-9-28-856 0 0,-24-2 327 0 0,-24-10 1242 0 0,8-16-2553 0 0,31-23-3117 0 0,21-1 2058 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="4">10723 2919 8288 0 0,'9'-47'864'0'0,"-10"44"-720"0"0,2-9 1811 0 0,1 9 5703 0 0,52-2-3242 0 0,-20 5-4222 0 0,66 2 1838 0 0,5 8-1085 0 0,231-13 1101 0 0,-146-1-1030 0 0,-64 8-540 0 0,34-1-45 0 0,11-13 803 0 0,-40-21-1236 0 0,-127 29-64 0 0,-4 2-273 0 0,20-11-2694 0 0,-18 11 2502 0 0,6 0-15 0 0,-3 5-3511 0 0,-2 1-4432 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="5">12221 2484 8288 0 0,'0'0'638'0'0,"-1"1"-414"0"0,-1 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,6 6 488 0 0,57 15 2067 0 0,-34-13-2223 0 0,43 21 954 0 0,-46-9-1577 0 0,36 39 370 0 0,-15 1-375 0 0,25 32 240 0 0,-69-89-712 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 2-23 0 0,-2 3 44 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1-1 0 0 0,1 0-44 0 0,-23 11 59 0 0,0-3-1 0 0,0 0 1 0 0,-1-2 0 0 0,0-3-1 0 0,0-1 1 0 0,-15 0-59 0 0,25-5-59 0 0,-63-10-1395 0 0,76 4-1171 0 0,8 5 1267 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="6">13160 2603 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-10 7 790 0 0,-11 10 150 0 0,-42 21 1099 0 0,5-4-1196 0 0,56-32-1165 0 0,-12 9 158 0 0,1 0 0 0 0,0 1-1 0 0,1 1 1 0 0,0 1 0 0 0,1-1 0 0 0,0 2 0 0 0,1 0 0 0 0,0 1-1 0 0,-5 11-202 0 0,13-22 65 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1-1 0 0,1 1 1 0 0,1-1-1 0 0,-1 2 1 0 0,1-1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1-64 0 0,1 2 108 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,0-1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,8 2-107 0 0,-4-1 42 0 0,-1-2-1 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 0 0 0,6-3-41 0 0,20-17-4007 0 0,-30 14-3607 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="7">13318 2943 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-4-9 655 0 0,4 3-930 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,2-1-345 0 0,-4 2 74 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-2 0 0 0,0 2 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0-1 0 0,1 2 1 0 0,1-2 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 2-73 0 0,1 5 95 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 9-95 0 0,-11 70 1049 0 0,11-81-938 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-111 0 0,2-3 23 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,2-1 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,1 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,-1-1-24 0 0,-1-1-63 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,3 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0-5 63 0 0,5-23-2404 0 0,-2 17 1056 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8">13746 2617 0 0 0,'-3'-6'-1709'0'0,"1"-5"9298"0"0,3 9 1867 0 0,-1 14-7849 0 0,4 100 2619 0 0,-7-23-3124 0 0,6 9 60 0 0,-7 39-1060 0 0,12-67-102 0 0,-6-64-68 0 0,-1-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="9">13727 2835 2304 0 0,'0'0'464'0'0,"4"-8"3648"0"0,-4 5 1786 0 0,25-41-750 0 0,9 4-2447 0 0,4 12-1313 0 0,-20 32-788 0 0,-16-4-482 0 0,-1 1-42 0 0,3 2-30 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 2-1 0 0,0-2 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-2 0 1 0 0,2 0-1 0 0,-1 1-46 0 0,19 88 1079 0 0,-11-66-711 0 0,-8-14-53 0 0,16 64 642 0 0,0-36-721 0 0,10-30-183 0 0,33-40-1154 0 0,-25-3-4448 0 0,-26 23 3543 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="10">14370 2437 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,7 2 583 0 0,-5-7-849 0 0,-2 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 17-2962 0 0,1 58 539 0 0,-5 69 472 0 0,-5 14 1084 0 0,7 78-784 0 0,9-190-592 0 0,1-26-84 0 0,11-17 3 0 0,-13-9-156 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1-3-35 0 0,42-41 80 0 0,-36 36-172 0 0,-7 8-92 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-3 184 0 0,1 0-1288 0 0,2-8-6336 0 0,-6 10 565 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="11">14374 2658 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,52-5 2910 0 0,-37 4-3513 0 0,5 0-489 0 0,-8 4-4783 0 0,-4 1-1037 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="12">14802 2682 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,4 5 4769 0 0,-1 0-4077 0 0,0-1-1648 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 3-394 0 0,-5 181 4855 0 0,0-66-3199 0 0,1-93-1224 0 0,5-9-3265 0 0,-1-14 1400 0 0,0-7-5540 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="13">14834 2916 456 0 0,'2'-11'295'0'0,"-1"9"1230"0"0,5-14 4652 0 0,-6 15-4821 0 0,8-16 3233 0 0,-3 7-3731 0 0,17-34 2412 0 0,-21 42-3133 0 0,0-2-1 0 0,1 1 1 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,2 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-137 0 0,33 1 1322 0 0,-33 1-1262 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 3-59 0 0,19 18 91 0 0,-7 1-240 0 0,-14-24-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="14">15243 2980 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,0-1 0 0 0,1-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,3-4-329 0 0,9-25 1366 0 0,18-4-185 0 0,-29 35-1119 0 0,-1 1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,2 2-62 0 0,38 64 531 0 0,-37-53-291 0 0,0-1-1 0 0,-2 1 1 0 0,2 1 0 0 0,-3 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,-2 10-239 0 0,-6 41 0 0 0,-10-24 1095 0 0,0-44-406 0 0,12 1-606 0 0,1 1-72 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,2 0 1 0 0,0 0 0 0 0,-3-2-11 0 0,2 0-209 0 0,0 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-6 209 0 0,0-20-4042 0 0,2 16-3529 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="15">15669 2358 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,3 8 590 0 0,9 66 2596 0 0,-17 147-2669 0 0,-2-75 14 0 0,7 85-1117 0 0,3-180 0 0 0,0-46-165 0 0,-2-4-698 0 0,-1-1-315 0 0,0-1-1352 0 0,3-5-5157 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="16">15919 2893 3568 0 0,'18'-11'1553'0'0,"-5"-5"1718"0"0,-2 11-2487 0 0,35-32 3450 0 0,-22 9-3218 0 0,30-43-474 0 0,-45 48-542 0 0,-6 15 0 0 0,-6-1 0 0 0,2 6-7 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,-4 0 6 0 0,0 2 11 0 0,-1-1 1 0 0,1 2-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-3 5-12 0 0,-13 25 272 0 0,-5 55 161 0 0,24-85-291 0 0,0 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 2 0 0 0,1-2-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-2-1-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,2-1-142 0 0,-1-1 13 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,3 0-13 0 0,56-24-2033 0 0,-51 16 586 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="17">16312 2610 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-1 1-172 0 0,-13 53 5027 0 0,7-27-3083 0 0,-6 32 478 0 0,11-49-2198 0 0,0 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,0 5-320 0 0,1 26 797 0 0,-2-36-713 0 0,1-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,3 3-83 0 0,-5-7 16 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-2 0 0 0 0,2 1 1 0 0,-1-1-1 0 0,0-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0-2-15 0 0,6-4 20 0 0,16-33 87 0 0,10-39-97 0 0,-30 73-49 0 0,1 0 0 0 0,-2 0-1 0 0,1-2 1 0 0,-1 2 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-6 39 0 0,-3-22-1383 0 0,3 36 837 0 0,-1 0-1200 0 0,-5-5-4721 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="18">15169 2437 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,1-1-292 0 0,5-4-365 0 0,1-2-1 0 0,-1 1 1 0 0,-1-1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-2-363 0 0,41-75 852 0 0,-32 68-781 0 0,-2 15-61 0 0,-8 6 2 0 0,-2 0 0 0 0,2 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 2-11 0 0,1 2-4 0 0,6 26 57 0 0,2-5-53 0 0,4 0-1856 0 0,-8-23-4807 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="19">7370 2668 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-10-2-24 0 0,6 2 8851 0 0,2 5-9133 0 0,-8 15-17 0 0,6-17-769 0 0,3-2-3236 0 0,1-1-1404 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="20">18030 2977 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-6 0-423 0 0,1-2-329 0 0,3 2-272 0 0,0-3-398 0 0,0-1-3749 0 0,-2-9 2451 0 0,3 11-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="21">17794 2702 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-12-3 2088 0 0,-5-4-821 0 0,17 7-1285 0 0,-13 3 543 0 0,-28 27 578 0 0,-3 49-1009 0 0,43-70-646 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1-74 0 0,21 24 398 0 0,-24-30-397 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,0-1-1 0 0,8 1-134 0 0,-8-1-167 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-2-1 0 0,0 1 1 0 0,-1 0 301 0 0,-3 2-105 0 0,12-9-1239 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="22">18209 2743 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,5 8 1656 0 0,-4-5-2461 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 1-229 0 0,1 73 2716 0 0,15 160 1049 0 0,-24-73-3749 0 0,-1-93-16 0 0,-1 20 0 0 0,10-87-64 0 0,1-3-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="23">18234 2818 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,4-7 616 0 0,18-28 2026 0 0,-4 18-2035 0 0,-16 16-1214 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,1-1 0 0 0,-2 2 0 0 0,2-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-84 0 0,2 5 138 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,-1 6-137 0 0,3-12 22 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-2 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0-21 0 0,-30 9 162 0 0,29-10-192 0 0,2 0 1 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,2-1-1 0 0,-4-2 30 0 0,-13-30-3512 0 0,16 21 1769 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="24">18629 2559 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="25">18612 2535 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="26">18600 2641 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="27">18572 2448 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,4 11 2392 0 0,11 80 1583 0 0,-15 34-1639 0 0,9 45-192 0 0,10-22-2656 0 0,-21-130 0 0 0,-2-3-337 0 0,3-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="28">18603 2871 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-1-17 3737 0 0,3-5 4077 0 0,7-20-4186 0 0,7 0-1366 0 0,-1 21-2142 0 0,-8 18-211 0 0,-7 8 222 0 0,17-9 1281 0 0,7 11-1444 0 0,-21 1-105 0 0,38 32-8 0 0,-19-4 744 0 0,-10-2-56 0 0,7 33-96 0 0,-13-20-16 0 0,4 13 191 0 0,-1-20-526 0 0,-1-3-59 0 0,-1-16-12 0 0,-5-14-90 0 0,13 3 16 0 0,16-2-96 0 0,-6-4-141 0 0,-25 2-596 0 0,25-10-4249 0 0,-14 3 1073 0 0,-6 3 1923 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="29">19111 2668 1376 0 0,'-14'6'65'0'0,"12"-5"277"0"0,2-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-5 12 5285 0 0,10 44-3424 0 0,-9-9-2068 0 0,1 48 541 0 0,-5-53-877 0 0,4 2-432 0 0,5 23-1088 0 0,8 8 915 0 0,-5-3-416 0 0,-3-60-545 0 0,-1 19 164 0 0,-5-12-45 0 0,5-18-557 0 0,0-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-5 0-797 0 0,4 0-5332 0 0,1 0 728 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="30">19073 2718 456 0 0,'28'-10'12581'0'0,"-19"4"-11549"0"0,16 5 3076 0 0,-4-5-1928 0 0,26 39 262 0 0,-16 2-1426 0 0,-9 17-48 0 0,-8-18-336 0 0,-13-30-440 0 0,-4 28-53 0 0,-6-11-60 0 0,-6-7 791 0 0,14-12-867 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-2 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1-3 0 0,-31-21-1713 0 0,11-2-2008 0 0,20 16 1827 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="31">16653 2634 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,2 14 1120 0 0,1 37 395 0 0,0 69 75 0 0,4-40-2940 0 0,3 8-252 0 0,-4-14-192 0 0,1-37-12 0 0,-7-35-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="32">16665 2796 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,4-14 2209 0 0,9-3-1077 0 0,27-23 345 0 0,-16 33-1146 0 0,-4 21-314 0 0,-16-11-177 0 0,0 2 0 0 0,0-1-1 0 0,-1 1 1 0 0,2-1 0 0 0,-2 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-37 0 0,-1-4 176 0 0,7 12 413 0 0,-7-13-998 0 0,9 6-4069 0 0,-10-7 3075 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="33">16939 3100 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,5-4 224 0 0,-3 3 3136 0 0,8-10-3493 0 0,-8 8-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="37">17276 2743 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 13 8138 0 0,-3 35-5693 0 0,3-50-1919 0 0,-3 17 1214 0 0,0 78 988 0 0,3-95-2320 0 0,0-2-72 0 0,0 7 75 0 0,-3 27-43 0 0,-3 44-122 0 0,6-75-45 0 0,0 1-235 0 0,0-1-3512 0 0,0-3-1706 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="38">17264 2886 5296 0 0,'3'7'472'0'0,"-3"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-23 1372 0 0,0 21-1542 0 0,0 0-40 0 0,5-28 954 0 0,-4 29-1144 0 0,11-28 1755 0 0,3 10-1413 0 0,-14 18-538 0 0,-1 1 0 0 0,0 0-6 0 0,13-2 374 0 0,-7 3-368 0 0,-5-1-159 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-2 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 2 0 0 0,0-2-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 1-24 0 0,13 60 908 0 0,-10-26-544 0 0,-4-13-78 0 0,1-22-204 0 0,0 22 170 0 0,1-20-204 0 0,2 5-36 0 0,0 0-1 0 0,0 0 42 0 0,3-4 13 0 0,-3-3-58 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,3-3-9 0 0,28-23-3222 0 0,-28 22-430 0 0,-3 5 1775 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">6030 3748 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-10 0 710 0 0,-68 11 2232 0 0,-104-9 113 0 0,78-16-2111 0 0,98 12-1711 0 0,3 0 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0 0-7 0 0,0 0 3 0 0,-1 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,-2-1-3 0 0,-5-1 53 0 0,-56 15 746 0 0,-4-32-422 0 0,-48 19 95 0 0,21 18-267 0 0,-1-27 255 0 0,19 6-262 0 0,-8-5 515 0 0,26 24-785 0 0,-8-11 316 0 0,71-3-237 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,2 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,1 5-384 0 0,-1 0-2483 0 0,0-5 1589 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">4792 3490 12384 0 0,'-15'-11'1277'0'0,"0"9"-438"0"0,-15 9 3998 0 0,8 3-3431 0 0,-21 14 690 0 0,-51 36-1014 0 0,26-27 402 0 0,7 19-1322 0 0,33-25-154 0 0,-9 15 872 0 0,35-39-855 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-2-1-1 0 0,2 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,2 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,3-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 1 0 0 0,-2-2-1 0 0,4 3-23 0 0,36 38 389 0 0,-27-34-394 0 0,-2-1 1 0 0,2 0-1 0 0,0-1 0 0 0,1-1 0 0 0,-2-1 1 0 0,2 1-1 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,0-1-1 0 0,5 0 4 0 0,-4 0-173 0 0,104 18-1371 0 0,-44 2-4118 0 0,-57-15-1845 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="2">3948 2850 2760 0 0,'9'14'125'0'0,"-24"-7"1798"0"0,-5 9-59 0 0,15-9 428 0 0,-23 6 4862 0 0,28-13-6578 0 0,0 0-15 0 0,0 0-34 0 0,-3 2 119 0 0,2-1-159 0 0,1-1 2989 0 0,56-16-1901 0 0,11 9-396 0 0,21 3-749 0 0,-23 1 156 0 0,42-1 469 0 0,21-4-497 0 0,-4-3-454 0 0,56-3 952 0 0,-54 8-543 0 0,-50-4-402 0 0,53-9 402 0 0,-69 8-745 0 0,4 11 112 0 0,-35-6 120 0 0,16 4 0 0 0,8-13 444 0 0,-25 4-280 0 0,12 0-164 0 0,-24 3 0 0 0,-5 7 0 0 0,17 7-1208 0 0,-27-5 877 0 0,7 3-1583 0 0,8 12-3659 0 0,-8-10 3847 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="3">5463 2400 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,9 22 9129 0 0,23-5-7935 0 0,-16-12-2328 0 0,61 29 1337 0 0,-62-23-2420 0 0,-5-6 346 0 0,0 1 1 0 0,0 0-1 0 0,-2 1 1 0 0,2 0-1 0 0,-2 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,4 8-255 0 0,7 66 1080 0 0,-27-5-224 0 0,-11-28-856 0 0,-29-1 327 0 0,-29-11 1242 0 0,10-15-2553 0 0,38-23-3117 0 0,24-1 2058 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="4">12064 2910 8288 0 0,'11'-46'864'0'0,"-13"43"-720"0"0,4-9 1811 0 0,0 9 5703 0 0,63-2-3242 0 0,-25 5-4222 0 0,80 2 1838 0 0,5 8-1085 0 0,277-13 1101 0 0,-174-1-1030 0 0,-78 8-540 0 0,42-1-45 0 0,12-13 803 0 0,-47-21-1236 0 0,-152 29-64 0 0,-5 2-273 0 0,23-10-2694 0 0,-20 10 2502 0 0,6 0-15 0 0,-3 4-3511 0 0,-2 2-4432 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="5">13855 2481 8288 0 0,'0'0'638'0'0,"-1"1"-414"0"0,-1 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,7 6 488 0 0,68 15 2067 0 0,-40-14-2223 0 0,51 22 954 0 0,-55-9-1577 0 0,43 38 370 0 0,-17 1-375 0 0,29 32 240 0 0,-83-88-712 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-3 1-23 0 0,-2 4 44 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-2-1 0 0 0,1 0-44 0 0,-27 11 59 0 0,0-3-1 0 0,0-1 1 0 0,-1-1 0 0 0,-1-3-1 0 0,1-1 1 0 0,-18 0-59 0 0,30-5-59 0 0,-76-10-1395 0 0,91 4-1171 0 0,10 5 1267 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="6">14979 2598 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-12 7 790 0 0,-13 10 150 0 0,-51 20 1099 0 0,7-3-1196 0 0,66-32-1165 0 0,-13 9 158 0 0,0 0 0 0 0,1 1-1 0 0,0 0 1 0 0,1 2 0 0 0,1-1 0 0 0,0 2 0 0 0,1 0 0 0 0,0 0-1 0 0,-6 12-202 0 0,15-22 65 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-2 1 1 0 0,2 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 1-64 0 0,1 1 108 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,8 2-107 0 0,-4-2 42 0 0,-1-1-1 0 0,0-1 0 0 0,1 0 0 0 0,-2-1 1 0 0,2 0-1 0 0,0-1 0 0 0,0 0 0 0 0,7-2-41 0 0,25-18-4007 0 0,-37 14-3607 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="7">15168 2934 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-5-9 655 0 0,5 3-930 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,4-1-345 0 0,-6 2 74 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,2 0-1 0 0,-2-1 1 0 0,1 1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-3 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 2-73 0 0,2 5 95 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 9-95 0 0,-13 69 1049 0 0,12-81-938 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,0-1-111 0 0,3-3 23 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-2 1 0 0 0,3-1 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2-1 0 0 0,3 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2-1 0 0 0,-2 1 1 0 0,0-1-24 0 0,-2-1-63 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,2-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0-5 63 0 0,6-22-2404 0 0,-3 16 1056 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8">15679 2612 0 0 0,'-3'-6'-1709'0'0,"1"-5"9298"0"0,3 9 1867 0 0,-1 14-7849 0 0,4 99 2619 0 0,-7-24-3124 0 0,6 10 60 0 0,-7 38-1060 0 0,13-66-102 0 0,-6-63-68 0 0,-2-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="9">15657 2827 2304 0 0,'0'0'464'0'0,"5"-8"3648"0"0,-5 5 1786 0 0,29-40-750 0 0,12 3-2447 0 0,5 13-1313 0 0,-25 31-788 0 0,-19-4-482 0 0,0 1-42 0 0,2 2-30 0 0,2 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-2 0 1 0 0,3 0-1 0 0,-2 1-46 0 0,24 86 1079 0 0,-14-64-711 0 0,-10-14-53 0 0,19 63 642 0 0,1-36-721 0 0,11-29-183 0 0,40-40-1154 0 0,-29-2-4448 0 0,-33 22 3543 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="10">16426 2435 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,8 2 583 0 0,-5-7-849 0 0,-3 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 16-2962 0 0,1 58 539 0 0,-6 68 472 0 0,-6 14 1084 0 0,8 77-784 0 0,11-188-592 0 0,2-25-84 0 0,12-17 3 0 0,-15-9-156 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1-3-35 0 0,50-40 80 0 0,-43 35-172 0 0,-8 8-92 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1-3 184 0 0,1 0-1288 0 0,2-8-6336 0 0,-7 10 565 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="11">16431 2653 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,62-5 2910 0 0,-44 4-3513 0 0,6 0-489 0 0,-9 4-4783 0 0,-5 1-1037 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="12">16943 2676 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,4 5 4769 0 0,0 0-4077 0 0,0-1-1648 0 0,-3 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 3-394 0 0,-6 179 4855 0 0,0-66-3199 0 0,2-91-1224 0 0,5-10-3265 0 0,-1-13 1400 0 0,0-7-5540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="13">16981 2907 456 0 0,'2'-11'295'0'0,"-1"9"1230"0"0,7-14 4652 0 0,-8 15-4821 0 0,9-15 3233 0 0,-3 6-3731 0 0,20-34 2412 0 0,-24 42-3133 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,1 0-137 0 0,41 1 1322 0 0,-41 1-1262 0 0,2 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-2 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 2-59 0 0,22 19 91 0 0,-8 1-240 0 0,-17-24-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="14">17470 2970 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,2-3-329 0 0,12-26 1366 0 0,21-4-185 0 0,-35 36-1119 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,1-1-1 0 0,-2 1 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 2-62 0 0,46 63 531 0 0,-44-52-291 0 0,0-1-1 0 0,-3 1 1 0 0,3 1 0 0 0,-4-1-1 0 0,2 0 1 0 0,-2 1 0 0 0,0-1-1 0 0,-2 10-239 0 0,-7 40 0 0 0,-13-24 1095 0 0,1-43-406 0 0,14 1-606 0 0,1 1-72 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,2-1 1 0 0,0 0 0 0 0,-3-2-11 0 0,2 0-209 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-6 209 0 0,0-19-4042 0 0,2 15-3529 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="15">17980 2357 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,3 8 590 0 0,11 65 2596 0 0,-19 145-2669 0 0,-4-74 14 0 0,9 83-1117 0 0,4-176 0 0 0,-1-46-165 0 0,-1-4-698 0 0,-2-1-315 0 0,0-1-1352 0 0,3-5-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="16">18279 2884 3568 0 0,'21'-10'1553'0'0,"-5"-6"1718"0"0,-3 11-2487 0 0,42-32 3450 0 0,-26 10-3218 0 0,35-43-474 0 0,-53 47-542 0 0,-8 15 0 0 0,-6-1 0 0 0,2 6-7 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 1 0 0 0,-3-1 1 0 0,2 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-4 0 6 0 0,0 2 11 0 0,-1-1 1 0 0,0 2-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-2-1 1 0 0,2 1-1 0 0,0 1 1 0 0,2-1-1 0 0,-1 1 1 0 0,-3 5-12 0 0,-16 24 272 0 0,-6 55 161 0 0,28-84-291 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-3-1-1 0 0,2 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-2 1 1 0 0,4-1-142 0 0,-2-1 13 0 0,0 0 0 0 0,-2-1 0 0 0,1 1 1 0 0,0-1-1 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,4 0-13 0 0,66-24-2033 0 0,-61 16 586 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="17">18749 2605 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-2 1-172 0 0,-14 52 5027 0 0,7-26-3083 0 0,-6 31 478 0 0,12-48-2198 0 0,1 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 0-1 0 0,2 0 1 0 0,0 0 0 0 0,2 1 0 0 0,-1 5-320 0 0,1 25 797 0 0,-2-35-713 0 0,1-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,2 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1-1-1 0 0,-1 1 1 0 0,3-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,5 3-83 0 0,-7-7 16 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2-1 0 0 0,-3 1 1 0 0,2-1-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1-1 0 0 0,2 1 1 0 0,-3 0-1 0 0,2 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1-2-15 0 0,6-4 20 0 0,19-32 87 0 0,13-39-97 0 0,-37 72-49 0 0,2 0 0 0 0,-2 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-2 0-1 0 0,1 0 1 0 0,-1-6 39 0 0,-4-21-1383 0 0,4 35 837 0 0,-1 0-1200 0 0,-6-5-4721 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="18">17382 2435 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,1-1-292 0 0,6-4-365 0 0,1-2-1 0 0,-1 1 1 0 0,-1-1 0 0 0,2-1-1 0 0,-2 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-363 0 0,51-75 852 0 0,-40 67-781 0 0,-1 15-61 0 0,-11 6 2 0 0,-1 0 0 0 0,2 1-1 0 0,-3-1 1 0 0,2 1 0 0 0,-2 0-1 0 0,2 0 1 0 0,-3 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-2 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 2-11 0 0,2 2-4 0 0,6 25 57 0 0,3-4-53 0 0,5 0-1856 0 0,-10-23-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="19">8053 2662 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-12-2-24 0 0,8 2 8851 0 0,1 5-9133 0 0,-9 15-17 0 0,7-17-769 0 0,4-2-3236 0 0,1-1-1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="20">20803 2967 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-7 0-423 0 0,1-2-329 0 0,4 2-272 0 0,0-3-398 0 0,-1-1-3749 0 0,-2-8 2451 0 0,4 10-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="21">20521 2696 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-14-3 2088 0 0,-6-4-821 0 0,20 7-1285 0 0,-16 3 543 0 0,-33 27 578 0 0,-4 48-1009 0 0,52-70-646 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,3 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,3 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 2-74 0 0,25 24 398 0 0,-28-30-397 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1-1 0 0,10 1-134 0 0,-11-1-167 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-2-1 0 0,0 1 1 0 0,-2 0 301 0 0,-3 2-105 0 0,15-9-1239 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="22">21018 2736 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,6 8 1656 0 0,-5-5-2461 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 2-229 0 0,1 72 2716 0 0,17 158 1049 0 0,-27-72-3749 0 0,-2-92-16 0 0,-1 20 0 0 0,11-86-64 0 0,2-3-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="23">21047 2810 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,5-7 616 0 0,22-27 2026 0 0,-6 17-2035 0 0,-19 16-1214 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-2 0 0 0 0,3 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-3 0 0 0 0,2 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1-84 0 0,3 5 138 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,-2 1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-2-1 0 0 0,0 7-137 0 0,3-12 22 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,3 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0-21 0 0,-35 9 162 0 0,34-10-192 0 0,2 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,3-1-1 0 0,-5-1 30 0 0,-15-31-3512 0 0,18 21 1769 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="24">21520 2555 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="25">21500 2531 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="26">21485 2636 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="27">21452 2445 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,5 11 2392 0 0,12 79 1583 0 0,-17 33-1639 0 0,11 45-192 0 0,12-22-2656 0 0,-25-128 0 0 0,-3-3-337 0 0,4-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="28">21489 2863 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-1-17 3737 0 0,3-4 4077 0 0,9-21-4186 0 0,8 1-1366 0 0,-1 20-2142 0 0,-10 18-211 0 0,-8 8 222 0 0,21-9 1281 0 0,7 11-1444 0 0,-24 1-105 0 0,45 32-8 0 0,-23-4 744 0 0,-11-3-56 0 0,7 33-96 0 0,-15-19-16 0 0,5 12 191 0 0,-1-19-526 0 0,-1-4-59 0 0,-2-15-12 0 0,-5-14-90 0 0,14 3 16 0 0,21-2-96 0 0,-9-4-141 0 0,-29 2-596 0 0,30-10-4249 0 0,-16 3 1073 0 0,-9 3 1923 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="29">22096 2662 1376 0 0,'-16'6'65'0'0,"13"-5"277"0"0,3-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-6 12 5285 0 0,12 43-3424 0 0,-10-8-2068 0 0,0 46 541 0 0,-6-51-877 0 0,6 1-432 0 0,5 23-1088 0 0,10 8 915 0 0,-7-3-416 0 0,-2-59-545 0 0,-2 19 164 0 0,-6-12-45 0 0,6-18-557 0 0,0-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-6 0-797 0 0,4 0-5332 0 0,2 0 728 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="30">22051 2712 456 0 0,'33'-10'12581'0'0,"-22"4"-11549"0"0,19 5 3076 0 0,-5-5-1928 0 0,31 39 262 0 0,-18 1-1426 0 0,-12 17-48 0 0,-9-17-336 0 0,-16-30-440 0 0,-5 27-53 0 0,-7-10-60 0 0,-6-7 791 0 0,15-12-867 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,1 1-1 0 0,-3-1 1 0 0,2 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,2 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,2 0-1 0 0,-1 0 1 0 0,-1-1-1 0 0,0 1-3 0 0,-38-21-1713 0 0,14-2-2008 0 0,23 16 1827 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="31">19156 2629 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,3 14 1120 0 0,0 36 395 0 0,1 68 75 0 0,4-39-2940 0 0,4 8-252 0 0,-4-14-192 0 0,0-36-12 0 0,-8-35-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="32">19171 2789 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,5-14 2209 0 0,10-3-1077 0 0,33-22 345 0 0,-19 32-1146 0 0,-5 21-314 0 0,-20-11-177 0 0,1 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-3 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0-37 0 0,-1-4 176 0 0,9 11 413 0 0,-9-12-998 0 0,11 6-4069 0 0,-12-7 3075 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="33">19499 3089 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,6-4 224 0 0,-4 3 3136 0 0,10-10-3493 0 0,-10 8-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="37">19902 2736 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 13 8138 0 0,-4 34-5693 0 0,4-49-1919 0 0,-4 17 1214 0 0,1 77 988 0 0,3-94-2320 0 0,0-2-72 0 0,0 7 75 0 0,-4 26-43 0 0,-3 44-122 0 0,7-74-45 0 0,0 1-235 0 0,0-1-3512 0 0,0-3-1706 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="38">19887 2877 5296 0 0,'4'7'472'0'0,"-4"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-22 1372 0 0,0 20-1542 0 0,0 0-40 0 0,6-28 954 0 0,-5 29-1144 0 0,13-28 1755 0 0,4 11-1413 0 0,-16 17-538 0 0,-2 1 0 0 0,0 0-6 0 0,15-2 374 0 0,-8 3-368 0 0,-6-1-159 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-2 1 0 0 0,3-1 0 0 0,-1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,0 1-24 0 0,15 60 908 0 0,-11-27-544 0 0,-6-12-78 0 0,2-22-204 0 0,0 21 170 0 0,2-19-204 0 0,1 5-36 0 0,1 0-1 0 0,-1 0 42 0 0,5-4 13 0 0,-5-3-58 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-3 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1-1 0 0,-2 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-2 0 1 0 0,4-3-9 0 0,33-22-3222 0 0,-33 21-430 0 0,-4 5 1775 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2358,86 +2370,86 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">213 659 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="310.099">552 676 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-2-9 10039 0 0,3 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="684.255">894 617 11976 0 0,'-1'5'296'0'0,"-4"5"4551"0"0,3-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1921.293">1194 700 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,1-6-6507 0 0,4-23-839 0 0,-6 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-12 79 971 0 0,11-78-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,2-28 325 0 0,-6 43 218 0 0,0 1 13 0 0,6-5-260 0 0,-1 9-230 0 0,-3 1 347 0 0,-11 35 365 0 0,8-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-9-12-214 0 0,18-43 40 0 0,0 48 757 0 0,-7 6-562 0 0,-2 1-34 0 0,12 15 96 0 0,-21 51 294 0 0,9-64 48 0 0,0-2-24 0 0,-10 10 14 0 0,9-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0-12 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,14-18-798 0 0,-5 23 705 0 0,10 17 39 0 0,-18-13 64 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 2-10 0 0,1-5 84 0 0,-5 17 237 0 0,-16-9-89 0 0,20-9-144 0 0,1 0 0 0 0,-6-10-1050 0 0,3-10-3857 0 0,2 11-3207 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8390.611">1448 417 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,7 57 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,2 17 113 0 0,-3-14-1404 0 0,0 51 981 0 0,-4-2-1688 0 0,1-59-1417 0 0,-2-32 962 0 0,-6-28-2248 0 0,3-5-5035 0 0,5-10 5419 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8997.239">1393 552 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,11-32 2722 0 0,-12 31-3180 0 0,13-15 1008 0 0,20-24 674 0 0,-31 36-2057 0 0,2 2 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,2-1 1 0 0,-2 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1-137 0 0,58 19 1009 0 0,-45 14 55 0 0,-4-18-600 0 0,19 47 1448 0 0,-20 2-2113 0 0,-13-61 230 0 0,0 1 0 0 0,-1-2 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-2 1-29 0 0,3-3 5 0 0,-8 22 399 0 0,1-11-337 0 0,7-8-104 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,-1 1 37 0 0,-29-1 653 0 0,-7-25-4978 0 0,29 19 2334 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11709.08">2594 382 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,3 48 1154 0 0,-10 24 2052 0 0,-2 33 1755 0 0,2 52-2463 0 0,3-54-962 0 0,-2 32-1172 0 0,6-140-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-2 13-2556 0 0,1-23 1622 0 0,1-1-894 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12315.019">2609 440 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,11-7 8 0 0,2-4 772 0 0,-12 10-801 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-250 0 0,8 4 395 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-2 1 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 1 1 0 0,4 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 2-1 0 0,-1-2 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,0 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,2 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 2-79 0 0,-1 0 4 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-3-1-4 0 0,-47-44-4198 0 0,48 42-3651 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10346.212">1924 78 3680 0 0,'-5'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,7 16-23 0 0,3-13-297 0 0,4 3-1604 0 0,-8 95 2 0 0,7-77 200 0 0,0-18-716 0 0,3-41-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10997.838">1859 649 1376 0 0,'4'-20'2159'0'0,"3"0"4223"0"0,5-6-3735 0 0,-3 5-1523 0 0,11-15 1153 0 0,3 11 523 0 0,-3 3-1591 0 0,19-17 135 0 0,-38 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 1-1 0 0,2-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 1 0 0,1 1-51 0 0,2 3 27 0 0,2 1 1 0 0,-2 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,-2 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 7-27 0 0,8 30 368 0 0,26 120 1443 0 0,-18-124-1634 0 0,1-14-84 0 0,-12-24-77 0 0,-4-1-29 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,1 2 0 0 0,-2-2 0 0 0,1-2 0 0 0,-1 2-1 0 0,1 0 1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 13 0 0,34-28-350 0 0,16-12-3834 0 0,-46 36 2533 0 0,3 3-12 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32289.342">1 256 6448 0 0,'6'21'6309'0'0,"-6"-18"-6682"0"0,4 54 3514 0 0,6 85-847 0 0,-1-44-690 0 0,-5-10-929 0 0,11 131 737 0 0,-24 34 57 0 0,5-177-1337 0 0,-2-48-256 0 0,6-13-955 0 0,0-12-4480 0 0,0-3-582 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35199.426">11 287 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,15-38 6274 0 0,-15 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,10-3 291 0 0,62-18 828 0 0,-33 5-729 0 0,11-5 96 0 0,43 12 370 0 0,-52 8-222 0 0,36 2-1079 0 0,-18-6 16 0 0,32-20 451 0 0,-26 15 1144 0 0,53 1-1448 0 0,3 19 224 0 0,-46-19-645 0 0,-26-1 1538 0 0,6 0-1123 0 0,-32 8-292 0 0,45 0 264 0 0,-22-6 20 0 0,48-26 70 0 0,8 18-205 0 0,11 9 34 0 0,-57-4 219 0 0,20-5-424 0 0,-5 12 192 0 0,-8 5 584 0 0,37 1-1352 0 0,-6 9 736 0 0,2 6 1017 0 0,-29-10-298 0 0,-10 0-1239 0 0,23-4 520 0 0,12 3 64 0 0,11 29 75 0 0,-53-11-166 0 0,14 1 523 0 0,-4-9-840 0 0,-18-6 749 0 0,-6-3-675 0 0,21 6 487 0 0,63-10-197 0 0,-18 21 0 0 0,-35-16-20 0 0,-39-2 0 0 0,-10-5 0 0 0,21 17 0 0 0,-33-3 0 0 0,4 6 0 0 0,12 23 64 0 0,-5 28 0 0 0,-7 23-64 0 0,-3 31-8 0 0,-1-49 125 0 0,-2 31-203 0 0,-8 34 295 0 0,8 44-190 0 0,-15-84 82 0 0,-1-41-13 0 0,5-44 96 0 0,5-13-234 0 0,0 2-1 0 0,0-2 1 0 0,1 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,-2 1 51 0 0,1-2 114 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 0-114 0 0,-12 0 158 0 0,-84 8-218 0 0,70-3 59 0 0,-1-1-1 0 0,1-2 1 0 0,0-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-19-6 1 0 0,3-4-9 0 0,-1 3 0 0 0,1 3 0 0 0,-1 2 0 0 0,-18 2 9 0 0,-97 0 332 0 0,120 4-330 0 0,0-1-1 0 0,-1-3 1 0 0,1-2-1 0 0,0-1 1 0 0,-7-7-2 0 0,19 9-18 0 0,0 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-18 4 18 0 0,-123 30 64 0 0,-3-12-136 0 0,-41-9 152 0 0,149-13-80 0 0,-80 0 11 0 0,-29-17 42 0 0,88 17-53 0 0,-20-13 80 0 0,19-11-176 0 0,-74-18 224 0 0,50 21-196 0 0,53 8 192 0 0,-53-4-124 0 0,43 11 0 0 0,40 13-499 0 0,28-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="78758.085">3259 863 13560 0 0,'0'0'306'0'0,"-11"-2"752"0"0,-20-5-12 0 0,30 7-11 0 0,-6-6 1119 0 0,7 5 2052 0 0,56 4-3188 0 0,26-6 262 0 0,139 30 512 0 0,-118-20-1336 0 0,134 27-663 0 0,-43 7 353 0 0,-4-7 891 0 0,-108-31-445 0 0,-66-3-541 0 0,0-1 0 0 0,0 0 0 0 0,0-2 1 0 0,0 0-1 0 0,0-1 0 0 0,8-4-51 0 0,63-36-278 0 0,-85 43 89 0 0,-2 1-156 0 0,3 0-611 0 0,-1 1-1432 0 0,-1-2-4991 0 0,-1 1-504 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="79175.854">4641 574 6448 0 0,'0'0'498'0'0,"1"-1"-28"0"0,26-3 10100 0 0,20 23-6654 0 0,-28-10-3356 0 0,1 1 0 0 0,-1 2 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,4 8-560 0 0,52 53 264 0 0,-67-64-125 0 0,-1 1-1 0 0,0 1 1 0 0,0 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 1 1 0 0,2 11-139 0 0,-5-12 187 0 0,0 0 1 0 0,0 2-1 0 0,0-2 1 0 0,-2 1-1 0 0,0-1 1 0 0,0 2 0 0 0,0-2-1 0 0,-2 1 1 0 0,1-1-1 0 0,-2 2 1 0 0,1-2-1 0 0,-1 0 1 0 0,0 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,-4 6-188 0 0,-21 30 165 0 0,-29-8 587 0 0,-77-23 352 0 0,107-18-1542 0 0,-19 5-2761 0 0,40 0 2491 0 0,-24 12-2399 0 0,14-3-3298 0 0,4 0-1217 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37346.914">5792 851 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,2 2 218 0 0,1-1 5134 0 0,18-14-8855 0 0,-14 9 1888 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37618.204">6115 895 10592 0 0,'-11'-13'818'0'0,"8"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,11-3-8082 0 0,-4 4-1569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37903.659">6415 805 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,4 0-232 0 0,-1 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38875.93">6729 895 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-38 1231 0 0,1 45-2463 0 0,-1 1 0 0 0,2 1 52 0 0,-4 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,6 8 88 0 0,-5-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,0 3-113 0 0,2-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-7-17 194 0 0,21-16-143 0 0,-11 33-62 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 11 0 0,1-1-43 0 0,2 1 32 0 0,1 10 23 0 0,-9 18 200 0 0,3-27-96 0 0,-6 4-695 0 0,12-7-611 0 0,7-10-5710 0 0,-6 6 446 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="44618.988">6973 526 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,9 21-45 0 0,-10-24-3788 0 0,2 9 1039 0 0,3 82 1637 0 0,6 83-1221 0 0,-12-86-1606 0 0,0-80-341 0 0,-1-2-56 0 0,0-6-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53832.509">7233 567 2760 0 0,'3'8'1828'0'0,"4"20"4892"0"0,4 25-3444 0 0,2 103 1947 0 0,-11-80-3937 0 0,-4-37-4508 0 0,2-36 1701 0 0,-4 5-229 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54557.219">7279 895 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,7-39 5734 0 0,4-11-521 0 0,-15 20-3279 0 0,10 10-1202 0 0,7-37 1 0 0,-12 56-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-2 2 0 0 0,2-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,3 0-93 0 0,1-2 95 0 0,-4 3-21 0 0,23 0-60 0 0,1 14-14 0 0,-4 7 0 0 0,-18-12 0 0 0,9 23 0 0 0,17 74 514 0 0,-17-52 356 0 0,5-19-278 0 0,-17-34-517 0 0,5 3 98 0 0,-3-2-141 0 0,0-1 0 0 0,-1 2-1 0 0,1-2 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,2-1 0 0 0,-1 1-1 0 0,-1-1 1 0 0,2 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-32 0 0,21-4-185 0 0,-5-27-4233 0 0,-19 31 2840 0 0,0 1-164 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56701.452">7958 623 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-9-2-143 0 0,-34-6 1747 0 0,36 9-1667 0 0,5-2 170 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0-107 0 0,-30 42-483 0 0,15 1 618 0 0,15 14 378 0 0,8 3-513 0 0,13-4 1899 0 0,22-11-1734 0 0,-10-18-165 0 0,-16-20 0 0 0,13 2 0 0 0,-20-10 0 0 0,-1 2 0 0 0,0-5-64 0 0,26-22-5497 0 0,-27 16 3530 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57367.528">8186 956 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,10-17 649 0 0,-7 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,8 19 784 0 0,-13 15 56 0 0,5-33-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="64361.857">8421 615 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,6 17 886 0 0,4 73 1352 0 0,-4-54-2105 0 0,-8 63 686 0 0,-1-6-314 0 0,2 68-530 0 0,5-113-273 0 0,-2-10 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-2-14-1557 0 0,1-2 195 0 0,-2 0-70 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="69762.645">8391 617 1376 0 0,'4'7'367'0'0,"-4"-6"1002"0"0,0-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,8-7 51 0 0,28-23 1588 0 0,-24 24-1245 0 0,-11 4-294 0 0,1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 1-100 0 0,2 2 108 0 0,1 1-1 0 0,-1 0 0 0 0,0-1 0 0 0,-1 2 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,0 2 0 0 0,1-2 1 0 0,0 6-108 0 0,7 27 435 0 0,1 58 787 0 0,-10-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-56 0 0,-38 35 929 0 0,38-35-879 0 0,0-1-45 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0 0 0 0,0-1-1 0 0,1 2 1 0 0,0-1 0 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 1-5 0 0,-2-1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-2-3 0 0 0,4-16-5381 0 0,0 15-2125 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70961.788">8802 348 0 0 0,'-10'13'0'0'0,"5"-16"140"0"0,3 3 2586 0 0,2 0 5496 0 0,13 20-7158 0 0,-12-19-552 0 0,6 30 3000 0 0,-11 31-1947 0 0,1 50 181 0 0,3 1 624 0 0,-6-41-881 0 0,9 38-1316 0 0,-10-26-173 0 0,7-43 0 0 0,12 2-2476 0 0,-10-39 2128 0 0,-2-3 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,0-1-2221 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="71766.961">8787 778 4376 0 0,'0'0'199'0'0,"8"-10"1918"0"0,-4-3 1016 0 0,9-10 683 0 0,-6-13-1297 0 0,-1-1-472 0 0,5 29-1272 0 0,-9 7-743 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,1 1-33 0 0,5 0 304 0 0,18 22 598 0 0,-22-17-674 0 0,2 0-1 0 0,-2 0 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,1 6-227 0 0,6 92 608 0 0,-7-65-165 0 0,0-12 997 0 0,23-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,10-10-60 0 0,-16 1-2985 0 0,-15 8-1180 0 0,-6 1 2595 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73476.329">9328 652 2760 0 0,'0'1'207'0'0,"0"45"6763"0"0,0-45-5925 0 0,0-1-21 0 0,2 8 598 0 0,1 13-344 0 0,-1 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 9-1278 0 0,-10 63 616 0 0,0-18 973 0 0,12 39-2158 0 0,1-87 962 0 0,-1-26-377 0 0,1-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="74025.376">9383 645 3224 0 0,'-1'-5'1144'0'0,"3"-6"9068"0"0,-1 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,49-25 1867 0 0,-47 27-2559 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-2 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,2 2-156 0 0,-1-1 96 0 0,2 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1-95 0 0,-1-1 94 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,-3 5-94 0 0,-37 57 1952 0 0,40-65-2012 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0-2 0 0 0,0 2 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-7-6-2618 0 0,5-2 1170 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128695.154">5097 1481 4144 0 0,'0'0'319'0'0,"-6"7"1871"0"0,2-2 3495 0 0,-24-2-688 0 0,1-4-2621 0 0,2-15 488 0 0,-15 7-1852 0 0,-6-1 1272 0 0,-22-14-812 0 0,3 4-939 0 0,0 3 998 0 0,-4 0-1171 0 0,-8 11-360 0 0,-100 12 1824 0 0,95 7-1887 0 0,33-8 230 0 0,-29-9-256 0 0,7-6 82 0 0,12 7 87 0 0,20 3-80 0 0,-65-14 0 0 0,44-2 0 0 0,-7 7 0 0 0,43 2 0 0 0,11 5-60 0 0,9 2-440 0 0,5 5-11674 0 0,-1-4 3997 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129337.391">3822 1149 8288 0 0,'0'2'227'0'0,"-1"-1"0"0"0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,0 1-227 0 0,-17 1 2894 0 0,12 2-2512 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 2 0 0 0,-5 4-381 0 0,-3 3 422 0 0,-13 14 408 0 0,-33 33 222 0 0,15-4-867 0 0,42-32 92 0 0,1-22-266 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 2-1 0 0,0-2 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2-1-1 0 0,2 1 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-11 0 0,22 11 26 0 0,84 21-304 0 0,-43-10-3852 0 0,-17 7-1623 0 0,-34-16 3707 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="133691.162">5216 3772 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-8 0 710 0 0,-60 11 2232 0 0,-88-9 113 0 0,65-16-2111 0 0,87 12-1711 0 0,0 0 0 0 0,1 1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-1 0 0,-2-1 1 0 0,2 1 0 0 0,-2 0-1 0 0,1 0-7 0 0,0 0 3 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 0 0 0 0,-4-1-3 0 0,-3-1 53 0 0,-49 15 746 0 0,-4-32-422 0 0,-40 19 95 0 0,19 18-267 0 0,-4-27 255 0 0,18 6-262 0 0,-6-5 515 0 0,21 24-785 0 0,-6-11 316 0 0,61-3-237 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,1 0 0 0 0,-1 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,0 5-384 0 0,1 0-2483 0 0,-1-5 1589 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="134078.302">4145 3509 12384 0 0,'-12'-11'1277'0'0,"-1"9"-438"0"0,-13 9 3998 0 0,7 3-3431 0 0,-19 15 690 0 0,-43 36-1014 0 0,22-27 402 0 0,6 19-1322 0 0,29-26-154 0 0,-8 16 872 0 0,30-40-855 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1-2-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-2-1 0 0,2 3-23 0 0,31 39 389 0 0,-23-35-394 0 0,-1-1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0 0 0 0,0-2 1 0 0,1 1-1 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,0-1-1 0 0,5 0 4 0 0,-5 0-173 0 0,90 18-1371 0 0,-36 3-4118 0 0,-51-16-1845 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136187.119">3415 2857 2760 0 0,'8'14'125'0'0,"-20"-6"1798"0"0,-6 8-59 0 0,14-9 428 0 0,-22 6 4862 0 0,26-13-6578 0 0,0 0-15 0 0,0 0-34 0 0,-1 2 119 0 0,0-1-159 0 0,1-1 2989 0 0,48-16-1901 0 0,10 9-396 0 0,18 3-749 0 0,-19 1 156 0 0,35-1 469 0 0,19-4-497 0 0,-4-4-454 0 0,48-2 952 0 0,-45 8-543 0 0,-44-4-402 0 0,45-10 402 0 0,-59 9-745 0 0,3 11 112 0 0,-29-6 120 0 0,13 4 0 0 0,6-13 444 0 0,-21 4-280 0 0,11-1-164 0 0,-21 4 0 0 0,-5 7 0 0 0,16 7-1208 0 0,-24-5 877 0 0,6 3-1583 0 0,6 13-3659 0 0,-7-11 3847 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136591.973">4726 2399 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,8 22 9129 0 0,20-4-7935 0 0,-15-13-2328 0 0,53 29 1337 0 0,-52-22-2420 0 0,-6-7 346 0 0,1 1 1 0 0,0 0-1 0 0,-1 1 1 0 0,-1 0-1 0 0,0 2 1 0 0,1-1-1 0 0,-2 0 1 0 0,1 1-1 0 0,3 8-255 0 0,7 68 1080 0 0,-24-5-224 0 0,-10-30-856 0 0,-24 0 327 0 0,-25-11 1242 0 0,7-15-2553 0 0,34-24-3117 0 0,21-1 2058 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="139663.33">10436 2918 8288 0 0,'10'-47'864'0'0,"-12"44"-720"0"0,4-9 1811 0 0,-1 9 5703 0 0,56-2-3242 0 0,-23 5-4222 0 0,70 2 1838 0 0,4 8-1085 0 0,240-13 1101 0 0,-152-1-1030 0 0,-65 8-540 0 0,35-1-45 0 0,10-13 803 0 0,-40-22-1236 0 0,-131 30-64 0 0,-5 2-273 0 0,20-10-2694 0 0,-18 10 2502 0 0,7 0-15 0 0,-5 4-3511 0 0,0 2-4432 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="140326.574">11985 2481 8288 0 0,'0'0'638'0'0,"0"1"-414"0"0,-2 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,6 6 488 0 0,60 16 2067 0 0,-37-15-2223 0 0,45 22 954 0 0,-47-8-1577 0 0,38 38 370 0 0,-16 1-375 0 0,25 33 240 0 0,-71-90-712 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1-23 0 0,-4 4 44 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-2 1 0 0,0 1-1 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1-1 0 0 0,0 0-44 0 0,-23 11 59 0 0,0-3-1 0 0,0 0 1 0 0,-1-2 0 0 0,0-3-1 0 0,0-1 1 0 0,-16 0-59 0 0,27-5-59 0 0,-66-10-1395 0 0,78 4-1171 0 0,9 5 1267 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151416.768">12958 2600 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-11 8 790 0 0,-11 9 150 0 0,-43 21 1099 0 0,5-4-1196 0 0,58-32-1165 0 0,-12 9 158 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,1 2 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-6 13-202 0 0,14-23 65 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1-64 0 0,0 1 108 0 0,2 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0-1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-2 0 0 0,-1 0-1 0 0,8 2-107 0 0,-3-2 42 0 0,-2-1-1 0 0,1-1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 0 0 0,7-2-41 0 0,20-19-4007 0 0,-31 15-3607 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="152065.555">13120 2943 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-3-9 655 0 0,3 2-930 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-2 0 0 0,-1 2 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,2-2-345 0 0,-3 3 74 0 0,-1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,0-1 1 0 0,-2 1 0 0 0,2 1-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,1 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 2-73 0 0,1 5 95 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 10-95 0 0,-11 69 1049 0 0,10-82-938 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-2-111 0 0,2-3 23 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,-2-1-24 0 0,1-2-63 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-2-1-1 0 0,2 1 1 0 0,-2-1-1 0 0,2 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1-2-1 0 0,1 2 1 0 0,-1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-2-1 0 0,0-4 63 0 0,6-22-2404 0 0,-4 15 1056 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153048.506">13564 2615 0 0 0,'-3'-6'-1709'0'0,"1"-6"9298"0"0,3 10 1867 0 0,-1 15-7849 0 0,3 100 2619 0 0,-5-25-3124 0 0,5 11 60 0 0,-7 39-1060 0 0,12-68-102 0 0,-6-64-68 0 0,-1-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153375.191">13544 2834 2304 0 0,'0'0'464'0'0,"4"-8"3648"0"0,-3 5 1786 0 0,24-41-750 0 0,10 3-2447 0 0,4 13-1313 0 0,-20 33-788 0 0,-17-5-482 0 0,0 1-42 0 0,2 2-30 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 2 1 0 0,-1-2-1 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1-46 0 0,20 88 1079 0 0,-11-66-711 0 0,-10-13-53 0 0,18 63 642 0 0,0-36-721 0 0,10-30-183 0 0,33-40-1154 0 0,-24-3-4448 0 0,-27 23 3543 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160253.303">14210 2434 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,6 2 583 0 0,-3-7-849 0 0,-3 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 17-2962 0 0,1 58 539 0 0,-5 70 472 0 0,-6 14 1084 0 0,8 79-784 0 0,9-192-592 0 0,2-26-84 0 0,10-17 3 0 0,-13-9-156 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,2-4-35 0 0,42-39 80 0 0,-37 34-172 0 0,-7 9-92 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-3 184 0 0,2 0-1288 0 0,0-8-6336 0 0,-5 9 565 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160816.746">14214 2656 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,53-5 2910 0 0,-37 4-3513 0 0,4 0-489 0 0,-7 4-4783 0 0,-4 1-1037 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="165875.957">14657 2680 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,3 5 4769 0 0,1 0-4077 0 0,-2-1-1648 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 3-394 0 0,-5 183 4855 0 0,0-68-3199 0 0,1-92-1224 0 0,5-11-3265 0 0,-1-13 1400 0 0,0-7-5540 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="166400.987">14690 2915 456 0 0,'1'-11'295'0'0,"0"9"1230"0"0,5-14 4652 0 0,-5 15-4821 0 0,7-16 3233 0 0,-3 7-3731 0 0,18-35 2412 0 0,-22 43-3133 0 0,0-1-1 0 0,1 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-137 0 0,34 1 1322 0 0,-33 1-1262 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,2 2-59 0 0,18 20 91 0 0,-6 0-240 0 0,-15-24-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167273.982">15113 2979 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,2-3-329 0 0,9-27 1366 0 0,19-4-185 0 0,-30 37-1119 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,2 2-62 0 0,39 65 531 0 0,-38-54-291 0 0,1-1-1 0 0,-3 2 1 0 0,2 0 0 0 0,-2-1-1 0 0,-1 0 1 0 0,0 2 0 0 0,0-2-1 0 0,-2 10-239 0 0,-6 42 0 0 0,-11-26 1095 0 0,1-43-406 0 0,12 1-606 0 0,0 1-72 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,2-1 1 0 0,-1 0 0 0 0,-2-3-11 0 0,2 1-209 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0-2 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-6 209 0 0,0-20-4042 0 0,2 16-3529 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167927.933">15554 2355 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,2 8 590 0 0,11 66 2596 0 0,-19 148-2669 0 0,-1-75 14 0 0,7 85-1117 0 0,4-181 0 0 0,-2-45-165 0 0,-1-5-698 0 0,-1-1-315 0 0,1-1-1352 0 0,2-6-5157 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="189572.02">15812 2892 3568 0 0,'19'-10'1553'0'0,"-6"-7"1718"0"0,-1 12-2487 0 0,35-32 3450 0 0,-22 9-3218 0 0,31-43-474 0 0,-47 47-542 0 0,-6 16 0 0 0,-6-1 0 0 0,2 6-7 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,2 1 1 0 0,-4 0 6 0 0,0 2 11 0 0,-1-1 1 0 0,1 2-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-4 5-12 0 0,-12 25 272 0 0,-6 56 161 0 0,25-86-291 0 0,0 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,1-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,1-1 0 0 0,-2-1-1 0 0,2 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,1-1-142 0 0,-1-1 13 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,3 0-13 0 0,59-24-2033 0 0,-54 16 586 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190134.967">16219 2608 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-1 1-172 0 0,-14 53 5027 0 0,8-27-3083 0 0,-6 32 478 0 0,10-49-2198 0 0,1 2 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 1 0 0 0,1 0 0 0 0,1 5-320 0 0,-1 26 797 0 0,-1-36-713 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 2 1 0 0,-1-2 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,5 3-83 0 0,-6-7 16 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,1-2-15 0 0,5-4 20 0 0,16-33 87 0 0,12-39-97 0 0,-32 73-49 0 0,1 0 0 0 0,-2-1-1 0 0,1 0 1 0 0,0 1 0 0 0,-2-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-6 39 0 0,-4-22-1383 0 0,4 36 837 0 0,-1 0-1200 0 0,-5-5-4721 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192408.343">15036 2434 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,1-1-292 0 0,5-4-365 0 0,1-2-1 0 0,-1 1 1 0 0,0-1 0 0 0,1-1-1 0 0,-2 1 1 0 0,0-2 0 0 0,0 1-1 0 0,-1 0 1 0 0,2-1-363 0 0,42-77 852 0 0,-34 69-781 0 0,-1 15-61 0 0,-10 6 2 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 2-11 0 0,2 2-4 0 0,5 26 57 0 0,2-4-53 0 0,5-1-1856 0 0,-9-23-4807 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="211829.387">6966 2666 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-10-2-24 0 0,7 2 8851 0 0,0 5-9133 0 0,-7 15-17 0 0,5-17-769 0 0,4-2-3236 0 0,1-1-1404 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-211952.654">17997 2976 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-7 0-423 0 0,2-2-329 0 0,3 2-272 0 0,-1-3-398 0 0,2-1-3749 0 0,-4-8 2451 0 0,4 10-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212149.586">17752 2700 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-12-3 2088 0 0,-5-4-821 0 0,16 7-1285 0 0,-12 3 543 0 0,-30 28 578 0 0,-3 48-1009 0 0,46-71-646 0 0,-2 0 0 0 0,1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 2-74 0 0,22 25 398 0 0,-24-31-397 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,2-1-1 0 0,7 1-134 0 0,-8-1-167 0 0,0 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,2-1 1 0 0,-2 0-1 0 0,1 1 1 0 0,0-2-1 0 0,-1 1 1 0 0,1 0 301 0 0,-4 2-105 0 0,13-10-1239 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205932.193">18182 2741 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,5 8 1656 0 0,-4-5-2461 0 0,1 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2 0 1 0 0,-2 1-1 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 2-229 0 0,2 74 2716 0 0,17 160 1049 0 0,-27-73-3749 0 0,0-93-16 0 0,-2 19 0 0 0,11-86-64 0 0,1-4-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205389.214">18208 2816 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,3-7 616 0 0,20-27 2026 0 0,-4 16-2035 0 0,-17 17-1214 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,0-1-84 0 0,2 5 138 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-2 2 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-3 1 0 0 0,2-2 0 0 0,-1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 2 1 0 0,0-1-1 0 0,0 0 0 0 0,0-1 0 0 0,-3 7-137 0 0,4-12 22 0 0,0 2-1 0 0,-1-2 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 1-1 0 0,1-2 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0-21 0 0,-32 9 162 0 0,31-10-192 0 0,2 0 1 0 0,-2-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,2 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,2-2-1 0 0,-5 0 30 0 0,-12-31-3512 0 0,16 20 1769 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-204187.105">18616 2557 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203902.979">18599 2532 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203901.979">18586 2639 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203439.752">18557 2444 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,4 12 2392 0 0,11 79 1583 0 0,-14 35-1639 0 0,8 45-192 0 0,11-22-2656 0 0,-23-131 0 0 0,0-3-337 0 0,2-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202468.889">18589 2870 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-1-17 3737 0 0,3-5 4077 0 0,8-21-4186 0 0,6 1-1366 0 0,0 21-2142 0 0,-9 18-211 0 0,-7 8 222 0 0,17-9 1281 0 0,8 11-1444 0 0,-22 1-105 0 0,40 32-8 0 0,-21-3 744 0 0,-9-4-56 0 0,6 34-96 0 0,-12-19-16 0 0,3 12 191 0 0,-1-19-526 0 0,0-5-59 0 0,-2-14-12 0 0,-5-15-90 0 0,14 3 16 0 0,16-2-96 0 0,-7-4-141 0 0,-24 2-596 0 0,24-10-4249 0 0,-13 3 1073 0 0,-7 2 1923 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201801.05">19115 2666 1376 0 0,'-14'6'65'0'0,"11"-5"277"0"0,3-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-5 12 5285 0 0,10 44-3424 0 0,-8-8-2068 0 0,-1 47 541 0 0,-5-53-877 0 0,6 2-432 0 0,4 24-1088 0 0,7 7 915 0 0,-3-3-416 0 0,-3-59-545 0 0,-3 18 164 0 0,-4-12-45 0 0,4-18-557 0 0,1-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-4 0-797 0 0,2 0-5332 0 0,2 0 728 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201246.613">19075 2717 456 0 0,'29'-11'12581'0'0,"-19"5"-11549"0"0,15 5 3076 0 0,-3-5-1928 0 0,27 40 262 0 0,-17 0-1426 0 0,-9 18-48 0 0,-8-17-336 0 0,-15-31-440 0 0,-3 28-53 0 0,-6-11-60 0 0,-7-7 791 0 0,15-12-867 0 0,0-1 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,2-1 0 0 0,-2 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-3 1-3 0 0,-31-22-1713 0 0,11-1-2008 0 0,21 16 1827 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190828.747">16571 2632 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,3 14 1120 0 0,-1 37 395 0 0,2 69 75 0 0,3-39-2940 0 0,3 8-252 0 0,-3-15-192 0 0,0-36-12 0 0,-7-36-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="191215.919">16584 2795 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,4-14 2209 0 0,9-4-1077 0 0,29-21 345 0 0,-17 32-1146 0 0,-4 21-314 0 0,-17-11-177 0 0,0 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-37 0 0,-1-4 176 0 0,7 11 413 0 0,-7-12-998 0 0,10 7-4069 0 0,-11-8 3075 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="199554.903">16867 3101 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,6-4 224 0 0,-4 3 3136 0 0,8-11-3493 0 0,-8 9-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174270.903">17216 2741 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 13 8138 0 0,-3 35-5693 0 0,3-50-1919 0 0,-3 18 1214 0 0,0 78 988 0 0,3-96-2320 0 0,0-2-72 0 0,0 7 75 0 0,-4 26-43 0 0,-2 46-122 0 0,6-76-45 0 0,0 1-235 0 0,0-1-3512 0 0,0-3-1706 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173620.241">17203 2885 5296 0 0,'4'7'472'0'0,"-4"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-22 1372 0 0,0 19-1542 0 0,0 1-40 0 0,5-28 954 0 0,-4 29-1144 0 0,11-29 1755 0 0,4 12-1413 0 0,-15 17-538 0 0,-1 1 0 0 0,0 0-6 0 0,13-2 374 0 0,-7 3-368 0 0,-4-1-159 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-2 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1-24 0 0,12 62 908 0 0,-9-29-544 0 0,-5-11-78 0 0,1-23-204 0 0,0 21 170 0 0,1-19-204 0 0,1 5-36 0 0,2 1-1 0 0,-1-1 42 0 0,3-4 13 0 0,-3-3-58 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,2 1 0 0 0,0-1 0 0 0,-2-2 0 0 0,2 2 0 0 0,-1 0-1 0 0,-1 0 1 0 0,3-3-9 0 0,30-22-3222 0 0,-30 21-430 0 0,-3 5 1775 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="-165827.57">12107 3608 920 0 0,'0'0'411'0'0,"0"0"1389"0"0,0 0 609 0 0,0 0 119 0 0,0 0-215 0 0,0 0-1014 0 0,0 0-445 0 0,0 0-87 0 0,0 0-46 0 0,0 0-109 0 0,0 0-48 0 0,0 0-10 0 0,0 0 0 0 0,0 0 11 0 0,-13-2 1750 0 0,-6-2-885 0 0,-1 1-1 0 0,1 2 1 0 0,-1 0-1 0 0,1 1 1 0 0,-12 2-1430 0 0,-35 10 1057 0 0,-22-11-2 0 0,27-4-630 0 0,-73 0 196 0 0,30-8-298 0 0,33-8 8 0 0,59 14-305 0 0,0 2-1 0 0,0 0 1 0 0,0 1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 2 0 0 0,1 0 0 0 0,0 0-1 0 0,-4 2-25 0 0,-40 13 22 0 0,11-7 31 0 0,9-13 11 0 0,-68-2 64 0 0,50 27-128 0 0,-20 2 0 0 0,41-22 0 0 0,-9-5 0 0 0,-20 7 0 0 0,33 4 0 0 0,-11-14 0 0 0,-2-24 0 0 0,-6 29 0 0 0,3-3 0 0 0,30 3-632 0 0,13 1 769 0 0,0 1-984 0 0,2 0-6440 0 0,5-2 5260 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-62540.216">5345 243 9240 0 0,'0'0'208'0'0,"0"0"33"0"0,0 0 14 0 0,0 0 69 0 0,0 0 284 0 0,0 0 120 0 0,0 0 28 0 0,0 0-30 0 0,0 0-139 0 0,0 0-62 0 0,0 16 1654 0 0,-6 124 2954 0 0,-2 16-3081 0 0,7 59-343 0 0,8 152 170 0 0,1-204-1465 0 0,-8-131-531 0 0,0-30-556 0 0,0-4-270 0 0,-3-26-3089 0 0,0 17 1904 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-50190.827">5317 279 3224 0 0,'0'0'387'0'0,"0"0"414"0"0,0 0 183 0 0,0 0 37 0 0,-11-2 2900 0 0,4 0 1482 0 0,3 5 686 0 0,19 7-5649 0 0,73-9 731 0 0,-29-11-391 0 0,59 6-160 0 0,44-6-302 0 0,-61-2-104 0 0,23 7 148 0 0,-6 3 150 0 0,-10 2-320 0 0,21 3-48 0 0,-24 4 171 0 0,57 16 58 0 0,-52-10 92 0 0,7-8 14 0 0,-7-13-479 0 0,-41 3 68 0 0,-53 2-39 0 0,1 2-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 1-1 0 0,0 1 1 0 0,9 2-29 0 0,33 5 0 0 0,27-4 0 0 0,-11-1 0 0 0,-7-1 0 0 0,-32 7 0 0 0,41-4 0 0 0,44-8 0 0 0,-86-1 0 0 0,39 5 0 0 0,-62 1 5 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,4-1-5 0 0,57-5 19 0 0,83 21-8 0 0,-92-7 95 0 0,18-6-31 0 0,-16-10-11 0 0,84 1 0 0 0,-71 2 0 0 0,7 1-64 0 0,-40-3 53 0 0,33 0-42 0 0,-40 9-11 0 0,52-4 0 0 0,17 0 0 0 0,-30 16 0 0 0,179-10 0 0 0,-113-19 0 0 0,-75 10 0 0 0,36 0 0 0 0,-25 11 0 0 0,-30 3 0 0 0,25-6 64 0 0,-4-6 128 0 0,53 5-192 0 0,-94 4 0 0 0,-1-1 0 0 0,-22-3 0 0 0,-2 0-12 0 0,-4 0-53 0 0,-1 0-170 0 0,0 0-576 0 0,0 0-247 0 0,0 0-49 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-49193.598">10117 195 5928 0 0,'0'0'266'0'0,"0"0"1"0"0,0 1-171 0 0,0 4 92 0 0,0-4 732 0 0,-2 15 4758 0 0,4 14-1191 0 0,7 35 169 0 0,-12-10-3447 0 0,-3 119 1305 0 0,2-61-2021 0 0,-1-7-60 0 0,4 51 591 0 0,7-35-728 0 0,-3-90-284 0 0,-2 1 204 0 0,-1-32-157 0 0,0-1 6 0 0,0 0-26 0 0,0 0-98 0 0,0 0-9 0 0,0 0 4 0 0,0 0 0 0 0,0 0-43 0 0,0 0-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0-98 0 0,0 0-410 0 0,0 0-182 0 0,0 0-42 0 0,0 0-73 0 0,0 0-285 0 0,0 0-126 0 0,0 0-983 0 0,0 0-3823 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-48911.614">10104 1101 456 0 0,'0'0'1737'0'0,"0"0"207"0"0,0 0 88 0 0,0 0-76 0 0,0 0-381 0 0,0 0-174 0 0,0 0-32 0 0,0 0-62 0 0,0 0-231 0 0,0 3-99 0 0,0 75 4474 0 0,4-45-4150 0 0,1 16 250 0 0,-4 2-1349 0 0,-2-22-20 0 0,1-21-172 0 0,0 5 904 0 0,0-13-2338 0 0,0 3-8055 0 0,0-3 3197 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-46458.211">10126 1337 3224 0 0,'-10'8'2653'0'0,"-37"20"4634"0"0,46-28-6665 0 0,-1 0 33 0 0,-41-7 3329 0 0,-32 1 217 0 0,48 7-3372 0 0,-71-2 683 0 0,42-21 54 0 0,27 12-1308 0 0,13 5-82 0 0,1 1 1 0 0,-1 0-1 0 0,1 2 0 0 0,-1 0 0 0 0,0 2 0 0 0,0 0 1 0 0,-10 2-177 0 0,-13-1 177 0 0,-36-8 419 0 0,12-3-51 0 0,-54 6 350 0 0,23 11-662 0 0,13 3-169 0 0,11-2-64 0 0,-14-16 140 0 0,-53 7 320 0 0,42 2-460 0 0,6-13 83 0 0,15 0-30 0 0,28 6-53 0 0,-35 0 0 0 0,-55 6 0 0 0,-18-4 0 0 0,69 1 0 0 0,0 5 0 0 0,-41-4 0 0 0,8-6 0 0 0,-127 8 0 0 0,171 5 0 0 0,-32-10 117 0 0,8-7 118 0 0,43 8-410 0 0,-94 8 326 0 0,90-8-162 0 0,-76-1 37 0 0,3 9-289 0 0,7 5 263 0 0,-31-1 208 0 0,57 0-413 0 0,-44-5 194 0 0,32-6 11 0 0,-33 22 344 0 0,67-5-608 0 0,-58 4 160 0 0,67-15 104 0 0,-33-3 968 0 0,13-11-1140 0 0,11 11-113 0 0,21 10 214 0 0,-36-5 71 0 0,63-6-97 0 0,22 2 121 0 0,4-1-4216 0 0,3 0-5767 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-41895.864">5460 2561 5264 0 0,'3'0'1129'0'0,"6"0"-2200"0"0,-6 0 4901 0 0,-2 1 4833 0 0,6 41-6741 0 0,-7 54 512 0 0,-7 20-998 0 0,14 103 1044 0 0,6-75-1600 0 0,-3-46-128 0 0,3 49-792 0 0,-7-71 515 0 0,-6-35 182 0 0,-4-16 138 0 0,0-14-1692 0 0,4-11-2271 0 0,1-8 1285 0 0,0-1-408 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-39644.648">5427 2564 456 0 0,'0'0'1548'0'0,"0"0"185"0"0,0 0 82 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-42 0 0,0 0-140 0 0,0 0-57 0 0,0 0-16 0 0,0 0-1 0 0,0 0 12 0 0,0 0 2 0 0,0 0-1 0 0,0 0-47 0 0,0 0-202 0 0,0 0-92 0 0,2 0-11 0 0,45-7 2042 0 0,42 1 147 0 0,61 5-222 0 0,-21 11-1432 0 0,-17-16-175 0 0,125-12 402 0 0,-106-6-820 0 0,-48 7 18 0 0,-49 10-382 0 0,2 2 1 0 0,-1 2-1 0 0,28 1 7 0 0,57 2 256 0 0,-80 0-256 0 0,38 0 181 0 0,-19 10-106 0 0,6-4 1 0 0,-3-2 68 0 0,50 0-1 0 0,-71-1-90 0 0,74-4 144 0 0,166-8-122 0 0,-224 12-75 0 0,39 8 0 0 0,18-8 0 0 0,-59 5 0 0 0,-3-3 0 0 0,50-5 0 0 0,14 0 0 0 0,-57 11 0 0 0,-20-4 64 0 0,57-18 0 0 0,-35 1-64 0 0,47-3-67 0 0,38 24 54 0 0,-84-12 13 0 0,-38-3 11 0 0,2 2-1 0 0,-2 1 1 0 0,0 1 0 0 0,0 1-1 0 0,23 5-10 0 0,8-3 11 0 0,69-6-74 0 0,-45-3 30 0 0,42 19 33 0 0,13-3 152 0 0,-80-3-152 0 0,-20-6-172 0 0,39 4 160 0 0,10-5 12 0 0,-24 0 0 0 0,-7-3 0 0 0,-21 3 0 0 0,2 0-16 0 0,-32 0-61 0 0,-1 0-6 0 0,0 0-138 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1739 0 0,0 0-6757 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-38736.343">9765 2513 1376 0 0,'0'0'65'0'0,"0"0"341"0"0,0 0 1404 0 0,0 0 611 0 0,8 0 3921 0 0,-6 1-6029 0 0,0 0 0 0 0,1-1-1 0 0,-2 1 1 0 0,1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 3-313 0 0,5 61 2731 0 0,17 121-151 0 0,-13-101-1558 0 0,-14 40 98 0 0,13 24 148 0 0,-4-78-785 0 0,-3-29-243 0 0,-2 26 129 0 0,1 22 111 0 0,-1-56-253 0 0,0-34-205 0 0,0-1-106 0 0,0 0-8 0 0,-17 20-828 0 0,17-20 767 0 0,-9 16-1455 0 0,8-15 1350 0 0,1-1-81 0 0,0 0-40 0 0,0 0-5 0 0,0 0-101 0 0,0 0-426 0 0,0 0-185 0 0,0 0-37 0 0,0 0-102 0 0,0 0-386 0 0,0 0-166 0 0,0 0-32 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36969.387">9836 3547 3224 0 0,'-6'11'5642'0'0,"-7"14"-878"0"0,13-23-3930 0 0,-1-1-138 0 0,-29 28 3385 0 0,-31-14 128 0 0,32-13-2861 0 0,-118 22 765 0 0,99-14-1621 0 0,-90-3 1168 0 0,18-23-712 0 0,-119 2-243 0 0,132 17-482 0 0,-27 1 141 0 0,44-5-364 0 0,-162 8 0 0 0,157 3 0 0 0,-253-7 0 0 0,192 1 228 0 0,-51-31 541 0 0,114 17-750 0 0,-55-4-19 0 0,103 7 0 0 0,24 6 0 0 0,0-2 0 0 0,0-1 0 0 0,0-1 0 0 0,1 0 0 0 0,-7-5 0 0 0,17 7 0 0 0,-34-14 0 0 0,-2 4 0 0 0,1 2 0 0 0,-1 3 0 0 0,0 1 0 0 0,-13 3 0 0 0,-24 7 0 0 0,25 3 0 0 0,-76-8 0 0 0,76-2 0 0 0,-67 7 0 0 0,44 10-21 0 0,2-3-5 0 0,-28 0-287 0 0,75-4 334 0 0,-11-1 286 0 0,-67-12-307 0 0,28-7-103 0 0,3 11-9 0 0,47 6 23 0 0,-4-3 89 0 0,-9 13 0 0 0,-50 6 73 0 0,46-10-143 0 0,3-2 403 0 0,4-9-333 0 0,16 4 0 0 0,-14-4-32 0 0,41 2-137 0 0,-2 9-3011 0 0,2-6 1857 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1488.941">12517 2225 3224 0 0,'0'0'389'0'0,"0"0"426"0"0,0 0 185 0 0,0 0 37 0 0,0 0-41 0 0,0 0-211 0 0,7 15 2921 0 0,1 0-2586 0 0,-7-14-544 0 0,-1 0 0 0 0,13 148 6159 0 0,-20 6-3759 0 0,5-42-1768 0 0,4 60 608 0 0,2 45-811 0 0,19 106 755 0 0,-10-183-1237 0 0,-7 21-2562 0 0,-6-171-744 0 0,0-8-6530 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="854.454">12511 2182 3224 0 0,'-3'-1'-2321'0'0,"0"-2"3355"0"0,-4-5 11775 0 0,9 6-10726 0 0,-1 1-1175 0 0,-1 1-164 0 0,10-2 590 0 0,105 15 3826 0 0,119-6-1952 0 0,0 0-2760 0 0,-67-11 16 0 0,-39-10 16 0 0,41-9 88 0 0,-23 6-187 0 0,37 1-162 0 0,-29 5-75 0 0,31-4 144 0 0,-5 2-149 0 0,-41 2-22 0 0,58-6-205 0 0,-5 11 211 0 0,49 5 714 0 0,-26 8-953 0 0,36 10-59 0 0,-146-3 482 0 0,5-11-635 0 0,-9 1 267 0 0,74 19 74 0 0,-27-1-13 0 0,19-2-88 0 0,15-10 152 0 0,11-10-64 0 0,-68-3 0 0 0,-38-4 0 0 0,148-3 0 0 0,-102 7 0 0 0,66 2 0 0 0,-124 11 0 0 0,63-3 0 0 0,-9 0 0 0 0,-53 8 0 0 0,51 5 0 0 0,-77-8 0 0 0,50-1 0 0 0,33 1 0 0 0,8 1 0 0 0,-65-7 400 0 0,-6 1-480 0 0,65-11 133 0 0,-11 1-106 0 0,-93 3 53 0 0,52-1-64 0 0,-19-4 64 0 0,-18 2 11 0 0,65 1 375 0 0,-58-15-452 0 0,-25 11 108 0 0,32-4-95 0 0,-36 10 53 0 0,-24 19-245 0 0,-2-15 238 0 0,2-4 7 0 0,-1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,10 61 0 0 0,-1-27 0 0 0,-10 4 0 0 0,16 3 0 0 0,-20 3 0 0 0,7-27 0 0 0,-1-9 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 5 0 0 0,-9 82-11 0 0,-7-3-42 0 0,15-3 53 0 0,8 36 0 0 0,0-59 0 0 0,-3-8 12 0 0,0-52 4 0 0,-1 40 108 0 0,-29 62-44 0 0,18-59-80 0 0,4-38 0 0 0,-2 21 0 0 0,6 34 0 0 0,11-32 0 0 0,-7 3 0 0 0,-6-26 0 0 0,3 1 0 0 0,-2 29 99 0 0,1-29 95 0 0,-7 13-174 0 0,3-7 27 0 0,7-8-47 0 0,5-2 0 0 0,1-1 0 0 0,-6-1 0 0 0,5-3-20 0 0,-4-2-73 0 0,-2-1 7 0 0,-2 0-3 0 0,1 0-9 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 98 0 0,4-6-6888 0 0,-3 1-1987 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6517.426">12583 3720 7688 0 0,'0'0'349'0'0,"0"0"-2"0"0,0 0-90 0 0,0 0 455 0 0,0 0 227 0 0,0 0 42 0 0,13 5 4082 0 0,49-12-625 0 0,2 6-2566 0 0,-13 4-1407 0 0,110-3 623 0 0,-13 5-464 0 0,-41 12 788 0 0,23-6-770 0 0,155-36 656 0 0,-179 25-914 0 0,-56 3-169 0 0,117-13 21 0 0,-19-2-119 0 0,-85 21-53 0 0,9 4 128 0 0,-27-6-192 0 0,43 4-8 0 0,47-1 144 0 0,-55 3-136 0 0,10 0 32 0 0,-61-9 64 0 0,10-4-335 0 0,9 4 142 0 0,17 7 97 0 0,-3-8 168 0 0,71-14-96 0 0,-70 5-8 0 0,8-5-240 0 0,-12 17 64 0 0,32-15 96 0 0,-6-1 167 0 0,27-3-62 0 0,-63 13-25 0 0,97-18-57 0 0,-87 8-318 0 0,94 5 639 0 0,36-2-696 0 0,-25 21 1344 0 0,-54-5-976 0 0,-14-3 0 0 0,-6-3 0 0 0,15 7 200 0 0,-52 3-40 0 0,181 4-64 0 0,-25-9 203 0 0,-144-11-246 0 0,62 13 139 0 0,117-7-128 0 0,-132-6 428 0 0,-1-5 0 0 0,2-8-492 0 0,28-1 0 0 0,136-24-11 0 0,-160 24-42 0 0,13 1 53 0 0,-42 11 0 0 0,-69 3 0 0 0,0 2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 3 0 0 0,17 3 0 0 0,63 6 0 0 0,14-3 0 0 0,51 0 0 0 0,-94-9 0 0 0,-41-6 0 0 0,8-1 0 0 0,33-7 0 0 0,-18 6 0 0 0,-41 7 0 0 0,-5 0 0 0 0,5 0-16 0 0,-10 0-68 0 0,-1 0-32 0 0,14 3-689 0 0,-18 1-1817 0 0,-7 5-1623 0 0,-23 7 1843 0 0,-6-4-20 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">246 638 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="310.099">638 654 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-8 10039 0 0,4 3-11103 0 0,-2 0-133 0 0,2 0-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="684.255">1033 598 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1921.293">1380 678 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,4-21-839 0 0,-7 30-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 76 971 0 0,12-75-904 0 0,2-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,5-15-522 0 0,2-29 325 0 0,-7 43 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 35 365 0 0,9-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-41 40 0 0,-1 46 757 0 0,-8 6-562 0 0,-2 1-34 0 0,13 14 96 0 0,-22 50 294 0 0,9-62 48 0 0,0-2-24 0 0,-12 9 14 0 0,11-9-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-2-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-2 1-12 0 0,0-1-1 0 0,1 0 1 0 0,0-1-1 0 0,-2 1 0 0 0,3 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-3 1 0 0,16-18-798 0 0,-5 22 705 0 0,11 17 39 0 0,-21-14 64 0 0,1 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 3-10 0 0,1-5 84 0 0,-4 17 237 0 0,-21-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 12-3207 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8390.611">1673 404 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 55 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,1 16 113 0 0,-2-14-1404 0 0,-1 50 981 0 0,-4-3-1688 0 0,1-56-1417 0 0,-2-31 962 0 0,-7-27-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8997.239">1609 535 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-32 2722 0 0,-14 31-3180 0 0,15-13 1008 0 0,23-26 674 0 0,-35 37-2057 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 2 1 0 0,-1-2 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 18 1009 0 0,-52 14 55 0 0,-5-17-600 0 0,22 45 1448 0 0,-23 2-2113 0 0,-15-59 230 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 21 399 0 0,1-10-337 0 0,8-8-104 0 0,-3-1 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,3 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 37 0 0,-34-1 653 0 0,-9-24-4978 0 0,35 18 2334 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11709.08">2997 370 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 46 1154 0 0,-12 23 2052 0 0,-3 33 1755 0 0,3 50-2463 0 0,4-53-962 0 0,-3 31-1172 0 0,7-135-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-2 13-2556 0 0,0-23 1622 0 0,2-1-894 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12315.019">3015 426 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-3 772 0 0,-14 9-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-3 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 2 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,3 5-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 2-174 0 0,-2 33 278 0 0,-1-40-199 0 0,1-2 0 0 0,-1 2 1 0 0,0-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,-1-1 1 0 0,3 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-3-1-4 0 0,-55-43-4198 0 0,56 41-3651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10346.212">2223 76 3680 0 0,'-6'46'613'0'0,"2"-9"6816"0"0,-8 23-4591 0 0,9 15-23 0 0,3-12-297 0 0,4 3-1604 0 0,-8 92 2 0 0,7-75 200 0 0,0-17-716 0 0,4-40-126 0 0,-7-20-115 0 0,-4 1-1048 0 0,1 4-4224 0 0,3-11 3723 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10997.838">2148 629 1376 0 0,'4'-20'2159'0'0,"5"1"4223"0"0,4-7-3735 0 0,-2 7-1523 0 0,12-17 1153 0 0,4 13 523 0 0,-4 1-1591 0 0,22-16 135 0 0,-44 37-1294 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 1-1 0 0,3-1 0 0 0,-1 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-2-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 1 0 0,0 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-3 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-2 1 0 0,0 1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 7-27 0 0,9 28 368 0 0,31 117 1443 0 0,-21-120-1634 0 0,1-14-84 0 0,-14-23-77 0 0,-5-1-29 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,2 0 0 0 0,1 1 0 0 0,-3-1 0 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,3 0 0 0 0,-1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 13 0 0,38-27-350 0 0,20-12-3834 0 0,-54 35 2533 0 0,3 3-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32289.342">1 248 6448 0 0,'7'20'6309'0'0,"-7"-17"-6682"0"0,5 53 3514 0 0,6 81-847 0 0,0-42-690 0 0,-7-10-929 0 0,13 128 737 0 0,-27 31 57 0 0,5-171-1337 0 0,-1-45-256 0 0,6-13-955 0 0,0-12-4480 0 0,0-3-582 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35199.426">13 278 6248 0 0,'0'12'190'0'0,"0"-22"349"0"0,17-37 6274 0 0,-17 45-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,11-3 291 0 0,73-18 828 0 0,-39 5-729 0 0,13-3 96 0 0,49 10 370 0 0,-60 8-222 0 0,42 2-1079 0 0,-20-6 16 0 0,36-20 451 0 0,-30 16 1144 0 0,61 0-1448 0 0,4 19 224 0 0,-53-19-645 0 0,-30 0 1538 0 0,6-1-1123 0 0,-36 8-292 0 0,51 0 264 0 0,-24-6 20 0 0,53-25 70 0 0,11 18-205 0 0,13 8 34 0 0,-66-3 219 0 0,22-6-424 0 0,-5 12 192 0 0,-9 5 584 0 0,43 1-1352 0 0,-7 9 736 0 0,2 5 1017 0 0,-34-9-298 0 0,-11-1-1239 0 0,26-3 520 0 0,15 3 64 0 0,12 28 75 0 0,-61-10-166 0 0,16-1 523 0 0,-5-7-840 0 0,-21-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,73-10-197 0 0,-21 19 0 0 0,-41-14-20 0 0,-45-2 0 0 0,-11-5 0 0 0,24 16 0 0 0,-38-2 0 0 0,5 5 0 0 0,13 23 64 0 0,-5 27 0 0 0,-9 22-64 0 0,-2 30-8 0 0,-3-48 125 0 0,-1 31-203 0 0,-10 32 295 0 0,10 43-190 0 0,-18-81 82 0 0,0-40-13 0 0,4-42 96 0 0,7-13-234 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1-1 0 0 0,-1 1-1 0 0,-1 1 51 0 0,0-2 114 0 0,2 0 0 0 0,-3 0 0 0 0,1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1-1 0 0 0,1 0-114 0 0,-15 0 158 0 0,-97 8-218 0 0,81-3 59 0 0,-1-1-1 0 0,2-2 1 0 0,-1-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-22-6 1 0 0,4-3-9 0 0,-2 3 0 0 0,2 2 0 0 0,-1 2 0 0 0,-22 2 9 0 0,-111 0 332 0 0,138 4-330 0 0,1-1-1 0 0,-2-3 1 0 0,1-2-1 0 0,0-1 1 0 0,-8-6-2 0 0,23 8-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-20 4 18 0 0,-143 29 64 0 0,-4-12-136 0 0,-46-9 152 0 0,171-12-80 0 0,-91 0 11 0 0,-34-16 42 0 0,101 16-53 0 0,-23-12 80 0 0,22-12-176 0 0,-85-17 224 0 0,57 22-196 0 0,62 6 192 0 0,-62-4-124 0 0,51 11 0 0 0,45 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="78758.085">3766 836 13560 0 0,'0'0'306'0'0,"-12"-2"752"0"0,-24-5-12 0 0,35 7-11 0 0,-8-6 1119 0 0,9 5 2052 0 0,65 4-3188 0 0,30-6 262 0 0,160 30 512 0 0,-136-20-1336 0 0,154 25-663 0 0,-48 8 353 0 0,-6-7 891 0 0,-124-30-445 0 0,-76-3-541 0 0,-1-1 0 0 0,1 0 0 0 0,-1-2 1 0 0,1 0-1 0 0,-1-1 0 0 0,10-4-51 0 0,72-34-278 0 0,-97 41 89 0 0,-3 1-156 0 0,3 0-611 0 0,0 1-1432 0 0,-2-2-4991 0 0,-1 1-504 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="79175.854">5363 556 6448 0 0,'0'0'498'0'0,"1"-1"-28"0"0,30-3 10100 0 0,24 22-6654 0 0,-34-9-3356 0 0,3 1 0 0 0,-2 1 1 0 0,0 1-1 0 0,-2 1 0 0 0,1 0 0 0 0,5 6-560 0 0,59 53 264 0 0,-77-62-125 0 0,-1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,-2 0 1 0 0,0-1-1 0 0,1 1 1 0 0,2 12-139 0 0,-5-12 187 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-3 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,-3 0 1 0 0,2 0-1 0 0,-2 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,-1-1-1 0 0,0 0 1 0 0,-4 7-188 0 0,-25 28 165 0 0,-33-7 587 0 0,-89-22 352 0 0,124-18-1542 0 0,-23 5-2761 0 0,47 0 2491 0 0,-28 11-2399 0 0,17-3-3298 0 0,4 1-1217 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37346.914">6693 824 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,21-14-8855 0 0,-15 9 1888 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37618.204">7066 866 10592 0 0,'-13'-11'818'0'0,"10"7"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37903.659">7413 780 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,4 0-232 0 0,0 0-5476 0 0,-5 0-2114 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38875.93">7776 866 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-9-13 464 0 0,13-39 1231 0 0,1 44-2463 0 0,-2 2 0 0 0,3 0 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-5-189 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 4-113 0 0,1-4 41 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-14-143 0 0,-13 31-62 0 0,1 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-3-1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-1-43 0 0,3 1 32 0 0,1 9 23 0 0,-11 19 200 0 0,4-27-96 0 0,-6 4-695 0 0,12-7-611 0 0,9-10-5710 0 0,-6 6 446 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="44618.988">8058 509 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 21-45 0 0,-12-24-3788 0 0,3 8 1039 0 0,3 80 1637 0 0,7 80-1221 0 0,-14-82-1606 0 0,0-78-341 0 0,-2-3-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53832.509">8358 549 2760 0 0,'4'8'1828'0'0,"4"19"4892"0"0,4 25-3444 0 0,3 99 1947 0 0,-12-78-3937 0 0,-6-35-4508 0 0,3-35 1701 0 0,-4 5-229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54557.219">8411 866 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,8-37 5734 0 0,5-11-521 0 0,-17 19-3279 0 0,10 9-1202 0 0,9-35 1 0 0,-13 54-738 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,3 0-93 0 0,1-2 95 0 0,-5 3-21 0 0,27 0-60 0 0,1 13-14 0 0,-5 8 0 0 0,-20-12 0 0 0,10 22 0 0 0,20 71 514 0 0,-20-50 356 0 0,5-17-278 0 0,-18-34-517 0 0,4 3 98 0 0,-2-2-141 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,3-1 0 0 0,-1 1-1 0 0,-2-1 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-28-4233 0 0,-22 31 2840 0 0,0 1-164 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56701.452">9196 603 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-38-6 1747 0 0,40 9-1667 0 0,7-2 170 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-3-1 0 0 0,1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,3 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 40-483 0 0,18 3 618 0 0,16 11 378 0 0,10 4-513 0 0,15-4 1899 0 0,26-10-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 1 0 0 0,-22-9 0 0 0,-2 2 0 0 0,0-5-64 0 0,30-21-5497 0 0,-31 15 3530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57367.528">9460 926 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-16 649 0 0,-9 18-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 19 784 0 0,-16 13 56 0 0,6-31-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="64361.857">9731 596 1840 0 0,'0'5'396'0'0,"0"-3"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 70 1352 0 0,-5-52-2105 0 0,-9 61 686 0 0,-2-6-314 0 0,3 65-530 0 0,6-108-273 0 0,-3-11 0 0 0,-6-11-45 0 0,4-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-2-14-1557 0 0,1-1 195 0 0,-2 0-70 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="69762.645">9697 598 1376 0 0,'4'6'367'0'0,"-4"-5"1002"0"0,0-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,2 0 1 0 0,-2 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,9-7 51 0 0,33-22 1588 0 0,-29 23-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,1 2 108 0 0,2 1-1 0 0,-1 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,1-1-1 0 0,-2 0 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,2-1-1 0 0,-3 1 0 0 0,0 1 0 0 0,1-1 1 0 0,0 6-108 0 0,9 26 435 0 0,0 56 787 0 0,-11-79-980 0 0,0-12-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1-56 0 0,-43 35 929 0 0,42-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-2 0 1 0 0,3 0 0 0 0,-2 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-2-1 0 0 0,1 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,2 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-3-1 0 0 0,3 0 0 0 0,-3 0 0 0 0,1 0 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-3-4 0 0 0,5-16-5381 0 0,0 15-2125 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70961.788">10171 338 0 0 0,'-12'11'0'0'0,"7"-14"140"0"0,2 3 2586 0 0,3 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 29 3000 0 0,-14 30-1947 0 0,1 48 181 0 0,4 2 624 0 0,-6-40-881 0 0,9 37-1316 0 0,-11-26-173 0 0,8-42 0 0 0,14 3-2476 0 0,-12-39 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,2 1-1 0 0,-2-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-2 0-1 0 0,2-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="71766.961">10154 754 4376 0 0,'0'0'199'0'0,"9"-10"1918"0"0,-5-3 1016 0 0,11-9 683 0 0,-6-13-1297 0 0,-2-1-472 0 0,5 29-1272 0 0,-9 6-743 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-3-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 20 598 0 0,-25-15-674 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,2 7-227 0 0,6 89 608 0 0,-7-64-165 0 0,-1-10 997 0 0,27-2-1275 0 0,-6-26-165 0 0,7-1 0 0 0,12-10-60 0 0,-19 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73476.329">10779 632 2760 0 0,'0'1'207'0'0,"0"43"6763"0"0,0-43-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 12-344 0 0,-2 0 0 0 0,0 0 1 0 0,-2 1-1 0 0,0 0 1 0 0,-1-2-1 0 0,-2 11-1278 0 0,-12 60 616 0 0,0-17 973 0 0,14 37-2158 0 0,1-84 962 0 0,-2-25-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="74025.376">10843 625 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,57-24 1867 0 0,-54 26-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,-2 0 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-2 0 0 0 0,3 1-156 0 0,-2 0 96 0 0,3 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-2 1-1 0 0,2 1 1 0 0,-1-2-1 0 0,0 1 1 0 0,0 1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,2 1-95 0 0,-2-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 4-94 0 0,-43 57 1952 0 0,47-65-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128695.154">5890 1434 4144 0 0,'0'0'319'0'0,"-7"7"1871"0"0,2-2 3495 0 0,-27-2-688 0 0,1-4-2621 0 0,2-15 488 0 0,-17 8-1852 0 0,-8-2 1272 0 0,-24-14-812 0 0,3 6-939 0 0,0 1 998 0 0,-5 0-1171 0 0,-9 11-360 0 0,-116 12 1824 0 0,110 7-1887 0 0,39-8 230 0 0,-34-9-256 0 0,8-6 82 0 0,13 7 87 0 0,24 3-80 0 0,-75-13 0 0 0,51-2 0 0 0,-9 6 0 0 0,50 2 0 0 0,13 5-60 0 0,11 2-440 0 0,5 5-11674 0 0,-1-4 3997 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129337.391">4416 1113 8288 0 0,'0'2'227'0'0,"-1"-1"0"0"0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,2 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,0 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-3 0 0 0 0,2-1 0 0 0,0 1-227 0 0,-20 1 2894 0 0,14 2-2512 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,2 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,2 1 0 0 0,-7 5-381 0 0,-3 3 422 0 0,-15 13 408 0 0,-37 32 222 0 0,17-4-867 0 0,47-30 92 0 0,2-22-266 0 0,0-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-2-1-1 0 0,3 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-11 0 0,26 11 26 0 0,95 20-304 0 0,-47-10-3852 0 0,-21 7-1623 0 0,-39-15 3707 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="133691.162">6028 3653 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-10 0 710 0 0,-68 11 2232 0 0,-103-9 113 0 0,76-16-2111 0 0,101 12-1711 0 0,-1 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,2 1-1 0 0,-3-1 1 0 0,2 1 0 0 0,-1 0-1 0 0,0 0-7 0 0,0 0 3 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-2 0 1 0 0,3 0 0 0 0,-1 0 0 0 0,-4-1-3 0 0,-4-1 53 0 0,-56 15 746 0 0,-5-31-422 0 0,-46 18 95 0 0,21 17-267 0 0,-3-26 255 0 0,19 7-262 0 0,-6-6 515 0 0,25 23-785 0 0,-8-10 316 0 0,71-3-237 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,2 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,2 0 0 0 0,-2 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,0 5-384 0 0,1 0-2483 0 0,-1-5 1589 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="134078.302">4789 3399 12384 0 0,'-13'-11'1277'0'0,"-2"9"-438"0"0,-16 9 3998 0 0,10 3-3431 0 0,-23 13 690 0 0,-50 37-1014 0 0,26-28 402 0 0,6 19-1322 0 0,35-24-154 0 0,-10 15 872 0 0,34-40-855 0 0,2 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1-2 0 0 0,-2 2 0 0 0,2-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-2-1 0 0,1 3-23 0 0,37 38 389 0 0,-28-35-394 0 0,0 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0-1 0 0 0,0-1 1 0 0,1 1-1 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,0-1-1 0 0,6 0 4 0 0,-6 0-173 0 0,104 17-1371 0 0,-42 3-4118 0 0,-58-15-1845 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136187.119">3947 2767 2760 0 0,'9'14'125'0'0,"-23"-7"1798"0"0,-7 9-59 0 0,17-9 428 0 0,-27 5 4862 0 0,31-12-6578 0 0,0 0-15 0 0,0 0-34 0 0,-1 2 119 0 0,0-1-159 0 0,1-1 2989 0 0,56-15-1901 0 0,11 8-396 0 0,21 3-749 0 0,-23 1 156 0 0,41-1 469 0 0,22-4-497 0 0,-4-3-454 0 0,55-3 952 0 0,-52 8-543 0 0,-51-4-402 0 0,53-8 402 0 0,-69 7-745 0 0,3 11 112 0 0,-33-6 120 0 0,16 4 0 0 0,6-13 444 0 0,-25 4-280 0 0,14 0-164 0 0,-25 4 0 0 0,-6 6 0 0 0,19 6-1208 0 0,-28-4 877 0 0,8 3-1583 0 0,6 12-3659 0 0,-9-10 3847 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136591.973">5461 2323 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,9 22 9129 0 0,24-6-7935 0 0,-18-11-2328 0 0,61 29 1337 0 0,-60-23-2420 0 0,-7-6 346 0 0,2 0 1 0 0,-1 1-1 0 0,0 1 1 0 0,-2 0-1 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,4 7-255 0 0,7 66 1080 0 0,-27-5-224 0 0,-12-27-856 0 0,-27-2 327 0 0,-29-11 1242 0 0,8-14-2553 0 0,39-23-3117 0 0,24-1 2058 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="139663.33">12060 2826 8288 0 0,'11'-45'864'0'0,"-13"42"-720"0"0,4-9 1811 0 0,0 9 5703 0 0,63-2-3242 0 0,-25 5-4222 0 0,80 2 1838 0 0,5 8-1085 0 0,276-13 1101 0 0,-174-1-1030 0 0,-76 8-540 0 0,41-1-45 0 0,11-13 803 0 0,-45-20-1236 0 0,-153 28-64 0 0,-5 2-273 0 0,24-10-2694 0 0,-22 10 2502 0 0,8 0-15 0 0,-5 4-3511 0 0,0 2-4432 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="140326.574">13849 2403 8288 0 0,'0'0'638'0'0,"0"1"-414"0"0,-2 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,7 6 488 0 0,69 15 2067 0 0,-42-15-2223 0 0,51 23 954 0 0,-53-9-1577 0 0,43 37 370 0 0,-19 1-375 0 0,30 32 240 0 0,-83-87-712 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 0 0 0,2 1 1 0 0,-3 0-1 0 0,2-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-23 0 0,-5 4 44 0 0,0 0 1 0 0,0-2-1 0 0,-1 2 0 0 0,0-1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0-1-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-2-1 0 0 0,1 0-44 0 0,-27 11 59 0 0,0-3-1 0 0,0-1 1 0 0,-1-1 0 0 0,-1-3-1 0 0,1-1 1 0 0,-18-1-59 0 0,30-4-59 0 0,-75-9-1395 0 0,89 3-1171 0 0,11 5 1267 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151416.768">14974 2518 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-12 7 790 0 0,-14 10 150 0 0,-49 20 1099 0 0,6-4-1196 0 0,66-31-1165 0 0,-13 9 158 0 0,0 0 0 0 0,1 1-1 0 0,0 0 1 0 0,1 1 0 0 0,1 0 0 0 0,1 2 0 0 0,-1 0 0 0 0,1 0-1 0 0,-6 11-202 0 0,15-21 65 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,3 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 1-64 0 0,1 1 108 0 0,1 0 0 0 0,-1 1-1 0 0,2-2 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,1 0-1 0 0,-1-2 1 0 0,1 2 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,10 2-107 0 0,-5-2 42 0 0,-1-1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 0 0 0 0,9-2-41 0 0,23-18-4007 0 0,-37 14-3607 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="152065.555">15162 2850 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-4-9 655 0 0,4 3-930 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 2 0 0 0,2-2 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 2 0 0 0,1-2 0 0 0,0 1 0 0 0,2-1-345 0 0,-4 2 74 0 0,-1 0 0 0 0,-1 0-1 0 0,2 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,2 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 1-1 0 0,1-1 1 0 0,-3 0 0 0 0,2 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 2-73 0 0,2 4 95 0 0,-1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 9-95 0 0,-13 68 1049 0 0,12-80-938 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-2-2-1 0 0,1 2 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-111 0 0,1-3 23 0 0,0 0 0 0 0,2 0 0 0 0,-3 0 1 0 0,2-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-3 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-2-1-24 0 0,0-1-63 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 2 1 0 0,-1-2-1 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0-1-1 0 0,2 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-6 63 0 0,7-22-2404 0 0,-5 16 1056 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153048.506">15674 2532 0 0 0,'-4'-6'-1709'0'0,"2"-5"9298"0"0,3 10 1867 0 0,-1 12-7849 0 0,4 99 2619 0 0,-7-24-3124 0 0,7 9 60 0 0,-9 39-1060 0 0,14-66-102 0 0,-6-62-68 0 0,-2-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153375.191">15651 2744 2304 0 0,'0'0'464'0'0,"4"-7"3648"0"0,-3 4 1786 0 0,28-40-750 0 0,12 4-2447 0 0,4 12-1313 0 0,-23 31-788 0 0,-20-4-482 0 0,0 1-42 0 0,3 2-30 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 0 0 0,-1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 1-46 0 0,24 85 1079 0 0,-14-64-711 0 0,-11-13-53 0 0,21 62 642 0 0,0-36-721 0 0,12-28-183 0 0,38-39-1154 0 0,-28-3-4448 0 0,-32 22 3543 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160253.303">16421 2358 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,6 2 583 0 0,-2-7-849 0 0,-4 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 15-2962 0 0,1 58 539 0 0,-6 67 472 0 0,-7 14 1084 0 0,10 76-784 0 0,10-186-592 0 0,2-24-84 0 0,12-17 3 0 0,-15-9-156 0 0,1 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-3 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,3-3-35 0 0,49-39 80 0 0,-43 34-172 0 0,-8 8-92 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,-1-2 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1-3 184 0 0,2 0-1288 0 0,-1-8-6336 0 0,-4 11 565 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160816.746">16425 2573 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,62-5 2910 0 0,-44 4-3513 0 0,6 0-489 0 0,-9 4-4783 0 0,-5 1-1037 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="165875.957">16937 2595 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,4 5 4769 0 0,0 0-4077 0 0,-1-1-1648 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 2-394 0 0,-6 178 4855 0 0,1-66-3199 0 0,0-89-1224 0 0,6-10-3265 0 0,-1-13 1400 0 0,0-7-5540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="166400.987">16975 2823 456 0 0,'2'-10'295'0'0,"-1"8"1230"0"0,6-14 4652 0 0,-6 15-4821 0 0,8-15 3233 0 0,-3 6-3731 0 0,20-33 2412 0 0,-24 41-3133 0 0,-1-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-137 0 0,40 1 1322 0 0,-39 1-1262 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-3 1-1 0 0,2-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 2-59 0 0,22 18 91 0 0,-8 2-240 0 0,-17-24-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167273.982">17464 2886 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 1 0 0,2 0-1 0 0,0 1 0 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 2-1 0 0,0-2 0 0 0,2 1 0 0 0,-3-1 0 0 0,2 1 0 0 0,2-3-329 0 0,12-26 1366 0 0,21-3-185 0 0,-35 35-1119 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,3 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,2 2-62 0 0,46 62 531 0 0,-45-51-291 0 0,2-2-1 0 0,-3 2 1 0 0,1 1 0 0 0,-1-1-1 0 0,-2 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-2 10-239 0 0,-7 39 0 0 0,-13-23 1095 0 0,1-43-406 0 0,14 1-606 0 0,1 1-72 0 0,-1 0 0 0 0,1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 0 0 0 0,-3-2-11 0 0,2 0-209 0 0,2 1 0 0 0,-2 0-1 0 0,1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-5 209 0 0,0-20-4042 0 0,2 15-3529 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167927.933">17974 2281 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,3 8 590 0 0,12 64 2596 0 0,-22 143-2669 0 0,-1-73 14 0 0,8 82-1117 0 0,4-174 0 0 0,-2-45-165 0 0,0-4-698 0 0,-2-1-315 0 0,1-1-1352 0 0,2-5-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="189572.02">18272 2801 3568 0 0,'22'-10'1553'0'0,"-7"-6"1718"0"0,-2 11-2487 0 0,42-31 3450 0 0,-26 9-3218 0 0,35-42-474 0 0,-53 46-542 0 0,-8 15 0 0 0,-6-1 0 0 0,2 6-7 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,3 1 1 0 0,-5 0 6 0 0,0 2 11 0 0,-1-1 1 0 0,1 2-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 2 1 0 0,1-1-1 0 0,0 1 1 0 0,-4 5-12 0 0,-14 24 272 0 0,-7 53 161 0 0,28-82-291 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,2-1 0 0 0,-2 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,2-1-142 0 0,-2-1 13 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 1 0 0,1-1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,3 0-13 0 0,68-24-2033 0 0,-62 16 586 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190134.967">18742 2525 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-1 1-172 0 0,-17 52 5027 0 0,10-27-3083 0 0,-7 32 478 0 0,12-49-2198 0 0,1 2 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,2 6-320 0 0,-2 25 797 0 0,-1-36-713 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-2 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,5 3-83 0 0,-7-7 16 0 0,0 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-2 0 1 0 0,1-1-1 0 0,1-2-15 0 0,6-4 20 0 0,19-32 87 0 0,13-38-97 0 0,-36 71-49 0 0,0 1 0 0 0,-1-1-1 0 0,0-1 1 0 0,1 1 0 0 0,-3-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-5 39 0 0,-4-22-1383 0 0,4 35 837 0 0,-1 0-1200 0 0,-6-5-4721 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192408.343">17375 2358 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,2-1-292 0 0,4-4-365 0 0,3-2-1 0 0,-2 1 1 0 0,-1-1 0 0 0,3-1-1 0 0,-4 1 1 0 0,1-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-363 0 0,50-75 852 0 0,-40 66-781 0 0,-1 15-61 0 0,-11 6 2 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 2-11 0 0,2 2-4 0 0,7 24 57 0 0,1-3-53 0 0,6 0-1856 0 0,-10-23-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="211829.387">8050 2582 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-12-2-24 0 0,8 2 8851 0 0,1 5-9133 0 0,-9 14-17 0 0,7-16-769 0 0,4-2-3236 0 0,1-1-1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-211952.654">20797 2883 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-8 0-423 0 0,2-2-329 0 0,4 2-272 0 0,-1-3-398 0 0,1-1-3749 0 0,-3-8 2451 0 0,4 10-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212149.586">20514 2615 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-14-3 2088 0 0,-5-4-821 0 0,17 7-1285 0 0,-13 3 543 0 0,-34 27 578 0 0,-5 47-1009 0 0,54-69-646 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,3 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,3 0 0 0 0,-2-1 0 0 0,1 2-74 0 0,27 23 398 0 0,-29-29-397 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,2-1-1 0 0,7 1-134 0 0,-8-1-167 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-2-1 0 0,-2 1 1 0 0,2 0 301 0 0,-5 2-105 0 0,15-8-1239 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205932.193">21011 2655 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,6 8 1656 0 0,-5-6-2461 0 0,1 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 2-229 0 0,2 71 2716 0 0,19 156 1049 0 0,-30-72-3749 0 0,-1-90-16 0 0,-2 20 0 0 0,13-85-64 0 0,1-3-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205389.214">21041 2728 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,4-7 616 0 0,22-27 2026 0 0,-4 17-2035 0 0,-19 16-1214 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-3-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,3 1 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,3 0 0 0 0,-1 0-84 0 0,3 5 138 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 1 0 0 0,-4 0 0 0 0,2-1 0 0 0,-1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,-4 7-137 0 0,5-12 22 0 0,0 1-1 0 0,-1-2 0 0 0,1 1 1 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,-2 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0-21 0 0,-38 9 162 0 0,36-10-192 0 0,3 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,1-1-1 0 0,-5-1 30 0 0,-13-31-3512 0 0,17 22 1769 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-204187.105">21512 2476 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203902.979">21492 2452 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203901.979">21477 2556 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203439.752">21444 2367 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,4 11 2392 0 0,14 78 1583 0 0,-17 33-1639 0 0,9 43-192 0 0,13-21-2656 0 0,-26-126 0 0 0,-1-3-337 0 0,3-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202468.889">21481 2780 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-2-17 3737 0 0,5-3 4077 0 0,8-22-4186 0 0,8 2-1366 0 0,-1 19-2142 0 0,-10 19-211 0 0,-8 7 222 0 0,20-9 1281 0 0,9 11-1444 0 0,-26 1-105 0 0,47 31-8 0 0,-24-3 744 0 0,-11-4-56 0 0,7 34-96 0 0,-14-20-16 0 0,3 12 191 0 0,0-18-526 0 0,-1-4-59 0 0,-2-16-12 0 0,-6-13-90 0 0,17 3 16 0 0,18-2-96 0 0,-8-4-141 0 0,-28 2-596 0 0,28-10-4249 0 0,-15 4 1073 0 0,-8 2 1923 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201801.05">22089 2582 1376 0 0,'-16'6'65'0'0,"12"-5"277"0"0,4-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-6 11 5285 0 0,12 44-3424 0 0,-9-9-2068 0 0,-2 46 541 0 0,-5-51-877 0 0,6 2-432 0 0,5 22-1088 0 0,8 8 915 0 0,-3-3-416 0 0,-3-58-545 0 0,-5 18 164 0 0,-3-11-45 0 0,3-18-557 0 0,2-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-4 0-797 0 0,2 0-5332 0 0,2 0 728 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201246.613">22042 2631 456 0 0,'34'-10'12581'0'0,"-22"4"-11549"0"0,16 5 3076 0 0,-2-5-1928 0 0,31 39 262 0 0,-20 0-1426 0 0,-11 18-48 0 0,-9-18-336 0 0,-17-29-440 0 0,-3 27-53 0 0,-7-10-60 0 0,-9-8 791 0 0,18-11-867 0 0,0-1 1 0 0,-2 1-1 0 0,3-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 0-1 0 0,1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-2-1-1 0 0,1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-2-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,-2 1-3 0 0,-37-21-1713 0 0,14-1-2008 0 0,23 15 1827 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190828.747">19149 2549 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,3 14 1120 0 0,0 35 395 0 0,1 68 75 0 0,4-39-2940 0 0,4 7-252 0 0,-4-12-192 0 0,0-37-12 0 0,-8-34-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="191215.919">19164 2707 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,4-14 2209 0 0,12-3-1077 0 0,32-21 345 0 0,-19 31-1146 0 0,-5 21-314 0 0,-19-11-177 0 0,-1 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-37 0 0,-1-4 176 0 0,9 11 413 0 0,-9-12-998 0 0,11 6-4069 0 0,-12-7 3075 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="199554.903">19491 3003 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,7-4 224 0 0,-5 3 3136 0 0,10-10-3493 0 0,-10 8-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174270.903">19894 2655 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 12 8138 0 0,-3 35-5693 0 0,3-49-1919 0 0,-3 16 1214 0 0,-1 77 988 0 0,4-93-2320 0 0,0-2-72 0 0,0 7 75 0 0,-5 26-43 0 0,-2 43-122 0 0,7-73-45 0 0,0 0-235 0 0,0 0-3512 0 0,0-3-1706 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173620.241">19879 2794 5296 0 0,'5'7'472'0'0,"-5"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-22 1372 0 0,0 20-1542 0 0,0 0-40 0 0,6-28 954 0 0,-5 29-1144 0 0,13-27 1755 0 0,4 10-1413 0 0,-16 17-538 0 0,-2 1 0 0 0,0 0-6 0 0,15-2 374 0 0,-9 3-368 0 0,-3-1-159 0 0,-2 0 0 0 0,1 0-1 0 0,1 0 1 0 0,-3 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0 0 0 0,3 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,0 0 0 0 0,2 0-1 0 0,-3 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,2 1 0 0 0,-2-1-1 0 0,1 1-24 0 0,14 59 908 0 0,-11-27-544 0 0,-5-11-78 0 0,1-22-204 0 0,0 21 170 0 0,1-19-204 0 0,2 5-36 0 0,1-1-1 0 0,0 1 42 0 0,3-4 13 0 0,-4-3-58 0 0,1 0 1 0 0,-1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,3 1 0 0 0,-1-1 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,2-3-9 0 0,35-22-3222 0 0,-34 21-430 0 0,-4 5 1775 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="-165827.57">13990 3494 920 0 0,'0'0'411'0'0,"0"0"1389"0"0,0 0 609 0 0,0 0 119 0 0,0 0-215 0 0,0 0-1014 0 0,0 0-445 0 0,0 0-87 0 0,0 0-46 0 0,0 0-109 0 0,0 0-48 0 0,0 0-10 0 0,0 0 0 0 0,0 0 11 0 0,-15-2 1750 0 0,-7-1-885 0 0,-1 0-1 0 0,1 2 1 0 0,-1 0-1 0 0,1 1 1 0 0,-14 2-1430 0 0,-40 9 1057 0 0,-26-10-2 0 0,32-4-630 0 0,-85 0 196 0 0,35-7-298 0 0,38-9 8 0 0,68 15-305 0 0,0 1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 1 0 0 0,1 0 0 0 0,-3 0 0 0 0,1 2 0 0 0,2 0 0 0 0,-1 0-1 0 0,-5 2-25 0 0,-46 12 22 0 0,13-6 31 0 0,11-13 11 0 0,-79-2 64 0 0,57 27-128 0 0,-21 1 0 0 0,46-21 0 0 0,-11-5 0 0 0,-23 7 0 0 0,39 3 0 0 0,-13-12 0 0 0,-3-24 0 0 0,-7 28 0 0 0,4-3 0 0 0,35 3-632 0 0,15 1 769 0 0,-1 1-984 0 0,3 0-6440 0 0,6-2 5260 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-62540.216">6177 235 9240 0 0,'0'0'208'0'0,"0"0"33"0"0,0 0 14 0 0,0 0 69 0 0,0 0 284 0 0,0 0 120 0 0,0 0 28 0 0,0 0-30 0 0,0 0-139 0 0,0 0-62 0 0,0 16 1654 0 0,-7 120 2954 0 0,-3 15-3081 0 0,9 57-343 0 0,9 147 170 0 0,2-197-1465 0 0,-10-127-531 0 0,0-29-556 0 0,0-4-270 0 0,-4-25-3089 0 0,1 16 1904 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-50190.827">6144 270 3224 0 0,'0'0'387'0'0,"0"0"414"0"0,0 0 183 0 0,0 0 37 0 0,-12-2 2900 0 0,3 0 1482 0 0,5 5 686 0 0,21 7-5649 0 0,85-9 731 0 0,-34-11-391 0 0,69 6-160 0 0,50-5-302 0 0,-70-3-104 0 0,26 7 148 0 0,-7 3 150 0 0,-12 2-320 0 0,25 3-48 0 0,-27 4 171 0 0,65 15 58 0 0,-60-9 92 0 0,8-9 14 0 0,-8-11-479 0 0,-47 2 68 0 0,-61 2-39 0 0,0 2-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 1-1 0 0,1 1 1 0 0,10 2-29 0 0,38 5 0 0 0,32-5 0 0 0,-14 0 0 0 0,-7-1 0 0 0,-38 7 0 0 0,48-4 0 0 0,51-8 0 0 0,-99-1 0 0 0,44 5 0 0 0,-71 1 5 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-2-1 0 0 0,6-1-5 0 0,65-5 19 0 0,97 21-8 0 0,-107-7 95 0 0,20-6-31 0 0,-17-10-11 0 0,96 1 0 0 0,-82 2 0 0 0,8 1-64 0 0,-46-2 53 0 0,38-1-42 0 0,-45 9-11 0 0,59-4 0 0 0,20 0 0 0 0,-35 16 0 0 0,207-10 0 0 0,-131-19 0 0 0,-86 11 0 0 0,41-1 0 0 0,-28 11 0 0 0,-35 3 0 0 0,28-6 64 0 0,-4-6 128 0 0,62 5-192 0 0,-110 4 0 0 0,0-2 0 0 0,-26-2 0 0 0,-2 0-12 0 0,-5 0-53 0 0,-1 0-170 0 0,0 0-576 0 0,0 0-247 0 0,0 0-49 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-49193.598">11691 188 5928 0 0,'0'0'266'0'0,"0"0"1"0"0,0 1-171 0 0,0 4 92 0 0,0-4 732 0 0,-2 15 4758 0 0,4 13-1191 0 0,8 34 169 0 0,-13-10-3447 0 0,-4 116 1305 0 0,2-59-2021 0 0,0-8-60 0 0,3 50 591 0 0,9-33-728 0 0,-3-89-284 0 0,-3 2 204 0 0,-1-31-157 0 0,0-1 6 0 0,0 0-26 0 0,0 0-98 0 0,0 0-9 0 0,0 0 4 0 0,0 0 0 0 0,0 0-43 0 0,0 0-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0-98 0 0,0 0-410 0 0,0 0-182 0 0,0 0-42 0 0,0 0-73 0 0,0 0-285 0 0,0 0-126 0 0,0 0-983 0 0,0 0-3823 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-48911.614">11676 1067 456 0 0,'0'0'1737'0'0,"0"0"207"0"0,0 0 88 0 0,0 0-76 0 0,0 0-381 0 0,0 0-174 0 0,0 0-32 0 0,0 0-62 0 0,0 0-231 0 0,0 2-99 0 0,0 74 4474 0 0,5-45-4150 0 0,0 17 250 0 0,-3 2-1349 0 0,-4-22-20 0 0,2-20-172 0 0,0 4 904 0 0,0-12-2338 0 0,0 3-8055 0 0,0-3 3197 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-46458.211">11701 1295 3224 0 0,'-11'8'2653'0'0,"-43"18"4634"0"0,52-26-6665 0 0,0 0 33 0 0,-48-6 3329 0 0,-36 0 217 0 0,54 7-3372 0 0,-81-2 683 0 0,48-20 54 0 0,32 11-1308 0 0,14 5-82 0 0,2 1 1 0 0,-1 1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 2 0 0 0,1 0 1 0 0,-12 2-177 0 0,-15-1 177 0 0,-42-8 419 0 0,14-3-51 0 0,-62 6 350 0 0,26 11-662 0 0,16 3-169 0 0,12-3-64 0 0,-16-14 140 0 0,-62 6 320 0 0,49 2-460 0 0,7-13 83 0 0,18 0-30 0 0,32 6-53 0 0,-40 1 0 0 0,-64 5 0 0 0,-21-4 0 0 0,80 1 0 0 0,-1 5 0 0 0,-46-4 0 0 0,8-5 0 0 0,-146 7 0 0 0,198 4 0 0 0,-38-8 117 0 0,10-8 118 0 0,49 8-410 0 0,-108 8 326 0 0,104-8-162 0 0,-88-1 37 0 0,3 9-289 0 0,9 5 263 0 0,-37-1 208 0 0,67-1-413 0 0,-52-4 194 0 0,39-6 11 0 0,-39 21 344 0 0,77-4-608 0 0,-67 3 160 0 0,77-14 104 0 0,-38-3 968 0 0,15-10-1140 0 0,13 10-113 0 0,25 9 214 0 0,-43-4 71 0 0,74-6-97 0 0,25 2 121 0 0,4-1-4216 0 0,4 0-5767 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-41895.864">6310 2480 5264 0 0,'3'0'1129'0'0,"7"0"-2200"0"0,-6 0 4901 0 0,-3 1 4833 0 0,7 40-6741 0 0,-8 52 512 0 0,-8 20-998 0 0,16 99 1044 0 0,7-73-1600 0 0,-3-44-128 0 0,3 47-792 0 0,-8-68 515 0 0,-7-35 182 0 0,-5-14 138 0 0,0-15-1692 0 0,5-10-2271 0 0,2-7 1285 0 0,-1-2-408 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-39644.648">6271 2483 456 0 0,'0'0'1548'0'0,"0"0"185"0"0,0 0 82 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-42 0 0,0 0-140 0 0,0 0-57 0 0,0 0-16 0 0,0 0-1 0 0,0 0 12 0 0,0 0 2 0 0,0 0-1 0 0,0 0-47 0 0,0 0-202 0 0,0 0-92 0 0,3 0-11 0 0,51-7 2042 0 0,49 2 147 0 0,70 4-222 0 0,-24 10-1432 0 0,-19-15-175 0 0,143-11 402 0 0,-122-6-820 0 0,-55 7 18 0 0,-56 9-382 0 0,1 2 1 0 0,0 2-1 0 0,32 1 7 0 0,65 2 256 0 0,-92 0-256 0 0,45 0 181 0 0,-23 10-106 0 0,7-4 1 0 0,-3-2 68 0 0,57-1-1 0 0,-81 0-90 0 0,84-4 144 0 0,193-7-122 0 0,-259 11-75 0 0,45 7 0 0 0,21-7 0 0 0,-68 4 0 0 0,-4-2 0 0 0,58-5 0 0 0,16 0 0 0 0,-66 11 0 0 0,-23-4 64 0 0,66-18 0 0 0,-41 1-64 0 0,55-2-67 0 0,43 22 54 0 0,-96-11 13 0 0,-45-2 11 0 0,4 1-1 0 0,-4 1 1 0 0,1 1 0 0 0,0 1-1 0 0,26 4-10 0 0,10-2 11 0 0,79-6-74 0 0,-52-2 30 0 0,49 17 33 0 0,15-2 152 0 0,-92-3-152 0 0,-24-6-172 0 0,45 4 160 0 0,12-5 12 0 0,-28 0 0 0 0,-8-3 0 0 0,-24 3 0 0 0,2 0-16 0 0,-36 0-61 0 0,-2 0-6 0 0,0 0-138 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1739 0 0,0 0-6757 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-38736.343">11284 2434 1376 0 0,'0'0'65'0'0,"0"0"341"0"0,0 0 1404 0 0,0 0 611 0 0,9 0 3921 0 0,-6 1-6029 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 2-313 0 0,6 60 2731 0 0,20 118-151 0 0,-16-99-1558 0 0,-15 39 98 0 0,14 23 148 0 0,-4-75-785 0 0,-4-28-243 0 0,-2 25 129 0 0,1 21 111 0 0,-1-55-253 0 0,0-32-205 0 0,0-1-106 0 0,0 0-8 0 0,-19 20-828 0 0,19-20 767 0 0,-11 16-1455 0 0,10-15 1350 0 0,1-1-81 0 0,0 0-40 0 0,0 0-5 0 0,0 0-101 0 0,0 0-426 0 0,0 0-185 0 0,0 0-37 0 0,0 0-102 0 0,0 0-386 0 0,0 0-166 0 0,0 0-32 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36969.387">11366 3435 3224 0 0,'-7'11'5642'0'0,"-8"13"-878"0"0,15-22-3930 0 0,-1-1-138 0 0,-34 27 3385 0 0,-35-14 128 0 0,36-12-2861 0 0,-136 22 765 0 0,115-14-1621 0 0,-105-3 1168 0 0,22-23-712 0 0,-139 2-243 0 0,154 17-482 0 0,-32 1 141 0 0,51-5-364 0 0,-187 8 0 0 0,182 3 0 0 0,-294-7 0 0 0,223 1 228 0 0,-59-31 541 0 0,131 17-750 0 0,-63-3-19 0 0,119 6 0 0 0,28 6 0 0 0,0-2 0 0 0,-1-1 0 0 0,1 0 0 0 0,1-1 0 0 0,-8-5 0 0 0,19 7 0 0 0,-39-13 0 0 0,-2 3 0 0 0,1 2 0 0 0,-1 3 0 0 0,0 1 0 0 0,-15 4 0 0 0,-28 5 0 0 0,29 4 0 0 0,-88-8 0 0 0,88-2 0 0 0,-78 7 0 0 0,51 10-21 0 0,3-3-5 0 0,-33 0-287 0 0,87-4 334 0 0,-12-2 286 0 0,-77-10-307 0 0,31-8-103 0 0,3 11-9 0 0,55 6 23 0 0,-4-3 89 0 0,-11 13 0 0 0,-58 5 73 0 0,53-9-143 0 0,4-2 403 0 0,5-9-333 0 0,18 4 0 0 0,-17-4-32 0 0,48 2-137 0 0,-2 8-3011 0 0,2-5 1857 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1488.941">14464 2155 3224 0 0,'0'0'389'0'0,"0"0"426"0"0,0 0 185 0 0,0 0 37 0 0,0 0-41 0 0,0 0-211 0 0,9 14 2921 0 0,0 1-2586 0 0,-8-14-544 0 0,-1 0 0 0 0,15 143 6159 0 0,-23 6-3759 0 0,6-40-1768 0 0,4 57 608 0 0,2 44-811 0 0,23 103 755 0 0,-12-178-1237 0 0,-8 21-2562 0 0,-7-166-744 0 0,0-6-6530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="854.454">14458 2113 3224 0 0,'-4'-1'-2321'0'0,"1"-2"3355"0"0,-6-4 11775 0 0,12 5-10726 0 0,-2 1-1175 0 0,-1 1-164 0 0,12-2 590 0 0,120 14 3826 0 0,139-5-1952 0 0,-1 0-2760 0 0,-77-11 16 0 0,-45-9 16 0 0,47-10 88 0 0,-26 6-187 0 0,42 3-162 0 0,-33 3-75 0 0,36-4 144 0 0,-6 2-149 0 0,-47 3-22 0 0,67-6-205 0 0,-7 10 211 0 0,58 5 714 0 0,-30 8-953 0 0,41 9-59 0 0,-169-3 482 0 0,5-10-635 0 0,-9 1 267 0 0,85 19 74 0 0,-31-3-13 0 0,22 0-88 0 0,18-10 152 0 0,12-10-64 0 0,-79-3 0 0 0,-43-4 0 0 0,171-3 0 0 0,-119 7 0 0 0,78 2 0 0 0,-145 11 0 0 0,74-3 0 0 0,-11 0 0 0 0,-61 7 0 0 0,59 6 0 0 0,-90-9 0 0 0,58 0 0 0 0,39 0 0 0 0,9 2 0 0 0,-75-7 400 0 0,-8 1-480 0 0,77-11 133 0 0,-14 1-106 0 0,-107 3 53 0 0,60-1-64 0 0,-22-4 64 0 0,-21 2 11 0 0,75 1 375 0 0,-67-14-452 0 0,-28 10 108 0 0,36-4-95 0 0,-41 10 53 0 0,-28 19-245 0 0,-2-16 238 0 0,2-3 7 0 0,-2 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-2 1 1 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,2-1 0 0 0,10 59 0 0 0,0-26 0 0 0,-12 4 0 0 0,18 3 0 0 0,-22 2 0 0 0,7-25 0 0 0,0-9 0 0 0,-3 0 0 0 0,1 1 0 0 0,0-2 0 0 0,-1 2 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-2 5 0 0 0,-9 79-11 0 0,-9-3-42 0 0,17-3 53 0 0,10 36 0 0 0,0-59 0 0 0,-4-7 12 0 0,0-50 4 0 0,0 38 108 0 0,-35 61-44 0 0,22-58-80 0 0,4-36 0 0 0,-3 21 0 0 0,8 31 0 0 0,13-30 0 0 0,-9 3 0 0 0,-7-25 0 0 0,4 1 0 0 0,-2 27 99 0 0,0-27 95 0 0,-7 12-174 0 0,3-7 27 0 0,8-7-47 0 0,6-3 0 0 0,1 0 0 0 0,-7-1 0 0 0,6-3-20 0 0,-4-2-73 0 0,-3-1 7 0 0,-3 0-3 0 0,2 0-9 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1-1 0 0,-2 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1-1 0 0,2 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 98 0 0,5-6-6888 0 0,-4 2-1987 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6517.426">14541 3603 7688 0 0,'0'0'349'0'0,"0"0"-2"0"0,0 0-90 0 0,0 0 455 0 0,0 0 227 0 0,0 0 42 0 0,15 5 4082 0 0,56-12-625 0 0,3 6-2566 0 0,-15 4-1407 0 0,127-3 623 0 0,-14 5-464 0 0,-49 11 788 0 0,28-5-770 0 0,177-35 656 0 0,-205 24-914 0 0,-66 3-169 0 0,136-13 21 0 0,-22-2-119 0 0,-98 21-53 0 0,11 4 128 0 0,-32-7-192 0 0,49 5-8 0 0,55-2 144 0 0,-63 4-136 0 0,11 0 32 0 0,-71-10 64 0 0,12-3-335 0 0,11 4 142 0 0,19 7 97 0 0,-3-8 168 0 0,82-14-96 0 0,-82 5-8 0 0,10-4-240 0 0,-13 16 64 0 0,36-15 96 0 0,-7-1 167 0 0,32-2-62 0 0,-74 12-25 0 0,113-18-57 0 0,-101 9-318 0 0,108 4 639 0 0,43-2-696 0 0,-30 21 1344 0 0,-62-6-976 0 0,-16-2 0 0 0,-7-3 0 0 0,18 7 200 0 0,-61 2-40 0 0,209 5-64 0 0,-28-10 203 0 0,-167-10-246 0 0,72 13 139 0 0,135-7-128 0 0,-152-6 428 0 0,-2-5 0 0 0,2-7-492 0 0,33-2 0 0 0,157-22-11 0 0,-185 22-42 0 0,15 1 53 0 0,-48 13 0 0 0,-80 1 0 0 0,0 2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,19 5 0 0 0,74 6 0 0 0,15-3 0 0 0,60 0 0 0 0,-109-9 0 0 0,-48-6 0 0 0,10-1 0 0 0,38-7 0 0 0,-21 6 0 0 0,-47 7 0 0 0,-6 0 0 0 0,5 0-16 0 0,-10 0-68 0 0,-2 0-32 0 0,16 3-689 0 0,-21 1-1817 0 0,-8 5-1623 0 0,-26 7 1843 0 0,-7-5-20 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2473,33 +2485,33 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2006 764 2760 0 0,'0'0'531'0'0,"0"0"1186"0"0,0 0 519 0 0,0 0 106 0 0,0 0-166 0 0,0 0-792 0 0,0 0-346 0 0,0 0-70 0 0,0 0-47 0 0,0 0-163 0 0,0 0-71 0 0,0 0-14 0 0,0 0 10 0 0,0 0 42 0 0,0 0 13 0 0,0 9 699 0 0,-5 116 2364 0 0,10 24-1865 0 0,5 117-247 0 0,3-21-814 0 0,-10-50-319 0 0,-16-69 500 0 0,19-96-2539 0 0,-6-29 905 0 0,0-1-60 0 0,0 0-15 0 0,0 0-116 0 0,0 0-476 0 0,0 0-209 0 0,2 0-39 0 0,6-2-10 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2597.859">1857 679 4144 0 0,'0'0'319'0'0,"0"0"23"0"0,0 0 881 0 0,4-5 1496 0 0,0 3 846 0 0,42-24 2209 0 0,15 21-278 0 0,110-4-967 0 0,-100-1-3873 0 0,5-1-272 0 0,97-9 368 0 0,-40 17-373 0 0,-130 3-377 0 0,51 0 316 0 0,0-2-1 0 0,48-11-317 0 0,27-6 240 0 0,36-9-96 0 0,-46 18-73 0 0,-39 6 277 0 0,24 2-231 0 0,71-12 51 0 0,-32 4-88 0 0,-32 17-27 0 0,-51-1-42 0 0,-39-3 14 0 0,-2-2 0 0 0,1 0-1 0 0,1-2 1 0 0,-2 0 0 0 0,18-4-25 0 0,46-3 73 0 0,16 5 130 0 0,-63 3-371 0 0,49-10 88 0 0,45-23 197 0 0,-50 15-106 0 0,-32 12 42 0 0,104 8-170 0 0,-79-2 117 0 0,-22 5 64 0 0,77-3-64 0 0,40 5 0 0 0,-50-1 0 0 0,52-9 0 0 0,-50 10-64 0 0,3 0 75 0 0,-40 1 31 0 0,50-2-95 0 0,40 4 53 0 0,-31 10-160 0 0,-53-14 107 0 0,0-2-22 0 0,-9 7 11 0 0,34-9 53 0 0,-51 5-42 0 0,78-6-339 0 0,-16 6 280 0 0,32-3 32 0 0,-111-3 80 0 0,103 4 0 0 0,-27-15 177 0 0,-1-3-378 0 0,-17 15 201 0 0,-21-12 0 0 0,-39 2 46 0 0,1 1 0 0 0,0 4-1 0 0,11 1-45 0 0,68-2-5 0 0,19 1-127 0 0,-34-6 284 0 0,88-8-13 0 0,51 9-422 0 0,-129-1 407 0 0,10-3 201 0 0,-102 18-371 0 0,-25-5-57 0 0,7 0-101 0 0,-3 1 124 0 0,26 8 64 0 0,-7-1 16 0 0,-8 10 0 0 0,-7-2 0 0 0,2 23 0 0 0,-6 5 0 0 0,-9 6 0 0 0,-3 10 257 0 0,-1-14-154 0 0,7 20 193 0 0,-9 33-376 0 0,0-11-72 0 0,-4-5 152 0 0,-1 49 64 0 0,3-29-64 0 0,4-12 64 0 0,9-28-53 0 0,-5-3 42 0 0,1-3-53 0 0,-4 26 75 0 0,0-36 31 0 0,2-12-84 0 0,1-28 20 0 0,6-1-31 0 0,0 0-11 0 0,0 11-21 0 0,-3-16-85 0 0,0-2-15 0 0,0 0 1 0 0,-2 1-73 0 0,-4 4-309 0 0,4-4-135 0 0,2-1-31 0 0,-3 3-3225 0 0,3-3 2170 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4154.481">8975 1816 456 0 0,'0'0'1935'0'0,"0"0"230"0"0,0 0 105 0 0,6 0 2569 0 0,-14 0 1235 0 0,7 0-5318 0 0,-6 0 604 0 0,-34 0 319 0 0,-3 3 418 0 0,5 4-841 0 0,-2-1-398 0 0,-116-19 1481 0 0,-3 0-1024 0 0,52 19-770 0 0,47 5-530 0 0,-130 23 160 0 0,39-26 530 0 0,-102-4-273 0 0,30 7-305 0 0,17-8 282 0 0,73-17-409 0 0,-57 12 0 0 0,-399 82 0 0 0,539-73 12 0 0,1-4 1 0 0,-1-2-1 0 0,0-3 1 0 0,1-4-1 0 0,-1-1 1 0 0,-37-12-13 0 0,-137-32 117 0 0,56 21-117 0 0,46 17 89 0 0,-79 6-89 0 0,-154-10-97 0 0,229 30 97 0 0,-161-30 0 0 0,63-8 0 0 0,127 13 11 0 0,-70 5 138 0 0,-88 7-149 0 0,171 3 0 0 0,-27-10 0 0 0,-50 7 45 0 0,67 4-26 0 0,0 6-322 0 0,-169 15 758 0 0,189-19-455 0 0,-114-5 344 0 0,17 8-365 0 0,95-3-99 0 0,-26 5 109 0 0,43-15 11 0 0,34-1 0 0 0,-23 1 0 0 0,-50 10-368 0 0,48 4-707 0 0,36-6-1382 0 0,14-4 988 0 0,1 0-298 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8166.184">1641 1826 2760 0 0,'6'32'2136'0'0,"-6"-31"-1553"0"0,0-1-342 0 0,0 0-148 0 0,30 15 2680 0 0,-29-15-2055 0 0,-1 0 30 0 0,0 0 117 0 0,0 0 51 0 0,0 0 11 0 0,0 0-21 0 0,0 0-87 0 0,0 0-34 0 0,0 0-7 0 0,0 0-4 0 0,0 0-6 0 0,0 0-7 0 0,0 0-1 0 0,0 0-33 0 0,0 0-140 0 0,0 0-62 0 0,-12 6 796 0 0,-31 1 55 0 0,-15 10 107 0 0,-24-10 121 0 0,-53 7-11 0 0,31 2-921 0 0,36-16-416 0 0,20-4-63 0 0,-59-16 422 0 0,81 14-425 0 0,-1 1-1 0 0,1 2 0 0 0,-1 0 1 0 0,0 3-1 0 0,-3 1-189 0 0,12-1 26 0 0,-56-1-15 0 0,-56 41-11 0 0,63-37 0 0 0,-23-2 0 0 0,63-5 0 0 0,8-5-11 0 0,0-1-554 0 0,18 9 409 0 0,-9-10-997 0 0,6-3-1235 0 0,-1-3-4013 0 0,4 15 1126 0 0,-2-5-1271 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8769.491">422 1697 4144 0 0,'-3'0'371'0'0,"-32"10"5674"0"0,9-4 1575 0 0,8 1-6482 0 0,-46 24 2093 0 0,-51 54-822 0 0,18 27-2088 0 0,39-17 366 0 0,57-91-645 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,2 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 0-1 0 0,1 0-42 0 0,8 8 113 0 0,1-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-2 0 0 0,13 2-113 0 0,35 7 53 0 0,29-4-769 0 0,-90-9-139 0 0,-1 0-1079 0 0,2 1-4291 0 0,4 2-1841 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11563.093">9347 621 1376 0 0,'0'0'65'0'0,"0"0"-6"0"0,-2 2 265 0 0,2 0 1296 0 0,-9 5 9233 0 0,6-5-11305 0 0,-2 2 8571 0 0,9-3-7501 0 0,-2-1-153 0 0,-2 0-1 0 0,0 0-25 0 0,8-1 177 0 0,122-26 2488 0 0,158-23-951 0 0,-131 25-1665 0 0,-88 16-280 0 0,56 5-144 0 0,-58 7 3 0 0,9 1 63 0 0,66 2 73 0 0,-96-15-234 0 0,-44 4 49 0 0,-1 3-3067 0 0,-1 2-3310 0 0,0 0 4316 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12290.505">10534 204 13104 0 0,'0'0'297'0'0,"0"0"39"0"0,0 0 19 0 0,0 0-34 0 0,0 0-126 0 0,0 0 250 0 0,0 0 130 0 0,0 0 29 0 0,0 0-13 0 0,8 6 913 0 0,38 15 1575 0 0,33 14-91 0 0,-70-31-2871 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,3 3-117 0 0,16 48 400 0 0,-19-14-62 0 0,1-7 43 0 0,-1 10 309 0 0,-28 11 92 0 0,10-40-673 0 0,-1-2 0 0 0,1 0 0 0 0,-2-1 0 0 0,1-1 0 0 0,-16 14-109 0 0,16-19 53 0 0,1-1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-2-1 1 0 0,1-1-1 0 0,-13 6-53 0 0,-10-12-351 0 0,32-4-332 0 0,1-1-1543 0 0,2 3-4239 0 0,-1 1-1953 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="90996.656">11571 1191 920 0 0,'0'0'304'0'0,"0"0"941"0"0,0 0 414 0 0,0-1 1565 0 0,5-8-1987 0 0,32-69 3794 0 0,-34 71-4715 0 0,0 1 1 0 0,2 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0-316 0 0,-3 4 87 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,2 1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0-86 0 0,7 24 477 0 0,-1-1 0 0 0,-1 0 0 0 0,-1 2 0 0 0,0-1-1 0 0,-1 28-476 0 0,-8 54 1538 0 0,4-107-1494 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-2 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-45 0 0,-2 1 47 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,-1-2-47 0 0,-2-3-7 0 0,2 0-1 0 0,-2-1 0 0 0,1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-3 0 0 0,1 2 1 0 0,0-1-1 0 0,1 0 1 0 0,1 0-1 0 0,-4-11 8 0 0,5 15-502 0 0,2 0 0 0 0,-1-2 0 0 0,0 2 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 502 0 0,5-10-7366 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="91897.027">12041 897 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-132 0 0,0 0-646 0 0,0 0-278 0 0,1-1-58 0 0,10-8 2229 0 0,-10 9-2573 0 0,-1 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-13 0 0,0 0-49 0 0,8 5 828 0 0,-6-1-1148 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 1 0 0,-1-2-140 0 0,-1 25 426 0 0,-14 195 876 0 0,16-147-1182 0 0,0-76-384 0 0,0 4 981 0 0,0 1-1983 0 0,0 6-3464 0 0,0-12 2540 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="92647.981">12063 1097 920 0 0,'0'1'67'0'0,"0"3"290"0"0,0-3 1430 0 0,0-1 622 0 0,0 0 119 0 0,0 0-204 0 0,0 0-970 0 0,0 0-423 0 0,0 0-88 0 0,4-22 1733 0 0,-4 21-2071 0 0,1-1-229 0 0,9-15 61 0 0,-8 15-136 0 0,3-4 690 0 0,24-29 1892 0 0,5 12-882 0 0,-29 22-1876 0 0,-2 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1-25 0 0,16 33 1472 0 0,-2 11-864 0 0,-15-18-608 0 0,8 11 0 0 0,-7-3 72 0 0,-3-34 299 0 0,0-2 117 0 0,17 14 597 0 0,4-2-1750 0 0,-20-11 404 0 0,15-8-493 0 0,11-20-1947 0 0,-16 1-3478 0 0,-9 18-300 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="93989.379">12764 962 456 0 0,'0'0'1413'0'0,"0"0"159"0"0,0 0 76 0 0,0 0-140 0 0,0 0-647 0 0,0 0-278 0 0,0 0-58 0 0,0-7 1476 0 0,-1 6 4407 0 0,-7 1-5892 0 0,0 0-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,2 0 0 0 0,-7 5-515 0 0,-5 5 424 0 0,13-12-374 0 0,2 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 3-50 0 0,-11 43 264 0 0,12 1-125 0 0,3-41-85 0 0,0 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,2 2 1 0 0,0-2-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,6 8-54 0 0,-8-13-18 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,3 0 18 0 0,31-6-3249 0 0,-32 2 1306 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95267.643">13094 510 920 0 0,'0'0'341'0'0,"0"0"1098"0"0,0 0 480 0 0,0 0 96 0 0,0 0-104 0 0,0 0-531 0 0,0 0-237 0 0,1 2-45 0 0,2 14 790 0 0,-3-15-1129 0 0,0-1-20 0 0,0 2-30 0 0,0 129 4843 0 0,-4-36-3927 0 0,-2 119 184 0 0,3-54-1385 0 0,3-133-472 0 0,0 5-118 0 0,0-9-6313 0 0,0-23 4748 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95643.07">13107 648 920 0 0,'10'-7'6425'0'0,"11"-16"3843"0"0,19 3-5971 0 0,-33 17-3958 0 0,-2 1 0 0 0,2 0-1 0 0,0 0 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 2 1 0 0,6 0-339 0 0,29 11 773 0 0,-11-1-4595 0 0,-23-11-1695 0 0,-1 0-1564 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98550.722">13464 865 920 0 0,'0'0'241'0'0,"0"0"678"0"0,0 0 296 0 0,0 0 58 0 0,0 0-53 0 0,0 0-254 0 0,0 0-114 0 0,0 0-20 0 0,0 0-22 0 0,0 0-70 0 0,0 0-32 0 0,0 26 3129 0 0,-10 230 4156 0 0,12-97-6298 0 0,2-95-1707 0 0,-4-63-70 0 0,0-1-160 0 0,0 0-685 0 0,0-7-2761 0 0,0-3-3454 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98832.077">13486 607 7976 0 0,'0'14'364'0'0,"0"-10"-8"0"0,0 3-212 0 0,0-1-7 0 0,0-5 574 0 0,0-1 238 0 0,0 11 1235 0 0,0-10 2609 0 0,1-1-5097 0 0,1-9-870 0 0,1 6-3805 0 0,-3 3 790 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="100011.114">13794 1184 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-6 6 0 0,-5-42 6095 0 0,12 11-2868 0 0,25-8-2391 0 0,-11 28 397 0 0,-18 17-1428 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 3-36 0 0,9 80 216 0 0,-19 14 176 0 0,-5-61 1491 0 0,14-38-1877 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0-6 0 0,-13-9 9 0 0,-28-33 46 0 0,24-18-327 0 0,18 56 112 0 0,0-1-1 0 0,1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 1 0 0,1-1 160 0 0,20-36-6577 0 0,-14 32 179 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="112707.469">11396 862 6192 0 0,'0'0'133'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 66 0 0,0 0 226 0 0,1-22 6285 0 0,-2-21-2539 0 0,-8 24-3101 0 0,-34-45-120 0 0,-13 22-726 0 0,37 36-73 0 0,-17 9 54 0 0,-17 21-89 0 0,21 31-88 0 0,10 8-64 0 0,12 26 80 0 0,7-63 60 0 0,2 1 0 0 0,1 0 0 0 0,0 0 0 0 0,2-1 0 0 0,1 1 0 0 0,3 10-140 0 0,6 89 1072 0 0,-3-56-1705 0 0,3 4-463 0 0,-11-62-34 0 0,-1-9-5836 0 0,0-3 1152 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="113106.261">11112 1036 11952 0 0,'0'0'546'0'0,"0"0"-10"0"0,5-5-322 0 0,1 1 384 0 0,1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1 1-1 0 0,2-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 1-599 0 0,14-4 579 0 0,16 8 986 0 0,1-1-980 0 0,-15 0-2039 0 0,-7-2-3511 0 0,-3-1-1716 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119095.651">14207 972 920 0 0,'0'0'215'0'0,"0"0"565"0"0,0 0 246 0 0,0 0 50 0 0,0 0-38 0 0,0 0-207 0 0,0 0-88 0 0,-9-18 1465 0 0,9 18-2144 0 0,-4-8 120 0 0,4 3-161 0 0,0 4 46 0 0,0 1 50 0 0,0 0 7 0 0,0 0-4 0 0,-1-6-39 0 0,0 6 8497 0 0,-10 47-6476 0 0,6 52 348 0 0,2-28-1794 0 0,8 71 1307 0 0,-5-54-1940 0 0,1-75 372 0 0,-1 1-4686 0 0,0-14 2473 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119948.343">14189 1191 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-112 0 0,0 0 219 0 0,6-5 2204 0 0,11-20-38 0 0,-16 24-2011 0 0,-1-21 3079 0 0,2 8-2359 0 0,12-37 1842 0 0,8 21-1982 0 0,7 5 8 0 0,-23 24-1121 0 0,-4 2 6 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1 0 0 0,-2 0-1 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 3-22 0 0,10 9-263 0 0,-10-10 258 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 1 5 0 0,5 19 825 0 0,7 57 291 0 0,-2-48-1116 0 0,0-12 562 0 0,10-21 72 0 0,-17-2-761 0 0,1-1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,1-1 0 0 0,0 1 0 0 0,-1-2 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-2 1-1 0 0,3-2 127 0 0,2-1-1228 0 0,16-13-4345 0 0,-21 17 3808 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121219.819">14777 503 3224 0 0,'-3'12'2653'0'0,"0"28"1684"0"0,-7-1-951 0 0,6 30-459 0 0,-2 41-127 0 0,5 44-152 0 0,0-92-2024 0 0,3 2 194 0 0,-2-3 190 0 0,-9 26-96 0 0,0 83-482 0 0,4-149-526 0 0,3-19 68 0 0,2-2-108 0 0,0 0-10 0 0,0 0 8 0 0,0 0-167 0 0,0 0-710 0 0,-1-10-2894 0 0,-1-3-3509 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121883.773">14777 551 11024 0 0,'0'0'248'0'0,"0"0"34"0"0,0 0 22 0 0,0 0-29 0 0,1 1-54 0 0,41 5 5667 0 0,-3 9-4316 0 0,3 7 205 0 0,2 19-391 0 0,-15-4-436 0 0,-10-6-482 0 0,25 67 576 0 0,-24-42-556 0 0,1 40 243 0 0,-20-77-582 0 0,0-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-3-1 1 0 0,1 0-1 0 0,-2 3-149 0 0,-13 98 744 0 0,-1-15 79 0 0,11-81-656 0 0,4-15-103 0 0,2 1 0 0 0,-2 0 0 0 0,1-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,0-1 0 0 0,-2 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,-5 6-64 0 0,4-8 14 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 0-14 0 0,-34-13-1612 0 0,35 10 372 0 0,2 2 9 0 0,1-6-3128 0 0,-1-6 2299 0 0,4 11-11 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122684.061">15346 510 6968 0 0,'0'0'316'0'0,"0"0"-3"0"0,0 0-49 0 0,0 0 543 0 0,0 0 258 0 0,0 0 50 0 0,3 11 2997 0 0,-3 30-882 0 0,-3 12-957 0 0,-23 120 1538 0 0,-1 74-1086 0 0,17-111-1413 0 0,6-17-1045 0 0,4-61-214 0 0,0-50-2118 0 0,-2-6-5266 0 0,1-2 4284 0 0,4-10-3949 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="123499.345">15400 527 1376 0 0,'0'0'455'0'0,"0"0"1373"0"0,0 0 605 0 0,0 0 119 0 0,0 0-232 0 0,0 0-1087 0 0,0 0-473 0 0,0 0-96 0 0,0 0-7 0 0,0 0 58 0 0,0 0 21 0 0,0 0 7 0 0,0 0-22 0 0,2 0-96 0 0,31-7 3303 0 0,-31 7-3725 0 0,2-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,2 1-203 0 0,1 1 237 0 0,69 38 1652 0 0,-67-34-1701 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 1 0 0 0,3 5-188 0 0,-7-11 45 0 0,23 89 375 0 0,-25-88-406 0 0,0-1 0 0 0,0 1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 1 0 0,-1-1-1 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,0 2-14 0 0,-2-1 56 0 0,0 2 0 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,-3 1-56 0 0,-14 6 176 0 0,13-11-196 0 0,36 13-457 0 0,-19-11 473 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 4 4 0 0,-17 89 137 0 0,11-82 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-4 7-137 0 0,-10 12 332 0 0,-31 38 176 0 0,28-51-504 0 0,-8-41-3300 0 0,31 16 1814 0 0,-1-2-56 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="126421.51">10864 1874 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-2 10-158 0 0,1-10 318 0 0,1 0 203 0 0,-3-17 4327 0 0,9-85 858 0 0,7-11-4362 0 0,-9-52-443 0 0,-5 32-346 0 0,12-67-590 0 0,-6 45 735 0 0,2-20-741 0 0,-5-31-100 0 0,17-20 802 0 0,14 48-1204 0 0,-8 60 526 0 0,-16 95-375 0 0,12-25 96 0 0,-9 34 0 0 0,-7 11 11 0 0,2-3 42 0 0,6 5-120 0 0,133 32 118 0 0,-66-21-51 0 0,19 1 0 0 0,79 28 0 0 0,-33-11 13 0 0,-50-7 12 0 0,2-6 1 0 0,81-1-26 0 0,320-33 619 0 0,-219-3-286 0 0,178-2 704 0 0,-107 2-1079 0 0,305 34 539 0 0,-111-24-461 0 0,-336-3-36 0 0,-36 6 0 0 0,-23 0-89 0 0,199 1 178 0 0,34 58-89 0 0,-137-19-53 0 0,-165-27 106 0 0,-68 13-53 0 0,-10-12 0 0 0,0 1 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 5 0 0 0,-3 26 0 0 0,-11 134 0 0 0,-14 51 0 0 0,-9 74 0 0 0,-6 64 0 0 0,14-181 0 0 0,17-107 0 0 0,-30 107 0 0 0,21-89 0 0 0,-1 10 0 0 0,14-49 0 0 0,-10 31 0 0 0,-10-22 0 0 0,24-52 0 0 0,-15 9 0 0 0,-2-1 0 0 0,-52 12 0 0 0,19-22-89 0 0,-244-1 178 0 0,115 1-89 0 0,-113-18 0 0 0,26-3 0 0 0,-311 8-364 0 0,303 23 728 0 0,-61-30-364 0 0,103 7-488 0 0,133 6 351 0 0,-222 9-206 0 0,233-2 409 0 0,-1-6 0 0 0,-53-9-66 0 0,-83-18 67 0 0,-46-1 57 0 0,82 20-596 0 0,-17-13 472 0 0,145 14 141 0 0,-146-19 66 0 0,94 7-414 0 0,-188-35 751 0 0,205 45-712 0 0,56 2-1600 0 0,25 7-7788 0 0,14 0 569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128916.561">10598 1626 1376 0 0,'1'0'379'0'0,"1"0"-255"0"0,2-1 1065 0 0,17-35 2596 0 0,-17 28-3929 0 0,-1-24 6888 0 0,-3 31-6157 0 0,-13 1 1265 0 0,-35 24 2723 0 0,-92 15-187 0 0,70-26-3294 0 0,-1-5 0 0 0,-1-4 0 0 0,1-3 0 0 0,-1-5-1094 0 0,-33-3 693 0 0,-172-34-271 0 0,205 28-246 0 0,-5 6 42 0 0,-21-2-111 0 0,66 27-215 0 0,31-17-45 0 0,-6-3-2 0 0,5 1-5493 0 0,2 1 3616 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129317.678">9656 1385 12496 0 0,'0'0'572'0'0,"-7"4"186"0"0,-90 25 4653 0 0,-32 34-21 0 0,-1 45-3631 0 0,90-44-1578 0 0,28-15 21 0 0,11-48-198 0 0,0 2 21 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-26 0 0,28 54 343 0 0,15-18 88 0 0,20-2-135 0 0,94 33-1529 0 0,-139-64-94 0 0,-2-4-65 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2378 755 2760 0 0,'0'0'531'0'0,"0"0"1186"0"0,0 0 519 0 0,0 0 106 0 0,0 0-166 0 0,0 0-792 0 0,0 0-346 0 0,0 0-70 0 0,0 0-47 0 0,0 0-163 0 0,0 0-71 0 0,0 0-14 0 0,0 0 10 0 0,0 0 42 0 0,0 0 13 0 0,0 9 699 0 0,-6 115 2364 0 0,12 23-1865 0 0,5 116-247 0 0,5-21-814 0 0,-13-49-319 0 0,-18-69 500 0 0,22-94-2539 0 0,-7-29 905 0 0,0-1-60 0 0,0 0-15 0 0,0 0-116 0 0,0 0-476 0 0,0 0-209 0 0,2 0-39 0 0,8-2-10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2597.859">2201 671 4144 0 0,'0'0'319'0'0,"0"0"23"0"0,0 0 881 0 0,5-5 1496 0 0,-1 3 846 0 0,51-23 2209 0 0,17 20-278 0 0,131-4-967 0 0,-119-1-3873 0 0,6-1-272 0 0,115-9 368 0 0,-47 17-373 0 0,-155 3-377 0 0,61 0 316 0 0,0-2-1 0 0,57-11-317 0 0,32-5 240 0 0,43-10-96 0 0,-55 18-73 0 0,-46 6 277 0 0,28 2-231 0 0,84-12 51 0 0,-37 4-88 0 0,-38 17-27 0 0,-61-1-42 0 0,-46-3 14 0 0,-3-2 0 0 0,2 0-1 0 0,1-2 1 0 0,-3 0 0 0 0,22-4-25 0 0,54-3 73 0 0,20 5 130 0 0,-76 3-371 0 0,59-10 88 0 0,53-22 197 0 0,-59 14-106 0 0,-38 12 42 0 0,123 8-170 0 0,-93-2 117 0 0,-27 5 64 0 0,92-3-64 0 0,47 5 0 0 0,-59-1 0 0 0,61-9 0 0 0,-58 10-64 0 0,2 0 75 0 0,-46 1 31 0 0,58-2-95 0 0,49 3 53 0 0,-38 11-160 0 0,-63-14 107 0 0,1-2-22 0 0,-11 7 11 0 0,40-9 53 0 0,-61 5-42 0 0,94-6-339 0 0,-20 6 280 0 0,38-3 32 0 0,-132-3 80 0 0,123 4 0 0 0,-32-15 177 0 0,-2-3-378 0 0,-20 15 201 0 0,-24-12 0 0 0,-47 2 46 0 0,1 1 0 0 0,1 4-1 0 0,12 1-45 0 0,81-2-5 0 0,22 1-127 0 0,-39-6 284 0 0,103-7-13 0 0,61 8-422 0 0,-153-1 407 0 0,12-3 201 0 0,-121 18-371 0 0,-30-5-57 0 0,9 0-101 0 0,-4 1 124 0 0,31 8 64 0 0,-8-1 16 0 0,-10 9 0 0 0,-8-1 0 0 0,2 23 0 0 0,-7 4 0 0 0,-10 7 0 0 0,-5 9 257 0 0,0-14-154 0 0,8 21 193 0 0,-11 31-376 0 0,1-10-72 0 0,-6-5 152 0 0,0 49 64 0 0,3-29-64 0 0,4-12 64 0 0,12-28-53 0 0,-7-3 42 0 0,2-2-53 0 0,-5 25 75 0 0,0-36 31 0 0,2-11-84 0 0,1-28 20 0 0,8-2-31 0 0,-1 1-11 0 0,1 11-21 0 0,-4-16-85 0 0,0-2-15 0 0,0 0 1 0 0,-2 1-73 0 0,-5 4-309 0 0,4-4-135 0 0,3-1-31 0 0,-3 3-3225 0 0,3-3 2170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4154.481">10638 1795 456 0 0,'0'0'1935'0'0,"0"0"230"0"0,0 0 105 0 0,7 0 2569 0 0,-16 0 1235 0 0,8 0-5318 0 0,-8 0 604 0 0,-39 0 319 0 0,-4 3 418 0 0,5 4-841 0 0,-1-1-398 0 0,-138-19 1481 0 0,-4 0-1024 0 0,62 19-770 0 0,56 5-530 0 0,-155 22 160 0 0,47-25 530 0 0,-121-4-273 0 0,35 7-305 0 0,21-8 282 0 0,86-17-409 0 0,-67 12 0 0 0,-473 81 0 0 0,638-72 12 0 0,2-4 1 0 0,-2-2-1 0 0,1-3 1 0 0,1-4-1 0 0,-2-1 1 0 0,-43-11-13 0 0,-163-33 117 0 0,67 22-117 0 0,54 16 89 0 0,-93 6-89 0 0,-183-10-97 0 0,271 30 97 0 0,-190-30 0 0 0,74-8 0 0 0,151 14 11 0 0,-83 4 138 0 0,-105 7-149 0 0,204 3 0 0 0,-33-10 0 0 0,-59 7 45 0 0,79 4-26 0 0,1 6-322 0 0,-201 14 758 0 0,224-18-455 0 0,-135-5 344 0 0,20 8-365 0 0,113-3-99 0 0,-32 5 109 0 0,52-15 11 0 0,41-1 0 0 0,-29 1 0 0 0,-58 10-368 0 0,57 4-707 0 0,42-6-1382 0 0,17-4 988 0 0,1 0-298 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8166.184">1945 1805 2760 0 0,'7'31'2136'0'0,"-7"-30"-1553"0"0,0-1-342 0 0,0 0-148 0 0,36 15 2680 0 0,-35-15-2055 0 0,-1 0 30 0 0,0 0 117 0 0,0 0 51 0 0,0 0 11 0 0,0 0-21 0 0,0 0-87 0 0,0 0-34 0 0,0 0-7 0 0,0 0-4 0 0,0 0-6 0 0,0 0-7 0 0,0 0-1 0 0,0 0-33 0 0,0 0-140 0 0,0 0-62 0 0,-14 6 796 0 0,-37 1 55 0 0,-18 10 107 0 0,-28-10 121 0 0,-63 7-11 0 0,36 2-921 0 0,44-16-416 0 0,23-4-63 0 0,-70-16 422 0 0,96 14-425 0 0,-1 1-1 0 0,1 2 0 0 0,-1 0 1 0 0,0 3-1 0 0,-3 1-189 0 0,13-1 26 0 0,-65-1-15 0 0,-67 41-11 0 0,74-38 0 0 0,-26-1 0 0 0,74-4 0 0 0,9-6-11 0 0,1-1-554 0 0,20 9 409 0 0,-9-10-997 0 0,6-3-1235 0 0,-1-3-4013 0 0,5 15 1126 0 0,-3-5-1271 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8769.491">500 1677 4144 0 0,'-4'0'371'0'0,"-37"10"5674"0"0,10-4 1575 0 0,10 1-6482 0 0,-55 24 2093 0 0,-60 53-822 0 0,21 26-2088 0 0,46-16 366 0 0,68-90-645 0 0,0-1 1 0 0,1 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,2 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-2-2 1 0 0,3 1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,2 0-42 0 0,9 8 113 0 0,1-1 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1-1-1 0 0,2-2 1 0 0,-2 2 0 0 0,2-2 0 0 0,15 2-113 0 0,41 7 53 0 0,35-4-769 0 0,-107-9-139 0 0,-1 0-1079 0 0,2 1-4291 0 0,6 2-1841 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11563.093">11079 614 1376 0 0,'0'0'65'0'0,"0"0"-6"0"0,-2 2 265 0 0,2 0 1296 0 0,-11 5 9233 0 0,7-5-11305 0 0,-1 2 8571 0 0,9-3-7501 0 0,-1-1-153 0 0,-3 0-1 0 0,0 0-25 0 0,9-1 177 0 0,145-26 2488 0 0,188-22-951 0 0,-156 24-1665 0 0,-105 16-280 0 0,68 5-144 0 0,-70 7 3 0 0,11 1 63 0 0,78 2 73 0 0,-113-15-234 0 0,-53 4 49 0 0,0 3-3067 0 0,-2 2-3310 0 0,0 0 4316 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12290.505">12486 202 13104 0 0,'0'0'297'0'0,"0"0"39"0"0,0 0 19 0 0,0 0-34 0 0,0 0-126 0 0,0 0 250 0 0,0 0 130 0 0,0 0 29 0 0,0 0-13 0 0,10 6 913 0 0,44 14 1575 0 0,40 15-91 0 0,-84-31-2871 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 1 1 0 0,1-2-1 0 0,-1 2 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1 1 0 0 0,4 3-117 0 0,18 47 400 0 0,-21-13-62 0 0,0-8 43 0 0,-1 11 309 0 0,-33 10 92 0 0,12-39-673 0 0,-2-2 0 0 0,2-1 0 0 0,-3 0 0 0 0,2-1 0 0 0,-19 14-109 0 0,18-20 53 0 0,2 0 1 0 0,-3-1-1 0 0,2 0 0 0 0,-3-1 1 0 0,2-1-1 0 0,-16 6-53 0 0,-12-12-351 0 0,38-4-332 0 0,1-1-1543 0 0,3 3-4239 0 0,-2 1-1953 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="90996.656">13715 1177 920 0 0,'0'0'304'0'0,"0"0"941"0"0,0 0 414 0 0,0-1 1565 0 0,6-8-1987 0 0,38-68 3794 0 0,-40 70-4715 0 0,-1 1 1 0 0,3 0-1 0 0,-1 2 1 0 0,0-2-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0-316 0 0,-4 4 87 0 0,2-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-3 0 1 0 0,3 1 0 0 0,-3 1-1 0 0,3-1 1 0 0,-2 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,-1 1-1 0 0,1-2 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0-86 0 0,9 24 477 0 0,-2-1 0 0 0,-1-1 0 0 0,-1 3 0 0 0,0-1-1 0 0,-1 27-476 0 0,-10 54 1538 0 0,5-106-1494 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-2 0-1 0 0,2-2 1 0 0,-2 1 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-45 0 0,-3 1 47 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,-1-2-47 0 0,-3-3-7 0 0,3 0-1 0 0,-2 0 0 0 0,0-1 1 0 0,2 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-3 0 0 0,1 2 1 0 0,0-1-1 0 0,1 0 1 0 0,2 1-1 0 0,-5-12 8 0 0,5 15-502 0 0,3 0 0 0 0,-1-2 0 0 0,0 2 0 0 0,0 0-1 0 0,-1 0 1 0 0,2-1 0 0 0,2 2 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,0-1 502 0 0,7-10-7366 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="91897.027">14272 887 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-132 0 0,0 0-646 0 0,0 0-278 0 0,2-1-58 0 0,11-8 2229 0 0,-12 9-2573 0 0,-1 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-13 0 0,0 0-49 0 0,9 5 828 0 0,-6-1-1148 0 0,-1 0 0 0 0,-1 1 0 0 0,0-2 1 0 0,1 1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 1 0 0,-1-2-140 0 0,-2 25 426 0 0,-16 192 876 0 0,19-145-1182 0 0,0-75-384 0 0,0 4 981 0 0,0 1-1983 0 0,0 6-3464 0 0,0-12 2540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="92647.981">14298 1084 920 0 0,'0'1'67'0'0,"0"3"290"0"0,0-3 1430 0 0,0-1 622 0 0,0 0 119 0 0,0 0-204 0 0,0 0-970 0 0,0 0-423 0 0,0 0-88 0 0,5-22 1733 0 0,-5 21-2071 0 0,1 0-229 0 0,11-16 61 0 0,-9 15-136 0 0,2-4 690 0 0,30-29 1892 0 0,5 12-882 0 0,-34 22-1876 0 0,-2 1 0 0 0,-1 0 0 0 0,2-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,2 1 1 0 0,-1 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-25 0 0,20 33 1472 0 0,-3 10-864 0 0,-18-17-608 0 0,10 11 0 0 0,-8-4 72 0 0,-4-33 299 0 0,0-2 117 0 0,20 14 597 0 0,5-2-1750 0 0,-24-11 404 0 0,18-8-493 0 0,13-20-1947 0 0,-19 2-3478 0 0,-11 17-300 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="93989.379">15129 951 456 0 0,'0'0'1413'0'0,"0"0"159"0"0,0 0 76 0 0,0 0-140 0 0,0 0-647 0 0,0 0-278 0 0,0 0-58 0 0,0-7 1476 0 0,-1 6 4407 0 0,-8 1-5892 0 0,-1 0-1 0 0,1 1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,2 0 1 0 0,-2 1-1 0 0,2 0 0 0 0,-1 0 1 0 0,-1 1-1 0 0,3 0 0 0 0,-8 5-515 0 0,-7 4 424 0 0,16-11-374 0 0,3 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,3 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-2 1 1 0 0,2 1-1 0 0,0-1 0 0 0,-2 3-50 0 0,-13 42 264 0 0,15 2-125 0 0,3-41-85 0 0,0-1 0 0 0,1 0 1 0 0,1 1-1 0 0,-2-1 0 0 0,3 2 1 0 0,-1-2-1 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-2-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,7 8-54 0 0,-9-13-18 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,2 0 1 0 0,-1 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,3 0 18 0 0,37-6-3249 0 0,-38 2 1306 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95267.643">15520 504 920 0 0,'0'0'341'0'0,"0"0"1098"0"0,0 0 480 0 0,0 0 96 0 0,0 0-104 0 0,0 0-531 0 0,0 0-237 0 0,2 2-45 0 0,1 14 790 0 0,-3-15-1129 0 0,0-1-20 0 0,0 2-30 0 0,0 127 4843 0 0,-5-35-3927 0 0,-2 118 184 0 0,4-54-1385 0 0,3-131-472 0 0,0 4-118 0 0,0-8-6313 0 0,0-23 4748 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95643.07">15536 641 920 0 0,'12'-7'6425'0'0,"13"-16"3843"0"0,22 3-5971 0 0,-39 17-3958 0 0,-2 1 0 0 0,3 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1-1-1 0 0,0 2 1 0 0,8 0-339 0 0,33 11 773 0 0,-12-1-4595 0 0,-27-11-1695 0 0,-2 0-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98550.722">15959 855 920 0 0,'0'0'241'0'0,"0"0"678"0"0,0 0 296 0 0,0 0 58 0 0,0 0-53 0 0,0 0-254 0 0,0 0-114 0 0,0 0-20 0 0,0 0-22 0 0,0 0-70 0 0,0 0-32 0 0,0 26 3129 0 0,-12 227 4156 0 0,15-96-6298 0 0,1-94-1707 0 0,-4-62-70 0 0,0-1-160 0 0,0 0-685 0 0,0-7-2761 0 0,0-3-3454 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98832.077">15985 600 7976 0 0,'0'14'364'0'0,"0"-10"-8"0"0,0 3-212 0 0,0-1-7 0 0,0-5 574 0 0,0-1 238 0 0,0 10 1235 0 0,0-9 2609 0 0,1-1-5097 0 0,2-8-870 0 0,0 5-3805 0 0,-3 3 790 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="100011.114">16350 1170 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-6 6 0 0,-6-41 6095 0 0,15 10-2868 0 0,29-7-2391 0 0,-14 27 397 0 0,-20 17-1428 0 0,-2-1 1 0 0,2 1-1 0 0,-2 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 2 0 0 0,0-2 0 0 0,0 1 0 0 0,-2 0 0 0 0,3-1 0 0 0,-2 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 3-36 0 0,11 79 216 0 0,-23 14 176 0 0,-6-61 1491 0 0,17-37-1877 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,3 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,1 0 0 0 0,-2 0-6 0 0,-16-8 9 0 0,-33-34 46 0 0,29-17-327 0 0,20 55 112 0 0,1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-2 1 0 0 0,3 1 1 0 0,0-2 160 0 0,25-36-6577 0 0,-18 32 179 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="112707.469">13508 852 6192 0 0,'0'0'133'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 66 0 0,0 0 226 0 0,1-22 6285 0 0,-2-20-2539 0 0,-10 23-3101 0 0,-40-44-120 0 0,-15 21-726 0 0,43 36-73 0 0,-19 9 54 0 0,-21 21-89 0 0,25 30-88 0 0,12 9-64 0 0,14 25 80 0 0,8-63 60 0 0,3 2 0 0 0,1 0 0 0 0,0-1 0 0 0,3 0 0 0 0,0 1 0 0 0,4 9-140 0 0,7 89 1072 0 0,-3-56-1705 0 0,3 4-463 0 0,-12-61-34 0 0,-2-9-5836 0 0,0-3 1152 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="113106.261">13171 1024 11952 0 0,'0'0'546'0'0,"0"0"-10"0"0,6-5-322 0 0,1 1 384 0 0,2 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,-1 1-1 0 0,3-1 1 0 0,-2 1 0 0 0,0 0 0 0 0,1 1-1 0 0,0 0 1 0 0,-1 1-599 0 0,17-4 579 0 0,19 8 986 0 0,1-1-980 0 0,-18 0-2039 0 0,-8-2-3511 0 0,-3-1-1716 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119095.651">16840 961 920 0 0,'0'0'215'0'0,"0"0"565"0"0,0 0 246 0 0,0 0 50 0 0,0 0-38 0 0,0 0-207 0 0,0 0-88 0 0,-11-18 1465 0 0,11 18-2144 0 0,-5-8 120 0 0,5 3-161 0 0,0 4 46 0 0,0 1 50 0 0,0 0 7 0 0,0 0-4 0 0,-1-6-39 0 0,0 6 8497 0 0,-12 47-6476 0 0,7 50 348 0 0,2-26-1794 0 0,10 69 1307 0 0,-6-53-1940 0 0,2-74 372 0 0,-2 1-4686 0 0,0-14 2473 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119948.343">16818 1177 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-112 0 0,0 0 219 0 0,8-5 2204 0 0,12-19-38 0 0,-19 23-2011 0 0,-1-21 3079 0 0,2 8-2359 0 0,15-36 1842 0 0,9 20-1982 0 0,8 5 8 0 0,-27 24-1121 0 0,-4 2 6 0 0,-1-1 0 0 0,-1 0-1 0 0,2 0 1 0 0,0 1 0 0 0,-2 0-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0 3-22 0 0,12 9-263 0 0,-12-10 258 0 0,2 0 0 0 0,-2 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-2 0 0 0 0,3 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 1 5 0 0,6 19 825 0 0,9 56 291 0 0,-4-48-1116 0 0,1-11 562 0 0,12-21 72 0 0,-21-2-761 0 0,2-1 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-2 1 0 0,2 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,2-2 127 0 0,3-1-1228 0 0,19-12-4345 0 0,-24 16 3808 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121219.819">17515 497 3224 0 0,'-3'12'2653'0'0,"-1"28"1684"0"0,-8-2-951 0 0,8 30-459 0 0,-3 41-127 0 0,5 43-152 0 0,1-90-2024 0 0,4 1 194 0 0,-3-3 190 0 0,-11 26-96 0 0,0 82-482 0 0,5-147-526 0 0,4-19 68 0 0,2-2-108 0 0,0 0-10 0 0,0 0 8 0 0,0 0-167 0 0,0 0-710 0 0,-1-10-2894 0 0,-2-3-3509 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121883.773">17515 545 11024 0 0,'0'0'248'0'0,"0"0"34"0"0,0 0 22 0 0,0 0-29 0 0,2 1-54 0 0,47 5 5667 0 0,-2 8-4316 0 0,2 8 205 0 0,4 19-391 0 0,-19-5-436 0 0,-12-5-482 0 0,31 66 576 0 0,-30-42-556 0 0,2 40 243 0 0,-24-76-582 0 0,1-1 1 0 0,-2 0-1 0 0,-2 0 1 0 0,2 1-1 0 0,-3-1 1 0 0,0-1-1 0 0,-1 4-149 0 0,-16 97 744 0 0,-2-15 79 0 0,14-81-656 0 0,4-14-103 0 0,3 1 0 0 0,-2 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-6 6-64 0 0,5-8 14 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 0-14 0 0,-39-13-1612 0 0,40 10 372 0 0,3 2 9 0 0,2-6-3128 0 0,-2-6 2299 0 0,5 11-11 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122684.061">18190 504 6968 0 0,'0'0'316'0'0,"0"0"-3"0"0,0 0-49 0 0,0 0 543 0 0,0 0 258 0 0,0 0 50 0 0,3 11 2997 0 0,-3 29-882 0 0,-3 13-957 0 0,-28 118 1538 0 0,-1 73-1086 0 0,20-110-1413 0 0,7-16-1045 0 0,5-61-214 0 0,0-49-2118 0 0,-2-6-5266 0 0,1-2 4284 0 0,4-10-3949 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="123499.345">18254 521 1376 0 0,'0'0'455'0'0,"0"0"1373"0"0,0 0 605 0 0,0 0 119 0 0,0 0-232 0 0,0 0-1087 0 0,0 0-473 0 0,0 0-96 0 0,0 0-7 0 0,0 0 58 0 0,0 0 21 0 0,0 0 7 0 0,0 0-22 0 0,2 0-96 0 0,37-7 3303 0 0,-36 7-3725 0 0,1-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,3 0 1 0 0,-3 0-1 0 0,3 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,3 1-203 0 0,2 1 237 0 0,80 37 1652 0 0,-78-33-1701 0 0,-1 0 1 0 0,1 1-1 0 0,-2 0 0 0 0,0 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,3 6-188 0 0,-7-11 45 0 0,26 88 375 0 0,-29-87-406 0 0,0-1 0 0 0,0 1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1-1 0 0 0,0 2 1 0 0,-2-1-1 0 0,3 0 0 0 0,-2 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,-1 2-14 0 0,-2-1 56 0 0,0 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1-2 0 0 0,-1 1 0 0 0,-4 1-56 0 0,-17 6 176 0 0,16-11-196 0 0,42 13-457 0 0,-22-11 473 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 3 4 0 0,-20 89 137 0 0,13-81 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1-1 0 0 0,-2-1 0 0 0,0 1 0 0 0,-6 7-137 0 0,-11 12 332 0 0,-37 37 176 0 0,33-50-504 0 0,-9-41-3300 0 0,36 16 1814 0 0,0-2-56 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="126421.51">12877 1852 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-2 10-158 0 0,1-10 318 0 0,1 0 203 0 0,-4-17 4327 0 0,11-83 858 0 0,9-12-4362 0 0,-12-51-443 0 0,-5 31-346 0 0,14-65-590 0 0,-7 43 735 0 0,2-19-741 0 0,-5-30-100 0 0,19-21 802 0 0,17 49-1204 0 0,-9 58 526 0 0,-19 94-375 0 0,14-24 96 0 0,-11 33 0 0 0,-8 11 11 0 0,2-3 42 0 0,7 5-120 0 0,159 32 118 0 0,-80-21-51 0 0,24 0 0 0 0,93 29 0 0 0,-39-11 13 0 0,-60-8 12 0 0,3-5 1 0 0,96-1-26 0 0,379-33 619 0 0,-259-2-286 0 0,211-3 704 0 0,-127 2-1079 0 0,361 34 539 0 0,-131-24-461 0 0,-399-3-36 0 0,-42 6 0 0 0,-27 0-89 0 0,235 2 178 0 0,41 56-89 0 0,-162-18-53 0 0,-197-27 106 0 0,-79 12-53 0 0,-13-11 0 0 0,0 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1 4 0 0 0,-2 27 0 0 0,-14 132 0 0 0,-16 51 0 0 0,-11 72 0 0 0,-8 64 0 0 0,18-179 0 0 0,19-106 0 0 0,-35 106 0 0 0,25-88 0 0 0,-1 10 0 0 0,16-49 0 0 0,-11 31 0 0 0,-12-22 0 0 0,28-51 0 0 0,-18 9 0 0 0,-2-1 0 0 0,-62 12 0 0 0,23-22-89 0 0,-290-1 178 0 0,137 0-89 0 0,-134-16 0 0 0,31-4 0 0 0,-369 8-364 0 0,360 23 728 0 0,-73-30-364 0 0,122 7-488 0 0,157 6 351 0 0,-262 9-206 0 0,276-2 409 0 0,-2-6 0 0 0,-62-9-66 0 0,-99-18 67 0 0,-54 0 57 0 0,97 19-596 0 0,-20-13 472 0 0,172 14 141 0 0,-173-19 66 0 0,111 7-414 0 0,-223-34 751 0 0,243 44-712 0 0,67 2-1600 0 0,29 7-7788 0 0,17 0 569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128916.561">12562 1607 1376 0 0,'1'0'379'0'0,"1"0"-255"0"0,3-1 1065 0 0,20-34 2596 0 0,-20 27-3929 0 0,-2-24 6888 0 0,-3 31-6157 0 0,-15 1 1265 0 0,-42 24 2723 0 0,-109 14-187 0 0,83-25-3294 0 0,-1-5 0 0 0,-1-4 0 0 0,1-3 0 0 0,-2-5-1094 0 0,-38-3 693 0 0,-205-33-271 0 0,244 27-246 0 0,-6 6 42 0 0,-25-2-111 0 0,78 27-215 0 0,36-17-45 0 0,-6-3-2 0 0,6 1-5493 0 0,2 1 3616 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129317.678">11445 1369 12496 0 0,'0'0'572'0'0,"-8"4"186"0"0,-107 25 4653 0 0,-38 33-21 0 0,-1 45-3631 0 0,107-44-1578 0 0,32-15 21 0 0,14-47-198 0 0,0 2 21 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,0 1-26 0 0,34 53 343 0 0,17-18 88 0 0,24-1-135 0 0,111 32-1529 0 0,-164-63-94 0 0,-2-4-65 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2859,10 +2871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3589,7 +3601,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A78" s="9">
+      <c r="A78" s="8">
         <v>43566</v>
       </c>
       <c r="B78" s="7">
@@ -3670,7 +3682,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A87" s="9">
+      <c r="A87" s="8">
         <v>43567</v>
       </c>
       <c r="B87" s="7">
@@ -3697,8 +3709,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A90" s="9">
-        <v>43568</v>
+      <c r="A90" s="8">
+        <v>43570</v>
       </c>
       <c r="B90" s="7">
         <v>0.3125</v>
@@ -3752,14 +3764,50 @@
         <v>112</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C97" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C98" s="2" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A99" s="8">
+        <v>43571</v>
+      </c>
+      <c r="B99" s="7">
+        <v>0.3125</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B100" s="7">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B101" s="7">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B102" s="7"/>
+      <c r="C102" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3774,10 +3822,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="A1:C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="49.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3927,7 +3975,9 @@
       <c r="B13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
@@ -3949,6 +3999,14 @@
       </c>
       <c r="C15" s="2" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3962,8 +4020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405881BC-250B-44EF-9833-781DFFD746B9}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="72" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3972,7 +4030,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified Documentation + logBook
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="581" documentId="14_{9F97C56A-0847-4B13-96CB-9482C5495C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7D68FEF2-323C-4779-8FC8-A381F2E88FFB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Journal De Bord" sheetId="1" r:id="rId1"/>
     <sheet name="Question" sheetId="2" r:id="rId2"/>
     <sheet name="Dessin" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="120">
   <si>
     <t>Documentation</t>
   </si>
@@ -62,9 +61,6 @@
     <t>Mail Planification</t>
   </si>
   <si>
-    <t xml:space="preserve"> création de V 0.1 passage de V0.1 aV0.2</t>
-  </si>
-  <si>
     <t>Création GitHub</t>
   </si>
   <si>
@@ -87,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">Aide par Clément Christensen </t>
-  </si>
-  <si>
-    <t>V0.2 a V0.3</t>
   </si>
   <si>
     <t>Question</t>
@@ -336,9 +329,6 @@
     <t>réponse Q11</t>
   </si>
   <si>
-    <t>Réponse q11</t>
-  </si>
-  <si>
     <t>Faudrait-it mettre des image pour le dictionnaire de données ?</t>
   </si>
   <si>
@@ -406,12 +396,15 @@
   </si>
   <si>
     <t>Admin dans DB ?</t>
+  </si>
+  <si>
+    <t>Réponse Q11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1642,33 +1635,33 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">247 705 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">640 722 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-9 10039 0 0,4 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1036 664 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1384 746 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,4-23-839 0 0,-7 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 79 971 0 0,13-78-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,3-28 325 0 0,-7 43 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 35 365 0 0,9-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-43 40 0 0,-1 48 757 0 0,-8 6-562 0 0,-2 1-34 0 0,14 15 96 0 0,-24 51 294 0 0,10-64 48 0 0,0-2-24 0 0,-12 10 14 0 0,11-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-12 0 0,-1-2-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,16-18-798 0 0,-5 23 705 0 0,11 17 39 0 0,-21-13 64 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 2-10 0 0,2-5 84 0 0,-5 17 237 0 0,-20-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 11-3207 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">1678 463 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 57 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,1 17 113 0 0,-2-14-1404 0 0,-1 51 981 0 0,-4-2-1688 0 0,1-59-1417 0 0,-2-32 962 0 0,-7-28-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">1614 598 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-32 2722 0 0,-14 31-3180 0 0,15-15 1008 0 0,23-24 674 0 0,-35 36-2057 0 0,1 2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 19 1009 0 0,-52 14 55 0 0,-5-18-600 0 0,22 47 1448 0 0,-23 2-2113 0 0,-15-60 230 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 22 399 0 0,1-11-337 0 0,7-8-104 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 37 0 0,-35-1 653 0 0,-7-25-4978 0 0,34 19 2334 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">3006 428 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 48 1154 0 0,-12 24 2052 0 0,-3 33 1755 0 0,3 52-2463 0 0,4-54-962 0 0,-3 32-1172 0 0,7-140-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-3 13-2556 0 0,2-23 1622 0 0,1-1-894 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">3024 486 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-4 772 0 0,-14 10-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,3 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 2-1 0 0,0-2 1 0 0,1 1-1 0 0,-2 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-4-1-4 0 0,-53-44-4198 0 0,55 42-3651 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">2230 124 3680 0 0,'-6'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,8 16-23 0 0,2-13-297 0 0,6 3-1604 0 0,-9 95 2 0 0,7-77 200 0 0,1-18-716 0 0,2-41-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">2155 695 1376 0 0,'5'-20'2159'0'0,"2"0"4223"0"0,7-6-3735 0 0,-3 6-1523 0 0,12-17 1153 0 0,4 12 523 0 0,-4 3-1591 0 0,22-17 135 0 0,-44 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 7-27 0 0,10 30 368 0 0,29 120 1443 0 0,-19-124-1634 0 0,0-14-84 0 0,-14-23-77 0 0,-5-2-29 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 13 0 0,40-28-350 0 0,19-12-3834 0 0,-54 36 2533 0 0,3 3-12 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">1 302 6448 0 0,'7'21'6309'0'0,"-7"-18"-6682"0"0,4 54 3514 0 0,8 85-847 0 0,-2-44-690 0 0,-5-10-929 0 0,13 132 737 0 0,-29 32 57 0 0,6-176-1337 0 0,-1-48-256 0 0,5-13-955 0 0,1-11-4480 0 0,0-4-582 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">12 333 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,18-38 6274 0 0,-18 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,12-3 291 0 0,71-18 828 0 0,-38 5-729 0 0,13-5 96 0 0,50 12 370 0 0,-61 8-222 0 0,43 2-1079 0 0,-22-6 16 0 0,38-20 451 0 0,-31 15 1144 0 0,61 1-1448 0 0,5 19 224 0 0,-54-19-645 0 0,-30-1 1538 0 0,6 0-1123 0 0,-36 8-292 0 0,52 0 264 0 0,-25-6 20 0 0,54-26 70 0 0,10 18-205 0 0,14 9 34 0 0,-67-4 219 0 0,22-5-424 0 0,-4 12 192 0 0,-11 5 584 0 0,45 1-1352 0 0,-8 9 736 0 0,1 6 1017 0 0,-32-10-298 0 0,-11 0-1239 0 0,25-4 520 0 0,15 3 64 0 0,12 29 75 0 0,-60-11-166 0 0,14 1 523 0 0,-3-9-840 0 0,-22-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,74-9-197 0 0,-22 19 0 0 0,-41-15-20 0 0,-44-2 0 0 0,-13-5 0 0 0,25 17 0 0 0,-38-3 0 0 0,6 6 0 0 0,12 23 64 0 0,-5 28 0 0 0,-8 23-64 0 0,-5 32-8 0 0,1-51 125 0 0,-4 32-203 0 0,-8 34 295 0 0,8 44-190 0 0,-17-84 82 0 0,-1-41-13 0 0,6-44 96 0 0,6-12-234 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 2 51 0 0,0-3 114 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0-114 0 0,-14 0 158 0 0,-97 8-218 0 0,81-3 59 0 0,0-1-1 0 0,0-2 1 0 0,0-1 0 0 0,-1-2-1 0 0,1-1 1 0 0,-22-6 1 0 0,4-4-9 0 0,-1 3 0 0 0,0 3 0 0 0,0 2 0 0 0,-23 2 9 0 0,-110 0 332 0 0,138 4-330 0 0,0-1-1 0 0,0-3 1 0 0,-1-2-1 0 0,1-1 1 0 0,-8-7-2 0 0,23 9-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-20 4 18 0 0,-144 30 64 0 0,-2-12-136 0 0,-49-9 152 0 0,173-13-80 0 0,-93 0 11 0 0,-32-17 42 0 0,100 17-53 0 0,-22-13 80 0 0,22-11-176 0 0,-86-18 224 0 0,58 22-196 0 0,62 6 192 0 0,-62-3-124 0 0,50 11 0 0 0,46 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">6713 897 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,22-14-8855 0 0,-18 9 1888 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">7088 941 10592 0 0,'-13'-13'818'0'0,"10"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">7435 851 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,5 0-232 0 0,-2 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">7798 941 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-38 1231 0 0,1 45-2463 0 0,0 1 0 0 0,2 1 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,-1 3-113 0 0,3-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-16-143 0 0,-13 33-62 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-2-43 0 0,3 2 32 0 0,1 10 23 0 0,-10 18 200 0 0,3-27-96 0 0,-7 4-695 0 0,14-7-611 0 0,7-10-5710 0 0,-6 6 446 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">8082 572 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 22-45 0 0,-12-25-3788 0 0,3 8 1039 0 0,3 83 1637 0 0,7 83-1221 0 0,-14-86-1606 0 0,0-79-341 0 0,-2-4-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">8383 613 2760 0 0,'4'8'1828'0'0,"4"20"4892"0"0,5 25-3444 0 0,1 103 1947 0 0,-11-80-3937 0 0,-6-37-4508 0 0,3-36 1701 0 0,-4 6-229 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">8436 941 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,9-39 5734 0 0,3-11-521 0 0,-16 20-3279 0 0,11 10-1202 0 0,8-37 1 0 0,-14 56-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,3 0-93 0 0,2-2 95 0 0,-4 3-21 0 0,26 0-60 0 0,1 14-14 0 0,-4 7 0 0 0,-21-12 0 0 0,10 23 0 0 0,19 74 514 0 0,-19-52 356 0 0,6-19-278 0 0,-20-34-517 0 0,7 3 98 0 0,-5-1-141 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-29-4233 0 0,-22 32 2840 0 0,0 1-164 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">9223 669 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-39-6 1747 0 0,43 9-1667 0 0,4-2 170 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 42-483 0 0,18 2 618 0 0,16 12 378 0 0,10 4-513 0 0,15-4 1899 0 0,26-11-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 0 0 0 0,-22-9 0 0 0,-2 2 0 0 0,0-5-64 0 0,30-22-5497 0 0,-31 16 3530 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">9488 1002 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-17 649 0 0,-9 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 20 784 0 0,-16 13 56 0 0,6-32-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">9760 661 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 73 1352 0 0,-5-54-2105 0 0,-9 63 686 0 0,-2-6-314 0 0,3 68-530 0 0,6-113-273 0 0,-3-10 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-3-14-1557 0 0,2-1 195 0 0,-3-2-70 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">9725 664 1376 0 0,'4'6'367'0'0,"-3"-5"1002"0"0,-1-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,10-7 51 0 0,32-23 1588 0 0,-29 24-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,2 2 108 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 2 0 0 0,1-2 1 0 0,0 6-108 0 0,9 27 435 0 0,0 58 787 0 0,-11-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-56 0 0,-44 35 929 0 0,43-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-5 0 0 0,4-15-5381 0 0,0 15-2125 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">10202 395 0 0 0,'-12'12'0'0'0,"6"-15"140"0"0,4 3 2586 0 0,2 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 30 3000 0 0,-14 31-1947 0 0,1 50 181 0 0,4 1 624 0 0,-7-41-881 0 0,11 38-1316 0 0,-12-26-173 0 0,8-43 0 0 0,14 3-2476 0 0,-12-41 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">10184 825 4376 0 0,'0'0'199'0'0,"10"-11"1918"0"0,-6-2 1016 0 0,11-10 683 0 0,-6-13-1297 0 0,-2-1-472 0 0,5 29-1272 0 0,-10 7-743 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 22 598 0 0,-25-17-674 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 6-227 0 0,6 92 608 0 0,-7-65-165 0 0,-1-12 997 0 0,27-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,13-10-60 0 0,-20 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27">10811 698 2760 0 0,'0'1'207'0'0,"0"45"6763"0"0,0-45-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 13-344 0 0,-2 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 9-1278 0 0,-12 63 616 0 0,0-18 973 0 0,13 39-2158 0 0,3-87 962 0 0,-3-26-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28">10875 691 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,58-25 1867 0 0,-55 27-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,2 0-156 0 0,-1 0 96 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1-95 0 0,-1-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 5-94 0 0,-43 58 1952 0 0,47-67-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">246 704 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">638 721 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-9 10039 0 0,4 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1033 663 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1380 745 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,4-23-839 0 0,-7 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 79 971 0 0,13-78-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,3-28 325 0 0,-7 43 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 35 365 0 0,9-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-43 40 0 0,-1 48 757 0 0,-8 6-562 0 0,-2 1-34 0 0,14 15 96 0 0,-24 51 294 0 0,10-64 48 0 0,0-2-24 0 0,-12 10 14 0 0,11-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-12 0 0,-1-2-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,16-18-798 0 0,-5 23 705 0 0,11 17 39 0 0,-21-13 64 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 2-10 0 0,2-5 84 0 0,-5 17 237 0 0,-20-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 11-3207 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">1674 462 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 57 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,1 17 113 0 0,-2-14-1404 0 0,-1 51 981 0 0,-4-3-1688 0 0,1-58-1417 0 0,-2-32 962 0 0,-7-28-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">1610 597 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-32 2722 0 0,-14 31-3180 0 0,15-15 1008 0 0,23-24 674 0 0,-35 36-2057 0 0,1 2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 19 1009 0 0,-52 14 55 0 0,-5-18-600 0 0,22 47 1448 0 0,-23 2-2113 0 0,-15-60 230 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 22 399 0 0,1-11-337 0 0,7-8-104 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 37 0 0,-35-1 653 0 0,-7-25-4978 0 0,34 19 2334 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">2998 427 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 48 1154 0 0,-12 24 2052 0 0,-3 33 1755 0 0,3 52-2463 0 0,4-54-962 0 0,-3 31-1172 0 0,7-139-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-3 13-2556 0 0,2-23 1622 0 0,1-1-894 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">3016 485 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-4 772 0 0,-14 10-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,3 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 2-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-4-1-4 0 0,-53-44-4198 0 0,55 42-3651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">2224 124 3680 0 0,'-6'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,8 16-23 0 0,2-14-297 0 0,6 4-1604 0 0,-9 95 2 0 0,7-77 200 0 0,1-18-716 0 0,2-41-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">2149 694 1376 0 0,'5'-20'2159'0'0,"2"0"4223"0"0,7-6-3735 0 0,-3 6-1523 0 0,12-17 1153 0 0,4 12 523 0 0,-4 3-1591 0 0,22-17 135 0 0,-44 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 7-27 0 0,10 30 368 0 0,29 120 1443 0 0,-20-124-1634 0 0,1-14-84 0 0,-14-23-77 0 0,-5-2-29 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 13 0 0,40-28-350 0 0,19-12-3834 0 0,-54 36 2533 0 0,3 3-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">1 302 6448 0 0,'7'21'6309'0'0,"-7"-18"-6682"0"0,4 54 3514 0 0,8 84-847 0 0,-2-43-690 0 0,-5-10-929 0 0,13 132 737 0 0,-29 31 57 0 0,6-175-1337 0 0,-1-48-256 0 0,5-13-955 0 0,1-11-4480 0 0,0-4-582 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">12 333 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,18-38 6274 0 0,-18 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,12-3 291 0 0,71-18 828 0 0,-38 5-729 0 0,12-5 96 0 0,51 12 370 0 0,-61 8-222 0 0,43 2-1079 0 0,-22-6 16 0 0,37-20 451 0 0,-30 15 1144 0 0,61 1-1448 0 0,4 19 224 0 0,-53-19-645 0 0,-30-1 1538 0 0,6 0-1123 0 0,-36 8-292 0 0,52 0 264 0 0,-26-6 20 0 0,55-26 70 0 0,10 18-205 0 0,13 9 34 0 0,-66-4 219 0 0,22-5-424 0 0,-4 12 192 0 0,-11 5 584 0 0,44 1-1352 0 0,-7 9 736 0 0,1 6 1017 0 0,-32-10-298 0 0,-12 0-1239 0 0,26-4 520 0 0,15 3 64 0 0,12 29 75 0 0,-61-11-166 0 0,15 1 523 0 0,-3-9-840 0 0,-22-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,73-9-197 0 0,-21 19 0 0 0,-41-15-20 0 0,-44-2 0 0 0,-13-5 0 0 0,25 17 0 0 0,-38-3 0 0 0,5 6 0 0 0,13 23 64 0 0,-5 27 0 0 0,-8 24-64 0 0,-5 32-8 0 0,1-51 125 0 0,-4 32-203 0 0,-8 34 295 0 0,8 43-190 0 0,-17-83 82 0 0,-1-41-13 0 0,6-44 96 0 0,6-12-234 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 2 51 0 0,0-3 114 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0-114 0 0,-14 0 158 0 0,-97 8-218 0 0,81-3 59 0 0,0-1-1 0 0,0-2 1 0 0,0-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-22-6 1 0 0,4-4-9 0 0,-1 3 0 0 0,0 3 0 0 0,0 2 0 0 0,-22 2 9 0 0,-111 0 332 0 0,138 4-330 0 0,0-1-1 0 0,0-3 1 0 0,0-2-1 0 0,0-1 1 0 0,-8-7-2 0 0,23 9-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-20 4 18 0 0,-143 30 64 0 0,-3-12-136 0 0,-48-9 152 0 0,172-13-80 0 0,-92 0 11 0 0,-33-17 42 0 0,101 17-53 0 0,-23-13 80 0 0,22-11-176 0 0,-85-18 224 0 0,57 22-196 0 0,62 6 192 0 0,-62-3-124 0 0,51 11 0 0 0,45 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">6695 896 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,22-14-8855 0 0,-18 9 1888 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">7069 940 10592 0 0,'-13'-13'818'0'0,"10"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">7416 850 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,5 0-232 0 0,-2 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">7778 940 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-38 1231 0 0,1 45-2463 0 0,0 1 0 0 0,2 1 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,-1 3-113 0 0,3-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-16-143 0 0,-13 33-62 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-2-43 0 0,3 2 32 0 0,1 10 23 0 0,-10 18 200 0 0,3-27-96 0 0,-7 4-695 0 0,14-7-611 0 0,7-10-5710 0 0,-6 6 446 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">8061 571 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 22-45 0 0,-12-25-3788 0 0,3 8 1039 0 0,3 83 1637 0 0,7 83-1221 0 0,-14-86-1606 0 0,0-79-341 0 0,-2-4-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">8361 612 2760 0 0,'4'8'1828'0'0,"4"20"4892"0"0,5 25-3444 0 0,1 103 1947 0 0,-11-80-3937 0 0,-6-37-4508 0 0,3-36 1701 0 0,-4 6-229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">8414 940 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,9-39 5734 0 0,3-11-521 0 0,-16 20-3279 0 0,11 10-1202 0 0,8-37 1 0 0,-14 56-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,3 0-93 0 0,2-2 95 0 0,-4 3-21 0 0,26 0-60 0 0,1 14-14 0 0,-5 7 0 0 0,-20-12 0 0 0,10 23 0 0 0,19 74 514 0 0,-19-52 356 0 0,6-19-278 0 0,-20-34-517 0 0,7 3 98 0 0,-5-1-141 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-29-4233 0 0,-22 32 2840 0 0,0 1-164 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">9199 668 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-39-6 1747 0 0,43 9-1667 0 0,4-2 170 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 42-483 0 0,18 2 618 0 0,16 12 378 0 0,10 4-513 0 0,15-4 1899 0 0,26-11-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 0 0 0 0,-22-9 0 0 0,-2 2 0 0 0,0-5-64 0 0,30-22-5497 0 0,-31 16 3530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">9463 1001 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-17 649 0 0,-9 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 20 784 0 0,-16 13 56 0 0,6-32-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">9734 660 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 73 1352 0 0,-5-54-2105 0 0,-9 63 686 0 0,-2-6-314 0 0,3 67-530 0 0,6-112-273 0 0,-3-10 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-3-14-1557 0 0,2-1 195 0 0,-3-2-70 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">9700 663 1376 0 0,'4'6'367'0'0,"-3"-5"1002"0"0,-1-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,9-7 51 0 0,33-23 1588 0 0,-29 24-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,2 2 108 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 2 0 0 0,1-2 1 0 0,0 6-108 0 0,9 27 435 0 0,0 58 787 0 0,-11-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-56 0 0,-44 35 929 0 0,43-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-5 0 0 0,4-15-5381 0 0,0 15-2125 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">10175 394 0 0 0,'-12'12'0'0'0,"6"-15"140"0"0,4 3 2586 0 0,2 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 30 3000 0 0,-14 31-1947 0 0,1 50 181 0 0,4 1 624 0 0,-7-41-881 0 0,11 38-1316 0 0,-12-26-173 0 0,8-43 0 0 0,14 2-2476 0 0,-12-40 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">10157 824 4376 0 0,'0'0'199'0'0,"10"-11"1918"0"0,-6-2 1016 0 0,11-10 683 0 0,-6-13-1297 0 0,-2-1-472 0 0,5 29-1272 0 0,-10 7-743 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 22 598 0 0,-25-17-674 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 6-227 0 0,6 92 608 0 0,-7-65-165 0 0,-1-12 997 0 0,27-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,12-10-60 0 0,-19 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27">10783 697 2760 0 0,'0'1'207'0'0,"0"45"6763"0"0,0-45-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 13-344 0 0,-2 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 9-1278 0 0,-12 63 616 0 0,0-18 973 0 0,13 38-2158 0 0,3-86 962 0 0,-3-26-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28">10847 690 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,57-25 1867 0 0,-54 27-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,2 0-156 0 0,-1 0 96 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1-95 0 0,-1-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 5-94 0 0,-43 58 1952 0 0,47-67-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1731,7 +1724,7 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">170 594 2760 0 0,'-22'-8'3128'0'0,"16"0"-821"0"0,-31-60 5175 0 0,-4-46-4528 0 0,19 34-2212 0 0,-1 5-684 0 0,12 36 1037 0 0,3 9-46 0 0,8-11-1018 0 0,16 27 738 0 0,31-2 95 0 0,18-8-285 0 0,21 11 18 0 0,41-7 553 0 0,-102 10-836 0 0,25-13-4 0 0,8 12-300 0 0,11 18-3179 0 0,-62-7 1586 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">170 617 2760 0 0,'-22'-8'3128'0'0,"16"-1"-821"0"0,-31-61 5175 0 0,-4-49-4528 0 0,19 36-2212 0 0,-1 5-684 0 0,12 38 1037 0 0,3 9-46 0 0,8-12-1018 0 0,16 29 738 0 0,31-3 95 0 0,18-8-285 0 0,21 11 18 0 0,41-6 553 0 0,-102 9-836 0 0,25-13-4 0 0,8 13-300 0 0,11 18-3179 0 0,-62-7 1586 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1793,10 +1786,10 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">139 52 9728 0 0,'-3'28'446'0'0,"2"-22"-10"0"0,1-6-110 0 0,-7 21 5217 0 0,-4 37-376 0 0,-11 67-1014 0 0,-9 212-706 0 0,15-146-2342 0 0,10-95-825 0 0,-9 101-24 0 0,11-169-383 0 0,3-27-26 0 0,1-1-8 0 0,0 0-161 0 0,0 0-650 0 0,1-24-9059 0 0,3 5 1774 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="639.092">110 189 11776 0 0,'6'-17'1280'0'0,"0"-2"2430"0"0,2 1 2588 0 0,2 8-5875 0 0,-3 4 86 0 0,1-2-282 0 0,0 2 0 0 0,0-1 0 0 0,0 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 2 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,9-2-228 0 0,42 10 628 0 0,-56-3-593 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 2-36 0 0,10 9 14 0 0,30 34 450 0 0,-14 3 1116 0 0,-2 58-1568 0 0,-28-98 95 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-7 8-106 0 0,7-11 49 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,-3 2-50 0 0,-52 12 153 0 0,56-16-165 0 0,63-8 9 0 0,-45 7 6 0 0,-5-1-28 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,3 2 25 0 0,-1 0-62 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 3 62 0 0,5 54 641 0 0,-9-58-617 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,-2 3-24 0 0,-6 8 0 0 0,-1 0 0 0 0,0-1 0 0 0,-2-1 0 0 0,1 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,-13 8 0 0 0,8-8 0 0 0,-1-2 0 0 0,-1 0 0 0 0,0-1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0-1 0 0 0,-8 0 0 0 0,-74 23-80 0 0,17-7-16 0 0,86-24 358 0 0,-7 1-2469 0 0,5-10-7469 0 0,4 0 1106 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1210.204">893 1 14456 0 0,'0'0'330'0'0,"0"0"45"0"0,0 0 18 0 0,0 0-42 0 0,0 1-75 0 0,-3 72 6166 0 0,-5-9-4114 0 0,-18 141 1352 0 0,-4 59-2060 0 0,-11 14-805 0 0,7-75-674 0 0,26-176-350 0 0,8-26 82 0 0,-11-12-1918 0 0,6-8-4504 0 0,5 15 4273 0 0,-2-8-6349 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1636.656">935 115 1376 0 0,'7'-36'68'0'0,"7"3"5954"0"0,-5 12 1686 0 0,-8 20-7576 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-132 0 0,0 0 58 0 0,0 1 33 0 0,0-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,2 0-91 0 0,2 0 102 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,2 3-103 0 0,6 13 174 0 0,-10-14-111 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,3 1-63 0 0,34 21 581 0 0,7 34 291 0 0,-42-31-651 0 0,-1-1-1 0 0,-2 2 0 0 0,0-1 1 0 0,-2 0-1 0 0,-2 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,-1 0-1 0 0,-8 28-220 0 0,6-21 236 0 0,-2 1 0 0 0,-1-2 0 0 0,-1 1 0 0 0,-5 5-236 0 0,-23 55 424 0 0,30-82-365 0 0,1 3 31 0 0,-1 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,-9 8-90 0 0,14-15 26 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,-8 2-26 0 0,-115 9 33 0 0,-7-28-1057 0 0,71-9-4105 0 0,60 16 3206 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">139 53 9728 0 0,'-3'29'446'0'0,"2"-23"-10"0"0,1-6-110 0 0,-7 21 5217 0 0,-4 39-376 0 0,-11 67-1014 0 0,-9 218-706 0 0,15-150-2342 0 0,10-97-825 0 0,-9 103-24 0 0,11-172-383 0 0,3-28-26 0 0,1-1-8 0 0,0 0-161 0 0,0 0-650 0 0,1-25-9059 0 0,3 6 1774 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="639.092">110 193 11776 0 0,'6'-17'1280'0'0,"0"-3"2430"0"0,2 2 2588 0 0,2 8-5875 0 0,-3 4 86 0 0,1-3-282 0 0,0 3 0 0 0,0-1 0 0 0,0 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 2 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 1 0 0,9-2-228 0 0,42 10 628 0 0,-56-3-593 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 3-36 0 0,10 8 14 0 0,30 35 450 0 0,-14 3 1116 0 0,-2 60-1568 0 0,-28-101 95 0 0,0 0-1 0 0,0 0 0 0 0,-1 2 1 0 0,-1-2-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 2 1 0 0,-1-1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-7 8-106 0 0,7-11 49 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 1 1 0 0,1-2-1 0 0,-1 0 0 0 0,0-1 1 0 0,-3 2-50 0 0,-52 13 153 0 0,56-17-165 0 0,63-9 9 0 0,-45 9 6 0 0,-5-2-28 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,3 2 25 0 0,-1 0-62 0 0,-1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 2 1 0 0,0-2-1 0 0,0 3 62 0 0,5 55 641 0 0,-9-58-617 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 1 1 0 0,-1-2 0 0 0,0 1 0 0 0,-2 3-24 0 0,-6 8 0 0 0,-1 1 0 0 0,0-2 0 0 0,-2-1 0 0 0,1 1 0 0 0,-2-2 0 0 0,0 0 0 0 0,-13 9 0 0 0,8-9 0 0 0,-1-2 0 0 0,-1 1 0 0 0,0-2 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-8-1 0 0 0,-74 23-80 0 0,17-6-16 0 0,86-25 358 0 0,-7 1-2469 0 0,5-10-7469 0 0,4 0 1106 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1210.204">893 1 14456 0 0,'0'0'330'0'0,"0"0"45"0"0,0 0 18 0 0,0 0-42 0 0,0 1-75 0 0,-3 74 6166 0 0,-5-10-4114 0 0,-18 145 1352 0 0,-4 59-2060 0 0,-11 15-805 0 0,7-76-674 0 0,26-181-350 0 0,8-26 82 0 0,-11-12-1918 0 0,6-8-4504 0 0,5 15 4273 0 0,-2-9-6349 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1636.656">935 118 1376 0 0,'7'-37'68'0'0,"7"3"5954"0"0,-5 13 1686 0 0,-8 20-7576 0 0,-1-2 0 0 0,0 2 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-132 0 0,0 0 58 0 0,0 1 33 0 0,0-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,2 0-91 0 0,2 0 102 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,2 4-103 0 0,6 12 174 0 0,-10-14-111 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,3 1-63 0 0,34 22 581 0 0,7 34 291 0 0,-42-31-651 0 0,-1-2-1 0 0,-2 3 0 0 0,0-1 1 0 0,-2-1-1 0 0,-2 1 1 0 0,0 0-1 0 0,-2-1 1 0 0,-1 1-1 0 0,-8 28-220 0 0,6-21 236 0 0,-2 1 0 0 0,-1-3 0 0 0,-1 2 0 0 0,-5 5-236 0 0,-23 56 424 0 0,30-83-365 0 0,1 2 31 0 0,-1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-9 7-90 0 0,14-15 26 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,-8 2-26 0 0,-115 9 33 0 0,-7-28-1057 0 0,71-9-4105 0 0,60 15 3206 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1827,8 +1820,8 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">100 9 3224 0 0,'0'0'457'0'0,"0"0"711"0"0,0 0 311 0 0,0 0 66 0 0,0 0-146 0 0,0 0-671 0 0,0 0-295 0 0,0 0-60 0 0,0 0 9 0 0,0 0 83 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,0 0 102 0 0,0 0 22 0 0,0 14 1235 0 0,-10 56 4955 0 0,4 25-4234 0 0,17 7-97 0 0,-9-47-1040 0 0,-3-28-1012 0 0,0 47-267 0 0,-5 173 1877 0 0,1-157-1879 0 0,6-81-48 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-4 6 0 0 0,-11 12-801 0 0,-7-12-6747 0 0,18-17-982 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="412.914">107 87 2304 0 0,'0'-2'167'0'0,"8"-15"2093"0"0,18-20 9580 0 0,0 22-10365 0 0,-22 12-1240 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,3 2-235 0 0,-2-1 218 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,3 5-217 0 0,5 9 528 0 0,-7-11-392 0 0,1 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0 3-135 0 0,-3 105 1604 0 0,-35-42-855 0 0,31-71-713 0 0,-1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1-35 0 0,1-1-135 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-4-5 136 0 0,6 5-520 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 521 0 0,-5-25-2538 0 0,5 6-19 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">100 9 3224 0 0,'0'0'457'0'0,"0"0"711"0"0,0 0 311 0 0,0 0 66 0 0,0 0-146 0 0,0 0-671 0 0,0 0-295 0 0,0 0-60 0 0,0 0 9 0 0,0 0 83 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,0 0 102 0 0,0 0 22 0 0,0 15 1235 0 0,-10 56 4955 0 0,4 27-4234 0 0,17 6-97 0 0,-9-47-1040 0 0,-3-30-1012 0 0,0 49-267 0 0,-5 178 1877 0 0,1-162-1879 0 0,6-83-48 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,0-2 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-4 5 0 0 0,-11 13-801 0 0,-7-13-6747 0 0,18-17-982 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="412.914">107 89 2304 0 0,'0'-2'167'0'0,"8"-15"2093"0"0,18-21 9580 0 0,0 22-10365 0 0,-22 13-1240 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,3 2-235 0 0,-2-1 218 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,3 6-217 0 0,5 8 528 0 0,-7-11-392 0 0,1 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 3-135 0 0,-3 108 1604 0 0,-35-43-855 0 0,31-73-713 0 0,-1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-2 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1-35 0 0,1-1-135 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-4-4 136 0 0,6 5-520 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 521 0 0,-5-26-2538 0 0,5 6-19 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1859,8 +1852,8 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">67 100 10592 0 0,'0'0'818'0'0,"-3"11"2010"0"0,-12 32 2029 0 0,4 26-1721 0 0,0 16-649 0 0,-5 116 1221 0 0,12-81-2576 0 0,4 10-475 0 0,-3-113-1193 0 0,2-16-68 0 0,1-1-32 0 0,0 0-79 0 0,0 0-314 0 0,-2-14-8176 0 0,1 8 1651 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="332.092">71 90 11520 0 0,'5'-10'1224'0'0,"26"-25"6290"0"0,34 0-4470 0 0,-62 33-2967 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 2-77 0 0,4 15 316 0 0,0-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-1 0-1 0 0,-1 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-2 4-316 0 0,2-13 99 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,-3 5-100 0 0,5-11 18 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-18 0 0,-2-1-59 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-7-4 59 0 0,-47-32-3704 0 0,55 30 957 0 0,5-1-5943 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">67 103 10592 0 0,'0'0'818'0'0,"-3"11"2010"0"0,-12 34 2029 0 0,4 26-1721 0 0,0 16-649 0 0,-5 120 1221 0 0,12-83-2576 0 0,4 9-475 0 0,-3-115-1193 0 0,2-17-68 0 0,1-1-32 0 0,0 0-79 0 0,0 0-314 0 0,-2-14-8176 0 0,1 7 1651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="332.092">71 93 11520 0 0,'5'-11'1224'0'0,"26"-25"6290"0"0,34 0-4470 0 0,-62 34-2967 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 2 0 0 0,1-2 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 2-77 0 0,4 16 316 0 0,0-2 0 0 0,-1 2 0 0 0,-1-1 0 0 0,-1 1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,-2 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-2 5-316 0 0,2-14 99 0 0,0 1 1 0 0,-1-2-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,-3 6-100 0 0,5-12 18 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-18 0 0,-2-1-59 0 0,0 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-7-4 59 0 0,-47-33-3704 0 0,55 31 957 0 0,5-2-5943 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1891,8 +1884,8 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">142 9 3224 0 0,'-2'-8'1623'0'0,"2"7"4003"0"0,-1 1 5780 0 0,-3 42-9766 0 0,-7 14-232 0 0,-4 46-776 0 0,7 16-182 0 0,-7 69 1156 0 0,16-172-1404 0 0,-2 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,-1-1 1 0 0,-5 14-202 0 0,9 64 272 0 0,-1-85-248 0 0,1-6-103 0 0,0-1-12 0 0,0 0-71 0 0,0 0-341 0 0,-19-3-7577 0 0,14-4 457 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="423.109">0 598 2304 0 0,'0'0'101'0'0,"6"-12"5654"0"0,-2 1-935 0 0,1-12-218 0 0,24-24-1523 0 0,28-17-965 0 0,0 8-1362 0 0,-55 54-723 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,2 2-29 0 0,3 1 86 0 0,0 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-2 0-1 0 0,3 8-85 0 0,-8 81 1468 0 0,-2-79-1328 0 0,-4 13 188 0 0,1 0 0 0 0,2 1 1 0 0,1 0-1 0 0,2 0 0 0 0,1 18-328 0 0,17-52-374 0 0,15-38-3517 0 0,-22 27 1623 0 0,-1 3-436 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">142 9 3224 0 0,'-2'-8'1623'0'0,"2"7"4003"0"0,-1 1 5780 0 0,-3 43-9766 0 0,-7 15-232 0 0,-4 47-776 0 0,7 16-182 0 0,-7 72 1156 0 0,16-178-1404 0 0,-2 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,-5 14-202 0 0,9 65 272 0 0,-1-86-248 0 0,1-7-103 0 0,0-1-12 0 0,0 0-71 0 0,0 0-341 0 0,-19-4-7577 0 0,14-3 457 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="423.109">0 616 2304 0 0,'0'0'101'0'0,"6"-13"5654"0"0,-2 2-935 0 0,1-13-218 0 0,24-24-1523 0 0,28-18-965 0 0,0 8-1362 0 0,-55 56-723 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,2 2-29 0 0,3 1 86 0 0,0 1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 0-1 0 0,3 9-85 0 0,-8 82 1468 0 0,-2-80-1328 0 0,-4 13 188 0 0,1 0 0 0 0,2 1 1 0 0,1 0-1 0 0,2 0 0 0 0,1 18-328 0 0,17-53-374 0 0,15-39-3517 0 0,-22 27 1623 0 0,-1 4-436 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1928,251 +1921,251 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">23709 6389 0 0 0,'0'0'580'0'0,"0"0"-64"0"0,0 0 47 0 0,0 0-35 0 0,0 0-254 0 0,0 0-107 0 0,0 0-27 0 0,0 0 51 0 0,0 0 229 0 0,0 0 100 0 0,0 2 21 0 0,3 13 472 0 0,-3-13-554 0 0,0-2-3 0 0,0 0-54 0 0,0 0-223 0 0,0 0-98 0 0,0 0 51 0 0,0 0 272 0 0,0 0 95 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 0 0 0,0 6 0 0 0,0-7 0 0 0,0-1 0 0 0,0 0 36 0 0,0 0 150 0 0,0 0 66 0 0,0 0 18 0 0,0 0-29 0 0,0 6 436 0 0,2 51 2189 0 0,-4 62-643 0 0,-9-37-852 0 0,-7 67-1718 0 0,16-50-165 0 0,1-91 90 0 0,0 1-403 0 0,1 8-2730 0 0,-4-28-1033 0 0,-1 2-2741 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="208.461">23704 6445 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,8-3-112 0 0,0 0 125 0 0,-1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-2 1 0 0 0,1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1-346 0 0,48 68 1246 0 0,-52-64-1102 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-2 0 0 0,0 1-1 0 0,-2 1 1 0 0,0-1-1 0 0,0 2-143 0 0,2-4 57 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0-57 0 0,-96-6-816 0 0,65-14-3738 0 0,29 12 2908 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55956.919">25238 15461 456 0 0,'23'-41'0'0'0,"-7"27"2824"0"0,-7 3 664 0 0,-8 11-2678 0 0,-1 0 44 0 0,0 0 11 0 0,0 0 6 0 0,0 0 21 0 0,0 0 85 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,4-21 2411 0 0,-19 3-1851 0 0,14 16-1397 0 0,-1-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 1-117 0 0,-4 2 139 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-3 7-139 0 0,-20 33 224 0 0,-5 46 448 0 0,32 4 696 0 0,2-92-1368 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,2 0 1 0 0,-1 0 0 0 0,-2-1 16 0 0,1-1 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1-1 1 0 0,-1 2-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 0-16 0 0,4 0-124 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 0 125 0 0,12-6-613 0 0,19-15-2912 0 0,-19 11 1494 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55516.919">25596 15153 5984 0 0,'3'-41'472'0'0,"-1"1"5162"0"0,-2 38-3819 0 0,0 2-663 0 0,0 0-288 0 0,0 0-58 0 0,0 0-20 0 0,0 0-61 0 0,0 0-21 0 0,0 0-7 0 0,-9 5 1975 0 0,-17 107 1356 0 0,-29 205-3264 0 0,30-140-640 0 0,8-28-1060 0 0,16-133-1236 0 0,1-11-5747 0 0,0-5 911 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55296.919">25539 15329 9216 0 0,'0'0'706'0'0,"0"0"-114"0"0,4-5 3675 0 0,20-10 1993 0 0,17 5-3644 0 0,12-5-1858 0 0,5 19-1979 0 0,-52 6-2143 0 0,-3-2 1389 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-66366.92">24199 14907 6304 0 0,'15'-1'822'0'0,"-15"0"-83"0"0,0 1 249 0 0,0 0 48 0 0,0 0-31 0 0,0 0-170 0 0,0 0-71 0 0,0 0-17 0 0,0 0-27 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0 48 0 0,0 0 202 0 0,0 0 87 0 0,0 0 20 0 0,0 0-70 0 0,0 0-308 0 0,-1-1-137 0 0,-51-64 1234 0 0,-31 2 383 0 0,78 60-1902 0 0,-2 0 0 0 0,1 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-6 2-14 0 0,-30 31 373 0 0,8 2-682 0 0,-13 56 985 0 0,28-16-666 0 0,-1 44 460 0 0,17 9-108 0 0,14-12-298 0 0,19 15-7518 0 0,-27-128 13 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-66056.919">23723 15296 11976 0 0,'0'0'546'0'0,"5"-11"204"0"0,14 5 2195 0 0,37-8 2019 0 0,27-2-3091 0 0,-39 18-1743 0 0,0 2 0 0 0,-1 0 1 0 0,29 9-131 0 0,-23 0-3223 0 0,-34-9 2016 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-65316.919">24251 15504 920 0 0,'1'-3'80'0'0,"-1"2"-114"0"0,9-20 1775 0 0,21-24 8599 0 0,-15 35-9435 0 0,-1 2-70 0 0,-12 6-714 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,1 2-121 0 0,32 29 1528 0 0,-19 31 812 0 0,-18-55-2114 0 0,0-1 0 0 0,-1 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,1 0-226 0 0,-1-3 108 0 0,2 1 0 0 0,-2-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,2-1 0 0 0,-2 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,-5 1-108 0 0,6-3-56 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 0 1 0 0,-1 1 0 0 0,1-2-1 0 0,0 1 1 0 0,0-2 56 0 0,1-34-2485 0 0,3 21 635 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-57246.919">24609 15325 9616 0 0,'0'0'216'0'0,"0"0"32"0"0,1-2 12 0 0,9-22 16 0 0,9-31 4156 0 0,-19 53-3764 0 0,0 2 151 0 0,0 0 69 0 0,0 0 10 0 0,0 0-48 0 0,0 0-216 0 0,0 0-98 0 0,0 0-22 0 0,-8 60 3070 0 0,4-6-2456 0 0,-13 157 920 0 0,17-145-2048 0 0,-1-21-64 0 0,1-44-273 0 0,0-1-138 0 0,0 0-33 0 0,0 0-217 0 0,0-8-2919 0 0,1-4 1541 0 0,2 0-9 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-56836.919">24549 15470 10136 0 0,'0'0'42'0'0,"0"1"-1"0"0,0-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,2 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-42 0 0,31-33 4246 0 0,12 4-1699 0 0,-39 25-2345 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,3 0-202 0 0,29 18 1351 0 0,-32-11-1230 0 0,-2 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2 4-121 0 0,25 80 144 0 0,-18 1-545 0 0,-19-77-269 0 0,5-11-1904 0 0,0-3-3466 0 0,-1 0-762 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45426.919">25902 15501 456 0 0,'11'-3'13004'0'0,"-6"12"-6955"0"0,-9 19-4332 0 0,2-13-273 0 0,7 97-283 0 0,-3-72-2968 0 0,0-1-3416 0 0,-2-39-2002 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45206.919">25987 15146 5984 0 0,'0'0'273'0'0,"0"0"-5"0"0,0 0 121 0 0,0 0 1143 0 0,0 0 514 0 0,0 0 104 0 0,0 0-119 0 0,0 0-596 0 0,0 0-261 0 0,0 0-49 0 0,0 0-98 0 0,0 0-392 0 0,0 0-171 0 0,0 0-31 0 0,0 0-64 0 0,0 0-1670 0 0,0 0-5837 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44826.919">26134 15765 11232 0 0,'0'-4'1016'0'0,"-19"-76"3747"0"0,30 12-109 0 0,-8 60-4545 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 2 0 0 0,2-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 2 0 0 0,1-1 0 0 0,3-1-109 0 0,-6 3 0 0 0,-1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,2 0 0 0 0,15 39 10 0 0,-17-31 52 0 0,-7 48 1898 0 0,-36 27-1744 0 0,37-82-173 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-2-1 1 0 0,2 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-2 0 0 0,-1 2-1 0 0,2-1 1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-4-1-43 0 0,3-1-36 0 0,-2 1 0 0 0,0-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,0-2 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-3 36 0 0,5-34-2989 0 0,1 24 1539 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-43876.919">26557 15550 456 0 0,'0'0'83'0'0,"0"0"42"0"0,0 0 131 0 0,0 0 32 0 0,0 0 0 0 0,0 0 49 0 0,0 0 209 0 0,0 0 94 0 0,0 0 21 0 0,0 0-5 0 0,0 0-33 0 0,0 0-14 0 0,0 0-1 0 0,0 0-74 0 0,0 0-307 0 0,0 0-135 0 0,0-1-36 0 0,10-35 684 0 0,-2-6 547 0 0,-4 18-691 0 0,-4-24 2561 0 0,0 47-2790 0 0,0 1 1 0 0,0 0 0 0 0,0 7 8134 0 0,-4 25-7718 0 0,-10 120 1476 0 0,-1-82-2207 0 0,15-61-53 0 0,0-4-32 0 0,0-3-137 0 0,0-2-71 0 0,0 0-16 0 0,0 0-147 0 0,0 0-589 0 0,0 0-257 0 0,0 0-51 0 0,0 0-35 0 0,0 0-102 0 0,2 14-5517 0 0,-2-14 5738 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-43576.919">26564 15590 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,0 0-140 0 0,0 0 368 0 0,0 0 187 0 0,0 0 42 0 0,-7-6 963 0 0,6 2-1582 0 0,1-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-2 0 0 0,0 1 1 0 0,0 2-1 0 0,1-2 0 0 0,-1 0 0 0 0,4-2-240 0 0,-6 5 154 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,-1-1-153 0 0,8 3 222 0 0,18 15-38 0 0,-4 9-184 0 0,-21-24 130 0 0,0 1-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2 4-130 0 0,3 32 130 0 0,4-17-130 0 0,-1-19-97 0 0,23-10-2811 0 0,-19 1 1087 0 0,0-2-377 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1576.986">23215 6293 4608 0 0,'0'0'353'0'0,"5"10"155"0"0,-3-6 2425 0 0,10 26 3145 0 0,-10-8-3733 0 0,-12 21 1085 0 0,1 15-1742 0 0,3-7-736 0 0,11 42-312 0 0,-9-16-640 0 0,8-22 0 0 0,-17-9 0 0 0,13-41-9 0 0,0 0-146 0 0,0-1-4162 0 0,0-4-2729 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-759.69">23200 6581 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,4-3 272 0 0,1 1 2425 0 0,8-13-1132 0 0,8 6-314 0 0,-20 9-1141 0 0,10-10 879 0 0,28-21 835 0 0,9 16-867 0 0,-47 15-985 0 0,8-2 305 0 0,41 12-1282 0 0,-40-3 625 0 0,-7 27 186 0 0,-7 1 15 0 0,0-8 170 0 0,-3 12-74 0 0,5-38-411 0 0,2-1-12 0 0,0 0 37 0 0,3 10 308 0 0,16 8-12 0 0,-18-17-372 0 0,7 16-262 0 0,-1 9-1153 0 0,-6-25 785 0 0,-1-1-831 0 0,0 0-363 0 0,0 0-70 0 0,0 0-17 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2740.813">22729 6416 2304 0 0,'2'0'473'0'0,"3"-1"1939"0"0,-5 6 6695 0 0,-1 0-5123 0 0,2 2-5610 0 0,-4 31 3901 0 0,5 1 62 0 0,5 56-84 0 0,7 3-1147 0 0,-4-10 156 0 0,-10 10-32 0 0,-10 12-700 0 0,12-97-583 0 0,-2-12-216 0 0,0-1-65 0 0,0-2-2 0 0,2-34-3313 0 0,-6 24 1834 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2395.418">22751 6439 6912 0 0,'-12'-8'528'0'0,"30"-1"-128"0"0,7-9 4668 0 0,35 16 409 0 0,-56 2-5324 0 0,0 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0 0 0 0,1 2-153 0 0,35 67 2062 0 0,-24 7-1603 0 0,-15-3 1130 0 0,-1-69-1534 0 0,-2 0 1 0 0,2-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,-2-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1-55 0 0,-27 5 67 0 0,32-10-206 0 0,-2 0-58 0 0,-2 0-1 0 0,2-1 1 0 0,-2 1 0 0 0,2-1-1 0 0,0 0 1 0 0,-2 0-1 0 0,2-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-2-1 0 0,0 1 1 0 0,0-1-1 0 0,-1-1 198 0 0,-5-4-5692 0 0,-6-2-1767 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="75099.81">3490 14089 7488 0 0,'0'2'340'0'0,"-7"96"3520"0"0,14 108 4791 0 0,-6 31-4784 0 0,6-60-3019 0 0,4-71-648 0 0,2-64-288 0 0,-13-40-387 0 0,0-2-33 0 0,0 0-192 0 0,0 0-790 0 0,0-5-352 0 0,2-19-70 0 0,-2-4-7 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="75669.811">3540 14184 8288 0 0,'-4'16'381'0'0,"3"-13"-6"0"0,9-34-227 0 0,-7 16 279 0 0,2 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 1 0 0 0,6-6-427 0 0,-10 12 230 0 0,2-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 1 0 0 0,2 0-230 0 0,56-2 1008 0 0,-60 5-919 0 0,1 1 0 0 0,-2 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 2 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0-1 0 0,-2 1 1 0 0,5 3-89 0 0,1 5 277 0 0,-2-1 1 0 0,0 1-1 0 0,0-2 0 0 0,-1 3 0 0 0,0 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 8-277 0 0,10 84 608 0 0,-10-93-471 0 0,-2-1-1 0 0,1 1 1 0 0,-2 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-2 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,-2-3 1 0 0,1 2-1 0 0,-1 0 1 0 0,-1 0-1 0 0,0-2 1 0 0,-1 1-1 0 0,-1 2-136 0 0,0-6 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,-4 0 0 0 0,-11 7 0 0 0,-28 1 0 0 0,43-13-8 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,0 0 1 0 0,2-1-1 0 0,-3-1 8 0 0,-27-47-411 0 0,33 54 334 0 0,3 1 10 0 0,0 0 3 0 0,0 0 0 0 0,13 5-105 0 0,-8-1 109 0 0,2 0 0 0 0,-1-1 0 0 0,-1 2 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1 2 60 0 0,18 20-246 0 0,43 55 1336 0 0,-40-51-896 0 0,1-3 0 0 0,1 1 1 0 0,2-2-1 0 0,9 6-194 0 0,-17-15-3 0 0,77 44-2666 0 0,-82-55 1330 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="85949.811">4368 14718 920 0 0,'0'0'327'0'0,"0"0"1035"0"0,0 9 2340 0 0,-1-6-656 0 0,-1 22 2742 0 0,7-12-4840 0 0,-3-11-526 0 0,-2-2-26 0 0,0 0 12 0 0,0 0 68 0 0,0 0 32 0 0,1 1 4 0 0,47 6 1536 0 0,-7-3-1138 0 0,20-61-236 0 0,30-33 437 0 0,-51 21-618 0 0,-17 6-757 0 0,-23 61 329 0 0,1 0-31 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 1-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1-34 0 0,-5 0 41 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 1 0 0 0,2 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,-2 0-40 0 0,-23 13 98 0 0,24-13-115 0 0,-1-1 0 0 0,0 2 0 0 0,1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-2 0 0 0,-2 5 17 0 0,-18 40 618 0 0,15 23-194 0 0,28 32-1082 0 0,-15-97 704 0 0,1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,2 1 1 0 0,1-1 0 0 0,-2 0 0 0 0,2-2-1 0 0,-1 2 1 0 0,1-2 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 1 1 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0-2 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1-2 1 0 0,3 1-47 0 0,41-5-792 0 0,-52 4 622 0 0,2 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,1-1-1 0 0,-2 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-2 170 0 0,14-9-5654 0 0,-3 7-1513 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="87029.81">5243 14371 1376 0 0,'0'0'65'0'0,"0"0"287"0"0,0 0 1184 0 0,0 0 522 0 0,0 0 100 0 0,0 0-171 0 0,0-15 1609 0 0,18-83 4054 0 0,-10 70-6749 0 0,-8 25-797 0 0,0-3-41 0 0,0 5-160 0 0,0 1-19 0 0,0 0 92 0 0,0 0 344 0 0,0 0 154 0 0,0 0 34 0 0,0 0-97 0 0,0 0-403 0 0,0 0-59 0 0,0 0 127 0 0,0 0 15 0 0,0 0 21 0 0,0 0 128 0 0,0 1 59 0 0,-8 68 675 0 0,-15 51-478 0 0,10-30-496 0 0,1 78 642 0 0,11 77-1033 0 0,-2-167 1100 0 0,-5-19-1141 0 0,8-57 208 0 0,-7 0-1960 0 0,6-1 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="87299.81">5225 14482 12696 0 0,'11'-13'1376'0'0,"41"7"1778"0"0,13-4 1363 0 0,2 1-3125 0 0,4 22-1540 0 0,-47-6-2470 0 0,-18-2-4791 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="204899.81">6380 14813 8288 0 0,'14'-32'1072'0'0,"28"-2"4316"0"0,-38 33-5186 0 0,2 0 1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,-1 2 1 0 0,2-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-2 1 0 0 0,1 3-203 0 0,4 3 280 0 0,-2 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,-1 2 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 7-281 0 0,-1-10 347 0 0,2-5-303 0 0,-1-1 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1-44 0 0,1-1 8 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-2 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2-1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-2-2-8 0 0,-4-3-53 0 0,1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,1 2 0 0 0,0-2 0 0 0,1-1 0 0 0,-3-4 53 0 0,5 10-246 0 0,-1-3 1 0 0,2 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,1 1-1 0 0,-1-2 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-2 245 0 0,11-25-3579 0 0,-5 17-2927 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="203719.811">5759 14589 3224 0 0,'0'-2'240'0'0,"0"-1"25"0"0,0 2 855 0 0,0 1 359 0 0,0 0 66 0 0,0 0-81 0 0,0 0-397 0 0,0 0-178 0 0,0 0-32 0 0,0 0-13 0 0,0 0-24 0 0,0 0-10 0 0,0 0-2 0 0,0 0-18 0 0,0 0-74 0 0,5 29 1869 0 0,-13 143 1427 0 0,-5 3-2668 0 0,7-86-1106 0 0,6-88-198 0 0,1 18-364 0 0,-1-19 191 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 134 0 0,3-13-2091 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="204089.811">5775 14721 8288 0 0,'3'9'2948'0'0,"5"-25"1960"0"0,-3 7-5020 0 0,32-38 3418 0 0,18-5-299 0 0,-52 50-2908 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-99 0 0,22 30 274 0 0,20 32 16 0 0,-2-8-146 0 0,-12-20 0 0 0,-27-24-597 0 0,-3-10-3304 0 0,-2-2 2223 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35574.03">19737 6422 11888 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 14 0 0,1 10 69 0 0,-2 72 4760 0 0,-6-15-2346 0 0,7-29-2146 0 0,-1-34-594 0 0,-4 28-145 0 0,3-22-10 0 0,1-8-188 0 0,1-2-789 0 0,0 0-344 0 0,0 0-65 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35139.521">20015 6425 2304 0 0,'-3'1'3435'0'0,"8"5"13324"0"0,-2-4-18570 0 0,11 93 5563 0 0,1 27-2624 0 0,-6-50-1128 0 0,-7-63-133 0 0,-1-8-563 0 0,-1-1-257 0 0,0 0-922 0 0,0 0-3642 0 0,0 0-1564 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-34747.75">20034 6549 1840 0 0,'0'0'83'0'0,"0"0"373"0"0,0 0 1526 0 0,0 0 670 0 0,0 0 131 0 0,3-1 950 0 0,9-6-2192 0 0,8-23 2196 0 0,-3 12-2845 0 0,-15 13-638 0 0,2 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,5-2-254 0 0,22 15 16 0 0,-26-7-15 0 0,48 49 773 0 0,-49-45-785 0 0,-4-7-105 0 0,14 4-2683 0 0,-15-5 751 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44644.387">19044 6244 3224 0 0,'-1'0'2310'0'0,"-1"1"10093"0"0,1 0-11285 0 0,1 2-3278 0 0,-15 164 7048 0 0,-11 32-3120 0 0,21-142-1645 0 0,7 47-583 0 0,1-97 325 0 0,-3-7-3458 0 0,0 0 1850 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44417.264">18973 6317 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,2 0-220 0 0,59 3 3130 0 0,56 23-834 0 0,-58-19-4427 0 0,-57-7-69 0 0,5 0-4147 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36024.581">19318 6651 2304 0 0,'0'0'348'0'0,"0"0"620"0"0,-9-5 2737 0 0,4-52-382 0 0,5 56-2754 0 0,-8-16 2487 0 0,2-41 2906 0 0,7 52-5754 0 0,0 1-1 0 0,2 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,2-1-207 0 0,-4 3-36 0 0,2-1 14 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,2 1 0 0 0,-2 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,3 0 23 0 0,-3 0 21 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-2 2 0 0 0,2-1 1 0 0,-1 0-1 0 0,-1 1 0 0 0,2 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,2 1-1 0 0,-2 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2 1 0 0 0,1-2 1 0 0,-1 1-1 0 0,-1 1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 0-21 0 0,0 4 5 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 4-5 0 0,2-3 151 0 0,-1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0-1 1 0 0,1 2-1 0 0,-2-1 1 0 0,0 0-1 0 0,0-2 1 0 0,-1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,-3 3-151 0 0,6-8 28 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1-27 0 0,-4-2-27 0 0,0-2-1 0 0,2 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,1-1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0-1 27 0 0,-4-53-3584 0 0,10 56 2142 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33796.383">20397 6645 456 0 0,'0'0'2349'0'0,"0"0"293"0"0,0 0 128 0 0,0 0-221 0 0,0 0-1013 0 0,0 0-448 0 0,0 0-89 0 0,0 0-30 0 0,5 7 1768 0 0,-2-4-2425 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,1 0-312 0 0,58-6 2120 0 0,4-20-1296 0 0,-5-16-672 0 0,-24-1 656 0 0,-16-24-516 0 0,-38 13-160 0 0,14 51-153 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 2-1 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,-3 2 22 0 0,-3 4 44 0 0,1 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1 0 0 0,-5 8-44 0 0,0-2 32 0 0,1 3-32 0 0,0 1 0 0 0,1-2 0 0 0,2 1 0 0 0,-1 1 0 0 0,3 0 0 0 0,-2 7 0 0 0,4-20 8 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0-1-1 0 0,2 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,4 7-8 0 0,11 4 88 0 0,44-10-2149 0 0,-22-14-6089 0 0,-24 3 1076 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33464.079">20897 6642 13824 0 0,'0'0'314'0'0,"-8"7"872"0"0,2 10-891 0 0,5-11 1764 0 0,-1-4 3765 0 0,8-3-5807 0 0,9-6-1723 0 0,-7 1-236 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-28557.543">19783 6192 4144 0 0,'0'0'319'0'0,"0"0"295"0"0,0 0 2022 0 0,0 0 904 0 0,0 0 185 0 0,0 0-408 0 0,0 0-1846 0 0,0 0-815 0 0,0 0-161 0 0,0 0-25 0 0,0 0 16 0 0,0 0 8 0 0,0 0 2 0 0,0 0-64 0 0,0 0-1313 0 0,0 0-4508 0 0,0 0-1916 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19052.719">21172 6390 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 6 160 0 0,3-4 8708 0 0,21 85-4943 0 0,-17 5-3675 0 0,-14-10-98 0 0,10-75-623 0 0,0-6-63 0 0,0-1-165 0 0,0 0-726 0 0,0 0-316 0 0,0 0-65 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-9426.743">21459 6277 920 0 0,'1'-1'67'0'0,"0"-4"143"0"0,0 5 814 0 0,-1 0 355 0 0,0 0 70 0 0,0 0 5373 0 0,0 4-3378 0 0,0 17-2234 0 0,12 160 4151 0 0,-9-31-3309 0 0,1-102-1683 0 0,-1-30-1984 0 0,-1-1-3835 0 0,-2-17 3608 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-8994.302">21459 6439 3224 0 0,'0'6'527'0'0,"10"-30"8375"0"0,8-1-6343 0 0,-16 22-2627 0 0,0-1 178 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-2 1 0 0 0,1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 0-110 0 0,21 31 453 0 0,0 10 891 0 0,-19-24-1051 0 0,1 55 781 0 0,8 8 131 0 0,-5-37-1044 0 0,9-13-3885 0 0,-19-29 1631 0 0,-1-2-17 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7909.834">22089 6376 2760 0 0,'0'0'395'0'0,"0"0"617"0"0,0 0 274 0 0,0 0 53 0 0,0 0-86 0 0,0 0-380 0 0,0 0-163 0 0,0 0-36 0 0,0 0-28 0 0,0 0-85 0 0,6 0 260 0 0,-5-1 2703 0 0,-1 0-3426 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-98 0 0,-11 0 483 0 0,-31 6 677 0 0,-1 20-16 0 0,42-24-1069 0 0,-2 1-1 0 0,2-2 0 0 0,1 2 0 0 0,-2 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,2 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,3 4-74 0 0,28 82 784 0 0,-18-63-634 0 0,-12-21-112 0 0,2-1 0 0 0,-2 0 1 0 0,1 1-1 0 0,1-2 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,1-1-38 0 0,-3-1-114 0 0,0 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,1-1-1 0 0,-2 1 1 0 0,2-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,3-1 114 0 0,4-1-2547 0 0,1-3-5195 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7043.897">22348 6701 7112 0 0,'16'0'324'0'0,"-12"0"-4"0"0,-4 0-94 0 0,0 0 380 0 0,0 0 186 0 0,0 0 37 0 0,0 0 35 0 0,0 0 107 0 0,0 0 42 0 0,0 0 10 0 0,0 0-26 0 0,0 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-58 0 0,0 0-240 0 0,0 0-102 0 0,0 0-17 0 0,0 0-25 0 0,0 0-82 0 0,0 0-40 0 0,0 0-5 0 0,0 0-26 0 0,0 0-108 0 0,0 0-42 0 0,1-18-240 0 0,16 0 132 0 0,-17 17-8 0 0,0 1 88 0 0,0 0 35 0 0,0 0-18 0 0,-1 1-1 0 0,-1 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,2-1 0 0 0,-2 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0-67 0 0,1 1-279 0 0,-1-2-186 0 0,0 0-42 0 0,0 0-209 0 0,0 0-857 0 0,0 0-379 0 0,0 0-80 0 0,0 0-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2101.423">21179 6052 13304 0 0,'0'0'605'0'0,"0"0"-9"0"0,0-1-381 0 0,-2-3-42 0 0,1 2 600 0 0,1 2 260 0 0,0 0 45 0 0,0 0-26 0 0,0 0-144 0 0,0 0-63 0 0,-4 20 1994 0 0,14-13-5523 0 0,-8-7-4821 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122096.968">4045 774 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-120 0 0,0 0 193 0 0,-4-7 582 0 0,-49-23 3117 0 0,25 17-1623 0 0,-50-15-841 0 0,66 25-1311 0 0,2 1-1 0 0,-1 1 0 0 0,-2-1 1 0 0,2 2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 2-1 0 0,1 1 0 0 0,-11 4-284 0 0,17-7 41 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-2 0 0 0 0,2 1-1 0 0,0-1 1 0 0,1-1-1 0 0,-1 2 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 2-40 0 0,6 8 100 0 0,0 0 0 0 0,2-1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,3 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0-100 0 0,-7-6 32 0 0,72 80-590 0 0,-64-67 602 0 0,-1 1 1 0 0,-2 0-1 0 0,1 1 1 0 0,-2 0 0 0 0,0-1-1 0 0,-1 3 1 0 0,-2 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-2 2 1 0 0,-1-2 0 0 0,0 2-1 0 0,-2-2 1 0 0,0 2-1 0 0,-1 0 1 0 0,-3 19-45 0 0,0-26 91 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-2-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,0-2 1 0 0,-1 0-1 0 0,-2 3-91 0 0,7-9 67 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-2 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 1 0 0,-2 1-1 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 1 0 0,-7-2-68 0 0,8 0 4 0 0,-2 0 0 0 0,0 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1-5-4 0 0,-1 1-603 0 0,0 0 1 0 0,1 0-1 0 0,1-2 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-3 603 0 0,-4-12-1535 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122485.17">3932 513 13680 0 0,'0'0'306'0'0,"-5"7"421"0"0,-2 6-534 0 0,-1 0-1 0 0,2 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,2 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-2 11-193 0 0,1-4 459 0 0,-11 62 963 0 0,4 2 0 0 0,4-1 0 0 0,4-1 0 0 0,5 57-1422 0 0,-11 64 1773 0 0,-7-14-700 0 0,0 106-1515 0 0,19-237-1557 0 0,-2-33 952 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="142634.009">4405 1516 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 0 0 0 0,0 0 200 0 0,0 0 24 0 0,-3-7 8 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="185244.55">4559 1861 1376 0 0,'0'0'65'0'0,"0"0"321"0"0,0 0 1322 0 0,0 0 578 0 0,0 0 119 0 0,-2 2 764 0 0,-7 7-2143 0 0,8-9-849 0 0,0 1 1 0 0,0 0-1 0 0,-2 0 1 0 0,2-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-2 0 1 0 0,2 0-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-2-1 0 0 0,2 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1-177 0 0,-12-12 1364 0 0,0-23 743 0 0,15 2-644 0 0,-12-25-661 0 0,12 38-733 0 0,0 1-1 0 0,2 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-1 1 0 0 0,2-1-1 0 0,1 1 1 0 0,0 0-1 0 0,2 1 1 0 0,0 1-1 0 0,2-1 1 0 0,7-10-69 0 0,-7 9-213 0 0,26-24 417 0 0,-35 42-216 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,0 0 1 0 0,0 0 11 0 0,28 11-403 0 0,-14-10 372 0 0,0 10 529 0 0,-2-2 172 0 0,-11-7-605 0 0,2 1-1 0 0,-2-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,1-1-1 0 0,-2 1 0 0 0,0 2-64 0 0,12 25-60 0 0,2 48 132 0 0,-8-44-67 0 0,-6-32 15 0 0,1 1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,-1 5-20 0 0,-6 15 568 0 0,8-26-650 0 0,-3 7-326 0 0,3-8 412 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-4 0 0,-2-25 743 0 0,17-39-633 0 0,-3 28-110 0 0,15-30 0 0 0,23-16-320 0 0,-17 43-430 0 0,0 9 1668 0 0,12 3-918 0 0,-40 25-7 0 0,-1 1-32 0 0,-1 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1 0 38 0 0,-1-2 222 0 0,15 17 286 0 0,0 11-904 0 0,-2 22 920 0 0,-3 11-181 0 0,-7-24 197 0 0,-4 35-687 0 0,0-38 334 0 0,26 36-102 0 0,7-11-74 0 0,-31-56 31 0 0,2 1-20 0 0,29-6 135 0 0,-13-11 0 0 0,6-10-434 0 0,4-17 434 0 0,-20 23-314 0 0,3-2 685 0 0,5-10-776 0 0,-17 28 365 0 0,-1 1-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0 39 0 0,0 0 168 0 0,4-13-278 0 0,-3 10-5968 0 0,0 2-1741 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="186134.947">5706 1624 11288 0 0,'0'0'514'0'0,"-11"-9"196"0"0,9 7-539 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 2 0 0 0,0-2 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-171 0 0,41-45 2046 0 0,-31 39-1874 0 0,-7 6-154 0 0,-2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2 0-18 0 0,-2 0 60 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 1-60 0 0,-1 2 134 0 0,11 71 1428 0 0,-15-53-1106 0 0,-14 39 934 0 0,15-60-1313 0 0,0 1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,2-1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 0 0 0 0,-5 2-77 0 0,-28-4 728 0 0,21-4-305 0 0,14 4-401 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,-2 1 1 0 0,2-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 1 1 0 0,0-2-1 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-2-22 0 0,-1-2-121 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 121 0 0,25-44-8730 0 0,-13 28 1471 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="195187.748">6259 1353 456 0 0,'-7'20'336'0'0,"0"-2"10502"0"0,6-14-10470 0 0,1 53 5149 0 0,0 20-1998 0 0,12 52-1146 0 0,7-58-2293 0 0,15-24 752 0 0,-4-9-288 0 0,-22-31-468 0 0,2-6 16 0 0,33-4 116 0 0,9-22 32 0 0,-4-32-153 0 0,-16 13-38 0 0,-3 6-49 0 0,-6 13 0 0 0,15-37 64 0 0,-12 27-74 0 0,-16 26-44 0 0,3-21 54 0 0,-2 19 28 0 0,-4-7-2 0 0,3-4-69 0 0,-9 21 96 0 0,-3 19-9 0 0,-11 57-144 0 0,9-6 100 0 0,1-40 0 0 0,3 20 0 0 0,-9 41 254 0 0,-11 0-28 0 0,-11 29 293 0 0,6-56 286 0 0,17-40-797 0 0,-1 3 0 0 0,-1-3 1 0 0,-2 1-1 0 0,0-2 0 0 0,-2 1 0 0 0,-7 8-8 0 0,10-16 52 0 0,-1-1-1 0 0,0-1 1 0 0,0 1-1 0 0,-2-1 1 0 0,1-2-1 0 0,-2 0 0 0 0,-4 3-51 0 0,12-8 15 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-2-1 0 0,0 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-2-14 0 0,8 1-35 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0-1 0 0,-2 1 1 0 0,2 0 0 0 0,0-3 34 0 0,-1-1 20 0 0,11-78-2121 0 0,-10 52-659 0 0,0 18 1197 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="196354.103">6930 1723 1840 0 0,'1'-1'138'0'0,"-1"0"0"0"0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,2 0-1 0 0,-2 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,2-1-1 0 0,-2 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1-138 0 0,15 0 3296 0 0,41-8 1940 0 0,-37 1-4448 0 0,63-27 1921 0 0,-16-18-1408 0 0,-57 39-1068 0 0,-8 9-211 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0-1-21 0 0,-1 1 9 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 2 0 0 0,2-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-6-1-9 0 0,-3-4-199 0 0,11 6 228 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-2 1 0 0 0,2 0 0 0 0,0 1-1 0 0,-4-1-28 0 0,-15 4 307 0 0,18-4-243 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-1 4-64 0 0,-1 2 118 0 0,-3 3 3 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,2 0 0 0 0,0 1 0 0 0,0 1 1 0 0,1-2-1 0 0,0 2 0 0 0,2 1 0 0 0,-1-2 1 0 0,2 0-1 0 0,0 8-121 0 0,1-10 43 0 0,1-1-1 0 0,0-1 1 0 0,1 0 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1-1 0 0,0-2 1 0 0,1 1 0 0 0,-1-1 0 0 0,4 5-43 0 0,2 0 29 0 0,30 20 88 0 0,-31-28-139 0 0,1-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 0-1 0 0,0 0 0 0 0,2-1 23 0 0,58-5-3801 0 0,-48 6 2362 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="198120.726">7556 1386 4832 0 0,'2'63'3666'0'0,"1"-42"-222"0"0,-1-20-2786 0 0,-4 33 2622 0 0,4 71 551 0 0,-2-42-3103 0 0,0 44 110 0 0,0-37-4281 0 0,0-69-1079 0 0,0-1-1230 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="198513.93">7545 1647 3680 0 0,'0'0'284'0'0,"0"-1"-187"0"0,0-2 155 0 0,2-11 5681 0 0,8-11-2141 0 0,-4 12-2532 0 0,-5 9-1000 0 0,1-1-1 0 0,-1 2 0 0 0,1-2 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 2 0 0 0,0-1 1 0 0,1 0-260 0 0,31-19 850 0 0,-33 21-780 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1-70 0 0,33 30 293 0 0,34 46 1327 0 0,-72-78-1617 0 0,3 3 19 0 0,1 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1-1 0 0,1-2 1 0 0,-1 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 2-22 0 0,12 54 581 0 0,-21-33-1430 0 0,7-20-1922 0 0,-3 0 1115 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="209019.972">8181 1398 6880 0 0,'0'0'314'0'0,"0"0"-6"0"0,0 0-77 0 0,0 0 409 0 0,0 0 199 0 0,0 0 38 0 0,0 0-32 0 0,0 0-173 0 0,0 0-80 0 0,0 0-14 0 0,0 0-2 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 6 0 0,0 0 30 0 0,7 14 2401 0 0,12 30-517 0 0,-18 34-102 0 0,-9-14-1028 0 0,4-51-1323 0 0,2-1-1 0 0,0 0 1 0 0,1 2-1 0 0,0-1 1 0 0,1 1-1 0 0,0-2 1 0 0,2 6-35 0 0,1 55 86 0 0,1-17-106 0 0,-3-51 540 0 0,-2-5-4113 0 0,1 2-6903 0 0,0-2 5190 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="209481.323">8199 1594 1840 0 0,'0'0'403'0'0,"0"0"1018"0"0,0-5 1680 0 0,1 3 1760 0 0,30-57 991 0 0,-25 52-5592 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-2 0 0 0 0,3 1 1 0 0,2-2-260 0 0,-7 5 92 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 1-1 0 0,2 1-92 0 0,32 50 1184 0 0,-19-12-1184 0 0,-6 49 0 0 0,-7-45 848 0 0,-5-47-637 0 0,0 0-324 0 0,0 0-141 0 0,0 0-30 0 0,0 0-132 0 0,-6 8-4129 0 0,3-6-2469 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="210782.678">8749 1637 6304 0 0,'0'0'289'0'0,"0"0"-8"0"0,0 0-50 0 0,0 0 462 0 0,0 0 218 0 0,0 0 45 0 0,0 0-8 0 0,0 0-77 0 0,2 1-37 0 0,9 4 1041 0 0,-9-4-1679 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,2-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,2-1-197 0 0,68-46 1877 0 0,-8-9-1229 0 0,-54 44-648 0 0,-11 9 43 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-4 1-43 0 0,2 0 15 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 1 0 0 0,2-1 0 0 0,-2 2-15 0 0,0 2 78 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,2 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,0 1-1 0 0,-1 6-78 0 0,1-6 84 0 0,0 3-20 0 0,1 1 0 0 0,1-2 1 0 0,0 2-1 0 0,0 0 0 0 0,1-1 0 0 0,1 0 0 0 0,1 5-64 0 0,35 98 743 0 0,-36-112-717 0 0,0 0 0 0 0,0-2 0 0 0,1 2 0 0 0,-1-1 1 0 0,0 1-1 0 0,2-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,4-1-26 0 0,2-3-217 0 0,0-1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,5-9 217 0 0,26-18-3383 0 0,-26 23 1685 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212336.791">9254 1827 1376 0 0,'0'0'65'0'0,"0"0"286"0"0,0 0 1176 0 0,0 0 510 0 0,0 0 105 0 0,0 0-140 0 0,0 0-688 0 0,0 0-303 0 0,0 0-62 0 0,0 0-31 0 0,0 0-86 0 0,12-8 1503 0 0,26-84 2243 0 0,-1 5-2552 0 0,41-58-1672 0 0,36-14 444 0 0,-53 70 85 0 0,-48 67-1159 0 0,-12 21 177 0 0,-1 1 151 0 0,0 0 68 0 0,0 0 10 0 0,7 10-109 0 0,4 72 56 0 0,-14-3-233 0 0,3 117 500 0 0,4 116-424 0 0,3-244-61 0 0,-7-67-590 0 0,0-1-241 0 0,-1-1-1406 0 0,-5-5-5471 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212940.975">9330 1690 6448 0 0,'0'0'498'0'0,"4"-4"32"0"0,1 1 484 0 0,-4 2-660 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2-1-354 0 0,61-13 3164 0 0,41 29-2595 0 0,-88-14-475 0 0,-4 0-1562 0 0,-3-1-3055 0 0,-1-1-2147 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="213609.296">9944 1568 920 0 0,'0'0'295'0'0,"0"0"901"0"0,-4-15 3639 0 0,2 13-5213 0 0,-4-1 8750 0 0,4 3-7138 0 0,1 0-721 0 0,-7 4 1698 0 0,-14 25-994 0 0,1 21-137 0 0,12 6 52 0 0,23 22 127 0 0,-12-74-1227 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,2 1-32 0 0,-3-1 21 0 0,-1-1-1 0 0,2 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,0-2-20 0 0,58-48-20 0 0,-13-28-456 0 0,-38 41-464 0 0,-25 7-1392 0 0,13 33-2925 0 0,1 0-1661 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="214337.783">10430 1257 2304 0 0,'0'1'167'0'0,"4"23"1727"0"0,-10-6 5773 0 0,-3 113 1948 0 0,6-15-6975 0 0,6-36-2192 0 0,2 73-376 0 0,1-74-72 0 0,6-1-3116 0 0,-12-77 1546 0 0,0-1-280 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="214624.938">10415 1482 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,1-2-344 0 0,28-19 826 0 0,8 15 3479 0 0,3-2-2907 0 0,12 2-1414 0 0,-26 9-2102 0 0,-15 0-4791 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213551.059">10893 1660 10136 0 0,'9'12'230'0'0,"-7"-10"30"0"0,-2-2 19 0 0,0 0 104 0 0,-3 18 7879 0 0,4-17-7647 0 0,-1-1-21 0 0,1 1-38 0 0,10-1-436 0 0,-1 1-1 0 0,1-2 0 0 0,0 1 1 0 0,-1-2-1 0 0,0 1 0 0 0,1 0 1 0 0,0-2-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-2 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-2 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0-1 0 0 0,-2 1 1 0 0,1-2-1 0 0,-1 1 0 0 0,1-1 1 0 0,-3 0-1 0 0,4-5-119 0 0,8-47 69 0 0,-16 58-69 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-4 0 0 0 0,2 1 61 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1-1-61 0 0,-55 56-543 0 0,52-51 613 0 0,0 0 0 0 0,0-1 0 0 0,1 2-1 0 0,-1 0 1 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,-1 7-70 0 0,1-9 0 0 0,1 2 0 0 0,1-2 0 0 0,0 2 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,3-1 0 0 0,-2 0 0 0 0,1 1 0 0 0,0-2 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,7 5 0 0 0,-9-8-56 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,2-1 56 0 0,8-4-1098 0 0,2-2-56 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213242.538">11481 1492 4608 0 0,'-19'14'3105'0'0,"0"1"6005"0"0,11-1-7943 0 0,-4 9 1032 0 0,10 16-1221 0 0,-4 45 1209 0 0,5-77-2095 0 0,1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,2-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 0 0 0,2-2 1 0 0,-1 1-1 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 1 0 0,2-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,1-2 0 0 0,2 3-92 0 0,2-3 0 0 0,-7-5 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,19-28 0 0 0,-3-1 0 0 0,0-2 0 0 0,-2 1 0 0 0,-1-3 0 0 0,-8 12 0 0 0,-16 8-1384 0 0,7 17 600 0 0,2 1-1144 0 0,0 0-496 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212663.88">12024 1435 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0 88 0 0,0 0 1067 0 0,0 0 483 0 0,0 0 98 0 0,0 0-138 0 0,0 0-670 0 0,0 0-295 0 0,0 0-60 0 0,0 0-101 0 0,0 0-377 0 0,0 0-167 0 0,0 0-31 0 0,-3 9 1448 0 0,-1 88 1023 0 0,11-7-2584 0 0,-3-31 1296 0 0,3 90-752 0 0,-3-138-818 0 0,-3-10-854 0 0,-1-1-382 0 0,0 0-76 0 0,0 0-20 0 0,0 0-2 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212449.687">12046 1643 456 0 0,'-5'-9'365'0'0,"4"8"1529"0"0,1-5 6369 0 0,3-6-4715 0 0,18-27-181 0 0,-11 20-2471 0 0,-4 10-747 0 0,-5 7-63 0 0,1-1-1 0 0,0 0 0 0 0,-1 2 0 0 0,1-2 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0-85 0 0,-3 1 239 0 0,10 5 186 0 0,-6-3-373 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,2 4-52 0 0,6 5 0 0 0,-10-12-55 0 0,-1-1-16 0 0,6 5-460 0 0,-5-3-2608 0 0,-1-2-3526 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-206308.339">2988 2565 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,0 2-294 0 0,-5 8 6808 0 0,-1-7-3282 0 0,-9-19-2050 0 0,15 15-1469 0 0,-11-96 2153 0 0,11-133-1048 0 0,-4-1-752 0 0,-8-53-24 0 0,-2 48-128 0 0,2-94-168 0 0,8 158 559 0 0,-10-50-726 0 0,10 92-532 0 0,-3 19 446 0 0,3 38-11 0 0,-1 17 64 0 0,2 2 0 0 0,7-106 128 0 0,4 124-128 0 0,10 14 0 0 0,-10 19-4 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,8 3 4 0 0,33 10 0 0 0,-24-7 79 0 0,1 0 0 0 0,-1-2-1 0 0,1-1 1 0 0,0-1-1 0 0,1-1-78 0 0,35-2-104 0 0,1-3 0 0 0,-1-3-1 0 0,1-3 1 0 0,58-14 104 0 0,392-67 0 0 0,-394 80 0 0 0,0 4 0 0 0,1 6 0 0 0,36 8 0 0 0,19-2 0 0 0,4-5 99 0 0,1-7-1 0 0,84-15-98 0 0,-112 7 64 0 0,106 6-64 0 0,-165 11 41 0 0,0 4-1 0 0,38 10-40 0 0,8 1 143 0 0,76 4 11 0 0,3-10-1 0 0,165-12-153 0 0,37-21 125 0 0,-298 15-98 0 0,158 4 106 0 0,184 31 123 0 0,-73-1-170 0 0,356-32 188 0 0,-323 22 29 0 0,-187-5-190 0 0,-63-3-38 0 0,160-12-75 0 0,34-13 0 0 0,-173 6 128 0 0,41 10-128 0 0,331 41 0 0 0,-477-43 0 0 0,36-16 64 0 0,62-21-160 0 0,-135 34 85 0 0,22-1-42 0 0,26-26 429 0 0,-66 28-376 0 0,-17 8 0 0 0,-3 4 0 0 0,11 15 0 0 0,-13 3 0 0 0,20 61 0 0 0,-13 3-189 0 0,-6 2-1 0 0,6 91 190 0 0,-10 11 307 0 0,6 182-618 0 0,-12 110 606 0 0,2-144-200 0 0,5-3-14 0 0,-6-148-6 0 0,-5-175-59 0 0,0-1 1 0 0,-2 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-1 1-1 0 0,0-2 1 0 0,-4 11-17 0 0,6-23 9 0 0,1 0 0 0 0,-2 1 0 0 0,1-2 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-9 0 0,-48-3 22 0 0,1-3 0 0 0,0-1-1 0 0,2-4 1 0 0,-12-3-22 0 0,-92-17 52 0 0,-116 9-87 0 0,28 29 35 0 0,-364 9 0 0 0,-20-17 0 0 0,310 18 70 0 0,-15 15-70 0 0,-69 7 47 0 0,301-31-39 0 0,-409 17-5 0 0,-361-20-3 0 0,-353 31 240 0 0,658-43-256 0 0,118-15-48 0 0,24-5 64 0 0,-82 5 11 0 0,214 10 114 0 0,-76-25-85 0 0,-45-29-40 0 0,261 47 0 0 0,-15 5 0 0 0,-2 28 0 0 0,-40-12 0 0 0,87-8-100 0 0,111 4 7 0 0,7 3-64 0 0,1-1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1 156 0 0,1-9-10012 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202306.829">7690 2872 3224 0 0,'0'2'240'0'0,"19"54"4562"0"0,-8-8 530 0 0,-4-24-2824 0 0,-2 9-572 0 0,6 45 269 0 0,5 25-781 0 0,-2 48 0 0 0,6 108 552 0 0,-2-121-1272 0 0,9 149 568 0 0,-18-37-696 0 0,1-120-389 0 0,-2 41 722 0 0,-8-53-581 0 0,-4-1-93 0 0,8-7-91 0 0,-8 41-19 0 0,4-97-61 0 0,-4 83 0 0 0,-1-105-64 0 0,5-26-67 0 0,0-5-281 0 0,0-1-129 0 0,0 0-31 0 0,0 0-72 0 0,-4-17-3152 0 0,1 3-2356 0 0,-1-4-1623 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201855.109">7349 4585 12264 0 0,'0'0'273'0'0,"-5"13"786"0"0,5-3-595 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 2 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-2 0 0 0,2 7-464 0 0,-5-10 43 0 0,52 109 3185 0 0,30 114 95 0 0,-65-163-2734 0 0,2-1 0 0 0,28 55-589 0 0,19 11 416 0 0,-3-51-72 0 0,-52-71-248 0 0,-1 2-1 0 0,0-1 0 0 0,2 0 1 0 0,-1-1-1 0 0,1-1 1 0 0,12 6-96 0 0,-20-11 39 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-1-39 0 0,64-62 528 0 0,18-72-224 0 0,73-275-391 0 0,-145 378-257 0 0,24-55-4278 0 0,-33 80 2515 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186308.475">14143 1218 1840 0 0,'0'0'83'0'0,"0"0"-6"0"0,0 5 363 0 0,0-4 1761 0 0,0-1 766 0 0,1 18 5666 0 0,1 0-5371 0 0,2 17-970 0 0,-4-24-1727 0 0,-12 103 2961 0 0,-25 77-2557 0 0,41-152-1425 0 0,-4-39 48 0 0,0 0-940 0 0,0 0-410 0 0,1 0-88 0 0,4-5-10 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-185850.611">14511 1218 13040 0 0,'0'0'597'0'0,"0"0"-9"0"0,0 0-220 0 0,0 0 481 0 0,0 0 250 0 0,0-5 715 0 0,-1 4 3304 0 0,-5 3-5002 0 0,0 1 0 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 0 0 0,2 1 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,2-2-1 0 0,-2 2 1 0 0,1-1-1 0 0,1 1 0 0 0,-2 3-116 0 0,1 2 121 0 0,-1-1-1 0 0,2 1 1 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 1 1 0 0,0-2-1 0 0,1 2 1 0 0,0-1-1 0 0,1 0 1 0 0,0 0-1 0 0,2 1 1 0 0,-1-1-1 0 0,1-1 1 0 0,0 0-1 0 0,4 5-120 0 0,48 107 0 0 0,-49-92 0 0 0,-8-23 0 0 0,0-5 60 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 0 0 0 0,2-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,-2-2-60 0 0,-4-4-110 0 0,8 7-9 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 119 0 0,1-6-1959 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-187118.879">13464 897 13184 0 0,'0'0'604'0'0,"0"0"-14"0"0,0 0-252 0 0,0 0 326 0 0,0 0 185 0 0,0 0 41 0 0,2 0-12 0 0,-1-1-747 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2 0-131 0 0,6 17 493 0 0,-1-1 0 0 0,-1 0 0 0 0,1 2-1 0 0,-3-1 1 0 0,1 18-493 0 0,-3-32 76 0 0,-2 88 1295 0 0,1 19-942 0 0,-6-16-247 0 0,-2 114-43 0 0,13-167-247 0 0,-3-42-448 0 0,-1-1-176 0 0,0 0-32 0 0,3-21-3836 0 0,-2 2 2544 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186774.862">13540 1278 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-79 0 0,0 0-421 0 0,0 0-180 0 0,0 0-37 0 0,0-13 1908 0 0,1 8-2997 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0-346 0 0,14-9 712 0 0,-16 10-708 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,3 1-4 0 0,-2-1 90 0 0,2 2-1 0 0,-2-1 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,2 1 0 0 0,-2-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1-2 0 0 0,-1 2 1 0 0,0 1-1 0 0,1 0-89 0 0,54 195 1931 0 0,-52-175-1912 0 0,0-1 1 0 0,-1 1-1 0 0,-2 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,-2 4-19 0 0,0 4-4294 0 0,2-33-4235 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184500.214">14926 1102 11976 0 0,'-4'2'1082'0'0,"-18"92"550"0"0,1 52 3297 0 0,15 50-1046 0 0,9-96-3866 0 0,5-72-17 0 0,-8-26-850 0 0,0 3 2050 0 0,0-2-4324 0 0,0 3-3781 0 0,0-6 913 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184054.319">14990 1145 3224 0 0,'0'0'143'0'0,"1"1"-3"0"0,4 4 390 0 0,13 9 9462 0 0,3 0-5178 0 0,-16-11-4675 0 0,-2-1-1 0 0,1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 0-138 0 0,34 3-1260 0 0,-22-7 497 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-183416.48">14861 1231 5960 0 0,'-3'-8'266'0'0,"3"7"1"0"0,0-21 1002 0 0,10-16 3955 0 0,13-7-2882 0 0,-12-3-311 0 0,-9 45-2036 0 0,-6-13-175 0 0,-1 12-433 0 0,5 4-2775 0 0,0 0 1855 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-182333.102">15261 1519 0 0 0,'0'0'2721'0'0,"0"0"-302"0"0,0 0 223 0 0,1-1-119 0 0,9-8-671 0 0,-9 7-1682 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,2-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,2 0 1 0 0,-2 1-1 0 0,0-1 0 0 0,0 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,0 1-1 0 0,0 0-170 0 0,6 2 296 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-2 1 0 0 0,1-2 0 0 0,0 2 0 0 0,-2-1 0 0 0,2 2 1 0 0,-2-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,3 8-296 0 0,8 42 792 0 0,-13-54-721 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-3 2-71 0 0,5-4 2 0 0,-1 1 15 0 0,-1 1 1 0 0,-2-1-1 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,-2-2-18 0 0,1 1 49 0 0,-2-1 1 0 0,0 0-1 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,-1-1-1 0 0,2 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-2-49 0 0,3 2-126 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,3-3 126 0 0,13-34-3998 0 0,-3 21-3873 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-175901.286">15724 1488 4144 0 0,'0'0'191'0'0,"0"0"375"0"0,-4-9 14804 0 0,9 56-13610 0 0,3 16 8 0 0,3 27 351 0 0,-10-75-1781 0 0,8 24-3577 0 0,-9-38 1789 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172641.548">16474 1641 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,1 1-72 0 0,16 38 5565 0 0,-11-27-3129 0 0,-1-10-2556 0 0,2-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 0 0 0 0,2 1 0 0 0,-1-2 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,-2 1 0 0 0,5-4-209 0 0,67-62 153 0 0,-54 34-213 0 0,-21 34 61 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 0 0 0,-1-1 2 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 1 1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 1-2 0 0,-17 7 0 0 0,17-7 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 4 0 0 0,-6 11 27 0 0,7-10 0 0 0,-1-1-1 0 0,0 0 1 0 0,2 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,0-2 0 0 0,-1 2-1 0 0,2-1 1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,1 2-27 0 0,0-6-27 0 0,-1 0-1 0 0,1 1 1 0 0,0 0 0 0 0,1-2-1 0 0,0 1 1 0 0,-1 1-1 0 0,3-2 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,2 0-1 0 0,4 5 28 0 0,16-3 0 0 0,22-16-1385 0 0,-32 1-166 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172385.72">16998 1665 11832 0 0,'-38'14'7253'0'0,"35"-12"-6259"0"0,3-1-12 0 0,0-1-29 0 0,0 0-122 0 0,0 0-482 0 0,0 0-205 0 0,0 0-44 0 0,0 0-7 0 0,0 0 17 0 0,0 0 8 0 0,0 0 2 0 0,0 0-237 0 0,0 0-996 0 0,0 0-434 0 0,1 0-86 0 0,4 0-21 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170574.714">17831 1086 2760 0 0,'0'0'589'0'0,"0"0"1434"0"0,0 0 626 0 0,0 0 126 0 0,0 0-214 0 0,0 7 88 0 0,0 167 4329 0 0,0 88-4387 0 0,-1-163-2591 0 0,-4 26 0 0 0,5-61 0 0 0,-3-3-134 0 0,3-60-570 0 0,0-1-263 0 0,0 0-916 0 0,0-1-3632 0 0,-3-5-1553 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170137.543">17792 1532 5064 0 0,'0'0'389'0'0,"3"-3"794"0"0,-1 2 3071 0 0,27-32 3094 0 0,8-2-4244 0 0,21-5-1223 0 0,-52 39-1852 0 0,-2 1 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2-2 0 0 0,1 2 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-2-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,-1 1-29 0 0,5 14 310 0 0,-1 3 0 0 0,-1-1 0 0 0,-1 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,-1 8-310 0 0,-8 89 1048 0 0,8-91-908 0 0,6 1-148 0 0,10-34-432 0 0,5-13-1437 0 0,1 1-5762 0 0,-9 7 145 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172102.041">17333 1321 9760 0 0,'4'-25'2366'0'0,"-4"24"-894"0"0,0 1 68 0 0,0 0-60 0 0,0 0-321 0 0,0 0-139 0 0,0 0-27 0 0,0 0-34 0 0,0 0-114 0 0,-3 6 736 0 0,-8 70 997 0 0,2 34-801 0 0,-7 75-1676 0 0,10-113-101 0 0,2 24 0 0 0,3-85 704 0 0,-1 0-2693 0 0,1 3-6478 0 0,1-14 756 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-171739.932">17367 1321 16064 0 0,'5'-13'1715'0'0,"-3"9"-1471"0"0,0 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,4 0-244 0 0,-4 0 90 0 0,2 0 1 0 0,-2 0-1 0 0,2 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-2 0-1 0 0,1 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,2 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,-2 0-1 0 0,4 2-90 0 0,-3 7 116 0 0,0-1 0 0 0,1 0 0 0 0,-2 0-1 0 0,0 1 1 0 0,1 0 0 0 0,-3 0 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,-2-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-3-2 0 0 0,2 1 0 0 0,-2 0-1 0 0,0 0 1 0 0,-6 9-116 0 0,-44 65 1297 0 0,53-83-1274 0 0,1 1-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 0 1 0 0,2-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 0-22 0 0,-2-2-128 0 0,3 1 21 0 0,0 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,1-2 0 0 0,0 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,1 0 106 0 0,-1-9-1478 0 0,-3 1-66 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174133.091">16119 1371 4144 0 0,'0'0'319'0'0,"0"0"-7"0"0,0 0 751 0 0,0 0 355 0 0,0 0 71 0 0,0 0-42 0 0,0 0-234 0 0,0 0-101 0 0,0 0-21 0 0,0 18 3966 0 0,-10 4-3283 0 0,9-20-1264 0 0,1-2-29 0 0,0 2-8 0 0,-4 241 2166 0 0,-9-131-2099 0 0,7-59 33 0 0,-1 19-3333 0 0,8-73 56 0 0,2-7-4807 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173508.196">16078 1601 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,1-1 491 0 0,29-51 6288 0 0,-28 49-6862 0 0,-1-1 1 0 0,1 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2 0 0 0 0,-2-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,2 1-157 0 0,-1 0 54 0 0,1-1 0 0 0,-2 2 0 0 0,0-2 0 0 0,1 2-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 0-53 0 0,0-5-149 0 0,4 18-2358 0 0,-4-9 487 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-169732.621">18411 1347 18287 0 0,'0'0'414'0'0,"0"0"56"0"0,0 1 32 0 0,0 81 1564 0 0,-12 57 154 0 0,1 9-612 0 0,4-20 14 0 0,-2-49-1333 0 0,9-78-974 0 0,0-1-274 0 0,0 0-53 0 0,0 0-215 0 0,0 0-858 0 0,0 0-379 0 0,1-2-80 0 0,3-12-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168923.508">18476 1460 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,3-7-322 0 0,4-4-3 0 0,-4 5 250 0 0,1 1-1 0 0,-1-1 1 0 0,2 2 0 0 0,-2-1 0 0 0,1 0 0 0 0,1 0-1 0 0,1 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,-2 1-1 0 0,2 0-460 0 0,-3 0 236 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 2-1 0 0,1-1 1 0 0,-1 0-236 0 0,2 1 105 0 0,-2 2 0 0 0,2-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2 5-105 0 0,13 81 177 0 0,-29 76 1151 0 0,-12-105-745 0 0,20-60-571 0 0,1 0 0 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-2 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-2-1 0 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-2 0 0 0,0 1 0 0 0,-1-1-12 0 0,-4-2-508 0 0,0 1 0 0 0,0-2 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 2 0 0 0,0-3 0 0 0,0 1-1 0 0,0-1 1 0 0,-5-7 508 0 0,0 0-1504 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-130876.917">3193 5992 6448 0 0,'25'-2'672'0'0,"-21"1"-608"0"0,0 3 3996 0 0,-1 5-3602 0 0,-3-3 96 0 0,1-3 14 0 0,-4 12 453 0 0,10 160 2956 0 0,-12 68-1512 0 0,9-94-1338 0 0,4-70-1094 0 0,-5-69-94 0 0,-3-6-264 0 0,5-16-6236 0 0,-2 2 317 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-124973.04">3214 6042 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 0-79 0 0,0 0 561 0 0,0 0 272 0 0,-3 6 1195 0 0,-4-3 2766 0 0,8-9-4160 0 0,9-13-1197 0 0,-8 12 345 0 0,3 1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 0 0 0 0,3 0 0 0 0,-2 1 0 0 0,1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,4 0-78 0 0,-7 2-15 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 15 0 0,23 112 716 0 0,-25-113-672 0 0,3 2 51 0 0,-2 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-3 0 0 0,0 3 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1-95 0 0,-38 25 236 0 0,34-28-233 0 0,-3 2 17 0 0,0-1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2-2 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,-9 0-20 0 0,-29-5-116 0 0,47 0 127 0 0,2 2 42 0 0,11 13-2 0 0,40 47-118 0 0,71 108 1347 0 0,-71-100-1908 0 0,-31-54-2350 0 0,-10-7-4791 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123928.98">3716 6562 3224 0 0,'0'0'143'0'0,"0"0"315"0"0,0 0 1222 0 0,0 0 531 0 0,0 0 106 0 0,0 0-213 0 0,0 0-968 0 0,0 0-428 0 0,5 9 1069 0 0,1-7-1546 0 0,1 0-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 0-1 0 0,0 0 1 0 0,-2-1-1 0 0,2 0 1 0 0,0-1 0 0 0,0 1-1 0 0,-2-1 1 0 0,2-1-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,-1-1 1 0 0,3-2-231 0 0,-8 3-25 0 0,11-4 212 0 0,2 0-1 0 0,-2-1 0 0 0,1-1 0 0 0,-2 0 0 0 0,1-1 0 0 0,0-1 1 0 0,-2 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0-2-186 0 0,-6 7 3 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-2-4-3 0 0,1 7 35 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 2-1 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,0-1 0 0 0,-2 1-35 0 0,1-1 16 0 0,-2 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-2 0 0 0,-1 1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-16 0 0,-55 117 249 0 0,39-11-267 0 0,19-103 28 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,2-1-1 0 0,0 0 1 0 0,1-1 0 0 0,-2 0-1 0 0,5 4-9 0 0,-6-6 6 0 0,2-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0-1 1 0 0,1 1 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1-1 0 0 0,-1 1-1 0 0,2-1 1 0 0,-2 1 0 0 0,1-1-1 0 0,0-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,6-1-6 0 0,-5 0 57 0 0,26-6-1613 0 0,-10 1-3577 0 0,-3-4-2072 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123239.429">4355 6120 920 0 0,'0'0'279'0'0,"0"0"833"0"0,0 0 362 0 0,0 0 78 0 0,0 0-63 0 0,0 0-322 0 0,0 0-140 0 0,0 0-31 0 0,0 0-26 0 0,0 0-88 0 0,0 0-40 0 0,0 0-8 0 0,0 0-34 0 0,0 0-136 0 0,0 0-66 0 0,0 0-12 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0-42 0 0,0 6-12 0 0,-10 47 1334 0 0,2 12-600 0 0,0 49 252 0 0,9 94-1210 0 0,3-94-216 0 0,7-12 642 0 0,-4-88-1088 0 0,-6-13-25 0 0,-1-1-998 0 0,0 0-429 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122817.09">4326 6331 12176 0 0,'0'0'561'0'0,"0"0"-17"0"0,2 1-217 0 0,87 9 5294 0 0,-11 7-5284 0 0,-11 11-2062 0 0,-65-28 475 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122538.437">4797 6618 2304 0 0,'-12'-8'3825'0'0,"10"5"-3248"0"0,-2 1 1 0 0,2-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-2-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-4-578 0 0,1 3 116 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-2 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0-116 0 0,-1 1 36 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-2 0 0 0,0 2 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 2-36 0 0,57 58 1232 0 0,-54-50-822 0 0,0 1 0 0 0,0-1-1 0 0,-2 0 1 0 0,1 2-1 0 0,-2 0 1 0 0,0-2-1 0 0,-1 3 1 0 0,1-1-1 0 0,-3-1 1 0 0,1 1 0 0 0,-1 10-410 0 0,-14 35 100 0 0,11-55-42 0 0,1 1 0 0 0,0-2 1 0 0,0 2-1 0 0,-1-1 0 0 0,1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-2 0-1 0 0,2-2 0 0 0,-1 2 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-2 1-58 0 0,-2-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,1-1 0 0 0,-6-2 0 0 0,-33-45-1424 0 0,33 25-5473 0 0,4 13-533 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121496.511">5209 6416 15176 0 0,'0'0'340'0'0,"0"0"50"0"0,-2 1 26 0 0,-15 18 101 0 0,13-15-271 0 0,1 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,2 1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0-245 0 0,4 55-21 0 0,47 57 1584 0 0,-48-113-1524 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,3 0-39 0 0,-1-3-10 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-2 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,1-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,-1 0 0 0 0,2-1-1 0 0,-2 0 1 0 0,0-2 10 0 0,3-3 49 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1 1 0 0 0,1-2 0 0 0,-3 0-1 0 0,1 0 1 0 0,-2-11-49 0 0,1 10-17 0 0,0 17 17 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 0 0 0,-13 36-209 0 0,13 86 192 0 0,12-86-2918 0 0,-11-24 1407 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-118100.252">5728 6363 4608 0 0,'24'-31'2473'0'0,"-15"16"4749"0"0,-3 19-1038 0 0,-1 7-5674 0 0,0-1-1 0 0,0 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 2-509 0 0,6 35 445 0 0,-1 21-52 0 0,5 67-233 0 0,-8-74-380 0 0,6 3-218 0 0,-11-63 32 0 0,0-2-1020 0 0,0 0-4245 0 0,0 0-1815 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-117537.033">5781 6463 1376 0 0,'0'0'448'0'0,"0"0"1344"0"0,0 0 588 0 0,0 0 116 0 0,0 0-136 0 0,0 0-684 0 0,0 0-299 0 0,0 0-58 0 0,0 0-107 0 0,0 0-419 0 0,0 0-179 0 0,0 0-35 0 0,0 0-40 0 0,11-4 578 0 0,54-61 1084 0 0,-62 64-2155 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,2-1-45 0 0,43 32 240 0 0,-11 32 664 0 0,-36-64-973 0 0,-1-1-608 0 0,0 0-262 0 0,0 0-1349 0 0,0 0-5210 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116084.978">6328 6509 920 0 0,'0'17'0'0'0,"0"-17"80"0"0,0 0-80 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 352 0 0,0 0 64 0 0,0 0 0 0 0,0 0 8 0 0,0 6-424 0 0,0-6 0 0 0,0 0 0 0 0,2 11-96 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115526.386">6353 6310 7856 0 0,'0'0'174'0'0,"0"0"29"0"0,0 0 13 0 0,0 9 2112 0 0,7 26 1209 0 0,-5-8-1555 0 0,3 65 1712 0 0,0 26-2229 0 0,-1-45-1465 0 0,-3-29 69 0 0,-2-27-2628 0 0,1-12 952 0 0,0-5-279 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115183.311">6353 6559 11832 0 0,'0'-16'1285'0'0,"24"-58"4317"0"0,20 31-3283 0 0,-40 42-2299 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 1-1 0 0,2-1 1 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 1-20 0 0,19 37 831 0 0,19 53 83 0 0,-30-45-684 0 0,-7 9 68 0 0,-7-27-874 0 0,3-30 150 0 0,0-1-988 0 0,-1 1-436 0 0,-1 4-92 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-114236.626">6843 6575 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0 0 43 0 0,0 0 159 0 0,0 0 70 0 0,0 0 14 0 0,0 0 69 0 0,0 0 285 0 0,0 0 126 0 0,0 0 29 0 0,0 0-15 0 0,0 0-77 0 0,0 0-31 0 0,0 0-8 0 0,0 0-33 0 0,0 0-134 0 0,2 1-61 0 0,49 6 2321 0 0,-33-8-2644 0 0,36-20 394 0 0,-50 19-751 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,2 1-1 0 0,-3-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-4 19 0 0,-8-6 0 0 0,7 11 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,-2 1 76 0 0,0 1 0 0 0,1 1-1 0 0,-1-1 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,2-1-1 0 0,0 3-75 0 0,44 52 0 0 0,-45-59 25 0 0,0 0 0 0 0,2 0 0 0 0,-1-2 0 0 0,0 1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,3-1-25 0 0,49-22-3889 0 0,-46 16-4253 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-106495.084">7428 6399 2760 0 0,'-36'-28'1211'0'0,"35"27"-702"0"0,-15-6 1981 0 0,-3 8-1483 0 0,11 5-408 0 0,-29 17 451 0 0,16-22 2469 0 0,7-5 2535 0 0,20-3-4219 0 0,47-13 338 0 0,40 21-421 0 0,-86 2-1693 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,0 3-59 0 0,49 33-101 0 0,-17-39 802 0 0,-37-2-571 0 0,-1 1 4 0 0,0 0-4 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-2 0 0,0 0-6 0 0,-19 27 213 0 0,-29 2-28 0 0,13-8-202 0 0,-39 15-64 0 0,-29 23 212 0 0,55-16-359 0 0,22-15 389 0 0,21-19-217 0 0,2-3 36 0 0,4-5-46 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-14 0 0,51-13 417 0 0,162-21 582 0 0,-159 37-919 0 0,-12 12-3590 0 0,-43-16 1676 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101751.894">7867 6714 3680 0 0,'-7'16'1721'0'0,"6"-11"9907"0"0,15-11-8856 0 0,15-13-2535 0 0,54-86 2026 0 0,3-45-1063 0 0,54-113-374 0 0,13 12-1554 0 0,-126 226 728 0 0,-10 0 0 0 0,-17 26 24 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1-23 0 0,-1 23 138 0 0,-1-2 0 0 0,-2 2 0 0 0,0-3-1 0 0,-2 3 1 0 0,-6 17-138 0 0,-7 28 173 0 0,-12 72-35 0 0,23-43 4 0 0,8-80-93 0 0,-1 0 0 0 0,2-1 0 0 0,0 0 1 0 0,2 0-1 0 0,-1 1 0 0 0,1-2 1 0 0,2 7-50 0 0,1 1 36 0 0,8 20 71 0 0,12 0 53 0 0,-17-48 10 0 0,63-153 270 0 0,-2 17-376 0 0,55-136-64 0 0,-75 182 0 0 0,-36 77 0 0 0,-14 19-2 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 2 0 0,0 0-1 0 0,8 57-63 0 0,-4 41 64 0 0,-8 38 203 0 0,-7 2 7 0 0,-6 36-63 0 0,-5-60-94 0 0,8-21-185 0 0,7-62-625 0 0,7-30-572 0 0,0-1-410 0 0,0 0-1290 0 0,0 0-4861 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101158">9041 6595 11232 0 0,'0'0'256'0'0,"0"0"34"0"0,0 0 20 0 0,-2 0-40 0 0,-30-3 1829 0 0,31 3-1367 0 0,1-2 59 0 0,9-45 2427 0 0,-7 39-3131 0 0,1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,0 1 1 0 0,-1 1-1 0 0,2-2 1 0 0,-1 1-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,2 0-86 0 0,-5 2 36 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-2 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-36 0 0,4 7 185 0 0,-1-1 0 0 0,0-1 0 0 0,-1 2 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-2-1-1 0 0,0 2 0 0 0,0-1 0 0 0,-3 7-185 0 0,5-16 57 0 0,-1 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-2 1-1 0 0,2-1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-3-57 0 0,-4 1-194 0 0,2-1 0 0 0,0 0 0 0 0,-1-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,2 0 1 0 0,0-1 0 0 0,-3-4 194 0 0,-5-35-3540 0 0,7 26-4246 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-100410.518">9669 6366 8496 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 10 0 0,0 0 112 0 0,-1 1 406 0 0,-38 74 4453 0 0,12-34-3370 0 0,13-1-456 0 0,12-15-994 0 0,-10 29 976 0 0,12-51-1274 0 0,0 2 0 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-2-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1-81 0 0,7 1 0 0 0,-2 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,4-7 0 0 0,56-96 0 0 0,-30 21 1046 0 0,-29 50-920 0 0,-7 38-27 0 0,-1 1-10 0 0,0 0 6 0 0,0 0 29 0 0,8 1 281 0 0,-2 12-392 0 0,2 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,-3 1 0 0 0,2 0 0 0 0,-3 1 0 0 0,1 0 0 0 0,-1-2 0 0 0,-1 2-1 0 0,-1 0 1 0 0,1 1 0 0 0,-2-2 0 0 0,-2 6-13 0 0,-14 100 1090 0 0,1-77-947 0 0,-2 0 1 0 0,-1-2 0 0 0,-2 0 0 0 0,-2 0-1 0 0,-1-3 1 0 0,-11 12-144 0 0,22-33 225 0 0,-1-2 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-3 0 0 0,-1 1-1 0 0,1-1 1 0 0,-2-1 0 0 0,0-1 0 0 0,-16 9-225 0 0,30-18-3 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-2-2 3 0 0,2-5-150 0 0,1 0 0 0 0,0-1 1 0 0,0 2-1 0 0,1-2 0 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,2 0 0 0 0,-2 1 1 0 0,1-1-1 0 0,2 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,3 1 150 0 0,4-14-1149 0 0,3-3-679 0 0,-2 4-278 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-99222.683">10300 6615 10136 0 0,'2'14'230'0'0,"-2"-11"30"0"0,0-3 19 0 0,0 0 105 0 0,0 0 411 0 0,0 0 182 0 0,10 7 1891 0 0,-6-4-2546 0 0,2-1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-2-1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,-1-1-1 0 0,3 0-322 0 0,3-2 206 0 0,1 1 0 0 0,-2 0 0 0 0,0-2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,3-4-206 0 0,44-70 696 0 0,-52 72-668 0 0,-1 0-1 0 0,0 0 1 0 0,-1-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 2 0 0 0,-1-2 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,-1-5-28 0 0,3 11 5 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,1-1-1 0 0,-1 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-2 1 1 0 0,2-1-1 0 0,0 1 1 0 0,-2 0-1 0 0,2-1 1 0 0,0 1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-5 0 0,-5 6 19 0 0,1 1 1 0 0,-1-3 0 0 0,2 4 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1-1 0 0 0,2 2-1 0 0,-1-1 1 0 0,2 0 0 0 0,-1 2-20 0 0,0-1 77 0 0,0 1-1 0 0,2 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 2 1 0 0,2-1 0 0 0,0 0 0 0 0,2 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,2 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,2-1-1 0 0,0 0 1 0 0,1 1-77 0 0,-3-6 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,0 0-1 0 0,-2 0 1 0 0,3 0 0 0 0,37-17-1473 0 0,-26 4 614 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95784.39">10871 6370 4608 0 0,'0'0'353'0'0,"0"0"35"0"0,0 0 1008 0 0,0 0 461 0 0,0 0 95 0 0,0 0-104 0 0,0 0-522 0 0,0 0-228 0 0,0 0-46 0 0,1 2-59 0 0,11 17 2469 0 0,6 30-1092 0 0,-11 39-307 0 0,-1 15-686 0 0,-9 7-869 0 0,3-108-577 0 0,0-2-52 0 0,0 0-21 0 0,0 0-198 0 0,0 0-824 0 0,0 0-362 0 0,0-1-1274 0 0,-3-4-4833 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94862.106">10920 6585 10016 0 0,'0'0'462'0'0,"0"0"-12"0"0,0 0-148 0 0,1-4 1464 0 0,51-65 3773 0 0,4 10-3387 0 0,-30 49-1432 0 0,-25 9-464 0 0,7 5 586 0 0,-3 0-782 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 2-60 0 0,2 8 248 0 0,14 67 841 0 0,-1 6-628 0 0,-23-68-366 0 0,4-21-174 0 0,1-1-11 0 0,0 0-178 0 0,0 0-783 0 0,0 0-344 0 0,0 0-69 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93718.36">11474 6314 3224 0 0,'0'12'2345'0'0,"0"30"5493"0"0,-2 3-4114 0 0,0 47-712 0 0,6 10 343 0 0,-8-83-3334 0 0,2-11-891 0 0,-10 3-7476 0 0,6-9 8097 0 0,4-1-5157 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93135.977">11441 6585 456 0 0,'0'0'1763'0'0,"3"-14"5211"0"0,7-44-1110 0 0,14 41-1851 0 0,26-7-1678 0 0,-42 25-2203 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,3 6-132 0 0,21 37 1090 0 0,-25-40-1055 0 0,-2-2 0 0 0,0 2-1 0 0,1 1 1 0 0,-2-1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,-2-2-34 0 0,2 11-14 0 0,1-18-184 0 0,0-1-536 0 0,0 0-236 0 0,0 0-888 0 0,0 0-3561 0 0,0 0-1523 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-90762.018">11919 6615 8288 0 0,'-3'9'5575'0'0,"15"2"-3896"0"0,-11-11-1688 0 0,3 2 148 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,4-4-139 0 0,24-44 514 0 0,-21 26-481 0 0,-6 22-28 0 0,-2-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-3-4 0 0,1 5 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-63-9 0 0 0,60 9-6 0 0,-1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 1-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 2 1 0 0,-1-2 0 0 0,0 3 6 0 0,-1 0 50 0 0,0 0 1 0 0,2 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,2 0 1 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,2 0-1 0 0,0 1 1 0 0,0 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-2-1 0 0,0 2 1 0 0,1 0 0 0 0,2 6-51 0 0,-2-7 64 0 0,1-1 0 0 0,-1 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 1 0 0,2 1-1 0 0,-1 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,3 0-64 0 0,37 0-544 0 0,-24-10-5374 0 0,-5 1-1399 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88936.296">12466 6030 3224 0 0,'-3'16'4649'0'0,"-20"30"2676"0"0,3 37-3229 0 0,3 59-1931 0 0,18-126-1939 0 0,19 117 1016 0 0,14-34-627 0 0,-5-39 597 0 0,-26-58-1196 0 0,-2-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,2-1-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-3 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1-16 0 0,27-28 176 0 0,12-56-176 0 0,-15 3 0 0 0,-10-11 0 0 0,-5 15 0 0 0,-8-29 0 0 0,-3 6 43 0 0,0 101-266 0 0,0 1-29 0 0,0 0-4 0 0,0 0-141 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1251 0 0,0 0-4804 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87751.59">12989 6169 2304 0 0,'-4'14'3512'0'0,"4"-14"-3295"0"0,1 29 9139 0 0,9 17-4914 0 0,-8-36-4052 0 0,1-1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,0 2 1 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1-1 0 0 0,-2 6-389 0 0,0 28-162 0 0,2 43 39 0 0,6 31 299 0 0,-3-104 129 0 0,-2-1-2806 0 0,-1-12 1101 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87470.909">12996 6265 7832 0 0,'0'0'602'0'0,"1"1"-134"0"0,9 1 1838 0 0,32 7 3878 0 0,22-9-2721 0 0,12-8-2874 0 0,-43 7-6863 0 0,-25 1-248 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86426.787">13400 6422 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-128 0 0,1 2-606 0 0,9 93 6111 0 0,-10-23-5043 0 0,-3-7-2402 0 0,2-59 17 0 0,1-4-6835 0 0,0-2 4521 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86230.545">13727 6251 4144 0 0,'0'0'191'0'0,"-5"2"22"0"0,3 0 5833 0 0,-7 19 354 0 0,-8 11-4079 0 0,10 9-269 0 0,8-10-1028 0 0,-4-11-798 0 0,0 1 0 0 0,2-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,3 18-225 0 0,0 65 0 0 0,-10-38 0 0 0,5-55 13 0 0,1-3-3106 0 0,1-8 1973 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85578.149">13913 6472 3224 0 0,'0'15'553'0'0,"7"6"6334"0"0,-14 65 1088 0 0,2-10-6591 0 0,5-61-1121 0 0,0-2-3991 0 0,0-13-2374 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85386.832">13966 6320 17503 0 0,'0'0'776'0'0,"0"0"160"0"0,0 0-744 0 0,0 0-192 0 0,0 0 0 0 0,0 0 0 0 0,0 0 448 0 0,0 0 48 0 0,0 0 16 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1568 0 0,2 11-304 0 0,-2-11-64 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85026.437">13381 6225 18455 0 0,'0'0'408'0'0,"0"0"80"0"0,0 0 24 0 0,0 0 0 0 0,0 0-408 0 0,0 0-104 0 0,0 0 0 0 0,0 0 0 0 0,0 0 224 0 0,-7 0 16 0 0,7 0 8 0 0,0 0 0 0 0,0 0-992 0 0,0 0-200 0 0,0 0-40 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-83816.66">14285 6327 9584 0 0,'0'0'216'0'0,"-9"5"521"0"0,-49 33 3704 0 0,31-11-975 0 0,23-24-3254 0 0,-1 0 1 0 0,1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-1 1-1 0 0,1-2 1 0 0,-2 5-213 0 0,3-4 22 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,0-1 0 0 0,5 5-22 0 0,37 42 54 0 0,-20-34 918 0 0,-22-15-642 0 0,-2-1-115 0 0,8 3 109 0 0,0 9-171 0 0,-8-10-153 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,0 1 0 0 0,-2 1 0 0 0,0 0-4 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 5 0 0,-5-18-2397 0 0,9 8 122 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-79727.133">14503 6559 4632 0 0,'0'0'209'0'0,"1"-2"-5"0"0,32-59 6992 0 0,-32 61-6393 0 0,-1 0-31 0 0,21-7 2699 0 0,69 8 1055 0 0,-21-4-2917 0 0,-51 14-1448 0 0,-7 9-150 0 0,-12-20-7 0 0,1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 1 1 0 0,-1-1-4 0 0,-11-7 202 0 0,10 6-204 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 0 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1 1 0 0,-33 19 268 0 0,31-15-199 0 0,0 2-1 0 0,0-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,3 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,1 1-69 0 0,0-4 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,2 1 0 0 0,56-5-132 0 0,-53-2 154 0 0,-2-1 0 0 0,1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-1 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,3-3-22 0 0,44-59-80 0 0,-39 25 64 0 0,-5-3 16 0 0,1 162 0 0 0,-8-71 0 0 0,4 6 0 0 0,11 10 0 0 0,-4-4-2782 0 0,-7-45 64 0 0,-4 1-4789 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76952.167">15536 6625 2304 0 0,'0'0'464'0'0,"-1"1"2357"0"0,-5 6-1769 0 0,6-5 3151 0 0,0-1 4184 0 0,29 14-5739 0 0,-23-14-2588 0 0,0-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-2 0-1 0 0,4-3-59 0 0,4-6-111 0 0,-6 9 95 0 0,-1-2 0 0 0,1 1 0 0 0,-2 0 1 0 0,2-1-1 0 0,-2 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,0-2 16 0 0,-2 4-53 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-3-1 0 0 0,2 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-3-2 54 0 0,4 4-6 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 2 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-2 1 0 0 0,2 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-2 0 7 0 0,-3 7 93 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,0-1 0 0 0,1 2 0 0 0,0 0 0 0 0,1-2 0 0 0,-1 2 0 0 0,2 0 0 0 0,0-1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 2 0 0 0,1-1 0 0 0,5 11-93 0 0,-7-19 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,4 0 0 0 0,-3-1-22 0 0,11-6-6424 0 0,-11-2-869 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77950.243">15132 6159 1840 0 0,'0'0'307'0'0,"0"-2"615"0"0,-2-29 3370 0 0,2 31-4103 0 0,0 0-1 0 0,0 0 44 0 0,0 0 22 0 0,0 0 2 0 0,0 0 74 0 0,0 0 316 0 0,0 0 142 0 0,0 1 32 0 0,7 61 3244 0 0,-7 73 861 0 0,0 69-1667 0 0,4-81-1971 0 0,6 62-363 0 0,-9-143-963 0 0,-2-24-3502 0 0,1-18 1678 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77348.9">15125 6303 13504 0 0,'0'0'620'0'0,"0"0"-16"0"0,5-6-364 0 0,17-4 1491 0 0,-17 7-1438 0 0,-1 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,-1 1-293 0 0,85 5 662 0 0,-44 8-2436 0 0,-20-7-4491 0 0,-15 0 465 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76210.45">16117 6370 1840 0 0,'0'0'583'0'0,"-2"1"2720"0"0,-5 1-1116 0 0,-26 23 7260 0 0,28-17-9058 0 0,2 1 1 0 0,0-2-1 0 0,-1 2 0 0 0,1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,2 1 0 0 0,0 0 0 0 0,0 9-389 0 0,-4 48 2048 0 0,13 42-1440 0 0,-7-101-566 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,1 2-42 0 0,-3-6 48 0 0,-1-1 1 0 0,-1-1-1 0 0,1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2-1 0 0 0,2 0-48 0 0,8-6 0 0 0,-2 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,3-9 0 0 0,22-45 0 0 0,-2-10 0 0 0,-26 53 0 0 0,-4 15 0 0 0,-7 1-177 0 0,-8 13-4614 0 0,9-6-2832 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-72325.515">16603 6356 3224 0 0,'0'0'143'0'0,"0"0"-3"0"0,6 0 2973 0 0,-5-1 7737 0 0,-5 4-3072 0 0,3 3-10123 0 0,2 28 3033 0 0,-2-8 1192 0 0,1-25-1368 0 0,0 1 0 0 0,-17 76 715 0 0,7-14-1010 0 0,4-12-308 0 0,24 74-94 0 0,-14-90 185 0 0,-7-30-139 0 0,3-5-580 0 0,0-1-251 0 0,0-1-1544 0 0,3-8-6015 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45518.415">18391 6397 8288 0 0,'0'134'4740'0'0,"0"-117"-3699"0"0,0 12 42 0 0,0 2 0 0 0,1 0 0 0 0,3-2 1 0 0,0 2-1 0 0,7 20-1083 0 0,3-10-70 0 0,-7-27-1026 0 0,-5-13-85 0 0,-2-1-45 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45023.887">18787 6373 1376 0 0,'0'0'299'0'0,"0"0"715"0"0,0 0 313 0 0,0 0 66 0 0,-11-7 1242 0 0,7 6-2367 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2-1 1 0 0,0 2-1 0 0,-2 1-268 0 0,-49 87 3206 0 0,51-84-3121 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,0-1-1 0 0,0 1 1 0 0,2 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,2-2 0 0 0,-1 2 0 0 0,1-2-1 0 0,0 1 1 0 0,1 1-85 0 0,76 37 528 0 0,-80-43-518 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1-9 0 0,-1 2-25 0 0,0-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2-1 25 0 0,-9-14-3267 0 0,9 7-3203 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22924.697">16603 6555 920 0 0,'-5'10'80'0'0,"-5"6"5114"0"0,9-15-3500 0 0,1-1-770 0 0,0 0-336 0 0,0 0-68 0 0,0 0-20 0 0,0 0-51 0 0,0 0-22 0 0,0 0-3 0 0,0 0 25 0 0,0 0 107 0 0,0 0 48 0 0,0 0 11 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,7-21 5642 0 0,29-28-4223 0 0,12 16-1739 0 0,-43 32-286 0 0,3 2 1 0 0,4 10 96 0 0,-8-5-97 0 0,-4-5-115 0 0,2 0 1 0 0,-1 1-1 0 0,-1-1 0 0 0,1-1 0 0 0,0 2 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 105 0 0,10 2-1084 0 0,15-1-5055 0 0,-21-1 4517 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23746.448">17153 6271 1376 0 0,'0'0'331'0'0,"0"0"853"0"0,0 0 380 0 0,0 0 71 0 0,0 0-79 0 0,0 0-405 0 0,0 0-178 0 0,0 0-39 0 0,0 0-42 0 0,0 0-151 0 0,0 0-65 0 0,0 0-17 0 0,0 0 26 0 0,0 0 124 0 0,0 0 58 0 0,0 0 11 0 0,0 0-43 0 0,0 0-192 0 0,0 0-89 0 0,-16-3 1062 0 0,-29 16 904 0 0,-11 37-429 0 0,6 32-1643 0 0,27-36-267 0 0,5 48 275 0 0,14 17 391 0 0,10-78-660 0 0,-6-25-158 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,4 1-29 0 0,23 24 0 0 0,-21-27-4 0 0,-7-4-118 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,0 0 0 0 0,2-1-1 0 0,-2 0 1 0 0,0 1 0 0 0,1-2 122 0 0,26-17-6775 0 0,-23 11 184 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24081.144">17259 6442 456 0 0,'13'-35'1833'0'0,"7"16"8000"0"0,-6 2-4338 0 0,-13 16-4746 0 0,-1 1-12 0 0,9 1 2655 0 0,-4 4-3184 0 0,-2-1 0 0 0,2 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,-1 1 0 0 0,2 1-1 0 0,-2-1 1 0 0,0 1 0 0 0,0-2-1 0 0,1 2 1 0 0,-2 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 5-208 0 0,0-4 187 0 0,1 165 1174 0 0,-9-100-1017 0 0,-6-5-212 0 0,10-60-136 0 0,3-2 10 0 0,-1 1 0 0 0,1-2 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-2 1-5 0 0,-8 5-315 0 0,-30 22-6531 0 0,32-25 5010 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28120.561">17401 5865 4608 0 0,'3'-4'886'0'0,"1"-3"-1808"0"0,-3 2 5374 0 0,-1-3 4827 0 0,17 9-6424 0 0,-9 3-2408 0 0,-2 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-2 0 0 0 0,2 0 1 0 0,-1-1-1 0 0,-1 2 0 0 0,0-1 1 0 0,-1 1-1 0 0,3 3-447 0 0,11 26 1006 0 0,16 70 508 0 0,-23-23-882 0 0,4 232 416 0 0,-15-49-535 0 0,-11-43 14 0 0,-4 6-74 0 0,0-139-389 0 0,1-23 75 0 0,13-62-128 0 0,-21-1 223 0 0,-115-32-95 0 0,92 25-75 0 0,-7 7 28 0 0,-1-2 1 0 0,1-2-1 0 0,-22-4-92 0 0,-41-13 67 0 0,-164-68-67 0 0,246 78-114 0 0,-1 2 1 0 0,2 1-1 0 0,-2 2 0 0 0,0 1 0 0 0,1 2 1 0 0,-1 1-1 0 0,-15 4 114 0 0,-568 83 796 0 0,89-33-796 0 0,14 1 0 0 0,213-18 0 0 0,-12-8 0 0 0,-213-12 0 0 0,-406-17 0 0 0,604 6 0 0 0,-286-32 0 0 0,-71-18 0 0 0,157 25-457 0 0,-219-3 202 0 0,265-3-1 0 0,-150 18 256 0 0,320 4 172 0 0,-73 0 164 0 0,30-15-196 0 0,65 16 180 0 0,87 1-722 0 0,-30 1 8 0 0,-195-5 478 0 0,146-5 308 0 0,26-8-72 0 0,-251-16-1032 0 0,329 18 852 0 0,-73-9 432 0 0,-137-6-572 0 0,173 13 0 0 0,-39 19 0 0 0,-57-8 0 0 0,81-4 0 0 0,-88 33 0 0 0,23 12 0 0 0,124-47 0 0 0,16 18 0 0 0,55 0 0 0 0,96-6-20 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-2-1-1 0 0,2 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,2-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,2-1 20 0 0,-30-45-115 0 0,-8-62 687 0 0,-15-88-572 0 0,-19-88 0 0 0,48 48 0 0 0,-4 76 0 0 0,-3-19 0 0 0,22 72-796 0 0,10 23 1592 0 0,13 19-796 0 0,29-25 0 0 0,-36 82 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,1 0 0 0 0,8-7 0 0 0,73-37 0 0 0,82-24 0 0 0,-145 67 0 0 0,0 1 0 0 0,0 1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1 2 0 0 0,0 1 0 0 0,10 1 0 0 0,-37 1 0 0 0,125 0 0 0 0,0-4 0 0 0,29-9 0 0 0,23-14-712 0 0,88-19 1413 0 0,-160 30-697 0 0,0 5-1 0 0,1 5 1 0 0,64 5-4 0 0,284 18 0 0 0,-116-1 0 0 0,-271-12-72 0 0,2 2 1 0 0,-1 3-1 0 0,48 14 72 0 0,81 8-105 0 0,-66-21 425 0 0,59 12-320 0 0,-50 3 0 0 0,65 14 0 0 0,76 3 0 0 0,54 21 0 0 0,-179-26 0 0 0,53-2 0 0 0,44 3-796 0 0,-88-5 1592 0 0,3-10-831 0 0,9-27-250 0 0,-32 4 605 0 0,57 10-320 0 0,-95-7 0 0 0,86-19 0 0 0,-39-3 0 0 0,135 14 0 0 0,-189 5 0 0 0,-1-5 0 0 0,69-11 0 0 0,52-6 0 0 0,133 6 0 0 0,-39-6 0 0 0,-144 5 0 0 0,223 0 0 0 0,-102 15 0 0 0,104-19 0 0 0,83-11 0 0 0,-325 25 0 0 0,16-1 0 0 0,255 3 0 0 0,-138 15 0 0 0,-57-3 0 0 0,117-21 0 0 0,10 21 0 0 0,-209 0 0 0 0,7-11 0 0 0,-14-3 0 0 0,-16 7 0 0 0,10 4 0 0 0,31-11 0 0 0,57 14 0 0 0,-72 7 0 0 0,-80-16 0 0 0,165-4 0 0 0,-65 21 0 0 0,-84-5 0 0 0,49-2 0 0 0,-44 2 0 0 0,149 13 0 0 0,-59-8 0 0 0,-69-1 0 0 0,65 3 0 0 0,-77-15 0 0 0,35-5 0 0 0,-38 26-4336 0 0,-37-5-1782 0 0,-43-14-3483 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29020.976">17040 5625 1376 0 0,'0'0'591'0'0,"0"0"1942"0"0,0 0 851 0 0,0 0 174 0 0,0 0-327 0 0,-12 8 6223 0 0,15-5-9289 0 0,2 1 0 0 0,-2-2 0 0 0,0 1 0 0 0,2 0-1 0 0,-2-1 1 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,1-1 1 0 0,0-1-165 0 0,1 2 87 0 0,109 16 1139 0 0,-6 21-943 0 0,-61-22-166 0 0,6-26 11 0 0,-20 8-64 0 0,-17 18-64 0 0,-10 16 13 0 0,-7 5 198 0 0,-2 57 157 0 0,4-6-616 0 0,-1-30-3854 0 0,1-34-5107 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-134780.189">8866 7445 1376 0 0,'0'0'65'0'0,"0"0"189"0"0,0 0 767 0 0,0 0 335 0 0,0 0 69 0 0,0 0-94 0 0,0 8 1469 0 0,-2 70 3116 0 0,4-15-3609 0 0,-15 100-383 0 0,12-28-438 0 0,1-59-917 0 0,-3 0 598 0 0,2 102-205 0 0,-7 4-322 0 0,13 94-40 0 0,-2-180-336 0 0,-3 19 8 0 0,10 116 323 0 0,6-5 583 0 0,-4-60-1855 0 0,-6 84 952 0 0,0-53-94 0 0,-5-139-117 0 0,5-4-2277 0 0,-3-76-5567 0 0,-3 8 286 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-134240.189">8332 9545 5528 0 0,'0'0'422'0'0,"0"0"-88"0"0,0 0 656 0 0,0 16 2881 0 0,11 37-2527 0 0,8 40 2164 0 0,23-10-466 0 0,77 125 109 0 0,-79-145-2761 0 0,-30-44-296 0 0,1 0 0 0 0,2-1 1 0 0,-1 0-1 0 0,2 0 1 0 0,0-1-1 0 0,2-2 1 0 0,0 1-1 0 0,13 10-94 0 0,64 22 544 0 0,-89-45-475 0 0,2-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 1 0 0,0 0-1 0 0,-2 0 0 0 0,2-1 0 0 0,3-2-69 0 0,31-38 176 0 0,92-231 1624 0 0,-38 85-1872 0 0,-47 71-576 0 0,-27 65-2737 0 0,-12 38 1634 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-125200.19">3442 10359 13128 0 0,'0'-16'633'0'0,"0"15"-277"0"0,0 8 83 0 0,14 215 3164 0 0,20-12-1187 0 0,-8-1-1552 0 0,-28-122-897 0 0,-15-31-3046 0 0,14-47 1239 0 0,-5-5-71 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-124660.19">3358 10347 7056 0 0,'-2'-5'116'0'0,"1"0"0"0"0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,2-4-117 0 0,1-6 1073 0 0,-3 12-878 0 0,1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,0 2 1 0 0,-1-2 0 0 0,2 1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0-1 0 0,-2 1 1 0 0,4-1-195 0 0,-2 1 85 0 0,1 1 1 0 0,0 0-1 0 0,-2 0 0 0 0,2 0 0 0 0,-2 1 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,3 3-85 0 0,47 46 670 0 0,-25-19 265 0 0,23 36 175 0 0,-47-56-1010 0 0,-2 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-2-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-2 0 1 0 0,0 1-1 0 0,-2 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,-2 0 0 0 0,1 1 1 0 0,-2-2-1 0 0,-3 8-100 0 0,3-10 186 0 0,-1-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-2-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1-1-1 0 0,0 1 1 0 0,-3 0-186 0 0,7-5 12 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0-1-11 0 0,-43 6 164 0 0,48-5-225 0 0,18 13-71 0 0,38 30 57 0 0,-32-19 68 0 0,58 76 132 0 0,0 44-125 0 0,-41-67-5360 0 0,-35-58 3443 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123330.19">4190 11009 6912 0 0,'0'0'528'0'0,"0"0"-219"0"0,0 0 347 0 0,0 1 192 0 0,13 10 3088 0 0,49-14-2645 0 0,22-32-467 0 0,-31 6 415 0 0,-50 26-1110 0 0,-1 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1-128 0 0,-29-38 870 0 0,24 40-830 0 0,1 0 1 0 0,-1 0 0 0 0,-1 0-1 0 0,2 1 1 0 0,-2 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 2 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,2 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,2 1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-2 1 0 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,2 1-1 0 0,-1-2 1 0 0,-2 5-41 0 0,1 0 30 0 0,2 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1-30 0 0,20 102 84 0 0,-18-104-98 0 0,2-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,2-2 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0-1 0 0,-2 0 1 0 0,2-1 0 0 0,0 0 0 0 0,1 0 14 0 0,8 0-1085 0 0,-1-1-349 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122830.19">4767 10632 920 0 0,'1'2'67'0'0,"6"15"218"0"0,-7-15 1126 0 0,0-2 485 0 0,0 0 95 0 0,0 0-144 0 0,0 0-698 0 0,0 0-306 0 0,3 14 5156 0 0,5 68-3006 0 0,-1 139-2907 0 0,17-65 348 0 0,-10-95-1540 0 0,-9-54-81 0 0,-2-4-3107 0 0,-3-2-1448 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122530.19">4767 10714 5984 0 0,'0'0'464'0'0,"0"0"-82"0"0,11 12 5502 0 0,39-2-3006 0 0,32-10-1919 0 0,-26-4-2545 0 0,-43 4-3811 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2419.811">8287 10596 1840 0 0,'0'0'83'0'0,"0"7"10"0"0,-4-2 194 0 0,-4 6 6325 0 0,0 2-4677 0 0,5-7-1065 0 0,-4 25 3503 0 0,10 48-1185 0 0,1 46-2006 0 0,1-55-326 0 0,4-41-586 0 0,22 42 628 0 0,-29-69-870 0 0,2 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 0 1 0 0,1 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,2-1-28 0 0,5-5 21 0 0,-1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,0-2-1 0 0,0 1 0 0 0,3-8-21 0 0,23-41 0 0 0,-9-13 1099 0 0,1-23-934 0 0,-18 6-165 0 0,-2 60 0 0 0,-8-37 0 0 0,3 21-283 0 0,2 27-8605 0 0,-1 18 2172 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3219.811">8871 10537 8288 0 0,'-10'67'3321'0'0,"8"22"1356"0"0,4-7-2700 0 0,0-29-1241 0 0,1 128 440 0 0,-3-166-966 0 0,8 42-294 0 0,-7-56-163 0 0,-1-1-857 0 0,0-2-3536 0 0,0-5-1518 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3409.81">8853 10632 8288 0 0,'0'0'638'0'0,"8"-3"2018"0"0,19-2 1429 0 0,17 15-2828 0 0,-27-5-864 0 0,32 22-411 0 0,-42-22-355 0 0,15 19-3587 0 0,-13-14 2594 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3629.811">9261 10842 3680 0 0,'0'0'284'0'0,"3"8"797"0"0,-1-5 4784 0 0,0 30-1677 0 0,0 5-3145 0 0,-3 36-251 0 0,5-14-1216 0 0,-4-45-1299 0 0,0-6-3631 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4049.811">9560 10632 920 0 0,'-4'-13'343'0'0,"4"10"1102"0"0,0 3 482 0 0,0 0 96 0 0,0 0-124 0 0,0 0-614 0 0,0 0-269 0 0,0 0-50 0 0,0 0-57 0 0,0 0-212 0 0,0 0-90 0 0,0 2-20 0 0,-1 34 1508 0 0,-5 36-993 0 0,-6 80 402 0 0,8-54-494 0 0,12 54-140 0 0,3-72-1121 0 0,-11-79-772 0 0,0-1-333 0 0,0 0-68 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4549.811">9862 10933 456 0 0,'-6'20'0'0'0,"6"-19"651"0"0,-2 0 4741 0 0,-1 1 3820 0 0,3 2-9813 0 0,2 167 4824 0 0,3-121-4491 0 0,-5-45-754 0 0,0-4-326 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5199.81">10200 10907 10136 0 0,'0'0'464'0'0,"-2"0"-10"0"0,-5 0-222 0 0,-12 14 3123 0 0,17-13-3266 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1-89 0 0,25 49-256 0 0,-16-28 538 0 0,38 27 412 0 0,-14 3-275 0 0,-30-19-94 0 0,-20 4 1227 0 0,4-23-785 0 0,-15 4 957 0 0,14-17-1575 0 0,-9-2-133 0 0,-5-16-2201 0 0,23 10-250 0 0,3 4-4568 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6589.811">10483 11149 10136 0 0,'7'15'230'0'0,"-6"-11"30"0"0,-1-4 19 0 0,3-7 478 0 0,4-33 763 0 0,-5 38-1014 0 0,-1-1-2 0 0,8-25 334 0 0,-8 22-761 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,3 0-78 0 0,-5 4 167 0 0,29-15 1024 0 0,-28 15-1129 0 0,1 1 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-2 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2-1-1 0 0,1 1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0-61 0 0,27 30 1857 0 0,-28-31-1723 0 0,-1-1-46 0 0,0 0-22 0 0,0 0-2 0 0,0 0 2 0 0,0 0 4 0 0,-24 0 2 0 0,20 0-87 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,2-1 1 0 0,0 1-1 0 0,-3 1 16 0 0,-25 15-85 0 0,29-18 77 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-2 0 0 0,-2 2 0 0 0,2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,0 2 8 0 0,12 29-54 0 0,-12-31 57 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,2 1 0 0 0,-2-2 0 0 0,1 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-3 0 0,50 5 163 0 0,-45-9-205 0 0,-1 0-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-2 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,-1-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 2-1 0 0,-2-5 43 0 0,7-67-556 0 0,-7 77 622 0 0,0 1 34 0 0,0 0 10 0 0,-1 3-16 0 0,0 11 66 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,2 0-1 0 0,-1-1 0 0 0,3 11-160 0 0,2 24 76 0 0,16 26 0 0 0,-13-36-1057 0 0,-9-36-90 0 0,6 7-37 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7129.81">11097 10732 456 0 0,'0'-22'204'0'0,"0"10"5674"0"0,-3 12 1245 0 0,-6 24-4666 0 0,-2 52-110 0 0,11 93-830 0 0,-4 69-628 0 0,14-179-907 0 0,-9-53 2 0 0,-1-6-2564 0 0,0 0 1298 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7369.81">11059 10874 8752 0 0,'5'8'936'0'0,"13"-23"1798"0"0,43 15 2614 0 0,35 4-4455 0 0,-54 12-4124 0 0,-34-12 2047 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7929.811">11501 11216 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,2 1-40 0 0,41-7 2129 0 0,-18-1-968 0 0,-22 6-1318 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2 0-1 0 0,-2 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1-82 0 0,7-9 268 0 0,-5 10-243 0 0,-2-2 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 2 1 0 0,-1-2 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-4-3-25 0 0,6 5 20 0 0,-2 1 0 0 0,2-2-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,0 2-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0-1-20 0 0,-6 11 226 0 0,1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-2 0 0 0,1 1-1 0 0,1 1 1 0 0,0 1 0 0 0,1-2 0 0 0,0 2-1 0 0,1 3-225 0 0,-1-12 37 0 0,2 2 31 0 0,0-1-1 0 0,0 1 0 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 0 1 0 0,0-1-1 0 0,-1 2 0 0 0,2-1 1 0 0,-1 0-1 0 0,2 0-67 0 0,-2-2 33 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,3 0-33 0 0,45 7-313 0 0,-12-14-1742 0 0,-31 5 191 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8439.811">11998 11004 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,-11 3 2224 0 0,1 8-1481 0 0,8-9-561 0 0,2-2 0 0 0,-1 1 0 0 0,-33 38 1128 0 0,32-37-1631 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-9 0 0,0 19 74 0 0,-1-17-14 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,2 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1-1 0 0,2 1-59 0 0,61 32 164 0 0,-61-35-163 0 0,-2-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,2 0 1 0 0,-2-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2-1-1 0 0,1-1 0 0 0,27-38 0 0 0,-1-26 0 0 0,-23 38 0 0 0,-6-42 0 0 0,0 63 0 0 0,0 10-1 0 0,0 0 0 0 0,0-1 0 0 0,-2 1-1 0 0,2 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 2 0 0,-2 2-86 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,2 5 86 0 0,10 43-6882 0 0,-5-42 1085 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8909.811">12600 10864 3224 0 0,'4'17'240'0'0,"-19"12"5162"0"0,-8 22 1702 0 0,3 32-4883 0 0,10-45-1389 0 0,6 23 96 0 0,-2-23-476 0 0,6 22 178 0 0,-5 6-648 0 0,2-55 50 0 0,-1-6-3037 0 0,4-5 1818 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9219.811">12544 11082 10136 0 0,'2'9'1085'0'0,"48"-43"1390"0"0,-47 31-2239 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,2 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1 0 0 0 0,3-1-236 0 0,31-14 608 0 0,-11 30 520 0 0,-10 4-434 0 0,-15-17-580 0 0,16 13-10 0 0,-18-11-96 0 0,14 20-8 0 0,-14-18-92 0 0,-1-3-390 0 0,0 7-1954 0 0,3-1-3569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12429.81">13188 10743 2304 0 0,'0'0'101'0'0,"1"-2"1"0"0,1-4-3003 0 0,-1 1 4359 0 0,-6-3 14711 0 0,-4 14-13468 0 0,5-3-2385 0 0,1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,3 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,1 5-316 0 0,-1 96 1202 0 0,2-94-965 0 0,3 39-228 0 0,2 1 0 0 0,1-1 1 0 0,3-1-1 0 0,3 1 0 0 0,8 19-9 0 0,-11-39 0 0 0,-2-20 0 0 0,19 1-1058 0 0,12-29-4850 0 0,-27 9 3794 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12789.811">13558 10655 1376 0 0,'0'0'65'0'0,"0"0"454"0"0,0 0 1882 0 0,5 0 5023 0 0,4 0-3511 0 0,-6 2-3615 0 0,0-1-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,2 3-297 0 0,28 49 2384 0 0,-5-9-1738 0 0,-16-32-400 0 0,-1 2 0 0 0,0 1-1 0 0,-2-2 1 0 0,1 2 0 0 0,-2 1-1 0 0,-1 0-245 0 0,16 115 608 0 0,-17 65 104 0 0,-12-62-61 0 0,0-90-3304 0 0,-3-4-3362 0 0,8-31-807 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16819.81">14206 12060 3224 0 0,'0'0'143'0'0,"0"0"327"0"0,0 0 1271 0 0,0 0 550 0 0,0 0 114 0 0,0-3 988 0 0,1-10-1052 0 0,0-53 2752 0 0,8-2-2899 0 0,10-94-927 0 0,5-50-315 0 0,-9 75 489 0 0,-5-100-1441 0 0,-8 148 170 0 0,2 8 86 0 0,3-1-1 0 0,8-35-255 0 0,6-24 592 0 0,-7 23-253 0 0,-10 22 96 0 0,5 46-99 0 0,4-12-403 0 0,0 34 67 0 0,-7 12 13 0 0,-2-1 79 0 0,-8 7 139 0 0,-6-9-231 0 0,9 17 5 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1-5 0 0,-127 3 320 0 0,66 1-256 0 0,-64 5 61 0 0,-249 11 207 0 0,46 3-320 0 0,14 14 52 0 0,28 16-64 0 0,-287 56 128 0 0,368-86-117 0 0,82-14 98 0 0,-2-4 0 0 0,-35-7-109 0 0,21 0-2 0 0,-78-4 367 0 0,-91 1-133 0 0,-27-6-541 0 0,107-3 706 0 0,-14 0-710 0 0,58 5 634 0 0,-193-1-321 0 0,208-3-16 0 0,-39 1-155 0 0,-39-9 182 0 0,-116-12 65 0 0,213 22-88 0 0,-26 5 12 0 0,-51 3 64 0 0,19 0-64 0 0,-58-7 0 0 0,-328-30 64 0 0,408 26-64 0 0,-291-9 0 0 0,420 24 0 0 0,-156-10 0 0 0,75-5 0 0 0,-43-6 0 0 0,-25-1 0 0 0,-109 16 0 0 0,212 7 0 0 0,-54-15 0 0 0,31-5 0 0 0,90 14 0 0 0,0 1 0 0 0,-2 2 0 0 0,-35 4 0 0 0,-12 0 0 0 0,-248 7-11 0 0,124-34 22 0 0,-92-18-11 0 0,-50 38-64 0 0,269-5 128 0 0,57 8-64 0 0,0 0 0 0 0,1-2 0 0 0,-1-1 0 0 0,-24-7 0 0 0,33 6 0 0 0,6 0 0 0 0,0 2 0 0 0,-1-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,1 2 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1 0 0 0,-4 1 0 0 0,5 1 0 0 0,8-3 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-2 2 0 0 0,-15 70-244 0 0,45 138 168 0 0,-3-61 299 0 0,33 223-446 0 0,-6-28 520 0 0,1-173-530 0 0,-24-84 233 0 0,20 50 0 0 0,12-7 0 0 0,-47-115 0 0 0,59 74 0 0 0,-53-79 4 0 0,0-1 0 0 0,1-2 0 0 0,0 0 0 0 0,2-1-1 0 0,-1-2 1 0 0,0 1 0 0 0,0-3 0 0 0,2 1 0 0 0,5 0-4 0 0,29 11 140 0 0,88 14-242 0 0,-16-9 207 0 0,98 3-105 0 0,-87-10-23 0 0,80 2-132 0 0,6-8 155 0 0,503 21 0 0 0,-143-9 0 0 0,-62 2 0 0 0,86-19 53 0 0,-70-39-42 0 0,-161-16-11 0 0,48 10 0 0 0,-185 25 12 0 0,-11 10 112 0 0,98-8-204 0 0,51 20 149 0 0,16-8-58 0 0,-5-10-107 0 0,11 1 96 0 0,-177 3 96 0 0,113 12-192 0 0,-236 14 96 0 0,45-2 0 0 0,36-1 144 0 0,-55-18-240 0 0,4-2 192 0 0,-90 6-96 0 0,-1-1 0 0 0,2-3 0 0 0,-2-1 0 0 0,35-7 0 0 0,28-4-96 0 0,35 7 96 0 0,111 3 0 0 0,-122-9 80 0 0,-36 4-160 0 0,102-7 80 0 0,-80 19 11 0 0,90-17 42 0 0,-96-3-141 0 0,-17-6 94 0 0,1 2 0 0 0,63-4-6 0 0,-43 12 60 0 0,0 12-60 0 0,42 35 0 0 0,-53-17 0 0 0,-88-15 0 0 0,21 12 0 0 0,-27-7 59 0 0,-4-6-111 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 52 0 0,-5 4-1004 0 0,5-4-3898 0 0,1-1 2712 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25749.81">17857 6149 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0-10 1147 0 0,0 6-3619 0 0,1-4 9257 0 0,0 5 2091 0 0,-1 8-7632 0 0,13 187 1589 0 0,-17-100-2526 0 0,-5-7-90 0 0,3-5-182 0 0,16 6-118 0 0,-2-40-2244 0 0,-7-45 1548 0 0,-1-1-185 0 0,0 0-84 0 0,0 0-21 0 0,3 3-3895 0 0,-3-3 2635 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26679.81">17883 6566 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0 0-22 0 0,0-14 2511 0 0,15-69 5565 0 0,-3 58-6834 0 0,10 1-281 0 0,-5 8-550 0 0,-16 15-517 0 0,-1 1-6 0 0,3 0 3 0 0,21 7 472 0 0,-1 12 14 0 0,11 52 396 0 0,7 61-438 0 0,-29-81-450 0 0,-12-25-1627 0 0,0-12-6318 0 0,0-4 1470 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37589.811">14948 10926 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,4-8 1867 0 0,-3 7-1852 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-240 0 0,-5-2 274 0 0,-1-1-1 0 0,1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-2 0 0 0 0,1 0-1 0 0,-3 2-273 0 0,-9 5 0 0 0,12-1 0 0 0,-28 32 0 0 0,26-23 150 0 0,0 0 1 0 0,1 2-1 0 0,0-2 0 0 0,1 2 0 0 0,1 0 0 0 0,0 1 0 0 0,2-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 1 0 0,2-1-1 0 0,1 2 0 0 0,0 4-150 0 0,-1-1 104 0 0,-16 200-482 0 0,10-116 567 0 0,9-12-136 0 0,-1-93-229 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0 176 0 0,8-3-1901 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37999.811">14605 11225 5984 0 0,'0'0'464'0'0,"0"0"-100"0"0,0 0 717 0 0,0 0 346 0 0,0 0 69 0 0,0 0-71 0 0,0 0-330 0 0,0 0-146 0 0,7 12 1624 0 0,-3-8-2296 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1-1-1 0 0,1 1 1 0 0,1-1 0 0 0,-2 1 0 0 0,5-1-277 0 0,16 8 296 0 0,20 1 73 0 0,-37-7-712 0 0,21 10-175 0 0,-13 4-5552 0 0,-9-4-166 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38309.811">14918 11562 6624 0 0,'0'0'298'0'0,"0"0"-3"0"0,0-2-188 0 0,27-52 3721 0 0,-19 41-2931 0 0,-7 11-725 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 1 0 0,1-1-173 0 0,0 2 83 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 1 1 0 0,-1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 1-83 0 0,4 3 241 0 0,0 1 0 0 0,-2 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 6-241 0 0,-5 51 1376 0 0,-3-48-782 0 0,7-16-550 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1-44 0 0,-2-2-23 0 0,-1 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,2-1-1 0 0,-2 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,2 1 0 0 0,-1-1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0-2 24 0 0,-12-40-1750 0 0,9 20 132 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39549.811">15355 11538 4608 0 0,'0'0'101'0'0,"-3"-4"150"0"0,2-1-50 0 0,1 4 308 0 0,0 1 135 0 0,0-1 27 0 0,-2-36 1126 0 0,2 36-1534 0 0,0 1-330 0 0,0 0-71 0 0,0 0 38 0 0,0 0 152 0 0,0 0 68 0 0,0 0 9 0 0,0 1-17 0 0,2 1-16 0 0,-2-1 280 0 0,0-1 113 0 0,0 0 21 0 0,0 0-68 0 0,0 0-262 0 0,0 0-9 0 0,-1 6 712 0 0,0-6-575 0 0,1 0 4 0 0,0 0 26 0 0,0 0 113 0 0,0 0 49 0 0,0 0 11 0 0,0 0-57 0 0,0 0-239 0 0,0 0-102 0 0,0 0-17 0 0,0 0 18 0 0,0 0 99 0 0,0 0 47 0 0,0 0 11 0 0,0 0 0 0 0,0 0 1 0 0,0 0 0 0 0,2 7 268 0 0,10 24 656 0 0,-8 18 132 0 0,9 16 242 0 0,-7-33 28 0 0,-6 35-1582 0 0,-5-24-16 0 0,5-33 0 0 0,1-83 1117 0 0,-2 33-1650 0 0,6-48 37 0 0,-9-1 27 0 0,16 59 834 0 0,-9 23-365 0 0,25-6-1090 0 0,-27 13 1590 0 0,0 1-59 0 0,55 45-276 0 0,-22-3-165 0 0,-12 0 0 0 0,2 9 0 0 0,-14-10 0 0 0,-9-24 72 0 0,6 4-112 0 0,-7-20-81 0 0,0-2-30 0 0,13 5-660 0 0,11-3-2647 0 0,-19-9 2023 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41569.811">15867 11499 6448 0 0,'31'-48'4184'0'0,"-30"47"-3679"0"0,-1 1 6 0 0,0 0 1 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 0 0 0,0 0-24 0 0,0 0-100 0 0,0 0-42 0 0,0 0-8 0 0,0 0-20 0 0,0 0-74 0 0,0 0-39 0 0,0 0-5 0 0,0 0 26 0 0,0 0 104 0 0,0 0 44 0 0,0 0 8 0 0,0 0-31 0 0,13 2 130 0 0,-13-1-345 0 0,-19 8 299 0 0,-3 4-94 0 0,-34 31 589 0 0,18-11 20 0 0,23 12-70 0 0,15-43-729 0 0,0 0-40 0 0,-1 13 5 0 0,1-12-81 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,3-1-27 0 0,-1 2 24 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,4 0-23 0 0,28 6-16 0 0,2-12-321 0 0,0-16-1384 0 0,-19 18-2498 0 0,-8-2-2527 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42539.811">16247 11221 456 0 0,'0'0'1877'0'0,"0"0"225"0"0,0 0 96 0 0,0 0-174 0 0,0 0-800 0 0,0 0-352 0 0,0 2-68 0 0,-3 78 5406 0 0,0-8-3788 0 0,-5 6-533 0 0,0 106-938 0 0,9-89-994 0 0,-1-92-228 0 0,2 8 239 0 0,-1-4-2836 0 0,-1-12 836 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42759.811">16191 11355 10592 0 0,'0'0'818'0'0,"0"0"-382"0"0,0 0 375 0 0,2 0 224 0 0,52 12 3870 0 0,-12 3-4655 0 0,-17-8-2639 0 0,-24-6 1115 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="43219.811">16511 11548 920 0 0,'0'-6'1780'0'0,"-8"-29"5181"0"0,8 34-6117 0 0,0 1-63 0 0,4-5 1525 0 0,-2 2 782 0 0,7 22-961 0 0,-17 39 414 0 0,-1-12-2418 0 0,16-5-123 0 0,8 30-266 0 0,-15-69-1124 0 0,0-2-490 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="43559.811">16764 11579 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,-7-14-276 0 0,7 10-201 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 3 0 0 0,1-3 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0-59 0 0,-2 1 59 0 0,-1 1 0 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-61 0 0,14 46 1489 0 0,-15-38-1068 0 0,1 1-1 0 0,-1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,-1 0-420 0 0,2-10 47 0 0,-19 55 2134 0 0,-26 17-2086 0 0,45-72-50 0 0,-2 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-2-2-46 0 0,-36-47 76 0 0,20 3-2636 0 0,12 12-3921 0 0,2 11-600 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51949.811">17122 11365 2760 0 0,'3'6'3463'0'0,"-2"-2"5440"0"0,-10 22-3399 0 0,9 21-2728 0 0,-2 11-1732 0 0,-7 23 73 0 0,11 40-1117 0 0,1-94-2100 0 0,-3-29 527 0 0,4-4-370 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="52379.811">17111 11559 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0 0 240 0 0,0-8 1066 0 0,15-30 2918 0 0,33 1-1475 0 0,-31 30-2427 0 0,24-3-98 0 0,-32 12-954 0 0,45 18 0 0 0,15 46 242 0 0,-31 31 636 0 0,-28-60-878 0 0,-6-21 0 0 0,-8 8-49 0 0,4-23-207 0 0,0-1-87 0 0,0 0-917 0 0,0 0-3813 0 0,0 0-1633 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54319.811">17773 11086 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,0 17 1877 0 0,8 79 4244 0 0,-6-24-3972 0 0,-7 44-624 0 0,0-23-1860 0 0,4 85 1890 0 0,2-6-1730 0 0,3-159-88 0 0,-1 3-289 0 0,-2 2-5727 0 0,-4-34 687 0 0,-1 1 3586 0 0,8 2-135 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55229.81">17785 11132 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,3-7-177 0 0,-3 5 136 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-2 1-247 0 0,11-6 1678 0 0,45-7 1057 0 0,23 24-286 0 0,-63-6-2099 0 0,-5-1-94 0 0,0 1 0 0 0,1 1 0 0 0,-2 0 0 0 0,0-1 1 0 0,1 2-1 0 0,-2 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,4 6-256 0 0,13 29 768 0 0,8 35 88 0 0,-28-15-68 0 0,-12-16 336 0 0,-17-11-1124 0 0,16-32 144 0 0,-1 1 0 0 0,2 0-1 0 0,-2-1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,0-1-1 0 0,-5 1-143 0 0,-41 16 238 0 0,51-19-196 0 0,-2-1-31 0 0,1 2-27 0 0,62-29-776 0 0,16 17-152 0 0,-4 28-54 0 0,-20 15 92 0 0,-12 14 866 0 0,-29-27 40 0 0,-6-15 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,-2 2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 3 0 0 0,-27 31 1352 0 0,-11 1-736 0 0,25-32-497 0 0,-1 0-1 0 0,2-2 1 0 0,-2 0-1 0 0,-1-1 1 0 0,1-1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-2 1 0 0,0 0 0 0 0,0-1-1 0 0,-6-1-118 0 0,-62 7 387 0 0,28 10-334 0 0,29-16-53 0 0,-6-18-801 0 0,24 9-282 0 0,2 1-2237 0 0,2 2-3262 0 0,0-2-1015 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56249.811">18621 11103 14800 0 0,'0'0'332'0'0,"0"0"50"0"0,0 0 25 0 0,0 0-47 0 0,0 0-106 0 0,0 0 417 0 0,0 2 206 0 0,-9 52 3904 0 0,7-24-4120 0 0,-17 135 1824 0 0,-3-30-880 0 0,8-32-165 0 0,-13 131-832 0 0,26-228-672 0 0,1-5-273 0 0,0-1-138 0 0,0 3-1216 0 0,-2 4 3621 0 0,1-2-4753 0 0,1 0-9564 0 0,0-5 10339 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56479.811">18630 11155 920 0 0,'0'-5'1157'0'0,"1"2"5384"0"0,19-13-1079 0 0,30 8 55 0 0,25 14-2419 0 0,-3 11-1830 0 0,-11 12 320 0 0,18 44-1572 0 0,-20 12 2016 0 0,-53-72-1886 0 0,-1 1 0 0 0,-1-2 0 0 0,1 1 0 0 0,-2 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-2 1 0 0 0,0-1 0 0 0,-1 2 0 0 0,0-2-1 0 0,-1 1 1 0 0,-2 0 0 0 0,0 6-146 0 0,1 0 8 0 0,-2 0 0 0 0,1-1 0 0 0,-3-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-3-1 0 0 0,1 1 0 0 0,-1-2 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-2 0 0 0,-4 2-8 0 0,11-9 173 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,-4 0-174 0 0,-124-3-286 0 0,105-4-191 0 0,23 5 329 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-6-4 148 0 0,6 3-710 0 0,5 6-8073 0 0,3 0 434 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57489.811">19363 11722 7368 0 0,'0'0'333'0'0,"0"0"0"0"0,-9 4 14776 0 0,7-4-14374 0 0,2-2-710 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,2 0 1 0 0,-1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,1 0 0 0 0,0 1-25 0 0,-3 1 94 0 0,0 0 9 0 0,0 0 29 0 0,0 0 17 0 0,0 0 3 0 0,0 0 11 0 0,0 0 44 0 0,0 0 17 0 0,0 0 6 0 0,0 0 4 0 0,0 0 4 0 0,0 0 2 0 0,0 0 0 0 0,0 0-16 0 0,0 0-66 0 0,0 0-29 0 0,0 0-8 0 0,0 0-9 0 0,0 0-33 0 0,-1 0-25 0 0,-21 28-43 0 0,16-8 74 0 0,5-18-19 0 0,1-2 6 0 0,1-2-18 0 0,9-16-135 0 0,6 10 5 0 0,7 14-588 0 0,-17 2 664 0 0,2 16 16 0 0,-8-23 62 0 0,-5 8 297 0 0,-7-2-725 0 0,11-7 151 0 0,-9 8-801 0 0,1-8-2062 0 0,9 0 1532 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58349.811">19732 11281 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-3 420 0 0,0 3 3077 0 0,0 1 3963 0 0,-7 136-3072 0 0,-4-26-2600 0 0,-8 63-1021 0 0,8-65-304 0 0,4 23-619 0 0,7-132-213 0 0,0 0-69 0 0,0 0-12 0 0,0 0-139 0 0,0-53-6135 0 0,0 30 4451 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58689.811">19703 11320 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,1-1 21 0 0,2-2-256 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0-1 0 0,-2 1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,2 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,1 0-170 0 0,6 4 318 0 0,-2 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 1 0 0 0,0 0-1 0 0,-1 1-318 0 0,21 14-106 0 0,-26-19 167 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 2 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0 3-62 0 0,3 16 844 0 0,-5-16-830 0 0,2 1-1 0 0,-1-1 1 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-3 1 0 0 0,2 0-1 0 0,-2-2 1 0 0,-1 4-14 0 0,0-2 119 0 0,1-2-1 0 0,0 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,0 1-1 0 0,-1-2 1 0 0,0 1-1 0 0,-1-2 1 0 0,0-1-1 0 0,0 2 1 0 0,0-1-1 0 0,1 0 1 0 0,-2-1-1 0 0,0 0 1 0 0,0-1-1 0 0,-5 2-118 0 0,-7 5 128 0 0,18-8-128 0 0,2-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-2 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,2-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,-14-22-1234 0 0,14 3-3424 0 0,6 7-3433 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="59859.811">20211 11037 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-270 0 0,1 1 131 0 0,13 71 4572 0 0,-17-14-1957 0 0,3 6-1459 0 0,3 28-1321 0 0,-6 20-232 0 0,-4 70 0 0 0,-6-79 962 0 0,-11 12-720 0 0,24-114-750 0 0,0-1-89 0 0,0 0-360 0 0,0 0-163 0 0,-5-10-5760 0 0,1 0 563 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60069.811">20208 11531 1376 0 0,'0'0'65'0'0,"0"-2"389"0"0,27-31 11411 0 0,10-15-8036 0 0,4 18-1988 0 0,-39 29-1803 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,2 2 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1-38 0 0,7 4 156 0 0,34 75 888 0 0,-37-72-884 0 0,2 1-1 0 0,-1 0 1 0 0,-2 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2 7-159 0 0,-10 85 1127 0 0,5-94-1133 0 0,1-8-6257 0 0,0-1-578 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60829.81">20784 11343 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 2 21 0 0,-8 43 177 0 0,-10 35 3194 0 0,7 29-1553 0 0,-5 89-172 0 0,-1-87-257 0 0,11-98-2469 0 0,3-12-3087 0 0,3 0-3929 0 0,0-1 1033 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61029.81">20755 11343 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,15-6-181 0 0,-12 4-54 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 2 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 2 1 0 0,2-1-1 0 0,-2 0 0 0 0,4 2-301 0 0,0 0 145 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0 1-1 0 0,-2-1 1 0 0,2 1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-3 1-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 2 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,2 2 0 0 0,-1 4-144 0 0,7 61 1883 0 0,-26 14-1742 0 0,14-84-123 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,-3 0-18 0 0,-51 3 1171 0 0,-3 13-2729 0 0,57-16 1668 0 0,-17-4-935 0 0,1-8-3444 0 0,13 5 2477 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63909.811">16587 11202 3224 0 0,'0'-1'240'0'0,"0"-1"165"0"0,0 1 1443 0 0,0 1 616 0 0,0 0 116 0 0,0-1 259 0 0,0-3-1698 0 0,1 2 2411 0 0,12-14-2439 0 0,-11 10-1053 0 0,-2-4 606 0 0,0 6-4232 0 0,0 4 2520 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190399.81">5710 11136 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,3-8 314 0 0,20-65 850 0 0,-20 60-996 0 0,1 1 0 0 0,2-1-1 0 0,-1 2 1 0 0,1 0-1 0 0,0-1 1 0 0,2 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,4 2 1 0 0,7-8-478 0 0,-17 15 40 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-40 0 0,26 51 1331 0 0,-26-50-1287 0 0,3 11 148 0 0,-2 0 0 0 0,1-3 0 0 0,-2 3 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,-1 0 0 0 0,1-2 0 0 0,-3 0 0 0 0,-1 5-192 0 0,6-15 21 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-2 1 1 0 0,2 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0-1-22 0 0,-3-2-60 0 0,1 1-1 0 0,-1-2 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,2 0 1 0 0,-1 0-1 0 0,2-1 1 0 0,-1 2-1 0 0,1-2 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-7 60 0 0,-8-51-3591 0 0,10 42 1933 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192059.811">7263 11029 4144 0 0,'0'0'319'0'0,"-11"2"1818"0"0,10-1 2461 0 0,1 0 4419 0 0,7 0-8694 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 0-323 0 0,104-53 185 0 0,-77 19-185 0 0,-30 36 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,-32-36 0 0 0,32 36 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-5 1 0 0 0,-41 17 0 0 0,40-11 47 0 0,1 0 0 0 0,0 1 1 0 0,2-2-1 0 0,-1 3 0 0 0,0-1 0 0 0,0 1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,2 1-1 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-2 0 0 0,2 10-47 0 0,2-12 52 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-2-1 0 0,0 2 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,4 4-52 0 0,-5-6 15 0 0,-1-2 0 0 0,1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 0-15 0 0,49-5-958 0 0,-37-1-1726 0 0,-3-1-3307 0 0,-5 0-1687 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="193429.81">7807 10764 10304 0 0,'0'-4'934'0'0,"0"-9"-627"0"0,0 11 320 0 0,0-3 712 0 0,-1 3 3325 0 0,0 3-4568 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 2-95 0 0,-2 5 224 0 0,1 31 664 0 0,-7 114 1598 0 0,13-73-1828 0 0,-5-40-734 0 0,-2-33-364 0 0,1 8-1982 0 0,-2-11-5617 0 0,2-5 5673 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="193879.811">7713 10860 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,1-2-294 0 0,1-2 74 0 0,-1 3 886 0 0,14-7 3459 0 0,-11 6-4230 0 0,2 0-1 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,-2 1-1 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-348 0 0,36 4 963 0 0,-20-6-540 0 0,-15 0-358 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,2 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 1 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,2 2-64 0 0,53 63 377 0 0,-54-57-1065 0 0,-5 3-3411 0 0,-1-9 774 0 0,1-2-4194 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="196929.81">5341 10901 456 0 0,'0'-16'1413'0'0,"0"15"159"0"0,0-1 76 0 0,0-41 2855 0 0,0 42-3991 0 0,0 1 0 0 0,0 0-24 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0 47 0 0,0 0 207 0 0,0 0 89 0 0,0 0 21 0 0,0 0-24 0 0,-11 5 931 0 0,8-3-1418 0 0,2 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1-182 0 0,5 87 3864 0 0,2 20-3175 0 0,-12-58 34 0 0,4 17-176 0 0,1-67-729 0 0,-4 5 3 0 0,1-5-7687 0 0,2-2-336 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="197139.81">5333 10993 11976 0 0,'0'-4'180'0'0,"1"-1"0"0"0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,2-2-180 0 0,6-4 1628 0 0,-6 6-1094 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 1 1 0 0,5-1-535 0 0,-6 1 86 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 1 0 0 0,0-1 0 0 0,2 1 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,0 1-1 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 1 0 0 0,3 3-86 0 0,22 34 302 0 0,18 36 108 0 0,-32-47-1847 0 0,-8-22-150 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170686.919">6161 10870 456 0 0,'-2'29'10790'0'0,"-6"-4"-6142"0"0,-16 80 1001 0 0,22-98-5360 0 0,-2 2-52 0 0,2 0 0 0 0,0-1-1 0 0,0 2 1 0 0,-1-2-1 0 0,2 2 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-2 1 0 0,1 7-237 0 0,8 20 1589 0 0,-1-28-1573 0 0,-6-6-16 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1-1-1 0 0,-2 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-3 0 0 0,52-79 357 0 0,-55 84-357 0 0,57-128 184 0 0,-54 88-184 0 0,-5 34-21 0 0,-6 2 2 0 0,2 4-2431 0 0,5 0 1260 0 0,-8 0-578 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-169886.919">6558 10832 2304 0 0,'0'0'428'0'0,"0"0"959"0"0,0 0 422 0 0,0 0 81 0 0,0 0-74 0 0,0 0-388 0 0,0 0-168 0 0,0 0-38 0 0,0 0-52 0 0,0 0-190 0 0,0 0-85 0 0,0 0-21 0 0,-5 13 2869 0 0,10 28-896 0 0,6 19-821 0 0,-4 31-482 0 0,15 22-8 0 0,-18-106-1420 0 0,-4-5-17 0 0,4 4 78 0 0,14 27 298 0 0,-18-32-578 0 0,0-1-4 0 0,1 1 26 0 0,5 3 65 0 0,-1 7 16 0 0,2-15 203 0 0,32-92 1554 0 0,-17 18-2314 0 0,-2 29 1122 0 0,19-33-626 0 0,-23 58-1899 0 0,-2 6 396 0 0,-8 14-8315 0 0,-6 4 2000 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-167866.919">6946 14769 1376 0 0,'0'0'65'0'0,"0"0"298"0"0,0 0 1226 0 0,-5-11 8887 0 0,3 3-10689 0 0,2 7 20 0 0,0-12-1355 0 0,0 4-2483 0 0,0 6 619 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-167696.919">6942 14740 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 10 0 0 0,-3 2 1224 0 0,3-12 232 0 0,0 0 48 0 0,0 0 0 0 0,0 0-1128 0 0,0 0-232 0 0,0 0-48 0 0,0-6 0 0 0,0 3-96 0 0,0 3-128 0 0,0 0 32 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-166746.919">6934 14720 2760 0 0,'0'0'125'0'0,"0"-12"2231"0"0,-1 1 3939 0 0,-16 48-2743 0 0,8 55-695 0 0,18 30 396 0 0,17-18-1214 0 0,11-60-933 0 0,-33-43-1072 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,2-3-34 0 0,107-160 703 0 0,-81 109-639 0 0,-9-30-572 0 0,-20 75 468 0 0,0 9-31 0 0,-7-21-455 0 0,0 10-3508 0 0,6 10-3672 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-120276.919">10548 14792 11952 0 0,'0'-1'67'0'0,"0"1"0"0"0,-1-2 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-67 0 0,-38-9 5146 0 0,40 8-5069 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,2-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 2-77 0 0,-11 8 763 0 0,6-6-634 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,1 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,0 1-1 0 0,-1-2 1 0 0,1 2 0 0 0,1-1 0 0 0,0 0-1 0 0,-1 3-128 0 0,-1 1 108 0 0,-2 11 172 0 0,-1-1 0 0 0,3 1 0 0 0,-1-1 0 0 0,2 2 0 0 0,0-1 0 0 0,2 0-280 0 0,2 60 688 0 0,22-36-159 0 0,-8-32-346 0 0,-15-11-174 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1-9 0 0,11-9 35 0 0,-2-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,1-2 0 0 0,-2 1-1 0 0,6-10-34 0 0,31-40 89 0 0,-3 6-100 0 0,-19 21-55 0 0,-24 33-4 0 0,-2-1-103 0 0,2 2-332 0 0,1 1-119 0 0,0 0-16 0 0,-2 0-596 0 0,-1 1 165 0 0,1-2-2477 0 0,2 1 1724 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-119726.919">11042 14488 12064 0 0,'0'0'553'0'0,"0"0"-16"0"0,-9 14-151 0 0,-5 31 4878 0 0,5 28-1596 0 0,2-21-2083 0 0,-7 69 353 0 0,-2 18 194 0 0,1 135-900 0 0,14-183-1248 0 0,1-89-72 0 0,0-2-51 0 0,0 0-18 0 0,0 0-158 0 0,-3-24-4130 0 0,2 7-1692 0 0,-2-1-1669 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-119476.919">10954 14759 2304 0 0,'20'-56'224'0'0,"-11"35"1777"0"0,18 3 11624 0 0,10 20-9044 0 0,10 20-2754 0 0,-1 24-1302 0 0,-9-26-2042 0 0,-29-15-78 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-166306.919">7489 14624 10136 0 0,'-11'49'1272'0'0,"9"-43"-735"0"0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1-1-1 0 0,0 2 1 0 0,2-1-1 0 0,-2-1 0 0 0,1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,1 3-538 0 0,7 26 1513 0 0,21 67 1825 0 0,8 13-1726 0 0,11-9-228 0 0,-25-65-629 0 0,-2-15-113 0 0,-21-10-556 0 0,6-23-22 0 0,13-35 0 0 0,13-46 53 0 0,17 7-396 0 0,-11 31 158 0 0,-17-11 121 0 0,-6 10 0 0 0,5-4 0 0 0,-17 42-97 0 0,-6 12-406 0 0,0 1-165 0 0,8-8-841 0 0,-2 1-1411 0 0,-3 6-6017 0 0,3 2 8141 0 0,-5 0 11 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-164976.919">8173 14958 1840 0 0,'1'4'465'0'0,"-1"3"-969"0"0,-4-2 8499 0 0,4-4-5413 0 0,0-1-959 0 0,-3 14 3293 0 0,5-12-4747 0 0,1 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0 0 0 0,2-2-1 0 0,-2 1 1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,1 0-1 0 0,0 0-168 0 0,6-2 150 0 0,0-2 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,3-4-150 0 0,7-10 74 0 0,-1 0 1 0 0,-2 0-1 0 0,0-3 1 0 0,-1 2-1 0 0,-1-2 1 0 0,8-21-75 0 0,-19 43 4 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0-4 0 0,-7 2 35 0 0,-2 0-1 0 0,2 2 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,0 0 1 0 0,1 1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2-1 0 0 0,0 2 1 0 0,0-1-1 0 0,0 1 1 0 0,2 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 2-1 0 0,1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,2 1-1 0 0,1 3-34 0 0,0-9 18 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,2 0-1 0 0,-1-2 1 0 0,-1 2-1 0 0,2-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-18 0 0,5 1-63 0 0,2 1 0 0 0,-1-2 0 0 0,0 0 0 0 0,-1 0-1 0 0,2-1 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,11-2 63 0 0,-8 1-520 0 0,14-4-1481 0 0,-9 1-3720 0 0,0 1-1868 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-163966.919">8705 14498 6624 0 0,'3'19'-4'0'0,"-2"-6"534"0"0,-1 2 5466 0 0,0-15-4969 0 0,0 0-16 0 0,-7 43 3846 0 0,0 30-3228 0 0,2 1 0 0 0,5 39-1629 0 0,0-61 228 0 0,5 10-228 0 0,-5 42-16 0 0,-5-62-2758 0 0,5-29-1657 0 0,0-11 1925 0 0,0-1-3470 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-163606.919">8663 14848 10136 0 0,'23'-69'1056'0'0,"12"-14"3846"0"0,-33 78-4603 0 0,1 1 0 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,4-1-299 0 0,-5 3 72 0 0,0-1-1 0 0,1 1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 2 0 0 0,2-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,2 2-71 0 0,29 22 580 0 0,10 41 1278 0 0,-31-1-3924 0 0,-13-47-2692 0 0,-2-15 3016 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121546.919">9466 14304 5872 0 0,'0'0'266'0'0,"0"0"1"0"0,-3-11 1056 0 0,3 9 7600 0 0,-9 79-5279 0 0,9-26-2198 0 0,1 27 275 0 0,-4 1-1 0 0,-6 29-1720 0 0,-13 182 1691 0 0,18-167-981 0 0,5-111-1358 0 0,-2-19-2345 0 0,-6-50-991 0 0,2 16 1937 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121236.919">9240 14313 8752 0 0,'0'0'673'0'0,"11"7"4424"0"0,14 6-302 0 0,19-10-2564 0 0,-33-3-1654 0 0,61 1 445 0 0,-49-3-776 0 0,-1 1 0 0 0,1 1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1 1 0 0 0,11 3-246 0 0,-22-3 75 0 0,1 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1 1 1 0 0,-2 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1-75 0 0,38 47-3176 0 0,-43-44 1404 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-120726.919">9880 15028 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 0-276 0 0,-31 2 2318 0 0,14-7 1927 0 0,2-22-2183 0 0,18 22-2093 0 0,-2 0 0 0 0,1-1 0 0 0,1 2 0 0 0,0-2-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 2-1 0 0,0-1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,2-2-146 0 0,8-19 178 0 0,-9 17-156 0 0,1-1 1 0 0,1 1-1 0 0,1 0 0 0 0,-2 1 1 0 0,2 1-1 0 0,1-2 1 0 0,-2 1-1 0 0,3 1 0 0 0,1-3-22 0 0,-6 7 22 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1 0 0 0,3 0-22 0 0,-1 0 73 0 0,-2 1 0 0 0,2 0-1 0 0,-2 1 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-1-1 1 0 0,0 2 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 0 1 0 0,0 1 0 0 0,-2-1 0 0 0,2 1-1 0 0,-1 0 1 0 0,2 1-73 0 0,10 71 976 0 0,-13-59-728 0 0,-1 1 22 0 0,-2 2 1 0 0,-1-2-1 0 0,0 0 0 0 0,0 1 0 0 0,-3 0 0 0 0,1-3 1 0 0,-3 8-271 0 0,3-9 132 0 0,1-11-108 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1-2 1 0 0,0 2-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-2-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,-2 0-24 0 0,1-2 9 0 0,1 1-1 0 0,-1-2 1 0 0,0 1 0 0 0,0-1-1 0 0,2 1 1 0 0,-2-2-1 0 0,1 1 1 0 0,-1-1 0 0 0,2 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,-3-2-8 0 0,4 3-63 0 0,1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 2 1 0 0,0-2-1 0 0,0 0 0 0 0,1 1 0 0 0,-2-4 63 0 0,2 5-278 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 2 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,2-4 278 0 0,5-7-2146 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116106.919">12255 14896 3680 0 0,'0'0'284'0'0,"0"0"17"0"0,3-5 3845 0 0,5-2 6650 0 0,-23 226-6730 0 0,17-190-3860 0 0,0-2-3590 0 0,-2-27 1760 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115556.919">12612 14786 920 0 0,'-4'10'76'0'0,"-23"26"272"0"0,-6-6 6376 0 0,5-8-722 0 0,26-21-4979 0 0,-5 7 987 0 0,3 15 528 0 0,5-5-1218 0 0,4-12-1123 0 0,1-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,3 0-1 0 0,-1-1 1 0 0,-1 0 0 0 0,7 1-198 0 0,22 11 384 0 0,-31-13-322 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,0 2 0 0 0,-1-1 0 0 0,2 1 1 0 0,-2 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1-62 0 0,-2 3 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1-2 0 0 0,4 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,0-3 0 0 0,-1 1-326 0 0,-14-19-857 0 0,16 2-6482 0 0,3 11 584 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-117286.919">11613 14412 10824 0 0,'0'0'241'0'0,"0"7"331"0"0,-6 105 4121 0 0,-2 8-200 0 0,1-17-2317 0 0,-4 57-880 0 0,11 65-5334 0 0,0-224-1053 0 0,0-1-1451 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116916.919">11968 14428 2760 0 0,'-19'-15'247'0'0,"16"14"193"0"0,2 1 1710 0 0,-1 3 4946 0 0,-4 8-4369 0 0,4-5-1946 0 0,-28 37 1201 0 0,37-2-671 0 0,-29 121 670 0 0,-25 95 167 0 0,10-123-2609 0 0,30-119-2025 0 0,3-7-2648 0 0,-1 1-1568 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116696.92">11550 14809 9672 0 0,'0'0'748'0'0,"1"1"-492"0"0,3 3-231 0 0,-3-2 331 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 0-356 0 0,110 16 3649 0 0,-108-15-4114 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,4 4 465 0 0,10 8-1693 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-110456.919">14067 14762 1840 0 0,'0'2'133'0'0,"0"7"1371"0"0,-8 14 9957 0 0,3-11-10918 0 0,0 10 2807 0 0,4-14-2599 0 0,1-7-23 0 0,0-1-45 0 0,0 3-163 0 0,-7 41 1090 0 0,-8 98 530 0 0,11-18-1604 0 0,8-88-486 0 0,-4-34-216 0 0,0-2-402 0 0,0 0-174 0 0,5-17-2600 0 0,-2 6 1430 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-110046.919">14041 14941 4144 0 0,'0'0'319'0'0,"0"0"75"0"0,-2-4 5801 0 0,0-1-4842 0 0,2-5-34 0 0,10-35 4642 0 0,7 32-3827 0 0,27-1-548 0 0,-7 20-1696 0 0,-32-6 128 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1-18 0 0,35 8 0 0 0,-24-7 0 0 0,-9-1 0 0 0,8 10 0 0 0,-2 11-870 0 0,-15-21 616 0 0,2-2-383 0 0,0 1-179 0 0,-13 33-4440 0 0,12-31 3346 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-112086.92">13060 14458 3224 0 0,'0'0'143'0'0,"0"2"-3"0"0,-1-2 1084 0 0,-4 10-2538 0 0,2-8 6295 0 0,1-2 6252 0 0,3 16-9469 0 0,9 55 352 0 0,-24 132-1892 0 0,9-118 559 0 0,2-58-682 0 0,2-1 0 0 0,0 0 0 0 0,2 0 0 0 0,1 1 0 0 0,1 0-101 0 0,4 27-450 0 0,-11-46-56 0 0,1-6-6442 0 0,3-2 4901 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111836.919">13042 14624 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 0 21 0 0,3 0-42 0 0,107-19 3931 0 0,-43 8-2346 0 0,-40 15-4175 0 0,-19 3 964 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111476.919">13411 15004 7744 0 0,'0'0'356'0'0,"0"0"-8"0"0,0 0-63 0 0,0 0 571 0 0,-3 9 4563 0 0,-15-46-211 0 0,24-31-2906 0 0,28 41-1872 0 0,-15 14-315 0 0,-15 12-110 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-2 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 1-4 0 0,-1 1 59 0 0,2 0-1 0 0,-2 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,-2 0-1 0 0,2 1 1 0 0,-1-1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-2 1-59 0 0,2-4 22 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 0 0 0,2-1 1 0 0,0 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-23 0 0,-34 5 210 0 0,2-34-185 0 0,15 6-523 0 0,13-5-2557 0 0,8 16 1503 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111056.919">13785 14795 8288 0 0,'2'16'273'0'0,"-1"-32"1643"0"0,-1 16-472 0 0,0 0 76 0 0,0 0-55 0 0,0 0-287 0 0,0 2-123 0 0,-7 43 4957 0 0,-8-1-5210 0 0,14 91 812 0 0,6-39-1951 0 0,-5-90-1422 0 0,0-5-625 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-109556.919">13664 14562 8752 0 0,'22'16'1346'0'0,"-22"-14"-166"0"0,2-2-1575 0 0,3-4 4378 0 0,3-4 4520 0 0,3 1-11521 0 0,-6 3 1866 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-106806.919">14564 15024 6912 0 0,'79'11'8898'0'0,"-74"-10"-8618"0"0,1-1-1 0 0,0 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 0-1 0 0,-1 1 1 0 0,3-4-280 0 0,35-49 1321 0 0,-40 50-1321 0 0,0 1 1 0 0,1-1-1 0 0,0 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0-2-1 0 0,-19-33-90 0 0,15 38 124 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-34 0 0,-56 23 664 0 0,53-19-600 0 0,0 2 0 0 0,0-1 0 0 0,1 1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,2 1 0 0 0,-1-2 0 0 0,0 2 0 0 0,0 2-64 0 0,1 0 41 0 0,1 1 0 0 0,0-2 0 0 0,1 2 1 0 0,-1 0-1 0 0,2-1 0 0 0,1 2 0 0 0,-1-2 0 0 0,2 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,2 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,4 7-41 0 0,-4-10 98 0 0,2-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,5 6-98 0 0,-6-11 5 0 0,-1 0 0 0 0,2 0 0 0 0,-2-2 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 0-5 0 0,2-1-54 0 0,110-32-5788 0 0,-65 9 1619 0 0,-24 11 2079 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-102656.919">16086 14873 1840 0 0,'0'0'83'0'0,"0"0"169"0"0,0 0 668 0 0,0 0 288 0 0,0 0 58 0 0,0 0-22 0 0,0 0-144 0 0,0 0-63 0 0,0 0-11 0 0,0 0-2 0 0,0 8 2048 0 0,-3 18-266 0 0,2-2-362 0 0,1 76 1520 0 0,-3-31-3723 0 0,2 17-415 0 0,2-78 488 0 0,5 5-6100 0 0,0-7-783 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-102316.919">16091 15024 10136 0 0,'21'-55'5082'0'0,"10"10"-1747"0"0,-6 27-1698 0 0,-22 15-1500 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,2 0 1 0 0,0 0-137 0 0,1 1 60 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 1 0 0,-2-1-1 0 0,1 2 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 1 1 0 0,-1-2-1 0 0,2 2 0 0 0,-2 0 0 0 0,1 3-60 0 0,17 16 54 0 0,-6-14-897 0 0,-11-8-100 0 0,-1-1-37 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-104576.919">15247 14284 2304 0 0,'0'0'101'0'0,"0"0"294"0"0,0 0 1149 0 0,0 0 506 0 0,0 2 1554 0 0,0 9-1838 0 0,2 143 6571 0 0,-2 114-5024 0 0,-14-8-1402 0 0,10-160-1693 0 0,-6-27-376 0 0,9-72-114 0 0,1-1-766 0 0,-5-11-2968 0 0,-2-1-3447 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-104236.919">15220 14479 920 0 0,'0'-1'67'0'0,"-3"-7"403"0"0,4 0 4358 0 0,4-5-1924 0 0,-4 10-1691 0 0,20-31 4007 0 0,25-4-3052 0 0,7 6-888 0 0,-32 24-1087 0 0,-18 7-85 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 1-108 0 0,1 0 199 0 0,-2 1 0 0 0,2-1 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1-1 0 0,2 1 1 0 0,-2-1 0 0 0,4 4-199 0 0,30 58 460 0 0,-28-39-231 0 0,0 2 1 0 0,-2 0-1 0 0,-2-1 0 0 0,0 2 1 0 0,-2-2-1 0 0,0 1 0 0 0,-3 26-229 0 0,0-46 147 0 0,-2 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 1 0 0,-2 1-1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1-1 1 0 0,-1 1-1 0 0,2-1 0 0 0,-4 3-146 0 0,4-7 10 0 0,-2 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-4-2-10 0 0,-4-2-494 0 0,1-1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1-1 1 0 0,2 1-1 0 0,0-2 1 0 0,0 0-1 0 0,-4-5 495 0 0,4 0-5994 0 0,3-4-1719 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-103406.919">15645 15024 8288 0 0,'0'0'190'0'0,"5"-6"253"0"0,9-6-212 0 0,30 1 5159 0 0,2 6-1205 0 0,-17 13-2607 0 0,-5-3 202 0 0,-15-3-715 0 0,-16-5-592 0 0,-40 8 113 0 0,-39 16 500 0 0,81-19-1076 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 0 0 0 0,2 2 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-2 0 0 0,0 3-10 0 0,-2 6 2 0 0,0-6-2 0 0,2 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-2 0 0 0,3 7 0 0 0,13 14 0 0 0,-17-25 1 0 0,2 2 37 0 0,1 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1-2 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,1-1 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,1 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,3-1-39 0 0,48-28 241 0 0,-41 15-275 0 0,-1 2 0 0 0,1-3 0 0 0,-2-1 0 0 0,-1 2 0 0 0,0-3 0 0 0,-1 2 0 0 0,0-2 34 0 0,13-68-964 0 0,-15 34 382 0 0,-19 87 634 0 0,11-24-10 0 0,1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,3-2-1 0 0,-1 2 1 0 0,4 6-42 0 0,15 45 54 0 0,-9-43-1794 0 0,-7-20 730 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-98716.919">16757 14395 3224 0 0,'0'0'143'0'0,"0"0"279"0"0,0 0 1073 0 0,0 0 470 0 0,0 0 92 0 0,0 0-154 0 0,0 0-730 0 0,0 0-315 0 0,0 7 684 0 0,-3 1-898 0 0,3-6-48 0 0,0 7 1051 0 0,-8 45 1551 0 0,-37 294 1366 0 0,41-324-4246 0 0,3 2 0 0 0,0-1-1 0 0,2 0 1 0 0,0 1 0 0 0,3 0-1 0 0,-1-3 1 0 0,2 3-1 0 0,6 16-317 0 0,23 16 208 0 0,-32-53-186 0 0,1-2 0 0 0,1 2 0 0 0,-1-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2-2-1 0 0,1 2 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-2-2 1 0 0,2 1 0 0 0,0-1 0 0 0,-2 1-1 0 0,2-1 1 0 0,3 0-22 0 0,-5-2 31 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-2-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-2-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,0-1-30 0 0,-2 5 3 0 0,10-17 55 0 0,-2 1 1 0 0,0-2-1 0 0,0 1 0 0 0,-1 0 0 0 0,3-18-58 0 0,6-16 41 0 0,23-95-41 0 0,16-143-432 0 0,-49 253-57 0 0,-2 7-2509 0 0,-1 9-4848 0 0,-1 11 100 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-97336.919">17921 14907 2304 0 0,'0'0'101'0'0,"0"17"22"0"0,-8 5 6125 0 0,-3 17 4249 0 0,9-9-9080 0 0,-3 85 316 0 0,1-83-1477 0 0,0-19-426 0 0,3-12-721 0 0,1-1-329 0 0,0 0-75 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-96826.919">18180 14458 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 2-242 0 0,5 69 6774 0 0,-10 3-1144 0 0,-8 41-2340 0 0,2 48-2718 0 0,6-9-705 0 0,0 15-1521 0 0,5-159 244 0 0,0-8-61 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-96436.919">18445 14875 10136 0 0,'0'0'777'0'0,"-1"2"-505"0"0,-3 41 4407 0 0,3-11-457 0 0,3 76-789 0 0,-4-100-3589 0 0,2 0-1781 0 0,0-7 758 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95846.919">18878 14863 1376 0 0,'1'-2'299'0'0,"13"-56"5252"0"0,-16 42-5059 0 0,1 12-375 0 0,1 3 35 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,1-1-152 0 0,-4 1 283 0 0,1 0 0 0 0,1 1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-2 1 0 0 0,2-1 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 1-285 0 0,-9 12 754 0 0,-46 63 501 0 0,34-6-220 0 0,24-66-992 0 0,-1-1-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,2 0 1 0 0,-2 0-1 0 0,5 3-41 0 0,1 6 59 0 0,8 8 178 0 0,-13-19-112 0 0,-1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0-125 0 0,-14 16 28 0 0,10-19-9 0 0,0 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2-2 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1-19 0 0,-39 2-215 0 0,7 20-3705 0 0,33-14-4023 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95136.919">19221 14958 3680 0 0,'0'0'284'0'0,"0"0"109"0"0,2-1 1154 0 0,30-17 5762 0 0,36 17-2771 0 0,-36 11-2764 0 0,-17 0 1490 0 0,-63-16-3312 0 0,43 4 32 0 0,1 1 0 0 0,-2 0 1 0 0,0 0-1 0 0,2 1 1 0 0,-2-1-1 0 0,2 1 0 0 0,-2 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 1 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 1 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,-2 3 16 0 0,0-1 34 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 0 0 0,1 2 1 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,-1 3-33 0 0,4-7 57 0 0,1 0-1 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,2 2-56 0 0,-2-4 45 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 1 0 0,2-1-1 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1-1-45 0 0,103-151-3426 0 0,-105 155 3373 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,2-1 0 0 0,-2 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 53 0 0,-2 20 337 0 0,-17 78 1575 0 0,11 7-1206 0 0,16-62-7272 0 0,-5-33-749 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-98036.919">17596 14346 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 2 76 0 0,-5 11 2311 0 0,-8 36 3900 0 0,-2 112-3759 0 0,-18 84 806 0 0,3 40-2464 0 0,22-197-1627 0 0,8-87-756 0 0,-3-6-2095 0 0,3-4 1602 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-97796.919">17511 14618 11232 0 0,'-4'-28'1016'0'0,"5"28"-836"0"0,14-28 2777 0 0,66 23 2000 0 0,18 19-1797 0 0,-55 6-4345 0 0,-36-16-189 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93526.919">20179 15031 15664 0 0,'14'5'1187'0'0,"-11"-4"-976"0"0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 1 0 0,1 1-1 0 0,-2-1 0 0 0,1 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,2-1 1 0 0,-2 1-1 0 0,1-2-210 0 0,8-12-211 0 0,-4 9-129 0 0,-2-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,0-1 0 0 0,0 2 0 0 0,2-10 340 0 0,-9-34-1540 0 0,4 51 1562 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-2 1 0 0 0,2-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-22 0 0,-22 17 1568 0 0,19-13-1383 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,1-1 0 0 0,0 1-185 0 0,-7 31 308 0 0,5-27-103 0 0,1 2 0 0 0,0-2-1 0 0,0 1 1 0 0,1 1 0 0 0,1-1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,2 0 0 0 0,-1 2-205 0 0,16 19 1394 0 0,-17-33-1436 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 0 0 0 0,-2 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0 42 0 0,0-1-47 0 0,96-58-5723 0 0,-83 50 4417 0 0,-4 1-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94286.919">19741 14713 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0-6 199 0 0,4-20 284 0 0,-4 26 22 0 0,0 0 21 0 0,0 0 53 0 0,0 0 198 0 0,0 0 86 0 0,0 0 21 0 0,0 0-28 0 0,0 0-122 0 0,-11 86 4045 0 0,3-21-3014 0 0,-22 176 836 0 0,14-106-2456 0 0,14-119-5049 0 0,1-15-3688 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94056.92">19719 14830 19351 0 0,'0'0'439'0'0,"0"0"62"0"0,0 0 33 0 0,0 0-65 0 0,7-3-292 0 0,98-18 2799 0 0,-42 10-2385 0 0,-23 8-4619 0 0,-38 3 2335 0 0,-2 0-17 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-89026.919">20577 14917 920 0 0,'0'0'115'0'0,"0"0"146"0"0,0 0 68 0 0,2-1 14 0 0,12-24-975 0 0,0 11 771 0 0,-13 12 195 0 0,-1 2 149 0 0,0 0 590 0 0,0 0-1059 0 0,7-7 9846 0 0,-2 4-8006 0 0,-4 1-1530 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1-1-324 0 0,1-1 1337 0 0,0 4-893 0 0,-10 8-200 0 0,-32 57 2244 0 0,14 4-1504 0 0,26-15-648 0 0,2-53-335 0 0,1 7 28 0 0,0-1-1 0 0,1 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,2 0 0 0 0,-2-1-1 0 0,1 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,1 0-1 0 0,1 1-28 0 0,-2-3 14 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-2 0 0 0,4-1-13 0 0,35-21 64 0 0,-3-45 8 0 0,-17-10-72 0 0,-17 41-89 0 0,2-53-263 0 0,-10 91 324 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 29 0 0,-4 9-8024 0 0,2 0 350 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88466.92">21090 14792 2304 0 0,'0'0'101'0'0,"0"0"363"0"0,0 0 1439 0 0,0 0 626 0 0,0 0 126 0 0,0 0-194 0 0,3-13 1239 0 0,0 22 4485 0 0,-1 45-5205 0 0,-7 22-1571 0 0,2 34-565 0 0,-5-50-599 0 0,9 95 126 0 0,6-99-812 0 0,6-128-3199 0 0,-11 24-1172 0 0,-2 35 2865 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88226.92">21098 14932 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-150 0 0,-8-5 3377 0 0,18-30 352 0 0,36-15-1964 0 0,-39 47-2182 0 0,-4 1 153 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,4 1-123 0 0,37 11 165 0 0,-9 22-245 0 0,-10 20-3497 0 0,-24-52-1940 0 0,-1-2-1564 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86216.919">21772 14762 9416 0 0,'-2'-4'852'0'0,"-25"-9"284"0"0,16 11 6835 0 0,-12 30-4820 0 0,19-19-2774 0 0,-53 123 2838 0 0,26-37-1934 0 0,22-68-1118 0 0,2-2 0 0 0,1 3-1 0 0,1-1 1 0 0,1 0 0 0 0,2 0 0 0 0,1 1-1 0 0,0-2 1 0 0,3 8-163 0 0,-2-17-6 0 0,15 114-229 0 0,4-75-1218 0 0,-1-36-2030 0 0,-11-14-2522 0 0,-6-5-1562 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85956.919">22134 14717 11520 0 0,'0'0'886'0'0,"1"-1"-582"0"0,17 6 5156 0 0,-13-1-5008 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 2 1 0 0,0 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 5-452 0 0,6 12 803 0 0,7 60 1048 0 0,-12-35-1193 0 0,-4 49 394 0 0,-5 9-300 0 0,-12 6-403 0 0,-14 44-253 0 0,2-46-2616 0 0,-9-3-4080 0 0,20-60-2023 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-80646.919">2552 13338 2760 0 0,'-23'-10'247'0'0,"11"-3"39"0"0,11 13 290 0 0,-4-1-375 0 0,3-4 6201 0 0,1-1-5440 0 0,13 4 7229 0 0,-6 2-9038 0 0,103 43 4699 0 0,-31-7-2217 0 0,54-16-519 0 0,51 0-182 0 0,-22 27-394 0 0,-133-35-455 0 0,-4-1-32 0 0,1-1 0 0 0,0 0-1 0 0,-1-2 1 0 0,2-1-1 0 0,0 0 1 0 0,0-2-1 0 0,1-1 1 0 0,-1-2-1 0 0,1 0 1 0 0,7-2-53 0 0,158-29 1189 0 0,101-36-261 0 0,-105 43-928 0 0,-158 20 0 0 0,316-2 0 0 0,-26 31 15 0 0,28-10 250 0 0,14 11-174 0 0,-131-11 135 0 0,-11 4-42 0 0,132 18-48 0 0,-239-28-125 0 0,89 12 42 0 0,212 32 22 0 0,130 2 393 0 0,-222-18-403 0 0,378 58 135 0 0,-287-57-200 0 0,-53 1-61 0 0,-56-1 141 0 0,8 3-80 0 0,-109-22 0 0 0,84-1 0 0 0,171 5 0 0 0,-190-4 0 0 0,77-9 0 0 0,201-21 0 0 0,-320 10 0 0 0,-36 5 0 0 0,332-3 0 0 0,-286-12 0 0 0,437-12-9 0 0,-344 2 914 0 0,-19-9-1376 0 0,71 4 966 0 0,-87 29-599 0 0,-8 4-152 0 0,-143 2 112 0 0,-4 6 239 0 0,4-4 314 0 0,61 6-541 0 0,33-15-88 0 0,3-7 252 0 0,-122-4-160 0 0,211-26 128 0 0,-70-1 0 0 0,-48 7 11 0 0,10-2-22 0 0,127 6 11 0 0,-36 4 80 0 0,122 6-133 0 0,-167 16 42 0 0,207-16 11 0 0,-138 9 0 0 0,45 0 0 0 0,338 25 139 0 0,-143-28-86 0 0,-345 21 75 0 0,-19-2-128 0 0,-91-19 0 0 0,-9-8 148 0 0,27-13-132 0 0,-45 16-28 0 0,73 15 12 0 0,-54 6-96 0 0,-105-8 80 0 0,-11 3 5 0 0,-12 12-319 0 0,20-3 154 0 0,11 7-187 0 0,-9 4 347 0 0,0 58 16 0 0,-6 84 15 0 0,14 157 28 0 0,0-114-101 0 0,19 26 233 0 0,-5-4-91 0 0,-5 19-20 0 0,-29-44 106 0 0,-5-60-95 0 0,0-20-75 0 0,0 16 0 0 0,0-27 224 0 0,-7-28-160 0 0,15-81-64 0 0,1-2 0 0 0,-1 1 0 0 0,0-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-3 0 0 0 0,-17 8 0 0 0,3-8 0 0 0,-321 7 96 0 0,116-13-96 0 0,-246 3 0 0 0,58 3 71 0 0,-125 7-86 0 0,-159-20 71 0 0,45 0-136 0 0,61 4 80 0 0,94-1 0 0 0,-387-10 0 0 0,163 0 68 0 0,202 8 268 0 0,287 9-440 0 0,-610-17 204 0 0,283-18-164 0 0,114 4 77 0 0,-395-1 78 0 0,343 12-91 0 0,-3-16 0 0 0,25 5 0 0 0,97 15 0 0 0,81 9 0 0 0,-233 7 0 0 0,227 4 0 0 0,-873-1 0 0 0,303-45 0 0 0,322 8 0 0 0,-134-9 0 0 0,453 21 0 0 0,1-9 0 0 0,-76-9 0 0 0,184 29 0 0 0,0 5 0 0 0,-114 10 0 0 0,34 9 0 0 0,15 0 0 0 0,-40-10 0 0 0,24-12 0 0 0,-22 2 0 0 0,-182-3 0 0 0,193 17 0 0 0,-33-14 0 0 0,64 4 0 0 0,163 4 0 0 0,-132 7 0 0 0,-68-7 0 0 0,114-8 0 0 0,-54-10 0 0 0,63 10 0 0 0,-90 4 0 0 0,120-3 0 0 0,-80-1 0 0 0,50-4 0 0 0,92 10-60 0 0,5 1-252 0 0,1 0-111 0 0,0 0-1358 0 0,0 0-5615 0 0,0 0-2407 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-74756.919">2545 13229 1376 0 0,'0'0'65'0'0,"0"1"-6"0"0,0 16 154 0 0,0-15 831 0 0,0-2 358 0 0,0 0 65 0 0,0 0-83 0 0,0 0-422 0 0,0 0-186 0 0,0 0-38 0 0,0 0-28 0 0,0 0-88 0 0,0 0-40 0 0,0 0-6 0 0,0 0 2 0 0,0 0 12 0 0,0 0 2 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0-1 0 0,0 8 1801 0 0,7 103 2520 0 0,1-8-2608 0 0,3 111-760 0 0,-11-2-472 0 0,39 55-113 0 0,-33-230-854 0 0,24 98-208 0 0,-2 67 1907 0 0,-14-79-2238 0 0,19 168 898 0 0,-37-179-286 0 0,-54 138-20 0 0,51-153-169 0 0,7-49-56 0 0,-3 9 374 0 0,-15 49-182 0 0,17-22-546 0 0,9-13 992 0 0,4-1-446 0 0,-10-64-106 0 0,0-5-17 0 0,-2-1-234 0 0,-7-18-3530 0 0,7 9 2303 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151003.08">2638 7365 4144 0 0,'0'0'319'0'0,"-6"1"252"0"0,6-2 2376 0 0,25-31-2360 0 0,-30 15 5029 0 0,5 16-5505 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-2 1 1 0 0,2-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 1 0 0,-2 1-112 0 0,-54 22 1284 0 0,16 1-659 0 0,-31 35 50 0 0,19-10-590 0 0,-100 121 107 0 0,50-41-21 0 0,6 2 334 0 0,15-6-252 0 0,-18 47-182 0 0,-57 140 566 0 0,141-276-548 0 0,-62 172 254 0 0,2 97-151 0 0,40-56 504 0 0,15-105-216 0 0,8 103 134 0 0,10-132-457 0 0,-3 106 104 0 0,14-111-187 0 0,6 1-1 0 0,16 57-73 0 0,5-9 269 0 0,28 64-269 0 0,-6-39 164 0 0,18 64 46 0 0,-16-72 888 0 0,67 134-1098 0 0,17 33 320 0 0,-100-229-133 0 0,24 44 186 0 0,-3-45 46 0 0,18 56-249 0 0,-14-25-191 0 0,-22-54 21 0 0,25 52 139 0 0,-38-56-22 0 0,-29-77-141 0 0,-4-7-107 0 0,0-2-69 0 0,0 0-21 0 0,0-3-260 0 0,0-9-1082 0 0,-4-4-465 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151703.08">1900 12924 13824 0 0,'-55'23'1677'0'0,"53"-22"-740"0"0,30-3 3060 0 0,6 0-4365 0 0,78 35 323 0 0,1 33 373 0 0,-11 8 165 0 0,123 101 1071 0 0,-198-158-1495 0 0,-1-2-1 0 0,1-2 0 0 0,0-1 0 0 0,3 0 1 0 0,22 5-69 0 0,72 11 245 0 0,-56-21 458 0 0,-53-17 147 0 0,-14 8-799 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 2-1 0 0,-1-1 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-2-51 0 0,0-4 176 0 0,-22-110 411 0 0,-21-83-1189 0 0,0 63-4384 0 0,23 86 2801 0 0,-5 9-21 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="152993.08">2853 13293 2760 0 0,'-8'-3'248'0'0,"-37"-30"6865"0"0,26 5-6498 0 0,-15-20 774 0 0,-3-5 1367 0 0,2-27 825 0 0,8 6-1573 0 0,19 18-676 0 0,-1-14-560 0 0,12-73 1085 0 0,20 4-1137 0 0,-13 90-1006 0 0,-13 6-1132 0 0,0 7-1456 0 0,5 34 1591 0 0,3 0-48 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="154173.08">5186 10046 14976 0 0,'-27'21'1597'0'0,"-13"-8"-1817"0"0,39-13 85 0 0,1 0-121 0 0,-9-1-614 0 0,-4-21 1632 0 0,4-14 143 0 0,-9-55 2063 0 0,-1-14-936 0 0,1-80-705 0 0,13-24-328 0 0,1 22-897 0 0,2-162 234 0 0,0-25 12 0 0,10 194-193 0 0,-1-120-36 0 0,-9 150-1315 0 0,30 87-2477 0 0,-19 50 2086 0 0,1-14-2513 0 0,-9 23 1999 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="154583.08">4458 8026 18887 0 0,'0'0'863'0'0,"-1"-1"-14"0"0,1-12-806 0 0,-1 2-1 0 0,2 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,2-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,1-1 0 0 0,-1 3 1 0 0,1-2-1 0 0,2-1-42 0 0,-2 0-42 0 0,134-197-129 0 0,-67 108 171 0 0,31-2 0 0 0,-92 93 2 0 0,-2 0-1 0 0,1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 0 1 0 0,1 2-1 0 0,0-1 0 0 0,7 0-1 0 0,-12 5 48 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 2 1 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0-1 0 0,-2 0 1 0 0,1 1 0 0 0,0 0-1 0 0,-2 1 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-2 1 0 0 0,1-1-1 0 0,-1 2-47 0 0,79 209 1312 0 0,-21-36-1200 0 0,-30-60-32 0 0,-2-31-402 0 0,5-39-2524 0 0,-24-46 814 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="156043.08">2450 14790 13040 0 0,'-3'6'1185'0'0,"-26"30"-737"0"0,2-29 563 0 0,-34-20 2664 0 0,27-4-2667 0 0,-42-17 867 0 0,39 15-1425 0 0,0 1 0 0 0,2-4 0 0 0,0-2-1 0 0,2 1 1 0 0,-15-16-450 0 0,-183-168 1230 0 0,197 171-981 0 0,-32-27-91 0 0,4-5 0 0 0,4-2 1 0 0,-4-9-159 0 0,-141-215 786 0 0,-96-173 150 0 0,196 259-915 0 0,12-4 1 0 0,7-4-1 0 0,-6-58-21 0 0,-69-193 160 0 0,73 173-160 0 0,-51-190-216 0 0,82 253 184 0 0,10-2 0 0 0,3-63 32 0 0,3-70-64 0 0,10 67 0 0 0,17 182 64 0 0,5-2 0 0 0,7-106 0 0 0,3 162 0 0 0,6-73 0 0 0,21-93 0 0 0,29-109-80 0 0,59-143-171 0 0,-8 148-223 0 0,-17 94 455 0 0,-52 150 70 0 0,6 3 0 0 0,2 2-1 0 0,10-7-50 0 0,-25 41 25 0 0,88-112 30 0 0,45-1-129 0 0,10 30-44 0 0,37-36-58 0 0,-164 127 134 0 0,87-62-842 0 0,-137 104 868 0 0,27-14-1611 0 0,-14 11-5936 0 0,-12 3 272 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="156463.08">1538 5857 11976 0 0,'0'0'922'0'0,"-1"-2"-600"0"0,-8-9-54 0 0,8 10 932 0 0,-1-8 2652 0 0,0-5-2353 0 0,6 11-1499 0 0,-1-2-1 0 0,1 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,1 1 0 0 0,2-1 1 0 0,19-11-106 0 0,99-29-209 0 0,-114 38 308 0 0,0 0-1 0 0,1 2 1 0 0,0-1-1 0 0,-1 1 1 0 0,2 1-1 0 0,-1 0 1 0 0,-1 1-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 2-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,2 1-1 0 0,-2 0 1 0 0,0 0-1 0 0,0 0 0 0 0,7 6 8 0 0,-8-3 12 0 0,0 1 0 0 0,-1 1-1 0 0,0 1 1 0 0,0-2 0 0 0,-1 3-1 0 0,0-1 1 0 0,5 10-12 0 0,-4-4 37 0 0,0 2 0 0 0,-1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-3 1 1 0 0,4 16-38 0 0,-4 85 434 0 0,-31-12 5 0 0,14-74-354 0 0,-51 118 75 0 0,-68 116-1810 0 0,119-243 551 0 0,-1 0-48 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="157893.08">9277 5655 13360 0 0,'-5'-1'271'0'0,"2"0"1"0"0,-2 0 0 0 0,1 0-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-2 1 0 0,0 1-272 0 0,-1-3 27 0 0,1 1 0 0 0,0-1 0 0 0,1 2-1 0 0,0-2 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,1-4-27 0 0,-1-7 302 0 0,-11-125 1863 0 0,-7-4-421 0 0,-6-144 624 0 0,6 51-1161 0 0,-13-343-614 0 0,24 336-593 0 0,-1 77-104 0 0,8 163 61 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0-1 43 0 0,2 8-62 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 62 0 0,-8 15-1775 0 0,2 4-289 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="158203.08">8509 3407 22607 0 0,'0'0'514'0'0,"-1"-2"71"0"0,-2 0-530 0 0,2 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1-55 0 0,13-16-19 0 0,0-2-1 0 0,-1 3 0 0 0,3-2 1 0 0,0 3-1 0 0,-1 0 1 0 0,3 0-1 0 0,-1 1 0 0 0,3 2 1 0 0,-1 0-1 0 0,3-1 20 0 0,24-19-44 0 0,-38 26-32 0 0,0 1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 2 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0-1 0 0,0 2 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 1 76 0 0,-5 2-16 0 0,-1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-2 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-2 0 0 0 0,1-1-1 0 0,0 2 1 0 0,0 0 16 0 0,56 136 542 0 0,-32-88-361 0 0,1-1 0 0 0,4-1 1 0 0,17 24-182 0 0,44 46-220 0 0,-50-63-1394 0 0,-22-36-78 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">22570 6625 0 0 0,'0'0'580'0'0,"0"0"-64"0"0,0 0 47 0 0,0 0-35 0 0,0 0-254 0 0,0 0-107 0 0,0 0-27 0 0,0 0 51 0 0,0 0 229 0 0,0 0 100 0 0,0 3 21 0 0,3 12 472 0 0,-3-13-554 0 0,0-2-3 0 0,0 0-54 0 0,0 0-223 0 0,0 0-98 0 0,0 0 51 0 0,0 0 272 0 0,0 0 95 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 0 0 0,0 7 0 0 0,0-8 0 0 0,0-1 0 0 0,0 0 36 0 0,0 0 150 0 0,0 0 66 0 0,0 0 18 0 0,0 0-29 0 0,0 6 436 0 0,2 53 2189 0 0,-4 64-643 0 0,-8-38-852 0 0,-7 70-1718 0 0,15-52-165 0 0,1-95 90 0 0,0 1-403 0 0,1 9-2730 0 0,-4-30-1033 0 0,-1 3-2741 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="208.461">22566 6684 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,7-4-112 0 0,1 1 125 0 0,-2 1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-346 0 0,45 71 1246 0 0,-49-67-1102 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0-2 0 0 0,0 1-1 0 0,-2 2 1 0 0,1-2-1 0 0,-1 2-143 0 0,2-3 57 0 0,-1-2 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-2-2 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-2 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,2-1 1 0 0,-3 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 0-57 0 0,-91-6-816 0 0,62-15-3738 0 0,27 13 2908 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55956.919">24026 16033 456 0 0,'22'-42'0'0'0,"-7"27"2824"0"0,-6 4 664 0 0,-8 11-2678 0 0,-1 0 44 0 0,0 0 11 0 0,0 0 6 0 0,0 0 21 0 0,0 0 85 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,3-22 2411 0 0,-17 3-1851 0 0,13 17-1397 0 0,-1-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-2-1 0 0,-1 2 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 1 0 0 0,-2 0-117 0 0,-3 2 139 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,-3 6-139 0 0,-18 35 224 0 0,-6 47 448 0 0,32 5 696 0 0,1-96-1368 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0 0 0 0,-2-1 16 0 0,1 0 1 0 0,1-1-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,1-1 1 0 0,-1 2-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-2 1 1 0 0,2 0-1 0 0,0-1 0 0 0,0 0-16 0 0,4 0-124 0 0,-1 0-1 0 0,2 0 0 0 0,-1-1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,1-1-1 0 0,-2 0 0 0 0,2 0 0 0 0,-2-2 0 0 0,2 1 0 0 0,-2 0 125 0 0,12-6-613 0 0,19-16-2912 0 0,-19 11 1494 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55516.919">24367 15714 5984 0 0,'3'-43'472'0'0,"-2"2"5162"0"0,-1 39-3819 0 0,0 2-663 0 0,0 0-288 0 0,0 0-58 0 0,0 0-20 0 0,0 0-61 0 0,0 0-21 0 0,0 0-7 0 0,-8 5 1975 0 0,-17 111 1356 0 0,-27 213-3264 0 0,28-146-640 0 0,8-28-1060 0 0,15-138-1236 0 0,1-12-5747 0 0,0-5 911 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55296.919">24312 15896 9216 0 0,'0'0'706'0'0,"0"0"-114"0"0,4-5 3675 0 0,19-10 1993 0 0,16 4-3644 0 0,12-4-1858 0 0,4 19-1979 0 0,-50 6-2143 0 0,-2-1 1389 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-66366.92">23037 15459 6304 0 0,'14'-1'822'0'0,"-14"0"-83"0"0,0 1 249 0 0,0 0 48 0 0,0 0-31 0 0,0 0-170 0 0,0 0-71 0 0,0 0-17 0 0,0 0-27 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0 48 0 0,0 0 202 0 0,0 0 87 0 0,0 0 20 0 0,0 0-70 0 0,0 0-308 0 0,-1-1-137 0 0,-48-67 1234 0 0,-30 3 383 0 0,74 62-1902 0 0,-2 0 0 0 0,1 1 1 0 0,2-1-1 0 0,-3 0 0 0 0,1 2 1 0 0,1-1-1 0 0,-2 1 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 1 1 0 0,-1 1-1 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,2 1 1 0 0,-7 2-14 0 0,-28 33 373 0 0,8 1-682 0 0,-13 59 985 0 0,27-17-666 0 0,-1 45 460 0 0,16 10-108 0 0,13-13-298 0 0,19 16-7518 0 0,-26-132 13 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-66056.919">22584 15862 11976 0 0,'0'0'546'0'0,"4"-11"204"0"0,14 5 2195 0 0,36-9 2019 0 0,25-2-3091 0 0,-37 20-1743 0 0,0 1 0 0 0,-1 0 1 0 0,27 9-131 0 0,-21 1-3223 0 0,-33-10 2016 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-65316.919">23086 16078 920 0 0,'1'-3'80'0'0,"-1"2"-114"0"0,9-21 1775 0 0,19-25 8599 0 0,-13 37-9435 0 0,-2 2-70 0 0,-11 6-714 0 0,0 1 1 0 0,1 0-1 0 0,-1-2 1 0 0,-1 1 0 0 0,2 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,0 0 1 0 0,1 0-1 0 0,1 2-121 0 0,30 31 1528 0 0,-17 31 812 0 0,-18-57-2114 0 0,0-1 0 0 0,-1 3 0 0 0,-1-2 0 0 0,1 0 0 0 0,0 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-3-1 0 0 0,1 0-226 0 0,-1-3 108 0 0,2 1 0 0 0,-1 0-1 0 0,0-1 1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,2-1 0 0 0,-2 1 0 0 0,2-1-1 0 0,-2 0 1 0 0,0 1 0 0 0,1-1-1 0 0,0-1 1 0 0,-6 1-108 0 0,6-3-56 0 0,2 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,2-1 1 0 0,-2 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1-2-1 0 0,0 2 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1 0 0 0,-2-1-1 0 0,2-1 1 0 0,-1 2 0 0 0,1-2-1 0 0,0 1 1 0 0,0-2 56 0 0,1-36-2485 0 0,3 23 635 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-57246.919">23427 15892 9616 0 0,'0'0'216'0'0,"0"0"32"0"0,1-2 12 0 0,9-23 16 0 0,8-32 4156 0 0,-18 55-3764 0 0,0 2 151 0 0,0 0 69 0 0,0 0 10 0 0,0 0-48 0 0,0 0-216 0 0,0 0-98 0 0,0 0-22 0 0,-8 62 3070 0 0,4-6-2456 0 0,-12 163 920 0 0,16-150-2048 0 0,-1-23-64 0 0,1-45-273 0 0,0-1-138 0 0,0 0-33 0 0,0 0-217 0 0,0-8-2919 0 0,1-4 1541 0 0,2-1-9 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-56836.919">23370 16043 10136 0 0,'0'0'42'0'0,"0"1"-1"0"0,0-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,2 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-42 0 0,30-34 4246 0 0,11 4-1699 0 0,-37 26-2345 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,2 0-202 0 0,29 19 1351 0 0,-32-12-1230 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 2 0 0 0,-1-2 0 0 0,-1 1 0 0 0,2 5-121 0 0,23 82 144 0 0,-16 2-545 0 0,-19-81-269 0 0,5-10-1904 0 0,0-4-3466 0 0,0 0-762 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45426.919">24658 16075 456 0 0,'10'-3'13004'0'0,"-5"12"-6955"0"0,-9 20-4332 0 0,2-13-273 0 0,7 100-283 0 0,-3-75-2968 0 0,0 0-3416 0 0,-2-41-2002 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45206.919">24739 15707 5984 0 0,'0'0'273'0'0,"0"0"-5"0"0,0 0 121 0 0,0 0 1143 0 0,0 0 514 0 0,0 0 104 0 0,0 0-119 0 0,0 0-596 0 0,0 0-261 0 0,0 0-49 0 0,0 0-98 0 0,0 0-392 0 0,0 0-171 0 0,0 0-31 0 0,0 0-64 0 0,0 0-1670 0 0,0 0-5837 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44826.919">24879 16349 11232 0 0,'0'-5'1016'0'0,"-18"-78"3747"0"0,28 13-109 0 0,-7 62-4545 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,-2 2 0 0 0,3-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-2 3 0 0 0,2-1 0 0 0,3-1-109 0 0,-7 3 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2 0 0 0 0,14 40 10 0 0,-16-31 52 0 0,-7 49 1898 0 0,-34 28-1744 0 0,35-85-173 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-2 0 0 0,-2 2-1 0 0,2-1 1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-5-1-43 0 0,3-1-36 0 0,-2 1 0 0 0,1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-2 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,2 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-4 36 0 0,5-34-2989 0 0,1 24 1539 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-43876.919">25282 16126 456 0 0,'0'0'83'0'0,"0"0"42"0"0,0 0 131 0 0,0 0 32 0 0,0 0 0 0 0,0 0 49 0 0,0 0 209 0 0,0 0 94 0 0,0 0 21 0 0,0 0-5 0 0,0 0-33 0 0,0 0-14 0 0,0 0-1 0 0,0 0-74 0 0,0 0-307 0 0,0 0-135 0 0,0-1-36 0 0,9-37 684 0 0,-1-5 547 0 0,-5 18-691 0 0,-3-25 2561 0 0,0 49-2790 0 0,0 1 1 0 0,0 0 0 0 0,0 7 8134 0 0,-3 26-7718 0 0,-11 125 1476 0 0,0-85-2207 0 0,14-64-53 0 0,0-4-32 0 0,0-3-137 0 0,0-2-71 0 0,0 0-16 0 0,0 0-147 0 0,0 0-589 0 0,0 0-257 0 0,0 0-51 0 0,0 0-35 0 0,0 0-102 0 0,2 15-5517 0 0,-2-15 5738 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-43576.919">25288 16167 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,0 0-140 0 0,0 0 368 0 0,0 0 187 0 0,0 0 42 0 0,-6-6 963 0 0,5 2-1582 0 0,1-1 1 0 0,0-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 2 0 0 0,0-2 0 0 0,-1 1 1 0 0,1 2-1 0 0,1-2 0 0 0,-1 0 0 0 0,4-3-240 0 0,-6 6 154 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,-1-1-153 0 0,7 4 222 0 0,18 14-38 0 0,-4 10-184 0 0,-20-24 130 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,0-1 1 0 0,0 2-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 4-130 0 0,2 34 130 0 0,3-18-130 0 0,0-20-97 0 0,22-10-2811 0 0,-19 1 1087 0 0,1-3-377 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1576.986">22100 6526 4608 0 0,'0'0'353'0'0,"5"10"155"0"0,-3-6 2425 0 0,9 28 3145 0 0,-9-10-3733 0 0,-11 23 1085 0 0,0 15-1742 0 0,3-7-736 0 0,11 43-312 0 0,-9-16-640 0 0,8-23 0 0 0,-16-9 0 0 0,12-43-9 0 0,0 0-146 0 0,0 0-4162 0 0,0-5-2729 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-759.69">22086 6825 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,4-4 272 0 0,0 2 2425 0 0,9-13-1132 0 0,7 6-314 0 0,-19 9-1141 0 0,9-11 879 0 0,27-21 835 0 0,9 16-867 0 0,-45 16-985 0 0,7-2 305 0 0,40 13-1282 0 0,-38-4 625 0 0,-8 28 186 0 0,-5 2 15 0 0,-1-9 170 0 0,-3 12-74 0 0,5-39-411 0 0,2-1-12 0 0,0 0 37 0 0,3 10 308 0 0,15 9-12 0 0,-17-18-372 0 0,7 17-262 0 0,-2 9-1153 0 0,-5-26 785 0 0,-1-1-831 0 0,0 0-363 0 0,0 0-70 0 0,0 0-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2740.813">21637 6653 2304 0 0,'2'0'473'0'0,"3"-1"1939"0"0,-5 7 6695 0 0,-1-1-5123 0 0,2 2-5610 0 0,-4 32 3901 0 0,5 2 62 0 0,5 57-84 0 0,6 4-1147 0 0,-3-11 156 0 0,-10 11-32 0 0,-10 12-700 0 0,12-100-583 0 0,-2-13-216 0 0,0-1-65 0 0,0-3-2 0 0,2-34-3313 0 0,-6 25 1834 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2395.418">21658 6677 6912 0 0,'-11'-8'528'0'0,"28"-1"-128"0"0,7-10 4668 0 0,33 17 409 0 0,-53 2-5324 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 2 0 0 0,0-2 0 0 0,0 0 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,1 2-153 0 0,33 70 2062 0 0,-23 7-1603 0 0,-14-3 1130 0 0,0-72-1534 0 0,-3 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,-2-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,2-2 0 0 0,-1 1 1 0 0,-2 0-1 0 0,1 1 0 0 0,-1-2 0 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 0 0 0,-1 1-55 0 0,-25 6 67 0 0,30-11-206 0 0,-2 0-58 0 0,-2 0-1 0 0,3-1 1 0 0,-3 1 0 0 0,2-1-1 0 0,0 0 1 0 0,-2 0-1 0 0,2-1 1 0 0,0 1 0 0 0,0-2-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,2-2-1 0 0,-1 1 1 0 0,0-1-1 0 0,-1-1 198 0 0,-5-5-5692 0 0,-5-1-1767 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="75099.81">3322 14611 7488 0 0,'0'2'340'0'0,"-6"99"3520"0"0,12 113 4791 0 0,-5 32-4784 0 0,6-63-3019 0 0,4-73-648 0 0,1-66-288 0 0,-12-42-387 0 0,0-2-33 0 0,0 0-192 0 0,0 0-790 0 0,0-5-352 0 0,2-20-70 0 0,-2-4-7 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="75669.811">3370 14709 8288 0 0,'-4'17'381'0'0,"3"-14"-6"0"0,9-35-227 0 0,-7 16 279 0 0,2 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,1-1 0 0 0,0 2 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 2 0 0 0,7-7-427 0 0,-10 13 230 0 0,1-2 0 0 0,0 2 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,2 1 0 0 0,1 0-230 0 0,54-2 1008 0 0,-57 5-919 0 0,0 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0-1 0 0,-2 2 1 0 0,4 2-89 0 0,2 5 277 0 0,-2 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 2 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 8-277 0 0,10 86 608 0 0,-11-95-471 0 0,-1-2-1 0 0,1 2 1 0 0,-2 0-1 0 0,0-2 1 0 0,1 0-1 0 0,-3 1 1 0 0,1 0 0 0 0,-1 1-1 0 0,-2-4 1 0 0,1 3-1 0 0,0-1 1 0 0,-2 1-1 0 0,0-3 1 0 0,-1 2-1 0 0,0 1-136 0 0,-1-5 0 0 0,2-1 0 0 0,-2-1 0 0 0,-1 0 0 0 0,3 1 0 0 0,-3-2 0 0 0,1 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-2 0 0 0,1-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,-4 0 0 0 0,-11 8 0 0 0,-27 0 0 0 0,42-13-8 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,2-1 0 0 0,-1-2 0 0 0,0 1 1 0 0,3-1-1 0 0,-4-1 8 0 0,-25-49-411 0 0,31 56 334 0 0,3 1 10 0 0,0 0 3 0 0,0 0 0 0 0,12 5-105 0 0,-7-1 109 0 0,2 0 0 0 0,-1-1 0 0 0,-2 2 0 0 0,3 1 0 0 0,-2-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0 2 60 0 0,17 22-246 0 0,41 56 1336 0 0,-38-53-896 0 0,1-3 0 0 0,0 1 1 0 0,3-2-1 0 0,8 6-194 0 0,-16-15-3 0 0,73 46-2666 0 0,-77-58 1330 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="85949.811">4158 15263 920 0 0,'0'0'327'0'0,"0"0"1035"0"0,0 9 2340 0 0,-1-6-656 0 0,-1 23 2742 0 0,7-12-4840 0 0,-3-12-526 0 0,-2-2-26 0 0,0 0 12 0 0,0 0 68 0 0,0 0 32 0 0,1 1 4 0 0,45 6 1536 0 0,-7-3-1138 0 0,19-63-236 0 0,28-34 437 0 0,-47 21-618 0 0,-18 7-757 0 0,-21 63 329 0 0,1 0-31 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 1-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-2 1 0 0,-1 2-1 0 0,2 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1-34 0 0,-6 0 41 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 1 0 0 0,3 0-1 0 0,-3 0 1 0 0,1 0 0 0 0,1 2-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1-1 0 0,-3 0-40 0 0,-21 14 98 0 0,22-14-115 0 0,-1-1 0 0 0,1 2 0 0 0,0 0 0 0 0,2 1-1 0 0,-2 0 1 0 0,0 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 1 0 0 0,2-3 0 0 0,-3 5 17 0 0,-17 42 618 0 0,15 24-194 0 0,26 33-1082 0 0,-14-101 704 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,2 1 1 0 0,1 0 0 0 0,-2-1 0 0 0,1-2-1 0 0,0 2 1 0 0,1-1 0 0 0,0 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1-1 0 0,2-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,0-2 1 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0-1 0 0,2-2 1 0 0,2 1-47 0 0,40-6-792 0 0,-50 5 622 0 0,2 0-1 0 0,-2 2 1 0 0,1-2-1 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0-2-1 0 0,-1 2 1 0 0,2 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,2-1-1 0 0,-2 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-2 170 0 0,13-10-5654 0 0,-3 8-1513 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="87029.81">4991 14903 1376 0 0,'0'0'65'0'0,"0"0"287"0"0,0 0 1184 0 0,0 0 522 0 0,0 0 100 0 0,0 0-171 0 0,0-16 1609 0 0,17-85 4054 0 0,-9 72-6749 0 0,-8 26-797 0 0,0-4-41 0 0,0 6-160 0 0,0 1-19 0 0,0 0 92 0 0,0 0 344 0 0,0 0 154 0 0,0 0 34 0 0,0 0-97 0 0,0 0-403 0 0,0 0-59 0 0,0 0 127 0 0,0 0 15 0 0,0 0 21 0 0,0 0 128 0 0,0 1 59 0 0,-8 71 675 0 0,-14 52-478 0 0,10-30-496 0 0,1 80 642 0 0,10 80-1033 0 0,-2-173 1100 0 0,-5-20-1141 0 0,8-59 208 0 0,-6 0-1960 0 0,5-1 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="87299.81">4974 15018 12696 0 0,'11'-13'1376'0'0,"38"6"1778"0"0,13-3 1363 0 0,2 1-3125 0 0,3 22-1540 0 0,-44-6-2470 0 0,-17-1-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="204899.81">6074 15361 8288 0 0,'13'-33'1072'0'0,"27"-2"4316"0"0,-36 34-5186 0 0,1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,-1 2 1 0 0,2-1 0 0 0,-2 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-3 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-2 2 0 0 0,1 2-203 0 0,3 3 280 0 0,-1 1 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 1 0 0 0,-1-2 1 0 0,0 8-281 0 0,-1-11 347 0 0,2-5-303 0 0,-1 0 0 0 0,0-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1-44 0 0,1 0 8 0 0,-1-2 0 0 0,2 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-2 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-2 0 1 0 0,2-1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,2-1-1 0 0,0 0 1 0 0,-2 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-2-2-8 0 0,-3-3-53 0 0,0 1 0 0 0,1-1 0 0 0,1-2 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 1 0 0,1-2-1 0 0,0 2 0 0 0,1-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-3-5 53 0 0,5 11-246 0 0,-1-3 1 0 0,2 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,1 1-1 0 0,-1-2 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,0-2 1 0 0,-1 2 0 0 0,1-2 245 0 0,11-26-3579 0 0,-5 17-2927 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="203719.8109">5482 15129 3224 0 0,'0'-2'240'0'0,"0"-1"25"0"0,0 2 855 0 0,0 1 359 0 0,0 0 66 0 0,0 0-81 0 0,0 0-397 0 0,0 0-178 0 0,0 0-32 0 0,0 0-13 0 0,0 0-24 0 0,0 0-10 0 0,0 0-2 0 0,0 0-18 0 0,0 0-74 0 0,5 30 1869 0 0,-12 148 1427 0 0,-6 4-2668 0 0,8-90-1106 0 0,5-91-198 0 0,0 19-364 0 0,0-20 191 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 134 0 0,3-14-2091 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="204089.8109">5498 15266 8288 0 0,'3'9'2948'0'0,"4"-25"1960"0"0,-2 6-5020 0 0,30-38 3418 0 0,17-6-299 0 0,-49 52-2908 0 0,0 1 0 0 0,0-2 0 0 0,1 2 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-3 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,-1 0-99 0 0,22 31 274 0 0,19 33 16 0 0,-2-8-146 0 0,-12-20 0 0 0,-25-26-597 0 0,-3-10-3304 0 0,-2-2 2223 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35574.03">18789 6660 11888 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 14 0 0,1 10 69 0 0,-2 75 4760 0 0,-6-15-2346 0 0,7-31-2146 0 0,-1-35-594 0 0,-3 29-145 0 0,2-22-10 0 0,1-9-188 0 0,1-2-789 0 0,0 0-344 0 0,0 0-65 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35139.5208">19054 6663 2304 0 0,'-3'1'3435'0'0,"8"5"13324"0"0,-3-4-18570 0 0,12 97 5563 0 0,0 27-2624 0 0,-5-51-1128 0 0,-7-66-133 0 0,-1-8-563 0 0,-1-1-257 0 0,0 0-922 0 0,0 0-3642 0 0,0 0-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-34747.75">19072 6791 1840 0 0,'0'0'83'0'0,"0"0"373"0"0,0 0 1526 0 0,0 0 670 0 0,0 0 131 0 0,3-1 950 0 0,8-6-2192 0 0,8-24 2196 0 0,-3 12-2845 0 0,-14 14-638 0 0,2 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,-1 1 1 0 0,6-2-254 0 0,20 16 16 0 0,-24-8-15 0 0,45 51 773 0 0,-46-47-785 0 0,-4-7-105 0 0,13 4-2683 0 0,-14-5 751 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44644.387">18129 6475 3224 0 0,'-1'0'2310'0'0,"0"1"10093"0"0,0 0-11285 0 0,1 2-3278 0 0,-15 170 7048 0 0,-9 34-3120 0 0,19-148-1645 0 0,7 49-583 0 0,1-101 325 0 0,-3-7-3458 0 0,0 0 1850 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44417.2638">18062 6551 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,2 0-220 0 0,56 3 3130 0 0,53 24-834 0 0,-55-20-4427 0 0,-54-7-69 0 0,5 0-4147 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36024.581">18390 6897 2304 0 0,'0'0'348'0'0,"0"0"620"0"0,-8-5 2737 0 0,3-54-382 0 0,5 58-2754 0 0,-8-17 2487 0 0,3-42 2906 0 0,6 54-5754 0 0,-1 1-1 0 0,3 1 0 0 0,-2-2 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,0-2-1 0 0,-1 1 1 0 0,1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1-2-207 0 0,-3 4-36 0 0,2-1 14 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1-1 0 0 0,0 2 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,3 0 23 0 0,-4 0 21 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 2 0 0 0,2-1 1 0 0,-1 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,2 1-1 0 0,-3 0 0 0 0,1-1 1 0 0,2 2-1 0 0,-2 0 0 0 0,1-2 1 0 0,-1 1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0-21 0 0,0 5 5 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 2 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-2 5-5 0 0,2-4 151 0 0,-1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,2 1-1 0 0,-3-1 1 0 0,0 1-1 0 0,0-3 1 0 0,-1 2-1 0 0,0 0 1 0 0,1-1-1 0 0,-4 3-151 0 0,6-7 28 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 2 1 0 0,-1-2-1 0 0,0-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-2 0 1 0 0,2 1-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-2-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1-1-27 0 0,-4-2-27 0 0,1-3-1 0 0,1 2 0 0 0,-2-1 1 0 0,2 0-1 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,1 0 1 0 0,0-2-1 0 0,0 3 0 0 0,1-1 1 0 0,-1-1-1 0 0,1-1 1 0 0,1 0 27 0 0,-5-55-3584 0 0,10 58 2142 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33796.383">19417 6891 456 0 0,'0'0'2349'0'0,"0"0"293"0"0,0 0 128 0 0,0 0-221 0 0,0 0-1013 0 0,0 0-448 0 0,0 0-89 0 0,0 0-30 0 0,5 7 1768 0 0,-2-4-2425 0 0,1-1 0 0 0,-1-1 0 0 0,0 2 0 0 0,0-1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,3 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,0 0-312 0 0,56-6 2120 0 0,4-21-1296 0 0,-5-17-672 0 0,-23 0 656 0 0,-15-26-516 0 0,-36 14-160 0 0,13 53-153 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 2-1 0 0,1-1 1 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,1-1-1 0 0,-4 2 22 0 0,-3 4 44 0 0,2 2 0 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 2 0 0 0,-5 8-44 0 0,1-3 32 0 0,0 4-32 0 0,1 1 0 0 0,0-3 0 0 0,2 2 0 0 0,-1 1 0 0 0,4-1 0 0 0,-3 8 0 0 0,4-20 8 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 0-1 0 0,2 0 1 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,4 8-8 0 0,10 4 88 0 0,42-11-2149 0 0,-21-14-6089 0 0,-22 2 1076 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33464.079">19893 6888 13824 0 0,'0'0'314'0'0,"-7"7"872"0"0,1 11-891 0 0,5-12 1764 0 0,-1-4 3765 0 0,8-3-5807 0 0,8-6-1723 0 0,-6 1-236 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-28557.543">18833 6421 4144 0 0,'0'0'319'0'0,"0"0"295"0"0,0 0 2022 0 0,0 0 904 0 0,0 0 185 0 0,0 0-408 0 0,0 0-1846 0 0,0 0-815 0 0,0 0-161 0 0,0 0-25 0 0,0 0 16 0 0,0 0 8 0 0,0 0 2 0 0,0 0-64 0 0,0 0-1313 0 0,0 0-4508 0 0,0 0-1916 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19052.7189">20155 6627 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 6 160 0 0,3-4 8708 0 0,20 88-4943 0 0,-16 5-3675 0 0,-13-10-98 0 0,9-77-623 0 0,0-7-63 0 0,0-1-165 0 0,0 0-726 0 0,0 0-316 0 0,0 0-65 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-9426.743">20428 6509 920 0 0,'1'-1'67'0'0,"0"-4"143"0"0,0 5 814 0 0,-1 0 355 0 0,0 0 70 0 0,0 0 5373 0 0,0 4-3378 0 0,0 18-2234 0 0,12 166 4151 0 0,-9-33-3309 0 0,0-105-1683 0 0,0-31-1984 0 0,-1-2-3835 0 0,-2-17 3608 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-8994.302">20428 6677 3224 0 0,'0'7'527'0'0,"10"-32"8375"0"0,7-1-6343 0 0,-15 23-2627 0 0,0-2 178 0 0,1 0 0 0 0,0 1 0 0 0,-2 0 0 0 0,3 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,1-1 0 0 0,-3 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 0-110 0 0,19 32 453 0 0,1 11 891 0 0,-18-26-1051 0 0,0 58 781 0 0,9 8 131 0 0,-6-38-1044 0 0,9-14-3885 0 0,-18-30 1631 0 0,-1-2-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7909.834">21028 6612 2760 0 0,'0'0'395'0'0,"0"0"617"0"0,0 0 274 0 0,0 0 53 0 0,0 0-86 0 0,0 0-380 0 0,0 0-163 0 0,0 0-36 0 0,0 0-28 0 0,0 0-85 0 0,6 0 260 0 0,-5-1 2703 0 0,-1 0-3426 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-98 0 0,-10 0 483 0 0,-30 7 677 0 0,-1 20-16 0 0,40-25-1069 0 0,-2 1-1 0 0,2-2 0 0 0,1 2 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-2-1 0 0,0 1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 1 0 0 0,0-2 1 0 0,0 0-1 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 0 0 0,4 4-74 0 0,27 86 784 0 0,-18-66-634 0 0,-11-22-112 0 0,2-1 0 0 0,-2 0 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,1-1-38 0 0,-3-1-114 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 1 0 0 0,0-2-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-3 0-1 0 0,3 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,2-1 114 0 0,5-1-2547 0 0,0-4-5195 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7043.897">21275 6949 7112 0 0,'15'0'324'0'0,"-11"0"-4"0"0,-4 0-94 0 0,0 0 380 0 0,0 0 186 0 0,0 0 37 0 0,0 0 35 0 0,0 0 107 0 0,0 0 42 0 0,0 0 10 0 0,0 0-26 0 0,0 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-58 0 0,0 0-240 0 0,0 0-102 0 0,0 0-17 0 0,0 0-25 0 0,0 0-82 0 0,0 0-40 0 0,0 0-5 0 0,0 0-26 0 0,0 0-108 0 0,0 0-42 0 0,1-19-240 0 0,15 1 132 0 0,-16 17-8 0 0,0 1 88 0 0,0 0 35 0 0,0 0-18 0 0,-1 1-1 0 0,-1 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,2-1 0 0 0,-2 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0-67 0 0,1 1-279 0 0,-1-2-186 0 0,0 0-42 0 0,0 0-209 0 0,0 0-857 0 0,0 0-379 0 0,0 0-80 0 0,0 0-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2101.423">20162 6276 13304 0 0,'0'0'605'0'0,"0"0"-9"0"0,0-1-381 0 0,-2-3-42 0 0,1 2 600 0 0,1 2 260 0 0,0 0 45 0 0,0 0-26 0 0,0 0-144 0 0,0 0-63 0 0,-4 21 1994 0 0,14-14-5523 0 0,-8-7-4821 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122096.968">3851 803 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-120 0 0,0 0 193 0 0,-4-8 582 0 0,-46-23 3117 0 0,23 18-1623 0 0,-47-16-841 0 0,62 26-1311 0 0,3 1-1 0 0,-2 1 0 0 0,-1-2 1 0 0,1 3-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 2-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 2-1 0 0,2 1 0 0 0,-11 5-284 0 0,16-8 41 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 2-1 0 0,-2-2 1 0 0,2 0-1 0 0,1 0 1 0 0,-2 1 0 0 0,1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,0-1 1 0 0,1-1-1 0 0,-1 2 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 2-40 0 0,6 9 100 0 0,0-1 0 0 0,1 0 0 0 0,1-2 0 0 0,0 2 0 0 0,0-2 0 0 0,2 1 0 0 0,-2-2 0 0 0,4 0 0 0 0,-3 0 0 0 0,3-1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1-100 0 0,-7-6 32 0 0,68 83-590 0 0,-61-69 602 0 0,0 1 1 0 0,-3-1-1 0 0,2 2 1 0 0,-3-1 0 0 0,1 0-1 0 0,-2 3 1 0 0,-1 0-1 0 0,0-2 1 0 0,0 1-1 0 0,-3 2 1 0 0,0-3 0 0 0,0 3-1 0 0,-2-2 1 0 0,0 2-1 0 0,-1 0 1 0 0,-3 19-45 0 0,0-26 91 0 0,1-2 1 0 0,0 2-1 0 0,-2-2 1 0 0,0 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-2-1-1 0 0,0-1 1 0 0,0-1-1 0 0,-3 4-91 0 0,7-10 67 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,1-1 0 0 0,-1 2 0 0 0,2-2 0 0 0,-3 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 1 0 0,-6-2-68 0 0,7 0 4 0 0,-2 0 0 0 0,0 0 0 0 0,3-2 0 0 0,-3 1 0 0 0,1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0-5-4 0 0,-2 0-603 0 0,0 1 1 0 0,2 0-1 0 0,0-3 0 0 0,-1 1 1 0 0,2-1-1 0 0,0 1 1 0 0,1 1-1 0 0,-1-4 603 0 0,-4-12-1535 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122485.17">3743 532 13680 0 0,'0'0'306'0'0,"-5"7"421"0"0,-1 7-534 0 0,-2-1-1 0 0,2 2 1 0 0,2-2-1 0 0,-2 2 1 0 0,2-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 12-193 0 0,0-4 459 0 0,-10 64 963 0 0,3 2 0 0 0,5 0 0 0 0,3-2 0 0 0,5 59-1422 0 0,-11 66 1773 0 0,-6-13-700 0 0,0 109-1515 0 0,17-246-1557 0 0,-1-34 952 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="142634.009">4193 1572 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 0 0 0 0,0 0 200 0 0,0 0 24 0 0,-2-7 8 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="185244.55">4340 1930 1376 0 0,'0'0'65'0'0,"0"0"321"0"0,0 0 1322 0 0,0 0 578 0 0,0 0 119 0 0,-2 2 764 0 0,-6 7-2143 0 0,7-9-849 0 0,0 1 1 0 0,0 0-1 0 0,-2 0 1 0 0,2-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,-2 0 1 0 0,2 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,0-2 1 0 0,0 2-1 0 0,-2-1 0 0 0,2 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1-177 0 0,-13-12 1364 0 0,1-25 743 0 0,14 3-644 0 0,-12-26-661 0 0,12 39-733 0 0,0 2-1 0 0,2-1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 2 0 0 0,2-2-1 0 0,0 1 1 0 0,1 0-1 0 0,1 2 1 0 0,1 0-1 0 0,1-1 1 0 0,8-10-69 0 0,-8 10-213 0 0,25-26 417 0 0,-33 44-216 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,0 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,0 1 1 0 0,0-1 11 0 0,26 11-403 0 0,-13-10 372 0 0,1 11 529 0 0,-3-3 172 0 0,-10-7-605 0 0,2 1-1 0 0,-2 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-3 1 0 0 0,1 3-64 0 0,12 25-60 0 0,1 50 132 0 0,-7-46-67 0 0,-6-33 15 0 0,1 2 1 0 0,-1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 2 0 0 0,-2 4-20 0 0,-6 16 568 0 0,8-27-650 0 0,-3 7-326 0 0,3-8 412 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-4 0 0,-2-26 743 0 0,16-40-633 0 0,-2 29-110 0 0,13-32 0 0 0,23-16-320 0 0,-17 45-430 0 0,1 9 1668 0 0,11 3-918 0 0,-38 25-7 0 0,-2 2-32 0 0,0 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-3-1-1 0 0,2 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 2 1 0 0,-1-1 38 0 0,-1-2 222 0 0,14 17 286 0 0,1 12-904 0 0,-3 23 920 0 0,-3 11-181 0 0,-6-24 197 0 0,-4 35-687 0 0,0-38 334 0 0,25 36-102 0 0,6-11-74 0 0,-29-57 31 0 0,2 0-20 0 0,28-6 135 0 0,-13-12 0 0 0,5-10-434 0 0,5-17 434 0 0,-20 23-314 0 0,4-1 685 0 0,4-12-776 0 0,-16 30 365 0 0,-1 1-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0 39 0 0,0 0 168 0 0,4-13-278 0 0,-3 10-5968 0 0,0 2-1741 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="186134.947">5432 1684 11288 0 0,'0'0'514'0'0,"-10"-9"196"0"0,8 7-539 0 0,1 0 0 0 0,-1 0 0 0 0,1-2 0 0 0,0 2 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-171 0 0,39-46 2046 0 0,-30 39-1874 0 0,-6 7-154 0 0,-2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,0 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,2 0-18 0 0,-2 0 60 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-2 0 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 2 0 0 0,2-2 0 0 0,-1 1 0 0 0,0 1-60 0 0,-1 2 134 0 0,10 74 1428 0 0,-14-55-1106 0 0,-13 40 934 0 0,14-61-1313 0 0,0 0 0 0 0,-2-1 1 0 0,2 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,-5 2-77 0 0,-26-4 728 0 0,20-4-305 0 0,13 4-401 0 0,1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-3 1 1 0 0,2-1-1 0 0,0 1 1 0 0,0-2-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-2-1 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2-2 1 0 0,-1 2-1 0 0,0 0 1 0 0,0-2-22 0 0,-1-2-121 0 0,1 1 0 0 0,0 0 0 0 0,1-2 0 0 0,0 2 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-2 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 1 0 0 0,2 0 121 0 0,24-46-8730 0 0,-13 29 1471 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="195187.748">5958 1403 456 0 0,'-6'21'336'0'0,"-1"-3"10502"0"0,6-13-10470 0 0,1 54 5149 0 0,0 21-1998 0 0,12 53-1146 0 0,6-59-2293 0 0,14-25 752 0 0,-3-10-288 0 0,-22-32-468 0 0,3-6 16 0 0,31-4 116 0 0,8-23 32 0 0,-3-33-153 0 0,-16 14-38 0 0,-2 5-49 0 0,-6 14 0 0 0,14-38 64 0 0,-11 28-74 0 0,-16 26-44 0 0,4-21 54 0 0,-3 20 28 0 0,-3-8-2 0 0,2-4-69 0 0,-8 22 96 0 0,-3 20-9 0 0,-10 59-144 0 0,8-7 100 0 0,1-41 0 0 0,3 21 0 0 0,-8 43 254 0 0,-11-1-28 0 0,-11 30 293 0 0,6-57 286 0 0,17-42-797 0 0,-2 2 0 0 0,0-2 1 0 0,-3 1-1 0 0,1-2 0 0 0,-2 1 0 0 0,-7 8-8 0 0,9-16 52 0 0,0-2-1 0 0,-1 0 1 0 0,1 0-1 0 0,-3 0 1 0 0,2-3-1 0 0,-2 0 0 0 0,-4 4-51 0 0,11-9 15 0 0,-1-1-1 0 0,2 1 0 0 0,-2-1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,2-1 0 0 0,-2 1 1 0 0,1-2-1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,-1-2-14 0 0,7 1-35 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1-1-1 0 0,-2 2 1 0 0,2 0 0 0 0,0-3 34 0 0,-1-1 20 0 0,10-81-2121 0 0,-9 53-659 0 0,0 20 1197 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="196354.103">6597 1787 1840 0 0,'1'-1'138'0'0,"-1"0"0"0"0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,2-1-1 0 0,-2 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1-138 0 0,15 0 3296 0 0,38-8 1940 0 0,-35 1-4448 0 0,60-28 1921 0 0,-16-19-1408 0 0,-53 40-1068 0 0,-8 10-211 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-2 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0-1-21 0 0,-1 1 9 0 0,0-3 1 0 0,0 2-1 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 2 0 0 0,3-1 1 0 0,-2 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-5-1-9 0 0,-4-5-199 0 0,11 7 228 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0 1-1 0 0,-4-1-28 0 0,-14 4 307 0 0,18-4-243 0 0,-2 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-1 4-64 0 0,0 3 118 0 0,-4 2 3 0 0,2 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,3-1 0 0 0,-1 2 0 0 0,0 0 1 0 0,1-2-1 0 0,1 3 0 0 0,1 1 0 0 0,-1-3 1 0 0,2 1-1 0 0,0 7-121 0 0,1-9 43 0 0,1-2-1 0 0,0-1 1 0 0,1 1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,1 0 0 0 0,-1-1 0 0 0,3 6-43 0 0,3-1 29 0 0,28 21 88 0 0,-29-28-139 0 0,0-2-1 0 0,0 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 0 1 0 0,-1-1-1 0 0,0 0 0 0 0,-1-1 1 0 0,2 0-1 0 0,-1 0 0 0 0,2-1 23 0 0,56-5-3801 0 0,-46 6 2362 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="198120.726">7193 1437 4832 0 0,'2'66'3666'0'0,"1"-45"-222"0"0,-1-20-2786 0 0,-4 35 2622 0 0,4 73 551 0 0,-2-44-3103 0 0,0 46 110 0 0,0-39-4281 0 0,0-70-1079 0 0,0-2-1230 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="198513.93">7183 1708 3680 0 0,'0'0'284'0'0,"0"-1"-187"0"0,0-2 155 0 0,2-12 5681 0 0,7-11-2141 0 0,-3 13-2532 0 0,-5 9-1000 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 1 1 0 0,0-2-1 0 0,1 1 0 0 0,-2 1 1 0 0,1-1-1 0 0,1 2 0 0 0,0-1 1 0 0,1 0-260 0 0,29-20 850 0 0,-31 22-780 0 0,1 0 0 0 0,-2 1 0 0 0,0-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1-70 0 0,31 32 293 0 0,32 46 1327 0 0,-68-80-1617 0 0,3 4 19 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1-2 1 0 0,-1 2 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 2-22 0 0,11 57 581 0 0,-19-35-1430 0 0,6-21-1922 0 0,-3 0 1115 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="209019.972">7788 1450 6880 0 0,'0'0'314'0'0,"0"0"-6"0"0,0 0-77 0 0,0 0 409 0 0,0 0 199 0 0,0 0 38 0 0,0 0-32 0 0,0 0-173 0 0,0 0-80 0 0,0 0-14 0 0,0 0-2 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 6 0 0,0 0 30 0 0,7 14 2401 0 0,11 32-517 0 0,-17 35-102 0 0,-9-15-1028 0 0,4-52-1323 0 0,2-2-1 0 0,1 1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,0-2 1 0 0,2 7-35 0 0,0 57 86 0 0,2-18-106 0 0,-3-53 540 0 0,-2-5-4113 0 0,1 2-6903 0 0,0-2 5190 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="209481.3229">7805 1653 1840 0 0,'0'0'403'0'0,"0"0"1018"0"0,0-5 1680 0 0,1 3 1760 0 0,29-59 991 0 0,-25 53-5592 0 0,1 1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,-1 1-1 0 0,-1 0 0 0 0,3 1 1 0 0,1-3-260 0 0,-6 6 92 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,-2-1-1 0 0,1 2 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 1-1 0 0,2 1-92 0 0,30 53 1184 0 0,-18-14-1184 0 0,-6 52 0 0 0,-6-48 848 0 0,-5-48-637 0 0,0 0-324 0 0,0 0-141 0 0,0 0-30 0 0,0 0-132 0 0,-5 9-4129 0 0,2-7-2469 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="210782.678">8329 1698 6304 0 0,'0'0'289'0'0,"0"0"-8"0"0,0 0-50 0 0,0 0 462 0 0,0 0 218 0 0,0 0 45 0 0,0 0-8 0 0,0 0-77 0 0,2 1-37 0 0,8 4 1041 0 0,-8-4-1679 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,2-1 1 0 0,-1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,2-1-197 0 0,64-48 1877 0 0,-7-9-1229 0 0,-51 46-648 0 0,-11 8 43 0 0,0 0 1 0 0,1 1-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,2-1-1 0 0,-2 2 0 0 0,0-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-2-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-3 1-43 0 0,1 1 15 0 0,1-1 0 0 0,0 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 1 0 0 0,2 1 0 0 0,-1-2 1 0 0,2 1-1 0 0,-2 1 0 0 0,2-1 0 0 0,-2 2-15 0 0,0 3 78 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,0 0 0 0 0,0 2 0 0 0,1-2 1 0 0,0 1-1 0 0,-1 7-78 0 0,1-7 84 0 0,0 4-20 0 0,1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 1 0 0 0,1-2 0 0 0,1 1 0 0 0,1 5-64 0 0,33 101 743 0 0,-34-116-717 0 0,0 0 0 0 0,0-2 0 0 0,1 2 0 0 0,-1-1 1 0 0,-1 2-1 0 0,3-2 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,0 2 0 0 0,-1-2 0 0 0,2-1 0 0 0,-2 1 0 0 0,0-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,5-1-26 0 0,1-3-217 0 0,1-1 0 0 0,-1-2-1 0 0,1 1 1 0 0,-2 0 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,6-10 217 0 0,24-18-3383 0 0,-25 24 1685 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212336.791">8810 1895 1376 0 0,'0'0'65'0'0,"0"0"286"0"0,0 0 1176 0 0,0 0 510 0 0,0 0 105 0 0,0 0-140 0 0,0 0-688 0 0,0 0-303 0 0,0 0-62 0 0,0 0-31 0 0,0 0-86 0 0,11-9 1503 0 0,25-86 2243 0 0,-1 5-2552 0 0,40-61-1672 0 0,33-14 444 0 0,-50 73 85 0 0,-45 69-1159 0 0,-12 22 177 0 0,-1 1 151 0 0,0 0 68 0 0,0 0 10 0 0,6 11-109 0 0,5 74 56 0 0,-14-3-233 0 0,3 121 500 0 0,4 120-424 0 0,2-252-61 0 0,-6-70-590 0 0,0-1-241 0 0,-1-1-1406 0 0,-4-5-5471 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="212940.975">8882 1753 6448 0 0,'0'0'498'0'0,"4"-5"32"0"0,0 2 484 0 0,-3 2-660 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2-1-354 0 0,58-14 3164 0 0,39 31-2595 0 0,-84-15-475 0 0,-4 0-1562 0 0,-2-1-3055 0 0,-2-1-2147 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="213609.296">9466 1626 920 0 0,'0'0'295'0'0,"0"0"901"0"0,-3-16 3639 0 0,1 14-5213 0 0,-4-1 8750 0 0,4 3-7138 0 0,1 0-721 0 0,-6 4 1698 0 0,-14 27-994 0 0,1 20-137 0 0,11 7 52 0 0,22 23 127 0 0,-11-77-1227 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 2-1 0 0,1-2 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-2 1 1 0 0,3-1-1 0 0,2 1-32 0 0,-3-1 21 0 0,-1-1-1 0 0,1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,2 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-2 0-1 0 0,1 1 1 0 0,1-1-1 0 0,0-2-20 0 0,55-50-20 0 0,-13-29-456 0 0,-35 42-464 0 0,-24 8-1392 0 0,12 34-2925 0 0,1 0-1661 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="214337.783">9929 1304 2304 0 0,'0'1'167'0'0,"4"23"1727"0"0,-10-5 5773 0 0,-2 117 1948 0 0,5-16-6975 0 0,6-37-2192 0 0,1 76-376 0 0,2-77-72 0 0,6-1-3116 0 0,-12-80 1546 0 0,0-1-280 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="214624.938">9915 1537 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,1-2-344 0 0,26-20 826 0 0,9 16 3479 0 0,2-3-2907 0 0,11 3-1414 0 0,-24 9-2102 0 0,-15 0-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213551.0589">10370 1721 10136 0 0,'8'13'230'0'0,"-6"-11"30"0"0,-2-2 19 0 0,0 0 104 0 0,-3 19 7879 0 0,4-18-7647 0 0,-1-1-21 0 0,1 1-38 0 0,10-1-436 0 0,-2 1-1 0 0,2-2 0 0 0,-1 1 1 0 0,0-2-1 0 0,-1 1 0 0 0,2 0 1 0 0,-1-3-1 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-2 0 0 0,0 0 1 0 0,1 0-1 0 0,-2-1 0 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-3 1 1 0 0,2-3-1 0 0,-1 2 0 0 0,0-1 1 0 0,-2-1-1 0 0,4-4-119 0 0,7-49 69 0 0,-15 59-69 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-2 0 0 0,0 2 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-2 0 0 0,0 2 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-4 0 0 0 0,3 1 61 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,2 1 0 0 0,0-1-61 0 0,-54 58-543 0 0,51-53 613 0 0,-1 1 0 0 0,0-2 0 0 0,1 2-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1-1 0 0,3-1 1 0 0,-2 8-70 0 0,1-10 0 0 0,1 2 0 0 0,1-2 0 0 0,0 3 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,3 0 0 0 0,-2-1 0 0 0,0 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,6 6 0 0 0,-8-9-56 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 56 0 0,7-4-1098 0 0,2-3-56 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-213242.538">10930 1547 4608 0 0,'-18'15'3105'0'0,"-1"0"6005"0"0,12 0-7943 0 0,-5 9 1032 0 0,10 16-1221 0 0,-3 47 1209 0 0,4-80-2095 0 0,1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,2-1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-3-1 0 0 0,3 2 0 0 0,-1-1 1 0 0,2-1-1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,2 0-1 0 0,-2-1 0 0 0,2-2 0 0 0,2 3-92 0 0,1-2 0 0 0,-6-7 0 0 0,1 1 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-2 0 0 0,-1 2 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,18-28 0 0 0,-3-1 0 0 0,0-2 0 0 0,-2 0 0 0 0,0-2 0 0 0,-9 12 0 0 0,-14 8-1384 0 0,6 18 600 0 0,2 1-1144 0 0,0 0-496 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212663.8799">11447 1488 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0 88 0 0,0 0 1067 0 0,0 0 483 0 0,0 0 98 0 0,0 0-138 0 0,0 0-670 0 0,0 0-295 0 0,0 0-60 0 0,0 0-101 0 0,0 0-377 0 0,0 0-167 0 0,0 0-31 0 0,-3 9 1448 0 0,-1 92 1023 0 0,11-8-2584 0 0,-4-31 1296 0 0,4 92-752 0 0,-3-143-818 0 0,-3-9-854 0 0,-1-2-382 0 0,0 0-76 0 0,0 0-20 0 0,0 0-2 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212449.687">11467 1704 456 0 0,'-4'-10'365'0'0,"3"9"1529"0"0,1-5 6369 0 0,3-6-4715 0 0,17-29-181 0 0,-11 22-2471 0 0,-3 9-747 0 0,-5 8-63 0 0,1-1-1 0 0,0 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-85 0 0,-2 1 239 0 0,10 5 186 0 0,-6-3-373 0 0,-1 1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-2 1 0 0,0 1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 1 1 0 0,1 0-1 0 0,-2-1 1 0 0,3 4-52 0 0,6 5 0 0 0,-10-11-55 0 0,-1-2-16 0 0,5 5-460 0 0,-4-3-2608 0 0,-1-2-3526 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-206308.3389">2845 2660 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,0 2-294 0 0,-5 8 6808 0 0,-1-6-3282 0 0,-8-21-2050 0 0,14 16-1469 0 0,-11-100 2153 0 0,11-137-1048 0 0,-3-2-752 0 0,-9-54-24 0 0,-1 49-128 0 0,1-97-168 0 0,9 163 559 0 0,-11-51-726 0 0,10 95-532 0 0,-2 20 446 0 0,2 40-11 0 0,-1 16 64 0 0,2 3 0 0 0,7-109 128 0 0,4 127-128 0 0,9 15 0 0 0,-10 20-4 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,1 1 1 0 0,-2-1-1 0 0,2 2 0 0 0,-2-1 0 0 0,0 1 0 0 0,2 0 1 0 0,-2 1-1 0 0,2 0 0 0 0,-2 0 0 0 0,1 1 1 0 0,1 0-1 0 0,-2 0 0 0 0,8 3 4 0 0,32 11 0 0 0,-23-8 79 0 0,1 0 0 0 0,-2-1-1 0 0,2-2 1 0 0,0-1-1 0 0,1-1-78 0 0,33-2-104 0 0,1-3 0 0 0,-1-3-1 0 0,1-3 1 0 0,55-15 104 0 0,373-70 0 0 0,-375 84 0 0 0,1 4 0 0 0,0 6 0 0 0,34 8 0 0 0,19-1 0 0 0,3-6 99 0 0,2-8-1 0 0,79-14-98 0 0,-106 6 64 0 0,100 7-64 0 0,-156 11 41 0 0,-1 4-1 0 0,37 11-40 0 0,7 1 143 0 0,73 4 11 0 0,3-11-1 0 0,156-12-153 0 0,36-22 125 0 0,-284 16-98 0 0,151 4 106 0 0,175 32 123 0 0,-70-1-170 0 0,339-33 188 0 0,-307 23 29 0 0,-179-5-190 0 0,-59-4-38 0 0,152-12-75 0 0,32-14 0 0 0,-164 7 128 0 0,38 10-128 0 0,316 43 0 0 0,-454-45 0 0 0,34-17 64 0 0,59-21-160 0 0,-129 35 85 0 0,22-1-42 0 0,24-28 429 0 0,-63 30-376 0 0,-16 9 0 0 0,-3 3 0 0 0,11 16 0 0 0,-12 3 0 0 0,18 63 0 0 0,-12 4-189 0 0,-6 1-1 0 0,6 95 190 0 0,-9 11 307 0 0,5 189-618 0 0,-11 114 606 0 0,2-149-200 0 0,4-3-14 0 0,-5-154-6 0 0,-5-182-59 0 0,0 0 1 0 0,-2 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,-1 1-1 0 0,1-3 1 0 0,-5 12-17 0 0,6-24 9 0 0,1 1 0 0 0,-2 0 0 0 0,1-2 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-9 0 0,-45-4 22 0 0,0-2 0 0 0,1-1-1 0 0,1-4 1 0 0,-11-4-22 0 0,-87-17 52 0 0,-111 9-87 0 0,26 30 35 0 0,-346 10 0 0 0,-18-18 0 0 0,294 19 70 0 0,-14 15-70 0 0,-66 7 47 0 0,287-32-39 0 0,-390 18-5 0 0,-343-20-3 0 0,-337 31 240 0 0,627-44-256 0 0,113-16-48 0 0,22-5 64 0 0,-78 5 11 0 0,204 11 114 0 0,-72-27-85 0 0,-43-29-40 0 0,248 48 0 0 0,-14 6 0 0 0,-2 28 0 0 0,-38-12 0 0 0,82-8-100 0 0,107 4 7 0 0,6 3-64 0 0,1-1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1 156 0 0,1-9-10012 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202306.8289">7321 2978 3224 0 0,'0'2'240'0'0,"18"56"4562"0"0,-8-8 530 0 0,-3-25-2824 0 0,-2 9-572 0 0,5 47 269 0 0,5 26-781 0 0,-1 50 0 0 0,5 111 552 0 0,-2-125-1272 0 0,9 155 568 0 0,-18-39-696 0 0,2-124-389 0 0,-3 42 722 0 0,-7-54-581 0 0,-4-2-93 0 0,8-7-91 0 0,-8 43-19 0 0,4-101-61 0 0,-3 86 0 0 0,-2-109-64 0 0,5-27-67 0 0,0-5-281 0 0,0-1-129 0 0,0 0-31 0 0,0 0-72 0 0,-4-17-3152 0 0,1 2-2356 0 0,-1-4-1623 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201855.109">6996 4755 12264 0 0,'0'0'273'0'0,"-5"13"786"0"0,5-2-595 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,1-3 0 0 0,1 7-464 0 0,-4-9 43 0 0,50 112 3185 0 0,28 118 95 0 0,-62-168-2734 0 0,2-2 0 0 0,27 57-589 0 0,17 12 416 0 0,-2-53-72 0 0,-49-74-248 0 0,-2 3-1 0 0,1-2 0 0 0,1 0 1 0 0,-1 0-1 0 0,2-2 1 0 0,11 7-96 0 0,-20-12 39 0 0,0-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 0 0 0 0,-3 1 0 0 0,2-2 0 0 0,-1 1 0 0 0,1 0 1 0 0,-2-1-1 0 0,2-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1-1-39 0 0,61-64 528 0 0,17-75-224 0 0,69-286-391 0 0,-137 393-257 0 0,22-57-4278 0 0,-31 82 2515 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186308.475">13464 1263 1840 0 0,'0'0'83'0'0,"0"0"-6"0"0,0 5 363 0 0,0-4 1761 0 0,0-1 766 0 0,1 19 5666 0 0,1 0-5371 0 0,1 17-970 0 0,-3-25-1727 0 0,-11 108 2961 0 0,-24 79-2557 0 0,39-158-1425 0 0,-4-40 48 0 0,0 0-940 0 0,0 0-410 0 0,1 0-88 0 0,3-5-10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-185850.611">13814 1263 13040 0 0,'0'0'597'0'0,"0"0"-9"0"0,0 0-220 0 0,0 0 481 0 0,0 0 250 0 0,0-5 715 0 0,-1 4 3304 0 0,-5 3-5002 0 0,1 1 0 0 0,0-1 1 0 0,-1 2-1 0 0,1-1 0 0 0,1 2 1 0 0,-2-1-1 0 0,2 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2 1 1 0 0,2 0-1 0 0,-1 1 0 0 0,0 0 1 0 0,2-2-1 0 0,-1 2 1 0 0,0-1-1 0 0,1 2 0 0 0,-2 2-116 0 0,1 2 121 0 0,-1 0-1 0 0,3 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,3 2 1 0 0,-1-2-1 0 0,1 0 1 0 0,0-1-1 0 0,3 5-120 0 0,47 112 0 0 0,-48-96 0 0 0,-7-24 0 0 0,0-5 60 0 0,0 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-2-1 0 0 0,3 1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 0 0 0 0,3-1 1 0 0,-1 1-1 0 0,-1 0 0 0 0,-2-2-60 0 0,-4-4-110 0 0,9 7-9 0 0,-1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-2-1 0 0 0,2 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-2 119 0 0,1-5-1959 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-187118.8789">12817 930 13184 0 0,'0'0'604'0'0,"0"0"-14"0"0,0 0-252 0 0,0 0 326 0 0,0 0 185 0 0,0 0 41 0 0,2 0-12 0 0,-1-1-747 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,2 0 1 0 0,-2 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-2 0-131 0 0,6 18 493 0 0,-2-2 0 0 0,0 1 0 0 0,1 2-1 0 0,-3-2 1 0 0,1 20-493 0 0,-3-34 76 0 0,-2 91 1295 0 0,1 21-942 0 0,-6-18-247 0 0,-1 119-43 0 0,12-174-247 0 0,-4-42-448 0 0,0-2-176 0 0,0 0-32 0 0,3-22-3836 0 0,-2 2 2544 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-186774.862">12890 1325 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-79 0 0,0 0-421 0 0,0 0-180 0 0,0 0-37 0 0,0-13 1908 0 0,1 8-2997 0 0,0-1 1 0 0,0 2 0 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0 0 0 0 0,2 1 0 0 0,-2 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-3 0-346 0 0,15-9 712 0 0,-16 10-708 0 0,1 0 0 0 0,-2 0 1 0 0,3 0-1 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 1 0 0,1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,3 1-4 0 0,-2-1 90 0 0,1 2-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,2 2 0 0 0,-2-2 1 0 0,0 1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1-2 0 0 0,-1 2 1 0 0,0 1-1 0 0,1 1-89 0 0,51 201 1931 0 0,-49-181-1912 0 0,-1-1 1 0 0,0 1-1 0 0,-2 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,-2 4-19 0 0,0 4-4294 0 0,2-34-4235 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184500.214">14209 1143 11976 0 0,'-4'2'1082'0'0,"-17"95"550"0"0,1 55 3297 0 0,15 51-1046 0 0,8-99-3866 0 0,4-75-17 0 0,-7-27-850 0 0,0 3 2050 0 0,0-2-4324 0 0,0 3-3781 0 0,0-6 913 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-184054.319">14270 1187 3224 0 0,'0'0'143'0'0,"1"1"-3"0"0,4 5 390 0 0,12 8 9462 0 0,3 1-5178 0 0,-15-12-4675 0 0,-2-1-1 0 0,0 0 1 0 0,2 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-1-1 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,2 0-138 0 0,32 3-1260 0 0,-21-7 497 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-183416.4799">14147 1277 5960 0 0,'-3'-9'266'0'0,"3"8"1"0"0,0-22 1002 0 0,10-16 3955 0 0,12-8-2882 0 0,-12-2-311 0 0,-8 45-2036 0 0,-6-12-175 0 0,0 12-433 0 0,4 4-2775 0 0,0 0 1855 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-182333.102">14528 1575 0 0 0,'0'0'2721'0'0,"0"0"-302"0"0,0 0 223 0 0,1-1-119 0 0,9-8-671 0 0,-10 7-1682 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-2 0 0 0,0 1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,2 0 1 0 0,-2 1-1 0 0,0-1 0 0 0,0 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,-1 1-1 0 0,1 0-170 0 0,6 2 296 0 0,-1 1 0 0 0,0-1 0 0 0,0 2 0 0 0,0 0 0 0 0,-2-1 1 0 0,1 1-1 0 0,1 0 0 0 0,-3 2 0 0 0,2-3 0 0 0,0 2 0 0 0,-2-1 0 0 0,1 2 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,3 8-296 0 0,7 45 792 0 0,-12-57-721 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 2 0 0 0,-1-2 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-2 2-71 0 0,4-4 2 0 0,-1 1 15 0 0,-1 1 1 0 0,-2-1-1 0 0,2 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,-1-2-18 0 0,0 1 49 0 0,-2-1 1 0 0,1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-2-1 0 0,0 2 1 0 0,0-1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,2-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0-1-49 0 0,2 2-126 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 2 1 0 0,1-1-1 0 0,0 0 1 0 0,2-3 126 0 0,14-36-3998 0 0,-4 22-3873 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-175901.286">14969 1543 4144 0 0,'0'0'191'0'0,"0"0"375"0"0,-4-9 14804 0 0,9 57-13610 0 0,2 18 8 0 0,4 27 351 0 0,-10-77-1781 0 0,7 24-3577 0 0,-8-39 1789 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172641.548">15683 1702 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,1 1-72 0 0,15 39 5565 0 0,-10-27-3129 0 0,-2-11-2556 0 0,3-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-2 0 0 0 0,1 1 0 0 0,0-3 1 0 0,0 2-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-2-1 0 0,-1 1 0 0 0,5-5-209 0 0,63-63 153 0 0,-51 34-213 0 0,-20 36 61 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1 0 1 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 0 0 0,-1-1 2 0 0,1 1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 1-2 0 0,-16 7 0 0 0,17-7 0 0 0,0 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,3 0 0 0 0,-3 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 5 0 0 0,-5 10 27 0 0,6-9 0 0 0,0-2-1 0 0,-1 1 1 0 0,2 0 0 0 0,-1 0 0 0 0,2 2 0 0 0,1-3 0 0 0,-2 2-1 0 0,2 0 1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,1 2 0 0 0,0-1-1 0 0,1 1 1 0 0,1 1-27 0 0,0-6-27 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,1-2-1 0 0,-1 2 1 0 0,0 0-1 0 0,3-2 1 0 0,-2 1-1 0 0,2 0 1 0 0,-2 0 0 0 0,2-1-1 0 0,-1 0 1 0 0,2 1-1 0 0,3 4 28 0 0,16-3 0 0 0,21-16-1385 0 0,-31 1-166 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172385.72">16182 1727 11832 0 0,'-37'14'7253'0'0,"35"-12"-6259"0"0,2-1-12 0 0,0-1-29 0 0,0 0-122 0 0,0 0-482 0 0,0 0-205 0 0,0 0-44 0 0,0 0-7 0 0,0 0 17 0 0,0 0 8 0 0,0 0 2 0 0,0 0-237 0 0,0 0-996 0 0,0 0-434 0 0,1 0-86 0 0,3 0-21 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170574.714">16975 1126 2760 0 0,'0'0'589'0'0,"0"0"1434"0"0,0 0 626 0 0,0 0 126 0 0,0 0-214 0 0,0 7 88 0 0,0 174 4329 0 0,0 91-4387 0 0,-1-170-2591 0 0,-4 28 0 0 0,5-64 0 0 0,-3-2-134 0 0,3-63-570 0 0,0-1-263 0 0,0 0-916 0 0,0-1-3632 0 0,-3-6-1553 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170137.543">16938 1589 5064 0 0,'0'0'389'0'0,"2"-3"794"0"0,0 2 3071 0 0,26-34 3094 0 0,7-1-4244 0 0,20-5-1223 0 0,-49 40-1852 0 0,-2 1 1 0 0,2 0-1 0 0,-3 0 0 0 0,3 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,-2 0-1 0 0,0 0 0 0 0,2 1 0 0 0,-2-2 0 0 0,0 2 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,-2 1 0 0 0,2 0 1 0 0,-2-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,-1 2-29 0 0,5 13 310 0 0,-1 4 0 0 0,-2-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,-1 8-310 0 0,-7 92 1048 0 0,7-94-908 0 0,6 2-148 0 0,9-37-432 0 0,5-12-1437 0 0,1 0-5762 0 0,-9 8 145 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-172102.041">16501 1370 9760 0 0,'3'-26'2366'0'0,"-3"25"-894"0"0,0 1 68 0 0,0 0-60 0 0,0 0-321 0 0,0 0-139 0 0,0 0-27 0 0,0 0-34 0 0,0 0-114 0 0,-3 6 736 0 0,-7 73 997 0 0,1 35-801 0 0,-6 78-1676 0 0,10-117-101 0 0,1 24 0 0 0,3-87 704 0 0,-1-1-2693 0 0,1 3-6478 0 0,1-14 756 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-171739.932">16533 1370 16064 0 0,'5'-14'1715'0'0,"-3"10"-1471"0"0,-1 1-1 0 0,1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-2-1 1 0 0,5 0-244 0 0,-4 0 90 0 0,2 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-2 0-1 0 0,0 2 0 0 0,2-2 1 0 0,-2 1-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,-3 0-1 0 0,5 3-90 0 0,-3 6 116 0 0,0-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,-1 2 1 0 0,2-1 0 0 0,-3 1 0 0 0,1-2 0 0 0,-1 0-1 0 0,0 2 1 0 0,-1-1 0 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,-3-2 0 0 0,2 2 0 0 0,-2-1-1 0 0,1 1 1 0 0,-7 8-116 0 0,-41 69 1297 0 0,50-87-1274 0 0,1 1-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 0 1 0 0,2-1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-2 0-1 0 0,1 0 0 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1-1 1 0 0,2 1-1 0 0,-1 0-22 0 0,-1-2-128 0 0,2 1 21 0 0,0 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,1-2 0 0 0,0 1 0 0 0,1 0 1 0 0,-3-1-1 0 0,2 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,1 0 106 0 0,-1-10-1478 0 0,-3 2-66 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174133.0909">15345 1422 4144 0 0,'0'0'319'0'0,"0"0"-7"0"0,0 0 751 0 0,0 0 355 0 0,0 0 71 0 0,0 0-42 0 0,0 0-234 0 0,0 0-101 0 0,0 0-21 0 0,0 18 3966 0 0,-10 5-3283 0 0,9-21-1264 0 0,1-2-29 0 0,0 2-8 0 0,-3 250 2166 0 0,-10-135-2099 0 0,7-63 33 0 0,0 21-3333 0 0,7-76 56 0 0,2-7-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173508.196">15306 1660 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,1-1 491 0 0,27-53 6288 0 0,-26 51-6862 0 0,-1-1 1 0 0,1 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-3 1 0 0 0,1-1 0 0 0,2 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 1 1 0 0,2 1-157 0 0,-1 1 54 0 0,1-2 0 0 0,-3 2 0 0 0,1-2 0 0 0,1 2-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,-1 1-1 0 0,2-1 1 0 0,-1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,1 1-1 0 0,-2 0 1 0 0,2 1 0 0 0,-2-1 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 0-53 0 0,0-5-149 0 0,4 19-2358 0 0,-4-9 487 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-169732.6209">17527 1397 18287 0 0,'0'0'414'0'0,"0"0"56"0"0,0 1 32 0 0,0 84 1564 0 0,-12 59 154 0 0,2 10-612 0 0,3-22 14 0 0,-1-50-1333 0 0,8-81-974 0 0,0-1-274 0 0,0 0-53 0 0,0 0-215 0 0,0 0-858 0 0,0 0-379 0 0,1-2-80 0 0,2-12-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-168923.508">17589 1514 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,3-7-322 0 0,3-5-3 0 0,-3 6 250 0 0,1 1-1 0 0,-1-1 1 0 0,1 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,1 0-1 0 0,1 1 1 0 0,-3-1 0 0 0,3 1 0 0 0,-2 0-1 0 0,2 1-460 0 0,-4 0 236 0 0,2 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0-1 0 0,-2 0 1 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 2-1 0 0,1-1 1 0 0,-1 0-236 0 0,2 1 105 0 0,-3 2 0 0 0,3-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 2 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1 6-105 0 0,14 83 177 0 0,-29 79 1151 0 0,-11-108-745 0 0,19-63-571 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 0 0 0,1-2 1 0 0,-1 1-1 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0-1-1 0 0,1 1 0 0 0,-2-1 0 0 0,2 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-3 0 0 0,-1 2 0 0 0,-1-1-12 0 0,-3-2-508 0 0,-1 1 0 0 0,0-2 0 0 0,2 0 0 0 0,-2-2 0 0 0,2 3 0 0 0,-1-3 0 0 0,0 1-1 0 0,1-1 1 0 0,-6-8 508 0 0,1 1-1504 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-130876.9168">3040 6214 6448 0 0,'23'-2'672'0'0,"-19"1"-608"0"0,0 3 3996 0 0,-1 5-3602 0 0,-3-3 96 0 0,1-3 14 0 0,-4 13 453 0 0,10 165 2956 0 0,-12 71-1512 0 0,9-98-1338 0 0,3-72-1094 0 0,-4-71-94 0 0,-3-7-264 0 0,5-17-6236 0 0,-2 3 317 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-124973.04">3060 6266 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 0-79 0 0,0 0 561 0 0,0 0 272 0 0,-3 6 1195 0 0,-4-3 2766 0 0,8-9-4160 0 0,9-14-1197 0 0,-8 13 345 0 0,2 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,0-1-1 0 0,1 2 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,5 0-78 0 0,-7 2-15 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-2 2 0 0 0,1 0 0 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 15 0 0,22 117 716 0 0,-24-118-672 0 0,3 2 51 0 0,-3 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 1 0 0 0,0-3 0 0 0,1 4 0 0 0,-2-2 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0-95 0 0,-36 26 236 0 0,32-29-233 0 0,-2 2 17 0 0,-1 0 0 0 0,-1-2 0 0 0,1 1 0 0 0,-1-2 1 0 0,1 0-1 0 0,0 0 0 0 0,-1-1 0 0 0,-9 0-20 0 0,-28-5-116 0 0,45 0 127 0 0,2 2 42 0 0,11 14-2 0 0,38 48-118 0 0,67 112 1347 0 0,-67-104-1908 0 0,-30-55-2350 0 0,-10-8-4791 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123928.98">3538 6805 3224 0 0,'0'0'143'0'0,"0"0"315"0"0,0 0 1222 0 0,0 0 531 0 0,0 0 106 0 0,0 0-213 0 0,0 0-968 0 0,0 0-428 0 0,4 9 1069 0 0,2-7-1546 0 0,1 0-1 0 0,-1-1 1 0 0,-1 0 0 0 0,2 0-1 0 0,-1 1 1 0 0,-1-2-1 0 0,2 0 1 0 0,0-2 0 0 0,-1 2-1 0 0,-1-1 1 0 0,2-1-1 0 0,-1 1 1 0 0,-1-1 0 0 0,2 1-1 0 0,-2-1 1 0 0,4-2-231 0 0,-8 3-25 0 0,10-4 212 0 0,3 0-1 0 0,-3-2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1-2 1 0 0,-3 2-1 0 0,1-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-3-186 0 0,-5 8 3 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0-2 0 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-2-4-3 0 0,1 7 35 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,0 2-1 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,2 0 1 0 0,-3 0-1 0 0,1 1 0 0 0,0-1 0 0 0,-2 1-35 0 0,1-1 16 0 0,-1 1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,3-2 0 0 0,-2 1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 2 0 0 0,0-2 0 0 0,1 1-16 0 0,-54 121 249 0 0,38-11-267 0 0,18-106 28 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,0-2 0 0 0,0 1-1 0 0,1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,-1 2 1 0 0,1-2-1 0 0,1 0 1 0 0,1 0 0 0 0,-2-1-1 0 0,4 4-9 0 0,-5-6 6 0 0,2 0 0 0 0,-1-1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,1 1 0 0 0,-2 0-1 0 0,2 1 1 0 0,-2-2 0 0 0,2 1-1 0 0,-1-1 1 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0-1 1 0 0,-1 1 0 0 0,2-1 0 0 0,-2 0-1 0 0,2 0 1 0 0,-3 0 0 0 0,7-1-6 0 0,-5 0 57 0 0,24-6-1613 0 0,-9 1-3577 0 0,-3-5-2072 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123239.429">4146 6347 920 0 0,'0'0'279'0'0,"0"0"833"0"0,0 0 362 0 0,0 0 78 0 0,0 0-63 0 0,0 0-322 0 0,0 0-140 0 0,0 0-31 0 0,0 0-26 0 0,0 0-88 0 0,0 0-40 0 0,0 0-8 0 0,0 0-34 0 0,0 0-136 0 0,0 0-66 0 0,0 0-12 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0-42 0 0,0 6-12 0 0,-10 49 1334 0 0,3 12-600 0 0,-1 51 252 0 0,9 98-1210 0 0,3-98-216 0 0,6-12 642 0 0,-3-91-1088 0 0,-6-14-25 0 0,-1-1-998 0 0,0 0-429 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122817.09">4118 6565 12176 0 0,'0'0'561'0'0,"0"0"-17"0"0,2 1-217 0 0,83 10 5294 0 0,-11 6-5284 0 0,-10 12-2062 0 0,-62-29 475 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122538.437">4567 6863 2304 0 0,'-12'-8'3825'0'0,"10"5"-3248"0"0,-1 0 1 0 0,1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 1 1 0 0,1-2-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-5-578 0 0,1 4 116 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,1 0-116 0 0,-2 1 36 0 0,1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,3-1 0 0 0,-2 1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-2 2 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-2 0 0 0,-1 2 0 0 0,2 0 0 0 0,-2 0 0 0 0,2 2-36 0 0,54 60 1232 0 0,-51-51-822 0 0,-1 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,0 3-1 0 0,-1-1 1 0 0,0-1-1 0 0,-1 2 1 0 0,1 0-1 0 0,-3-2 1 0 0,1 2 0 0 0,-1 10-410 0 0,-14 36 100 0 0,11-57-42 0 0,1 1 0 0 0,0-2 1 0 0,0 2-1 0 0,0 0 0 0 0,0-1 0 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-2 1-1 0 0,2-3 0 0 0,-1 2 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 1 0 0,2 0-1 0 0,0-1 0 0 0,-2 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,2-1 0 0 0,-3 1-58 0 0,-2-1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,2-1 0 0 0,0-1 0 0 0,-5-3 0 0 0,-32-45-1424 0 0,31 25-5473 0 0,5 13-533 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121496.511">4959 6653 15176 0 0,'0'0'340'0'0,"0"0"50"0"0,-2 2 26 0 0,-14 17 101 0 0,12-15-271 0 0,1 1 0 0 0,1-1-1 0 0,-2-1 1 0 0,2 1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,1-1-245 0 0,4 57-21 0 0,45 59 1584 0 0,-47-117-1524 0 0,2 2 0 0 0,0-2 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 2 0 0 0,0-2 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,0-2 0 0 0,-2 1 0 0 0,4 0-39 0 0,-1-3-10 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1-2-1 0 0,1 2 1 0 0,1-2 0 0 0,-2 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-2-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-3 0 0 0 0,3-1 0 0 0,-2 1 0 0 0,-1 0 0 0 0,2-1-1 0 0,-2-1 1 0 0,0-1 10 0 0,2-4 49 0 0,0 0 0 0 0,0-2 0 0 0,-1 2 0 0 0,-1 0 0 0 0,1-1 0 0 0,-3-1-1 0 0,0 1 1 0 0,0-12-49 0 0,0 10-17 0 0,0 18 17 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 0 0 0,-12 37-209 0 0,12 90 192 0 0,11-90-2918 0 0,-10-25 1407 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-118100.252">5453 6599 4608 0 0,'23'-33'2473'0'0,"-15"18"4749"0"0,-2 19-1038 0 0,-1 7-5674 0 0,0 0-1 0 0,-1-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 1 1 0 0,-1 1-1 0 0,0-2 0 0 0,1 3-509 0 0,5 35 445 0 0,0 23-52 0 0,4 69-233 0 0,-7-77-380 0 0,5 4-218 0 0,-10-66 32 0 0,0-2-1020 0 0,0 0-4245 0 0,0 0-1815 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-117537.033">5503 6702 1376 0 0,'0'0'448'0'0,"0"0"1344"0"0,0 0 588 0 0,0 0 116 0 0,0 0-136 0 0,0 0-684 0 0,0 0-299 0 0,0 0-58 0 0,0 0-107 0 0,0 0-419 0 0,0 0-179 0 0,0 0-35 0 0,0 0-40 0 0,11-4 578 0 0,51-63 1084 0 0,-59 66-2155 0 0,-1-1-1 0 0,1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,-1 0-1 0 0,2-1-45 0 0,40 33 240 0 0,-9 33 664 0 0,-35-65-973 0 0,-1-2-608 0 0,0 0-262 0 0,0 0-1349 0 0,0 0-5210 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116084.978">6024 6750 920 0 0,'0'18'0'0'0,"0"-18"80"0"0,0 0-80 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 352 0 0,0 0 64 0 0,0 0 0 0 0,0 0 8 0 0,0 6-424 0 0,0-6 0 0 0,0 0 0 0 0,2 11-96 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115526.386">6048 6544 7856 0 0,'0'0'174'0'0,"0"0"29"0"0,0 0 13 0 0,0 9 2112 0 0,7 27 1209 0 0,-6-8-1555 0 0,4 68 1712 0 0,0 26-2229 0 0,-1-46-1465 0 0,-3-31 69 0 0,-2-27-2628 0 0,1-13 952 0 0,0-5-279 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115183.311">6048 6802 11832 0 0,'0'-17'1285'0'0,"23"-60"4317"0"0,19 33-3283 0 0,-39 43-2299 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,1-1-1 0 0,-2 0 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,2 1-20 0 0,18 39 831 0 0,18 54 83 0 0,-28-46-684 0 0,-7 9 68 0 0,-7-28-874 0 0,3-31 150 0 0,0-1-988 0 0,-1 1-436 0 0,-1 5-92 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-114236.626">6514 6818 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0 0 43 0 0,0 0 159 0 0,0 0 70 0 0,0 0 14 0 0,0 0 69 0 0,0 0 285 0 0,0 0 126 0 0,0 0 29 0 0,0 0-15 0 0,0 0-77 0 0,0 0-31 0 0,0 0-8 0 0,0 0-33 0 0,0 0-134 0 0,2 1-61 0 0,47 7 2321 0 0,-32-9-2644 0 0,34-21 394 0 0,-47 20-751 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-2 0 0 0,1 2 0 0 0,-2-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,2 1-1 0 0,-3-2 0 0 0,1 2 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-4 19 0 0,-7-7 0 0 0,6 12 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-2 0 0 0,1 2 0 0 0,-1 0 0 0 0,2 0 0 0 0,-3 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,2 1 0 0 0,-3 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,3 0 0 0 0,-3 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 2 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 1 0 0 0,-1 1 76 0 0,-1 2 0 0 0,1 0-1 0 0,-1-1 1 0 0,3 0 0 0 0,-2 1-1 0 0,1 0 1 0 0,0 0 0 0 0,1 2-1 0 0,0-2 1 0 0,1 1 0 0 0,0 1 0 0 0,0-2-1 0 0,0 1 1 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 2-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1-1 0 0,0-2 1 0 0,0 0 0 0 0,0 2 0 0 0,1-2-1 0 0,1 3-75 0 0,42 55 0 0 0,-43-62 25 0 0,0 0 0 0 0,1 0 0 0 0,0-2 0 0 0,0 1 0 0 0,0 2 0 0 0,0-2 1 0 0,0-1-1 0 0,2 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-3 0 0 0 0,3 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,2-1-25 0 0,47-23-3889 0 0,-43 17-4253 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-106495.084">7071 6636 2760 0 0,'-34'-29'1211'0'0,"33"28"-702"0"0,-14-6 1981 0 0,-3 8-1483 0 0,10 5-408 0 0,-27 18 451 0 0,15-23 2469 0 0,7-5 2535 0 0,18-4-4219 0 0,46-12 338 0 0,37 21-421 0 0,-81 2-1693 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 2-1 0 0,-1-1 0 0 0,1-1 0 0 0,0 3-59 0 0,46 35-101 0 0,-16-41 802 0 0,-35-2-571 0 0,-1 1 4 0 0,0 0-4 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-2 0 0,0 0-6 0 0,-18 28 213 0 0,-27 2-28 0 0,11-8-202 0 0,-36 15-64 0 0,-28 24 212 0 0,52-16-359 0 0,21-16 389 0 0,21-20-217 0 0,1-3 36 0 0,4-5-46 0 0,-1 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1-14 0 0,49-13 417 0 0,153-22 582 0 0,-150 38-919 0 0,-12 12-3590 0 0,-41-16 1676 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101751.894">7489 6963 3680 0 0,'-6'16'1721'0'0,"5"-11"9907"0"0,14-11-8856 0 0,15-14-2535 0 0,51-89 2026 0 0,2-46-1063 0 0,53-118-374 0 0,11 13-1554 0 0,-119 234 728 0 0,-10 0 0 0 0,-16 27 24 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 2 0 0 0,0-2 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0-2-1 0 0,1 2 0 0 0,-1-1-23 0 0,-1 24 138 0 0,-1-2 0 0 0,-2 2 0 0 0,1-3-1 0 0,-3 2 1 0 0,-6 19-138 0 0,-6 28 173 0 0,-11 75-35 0 0,21-44 4 0 0,8-83-93 0 0,-1-1 0 0 0,2 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,2 7-50 0 0,0 0 36 0 0,9 22 71 0 0,10 0 53 0 0,-15-51 10 0 0,59-158 270 0 0,-1 18-376 0 0,52-141-64 0 0,-71 188 0 0 0,-35 81 0 0 0,-13 19-2 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 2 0 0,0 0-1 0 0,8 59-63 0 0,-5 43 64 0 0,-6 39 203 0 0,-8 2 7 0 0,-5 37-63 0 0,-5-61-94 0 0,8-23-185 0 0,6-64-625 0 0,7-31-572 0 0,0-1-410 0 0,0 0-1290 0 0,0 0-4861 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-101158">8607 6839 11232 0 0,'0'0'256'0'0,"0"0"34"0"0,0 0 20 0 0,-2 0-40 0 0,-29-3 1829 0 0,30 3-1367 0 0,1-2 59 0 0,9-47 2427 0 0,-7 41-3131 0 0,1 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,2 0-86 0 0,-6 2 36 0 0,1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-1-1-1 0 0,-2 1 1 0 0,3 0-1 0 0,-2-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 2-36 0 0,4 6 185 0 0,-1-1 0 0 0,0 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 1 0 0,-2-1-1 0 0,0 3 0 0 0,0-2 0 0 0,-3 8-185 0 0,6-17 57 0 0,-2 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 1 0 0 0,1-2 1 0 0,0 1-1 0 0,1-1 1 0 0,-3 1-1 0 0,2-1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1-1 0 0,0-1 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-4-57 0 0,-4 2-194 0 0,3-1 0 0 0,-1 0 0 0 0,-1-1-1 0 0,2 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,0-2 0 0 0,-3-3 194 0 0,-4-37-3540 0 0,6 28-4246 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-100410.518">9205 6602 8496 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 10 0 0,0 0 112 0 0,-1 1 406 0 0,-36 76 4453 0 0,11-34-3370 0 0,13-2-456 0 0,11-15-994 0 0,-10 30 976 0 0,12-53-1274 0 0,0 3 0 0 0,2-2 0 0 0,-2 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-2 0 0 0,0 2 0 0 0,-1-1 0 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-2-1 0 0,1 2 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-81 0 0,7 1 0 0 0,-3 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,1-2 0 0 0,3-6 0 0 0,54-100 0 0 0,-29 21 1046 0 0,-27 53-920 0 0,-7 39-27 0 0,-1 1-10 0 0,0 0 6 0 0,0 0 29 0 0,8 1 281 0 0,-3 13-392 0 0,3-1 0 0 0,-2 2 0 0 0,0-2 0 0 0,-2 2 0 0 0,2-1 0 0 0,-3 2 0 0 0,0-1 0 0 0,0-1 0 0 0,-1 1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2-1 0 0 0,-2 6-13 0 0,-13 103 1090 0 0,1-79-947 0 0,-3-1 1 0 0,0-1 0 0 0,-2-1 0 0 0,-2 1-1 0 0,-1-4 1 0 0,-10 13-144 0 0,21-34 225 0 0,-2-3 0 0 0,0 1 0 0 0,1 0 0 0 0,-3-2 0 0 0,0 0-1 0 0,1 0 1 0 0,-2-2 0 0 0,-1 0 0 0 0,-14 8-225 0 0,28-17-3 0 0,0-1 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,2 0 1 0 0,-1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1-2 0 0 0,-2 2 0 0 0,2 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-2-2 3 0 0,3-5-150 0 0,0-1 0 0 0,0 0 1 0 0,0 2-1 0 0,1-3 0 0 0,0 2 0 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,2-1 0 0 0,2 1 0 0 0,-2 1 1 0 0,1-2-1 0 0,2 2 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,3 1 150 0 0,3-15-1149 0 0,4-3-679 0 0,-3 4-278 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-99222.683">9805 6860 10136 0 0,'2'14'230'0'0,"-2"-11"30"0"0,0-3 19 0 0,0 0 105 0 0,0 0 411 0 0,0 0 182 0 0,10 8 1891 0 0,-6-5-2546 0 0,1-1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,2-1 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,2 0-322 0 0,4-2 206 0 0,0 1 0 0 0,-1 0 0 0 0,-1-2 0 0 0,2 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1-1 0 0 0,4-3-206 0 0,41-73 696 0 0,-49 75-668 0 0,-1 0-1 0 0,-1-1 1 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,-1-3 0 0 0,0 2 0 0 0,0-1-1 0 0,-1 1 1 0 0,-1-5-28 0 0,3 11 5 0 0,-1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,1-1-1 0 0,-1 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0-2-1 0 0,1 1 0 0 0,-3 1 1 0 0,2-1-1 0 0,0 1 1 0 0,-2 0-1 0 0,2-1 1 0 0,0 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,3 0-1 0 0,-2 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,0 1-5 0 0,-5 7 19 0 0,2 0 1 0 0,-2-3 0 0 0,2 4 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-2 0 0 0,3 2-1 0 0,-2 0 1 0 0,2-1 0 0 0,-1 2-20 0 0,0 0 77 0 0,0 0-1 0 0,3 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 2 1 0 0,2 0 0 0 0,0-1 0 0 0,2 1-1 0 0,-1-2 1 0 0,0 2 0 0 0,2-1 0 0 0,-2 0-1 0 0,3 0 1 0 0,-1 0 0 0 0,2 0-1 0 0,0-1 1 0 0,0 2-77 0 0,-2-7 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1-2 0 0 0,-1 3 0 0 0,0-2 0 0 0,1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1-1 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,36-18-1473 0 0,-25 5 614 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95784.39">10349 6606 4608 0 0,'0'0'353'0'0,"0"0"35"0"0,0 0 1008 0 0,0 0 461 0 0,0 0 95 0 0,0 0-104 0 0,0 0-522 0 0,0 0-228 0 0,0 0-46 0 0,1 2-59 0 0,10 18 2469 0 0,6 30-1092 0 0,-10 42-307 0 0,-1 14-686 0 0,-9 9-869 0 0,3-113-577 0 0,0-2-52 0 0,0 0-21 0 0,0 0-198 0 0,0 0-824 0 0,0 0-362 0 0,0-1-1274 0 0,-3-5-4833 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94862.106">10396 6829 10016 0 0,'0'0'462'0'0,"0"0"-12"0"0,0 0-148 0 0,1-4 1464 0 0,48-68 3773 0 0,4 11-3387 0 0,-28 50-1432 0 0,-24 10-464 0 0,7 6 586 0 0,-4-1-782 0 0,1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,-2 0 0 0 0,2 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,-2 0 0 0 0,-1-1 0 0 0,2 2 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 3-60 0 0,1 7 248 0 0,14 70 841 0 0,0 7-628 0 0,-23-72-366 0 0,4-21-174 0 0,1-1-11 0 0,0 0-178 0 0,0 0-783 0 0,0 0-344 0 0,0 0-69 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93718.36">10923 6548 3224 0 0,'0'12'2345'0'0,"0"32"5493"0"0,-2 2-4114 0 0,0 50-712 0 0,6 10 343 0 0,-8-87-3334 0 0,2-10-891 0 0,-9 2-7476 0 0,5-9 8097 0 0,4-1-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93135.977">10892 6829 456 0 0,'0'0'1763'0'0,"2"-15"5211"0"0,8-45-1110 0 0,13 42-1851 0 0,24-6-1678 0 0,-39 25-2203 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-2-1 0 0 0,1 2 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 6-132 0 0,21 39 1090 0 0,-24-42-1055 0 0,-2-1 0 0 0,-1 1-1 0 0,2 1 1 0 0,-2 0 0 0 0,0-2-1 0 0,0 1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-1 1 0 0 0,0 0-1 0 0,-2-2-34 0 0,2 12-14 0 0,1-19-184 0 0,0-1-536 0 0,0 0-236 0 0,0 0-888 0 0,0 0-3561 0 0,0 0-1523 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-90762.018">11347 6860 8288 0 0,'-3'9'5575'0'0,"14"3"-3896"0"0,-10-12-1688 0 0,3 2 148 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,2-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,1-2 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-2 0 0 0 0,3 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-3 0 0 0 0,3-1 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,3-4-139 0 0,24-46 514 0 0,-20 27-481 0 0,-7 23-28 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-3-4 0 0,1 5 0 0 0,0-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-60-10 0 0 0,57 10-6 0 0,0 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 2-1 0 0,1-1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-1 1-1 0 0,2 0 1 0 0,-1 0 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-2-2 0 0 0,0 3 6 0 0,-1 0 50 0 0,1 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,0 2-1 0 0,0-1 1 0 0,-1-1 0 0 0,2 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 2 0 0 0,0-1-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,1 0 0 0 0,2 7-51 0 0,-2-8 64 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0-2-1 0 0,1 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-2-2 0 0 0,1-1 1 0 0,2 1-1 0 0,-2 0 0 0 0,0-1 0 0 0,2 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,4 0-64 0 0,34 0-544 0 0,-22-10-5374 0 0,-4 0-1399 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88936.2959">11867 6253 3224 0 0,'-3'17'4649'0'0,"-18"31"2676"0"0,2 38-3229 0 0,2 61-1931 0 0,18-131-1939 0 0,18 122 1016 0 0,14-35-627 0 0,-6-41 597 0 0,-24-60-1196 0 0,-2-1 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 2 1 0 0,2-2-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-2 0 1 0 0,0 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-3 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,1-2 0 0 0,0 2-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1-16 0 0,25-29 176 0 0,12-58-176 0 0,-14 3 0 0 0,-10-12 0 0 0,-4 16 0 0 0,-8-30 0 0 0,-3 7 43 0 0,0 104-266 0 0,0 1-29 0 0,0 0-4 0 0,0 0-141 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1251 0 0,0 0-4804 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87751.59">12365 6397 2304 0 0,'-4'15'3512'0'0,"4"-15"-3295"0"0,1 30 9139 0 0,9 18-4914 0 0,-8-38-4052 0 0,1-1-1 0 0,-1 2 1 0 0,-2-2-1 0 0,1 2 1 0 0,-1 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-2 0 0 0,-1 6-389 0 0,-1 30-162 0 0,2 44 39 0 0,5 33 299 0 0,-2-109 129 0 0,-2-1-2806 0 0,-1-12 1101 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-87470.909">12372 6497 7832 0 0,'0'0'602'0'0,"1"1"-134"0"0,8 1 1838 0 0,31 7 3878 0 0,21-9-2721 0 0,12-8-2874 0 0,-42 7-6863 0 0,-23 1-248 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86426.787">12756 6660 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-128 0 0,1 2-606 0 0,9 96 6111 0 0,-10-23-5043 0 0,-3-8-2402 0 0,2-60 17 0 0,1-5-6835 0 0,0-2 4521 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86230.545">13068 6482 4144 0 0,'0'0'191'0'0,"-5"2"22"0"0,3 1 5833 0 0,-6 18 354 0 0,-9 13-4079 0 0,11 8-269 0 0,7-10-1028 0 0,-4-11-798 0 0,0 1 0 0 0,2-2-1 0 0,-1 1 1 0 0,2 1-1 0 0,3 18-225 0 0,0 68 0 0 0,-10-39 0 0 0,5-58 13 0 0,1-3-3106 0 0,1-8 1973 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85578.149">13245 6712 3224 0 0,'0'15'553'0'0,"6"7"6334"0"0,-12 67 1088 0 0,1-10-6591 0 0,5-64-1121 0 0,0-1-3991 0 0,0-14-2374 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85386.832">13295 6554 17503 0 0,'0'0'776'0'0,"0"0"160"0"0,0 0-744 0 0,0 0-192 0 0,0 0 0 0 0,0 0 0 0 0,0 0 448 0 0,0 0 48 0 0,0 0 16 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1568 0 0,2 11-304 0 0,-2-11-64 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85026.4368">12738 6455 18455 0 0,'0'0'408'0'0,"0"0"80"0"0,0 0 24 0 0,0 0 0 0 0,0 0-408 0 0,0 0-104 0 0,0 0 0 0 0,0 0 0 0 0,0 0 224 0 0,-6 0 16 0 0,6 0 8 0 0,0 0 0 0 0,0 0-992 0 0,0 0-200 0 0,0 0-40 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-83816.66">13599 6561 9584 0 0,'0'0'216'0'0,"-9"5"521"0"0,-46 35 3704 0 0,29-12-975 0 0,23-25-3254 0 0,-2 0 1 0 0,1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,2 2 1 0 0,-2-2-1 0 0,1 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-1 2-1 0 0,1-3 1 0 0,-1 5-213 0 0,2-4 22 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-2 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,2 1 1 0 0,-2 0-1 0 0,0-2 0 0 0,5 5-22 0 0,34 44 54 0 0,-18-36 918 0 0,-21-15-642 0 0,-2-1-115 0 0,8 4 109 0 0,-1 8-171 0 0,-7-10-153 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,-1 0-4 0 0,0 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 5 0 0,-5-19-2397 0 0,9 9 122 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-79727.133">13806 6802 4632 0 0,'0'0'209'0'0,"1"-2"-5"0"0,31-62 6992 0 0,-31 64-6393 0 0,-1 0-31 0 0,20-7 2699 0 0,65 8 1055 0 0,-19-4-2917 0 0,-49 15-1448 0 0,-6 8-150 0 0,-12-20-7 0 0,1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,-1 1 1 0 0,1-2 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 1 1 0 0,-1-1-4 0 0,-10-8 202 0 0,9 7-204 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,2 1 1 0 0,-3 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,-1-1 0 0 0,2 1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,0 1 1 0 0,-2-1-1 0 0,2 1 1 0 0,-2-1 1 0 0,-31 19 268 0 0,29-14-199 0 0,0 1-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 1 0 0 0,2-2 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 2 0 0 0,2-1 0 0 0,-1 0 0 0 0,2-1 0 0 0,0 3 0 0 0,-1-2 0 0 0,1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,1 1-69 0 0,0-4 0 0 0,0 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,3 1 0 0 0,-2-1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 1 0 0 0,54-5-132 0 0,-50-2 154 0 0,-2-1 0 0 0,0-1 1 0 0,2 1-1 0 0,-1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-2 0 0 0,-2 2 0 0 0,0-1 1 0 0,1-1-1 0 0,0 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,3-3-22 0 0,41-62-80 0 0,-36 26 64 0 0,-6-2 16 0 0,2 167 0 0 0,-8-73 0 0 0,4 5 0 0 0,10 12 0 0 0,-4-5-2782 0 0,-6-47 64 0 0,-4 2-4789 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76952.167">14790 6870 2304 0 0,'0'0'464'0'0,"-1"1"2357"0"0,-5 7-1769 0 0,6-6 3151 0 0,0-1 4184 0 0,28 14-5739 0 0,-22-14-2588 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,2 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-2-1 1 0 0,2 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-2 0-1 0 0,3-3-59 0 0,5-7-111 0 0,-6 10 95 0 0,-2-2 0 0 0,2 1 0 0 0,-2-1 1 0 0,2 0-1 0 0,-2 1 0 0 0,-2-1 0 0 0,3 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0-2 16 0 0,-2 4-53 0 0,0-1 0 0 0,0 2-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,1 0 0 0 0,-3-1 0 0 0,2 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1-1 0 0,-3-2 54 0 0,4 4-6 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 2 1 0 0,2-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 1 1 0 0,1-2-1 0 0,1 2 1 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 2 1 0 0,0-2-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-2 1 0 0 0,2 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-2 0 7 0 0,-2 7 93 0 0,-1 2 0 0 0,0-1 0 0 0,1 1 0 0 0,1-2 0 0 0,0 2 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,3-1 0 0 0,-1-1 0 0 0,1 3 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,2-1 0 0 0,5 12-93 0 0,-7-20 0 0 0,0 2 0 0 0,0-1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 1 0 0 0,0-2 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,3 0 0 0 0,-2-1-22 0 0,10-6-6424 0 0,-10-3-869 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77950.2428">14405 6387 1840 0 0,'0'0'307'0'0,"0"-2"615"0"0,-2-30 3370 0 0,2 32-4103 0 0,0 0-1 0 0,0 0 44 0 0,0 0 22 0 0,0 0 2 0 0,0 0 74 0 0,0 0 316 0 0,0 0 142 0 0,0 1 32 0 0,7 63 3244 0 0,-7 76 861 0 0,0 72-1667 0 0,4-85-1971 0 0,5 65-363 0 0,-8-148-963 0 0,-2-26-3502 0 0,1-18 1678 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-77348.9">14399 6536 13504 0 0,'0'0'620'0'0,"0"0"-16"0"0,4-6-364 0 0,17-4 1491 0 0,-16 7-1438 0 0,-1 1 0 0 0,1 1 0 0 0,-2-2 0 0 0,3 2 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1-293 0 0,80 6 662 0 0,-41 7-2436 0 0,-19-7-4491 0 0,-15 1 465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-76210.45">15343 6606 1840 0 0,'0'0'583'0'0,"-2"1"2720"0"0,-5 1-1116 0 0,-24 24 7260 0 0,26-18-9058 0 0,2 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-2-1 0 0,2 1 0 0 0,0 1 0 0 0,0 8-389 0 0,-4 51 2048 0 0,13 43-1440 0 0,-7-105-566 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 2 0 0 0,0 1-42 0 0,-2-6 48 0 0,-1-1 1 0 0,-1-1-1 0 0,1 1 0 0 0,1 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-2-1 0 0 0,3 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 0-48 0 0,8-7 0 0 0,-3 2 0 0 0,1-1 0 0 0,-2-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,4-10 0 0 0,20-46 0 0 0,-1-11 0 0 0,-26 55 0 0 0,-3 16 0 0 0,-6 1-177 0 0,-9 13-4614 0 0,9-6-2832 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-72325.515">15806 6591 3224 0 0,'0'0'143'0'0,"0"0"-3"0"0,5 0 2973 0 0,-4-1 7737 0 0,-5 4-3072 0 0,4 4-10123 0 0,0 28 3033 0 0,0-8 1192 0 0,0-26-1368 0 0,0 1 0 0 0,-17 79 715 0 0,8-15-1010 0 0,3-12-308 0 0,23 77-94 0 0,-13-94 185 0 0,-7-31-139 0 0,3-5-580 0 0,0-1-251 0 0,0-1-1544 0 0,3-8-6015 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45518.415">17508 6634 8288 0 0,'0'139'4740'0'0,"0"-122"-3699"0"0,0 13 42 0 0,0 3 0 0 0,1-1 0 0 0,2-2 1 0 0,1 2-1 0 0,7 21-1083 0 0,2-11-70 0 0,-6-27-1026 0 0,-5-14-85 0 0,-2-1-45 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45023.887">17885 6609 1376 0 0,'0'0'299'0'0,"0"0"715"0"0,0 0 313 0 0,0 0 66 0 0,-11-7 1242 0 0,7 6-2367 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-3 0 0 0 0,2-1 1 0 0,0 2-1 0 0,-2 1-268 0 0,-46 91 3206 0 0,48-88-3121 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,2 1 0 0 0,0 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-1-1 0 0 0,0 2 0 0 0,0-1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,2-2 0 0 0,-2 2 0 0 0,2-1-1 0 0,0 0 1 0 0,1 1-85 0 0,72 39 528 0 0,-76-45-518 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,-1-2 1 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 1-1 0 0,1-2 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1-9 0 0,-1 2-25 0 0,1-1 0 0 0,-3 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,1 1 0 0 0,-1-2 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-2 0 0 0,0 1 0 0 0,1 0 0 0 0,-3-1 25 0 0,-9-14-3267 0 0,10 6-3203 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22924.697">15806 6798 920 0 0,'-5'10'80'0'0,"-5"7"5114"0"0,9-16-3500 0 0,1-1-770 0 0,0 0-336 0 0,0 0-68 0 0,0 0-20 0 0,0 0-51 0 0,0 0-22 0 0,0 0-3 0 0,0 0 25 0 0,0 0 107 0 0,0 0 48 0 0,0 0 11 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,7-22 5642 0 0,27-29-4223 0 0,12 17-1739 0 0,-41 33-286 0 0,2 2 1 0 0,5 10 96 0 0,-8-5-97 0 0,-4-5-115 0 0,2 1 1 0 0,-2 0-1 0 0,0-1 0 0 0,1-1 0 0 0,0 2 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 105 0 0,10 2-1084 0 0,13-1-5055 0 0,-19-1 4517 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23746.448">16329 6503 1376 0 0,'0'0'331'0'0,"0"0"853"0"0,0 0 380 0 0,0 0 71 0 0,0 0-79 0 0,0 0-405 0 0,0 0-178 0 0,0 0-39 0 0,0 0-42 0 0,0 0-151 0 0,0 0-65 0 0,0 0-17 0 0,0 0 26 0 0,0 0 124 0 0,0 0 58 0 0,0 0 11 0 0,0 0-43 0 0,0 0-192 0 0,0 0-89 0 0,-15-3 1062 0 0,-28 17 904 0 0,-10 37-429 0 0,5 34-1643 0 0,26-37-267 0 0,5 50 275 0 0,13 17 391 0 0,10-81-660 0 0,-6-26-158 0 0,1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 2 0 0 0,-1-2 0 0 0,0-1 0 0 0,2 2-1 0 0,0-2 1 0 0,-1 1 0 0 0,4 1-29 0 0,21 26 0 0 0,-19-29-4 0 0,-7-4-118 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 2-1 0 0,1-2 1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,0 0 0 0 0,2-1-1 0 0,-2 0 1 0 0,0 1 0 0 0,0-2 122 0 0,26-18-6775 0 0,-22 12 184 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24081.144">16430 6680 456 0 0,'12'-36'1833'0'0,"8"16"8000"0"0,-7 3-4338 0 0,-12 16-4746 0 0,-1 1-12 0 0,8 1 2655 0 0,-3 4-3184 0 0,-2-1 0 0 0,2 0 0 0 0,-2 1-1 0 0,0 1 1 0 0,0-2 0 0 0,-1 1 0 0 0,2 1-1 0 0,-2-1 1 0 0,0 2 0 0 0,0-3-1 0 0,1 2 1 0 0,-3 0 0 0 0,1-1 0 0 0,0 2-1 0 0,0-2 1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 6-208 0 0,0-5 187 0 0,1 171 1174 0 0,-8-103-1017 0 0,-7-6-212 0 0,10-61-136 0 0,4-3 10 0 0,-2 1 0 0 0,1-2 0 0 0,-1 1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-2 0 1 0 0,2-1 0 0 0,-2 1 0 0 0,1-1-1 0 0,-2 1-5 0 0,-7 5-315 0 0,-29 24-6531 0 0,30-27 5010 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28120.561">16565 6082 4608 0 0,'3'-4'886'0'0,"1"-3"-1808"0"0,-3 2 5374 0 0,-1-4 4827 0 0,16 10-6424 0 0,-8 3-2408 0 0,-3 2 1 0 0,2-1-1 0 0,0 0 1 0 0,-1 1-1 0 0,-1 0 0 0 0,2 1 1 0 0,-1-2-1 0 0,-2 2 0 0 0,1-1 1 0 0,-1 2-1 0 0,3 2-447 0 0,10 27 1006 0 0,15 73 508 0 0,-22-24-882 0 0,5 241 416 0 0,-15-51-535 0 0,-11-45 14 0 0,-3 6-74 0 0,0-143-389 0 0,0-25 75 0 0,13-64-128 0 0,-19 0 223 0 0,-111-34-95 0 0,88 25-75 0 0,-6 9 28 0 0,-2-3 1 0 0,2-2-1 0 0,-22-4-92 0 0,-38-14 67 0 0,-157-70-67 0 0,235 81-114 0 0,-1 1 1 0 0,1 2-1 0 0,-1 2 0 0 0,-1 1 0 0 0,2 2 1 0 0,-1 1-1 0 0,-15 4 114 0 0,-540 87 796 0 0,84-35-796 0 0,14 1 0 0 0,202-19 0 0 0,-11-8 0 0 0,-203-12 0 0 0,-386-18 0 0 0,575 7 0 0 0,-273-34 0 0 0,-67-19 0 0 0,150 26-457 0 0,-210-2 202 0 0,254-4-1 0 0,-144 19 256 0 0,305 4 172 0 0,-70 0 164 0 0,29-16-196 0 0,62 17 180 0 0,83 1-722 0 0,-29 1 8 0 0,-185-5 478 0 0,138-5 308 0 0,26-9-72 0 0,-240-16-1032 0 0,314 18 852 0 0,-70-8 432 0 0,-131-7-572 0 0,166 13 0 0 0,-38 20 0 0 0,-54-8 0 0 0,77-4 0 0 0,-84 33 0 0 0,22 14 0 0 0,119-50 0 0 0,14 20 0 0 0,53-1 0 0 0,91-6-20 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,-2-1-1 0 0,2 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,2-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,2-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,3-1 20 0 0,-30-47-115 0 0,-7-64 687 0 0,-14-92-572 0 0,-19-90 0 0 0,46 49 0 0 0,-3 79 0 0 0,-4-20 0 0 0,22 75-796 0 0,9 24 1592 0 0,12 19-796 0 0,28-25 0 0 0,-34 84 0 0 0,1 2 0 0 0,0 0 0 0 0,-1-1 0 0 0,3 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 2 0 0 0,0 0 0 0 0,9-8 0 0 0,68-38 0 0 0,79-25 0 0 0,-138 70 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 2 0 0 0,-1 1 0 0 0,0 2 0 0 0,1 1 0 0 0,9 1 0 0 0,-35 1 0 0 0,119 0 0 0 0,0-4 0 0 0,27-10 0 0 0,23-14-712 0 0,83-20 1413 0 0,-152 32-697 0 0,0 4-1 0 0,1 6 1 0 0,61 5-4 0 0,270 19 0 0 0,-111-2 0 0 0,-257-11-72 0 0,2 1 1 0 0,-2 3-1 0 0,47 15 72 0 0,76 8-105 0 0,-62-22 425 0 0,56 13-320 0 0,-48 3 0 0 0,62 15 0 0 0,73 2 0 0 0,50 23 0 0 0,-169-28 0 0 0,50-2 0 0 0,42 4-796 0 0,-84-6 1592 0 0,3-10-831 0 0,8-28-250 0 0,-30 4 605 0 0,54 10-320 0 0,-90-7 0 0 0,82-20 0 0 0,-38-2 0 0 0,129 14 0 0 0,-179 5 0 0 0,-2-6 0 0 0,66-10 0 0 0,49-7 0 0 0,127 6 0 0 0,-37-5 0 0 0,-137 4 0 0 0,212 0 0 0 0,-97 16 0 0 0,99-20 0 0 0,79-11 0 0 0,-310 26 0 0 0,16-1 0 0 0,243 3 0 0 0,-132 15 0 0 0,-54-3 0 0 0,111-21 0 0 0,10 21 0 0 0,-199 0 0 0 0,6-11 0 0 0,-12-3 0 0 0,-16 7 0 0 0,9 4 0 0 0,30-11 0 0 0,55 14 0 0 0,-70 7 0 0 0,-75-16 0 0 0,157-4 0 0 0,-63 22 0 0 0,-79-6 0 0 0,47-2 0 0 0,-43 3 0 0 0,143 13 0 0 0,-57-9 0 0 0,-66 0 0 0 0,63 2 0 0 0,-74-15 0 0 0,34-5 0 0 0,-37 27-4336 0 0,-35-5-1782 0 0,-41-15-3483 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29020.976">16222 5833 1376 0 0,'0'0'591'0'0,"0"0"1942"0"0,0 0 851 0 0,0 0 174 0 0,0 0-327 0 0,-12 9 6223 0 0,15-6-9289 0 0,2 1 0 0 0,-2-2 0 0 0,0 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 2 1 0 0,1-2 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,1-1-165 0 0,1 2 87 0 0,103 16 1139 0 0,-5 23-943 0 0,-58-24-166 0 0,5-26 11 0 0,-19 8-64 0 0,-16 18-64 0 0,-9 18 13 0 0,-7 4 198 0 0,-2 59 157 0 0,4-5-616 0 0,-1-32-3854 0 0,1-35-5107 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-134780.1889">8440 7721 1376 0 0,'0'0'65'0'0,"0"0"189"0"0,0 0 767 0 0,0 0 335 0 0,0 0 69 0 0,0 0-94 0 0,0 8 1469 0 0,-2 73 3116 0 0,4-16-3609 0 0,-14 104-383 0 0,11-29-438 0 0,1-61-917 0 0,-3 0 598 0 0,2 105-205 0 0,-7 5-322 0 0,13 97-40 0 0,-2-186-336 0 0,-3 19 8 0 0,10 121 323 0 0,5-6 583 0 0,-4-62-1855 0 0,-5 87 952 0 0,0-54-94 0 0,-5-145-117 0 0,4-4-2277 0 0,-2-79-5567 0 0,-3 9 286 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-134240.1889">7932 9898 5528 0 0,'0'0'422'0'0,"0"0"-88"0"0,0 0 656 0 0,0 17 2881 0 0,10 38-2527 0 0,8 41 2164 0 0,22-10-466 0 0,74 130 109 0 0,-76-151-2761 0 0,-29-45-296 0 0,2 0 0 0 0,1-2 1 0 0,0 1-1 0 0,1 0 1 0 0,0-2-1 0 0,2-1 1 0 0,1 1-1 0 0,11 10-94 0 0,62 22 544 0 0,-85-46-475 0 0,1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,1-1 0 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0 1 0 0,-2 0-1 0 0,2-1 0 0 0,-2 1 0 0 0,2-1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,2-1 0 0 0,2-2-69 0 0,30-39 176 0 0,88-241 1624 0 0,-36 89-1872 0 0,-46 74-576 0 0,-25 67-2737 0 0,-11 40 1634 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-125200.19">3277 10742 13128 0 0,'0'-16'633'0'0,"0"15"-277"0"0,0 8 83 0 0,13 223 3164 0 0,19-12-1187 0 0,-7-1-1552 0 0,-27-127-897 0 0,-14-32-3046 0 0,13-49 1239 0 0,-4-4-71 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-124660.19">3197 10730 7056 0 0,'-2'-5'116'0'0,"1"0"0"0"0,0-1 1 0 0,0 1-1 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,2-3-117 0 0,1-6 1073 0 0,-4 11-878 0 0,2 2 0 0 0,0-1-1 0 0,1-1 1 0 0,-1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,0 2 1 0 0,-2-2 0 0 0,3 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-1-1 0 0,1 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0-1 0 0,-3 1 1 0 0,5-1-195 0 0,-2 1 85 0 0,1 1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-1-1 0 0 0,3 3-85 0 0,44 48 670 0 0,-23-20 265 0 0,21 38 175 0 0,-44-59-1010 0 0,-2 0 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,-2 1 1 0 0,0 0-1 0 0,-2 1 0 0 0,0-1 1 0 0,0-1-1 0 0,1 1 0 0 0,-3-1 0 0 0,1 2 1 0 0,-2-3-1 0 0,-2 9-100 0 0,2-11 186 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,-2 0 0 0 0,2 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-4 0-186 0 0,7-5 12 0 0,1-1 0 0 0,-2 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0-1-11 0 0,-40 6 164 0 0,45-5-225 0 0,17 13-71 0 0,36 32 57 0 0,-30-20 68 0 0,55 78 132 0 0,0 47-125 0 0,-39-70-5360 0 0,-33-61 3443 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-123330.19">3989 11417 6912 0 0,'0'0'528'0'0,"0"0"-219"0"0,0 0 347 0 0,0 1 192 0 0,12 10 3088 0 0,47-14-2645 0 0,21-33-467 0 0,-29 5 415 0 0,-49 28-1110 0 0,0 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,0-1-128 0 0,-27-40 870 0 0,22 42-830 0 0,1 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-2 0 0 0 0,1 0-1 0 0,1-1 1 0 0,-2 2 0 0 0,1-1-1 0 0,-1 2 1 0 0,2-1-1 0 0,-2 0 1 0 0,0 1 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,2 1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-2 2-1 0 0,0-2 1 0 0,2 1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-2 1 0 0 0,1 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,2 0-1 0 0,0-2 1 0 0,-3 5-41 0 0,1 0 30 0 0,2 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,1-1 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 2-30 0 0,19 105 84 0 0,-17-108-98 0 0,2-1 0 0 0,-1 2 0 0 0,2-2 0 0 0,-3 1 0 0 0,3-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-2 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,2-2 1 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,1-2 0 0 0,1 0-1 0 0,-3 0 1 0 0,3-1 0 0 0,-1 0 0 0 0,2 0 14 0 0,7 0-1085 0 0,-1-1-349 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122830.19">4538 11026 920 0 0,'1'2'67'0'0,"6"15"218"0"0,-7-15 1126 0 0,0-2 485 0 0,0 0 95 0 0,0 0-144 0 0,0 0-698 0 0,0 0-306 0 0,3 15 5156 0 0,4 70-3006 0 0,0 144-2907 0 0,16-67 348 0 0,-10-99-1540 0 0,-8-56-81 0 0,-2-4-3107 0 0,-3-1-1448 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-122530.19">4538 11111 5984 0 0,'0'0'464'0'0,"0"0"-82"0"0,11 12 5502 0 0,36-2-3006 0 0,31-10-1919 0 0,-24-4-2545 0 0,-42 4-3811 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2419.811">7889 10988 1840 0 0,'0'0'83'0'0,"0"7"10"0"0,-4-1 194 0 0,-3 5 6325 0 0,-1 3-4677 0 0,5-8-1065 0 0,-4 26 3503 0 0,10 50-1185 0 0,1 47-2006 0 0,1-56-326 0 0,3-43-586 0 0,22 44 628 0 0,-28-72-870 0 0,2 0 0 0 0,-2 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-2 1-1 0 0,1 0 1 0 0,1 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,2-1-28 0 0,4-5 21 0 0,0-2 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,-2 1 1 0 0,1-2-1 0 0,0 0 0 0 0,2-7-21 0 0,23-44 0 0 0,-9-12 1099 0 0,1-25-934 0 0,-18 7-165 0 0,-1 62 0 0 0,-8-39 0 0 0,3 23-283 0 0,2 27-8605 0 0,-1 19 2172 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3219.811">8445 10927 8288 0 0,'-10'70'3321'0'0,"9"22"1356"0"0,2-7-2700 0 0,1-30-1241 0 0,1 133 440 0 0,-3-173-966 0 0,8 44-294 0 0,-7-58-163 0 0,-1-1-857 0 0,0-2-3536 0 0,0-5-1518 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3409.81">8428 11026 8288 0 0,'0'0'638'0'0,"7"-4"2018"0"0,19-1 1429 0 0,16 16-2828 0 0,-26-6-864 0 0,31 23-411 0 0,-40-23-355 0 0,13 20-3587 0 0,-11-15 2594 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3629.811">8816 11243 3680 0 0,'0'0'284'0'0,"3"9"797"0"0,-1-6 4784 0 0,0 31-1677 0 0,0 5-3145 0 0,-3 38-251 0 0,5-15-1216 0 0,-4-46-1299 0 0,0-7-3631 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4049.811">9101 11026 920 0 0,'-4'-14'343'0'0,"4"11"1102"0"0,0 3 482 0 0,0 0 96 0 0,0 0-124 0 0,0 0-614 0 0,0 0-269 0 0,0 0-50 0 0,0 0-57 0 0,0 0-212 0 0,0 0-90 0 0,0 2-20 0 0,-1 35 1508 0 0,-5 38-993 0 0,-5 83 402 0 0,7-57-494 0 0,12 57-140 0 0,2-75-1121 0 0,-10-82-772 0 0,0-1-333 0 0,0 0-68 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4549.811">9388 11338 456 0 0,'-5'20'0'0'0,"5"-19"651"0"0,-2 1 4741 0 0,-1 0 3820 0 0,3 2-9813 0 0,2 173 4824 0 0,3-125-4491 0 0,-5-47-754 0 0,0-4-326 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5199.81">9710 11311 10136 0 0,'0'0'464'0'0,"-2"0"-10"0"0,-4 0-222 0 0,-13 14 3123 0 0,18-13-3266 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1-89 0 0,23 51-256 0 0,-14-29 538 0 0,36 27 412 0 0,-14 4-275 0 0,-28-19-94 0 0,-19 3 1227 0 0,3-23-785 0 0,-14 3 957 0 0,14-16-1575 0 0,-9-3-133 0 0,-5-17-2201 0 0,23 11-250 0 0,2 4-4568 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6589.811">9980 11562 10136 0 0,'6'15'230'0'0,"-5"-11"30"0"0,-1-4 19 0 0,3-7 478 0 0,4-34 763 0 0,-5 39-1014 0 0,-1-2-2 0 0,7-25 334 0 0,-7 23-761 0 0,0 1 1 0 0,1 0 0 0 0,-1-1-1 0 0,2 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,2 0-78 0 0,-4 4 167 0 0,28-16 1024 0 0,-27 16-1129 0 0,1 1 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-2 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-2-1 0 0,1 1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0-61 0 0,25 31 1857 0 0,-26-32-1723 0 0,-1-1-46 0 0,0 0-22 0 0,0 0-2 0 0,0 0 2 0 0,0 0 4 0 0,-23 0 2 0 0,20 0-87 0 0,-2 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 3 0 0 0,-1-2 1 0 0,1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,2-1 1 0 0,1 1-1 0 0,-4 1 16 0 0,-24 16-85 0 0,28-19 77 0 0,1 0 0 0 0,-2 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,0-2 0 0 0,-2 2 0 0 0,2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0 2 8 0 0,11 31-54 0 0,-11-33 57 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,2 1 0 0 0,-2-2 0 0 0,0 2 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-3 0 0,47 5 163 0 0,-42-9-205 0 0,-2 0-1 0 0,1-1 1 0 0,-2 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-2-1 0 0,-1 2 1 0 0,0-2 0 0 0,0 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-2 1 0 0,-1 2 0 0 0,-2-1-1 0 0,3 0 1 0 0,-2-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1-1 0 0 0,1 3-1 0 0,-2-5 43 0 0,7-70-556 0 0,-7 80 622 0 0,0 1 34 0 0,0 0 10 0 0,-1 3-16 0 0,0 12 66 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,3 10-160 0 0,2 26 76 0 0,15 27 0 0 0,-13-38-1057 0 0,-8-37-90 0 0,6 8-37 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7129.81">10564 11129 456 0 0,'0'-23'204'0'0,"0"11"5674"0"0,-3 12 1245 0 0,-5 25-4666 0 0,-3 54-110 0 0,11 96-830 0 0,-4 72-628 0 0,14-186-907 0 0,-9-55 2 0 0,-1-6-2564 0 0,0 0 1298 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7369.81">10528 11277 8752 0 0,'5'8'936'0'0,"12"-24"1798"0"0,41 16 2614 0 0,33 4-4455 0 0,-51 13-4124 0 0,-32-13 2047 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7929.811">10949 11631 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,2 1-40 0 0,38-7 2129 0 0,-16-1-968 0 0,-21 6-1318 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-2-1-1 0 0,2 0-82 0 0,7-9 268 0 0,-5 10-243 0 0,-2-2 1 0 0,0 0 0 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 3 1 0 0,-1-2 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 1-1 0 0,3-1 1 0 0,-2 1-1 0 0,-1-2 1 0 0,0 2 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-1 0 0,-5-4-25 0 0,6 6 20 0 0,-2 1 0 0 0,2-2-1 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,-3 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1 0 0 0,0-1-1 0 0,1-1 1 0 0,0 2-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 1 1 0 0,0-2-20 0 0,-5 11 226 0 0,0 0-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,1 0-1 0 0,1 2 1 0 0,0 0 0 0 0,1-1 0 0 0,0 1-1 0 0,2 4-225 0 0,-2-13 37 0 0,2 2 31 0 0,0-1-1 0 0,0 2 0 0 0,2-1 1 0 0,-2 0-1 0 0,1-1 0 0 0,0 2 1 0 0,1-1-1 0 0,-1-1 0 0 0,2 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,2-1 1 0 0,-1 0-1 0 0,1 1-67 0 0,-1-3 33 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,4 0-33 0 0,42 8-313 0 0,-11-16-1742 0 0,-29 6 191 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8439.811">11422 11411 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,-11 3 2224 0 0,2 9-1481 0 0,7-10-561 0 0,2-2 0 0 0,-1 1 0 0 0,-31 39 1128 0 0,30-38-1631 0 0,1 2 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1-2 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-9 0 0,0 20 74 0 0,-1-18-14 0 0,0 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,1-2-1 0 0,-1 3 1 0 0,0-2 0 0 0,1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0 0 0 0,2 2-1 0 0,-2-2 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 0 0 0 0,-1-1-1 0 0,2 1-59 0 0,58 34 164 0 0,-59-37-163 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1-2 1 0 0,0 2-1 0 0,2 0 1 0 0,-2-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,1-1 0 0 0,26-39 0 0 0,-2-28 0 0 0,-21 40 0 0 0,-6-44 0 0 0,0 66 0 0 0,0 10-1 0 0,0 0 0 0 0,0-1 0 0 0,-2 1-1 0 0,2 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 2 0 0,-2 2-86 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,2 6 86 0 0,9 44-6882 0 0,-4-44 1085 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8909.811">11995 11266 3224 0 0,'4'18'240'0'0,"-19"12"5162"0"0,-6 23 1702 0 0,1 33-4883 0 0,11-47-1389 0 0,5 24 96 0 0,-2-23-476 0 0,6 22 178 0 0,-4 7-648 0 0,1-58 50 0 0,-1-6-3037 0 0,4-5 1818 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9219.811">11942 11492 10136 0 0,'1'10'1085'0'0,"47"-46"1390"0"0,-45 33-2239 0 0,1-1 0 0 0,0 1 0 0 0,-2 0 1 0 0,3 1-1 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,4-1-236 0 0,29-14 608 0 0,-10 30 520 0 0,-10 5-434 0 0,-14-18-580 0 0,15 13-10 0 0,-17-11-96 0 0,13 21-8 0 0,-13-19-92 0 0,-1-3-390 0 0,0 8-1954 0 0,3-2-3569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12429.81">12555 11141 2304 0 0,'0'0'101'0'0,"1"-2"1"0"0,0-5-3003 0 0,0 2 4359 0 0,-5-3 14711 0 0,-5 14-13468 0 0,5-3-2385 0 0,1 1 0 0 0,2-1 0 0 0,-3 2 0 0 0,2-1 0 0 0,0-1 0 0 0,-2 0 0 0 0,3 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-2 0 0 0,1 5-316 0 0,-1 100 1202 0 0,2-98-965 0 0,3 41-228 0 0,1 1 0 0 0,2-1 1 0 0,3-1-1 0 0,2 1 0 0 0,8 19-9 0 0,-10-40 0 0 0,-3-21 0 0 0,19 2-1058 0 0,11-31-4850 0 0,-25 10 3794 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12789.811">12907 11049 1376 0 0,'0'0'65'0'0,"0"0"454"0"0,0 0 1882 0 0,5 0 5023 0 0,3 0-3511 0 0,-5 2-3615 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-2 0 0 0 0,3 3-297 0 0,27 51 2384 0 0,-5-9-1738 0 0,-16-34-400 0 0,0 3 0 0 0,-1 0-1 0 0,-1-1 1 0 0,1 2 0 0 0,-3 0-1 0 0,0 1-245 0 0,15 119 608 0 0,-16 67 104 0 0,-12-64-61 0 0,1-93-3304 0 0,-4-5-3362 0 0,8-31-807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16819.8098">13524 12506 3224 0 0,'0'0'143'0'0,"0"0"327"0"0,0 0 1271 0 0,0 0 550 0 0,0 0 114 0 0,0-3 988 0 0,1-10-1052 0 0,0-56 2752 0 0,7-1-2899 0 0,10-98-927 0 0,5-52-315 0 0,-9 78 489 0 0,-4-104-1441 0 0,-8 154 170 0 0,2 8 86 0 0,2-1-1 0 0,9-36-255 0 0,5-26 592 0 0,-7 25-253 0 0,-9 22 96 0 0,4 49-99 0 0,5-14-403 0 0,-1 36 67 0 0,-6 13 13 0 0,-2-2 79 0 0,-8 8 139 0 0,-6-10-231 0 0,9 18 5 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1-5 0 0,-120 3 320 0 0,62 1-256 0 0,-61 5 61 0 0,-237 12 207 0 0,44 3-320 0 0,13 14 52 0 0,27 17-64 0 0,-274 58 128 0 0,351-89-117 0 0,78-14 98 0 0,-2-5 0 0 0,-33-7-109 0 0,20 0-2 0 0,-75-5 367 0 0,-86 2-133 0 0,-26-6-541 0 0,102-4 706 0 0,-13 1-710 0 0,55 4 634 0 0,-184 0-321 0 0,198-3-16 0 0,-36 0-155 0 0,-38-9 182 0 0,-111-12 65 0 0,203 23-88 0 0,-24 4 12 0 0,-49 4 64 0 0,18 0-64 0 0,-55-7 0 0 0,-313-32 64 0 0,390 28-64 0 0,-278-10 0 0 0,399 25 0 0 0,-147-10 0 0 0,70-6 0 0 0,-40-6 0 0 0,-24 0 0 0 0,-104 15 0 0 0,202 9 0 0 0,-51-17 0 0 0,29-5 0 0 0,86 15 0 0 0,0 1 0 0 0,-2 2 0 0 0,-34 4 0 0 0,-10 0 0 0 0,-237 8-11 0 0,118-36 22 0 0,-88-19-11 0 0,-47 40-64 0 0,256-5 128 0 0,55 8-64 0 0,-1 0 0 0 0,1-2 0 0 0,-1-2 0 0 0,-22-6 0 0 0,31 6 0 0 0,5 0 0 0 0,1 2 0 0 0,-1-2 0 0 0,0 3 0 0 0,0-1 0 0 0,0 2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,-4 1 0 0 0,4 2 0 0 0,9-4 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2 1 0 0 0,3-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-2 3 0 0 0,-14 71-244 0 0,43 144 168 0 0,-3-63 299 0 0,31 231-446 0 0,-5-29 520 0 0,0-180-530 0 0,-22-86 233 0 0,19 51 0 0 0,11-7 0 0 0,-45-120 0 0 0,57 78 0 0 0,-51-83 4 0 0,0 0 0 0 0,1-3 0 0 0,0 1 0 0 0,2-2-1 0 0,-1-2 1 0 0,0 2 0 0 0,0-4 0 0 0,2 1 0 0 0,5 0-4 0 0,27 12 140 0 0,84 14-242 0 0,-15-9 207 0 0,93 3-105 0 0,-82-10-23 0 0,75 1-132 0 0,6-7 155 0 0,479 21 0 0 0,-136-9 0 0 0,-59 2 0 0 0,82-20 53 0 0,-67-40-42 0 0,-153-17-11 0 0,45 10 0 0 0,-175 27 12 0 0,-11 9 112 0 0,93-7-204 0 0,49 20 149 0 0,15-8-58 0 0,-5-10-107 0 0,11 0 96 0 0,-169 4 96 0 0,108 12-192 0 0,-225 15 96 0 0,43-2 0 0 0,34-2 144 0 0,-52-18-240 0 0,4-2 192 0 0,-86 6-96 0 0,-1-1 0 0 0,2-3 0 0 0,-2-1 0 0 0,34-7 0 0 0,26-5-96 0 0,33 8 96 0 0,106 3 0 0 0,-116-10 80 0 0,-34 5-160 0 0,96-8 80 0 0,-75 20 11 0 0,85-17 42 0 0,-91-4-141 0 0,-16-6 94 0 0,0 3 0 0 0,61-5-6 0 0,-41 12 60 0 0,-1 13-60 0 0,41 36 0 0 0,-51-17 0 0 0,-84-16 0 0 0,21 13 0 0 0,-26-8 59 0 0,-5-6-111 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 52 0 0,-5 5-1004 0 0,5-5-3898 0 0,1-1 2712 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25749.8098">16999 6377 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0-11 1147 0 0,0 7-3619 0 0,1-4 9257 0 0,0 5 2091 0 0,-1 8-7632 0 0,13 194 1589 0 0,-17-104-2526 0 0,-5-6-90 0 0,4-7-182 0 0,14 8-118 0 0,-1-43-2244 0 0,-7-46 1548 0 0,-1-1-185 0 0,0 0-84 0 0,0 0-21 0 0,3 4-3895 0 0,-3-4 2635 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26679.8098">17024 6809 5672 0 0,'0'0'257'0'0,"0"0"-2"0"0,0 0-22 0 0,0-14 2511 0 0,14-73 5565 0 0,-2 62-6834 0 0,9 0-281 0 0,-5 8-550 0 0,-15 16-517 0 0,-1 1-6 0 0,3 0 3 0 0,20 7 472 0 0,-1 13 14 0 0,10 54 396 0 0,7 62-438 0 0,-28-83-450 0 0,-11-26-1627 0 0,0-12-6318 0 0,0-5 1470 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37589.811">14230 11330 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,4-8 1867 0 0,-3 7-1852 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-240 0 0,-5-2 274 0 0,-1-1-1 0 0,2-1 1 0 0,-1 2 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0-1 0 0,-1 1 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,-2 2-273 0 0,-9 5 0 0 0,11-1 0 0 0,-26 34 0 0 0,24-25 150 0 0,1 1 1 0 0,0 1-1 0 0,1-1 0 0 0,0 2 0 0 0,1-1 0 0 0,1 2 0 0 0,1-2 0 0 0,0 1 0 0 0,1 1 0 0 0,1-1 1 0 0,1 0-1 0 0,1 2 0 0 0,0 4-150 0 0,-1-2 104 0 0,-15 209-482 0 0,9-121 567 0 0,9-13-136 0 0,-1-96-229 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0 176 0 0,7-4-1901 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37999.811">13904 11641 5984 0 0,'0'0'464'0'0,"0"0"-100"0"0,0 0 717 0 0,0 0 346 0 0,0 0 69 0 0,0 0-71 0 0,0 0-330 0 0,0 0-146 0 0,6 12 1624 0 0,-2-8-2296 0 0,0 0 0 0 0,-1-1 0 0 0,1 2 0 0 0,-1-2-1 0 0,2 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1 0 0 0,5-1-277 0 0,15 9 296 0 0,19 0 73 0 0,-36-7-712 0 0,21 11-175 0 0,-13 3-5552 0 0,-8-3-166 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38309.811">14202 11990 6624 0 0,'0'0'298'0'0,"0"0"-3"0"0,0-2-188 0 0,25-54 3721 0 0,-17 42-2931 0 0,-7 12-725 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,2 1 0 0 0,-2 0 1 0 0,1-1-173 0 0,0 2 83 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,3 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 1 1 0 0,-1-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 2-83 0 0,3 2 241 0 0,1 1 0 0 0,-2 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,1 1 0 0 0,-2 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 7-241 0 0,-4 52 1376 0 0,-4-49-782 0 0,7-17-550 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,1 1-44 0 0,-2-2-23 0 0,-1 0-1 0 0,2 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-2 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,0-1-1 0 0,2 1 0 0 0,-1-2 1 0 0,-1 1-1 0 0,3 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1-2 24 0 0,-13-42-1750 0 0,9 21 132 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="39549.811">14618 11965 4608 0 0,'0'0'101'0'0,"-3"-4"150"0"0,2-1-50 0 0,1 4 308 0 0,0 1 135 0 0,0-1 27 0 0,-2-38 1126 0 0,2 38-1534 0 0,0 1-330 0 0,0 0-71 0 0,0 0 38 0 0,0 0 152 0 0,0 0 68 0 0,0 0 9 0 0,0 1-17 0 0,2 1-16 0 0,-2-1 280 0 0,0-1 113 0 0,0 0 21 0 0,0 0-68 0 0,0 0-262 0 0,0 0-9 0 0,-1 7 712 0 0,0-7-575 0 0,1 0 4 0 0,0 0 26 0 0,0 0 113 0 0,0 0 49 0 0,0 0 11 0 0,0 0-57 0 0,0 0-239 0 0,0 0-102 0 0,0 0-17 0 0,0 0 18 0 0,0 0 99 0 0,0 0 47 0 0,0 0 11 0 0,0 0 0 0 0,0 0 1 0 0,0 0 0 0 0,2 7 268 0 0,9 25 656 0 0,-7 19 132 0 0,8 16 242 0 0,-6-34 28 0 0,-6 37-1582 0 0,-5-25-16 0 0,5-35 0 0 0,1-86 1117 0 0,-2 35-1650 0 0,6-51 37 0 0,-9 0 27 0 0,16 61 834 0 0,-9 24-365 0 0,23-7-1090 0 0,-25 14 1590 0 0,0 1-59 0 0,52 47-276 0 0,-20-3-165 0 0,-12-1 0 0 0,2 10 0 0 0,-14-10 0 0 0,-8-26 72 0 0,6 5-112 0 0,-7-21-81 0 0,0-2-30 0 0,12 5-660 0 0,11-2-2647 0 0,-18-11 2023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="41569.811">15105 11925 6448 0 0,'29'-50'4184'0'0,"-28"49"-3679"0"0,-1 1 6 0 0,0 0 1 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0 0 0 0,0 0-24 0 0,0 0-100 0 0,0 0-42 0 0,0 0-8 0 0,0 0-20 0 0,0 0-74 0 0,0 0-39 0 0,0 0-5 0 0,0 0 26 0 0,0 0 104 0 0,0 0 44 0 0,0 0 8 0 0,0 0-31 0 0,13 2 130 0 0,-13-1-345 0 0,-18 8 299 0 0,-3 5-94 0 0,-33 31 589 0 0,18-10 20 0 0,22 11-70 0 0,14-44-729 0 0,0 0-40 0 0,-1 14 5 0 0,1-13-81 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-3 0 0 0,0 2 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,1-1-1 0 0,-1 2 0 0 0,0-2 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,3-1-27 0 0,-1 2 24 0 0,0-1-1 0 0,1 2 1 0 0,-1-2-1 0 0,1 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,3 0-23 0 0,28 6-16 0 0,1-12-321 0 0,0-17-1384 0 0,-18 19-2498 0 0,-7-2-2527 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42539.811">15467 11636 456 0 0,'0'0'1877'0'0,"0"0"225"0"0,0 0 96 0 0,0 0-174 0 0,0 0-800 0 0,0 0-352 0 0,0 2-68 0 0,-3 81 5406 0 0,0-8-3788 0 0,-5 6-533 0 0,1 110-938 0 0,8-93-994 0 0,-1-95-228 0 0,2 9 239 0 0,-1-5-2836 0 0,-1-12 836 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="42759.811">15413 11775 10592 0 0,'0'0'818'0'0,"0"0"-382"0"0,0 0 375 0 0,2 0 224 0 0,50 13 3870 0 0,-12 2-4655 0 0,-17-7-2639 0 0,-22-7 1115 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="43219.811">15718 11975 920 0 0,'0'-6'1780'0'0,"-8"-30"5181"0"0,8 35-6117 0 0,0 1-63 0 0,4-5 1525 0 0,-2 2 782 0 0,7 22-961 0 0,-17 41 414 0 0,0-12-2418 0 0,14-5-123 0 0,8 30-266 0 0,-14-71-1124 0 0,0-2-490 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="43559.811">15959 12008 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,-7-15-276 0 0,7 11-201 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 3 0 0 0,1-3 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,0-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,2 1-59 0 0,-3 1 59 0 0,0 1 0 0 0,2-1 1 0 0,-1 2-1 0 0,-1-2 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,3 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-61 0 0,14 48 1489 0 0,-16-40-1068 0 0,2 2-1 0 0,-1-2 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 1-420 0 0,1-11 47 0 0,-19 57 2134 0 0,-23 18-2086 0 0,42-75-50 0 0,-2 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-2-2-46 0 0,-34-49 76 0 0,19 3-2636 0 0,11 13-3921 0 0,3 11-600 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51949.811">16300 11786 2760 0 0,'3'6'3463'0'0,"-3"-2"5440"0"0,-8 23-3399 0 0,8 22-2728 0 0,-2 11-1732 0 0,-7 24 73 0 0,11 41-1117 0 0,1-97-2100 0 0,-3-30 527 0 0,4-4-370 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="52379.811">16289 11987 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0 0 240 0 0,0-8 1066 0 0,14-32 2918 0 0,32 2-1475 0 0,-30 31-2427 0 0,23-4-98 0 0,-30 13-954 0 0,42 19 0 0 0,15 47 242 0 0,-30 33 636 0 0,-26-63-878 0 0,-6-21 0 0 0,-8 8-49 0 0,4-24-207 0 0,0-1-87 0 0,0 0-917 0 0,0 0-3813 0 0,0 0-1633 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54319.811">16919 11496 10136 0 0,'0'0'230'0'0,"0"0"30"0"0,0 0 19 0 0,0 18 1877 0 0,8 82 4244 0 0,-6-26-3972 0 0,-7 47-624 0 0,0-25-1860 0 0,4 89 1890 0 0,2-7-1730 0 0,3-165-88 0 0,-1 4-289 0 0,-2 2-5727 0 0,-4-36 687 0 0,-1 1 3586 0 0,8 3-135 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="55229.81">16931 11544 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,3-7-177 0 0,-3 5 136 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1-247 0 0,11-7 1678 0 0,42-6 1057 0 0,22 24-286 0 0,-60-6-2099 0 0,-4 0-94 0 0,-1 0 0 0 0,2 1 0 0 0,-3 0 0 0 0,1-1 1 0 0,0 3-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 2 0 0 0,-2-2 0 0 0,2 1 0 0 0,3 7-256 0 0,13 29 768 0 0,7 37 88 0 0,-26-15-68 0 0,-12-18 336 0 0,-16-10-1124 0 0,15-34 144 0 0,0 1 0 0 0,1 0-1 0 0,-2 0 1 0 0,0-2 0 0 0,0 0 0 0 0,-1 0-1 0 0,3 0 1 0 0,-3 0 0 0 0,0 0-1 0 0,-4 0-143 0 0,-39 16 238 0 0,48-19-196 0 0,-2-1-31 0 0,1 3-27 0 0,59-31-776 0 0,16 17-152 0 0,-5 30-54 0 0,-18 15 92 0 0,-12 15 866 0 0,-27-28 40 0 0,-6-16 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 2 0 0 0,-26 32 1352 0 0,-10 2-736 0 0,24-34-497 0 0,-1 0-1 0 0,1-1 1 0 0,-1-1-1 0 0,-1-1 1 0 0,1-1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-2 1 0 0,0 1 0 0 0,0-2-1 0 0,-6-1-118 0 0,-59 7 387 0 0,27 10-334 0 0,27-15-53 0 0,-5-20-801 0 0,22 10-282 0 0,2 0-2237 0 0,3 3-3262 0 0,-1-2-1015 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56249.811">17727 11514 14800 0 0,'0'0'332'0'0,"0"0"50"0"0,0 0 25 0 0,0 0-47 0 0,0 0-106 0 0,0 0 417 0 0,0 2 206 0 0,-9 54 3904 0 0,7-25-4120 0 0,-16 140 1824 0 0,-3-31-880 0 0,8-33-165 0 0,-13 136-832 0 0,25-237-672 0 0,1-5-273 0 0,0-1-138 0 0,0 3-1216 0 0,-2 4 3621 0 0,1-1-4753 0 0,1-1-9564 0 0,0-5 10339 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56479.811">17735 11568 920 0 0,'0'-5'1157'0'0,"1"2"5384"0"0,18-14-1079 0 0,29 9 55 0 0,23 14-2419 0 0,-2 12-1830 0 0,-11 12 320 0 0,17 45-1572 0 0,-19 14 2016 0 0,-50-76-1886 0 0,-1 2 0 0 0,-1-3 0 0 0,0 1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,-2 1 0 0 0,0 6-146 0 0,1-1 8 0 0,-2 1 0 0 0,2-1 0 0 0,-4-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-2-2 0 0 0,0 2 0 0 0,0-3 0 0 0,-1 1 0 0 0,-2-1 0 0 0,2-1 0 0 0,-4 1-8 0 0,10-8 173 0 0,-1-1 1 0 0,2-1-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0-2 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,-3 0-174 0 0,-119-3-286 0 0,101-4-191 0 0,21 5 329 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,2-1 0 0 0,-2 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1-1 0 0 0,-5-3 148 0 0,5 3-710 0 0,5 6-8073 0 0,3 0 434 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57489.811">18433 12156 7368 0 0,'0'0'333'0'0,"0"0"0"0"0,-9 4 14776 0 0,8-4-14374 0 0,1-2-710 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,1-1 0 0 0,-1 2-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,2 0 1 0 0,-1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,1 2-25 0 0,-3 1 94 0 0,0 0 9 0 0,0 0 29 0 0,0 0 17 0 0,0 0 3 0 0,0 0 11 0 0,0 0 44 0 0,0 0 17 0 0,0 0 6 0 0,0 0 4 0 0,0 0 4 0 0,0 0 2 0 0,0 0 0 0 0,0 0-16 0 0,0 0-66 0 0,0 0-29 0 0,0 0-8 0 0,0 0-9 0 0,0 0-33 0 0,-1 0-25 0 0,-20 29-43 0 0,16-8 74 0 0,4-19-19 0 0,1-2 6 0 0,1-2-18 0 0,8-16-135 0 0,6 9 5 0 0,7 15-588 0 0,-16 3 664 0 0,2 16 16 0 0,-8-24 62 0 0,-5 8 297 0 0,-6-2-725 0 0,10-7 151 0 0,-9 9-801 0 0,1-9-2062 0 0,9 0 1532 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58349.811">18784 11699 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-4 420 0 0,0 4 3077 0 0,0 2 3963 0 0,-6 140-3072 0 0,-5-27-2600 0 0,-7 65-1021 0 0,8-67-304 0 0,3 24-619 0 0,7-137-213 0 0,0 0-69 0 0,0 0-12 0 0,0 0-139 0 0,0-55-6135 0 0,0 31 4451 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="58689.811">18757 11739 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,1-1 21 0 0,2-2-256 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,2 0-1 0 0,-2 1 1 0 0,1-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,3 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-1 0 0,2 1 1 0 0,-2-1 0 0 0,2 1 0 0 0,0 0-170 0 0,7 4 318 0 0,-3 0 1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,-1 2 0 0 0,1-1-1 0 0,-1 1-318 0 0,19 15-106 0 0,-24-20 167 0 0,0 2 0 0 0,1-2 1 0 0,-2 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-2 2 0 0 0,0-1 0 0 0,0 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,0 4-62 0 0,3 16 844 0 0,-5-17-830 0 0,2 1-1 0 0,-1 0 1 0 0,0-2 0 0 0,-1 1 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,-1 3-14 0 0,0-2 119 0 0,2-1-1 0 0,-1 0 1 0 0,-2-1-1 0 0,2 0 1 0 0,-1 2-1 0 0,-1-3 1 0 0,1 1-1 0 0,-2-2 1 0 0,0-1-1 0 0,1 3 1 0 0,-1-2-1 0 0,1 0 1 0 0,-1-1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-6 3-118 0 0,-6 4 128 0 0,18-8-128 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,1 0 1 0 0,-2 1-1 0 0,2 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 2-1 0 0,0-2 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-2 1 0 0,1 2-1 0 0,-1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,2-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 0 0 0,-15-23-1234 0 0,14 3-3424 0 0,6 8-3433 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="59859.811">19240 11446 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-270 0 0,1 1 131 0 0,13 73 4572 0 0,-17-14-1957 0 0,3 7-1459 0 0,3 28-1321 0 0,-6 21-232 0 0,-4 73 0 0 0,-5-82 962 0 0,-11 12-720 0 0,23-118-750 0 0,0-1-89 0 0,0 0-360 0 0,0 0-163 0 0,-5-10-5760 0 0,1-1 563 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60069.811">19237 11958 1376 0 0,'0'0'65'0'0,"0"-2"389"0"0,26-32 11411 0 0,9-16-8036 0 0,4 19-1988 0 0,-37 30-1803 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,1 2 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,2 2 0 0 0,-3 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-38 0 0,7 4 156 0 0,32 78 888 0 0,-36-75-884 0 0,3 2-1 0 0,-1-1 1 0 0,-2 1 0 0 0,0-2-1 0 0,0 1 1 0 0,0 1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 6-159 0 0,-8 89 1127 0 0,4-98-1133 0 0,1-8-6257 0 0,0-1-578 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="60829.81">19786 11763 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 2 21 0 0,-8 45 177 0 0,-9 36 3194 0 0,7 30-1553 0 0,-6 92-172 0 0,0-90-257 0 0,10-101-2469 0 0,4-13-3087 0 0,2 0-3929 0 0,0-1 1033 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="61029.81">19758 11763 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,14-6-181 0 0,-11 4-54 0 0,-1 0 1 0 0,2-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-2 0 0 0 0,2 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0-1 0 0 0,0 2 1 0 0,0-1-1 0 0,-1 0 0 0 0,0 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 2 1 0 0,2-1-1 0 0,-3 0 0 0 0,5 2-301 0 0,0 1 145 0 0,-2-2-1 0 0,2 1 0 0 0,0 0 1 0 0,-1 1-1 0 0,-1-1 1 0 0,2 1-1 0 0,-1 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,0 1 1 0 0,-2-1-1 0 0,1 0 0 0 0,-1 1 1 0 0,1 1-1 0 0,-1-2 1 0 0,-1 0-1 0 0,2 2 0 0 0,-1 5-144 0 0,6 63 1883 0 0,-24 14-1742 0 0,13-87-123 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,2-2 0 0 0,0 1 0 0 0,-2-1 0 0 0,-3 0-18 0 0,-48 3 1171 0 0,-3 13-2729 0 0,54-16 1668 0 0,-16-4-935 0 0,1-8-3444 0 0,12 4 2477 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="63909.811">15790 11617 3224 0 0,'0'-1'240'0'0,"0"-1"165"0"0,0 1 1443 0 0,0 1 616 0 0,0 0 116 0 0,0-2 259 0 0,0-2-1698 0 0,1 2 2411 0 0,12-14-2439 0 0,-11 9-1053 0 0,-2-3 606 0 0,0 6-4232 0 0,0 4 2520 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190399.81">5436 11548 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,3-8 314 0 0,19-68 850 0 0,-20 63-996 0 0,2 0 0 0 0,2 0-1 0 0,-1 1 1 0 0,0 1-1 0 0,1-1 1 0 0,2 0 0 0 0,-2 1-1 0 0,2 0 1 0 0,1 0 0 0 0,-3 1-1 0 0,5 1 1 0 0,6-7-478 0 0,-16 15 40 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 2 0 0 0,2-2 0 0 0,-2 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1-40 0 0,24 53 1331 0 0,-24-52-1287 0 0,3 12 148 0 0,-2-1 0 0 0,1-2 0 0 0,-2 2 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1-3 0 0 0,-2 0 0 0 0,-2 6-192 0 0,6-16 21 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2-1 0 0,-2 1 1 0 0,3 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,3 0-1 0 0,-2 0 1 0 0,0-1-22 0 0,-3-2-60 0 0,1 1-1 0 0,-1-2 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 1 1 0 0,-2-1-1 0 0,2 0 1 0 0,0 0-1 0 0,1-2 1 0 0,-1 3-1 0 0,1-2 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1-8 60 0 0,-7-52-3591 0 0,9 43 1933 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192059.8109">6914 11437 4144 0 0,'0'0'319'0'0,"-10"2"1818"0"0,9-1 2461 0 0,1 0 4419 0 0,6 0-8694 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,2-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,1 0-323 0 0,98-55 185 0 0,-72 19-185 0 0,-29 38 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,1-2 0 0 0,-1 2 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,-30-38 0 0 0,30 38 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,3 0 0 0 0,-1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-5 1 0 0 0,-38 18 0 0 0,37-12 47 0 0,2 0 0 0 0,-1 2 1 0 0,2-3-1 0 0,0 3 0 0 0,-1-1 0 0 0,0 2 0 0 0,2 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,0-1 0 0 0,1 3 0 0 0,0-2 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1-1 0 0 0,2 9-47 0 0,2-11 52 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1-2-1 0 0,0 3 1 0 0,1-2-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,4 4-52 0 0,-5-6 15 0 0,-1-2 0 0 0,1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 0-15 0 0,46-5-958 0 0,-35-2-1726 0 0,-3 0-3307 0 0,-4 0-1687 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="193429.81">7432 11162 10304 0 0,'0'-4'934'0'0,"0"-9"-627"0"0,0 11 320 0 0,0-3 712 0 0,-1 2 3325 0 0,0 5-4568 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 2-95 0 0,-2 6 224 0 0,1 31 664 0 0,-6 119 1598 0 0,12-76-1828 0 0,-6-42-734 0 0,0-33-364 0 0,0 7-1982 0 0,-2-11-5617 0 0,2-5 5673 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="193879.8109">7343 11262 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,1-2-294 0 0,0-2 74 0 0,0 3 886 0 0,14-8 3459 0 0,-12 7-4230 0 0,3 0-1 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,-3 1-1 0 0,3 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-2 1-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-348 0 0,34 4 963 0 0,-19-6-540 0 0,-15 0-358 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,2 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2 1 1 0 0,0 1-1 0 0,2-1 0 0 0,-2 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 2-64 0 0,51 65 377 0 0,-51-58-1065 0 0,-5 2-3411 0 0,-1-9 774 0 0,1-2-4194 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="196929.81">5085 11305 456 0 0,'0'-17'1413'0'0,"0"16"159"0"0,0-1 76 0 0,0-43 2855 0 0,0 44-3991 0 0,0 1 0 0 0,0 0-24 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0 47 0 0,0 0 207 0 0,0 0 89 0 0,0 0 21 0 0,0 0-24 0 0,-11 5 931 0 0,8-3-1418 0 0,2 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 2-182 0 0,5 89 3864 0 0,2 21-3175 0 0,-12-60 34 0 0,4 17-176 0 0,1-68-729 0 0,-4 4 3 0 0,1-5-7687 0 0,2-2-336 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="197139.81">5077 11400 11976 0 0,'0'-4'180'0'0,"1"-1"0"0"0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,1-2 0 0 0,-1 1 0 0 0,0 1 0 0 0,1-1 0 0 0,2-2-180 0 0,5-5 1628 0 0,-5 7-1094 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,1 1 0 0 0,0-1 1 0 0,-2-1-1 0 0,3 2 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,5-1-535 0 0,-7 1 86 0 0,0 1 0 0 0,2 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 1 0 0 0,-1-1 0 0 0,3 1 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 2 0 0 0,-1-2 1 0 0,2 1-1 0 0,-2-1 0 0 0,0 1 0 0 0,2 3-86 0 0,22 36 302 0 0,17 36 108 0 0,-31-48-1847 0 0,-7-22-150 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-170686.919">5865 11272 456 0 0,'-2'30'10790'0'0,"-5"-4"-6142"0"0,-16 83 1001 0 0,21-101-5360 0 0,-2 1-52 0 0,2 0 0 0 0,0-1-1 0 0,0 3 1 0 0,-1-3-1 0 0,3 3 1 0 0,0-2 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 6-237 0 0,7 21 1589 0 0,0-28-1573 0 0,-6-7-16 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1-1-1 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 1 0 0,-2 1-1 0 0,2-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-3 0 0 0,49-82 357 0 0,-52 87-357 0 0,54-133 184 0 0,-51 92-184 0 0,-5 34-21 0 0,-6 3 2 0 0,3 4-2431 0 0,4 0 1260 0 0,-8 0-578 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-169886.919">6243 11233 2304 0 0,'0'0'428'0'0,"0"0"959"0"0,0 0 422 0 0,0 0 81 0 0,0 0-74 0 0,0 0-388 0 0,0 0-168 0 0,0 0-38 0 0,0 0-52 0 0,0 0-190 0 0,0 0-85 0 0,0 0-21 0 0,-5 13 2869 0 0,10 30-896 0 0,6 19-821 0 0,-5 33-482 0 0,15 22-8 0 0,-17-110-1420 0 0,-4-5-17 0 0,4 4 78 0 0,13 29 298 0 0,-17-34-578 0 0,0-1-4 0 0,1 1 26 0 0,5 3 65 0 0,-2 7 16 0 0,3-15 203 0 0,30-96 1554 0 0,-16 20-2314 0 0,-2 29 1122 0 0,18-34-626 0 0,-22 60-1899 0 0,-1 6 396 0 0,-9 15-8315 0 0,-5 4 2000 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-167866.919">6612 15316 1376 0 0,'0'0'65'0'0,"0"0"298"0"0,0 0 1226 0 0,-4-12 8887 0 0,2 4-10689 0 0,2 7 20 0 0,0-13-1355 0 0,0 5-2483 0 0,0 6 619 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-167696.919">6609 15286 920 0 0,'0'0'80'0'0,"0"0"-80"0"0,0 0 0 0 0,0 10 0 0 0,-3 2 1224 0 0,3-12 232 0 0,0 0 48 0 0,0 0 0 0 0,0 0-1128 0 0,0 0-232 0 0,0 0-48 0 0,0-6 0 0 0,0 3-96 0 0,0 3-128 0 0,0 0 32 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-166746.919">6601 15265 2760 0 0,'0'0'125'0'0,"0"-13"2231"0"0,-1 2 3939 0 0,-15 49-2743 0 0,7 58-695 0 0,18 30 396 0 0,16-18-1214 0 0,10-62-933 0 0,-31-45-1072 0 0,-2 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-2 0 0 0,1 1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-3-34 0 0,103-166 703 0 0,-77 113-639 0 0,-9-32-572 0 0,-19 79 468 0 0,0 9-31 0 0,-7-22-455 0 0,0 11-3508 0 0,6 9-3672 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-120276.919">10041 15340 11952 0 0,'0'-1'67'0'0,"0"1"0"0"0,-1-3 0 0 0,1 2 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-67 0 0,-36-10 5146 0 0,38 9-5069 0 0,-2 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,-2 1 1 0 0,2-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 2-77 0 0,-10 8 763 0 0,5-6-634 0 0,1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,1 0 1 0 0,-2 1 0 0 0,3-1 0 0 0,-1 1-1 0 0,-1-2 1 0 0,1 2 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 3-128 0 0,-1 1 108 0 0,-2 12 172 0 0,0-1 0 0 0,2 1 0 0 0,-1-2 0 0 0,2 3 0 0 0,0-1 0 0 0,2 0-280 0 0,2 61 688 0 0,21-36-159 0 0,-8-33-346 0 0,-14-12-174 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 1-9 0 0,11-9 35 0 0,-3-2 0 0 0,1 1 0 0 0,-2-2 0 0 0,3 1 0 0 0,-4 0 0 0 0,2-3 0 0 0,-3 2-1 0 0,7-11-34 0 0,28-41 89 0 0,-2 6-100 0 0,-18 21-55 0 0,-23 35-4 0 0,-1-1-103 0 0,1 2-332 0 0,1 1-119 0 0,0 0-16 0 0,-2 0-596 0 0,-1 1 165 0 0,1-2-2477 0 0,2 1 1724 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-119726.919">10512 15024 12064 0 0,'0'0'553'0'0,"0"0"-16"0"0,-9 15-151 0 0,-4 31 4878 0 0,4 30-1596 0 0,3-22-2083 0 0,-8 72 353 0 0,-1 18 194 0 0,1 140-900 0 0,13-190-1248 0 0,1-92-72 0 0,0-2-51 0 0,0 0-18 0 0,0 0-158 0 0,-3-25-4130 0 0,2 8-1692 0 0,-2-2-1669 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-119476.919">10428 15305 2304 0 0,'19'-58'224'0'0,"-10"36"1777"0"0,16 4 11624 0 0,10 20-9044 0 0,10 21-2754 0 0,-1 24-1302 0 0,-9-26-2042 0 0,-27-16-78 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-166306.919">7129 15165 10136 0 0,'-10'51'1272'0'0,"8"-45"-735"0"0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,2-1-1 0 0,-2-1 0 0 0,1 1 1 0 0,0 1-1 0 0,1-1 1 0 0,0 3-538 0 0,8 28 1513 0 0,19 68 1825 0 0,8 15-1726 0 0,11-10-228 0 0,-24-68-629 0 0,-2-15-113 0 0,-21-10-556 0 0,7-25-22 0 0,12-35 0 0 0,12-48 53 0 0,17 7-396 0 0,-11 32 158 0 0,-16-12 121 0 0,-6 12 0 0 0,5-6 0 0 0,-17 45-97 0 0,-5 12-406 0 0,0 1-165 0 0,8-8-841 0 0,-2 0-1411 0 0,-3 7-6017 0 0,2 2 8141 0 0,-4 0 11 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-164976.919">7780 15512 1840 0 0,'1'4'465'0'0,"-1"3"-969"0"0,-3-2 8499 0 0,3-4-5413 0 0,0-1-959 0 0,-3 15 3293 0 0,5-13-4747 0 0,1 0-1 0 0,-2-1 1 0 0,1 1 0 0 0,0 0 0 0 0,2-2-1 0 0,-2 1 1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0-1 0 0,0 0 1 0 0,0 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,1 0-1 0 0,0 0-168 0 0,5-2 150 0 0,1-2 0 0 0,-2 0 1 0 0,2 0-1 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,3-3-150 0 0,6-11 74 0 0,-1 1 1 0 0,-2-1-1 0 0,1-3 1 0 0,-2 2-1 0 0,-1-2 1 0 0,8-22-75 0 0,-18 45 4 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-3 0 0 0,0 2 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 2 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0-4 0 0,-7 2 35 0 0,-1 0-1 0 0,1 2 0 0 0,0-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-2 1-1 0 0,3 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,-1 2 1 0 0,0-2-1 0 0,2 1 0 0 0,-1 0 1 0 0,2 2-1 0 0,-1 0 1 0 0,-1 0-1 0 0,3 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,3-1-1 0 0,-2 0 0 0 0,2 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 0 1 0 0,2 0-1 0 0,1 4-34 0 0,0-10 18 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 2 0 0 0,1-2 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,1 1 1 0 0,-1-2-1 0 0,0 1 0 0 0,0 0 1 0 0,2 0-1 0 0,-2-2 1 0 0,0 2-1 0 0,2-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-18 0 0,6 1-63 0 0,1 2 0 0 0,0-3 0 0 0,-1 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0-1 0 0 0,10-2 63 0 0,-8 1-520 0 0,14-5-1481 0 0,-9 2-3720 0 0,0 1-1868 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-163966.919">8287 15035 6624 0 0,'3'19'-4'0'0,"-2"-5"534"0"0,-1 1 5466 0 0,0-15-4969 0 0,0 0-16 0 0,-7 45 3846 0 0,0 31-3228 0 0,3 0 0 0 0,4 42-1629 0 0,0-64 228 0 0,4 10-228 0 0,-4 44-16 0 0,-4-65-2758 0 0,4-29-1657 0 0,0-12 1925 0 0,0-1-3470 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-163606.919">8247 15398 10136 0 0,'22'-72'1056'0'0,"11"-14"3846"0"0,-31 81-4603 0 0,1 1 0 0 0,0-3 0 0 0,0 3 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1-1 0 0 0,-1 2 0 0 0,0 0 0 0 0,5-1-299 0 0,-5 3 72 0 0,-1-1-1 0 0,2 1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-2 3 0 0 0,2-2-1 0 0,-3 0 1 0 0,2 0 0 0 0,-1 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1 1-1 0 0,2 3-71 0 0,27 22 580 0 0,10 42 1278 0 0,-30 0-3924 0 0,-12-50-2692 0 0,-2-14 3016 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121546.919">9011 14833 5872 0 0,'0'0'266'0'0,"0"0"1"0"0,-2-11 1056 0 0,2 9 7600 0 0,-9 82-5279 0 0,9-27-2198 0 0,1 28 275 0 0,-4 1-1 0 0,-5 30-1720 0 0,-13 188 1691 0 0,17-172-981 0 0,5-116-1358 0 0,-2-19-2345 0 0,-6-52-991 0 0,2 16 1937 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-121236.919">8796 14843 8752 0 0,'0'0'673'0'0,"11"7"4424"0"0,13 7-302 0 0,17-11-2564 0 0,-30-3-1654 0 0,57 1 445 0 0,-46-3-776 0 0,-1 1 0 0 0,1 1 0 0 0,-1 1-1 0 0,1 1 1 0 0,-1 1 0 0 0,10 3-246 0 0,-20-3 75 0 0,0 1-1 0 0,1 0 1 0 0,-2 2-1 0 0,2 0 1 0 0,-3 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,1 2-75 0 0,35 48-3176 0 0,-40-46 1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-120726.919">9406 15584 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 0-276 0 0,-30 2 2318 0 0,14-7 1927 0 0,2-23-2183 0 0,17 23-2093 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,1-2 0 0 0,-1 3-1 0 0,0-1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0-1 0 0,1-2-146 0 0,9-20 178 0 0,-9 18-156 0 0,0-2 1 0 0,2 2-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 2-1 0 0,2-2 1 0 0,-2 0-1 0 0,3 2 0 0 0,0-3-22 0 0,-5 7 22 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,-3 1 0 0 0,3-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 1 0 0 0,2 0-22 0 0,0 0 73 0 0,-2 1 0 0 0,2 0-1 0 0,-3 1 1 0 0,2-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-2 0 1 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 0 1 0 0,-1 1 0 0 0,-1 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,2 1-73 0 0,9 74 976 0 0,-12-61-728 0 0,-1 0 22 0 0,-2 3 1 0 0,-1-2-1 0 0,0 0 0 0 0,0 0 0 0 0,-3 1 0 0 0,2-3 1 0 0,-4 8-271 0 0,3-10 132 0 0,1-11-108 0 0,2 1 1 0 0,-1-1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-2 1 1 0 0,1 0-1 0 0,0-1 0 0 0,0-2 1 0 0,-1 2-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-2-1 0 0 0,2 1 1 0 0,-1-1-1 0 0,-3 0-24 0 0,1-2 9 0 0,2 1-1 0 0,-2-2 1 0 0,0 1 0 0 0,1-1-1 0 0,1 1 1 0 0,-2-2-1 0 0,1 1 1 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,2-2 0 0 0,-2 1-1 0 0,-3-2-8 0 0,5 3-63 0 0,0-1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,3-1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 2 1 0 0,0-2-1 0 0,0 0 0 0 0,2 0 0 0 0,-3-3 63 0 0,2 5-278 0 0,1-1-1 0 0,0 1 0 0 0,-1-2 0 0 0,1 3 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,0-2 0 0 0,1 2 0 0 0,-2 0 0 0 0,1 0 1 0 0,2-4 278 0 0,5-8-2146 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116106.919">11666 15447 3680 0 0,'0'0'284'0'0,"0"0"17"0"0,3-5 3845 0 0,5-2 6650 0 0,-22 234-6730 0 0,16-197-3860 0 0,-1-2-3590 0 0,-1-28 1760 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-115556.919">12006 15333 920 0 0,'-4'11'76'0'0,"-21"26"272"0"0,-7-6 6376 0 0,6-8-722 0 0,24-22-4979 0 0,-5 7 987 0 0,3 16 528 0 0,5-5-1218 0 0,4-13-1123 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,1-1 1 0 0,1-1-1 0 0,-2 0 1 0 0,0 0 0 0 0,3 0-1 0 0,-2-1 1 0 0,0 1 0 0 0,6 0-198 0 0,22 11 384 0 0,-30-13-322 0 0,0 0 0 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0-1 0 0 0,0 3 0 0 0,-1-2 0 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1-62 0 0,-2 3 0 0 0,0 0 0 0 0,0 0 0 0 0,-2-2 0 0 0,1 1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0-2 0 0 0,3 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,1-4 0 0 0,-2 2-326 0 0,-13-20-857 0 0,15 3-6482 0 0,3 10 584 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-117286.919">11055 14945 10824 0 0,'0'0'241'0'0,"0"8"331"0"0,-5 108 4121 0 0,-3 8-200 0 0,1-17-2317 0 0,-3 59-880 0 0,10 67-5334 0 0,0-232-1053 0 0,0-1-1451 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116916.919">11393 14962 2760 0 0,'-18'-15'247'0'0,"15"13"193"0"0,2 2 1710 0 0,-1 4 4946 0 0,-3 7-4369 0 0,3-5-1946 0 0,-27 39 1201 0 0,36-3-671 0 0,-28 126 670 0 0,-24 99 167 0 0,10-128-2609 0 0,28-124-2025 0 0,4-6-2648 0 0,-2 0-1568 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-116696.92">10995 15357 9672 0 0,'0'0'748'0'0,"1"1"-492"0"0,3 3-231 0 0,-3-2 331 0 0,0 1 1 0 0,1-2-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,2 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,0 0 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,2 0-356 0 0,105 17 3649 0 0,-104-16-4114 0 0,3 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,5 5 465 0 0,9 7-1693 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-110456.919">13391 15308 1840 0 0,'0'3'133'0'0,"0"6"1371"0"0,-7 15 9957 0 0,2-12-10918 0 0,0 11 2807 0 0,4-15-2599 0 0,1-7-23 0 0,0-1-45 0 0,0 3-163 0 0,-6 43 1090 0 0,-9 101 530 0 0,12-18-1604 0 0,6-92-486 0 0,-3-35-216 0 0,0-2-402 0 0,0 0-174 0 0,5-17-2600 0 0,-2 5 1430 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-110046.919">13367 15494 4144 0 0,'0'0'319'0'0,"0"0"75"0"0,-2-4 5801 0 0,0-1-4842 0 0,2-6-34 0 0,9-35 4642 0 0,8 32-3827 0 0,24 0-548 0 0,-5 20-1696 0 0,-32-6 128 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,1 0-18 0 0,33 8 0 0 0,-23-7 0 0 0,-8-1 0 0 0,7 11 0 0 0,-2 11-870 0 0,-14-22 616 0 0,2-2-383 0 0,0 1-179 0 0,-12 34-4440 0 0,11-32 3346 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-112086.92">12433 14993 3224 0 0,'0'0'143'0'0,"0"2"-3"0"0,-1-2 1084 0 0,-4 11-2538 0 0,2-9 6295 0 0,1-2 6252 0 0,3 16-9469 0 0,9 58 352 0 0,-24 136-1892 0 0,10-121 559 0 0,1-61-682 0 0,2-1 0 0 0,0 0 0 0 0,2-1 0 0 0,1 2 0 0 0,1 0-101 0 0,3 28-450 0 0,-10-47-56 0 0,2-7-6442 0 0,2-2 4901 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111836.919">12416 15165 15664 0 0,'0'0'356'0'0,"0"0"49"0"0,0 0 21 0 0,2 0-42 0 0,103-19 3931 0 0,-41 7-2346 0 0,-38 16-4175 0 0,-19 4 964 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111476.919">12767 15559 7744 0 0,'0'0'356'0'0,"0"0"-8"0"0,0 0-63 0 0,0 0 571 0 0,-3 10 4563 0 0,-14-49-211 0 0,23-31-2906 0 0,26 42-1872 0 0,-14 14-315 0 0,-14 13-110 0 0,-1-1-1 0 0,1 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 1 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 1 0 0 0,1-1 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 1-4 0 0,-1 2 59 0 0,1-1-1 0 0,-1 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 2-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-1 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-2 1-59 0 0,3-4 22 0 0,-1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-2 0 0 0 0,2-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-23 0 0,-32 6 210 0 0,2-37-185 0 0,14 8-523 0 0,12-7-2557 0 0,8 18 1503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-111056.919">13123 15343 8288 0 0,'2'16'273'0'0,"-1"-32"1643"0"0,-1 16-472 0 0,0 0 76 0 0,0 0-55 0 0,0 0-287 0 0,0 2-123 0 0,-7 44 4957 0 0,-7 0-5210 0 0,13 94 812 0 0,6-40-1951 0 0,-5-94-1422 0 0,0-5-625 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-109556.919">13008 15101 8752 0 0,'21'17'1346'0'0,"-21"-15"-166"0"0,2-2-1575 0 0,2-4 4378 0 0,4-5 4520 0 0,2 2-11521 0 0,-5 3 1866 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-106806.919">13865 15580 6912 0 0,'75'12'8898'0'0,"-70"-11"-8618"0"0,0-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,1-1-1 0 0,0-1 0 0 0,-3 0 1 0 0,3 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,-2 0 0 0 0,3-1 1 0 0,-1 0-1 0 0,-1 1 1 0 0,2-4-280 0 0,34-51 1321 0 0,-38 51-1321 0 0,0 2 1 0 0,1-1-1 0 0,0 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-2 1-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0-2-1 0 0,-18-35-90 0 0,15 40 124 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2 1 0 0 0,1-1 0 0 0,2 1 0 0 0,-3-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 1 0 0 0,1 0 0 0 0,-1 0-34 0 0,-53 24 664 0 0,51-20-600 0 0,-1 2 0 0 0,0 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,1 0 0 0 0,-1-2 0 0 0,1 3 0 0 0,-1 1-64 0 0,1 1 41 0 0,1 0 0 0 0,0-2 0 0 0,2 3 1 0 0,-2-1-1 0 0,2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 2 0 0 0,0-3 0 0 0,2 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,4 6-41 0 0,-5-9 98 0 0,3-2-1 0 0,-1 0 1 0 0,0 1-1 0 0,1-1 1 0 0,0-1-1 0 0,0 1 1 0 0,2 1-1 0 0,-1-2 0 0 0,0 0 1 0 0,6 7-98 0 0,-6-12 5 0 0,-1 0 0 0 0,1 0 0 0 0,-1-2 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,0-1 0 0 0,1 0-5 0 0,2-1-54 0 0,104-33-5788 0 0,-61 9 1619 0 0,-24 11 2079 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-102656.919">15313 15424 1840 0 0,'0'0'83'0'0,"0"0"169"0"0,0 0 668 0 0,0 0 288 0 0,0 0 58 0 0,0 0-22 0 0,0 0-144 0 0,0 0-63 0 0,0 0-11 0 0,0 0-2 0 0,0 8 2048 0 0,-2 19-266 0 0,1-2-362 0 0,1 78 1520 0 0,-3-31-3723 0 0,2 17-415 0 0,2-81 488 0 0,4 6-6100 0 0,1-8-783 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-102316.919">15318 15580 10136 0 0,'20'-57'5082'0'0,"10"10"-1747"0"0,-6 29-1698 0 0,-22 15-1500 0 0,0 1-1 0 0,0-2 1 0 0,0 2-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,2 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,2 0 1 0 0,0 0-137 0 0,0 1 60 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-2 0 0 0 0,3 2 0 0 0,-2-1 0 0 0,2 0 1 0 0,-2-1-1 0 0,0 2 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,1 1 1 0 0,-1-2-1 0 0,2 2 0 0 0,-2 1 0 0 0,1 2-60 0 0,16 17 54 0 0,-5-15-897 0 0,-12-8-100 0 0,0-1-37 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-104576.919">14515 14813 2304 0 0,'0'0'101'0'0,"0"0"294"0"0,0 0 1149 0 0,0 0 506 0 0,0 2 1554 0 0,0 9-1838 0 0,2 149 6571 0 0,-2 118-5024 0 0,-14-9-1402 0 0,11-165-1693 0 0,-7-28-376 0 0,9-75-114 0 0,1-1-766 0 0,-5-11-2968 0 0,-1-2-3447 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-104236.919">14489 15015 920 0 0,'0'-1'67'0'0,"-3"-7"403"0"0,4-1 4358 0 0,4-4-1924 0 0,-4 10-1691 0 0,19-33 4007 0 0,24-3-3052 0 0,6 6-888 0 0,-30 25-1087 0 0,-17 7-85 0 0,0-2 0 0 0,0 2 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,1 1-108 0 0,0 0 199 0 0,-1 2 0 0 0,2-2 0 0 0,-1 1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 2 1 0 0,-1-2 0 0 0,4 4-199 0 0,28 61 460 0 0,-26-41-231 0 0,-1 2 1 0 0,-1 0-1 0 0,-2-1 0 0 0,0 2 1 0 0,-3-2-1 0 0,1 1 0 0 0,-3 27-229 0 0,0-48 147 0 0,-2 1-1 0 0,1 0 0 0 0,-1-1 0 0 0,2 0 1 0 0,-3 0-1 0 0,0-1 0 0 0,0 2 0 0 0,-1-2 1 0 0,1 1-1 0 0,-1 0 0 0 0,0-2 1 0 0,-2 1-1 0 0,2-1 0 0 0,-3 4-146 0 0,3-8 10 0 0,-2 0 1 0 0,1 0-1 0 0,1-1 0 0 0,-2 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 0 0 0,-5-2-10 0 0,-3-2-494 0 0,0-1-1 0 0,1-2 1 0 0,1 1-1 0 0,-2-1 1 0 0,3 0-1 0 0,-1-1 1 0 0,1 0-1 0 0,-5-6 495 0 0,5 1-5994 0 0,2-5-1719 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-103406.919">14894 15580 8288 0 0,'0'0'190'0'0,"4"-6"253"0"0,10-7-212 0 0,28 2 5159 0 0,1 6-1205 0 0,-15 13-2607 0 0,-5-3 202 0 0,-15-3-715 0 0,-14-5-592 0 0,-39 9 113 0 0,-37 15 500 0 0,77-19-1076 0 0,3 0 0 0 0,-3 1 0 0 0,2-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1-1 0 0,2 0 1 0 0,-1-1 0 0 0,-1 0 0 0 0,2 2 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 3 0 0 0,2-2 0 0 0,-1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-2 0 0 0,0 3-10 0 0,-2 7 2 0 0,1-7-2 0 0,1 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1-2 0 0 0,3 7 0 0 0,12 15 0 0 0,-16-26 1 0 0,2 2 37 0 0,1 0 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,0-2 1 0 0,1 1 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,0 1 0 0 0,2-1-1 0 0,-2 0 1 0 0,3-1-39 0 0,45-29 241 0 0,-38 15-275 0 0,-2 3 0 0 0,2-4 0 0 0,-3-1 0 0 0,0 3 0 0 0,-1-4 0 0 0,0 3 0 0 0,-1-3 34 0 0,13-70-964 0 0,-14 35 382 0 0,-18 90 634 0 0,10-24-10 0 0,1 0 0 0 0,0-1 0 0 0,1 2 0 0 0,0-2-1 0 0,1 1 1 0 0,0-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,3-2-1 0 0,-2 3 1 0 0,5 5-42 0 0,14 48 54 0 0,-9-45-1794 0 0,-6-21 730 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-98716.919">15952 14928 3224 0 0,'0'0'143'0'0,"0"0"279"0"0,0 0 1073 0 0,0 0 470 0 0,0 0 92 0 0,0 0-154 0 0,0 0-730 0 0,0 0-315 0 0,0 7 684 0 0,-3 1-898 0 0,3-6-48 0 0,0 8 1051 0 0,-7 46 1551 0 0,-36 305 1366 0 0,39-336-4246 0 0,3 2 0 0 0,0-2-1 0 0,2 1 1 0 0,0 1 0 0 0,3 0-1 0 0,-1-3 1 0 0,2 3-1 0 0,5 17-317 0 0,22 16 208 0 0,-30-55-186 0 0,1-2 0 0 0,1 2 0 0 0,-1-1-1 0 0,2 1 1 0 0,-3-1 0 0 0,3 0 0 0 0,-2-2-1 0 0,1 2 1 0 0,1-1 0 0 0,-2 0 0 0 0,2 0-1 0 0,1 0 1 0 0,-2-1 0 0 0,1 1-1 0 0,-1-2 1 0 0,2 1 0 0 0,0-1 0 0 0,-3 1-1 0 0,3-1 1 0 0,3 0-22 0 0,-5-2 31 0 0,0 1-1 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,-1 0 1 0 0,0-2-1 0 0,2 2 1 0 0,-2-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1-1 0 0,-2-1 0 0 0,1 1 1 0 0,0-2-1 0 0,-1 1 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 0-1 0 0,1-1-30 0 0,-2 5 3 0 0,10-18 55 0 0,-3 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-2 1 0 0 0,4-20-58 0 0,5-16 41 0 0,22-98-41 0 0,16-149-432 0 0,-48 263-57 0 0,-1 7-2509 0 0,-1 9-4848 0 0,-1 12 100 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-97336.919">17060 15459 2304 0 0,'0'0'101'0'0,"0"17"22"0"0,-7 6 6125 0 0,-4 18 4249 0 0,9-10-9080 0 0,-2 88 316 0 0,0-86-1477 0 0,0-19-426 0 0,3-13-721 0 0,1-1-329 0 0,0 0-75 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-96826.919">17307 14993 8288 0 0,'0'0'381'0'0,"0"0"-6"0"0,0 2-242 0 0,5 72 6774 0 0,-10 3-1144 0 0,-8 42-2340 0 0,3 50-2718 0 0,5-9-705 0 0,0 15-1521 0 0,5-165 244 0 0,0-8-61 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-96436.919">17559 15426 10136 0 0,'0'0'777'0'0,"-1"2"-505"0"0,-3 42 4407 0 0,3-11-457 0 0,3 79-789 0 0,-4-103-3589 0 0,2-1-1781 0 0,0-7 758 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95846.919">17971 15413 1376 0 0,'1'-2'299'0'0,"13"-58"5252"0"0,-16 43-5059 0 0,1 13-375 0 0,1 3 35 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-2 0 0 0,-1 2 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,1-1-152 0 0,-4 1 283 0 0,1 1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-2 1 0 0 0,3-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 2 1 0 0,2-2-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 1-285 0 0,-8 13 754 0 0,-45 64 501 0 0,34-5-220 0 0,21-69-992 0 0,0 0-1 0 0,2 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 2 1 0 0,0-2-1 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-2 0 1 0 0,1-1-1 0 0,2 0 1 0 0,-2 1-1 0 0,4 2-41 0 0,2 6 59 0 0,7 9 178 0 0,-12-20-112 0 0,-1 0 0 0 0,0 2-1 0 0,0-1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1-1 0 0,1 2 1 0 0,-1-2 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 1-125 0 0,-14 15 28 0 0,10-19-9 0 0,1 0 0 0 0,-2 1 1 0 0,0-2-1 0 0,0 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0 1 0 0,3 1-1 0 0,-3-2 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1-19 0 0,-36 2-215 0 0,5 21-3705 0 0,32-15-4023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-95136.919">18298 15512 3680 0 0,'0'0'284'0'0,"0"0"109"0"0,2-1 1154 0 0,28-18 5762 0 0,35 18-2771 0 0,-35 11-2764 0 0,-15 1 1490 0 0,-61-18-3312 0 0,41 5 32 0 0,1 1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-2 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,1 1 1 0 0,1 0-1 0 0,-2 0 0 0 0,2 1 1 0 0,1 1-1 0 0,-3-1 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1 3 16 0 0,-1-1 34 0 0,-1 0-1 0 0,2 1 0 0 0,-1 0 0 0 0,1 1 1 0 0,1 0-1 0 0,-2-1 0 0 0,2 1 1 0 0,0 2-1 0 0,0-2 0 0 0,0 1 0 0 0,-1 4-33 0 0,4-8 57 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 2 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,2 2-56 0 0,-2-4 45 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-2 0 0 0,-2 1 0 0 0,3-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,2-1-1 0 0,-2-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1-2 0 0 0,-1 2 0 0 0,0-1 0 0 0,1-1-45 0 0,98-157-3426 0 0,-100 161 3373 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,2-1 0 0 0,-2 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 53 0 0,-2 21 337 0 0,-16 81 1575 0 0,10 7-1206 0 0,16-65-7272 0 0,-5-33-749 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-98036.919">16751 14877 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 2 76 0 0,-5 12 2311 0 0,-7 36 3900 0 0,-3 117-3759 0 0,-16 87 806 0 0,3 42-2464 0 0,20-205-1627 0 0,8-90-756 0 0,-3-6-2095 0 0,3-4 1602 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-97796.919">16670 15159 11232 0 0,'-4'-29'1016'0'0,"5"29"-836"0"0,13-29 2777 0 0,64 24 2000 0 0,16 19-1797 0 0,-52 7-4345 0 0,-35-17-189 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-93526.919">19210 15587 15664 0 0,'13'6'1187'0'0,"-10"-5"-976"0"0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,1 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,-1-2 1 0 0,1 2-1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,2-1 1 0 0,-2 1-1 0 0,1-3-210 0 0,8-11-211 0 0,-5 9-129 0 0,-1-2 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 2 0 0 0,2-11 340 0 0,-9-35-1540 0 0,4 53 1562 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-2 1 0 0 0,2-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-22 0 0,-20 18 1568 0 0,17-14-1383 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,2 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,2 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 0 0 0 0,1 0 0 0 0,0 0-185 0 0,-7 32 308 0 0,5-27-103 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,0 2 0 0 0,0-2 0 0 0,1-1-1 0 0,0 2 1 0 0,1-1 0 0 0,2 1 0 0 0,-1 1-205 0 0,15 20 1394 0 0,-16-34-1436 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 2-1 0 0,0-2 0 0 0,-1 0 0 0 0,1-2 1 0 0,-1 2-1 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,2 0 0 0 0,-2 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,1 0 42 0 0,0-1-47 0 0,91-60-5723 0 0,-78 51 4417 0 0,-5 2-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94286.919">18793 15258 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0-7 199 0 0,4-20 284 0 0,-4 27 22 0 0,0 0 21 0 0,0 0 53 0 0,0 0 198 0 0,0 0 86 0 0,0 0 21 0 0,0 0-28 0 0,0 0-122 0 0,-11 90 4045 0 0,4-23-3014 0 0,-22 183 836 0 0,14-110-2456 0 0,13-123-5049 0 0,1-16-3688 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-94056.92">18772 15379 19351 0 0,'0'0'439'0'0,"0"0"62"0"0,0 0 33 0 0,0 0-65 0 0,7-3-292 0 0,93-19 2799 0 0,-40 11-2385 0 0,-22 8-4619 0 0,-36 3 2335 0 0,-2 0-17 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-89026.919">19589 15469 920 0 0,'0'0'115'0'0,"0"0"146"0"0,0 0 68 0 0,2-1 14 0 0,11-25-975 0 0,0 12 771 0 0,-12 12 195 0 0,-1 2 149 0 0,0 0 590 0 0,0 0-1059 0 0,7-8 9846 0 0,-2 5-8006 0 0,-4 1-1530 0 0,1 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1-2-324 0 0,1 0 1337 0 0,0 4-893 0 0,-10 8-200 0 0,-30 60 2244 0 0,14 3-1504 0 0,24-15-648 0 0,2-55-335 0 0,1 8 28 0 0,0-2-1 0 0,1 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,-1 2 1 0 0,3-1 0 0 0,-2-1-1 0 0,1 0 1 0 0,1-1 0 0 0,-1 2-1 0 0,0-1 1 0 0,2 0-1 0 0,1 1-28 0 0,-2-3 14 0 0,0 0-1 0 0,0 0 0 0 0,2 1 0 0 0,-2-1 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-2 0 0 0,5-1-13 0 0,33-22 64 0 0,-3-47 8 0 0,-16-10-72 0 0,-17 43-89 0 0,3-55-263 0 0,-10 94 324 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 29 0 0,-3 9-8024 0 0,1 0 350 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88466.92">20077 15340 2304 0 0,'0'0'101'0'0,"0"0"363"0"0,0 0 1439 0 0,0 0 626 0 0,0 0 126 0 0,0 0-194 0 0,3-14 1239 0 0,0 23 4485 0 0,-1 47-5205 0 0,-7 23-1571 0 0,2 35-565 0 0,-5-51-599 0 0,9 97 126 0 0,6-102-812 0 0,5-132-3199 0 0,-10 24-1172 0 0,-2 36 2865 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-88226.92">20085 15485 11976 0 0,'0'0'546'0'0,"0"0"-10"0"0,0 0-150 0 0,-8-5 3377 0 0,18-32 352 0 0,33-15-1964 0 0,-36 49-2182 0 0,-4 1 153 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,3 1-123 0 0,36 11 165 0 0,-8 24-245 0 0,-11 20-3497 0 0,-22-54-1940 0 0,-1-2-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-86216.919">20726 15308 9416 0 0,'-2'-4'852'0'0,"-23"-9"284"0"0,14 11 6835 0 0,-11 31-4820 0 0,19-20-2774 0 0,-52 128 2838 0 0,26-38-1934 0 0,20-71-1118 0 0,3-3 0 0 0,0 4-1 0 0,1-1 1 0 0,1 0 0 0 0,2 0 0 0 0,1 2-1 0 0,0-4 1 0 0,3 10-163 0 0,-2-19-6 0 0,15 119-229 0 0,3-78-1218 0 0,-1-37-2030 0 0,-10-15-2522 0 0,-7-5-1562 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-85956.919">21071 15262 11520 0 0,'0'0'886'0'0,"1"-1"-582"0"0,16 6 5156 0 0,-12-1-5008 0 0,-1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,0 0 0 0 0,1 0-1 0 0,-2-1 1 0 0,-1 2 0 0 0,1-1-1 0 0,1 0 1 0 0,0 5-452 0 0,6 13 803 0 0,6 62 1048 0 0,-11-36-1193 0 0,-4 50 394 0 0,-5 10-300 0 0,-11 6-403 0 0,-14 46-253 0 0,3-48-2616 0 0,-10-3-4080 0 0,20-62-2023 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-80646.919">2429 13832 2760 0 0,'-21'-11'247'0'0,"9"-2"39"0"0,11 13 290 0 0,-4-1-375 0 0,4-4 6201 0 0,0-2-5440 0 0,12 5 7229 0 0,-5 2-9038 0 0,97 45 4699 0 0,-28-8-2217 0 0,50-16-519 0 0,50 0-182 0 0,-22 28-394 0 0,-126-37-455 0 0,-5-1-32 0 0,2 0 0 0 0,0-1-1 0 0,-1-2 1 0 0,2 0-1 0 0,-1-1 1 0 0,1-2-1 0 0,1-1 1 0 0,-1-2-1 0 0,0 0 1 0 0,8-2-53 0 0,149-30 1189 0 0,97-37-261 0 0,-100 44-928 0 0,-150 21 0 0 0,300-2 0 0 0,-24 32 15 0 0,26-10 250 0 0,14 11-174 0 0,-125-12 135 0 0,-11 5-42 0 0,126 18-48 0 0,-227-28-125 0 0,84 12 42 0 0,202 33 22 0 0,124 2 393 0 0,-211-19-403 0 0,359 61 135 0 0,-273-60-200 0 0,-50 2-61 0 0,-54-2 141 0 0,8 4-80 0 0,-104-23 0 0 0,81-2 0 0 0,162 6 0 0 0,-181-4 0 0 0,73-9 0 0 0,192-23 0 0 0,-305 11 0 0 0,-34 5 0 0 0,316-2 0 0 0,-272-14 0 0 0,415-12-9 0 0,-326 3 914 0 0,-19-10-1376 0 0,67 4 966 0 0,-82 30-599 0 0,-8 4-152 0 0,-135 3 112 0 0,-5 5 239 0 0,4-3 314 0 0,58 6-541 0 0,32-16-88 0 0,2-7 252 0 0,-115-5-160 0 0,200-26 128 0 0,-67-1 0 0 0,-45 7 11 0 0,10-2-22 0 0,120 6 11 0 0,-34 4 80 0 0,116 7-133 0 0,-159 16 42 0 0,198-17 11 0 0,-133 10 0 0 0,44 0 0 0 0,322 26 139 0 0,-137-29-86 0 0,-328 21 75 0 0,-18-1-128 0 0,-87-21 0 0 0,-9-7 148 0 0,27-14-132 0 0,-44 16-28 0 0,70 16 12 0 0,-51 7-96 0 0,-101-9 80 0 0,-9 3 5 0 0,-13 13-319 0 0,20-4 154 0 0,10 8-187 0 0,-8 4 347 0 0,0 60 16 0 0,-6 87 15 0 0,13 163 28 0 0,0-118-101 0 0,19 26 233 0 0,-6-3-91 0 0,-4 19-20 0 0,-28-45 106 0 0,-4-63-95 0 0,-1-20-75 0 0,1 16 0 0 0,-1-28 224 0 0,-6-29-160 0 0,14-83-64 0 0,1-3 0 0 0,-1 1 0 0 0,0-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-4-1 0 0 0,-16 8 0 0 0,3-8 0 0 0,-306 8 96 0 0,111-15-96 0 0,-234 4 0 0 0,55 4 71 0 0,-120 6-86 0 0,-150-20 71 0 0,42-1-136 0 0,59 5 80 0 0,89-1 0 0 0,-369-11 0 0 0,156 0 68 0 0,192 9 268 0 0,273 9-440 0 0,-581-17 204 0 0,270-20-164 0 0,108 5 77 0 0,-375-1 78 0 0,326 12-91 0 0,-3-16 0 0 0,23 5 0 0 0,94 15 0 0 0,76 10 0 0 0,-222 7 0 0 0,217 4 0 0 0,-832-1 0 0 0,289-46 0 0 0,307 7 0 0 0,-128-8 0 0 0,431 21 0 0 0,1-9 0 0 0,-72-10 0 0 0,174 31 0 0 0,1 5 0 0 0,-108 10 0 0 0,32 9 0 0 0,14 1 0 0 0,-39-11 0 0 0,24-13 0 0 0,-21 3 0 0 0,-173-3 0 0 0,183 17 0 0 0,-31-14 0 0 0,61 4 0 0 0,155 4 0 0 0,-126 7 0 0 0,-64-7 0 0 0,108-8 0 0 0,-51-11 0 0 0,59 11 0 0 0,-85 4 0 0 0,115-3 0 0 0,-77-2 0 0 0,47-3 0 0 0,89 10-60 0 0,4 1-252 0 0,1 0-111 0 0,0 0-1358 0 0,0 0-5615 0 0,0 0-2407 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-74756.919">2423 13719 1376 0 0,'0'0'65'0'0,"0"1"-6"0"0,0 16 154 0 0,0-15 831 0 0,0-2 358 0 0,0 0 65 0 0,0 0-83 0 0,0 0-422 0 0,0 0-186 0 0,0 0-38 0 0,0 0-28 0 0,0 0-88 0 0,0 0-40 0 0,0 0-6 0 0,0 0 2 0 0,0 0 12 0 0,0 0 2 0 0,0 0 0 0 0,0 0-2 0 0,0 0-4 0 0,0 0-2 0 0,0 0-1 0 0,0 9 1801 0 0,6 106 2520 0 0,2-8-2608 0 0,3 115-760 0 0,-11-3-472 0 0,37 58-113 0 0,-32-238-854 0 0,24 101-208 0 0,-2 69 1907 0 0,-14-81-2238 0 0,18 173 898 0 0,-34-184-286 0 0,-53 142-20 0 0,50-159-169 0 0,6-50-56 0 0,-3 9 374 0 0,-14 51-182 0 0,16-23-546 0 0,8-13 992 0 0,5-1-446 0 0,-10-67-106 0 0,0-5-17 0 0,-2-1-234 0 0,-7-19-3530 0 0,7 10 2303 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151003.0799">2511 7638 4144 0 0,'0'0'319'0'0,"-5"1"252"0"0,5-2 2376 0 0,23-33-2360 0 0,-27 17 5029 0 0,4 16-5505 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 1 0 0,-2 1-112 0 0,-51 23 1284 0 0,15 1-659 0 0,-29 36 50 0 0,17-10-590 0 0,-95 125 107 0 0,48-42-21 0 0,6 2 334 0 0,14-6-252 0 0,-17 48-182 0 0,-55 145 566 0 0,135-285-548 0 0,-59 178 254 0 0,2 100-151 0 0,37-58 504 0 0,15-109-216 0 0,8 108 134 0 0,9-138-457 0 0,-3 110 104 0 0,14-115-187 0 0,5 1-1 0 0,16 59-73 0 0,4-9 269 0 0,27 66-269 0 0,-6-40 164 0 0,18 66 46 0 0,-16-74 888 0 0,64 138-1098 0 0,16 35 320 0 0,-95-238-133 0 0,23 46 186 0 0,-3-47 46 0 0,17 59-249 0 0,-14-27-191 0 0,-20-56 21 0 0,24 55 139 0 0,-37-59-22 0 0,-27-80-141 0 0,-4-7-107 0 0,0-2-69 0 0,0 0-21 0 0,0-3-260 0 0,0-9-1082 0 0,-4-5-465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151703.0799">1809 13402 13824 0 0,'-53'24'1677'0'0,"52"-23"-740"0"0,27-3 3060 0 0,7 0-4365 0 0,73 36 323 0 0,2 35 373 0 0,-11 8 165 0 0,117 104 1071 0 0,-188-163-1495 0 0,-2-3-1 0 0,2-1 0 0 0,0-2 0 0 0,2 1 1 0 0,22 4-69 0 0,68 12 245 0 0,-53-21 458 0 0,-51-19 147 0 0,-13 9-799 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 2-1 0 0,-1-1 1 0 0,1-1 0 0 0,0 0 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,0-2-51 0 0,0-4 176 0 0,-21-115 411 0 0,-20-85-1189 0 0,0 65-4384 0 0,22 89 2801 0 0,-5 9-21 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="152993.0799">2716 13785 2760 0 0,'-8'-3'248'0'0,"-34"-31"6865"0"0,23 5-6498 0 0,-13-21 774 0 0,-3-5 1367 0 0,2-28 825 0 0,7 6-1573 0 0,18 19-676 0 0,0-14-560 0 0,11-77 1085 0 0,18 5-1137 0 0,-11 93-1006 0 0,-13 7-1132 0 0,0 6-1456 0 0,5 36 1591 0 0,3 0-48 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="154173.0799">4937 10418 14976 0 0,'-26'22'1597'0'0,"-12"-9"-1817"0"0,37-13 85 0 0,1 0-121 0 0,-8-1-614 0 0,-5-22 1632 0 0,5-14 143 0 0,-9-57 2063 0 0,-2-15-936 0 0,2-83-705 0 0,13-25-328 0 0,0 23-897 0 0,2-168 234 0 0,0-26 12 0 0,10 202-193 0 0,-2-125-36 0 0,-8 155-1315 0 0,29 91-2477 0 0,-18 51 2086 0 0,0-14-2513 0 0,-8 24 1999 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="154583.0799">4244 8323 18887 0 0,'0'0'863'0'0,"-1"-1"-14"0"0,1-12-806 0 0,-1 1-1 0 0,2 1 0 0 0,-1-2 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 2 0 0 0,2-1 0 0 0,-2 0 1 0 0,2 1-1 0 0,0-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,1 0 0 0 0,2 0 0 0 0,-1 2 1 0 0,0-1-1 0 0,3-1-42 0 0,-2-1-42 0 0,127-203-129 0 0,-64 111 171 0 0,30-2 0 0 0,-87 97 2 0 0,-3-1-1 0 0,1 2 0 0 0,2 0 0 0 0,-2 1 0 0 0,3-1 0 0 0,-2 1 1 0 0,1 2-1 0 0,1-1 0 0 0,6-1-1 0 0,-12 6 48 0 0,1 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0-1 0 0,2 1 1 0 0,0 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 2 1 0 0,-2-1 0 0 0,2 1-1 0 0,-1 0 1 0 0,1 2 0 0 0,0-1-1 0 0,-2 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 2 0 0 0,1-1-1 0 0,-2 0 1 0 0,0 1 0 0 0,1 0-1 0 0,-2 2 1 0 0,1-2 0 0 0,-1 0-1 0 0,0 2 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 3-47 0 0,75 216 1312 0 0,-20-38-1200 0 0,-28-61-32 0 0,-3-33-402 0 0,5-40-2524 0 0,-22-47 814 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="156043.0799">2332 15337 13040 0 0,'-2'7'1185'0'0,"-26"30"-737"0"0,2-30 563 0 0,-32-20 2664 0 0,26-5-2667 0 0,-41-17 867 0 0,38 15-1425 0 0,0 2 0 0 0,2-5 0 0 0,-1-2-1 0 0,3 1 1 0 0,-15-16-450 0 0,-174-175 1230 0 0,188 178-981 0 0,-31-29-91 0 0,4-4 0 0 0,4-3 1 0 0,-4-9-159 0 0,-134-223 786 0 0,-92-179 150 0 0,187 268-915 0 0,11-4 1 0 0,7-4-1 0 0,-5-60-21 0 0,-67-200 160 0 0,70 179-160 0 0,-48-197-216 0 0,78 263 184 0 0,9-3 0 0 0,3-65 32 0 0,3-72-64 0 0,9 69 0 0 0,17 188 64 0 0,4-1 0 0 0,7-111 0 0 0,3 169 0 0 0,5-76 0 0 0,21-96 0 0 0,27-114-80 0 0,56-148-171 0 0,-7 154-223 0 0,-16 97 455 0 0,-50 156 70 0 0,6 3 0 0 0,1 2-1 0 0,10-8-50 0 0,-23 43 25 0 0,83-116 30 0 0,43-1-129 0 0,9 31-44 0 0,36-37-58 0 0,-156 132 134 0 0,82-65-842 0 0,-130 108 868 0 0,26-15-1611 0 0,-14 12-5936 0 0,-11 3 272 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="156463.0799">1464 6074 11976 0 0,'0'0'922'0'0,"-1"-2"-600"0"0,-7-10-54 0 0,7 11 932 0 0,-1-8 2652 0 0,0-6-2353 0 0,6 12-1499 0 0,-1-2-1 0 0,0 1 0 0 0,0 0 0 0 0,2 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 1 1 0 0,2-1-1 0 0,-3 1 0 0 0,2 1 0 0 0,2-1 1 0 0,18-12-106 0 0,94-29-209 0 0,-109 39 308 0 0,0-1-1 0 0,2 3 1 0 0,-1-1-1 0 0,0 1 1 0 0,1 1-1 0 0,0 0 1 0 0,-2 1-1 0 0,2 1 0 0 0,0-1 1 0 0,-1 2-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 1 1 0 0,1 2-1 0 0,-2-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,8 6 8 0 0,-9-2 12 0 0,1 0 0 0 0,-2 1-1 0 0,1 2 1 0 0,-1-3 0 0 0,0 3-1 0 0,0 0 1 0 0,4 9-12 0 0,-4-3 37 0 0,1 2 0 0 0,-1-1 1 0 0,-2 1-1 0 0,1 0 0 0 0,-3 0 1 0 0,3 18-38 0 0,-3 87 434 0 0,-29-12 5 0 0,12-77-354 0 0,-48 123 75 0 0,-64 120-1810 0 0,112-252 551 0 0,0 0-48 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="157893.0799">8831 5864 13360 0 0,'-4'-1'271'0'0,"1"0"1"0"0,-2 0 0 0 0,1 0-1 0 0,0-1 1 0 0,2 0 0 0 0,-2 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,1 0 1 0 0,-2-1 0 0 0,2 1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1-1 0 0,1-2 1 0 0,1 1-272 0 0,-2-3 27 0 0,1 0 0 0 0,0 0 0 0 0,1 2-1 0 0,0-2 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-2 0 0 0,1-3-27 0 0,-1-8 302 0 0,-10-129 1863 0 0,-8-4-421 0 0,-4-150 624 0 0,4 53-1161 0 0,-11-355-614 0 0,22 347-593 0 0,0 81-104 0 0,7 169 61 0 0,0-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 1 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-2 0 0 0,-1-2 43 0 0,2 9-62 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 2 0 0 0,1-2 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-2 0 0 0,-2 2 0 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 62 0 0,-8 16-1775 0 0,2 4-289 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="158203.0799">8100 3533 22607 0 0,'0'0'514'0'0,"-1"-2"71"0"0,-1 0-530 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1-2-1 0 0,0 2 0 0 0,1-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0-1 0 0 0,0 2 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1-55 0 0,12-17-19 0 0,1-2-1 0 0,-2 4 0 0 0,3-3 1 0 0,0 3-1 0 0,0 1 1 0 0,2-1-1 0 0,-1 2 0 0 0,3 1 1 0 0,-1 1-1 0 0,3-2 20 0 0,23-19-44 0 0,-36 27-32 0 0,-1 0 0 0 0,2 2 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,3-2 0 0 0,-3 2 0 0 0,2 0-1 0 0,-1 2 1 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 1 76 0 0,-4 2-16 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 2 0 0 0,-2-1 0 0 0,1-1-1 0 0,0 2 1 0 0,0 0 16 0 0,53 142 542 0 0,-31-92-361 0 0,2-1 0 0 0,4-1 1 0 0,15 24-182 0 0,43 49-220 0 0,-48-66-1394 0 0,-21-37-78 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2203,33 +2196,33 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">247 705 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">640 722 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-9 10039 0 0,4 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1036 664 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1384 746 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,4-23-839 0 0,-7 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 79 971 0 0,13-78-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,3-28 325 0 0,-7 43 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 35 365 0 0,9-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-43 40 0 0,-1 48 757 0 0,-8 6-562 0 0,-2 1-34 0 0,14 15 96 0 0,-24 51 294 0 0,10-64 48 0 0,0-2-24 0 0,-12 10 14 0 0,11-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-12 0 0,-1-2-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,16-18-798 0 0,-5 23 705 0 0,11 17 39 0 0,-21-13 64 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 2-10 0 0,2-5 84 0 0,-5 17 237 0 0,-20-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 11-3207 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">1679 463 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 57 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,1 17 113 0 0,-2-14-1404 0 0,-1 51 981 0 0,-4-2-1688 0 0,1-59-1417 0 0,-2-32 962 0 0,-7-28-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">1615 598 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-32 2722 0 0,-14 31-3180 0 0,15-15 1008 0 0,23-24 674 0 0,-35 36-2057 0 0,1 2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 19 1009 0 0,-52 14 55 0 0,-4-18-600 0 0,21 47 1448 0 0,-23 2-2113 0 0,-15-60 230 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 22 399 0 0,1-11-337 0 0,7-8-104 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 37 0 0,-35-1 653 0 0,-7-25-4978 0 0,34 19 2334 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">3007 428 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 48 1154 0 0,-12 24 2052 0 0,-3 33 1755 0 0,3 52-2463 0 0,4-54-962 0 0,-3 32-1172 0 0,7-140-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-3 13-2556 0 0,2-23 1622 0 0,1-1-894 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">3025 486 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-4 772 0 0,-14 10-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 1 1 0 0,2 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 2-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-4-1-4 0 0,-53-44-4198 0 0,55 42-3651 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">2231 124 3680 0 0,'-6'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,8 16-23 0 0,2-13-297 0 0,6 3-1604 0 0,-9 95 2 0 0,7-77 200 0 0,1-18-716 0 0,2-41-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">2155 695 1376 0 0,'5'-20'2159'0'0,"2"0"4223"0"0,7-6-3735 0 0,-2 6-1523 0 0,11-17 1153 0 0,4 12 523 0 0,-4 3-1591 0 0,22-17 135 0 0,-44 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 7-27 0 0,10 30 368 0 0,29 120 1443 0 0,-20-124-1634 0 0,1-14-84 0 0,-13-23-77 0 0,-6-2-29 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 13 0 0,40-28-350 0 0,19-12-3834 0 0,-54 36 2533 0 0,3 3-12 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">1 302 6448 0 0,'7'21'6309'0'0,"-7"-18"-6682"0"0,4 54 3514 0 0,8 85-847 0 0,-2-44-690 0 0,-5-10-929 0 0,13 132 737 0 0,-29 32 57 0 0,6-176-1337 0 0,-1-48-256 0 0,5-13-955 0 0,1-11-4480 0 0,0-4-582 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">12 333 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,18-38 6274 0 0,-18 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,12-3 291 0 0,71-18 828 0 0,-37 5-729 0 0,11-5 96 0 0,51 12 370 0 0,-61 8-222 0 0,43 2-1079 0 0,-21-6 16 0 0,36-20 451 0 0,-30 15 1144 0 0,62 1-1448 0 0,3 19 224 0 0,-53-19-645 0 0,-30-1 1538 0 0,7 0-1123 0 0,-37 8-292 0 0,52 0 264 0 0,-26-6 20 0 0,55-26 70 0 0,11 18-205 0 0,12 9 34 0 0,-66-4 219 0 0,23-5-424 0 0,-5 12 192 0 0,-11 5 584 0 0,44 1-1352 0 0,-6 9 736 0 0,0 6 1017 0 0,-32-10-298 0 0,-12 0-1239 0 0,27-4 520 0 0,14 3 64 0 0,12 29 75 0 0,-60-11-166 0 0,14 1 523 0 0,-3-9-840 0 0,-22-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,74-9-197 0 0,-22 19 0 0 0,-41-15-20 0 0,-43-2 0 0 0,-14-5 0 0 0,25 17 0 0 0,-38-3 0 0 0,5 6 0 0 0,13 23 64 0 0,-5 28 0 0 0,-8 23-64 0 0,-5 32-8 0 0,1-51 125 0 0,-4 32-203 0 0,-8 34 295 0 0,8 44-190 0 0,-17-84 82 0 0,-1-41-13 0 0,6-44 96 0 0,6-12-234 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 2 51 0 0,0-3 114 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0-114 0 0,-14 0 158 0 0,-98 8-218 0 0,82-3 59 0 0,0-1-1 0 0,0-2 1 0 0,0-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-23-6 1 0 0,5-4-9 0 0,-1 3 0 0 0,0 3 0 0 0,0 2 0 0 0,-22 2 9 0 0,-112 0 332 0 0,139 4-330 0 0,0-1-1 0 0,-1-3 1 0 0,1-2-1 0 0,0-1 1 0 0,-8-7-2 0 0,23 9-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-21 4 18 0 0,-142 30 64 0 0,-4-12-136 0 0,-48-9 152 0 0,173-13-80 0 0,-92 0 11 0 0,-34-17 42 0 0,102 17-53 0 0,-24-13 80 0 0,23-11-176 0 0,-85-18 224 0 0,56 22-196 0 0,63 6 192 0 0,-62-3-124 0 0,50 11 0 0 0,46 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12">6715 897 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,22-14-8855 0 0,-18 9 1888 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13">7090 941 10592 0 0,'-13'-13'818'0'0,"10"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">7438 851 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,5 0-232 0 0,-2 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">7801 941 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-38 1231 0 0,1 45-2463 0 0,0 1 0 0 0,2 1 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,-1 3-113 0 0,3-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-16-143 0 0,-13 33-62 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-2-43 0 0,3 2 32 0 0,1 10 23 0 0,-10 18 200 0 0,3-27-96 0 0,-7 4-695 0 0,14-7-611 0 0,7-10-5710 0 0,-6 6 446 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">8085 572 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 22-45 0 0,-12-25-3788 0 0,3 8 1039 0 0,3 83 1637 0 0,7 83-1221 0 0,-14-86-1606 0 0,0-79-341 0 0,-2-4-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">8386 613 2760 0 0,'4'8'1828'0'0,"4"20"4892"0"0,5 25-3444 0 0,1 103 1947 0 0,-11-80-3937 0 0,-6-37-4508 0 0,3-36 1701 0 0,-4 6-229 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">8439 941 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,9-39 5734 0 0,3-11-521 0 0,-16 20-3279 0 0,11 10-1202 0 0,8-37 1 0 0,-14 56-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,3 0-93 0 0,2-2 95 0 0,-4 3-21 0 0,26 0-60 0 0,2 14-14 0 0,-6 7 0 0 0,-20-12 0 0 0,10 23 0 0 0,19 74 514 0 0,-19-52 356 0 0,6-19-278 0 0,-20-34-517 0 0,7 3 98 0 0,-5-1-141 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-29-4233 0 0,-22 32 2840 0 0,0 1-164 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">9226 669 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-39-6 1747 0 0,43 9-1667 0 0,4-2 170 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 42-483 0 0,18 2 618 0 0,16 12 378 0 0,10 4-513 0 0,15-4 1899 0 0,26-11-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 0 0 0 0,-22-9 0 0 0,-2 2 0 0 0,0-5-64 0 0,31-22-5497 0 0,-32 16 3530 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">9491 1002 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-17 649 0 0,-9 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 20 784 0 0,-16 13 56 0 0,6-32-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">9763 661 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 73 1352 0 0,-5-54-2105 0 0,-9 63 686 0 0,-2-6-314 0 0,3 68-530 0 0,6-113-273 0 0,-3-10 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-3-14-1557 0 0,2-1 195 0 0,-3-2-70 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">9729 664 1376 0 0,'4'6'367'0'0,"-3"-5"1002"0"0,-1-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,9-7 51 0 0,33-23 1588 0 0,-29 24-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,2 2 108 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 2 0 0 0,1-2 1 0 0,0 6-108 0 0,10 27 435 0 0,-1 58 787 0 0,-11-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-3 0 0 0 0,2 0 0 0 0,0 0-56 0 0,-44 35 929 0 0,43-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-5 0 0 0,4-15-5381 0 0,0 15-2125 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">10205 395 0 0 0,'-12'12'0'0'0,"6"-15"140"0"0,4 3 2586 0 0,2 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 30 3000 0 0,-14 31-1947 0 0,1 50 181 0 0,4 1 624 0 0,-7-41-881 0 0,11 38-1316 0 0,-12-26-173 0 0,8-43 0 0 0,14 3-2476 0 0,-12-41 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">10187 825 4376 0 0,'0'0'199'0'0,"10"-11"1918"0"0,-6-2 1016 0 0,11-10 683 0 0,-6-13-1297 0 0,-2-1-472 0 0,5 29-1272 0 0,-10 7-743 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 22 598 0 0,-25-17-674 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 6-227 0 0,6 92 608 0 0,-7-65-165 0 0,-1-12 997 0 0,27-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,12-10-60 0 0,-19 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">10815 698 2760 0 0,'0'1'207'0'0,"0"45"6763"0"0,0-45-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 13-344 0 0,-2 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 9-1278 0 0,-12 63 616 0 0,0-18 973 0 0,13 39-2158 0 0,3-87 962 0 0,-3-26-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">10879 691 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,58-25 1867 0 0,-55 27-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,2 0-156 0 0,-1 0 96 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1-95 0 0,-1-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 5-94 0 0,-43 58 1952 0 0,47-67-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">246 709 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">638 726 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-9 10039 0 0,4 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1033 668 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1380 751 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-7-6507 0 0,4-22-839 0 0,-7 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 80 971 0 0,13-79-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,3-29 325 0 0,-7 44 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 36 365 0 0,9-39-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-44 40 0 0,-1 49 757 0 0,-8 6-562 0 0,-2 1-34 0 0,14 15 96 0 0,-24 52 294 0 0,10-65 48 0 0,0-2-24 0 0,-12 10 14 0 0,11-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-12 0 0,-1-2-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-2 1 0 0,0 2-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,16-18-798 0 0,-5 23 705 0 0,11 17 39 0 0,-21-13 64 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 2-10 0 0,2-5 84 0 0,-5 17 237 0 0,-20-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 11-3207 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">1674 466 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 57 3341 0 0,0-33-2076 0 0,-3 52 1115 0 0,1 17 113 0 0,-2-15-1404 0 0,-1 52 981 0 0,-4-2-1688 0 0,1-60-1417 0 0,-2-31 962 0 0,-7-29-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">1610 602 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-33 2722 0 0,-14 32-3180 0 0,15-15 1008 0 0,23-24 674 0 0,-35 36-2057 0 0,1 2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 19 1009 0 0,-52 14 55 0 0,-5-18-600 0 0,22 48 1448 0 0,-23 1-2113 0 0,-15-60 230 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 22 399 0 0,1-10-337 0 0,7-9-104 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 37 0 0,-35-1 653 0 0,-7-25-4978 0 0,34 19 2334 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">2998 430 7488 0 0,'0'0'166'0'0,"0"8"236"0"0,4 47 1154 0 0,-12 24 2052 0 0,-3 34 1755 0 0,3 52-2463 0 0,4-54-962 0 0,-3 32-1172 0 0,7-141-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-3 13-2556 0 0,2-23 1622 0 0,1-1-894 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">3016 489 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-4 772 0 0,-14 10-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,3 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 2-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 2-1 0 0,-1-2 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 1 0 0,-1-2-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-4-1-4 0 0,-53-45-4198 0 0,55 43-3651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">2224 125 3680 0 0,'-6'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,8 17-23 0 0,2-14-297 0 0,6 4-1604 0 0,-9 95 2 0 0,7-78 200 0 0,1-17-716 0 0,2-42-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">2149 699 1376 0 0,'5'-20'2159'0'0,"2"0"4223"0"0,7-6-3735 0 0,-3 6-1523 0 0,12-18 1153 0 0,4 13 523 0 0,-4 3-1591 0 0,22-17 135 0 0,-44 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 8-27 0 0,10 29 368 0 0,29 121 1443 0 0,-20-125-1634 0 0,1-14-84 0 0,-14-23-77 0 0,-5-2-29 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 13 0 0,40-28-350 0 0,19-12-3834 0 0,-54 36 2533 0 0,3 3-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">1 304 6448 0 0,'7'21'6309'0'0,"-7"-18"-6682"0"0,4 54 3514 0 0,8 86-847 0 0,-2-44-690 0 0,-5-11-929 0 0,13 134 737 0 0,-29 31 57 0 0,6-176-1337 0 0,-1-49-256 0 0,5-13-955 0 0,1-11-4480 0 0,0-4-582 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">12 335 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,18-38 6274 0 0,-18 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,12-3 291 0 0,71-19 828 0 0,-38 6-729 0 0,12-5 96 0 0,51 12 370 0 0,-61 8-222 0 0,43 2-1079 0 0,-22-6 16 0 0,37-20 451 0 0,-30 15 1144 0 0,61 1-1448 0 0,4 19 224 0 0,-53-19-645 0 0,-30-1 1538 0 0,6 0-1123 0 0,-36 8-292 0 0,52 0 264 0 0,-26-6 20 0 0,55-27 70 0 0,10 19-205 0 0,13 9 34 0 0,-66-4 219 0 0,22-5-424 0 0,-4 12 192 0 0,-11 5 584 0 0,44 1-1352 0 0,-7 9 736 0 0,1 6 1017 0 0,-32-10-298 0 0,-12 0-1239 0 0,26-4 520 0 0,15 3 64 0 0,12 30 75 0 0,-61-12-166 0 0,15 1 523 0 0,-3-9-840 0 0,-22-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,73-9-197 0 0,-21 19 0 0 0,-41-15-20 0 0,-44-2 0 0 0,-13-5 0 0 0,25 18 0 0 0,-38-4 0 0 0,5 6 0 0 0,13 23 64 0 0,-5 29 0 0 0,-8 22-64 0 0,-5 33-8 0 0,1-52 125 0 0,-4 33-203 0 0,-8 34 295 0 0,8 44-190 0 0,-17-84 82 0 0,-1-42-13 0 0,6-44 96 0 0,6-11-234 0 0,0-1-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 2 51 0 0,0-3 114 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0-114 0 0,-14 0 158 0 0,-97 8-218 0 0,81-3 59 0 0,0-1-1 0 0,0-2 1 0 0,0-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-22-6 1 0 0,4-4-9 0 0,-1 3 0 0 0,0 3 0 0 0,0 2 0 0 0,-22 2 9 0 0,-111 0 332 0 0,138 4-330 0 0,0-1-1 0 0,0-3 1 0 0,0-2-1 0 0,0-1 1 0 0,-8-8-2 0 0,23 10-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-20 4 18 0 0,-143 31 64 0 0,-3-13-136 0 0,-48-9 152 0 0,172-13-80 0 0,-92 0 11 0 0,-33-17 42 0 0,101 17-53 0 0,-23-13 80 0 0,22-11-176 0 0,-85-19 224 0 0,57 23-196 0 0,62 6 192 0 0,-62-3-124 0 0,51 11 0 0 0,45 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12">6695 903 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,22-15-8855 0 0,-18 10 1888 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13">7069 947 10592 0 0,'-13'-13'818'0'0,"10"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">7416 856 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,5 0-232 0 0,-2 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">7778 947 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-39 1231 0 0,1 46-2463 0 0,0 1 0 0 0,2 1 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,-1 3-113 0 0,3-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-16-143 0 0,-13 33-62 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1-1 0 0,1 2 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-2-43 0 0,3 2 32 0 0,1 10 23 0 0,-10 19 200 0 0,3-28-96 0 0,-7 4-695 0 0,14-7-611 0 0,7-10-5710 0 0,-6 5 446 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">8061 575 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 23-45 0 0,-12-26-3788 0 0,3 8 1039 0 0,3 83 1637 0 0,7 84-1221 0 0,-14-86-1606 0 0,0-80-341 0 0,-2-4-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">8361 617 2760 0 0,'4'8'1828'0'0,"4"20"4892"0"0,5 25-3444 0 0,1 104 1947 0 0,-11-80-3937 0 0,-6-38-4508 0 0,3-36 1701 0 0,-4 6-229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">8414 947 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,9-39 5734 0 0,3-12-521 0 0,-16 21-3279 0 0,11 10-1202 0 0,8-38 1 0 0,-14 57-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,3 0-93 0 0,2-2 95 0 0,-4 3-21 0 0,26 0-60 0 0,1 14-14 0 0,-5 7 0 0 0,-20-11 0 0 0,10 22 0 0 0,19 74 514 0 0,-19-51 356 0 0,6-20-278 0 0,-20-34-517 0 0,7 3 98 0 0,-5-1-141 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-29-4233 0 0,-22 32 2840 0 0,0 1-164 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">9199 673 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-39-6 1747 0 0,43 9-1667 0 0,4-2 170 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 42-483 0 0,18 3 618 0 0,16 11 378 0 0,10 4-513 0 0,15-3 1899 0 0,26-12-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 0 0 0 0,-22-8 0 0 0,-2 1 0 0 0,0-5-64 0 0,30-23-5497 0 0,-31 17 3530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">9463 1008 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-17 649 0 0,-9 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 20 784 0 0,-16 13 56 0 0,6-32-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">9734 665 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 74 1352 0 0,-5-55-2105 0 0,-9 64 686 0 0,-2-7-314 0 0,3 69-530 0 0,6-113-273 0 0,-3-11 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-3-14-1557 0 0,2-1 195 0 0,-3-2-70 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">9700 668 1376 0 0,'4'6'367'0'0,"-3"-5"1002"0"0,-1-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,9-7 51 0 0,33-23 1588 0 0,-29 24-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,2 2 108 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 2 0 0 0,1-2 1 0 0,0 6-108 0 0,9 28 435 0 0,0 57 787 0 0,-11-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-56 0 0,-44 35 929 0 0,43-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-5 0 0 0,4-15-5381 0 0,0 14-2125 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">10175 397 0 0 0,'-12'12'0'0'0,"6"-15"140"0"0,4 3 2586 0 0,2 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 31 3000 0 0,-14 30-1947 0 0,1 51 181 0 0,4 1 624 0 0,-7-42-881 0 0,11 39-1316 0 0,-12-27-173 0 0,8-43 0 0 0,14 4-2476 0 0,-12-42 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">10157 830 4376 0 0,'0'0'199'0'0,"10"-11"1918"0"0,-6-2 1016 0 0,11-10 683 0 0,-6-13-1297 0 0,-2-2-472 0 0,5 30-1272 0 0,-10 7-743 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 22 598 0 0,-25-17-674 0 0,1 0-1 0 0,-1 1 1 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 6-227 0 0,6 93 608 0 0,-7-66-165 0 0,-1-12 997 0 0,27-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,12-10-60 0 0,-19 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">10783 702 2760 0 0,'0'1'207'0'0,"0"46"6763"0"0,0-46-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 13-344 0 0,-2 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 10-1278 0 0,-12 62 616 0 0,0-17 973 0 0,13 38-2158 0 0,3-86 962 0 0,-3-27-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">10847 695 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,57-25 1867 0 0,-54 27-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,2 0-156 0 0,-1 0 96 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1-95 0 0,-1 0 94 0 0,1-1 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 5-94 0 0,-43 59 1952 0 0,47-68-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2265,42 +2258,42 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">6030 3748 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-10 0 710 0 0,-68 11 2232 0 0,-104-9 113 0 0,78-16-2111 0 0,98 12-1711 0 0,3 0 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0 0-7 0 0,0 0 3 0 0,-1 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,-2-1-3 0 0,-5-1 53 0 0,-56 15 746 0 0,-4-32-422 0 0,-48 19 95 0 0,21 18-267 0 0,-1-27 255 0 0,19 6-262 0 0,-8-5 515 0 0,26 24-785 0 0,-8-11 316 0 0,71-3-237 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,2 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,1 5-384 0 0,-1 0-2483 0 0,0-5 1589 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">4792 3490 12384 0 0,'-15'-11'1277'0'0,"0"9"-438"0"0,-15 9 3998 0 0,8 3-3431 0 0,-21 14 690 0 0,-51 36-1014 0 0,26-27 402 0 0,7 19-1322 0 0,33-25-154 0 0,-9 15 872 0 0,35-39-855 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-2-1-1 0 0,2 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,2 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,3-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 1 0 0 0,-2-2-1 0 0,4 3-23 0 0,36 38 389 0 0,-27-34-394 0 0,-2-1 1 0 0,2 0-1 0 0,0-1 0 0 0,1-1 0 0 0,-2-1 1 0 0,2 1-1 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,0-1-1 0 0,5 0 4 0 0,-4 0-173 0 0,104 18-1371 0 0,-44 2-4118 0 0,-57-15-1845 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="2">3948 2850 2760 0 0,'9'14'125'0'0,"-24"-7"1798"0"0,-5 9-59 0 0,15-9 428 0 0,-23 6 4862 0 0,28-13-6578 0 0,0 0-15 0 0,0 0-34 0 0,-3 2 119 0 0,2-1-159 0 0,1-1 2989 0 0,56-16-1901 0 0,11 9-396 0 0,21 3-749 0 0,-23 1 156 0 0,42-1 469 0 0,21-4-497 0 0,-4-3-454 0 0,56-3 952 0 0,-54 8-543 0 0,-50-4-402 0 0,53-9 402 0 0,-69 8-745 0 0,4 11 112 0 0,-35-6 120 0 0,16 4 0 0 0,8-13 444 0 0,-25 4-280 0 0,12 0-164 0 0,-24 3 0 0 0,-5 7 0 0 0,17 7-1208 0 0,-27-5 877 0 0,7 3-1583 0 0,8 12-3659 0 0,-8-10 3847 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="3">5463 2400 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,9 22 9129 0 0,23-5-7935 0 0,-16-12-2328 0 0,61 29 1337 0 0,-62-23-2420 0 0,-5-6 346 0 0,0 1 1 0 0,0 0-1 0 0,-2 1 1 0 0,2 0-1 0 0,-2 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,4 8-255 0 0,7 66 1080 0 0,-27-5-224 0 0,-11-28-856 0 0,-29-1 327 0 0,-29-11 1242 0 0,10-15-2553 0 0,38-23-3117 0 0,24-1 2058 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="4">12064 2910 8288 0 0,'11'-46'864'0'0,"-13"43"-720"0"0,4-9 1811 0 0,0 9 5703 0 0,63-2-3242 0 0,-25 5-4222 0 0,80 2 1838 0 0,5 8-1085 0 0,277-13 1101 0 0,-174-1-1030 0 0,-78 8-540 0 0,42-1-45 0 0,12-13 803 0 0,-47-21-1236 0 0,-152 29-64 0 0,-5 2-273 0 0,23-10-2694 0 0,-20 10 2502 0 0,6 0-15 0 0,-3 4-3511 0 0,-2 2-4432 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="5">13855 2481 8288 0 0,'0'0'638'0'0,"-1"1"-414"0"0,-1 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,7 6 488 0 0,68 15 2067 0 0,-40-14-2223 0 0,51 22 954 0 0,-55-9-1577 0 0,43 38 370 0 0,-17 1-375 0 0,29 32 240 0 0,-83-88-712 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-3 1-23 0 0,-2 4 44 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-2-1 0 0 0,1 0-44 0 0,-27 11 59 0 0,0-3-1 0 0,0-1 1 0 0,-1-1 0 0 0,-1-3-1 0 0,1-1 1 0 0,-18 0-59 0 0,30-5-59 0 0,-76-10-1395 0 0,91 4-1171 0 0,10 5 1267 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="6">14979 2598 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-12 7 790 0 0,-13 10 150 0 0,-51 20 1099 0 0,7-3-1196 0 0,66-32-1165 0 0,-13 9 158 0 0,0 0 0 0 0,1 1-1 0 0,0 0 1 0 0,1 2 0 0 0,1-1 0 0 0,0 2 0 0 0,1 0 0 0 0,0 0-1 0 0,-6 12-202 0 0,15-22 65 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-2 1 1 0 0,2 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 1-64 0 0,1 1 108 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,8 2-107 0 0,-4-2 42 0 0,-1-1-1 0 0,0-1 0 0 0,1 0 0 0 0,-2-1 1 0 0,2 0-1 0 0,0-1 0 0 0,0 0 0 0 0,7-2-41 0 0,25-18-4007 0 0,-37 14-3607 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="7">15168 2934 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-5-9 655 0 0,5 3-930 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,2-1 0 0 0,-2 1 0 0 0,4-1-345 0 0,-6 2 74 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,2 0-1 0 0,-2-1 1 0 0,1 1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-3 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 2-73 0 0,2 5 95 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 9-95 0 0,-13 69 1049 0 0,12-81-938 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,0-1-111 0 0,3-3 23 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-2 1 0 0 0,3-1 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2-1 0 0 0,3 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2-1 0 0 0,-2 1 1 0 0,0-1-24 0 0,-2-1-63 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,2-1-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0-5 63 0 0,6-22-2404 0 0,-3 16 1056 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8">15679 2612 0 0 0,'-3'-6'-1709'0'0,"1"-5"9298"0"0,3 9 1867 0 0,-1 14-7849 0 0,4 99 2619 0 0,-7-24-3124 0 0,6 10 60 0 0,-7 38-1060 0 0,13-66-102 0 0,-6-63-68 0 0,-2-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="9">15657 2827 2304 0 0,'0'0'464'0'0,"5"-8"3648"0"0,-5 5 1786 0 0,29-40-750 0 0,12 3-2447 0 0,5 13-1313 0 0,-25 31-788 0 0,-19-4-482 0 0,0 1-42 0 0,2 2-30 0 0,2 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-2 0 1 0 0,3 0-1 0 0,-2 1-46 0 0,24 86 1079 0 0,-14-64-711 0 0,-10-14-53 0 0,19 63 642 0 0,1-36-721 0 0,11-29-183 0 0,40-40-1154 0 0,-29-2-4448 0 0,-33 22 3543 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="10">16426 2435 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,8 2 583 0 0,-5-7-849 0 0,-3 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 16-2962 0 0,1 58 539 0 0,-6 68 472 0 0,-6 14 1084 0 0,8 77-784 0 0,11-188-592 0 0,2-25-84 0 0,12-17 3 0 0,-15-9-156 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1-3-35 0 0,50-40 80 0 0,-43 35-172 0 0,-8 8-92 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1-3 184 0 0,1 0-1288 0 0,2-8-6336 0 0,-7 10 565 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="11">16431 2653 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,62-5 2910 0 0,-44 4-3513 0 0,6 0-489 0 0,-9 4-4783 0 0,-5 1-1037 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="12">16943 2676 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,4 5 4769 0 0,0 0-4077 0 0,0-1-1648 0 0,-3 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 3-394 0 0,-6 179 4855 0 0,0-66-3199 0 0,2-91-1224 0 0,5-10-3265 0 0,-1-13 1400 0 0,0-7-5540 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="13">16981 2907 456 0 0,'2'-11'295'0'0,"-1"9"1230"0"0,7-14 4652 0 0,-8 15-4821 0 0,9-15 3233 0 0,-3 6-3731 0 0,20-34 2412 0 0,-24 42-3133 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-2 0 1 0 0,1 0-137 0 0,41 1 1322 0 0,-41 1-1262 0 0,2 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,2-1 1 0 0,-2 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 2-59 0 0,22 19 91 0 0,-8 1-240 0 0,-17-24-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="14">17470 2970 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,2-3-329 0 0,12-26 1366 0 0,21-4-185 0 0,-35 36-1119 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,1-1-1 0 0,-2 1 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 2-62 0 0,46 63 531 0 0,-44-52-291 0 0,0-1-1 0 0,-3 1 1 0 0,3 1 0 0 0,-4-1-1 0 0,2 0 1 0 0,-2 1 0 0 0,0-1-1 0 0,-2 10-239 0 0,-7 40 0 0 0,-13-24 1095 0 0,1-43-406 0 0,14 1-606 0 0,1 1-72 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,2-1 1 0 0,0 0 0 0 0,-3-2-11 0 0,2 0-209 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-6 209 0 0,0-19-4042 0 0,2 15-3529 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="15">17980 2357 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,3 8 590 0 0,11 65 2596 0 0,-19 145-2669 0 0,-4-74 14 0 0,9 83-1117 0 0,4-176 0 0 0,-1-46-165 0 0,-1-4-698 0 0,-2-1-315 0 0,0-1-1352 0 0,3-5-5157 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="16">18279 2884 3568 0 0,'21'-10'1553'0'0,"-5"-6"1718"0"0,-3 11-2487 0 0,42-32 3450 0 0,-26 10-3218 0 0,35-43-474 0 0,-53 47-542 0 0,-8 15 0 0 0,-6-1 0 0 0,2 6-7 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 1 0 0 0,-3-1 1 0 0,2 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-4 0 6 0 0,0 2 11 0 0,-1-1 1 0 0,0 2-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-2-1 1 0 0,2 1-1 0 0,0 1 1 0 0,2-1-1 0 0,-1 1 1 0 0,-3 5-12 0 0,-16 24 272 0 0,-6 55 161 0 0,28-84-291 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-3-1-1 0 0,2 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-2 1 1 0 0,4-1-142 0 0,-2-1 13 0 0,0 0 0 0 0,-2-1 0 0 0,1 1 1 0 0,0-1-1 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,4 0-13 0 0,66-24-2033 0 0,-61 16 586 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="17">18749 2605 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-2 1-172 0 0,-14 52 5027 0 0,7-26-3083 0 0,-6 31 478 0 0,12-48-2198 0 0,1 1 0 0 0,0 1 0 0 0,2-1 0 0 0,-2 0-1 0 0,2 0 1 0 0,0 0 0 0 0,2 1 0 0 0,-1 5-320 0 0,1 25 797 0 0,-2-35-713 0 0,1-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,2 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1-1-1 0 0,-1 1 1 0 0,3-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,5 3-83 0 0,-7-7 16 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2-1 0 0 0,-3 1 1 0 0,2-1-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1-1 0 0 0,2 1 1 0 0,-3 0-1 0 0,2 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1-2-15 0 0,6-4 20 0 0,19-32 87 0 0,13-39-97 0 0,-37 72-49 0 0,2 0 0 0 0,-2 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-2 0-1 0 0,1 0 1 0 0,-1-6 39 0 0,-4-21-1383 0 0,4 35 837 0 0,-1 0-1200 0 0,-6-5-4721 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="18">17382 2435 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,1-1-292 0 0,6-4-365 0 0,1-2-1 0 0,-1 1 1 0 0,-1-1 0 0 0,2-1-1 0 0,-2 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-1-363 0 0,51-75 852 0 0,-40 67-781 0 0,-1 15-61 0 0,-11 6 2 0 0,-1 0 0 0 0,2 1-1 0 0,-3-1 1 0 0,2 1 0 0 0,-2 0-1 0 0,2 0 1 0 0,-3 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-2 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 2-11 0 0,2 2-4 0 0,6 25 57 0 0,3-4-53 0 0,5 0-1856 0 0,-10-23-4807 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="19">8053 2662 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-12-2-24 0 0,8 2 8851 0 0,1 5-9133 0 0,-9 15-17 0 0,7-17-769 0 0,4-2-3236 0 0,1-1-1404 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="20">20803 2967 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-7 0-423 0 0,1-2-329 0 0,4 2-272 0 0,0-3-398 0 0,-1-1-3749 0 0,-2-8 2451 0 0,4 10-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="21">20521 2696 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-14-3 2088 0 0,-6-4-821 0 0,20 7-1285 0 0,-16 3 543 0 0,-33 27 578 0 0,-4 48-1009 0 0,52-70-646 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,3 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2-1 0 0 0,3 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1-1 0 0 0,2 2-74 0 0,25 24 398 0 0,-28-30-397 0 0,0 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,1-1-1 0 0,10 1-134 0 0,-11-1-167 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-2-1 0 0,0 1 1 0 0,-2 0 301 0 0,-3 2-105 0 0,15-9-1239 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="22">21018 2736 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,6 8 1656 0 0,-5-5-2461 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 2-229 0 0,1 72 2716 0 0,17 158 1049 0 0,-27-72-3749 0 0,-2-92-16 0 0,-1 20 0 0 0,11-86-64 0 0,2-3-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="23">21047 2810 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,5-7 616 0 0,22-27 2026 0 0,-6 17-2035 0 0,-19 16-1214 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-2 0 0 0 0,3 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-3 0 0 0 0,2 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1-84 0 0,3 5 138 0 0,1 0-1 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,-2 1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-2-1 0 0 0,0 7-137 0 0,3-12 22 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,3 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0-21 0 0,-35 9 162 0 0,34-10-192 0 0,2 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,3-1-1 0 0,-5-1 30 0 0,-15-31-3512 0 0,18 21 1769 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="24">21520 2555 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="25">21500 2531 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="26">21485 2636 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="27">21452 2445 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,5 11 2392 0 0,12 79 1583 0 0,-17 33-1639 0 0,11 45-192 0 0,12-22-2656 0 0,-25-128 0 0 0,-3-3-337 0 0,4-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="28">21489 2863 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-1-17 3737 0 0,3-4 4077 0 0,9-21-4186 0 0,8 1-1366 0 0,-1 20-2142 0 0,-10 18-211 0 0,-8 8 222 0 0,21-9 1281 0 0,7 11-1444 0 0,-24 1-105 0 0,45 32-8 0 0,-23-4 744 0 0,-11-3-56 0 0,7 33-96 0 0,-15-19-16 0 0,5 12 191 0 0,-1-19-526 0 0,-1-4-59 0 0,-2-15-12 0 0,-5-14-90 0 0,14 3 16 0 0,21-2-96 0 0,-9-4-141 0 0,-29 2-596 0 0,30-10-4249 0 0,-16 3 1073 0 0,-9 3 1923 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="29">22096 2662 1376 0 0,'-16'6'65'0'0,"13"-5"277"0"0,3-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-6 12 5285 0 0,12 43-3424 0 0,-10-8-2068 0 0,0 46 541 0 0,-6-51-877 0 0,6 1-432 0 0,5 23-1088 0 0,10 8 915 0 0,-7-3-416 0 0,-2-59-545 0 0,-2 19 164 0 0,-6-12-45 0 0,6-18-557 0 0,0-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-6 0-797 0 0,4 0-5332 0 0,2 0 728 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="30">22051 2712 456 0 0,'33'-10'12581'0'0,"-22"4"-11549"0"0,19 5 3076 0 0,-5-5-1928 0 0,31 39 262 0 0,-18 1-1426 0 0,-12 17-48 0 0,-9-17-336 0 0,-16-30-440 0 0,-5 27-53 0 0,-7-10-60 0 0,-6-7 791 0 0,15-12-867 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,1 1-1 0 0,-3-1 1 0 0,2 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,2 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,2 0-1 0 0,-1 0 1 0 0,-1-1-1 0 0,0 1-3 0 0,-38-21-1713 0 0,14-2-2008 0 0,23 16 1827 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="31">19156 2629 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,3 14 1120 0 0,0 36 395 0 0,1 68 75 0 0,4-39-2940 0 0,4 8-252 0 0,-4-14-192 0 0,0-36-12 0 0,-8-35-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="32">19171 2789 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,5-14 2209 0 0,10-3-1077 0 0,33-22 345 0 0,-19 32-1146 0 0,-5 21-314 0 0,-20-11-177 0 0,1 1 0 0 0,0 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-3 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0-37 0 0,-1-4 176 0 0,9 11 413 0 0,-9-12-998 0 0,11 6-4069 0 0,-12-7 3075 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="33">19499 3089 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,6-4 224 0 0,-4 3 3136 0 0,10-10-3493 0 0,-10 8-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="37">19902 2736 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 13 8138 0 0,-4 34-5693 0 0,4-49-1919 0 0,-4 17 1214 0 0,1 77 988 0 0,3-94-2320 0 0,0-2-72 0 0,0 7 75 0 0,-4 26-43 0 0,-3 44-122 0 0,7-74-45 0 0,0 1-235 0 0,0-1-3512 0 0,0-3-1706 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="38">19887 2877 5296 0 0,'4'7'472'0'0,"-4"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-22 1372 0 0,0 20-1542 0 0,0 0-40 0 0,6-28 954 0 0,-5 29-1144 0 0,13-28 1755 0 0,4 11-1413 0 0,-16 17-538 0 0,-2 1 0 0 0,0 0-6 0 0,15-2 374 0 0,-8 3-368 0 0,-6-1-159 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-2 1 0 0 0,3-1 0 0 0,-1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 0 0 0 0,2 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,0 1-24 0 0,15 60 908 0 0,-11-27-544 0 0,-6-12-78 0 0,2-22-204 0 0,0 21 170 0 0,2-19-204 0 0,1 5-36 0 0,1 0-1 0 0,-1 0 42 0 0,5-4 13 0 0,-5-3-58 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-3 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 0-1 0 0,-2 0 1 0 0,2 0 0 0 0,-2 0 0 0 0,2-1 0 0 0,-2 1 0 0 0,2-1-1 0 0,-2 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-2 0 1 0 0,4-3-9 0 0,33-22-3222 0 0,-33 21-430 0 0,-4 5 1775 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">5875 3788 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-10 0 710 0 0,-62 11 2232 0 0,-97-8 113 0 0,73-18-2111 0 0,90 13-1711 0 0,3 0 0 0 0,0 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-2 1 0 0 0,0 0-1 0 0,1 0-7 0 0,-1 0 3 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-3-1-3 0 0,-4-1 53 0 0,-52 15 746 0 0,-4-32-422 0 0,-44 19 95 0 0,19 18-267 0 0,0-27 255 0 0,17 6-262 0 0,-8-6 515 0 0,25 26-785 0 0,-8-12 316 0 0,66-3-237 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,-1 1 0 0 0,2 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,1 5-384 0 0,-1 0-2483 0 0,0-5 1589 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">4726 3523 12384 0 0,'-14'-11'1277'0'0,"1"9"-438"0"0,-15 9 3998 0 0,7 3-3431 0 0,-19 15 690 0 0,-47 37-1014 0 0,24-29 402 0 0,7 21-1322 0 0,30-26-154 0 0,-9 15 872 0 0,33-40-855 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,-2-1-1 0 0,2 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,2 0-1 0 0,-1 1 1 0 0,0-2 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,3-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 2 0 0 0,-2-3-1 0 0,4 3-23 0 0,33 39 389 0 0,-25-35-394 0 0,-2-1 1 0 0,2 1-1 0 0,0-2 0 0 0,1-1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-2 0 0 0,1 0 0 0 0,0-1 1 0 0,0 0-1 0 0,5-1 4 0 0,-4 0-173 0 0,96 18-1371 0 0,-41 3-4118 0 0,-52-16-1845 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="2">3943 2866 2760 0 0,'9'14'125'0'0,"-23"-6"1798"0"0,-5 8-59 0 0,15-9 428 0 0,-22 7 4862 0 0,26-14-6578 0 0,0 0-15 0 0,0 0-34 0 0,-3 2 119 0 0,2-1-159 0 0,1-1 2989 0 0,52-17-1901 0 0,10 10-396 0 0,20 3-749 0 0,-22 1 156 0 0,39-1 469 0 0,20-5-497 0 0,-4-2-454 0 0,52-3 952 0 0,-50 8-543 0 0,-47-5-402 0 0,50-8 402 0 0,-64 8-745 0 0,3 11 112 0 0,-32-7 120 0 0,15 5 0 0 0,7-13 444 0 0,-23 4-280 0 0,11-1-164 0 0,-22 4 0 0 0,-5 7 0 0 0,16 7-1208 0 0,-25-5 877 0 0,6 3-1583 0 0,8 13-3659 0 0,-7-11 3847 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="3">5349 2404 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,8 23 9129 0 0,22-6-7935 0 0,-15-12-2328 0 0,56 30 1337 0 0,-57-23-2420 0 0,-5-7 346 0 0,1 1 1 0 0,-1 0-1 0 0,-2 1 1 0 0,3 1-1 0 0,-3 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 2-1 0 0,4 7-255 0 0,7 68 1080 0 0,-25-4-224 0 0,-11-30-856 0 0,-27-1 327 0 0,-26-11 1242 0 0,9-15-2553 0 0,35-24-3117 0 0,22-1 2058 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="4">11472 2928 8288 0 0,'10'-48'864'0'0,"-12"45"-720"0"0,4-9 1811 0 0,0 9 5703 0 0,58-2-3242 0 0,-23 5-4222 0 0,75 2 1838 0 0,4 8-1085 0 0,257-13 1101 0 0,-162-1-1030 0 0,-72 8-540 0 0,39-1-45 0 0,12-13 803 0 0,-45-22-1236 0 0,-140 30-64 0 0,-5 2-273 0 0,21-10-2694 0 0,-18 10 2502 0 0,5 0-15 0 0,-2 4-3511 0 0,-2 2-4432 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="5">13133 2487 8288 0 0,'0'0'638'0'0,"-1"1"-414"0"0,0 2-28 0 0,1-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,6 6 488 0 0,64 16 2067 0 0,-38-15-2223 0 0,48 23 954 0 0,-51-10-1577 0 0,39 40 370 0 0,-15 1-375 0 0,27 32 240 0 0,-77-90-712 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 2 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 1 1 0 0,1-1-1 0 0,-3 1-23 0 0,-2 4 44 0 0,0 0 1 0 0,-1-1-1 0 0,0 2 0 0 0,-1-2 0 0 0,1-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,0-2 0 0 0,-2 1 0 0 0,1-1 1 0 0,-1-1-1 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,0-2-1 0 0,-1-1 0 0 0,1 0-44 0 0,-26 11 59 0 0,1-2-1 0 0,0-2 1 0 0,-2-1 0 0 0,0-3-1 0 0,1-1 1 0 0,-17 0-59 0 0,28-5-59 0 0,-71-10-1395 0 0,85 4-1171 0 0,9 5 1267 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="6">14176 2607 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-11 7 790 0 0,-12 11 150 0 0,-48 20 1099 0 0,7-3-1196 0 0,61-33-1165 0 0,-11 9 158 0 0,-1 0 0 0 0,1 2-1 0 0,0-1 1 0 0,1 2 0 0 0,1 0 0 0 0,0 1 0 0 0,1 1 0 0 0,0-1-1 0 0,-6 13-202 0 0,14-23 65 0 0,0 0-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-2 1 1 0 0,2 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 1-64 0 0,1 2 108 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,2 1 0 0 0,0-2-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 0 1 0 0,-1-1 0 0 0,2 0-1 0 0,-2-1 1 0 0,2 2 0 0 0,-1-2-1 0 0,1 0 1 0 0,-1-1 0 0 0,2 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,8 2-107 0 0,-4-1 42 0 0,-1-2-1 0 0,0-1 0 0 0,2 0 0 0 0,-3-1 1 0 0,2 0-1 0 0,0-1 0 0 0,0 0 0 0 0,7-2-41 0 0,23-19-4007 0 0,-35 15-3607 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="7">14351 2952 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-4-9 655 0 0,4 3-930 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-2 0 0 0,-3 2 1 0 0,3 0-1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0 0 0 0 0,0-2 0 0 0,1 2 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,4-1-345 0 0,-7 2 74 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-2 0-1 0 0,1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1-1 0 0 0,-1 2-1 0 0,0-1 1 0 0,0 1 0 0 0,2 0-1 0 0,-2-1 1 0 0,0 1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 2 0 0 0,-1-1-1 0 0,2 0 1 0 0,-3 0 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 2-73 0 0,1 5 95 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-2 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 8-95 0 0,-12 71 1049 0 0,12-82-938 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 2 0 0 0,-1-2 1 0 0,-1 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-3 0 1 0 0,0-1-111 0 0,4-3 23 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,2-1 0 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,2 0-1 0 0,-3-1 0 0 0,3 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2-1 0 0 0,-2 1 1 0 0,1-1-24 0 0,-3-1-63 0 0,1-1 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 1 0 0,2-2-1 0 0,-1 2 1 0 0,-1-1-1 0 0,2 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-2 1 1 0 0,2-1-1 0 0,0 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-5 63 0 0,5-23-2404 0 0,-2 17 1056 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8">14825 2622 0 0 0,'-2'-7'-1709'0'0,"0"-4"9298"0"0,3 9 1867 0 0,-1 14-7849 0 0,3 102 2619 0 0,-5-24-3124 0 0,4 9 60 0 0,-5 40-1060 0 0,11-68-102 0 0,-5-65-68 0 0,-2-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="9">14805 2842 2304 0 0,'0'0'464'0'0,"5"-8"3648"0"0,-5 5 1786 0 0,27-41-750 0 0,11 3-2447 0 0,4 13-1313 0 0,-22 32-788 0 0,-18-4-482 0 0,-1 1-42 0 0,3 2-30 0 0,2 1 0 0 0,-2-1 1 0 0,1 2-1 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 2 1 0 0,-1-2-1 0 0,1 1 0 0 0,-2 0 1 0 0,3 0-1 0 0,-2 1-46 0 0,22 89 1079 0 0,-13-66-711 0 0,-9-15-53 0 0,17 65 642 0 0,2-37-721 0 0,9-29-183 0 0,38-42-1154 0 0,-27-2-4448 0 0,-31 23 3543 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="10">15518 2440 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,8 2 583 0 0,-5-7-849 0 0,-3 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,0 5 2437 0 0,0 16-2962 0 0,0 60 539 0 0,-6 70 472 0 0,-5 15 1084 0 0,7 78-784 0 0,11-192-592 0 0,1-27-84 0 0,11-17 3 0 0,-13-9-156 0 0,1 0 0 0 0,-2-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,2-4-35 0 0,46-40 80 0 0,-40 36-172 0 0,-8 8-92 0 0,1-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,1-2 0 0 0,1-2 184 0 0,0 0-1288 0 0,3-9-6336 0 0,-7 11 565 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="11">15523 2664 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,57-5 2910 0 0,-40 3-3513 0 0,5 1-489 0 0,-8 5-4783 0 0,-5 0-1037 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="12">15998 2687 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,4 5 4769 0 0,-1 1-4077 0 0,1-2-1648 0 0,-3 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 3-394 0 0,-6 184 4855 0 0,1-67-3199 0 0,1-95-1224 0 0,5-9-3265 0 0,-1-14 1400 0 0,0-7-5540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="13">16033 2925 456 0 0,'2'-12'295'0'0,"-1"10"1230"0"0,6-14 4652 0 0,-7 15-4821 0 0,9-16 3233 0 0,-4 7-3731 0 0,19-35 2412 0 0,-22 43-3133 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,0 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-137 0 0,38 1 1322 0 0,-39 1-1262 0 0,3 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-2 1-1 0 0,3-1 1 0 0,-2 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,2 1-59 0 0,20 19 91 0 0,-7 2-240 0 0,-16-25-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="14">16487 2989 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,2 2-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,3-3-329 0 0,11-27 1366 0 0,19-4-185 0 0,-32 37-1119 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 0 1 0 0,2-1-1 0 0,-2 1 1 0 0,1 0-1 0 0,1 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-2-1 0 0 0,3 2-62 0 0,43 65 531 0 0,-42-54-291 0 0,1 0-1 0 0,-3 0 1 0 0,2 1 0 0 0,-3 0-1 0 0,2-1 1 0 0,-2 1 0 0 0,0 0-1 0 0,-2 9-239 0 0,-6 42 0 0 0,-13-25 1095 0 0,2-44-406 0 0,12 1-606 0 0,1 1-72 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,2-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,2 0 0 0 0,-3-1-1 0 0,2 0 1 0 0,1 0 0 0 0,-4-2-11 0 0,3 0-209 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-2 0 0 0,0 2-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-7 209 0 0,0-19-4042 0 0,2 16-3529 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="15">16960 2360 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,3 8 590 0 0,10 67 2596 0 0,-18 149-2669 0 0,-3-76 14 0 0,8 85-1117 0 0,3-181 0 0 0,0-47-165 0 0,-1-4-698 0 0,-2-1-315 0 0,0-1-1352 0 0,3-5-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="16">17237 2901 3568 0 0,'20'-10'1553'0'0,"-5"-7"1718"0"0,-3 12-2487 0 0,39-33 3450 0 0,-24 10-3218 0 0,32-44-474 0 0,-49 49-542 0 0,-7 15 0 0 0,-6-2 0 0 0,2 7-7 0 0,-1 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,1 1 0 0 0,-3-1 1 0 0,3 1-1 0 0,-2 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1 0 0 0 0,0 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-3 0 6 0 0,-1 2 11 0 0,0-1 1 0 0,-1 2-1 0 0,2-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,-2 5-12 0 0,-15 25 272 0 0,-6 56 161 0 0,26-85-291 0 0,1-1-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-1 1-1 0 0,-1-2 1 0 0,1 1 0 0 0,2-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,2 0 0 0 0,-3 0-1 0 0,1-1 1 0 0,2 0 0 0 0,-2 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,3-1-142 0 0,-1-1 13 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,2-1 0 0 0,-2 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,5 0-13 0 0,60-24-2033 0 0,-56 15 586 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="17">17673 2614 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-2 1-172 0 0,-12 54 5027 0 0,5-27-3083 0 0,-5 31 478 0 0,11-49-2198 0 0,2 2 0 0 0,-1 0 0 0 0,2-1 0 0 0,-2 1-1 0 0,2-1 1 0 0,0 0 0 0 0,2 2 0 0 0,-1 4-320 0 0,1 26 797 0 0,-2-36-713 0 0,0-1-1 0 0,2 2 1 0 0,-2-2-1 0 0,2 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-1-1 0 0,2 0 1 0 0,-1-1-1 0 0,-1 1 1 0 0,2-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-2 0-1 0 0,6 3-83 0 0,-7-7 16 0 0,0 0-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-2 1 1 0 0,2-1-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,2 0-1 0 0,-2-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,2 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 0 1 0 0,-1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,1-2-15 0 0,6-4 20 0 0,17-33 87 0 0,12-40-97 0 0,-34 73-49 0 0,1 1 0 0 0,-1 0-1 0 0,0-1 1 0 0,0 0 0 0 0,-2 0-1 0 0,1 1 1 0 0,0-1 0 0 0,-2-1-1 0 0,1 1 1 0 0,-1-6 39 0 0,-4-22-1383 0 0,4 36 837 0 0,-1 0-1200 0 0,-5-5-4721 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="18">16405 2440 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,1-1-292 0 0,6-4-365 0 0,0-3-1 0 0,-1 2 1 0 0,0-1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-2 0 0 0,-1 1-1 0 0,1 0 1 0 0,-2-1-363 0 0,48-77 852 0 0,-37 68-781 0 0,-1 16-61 0 0,-10 6 2 0 0,-1 0 0 0 0,1 1-1 0 0,-2-1 1 0 0,2 2 0 0 0,-2-1-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-2 0-1 0 0,1 2 1 0 0,-1-2-1 0 0,0 2-11 0 0,1 2-4 0 0,7 26 57 0 0,2-4-53 0 0,5 0-1856 0 0,-10-24-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="19">7751 2673 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-11-2-24 0 0,7 2 8851 0 0,2 5-9133 0 0,-9 16-17 0 0,6-18-769 0 0,4-2-3236 0 0,1-1-1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="20">19579 2986 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-7 0-423 0 0,1-2-329 0 0,5 2-272 0 0,-1-3-398 0 0,-1-1-3749 0 0,-2-8 2451 0 0,4 9-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="21">19317 2708 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-13-3 2088 0 0,-6-4-821 0 0,19 7-1285 0 0,-14 3 543 0 0,-32 27 578 0 0,-3 51-1009 0 0,48-73-646 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,3 0 0 0 0,-3 0 0 0 0,3 0 0 0 0,-2-1 0 0 0,3 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-2 0 0 0,1 2-74 0 0,24 25 398 0 0,-26-31-397 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,0 1 0 0 0,1-1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,1-1-1 0 0,9 1-134 0 0,-11-1-167 0 0,2 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 1 0 0,-2 0-1 0 0,1 1 1 0 0,1-2-1 0 0,-1 0 1 0 0,-1 1 301 0 0,-3 2-105 0 0,14-9-1239 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="22">19778 2749 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,6 8 1656 0 0,-6-5-2461 0 0,2 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 2 0 0 0,-1-2 1 0 0,0 0-1 0 0,0 2-229 0 0,1 74 2716 0 0,16 162 1049 0 0,-25-73-3749 0 0,-3-95-16 0 0,0 20 0 0 0,11-88-64 0 0,1-3-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="23">19805 2825 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,5-7 616 0 0,20-28 2026 0 0,-6 17-2035 0 0,-17 17-1214 0 0,0-1 0 0 0,1 1 0 0 0,-3 0 0 0 0,3 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-3 0 0 0 0,1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1-84 0 0,3 5 138 0 0,0 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,-3 1 1 0 0,2 0-1 0 0,0 2 0 0 0,-1-2 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 1 0 0 0,-1-2 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-2 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-3 0 0 0 0,0 6-137 0 0,3-12 22 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-2 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0-21 0 0,-32 9 162 0 0,32-10-192 0 0,1 0 1 0 0,-1-1 0 0 0,1 1 0 0 0,1-1 0 0 0,-2 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,3-1-1 0 0,-5-1 30 0 0,-13-32-3512 0 0,16 21 1769 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="24">20244 2563 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="25">20225 2538 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="26">20211 2646 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="27">20181 2450 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,4 11 2392 0 0,12 82 1583 0 0,-16 33-1639 0 0,10 47-192 0 0,12-23-2656 0 0,-24-132 0 0 0,-3-3-337 0 0,4-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="28">20215 2879 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-1-18 3737 0 0,3-3 4077 0 0,8-23-4186 0 0,8 2-1366 0 0,-2 20-2142 0 0,-8 19-211 0 0,-8 8 222 0 0,19-9 1281 0 0,7 11-1444 0 0,-22 1-105 0 0,41 33-8 0 0,-20-4 744 0 0,-12-4-56 0 0,8 35-96 0 0,-15-20-16 0 0,5 13 191 0 0,0-21-526 0 0,-2-3-59 0 0,-2-15-12 0 0,-4-15-90 0 0,13 3 16 0 0,19-2-96 0 0,-8-4-141 0 0,-27 2-596 0 0,28-11-4249 0 0,-15 4 1073 0 0,-8 3 1923 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="29">20778 2673 1376 0 0,'-15'6'65'0'0,"12"-5"277"0"0,3-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-5 12 5285 0 0,10 45-3424 0 0,-8-9-2068 0 0,-1 48 541 0 0,-5-53-877 0 0,5 1-432 0 0,5 24-1088 0 0,9 8 915 0 0,-6-3-416 0 0,-2-61-545 0 0,-2 20 164 0 0,-6-13-45 0 0,6-18-557 0 0,0-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-5 0-797 0 0,3 0-5332 0 0,2 0 728 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="30">20736 2724 456 0 0,'31'-10'12581'0'0,"-21"4"-11549"0"0,18 5 3076 0 0,-5-5-1928 0 0,29 40 262 0 0,-17 0-1426 0 0,-11 19-48 0 0,-8-18-336 0 0,-15-31-440 0 0,-5 28-53 0 0,-6-11-60 0 0,-6-6 791 0 0,15-13-867 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,1 1-1 0 0,-3-1 1 0 0,2 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 0-1 0 0,2 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,-1-1 0 0 0,2 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1-3 0 0,-35-21-1713 0 0,13-3-2008 0 0,21 17 1827 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="31">18051 2639 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,3 14 1120 0 0,-1 38 395 0 0,2 69 75 0 0,3-40-2940 0 0,5 8-252 0 0,-5-14-192 0 0,0-37-12 0 0,-7-36-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="32">18065 2803 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,4-14 2209 0 0,10-4-1077 0 0,31-22 345 0 0,-18 33-1146 0 0,-5 22-314 0 0,-18-12-177 0 0,0 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-2 1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0-37 0 0,-1-3 176 0 0,8 10 413 0 0,-8-12-998 0 0,10 6-4069 0 0,-11-7 3075 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="33">18369 3111 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,5-4 224 0 0,-3 3 3136 0 0,9-10-3493 0 0,-9 8-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="37">18743 2749 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 13 8138 0 0,-4 36-5693 0 0,4-51-1919 0 0,-4 17 1214 0 0,2 80 988 0 0,2-97-2320 0 0,0-2-72 0 0,0 7 75 0 0,-4 27-43 0 0,-3 45-122 0 0,7-76-45 0 0,0 1-235 0 0,0-1-3512 0 0,0-3-1706 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="38">18729 2894 5296 0 0,'4'7'472'0'0,"-4"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-23 1372 0 0,0 21-1542 0 0,0 0-40 0 0,5-28 954 0 0,-4 29-1144 0 0,12-29 1755 0 0,4 11-1413 0 0,-15 18-538 0 0,-2 1 0 0 0,0 0-6 0 0,14-2 374 0 0,-8 3-368 0 0,-5-1-159 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,3-1 0 0 0,-1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 0 0 0 0,2 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,0 1-24 0 0,14 62 908 0 0,-10-28-544 0 0,-6-13-78 0 0,2-22-204 0 0,0 22 170 0 0,2-20-204 0 0,1 5-36 0 0,0 0-1 0 0,0 1 42 0 0,4-5 13 0 0,-4-3-58 0 0,1 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,2 0 0 0 0,-3 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,2-2-1 0 0,-2 1 1 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0-1 0 0,-2 0 1 0 0,3-3-9 0 0,32-23-3222 0 0,-32 22-430 0 0,-3 5 1775 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2331,10 +2324,10 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">76 216 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0 0 240 0 0,0 0 43 0 0,0 0-73 0 0,0 0-345 0 0,0 0-150 0 0,0 0-28 0 0,0 0 21 0 0,0 0 115 0 0,7 3 1247 0 0,-5-2-1608 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-193 0 0,4 18 1030 0 0,-3-19-673 0 0,-5 5 279 0 0,-3 67 1076 0 0,-4 32-280 0 0,7-28-400 0 0,-11 43 496 0 0,-3 45-1568 0 0,14-85 184 0 0,7 2-144 0 0,0-21 0 0 0,-3-57 130 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 2-1 0 0,0-2-129 0 0,-10 45-329 0 0,20 5-50 0 0,-8-33-4669 0 0,-8-50-385 0 0,8 12 3507 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1970.78">91 130 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-129 0 0,0 0 200 0 0,0 0 108 0 0,0 0 24 0 0,9 0 2199 0 0,29 0-1100 0 0,-36 0-1400 0 0,-2 0 18 0 0,7-1 404 0 0,107-18 2883 0 0,-15 18-2302 0 0,-36 2-385 0 0,31-30 289 0 0,-78 25-961 0 0,1 0 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 2 1 0 0,0 0 0 0 0,-1 0-1 0 0,12 2-147 0 0,10 4-51 0 0,87 7 245 0 0,-76-12 432 0 0,30 0 101 0 0,-2 11-519 0 0,29-2-51 0 0,5-14 91 0 0,1-20 123 0 0,73-3 48 0 0,8 22-113 0 0,12-19 369 0 0,-127 16-555 0 0,-5 6-351 0 0,-21 6 134 0 0,87 14 97 0 0,-54-6 53 0 0,9-22 230 0 0,-22 11-283 0 0,36 5 0 0 0,0 25-96 0 0,-64-21 96 0 0,47 8 16 0 0,-23-9-16 0 0,15 1 64 0 0,35 16-48 0 0,21 8-16 0 0,-80-26-96 0 0,118-13 96 0 0,-23 18 53 0 0,-71-8-42 0 0,49-4-11 0 0,-9-7-19 0 0,-117 7 21 0 0,33-1 0 0 0,0 2 1 0 0,0 2-1 0 0,-1 1 0 0 0,35 9-2 0 0,-60-11-4 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-2 1 0 0,1 0 0 0 0,-1-3-1 0 0,0 2 1 0 0,3-2 4 0 0,52-3-32 0 0,15 2 19 0 0,8 4 93 0 0,-16 4-80 0 0,29-11 64 0 0,60-3-1144 0 0,-163 10 588 0 0,-1 0-421 0 0,0 0-189 0 0,0 0-1663 0 0,0 0-6530 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2876.335">5022 167 11488 0 0,'0'0'528'0'0,"0"0"-16"0"0,0 1-326 0 0,-10 30 3021 0 0,8 61 849 0 0,-27 143 1534 0 0,21-140-5590 0 0,4 56 1815 0 0,-11-5-1045 0 0,8-51 113 0 0,3-44-550 0 0,-3-4-190 0 0,10-29-15 0 0,-3-2-205 0 0,1-13 119 0 0,-5 37-31 0 0,3-30-11 0 0,-2-1 11 0 0,3-7-103 0 0,0-2-600 0 0,0 0-268 0 0,0 0-1097 0 0,0 0-4403 0 0,0 0-1889 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4565.136">0 1294 5528 0 0,'0'0'422'0'0,"0"0"-34"0"0,0 0 887 0 0,0 0 416 0 0,0 0 79 0 0,0 17 2778 0 0,3 7-429 0 0,13-18-2249 0 0,48-19-14 0 0,31 6 228 0 0,-39 11-2068 0 0,13 12 56 0 0,24 13 1888 0 0,-21-1-1944 0 0,39-6-16 0 0,-40-14 0 0 0,57 11 0 0 0,-43-4 0 0 0,179 7 952 0 0,-249-23-877 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,0-1-1 0 0,0-1 0 0 0,7-4-75 0 0,66-14 289 0 0,19 9-114 0 0,0 5-1 0 0,48 5-174 0 0,-109 1 103 0 0,57 7-95 0 0,-20 24-140 0 0,230-11 1020 0 0,-60-14-517 0 0,-124-2-155 0 0,166 4 61 0 0,-79-14 534 0 0,28 1-910 0 0,-109 1 187 0 0,51 0 104 0 0,-100 5-192 0 0,0 3 0 0 0,24 7 0 0 0,42-22 256 0 0,-12 4-200 0 0,-12 9-123 0 0,-60-8-10 0 0,5 3 88 0 0,9 12 122 0 0,-36-11-133 0 0,-12 10 0 0 0,-12-13 0 0 0,16-6 0 0 0,4-3 0 0 0,-7 4-113 0 0,-27 10 27 0 0,-5 1 12 0 0,-2 2-5 0 0,26-7-753 0 0,-20 7 648 0 0,11-1 96 0 0,-9 3 88 0 0,3 8-17 0 0,-11-8-67 0 0,-1-2-6 0 0,0 0 9 0 0,0 0-139 0 0,0 0-588 0 0,0 0-257 0 0,0 0-1738 0 0,0 0-6757 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">76 217 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0 0 240 0 0,0 0 43 0 0,0 0-73 0 0,0 0-345 0 0,0 0-150 0 0,0 0-28 0 0,0 0 21 0 0,0 0 115 0 0,7 3 1247 0 0,-5-2-1608 0 0,-1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-193 0 0,4 19 1030 0 0,-3-20-673 0 0,-5 5 279 0 0,-3 67 1076 0 0,-4 33-280 0 0,7-29-400 0 0,-11 44 496 0 0,-3 45-1568 0 0,14-86 184 0 0,7 2-144 0 0,0-20 0 0 0,-3-58 130 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 2-1 0 0,0-2-129 0 0,-10 45-329 0 0,20 6-50 0 0,-8-34-4669 0 0,-8-50-385 0 0,8 12 3507 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1970.78">91 131 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-129 0 0,0 0 200 0 0,0 0 108 0 0,0 0 24 0 0,9 0 2199 0 0,29 0-1100 0 0,-36 0-1400 0 0,-2 0 18 0 0,7-1 404 0 0,106-18 2883 0 0,-14 18-2302 0 0,-36 2-385 0 0,30-31 289 0 0,-77 26-961 0 0,1 0 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 2 1 0 0,0 0 0 0 0,-1 0-1 0 0,12 2-147 0 0,10 4-51 0 0,86 7 245 0 0,-75-12 432 0 0,30 0 101 0 0,-2 11-519 0 0,28-1-51 0 0,6-15 91 0 0,1-21 123 0 0,72-2 48 0 0,8 22-113 0 0,13-19 369 0 0,-127 16-555 0 0,-6 6-351 0 0,-20 6 134 0 0,87 14 97 0 0,-55-6 53 0 0,10-22 230 0 0,-22 11-283 0 0,36 5 0 0 0,-1 25-96 0 0,-63-21 96 0 0,47 8 16 0 0,-23-9-16 0 0,14 2 64 0 0,36 15-48 0 0,21 8-16 0 0,-81-26-96 0 0,119-13 96 0 0,-24 18 53 0 0,-70-8-42 0 0,49-4-11 0 0,-10-7-19 0 0,-116 7 21 0 0,33-1 0 0 0,0 2 1 0 0,0 2-1 0 0,-1 1 0 0 0,34 9-2 0 0,-59-11-4 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-2 1 0 0,1 0 0 0 0,-1-3-1 0 0,0 2 1 0 0,3-2 4 0 0,52-3-32 0 0,15 2 19 0 0,7 4 93 0 0,-15 4-80 0 0,29-11 64 0 0,59-3-1144 0 0,-162 10 588 0 0,-1 0-421 0 0,0 0-189 0 0,0 0-1663 0 0,0 0-6530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2876.335">5006 168 11488 0 0,'0'0'528'0'0,"0"0"-16"0"0,0 1-326 0 0,-10 30 3021 0 0,8 62 849 0 0,-27 143 1534 0 0,21-141-5590 0 0,4 57 1815 0 0,-11-5-1045 0 0,8-52 113 0 0,3-43-550 0 0,-3-5-190 0 0,10-29-15 0 0,-3-2-205 0 0,1-13 119 0 0,-5 37-31 0 0,3-30-11 0 0,-2 0 11 0 0,3-8-103 0 0,0-2-600 0 0,0 0-268 0 0,0 0-1097 0 0,0 0-4403 0 0,0 0-1889 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4565.136">0 1301 5528 0 0,'0'0'422'0'0,"0"0"-34"0"0,0 0 887 0 0,0 0 416 0 0,0 0 79 0 0,0 17 2778 0 0,3 7-429 0 0,13-18-2249 0 0,48-19-14 0 0,30 6 228 0 0,-38 11-2068 0 0,13 12 56 0 0,24 13 1888 0 0,-21 0-1944 0 0,38-7-16 0 0,-39-14 0 0 0,57 11 0 0 0,-44-4 0 0 0,179 7 952 0 0,-248-23-877 0 0,0 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0-1 1 0 0,0-1-1 0 0,0-1 0 0 0,7-4-75 0 0,66-14 289 0 0,18 9-114 0 0,1 5-1 0 0,48 5-174 0 0,-110 1 103 0 0,58 7-95 0 0,-20 24-140 0 0,229-11 1020 0 0,-60-14-517 0 0,-123-2-155 0 0,165 4 61 0 0,-79-14 534 0 0,28 1-910 0 0,-108 1 187 0 0,50 0 104 0 0,-99 5-192 0 0,0 3 0 0 0,23 7 0 0 0,43-22 256 0 0,-13 4-200 0 0,-11 9-123 0 0,-60-8-10 0 0,4 3 88 0 0,10 12 122 0 0,-36-11-133 0 0,-12 10 0 0 0,-12-13 0 0 0,16-7 0 0 0,4-2 0 0 0,-7 4-113 0 0,-27 10 27 0 0,-6 1 12 0 0,-1 2-5 0 0,26-7-753 0 0,-20 7 648 0 0,11-1 96 0 0,-9 3 88 0 0,3 8-17 0 0,-11-8-67 0 0,-1-2-6 0 0,0 0 9 0 0,0 0-139 0 0,0 0-588 0 0,0 0-257 0 0,0 0-1738 0 0,0 0-6757 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2370,86 +2363,86 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">246 638 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="310.099">638 654 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-8 10039 0 0,4 3-11103 0 0,-2 0-133 0 0,2 0-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="684.255">1033 598 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1921.293">1380 678 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,4-21-839 0 0,-7 30-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 76 971 0 0,12-75-904 0 0,2-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,5-15-522 0 0,2-29 325 0 0,-7 43 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 35 365 0 0,9-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-41 40 0 0,-1 46 757 0 0,-8 6-562 0 0,-2 1-34 0 0,13 14 96 0 0,-22 50 294 0 0,9-62 48 0 0,0-2-24 0 0,-12 9 14 0 0,11-9-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-2-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-2 1-12 0 0,0-1-1 0 0,1 0 1 0 0,0-1-1 0 0,-2 1 0 0 0,3 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-3 1 0 0,16-18-798 0 0,-5 22 705 0 0,11 17 39 0 0,-21-14 64 0 0,1 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 3-10 0 0,1-5 84 0 0,-4 17 237 0 0,-21-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 12-3207 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8390.611">1673 404 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 55 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,1 16 113 0 0,-2-14-1404 0 0,-1 50 981 0 0,-4-3-1688 0 0,1-56-1417 0 0,-2-31 962 0 0,-7-27-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8997.239">1609 535 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-32 2722 0 0,-14 31-3180 0 0,15-13 1008 0 0,23-26 674 0 0,-35 37-2057 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 2 1 0 0,-1-2 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 18 1009 0 0,-52 14 55 0 0,-5-17-600 0 0,22 45 1448 0 0,-23 2-2113 0 0,-15-59 230 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 21 399 0 0,1-10-337 0 0,8-8-104 0 0,-3-1 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,3 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 37 0 0,-34-1 653 0 0,-9-24-4978 0 0,35 18 2334 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11709.08">2997 370 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 46 1154 0 0,-12 23 2052 0 0,-3 33 1755 0 0,3 50-2463 0 0,4-53-962 0 0,-3 31-1172 0 0,7-135-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-2 13-2556 0 0,0-23 1622 0 0,2-1-894 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12315.019">3015 426 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-3 772 0 0,-14 9-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-3 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,-1 2 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,3 5-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 2-174 0 0,-2 33 278 0 0,-1-40-199 0 0,1-2 0 0 0,-1 2 1 0 0,0-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,-1-1 1 0 0,3 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-3-1-4 0 0,-55-43-4198 0 0,56 41-3651 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10346.212">2223 76 3680 0 0,'-6'46'613'0'0,"2"-9"6816"0"0,-8 23-4591 0 0,9 15-23 0 0,3-12-297 0 0,4 3-1604 0 0,-8 92 2 0 0,7-75 200 0 0,0-17-716 0 0,4-40-126 0 0,-7-20-115 0 0,-4 1-1048 0 0,1 4-4224 0 0,3-11 3723 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10997.838">2148 629 1376 0 0,'4'-20'2159'0'0,"5"1"4223"0"0,4-7-3735 0 0,-2 7-1523 0 0,12-17 1153 0 0,4 13 523 0 0,-4 1-1591 0 0,22-16 135 0 0,-44 37-1294 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 1-1 0 0,3-1 0 0 0,-1 1 1 0 0,-1-1-1 0 0,2 1 0 0 0,-2-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 1 0 0,0 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-3 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-2 1 0 0,0 1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 7-27 0 0,9 28 368 0 0,31 117 1443 0 0,-21-120-1634 0 0,1-14-84 0 0,-14-23-77 0 0,-5-1-29 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,2 0 0 0 0,1 1 0 0 0,-3-1 0 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,3 0 0 0 0,-1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1-1 13 0 0,38-27-350 0 0,20-12-3834 0 0,-54 35 2533 0 0,3 3-12 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32289.342">1 248 6448 0 0,'7'20'6309'0'0,"-7"-17"-6682"0"0,5 53 3514 0 0,6 81-847 0 0,0-42-690 0 0,-7-10-929 0 0,13 128 737 0 0,-27 31 57 0 0,5-171-1337 0 0,-1-45-256 0 0,6-13-955 0 0,0-12-4480 0 0,0-3-582 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35199.426">13 278 6248 0 0,'0'12'190'0'0,"0"-22"349"0"0,17-37 6274 0 0,-17 45-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,11-3 291 0 0,73-18 828 0 0,-39 5-729 0 0,13-3 96 0 0,49 10 370 0 0,-60 8-222 0 0,42 2-1079 0 0,-20-6 16 0 0,36-20 451 0 0,-30 16 1144 0 0,61 0-1448 0 0,4 19 224 0 0,-53-19-645 0 0,-30 0 1538 0 0,6-1-1123 0 0,-36 8-292 0 0,51 0 264 0 0,-24-6 20 0 0,53-25 70 0 0,11 18-205 0 0,13 8 34 0 0,-66-3 219 0 0,22-6-424 0 0,-5 12 192 0 0,-9 5 584 0 0,43 1-1352 0 0,-7 9 736 0 0,2 5 1017 0 0,-34-9-298 0 0,-11-1-1239 0 0,26-3 520 0 0,15 3 64 0 0,12 28 75 0 0,-61-10-166 0 0,16-1 523 0 0,-5-7-840 0 0,-21-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,73-10-197 0 0,-21 19 0 0 0,-41-14-20 0 0,-45-2 0 0 0,-11-5 0 0 0,24 16 0 0 0,-38-2 0 0 0,5 5 0 0 0,13 23 64 0 0,-5 27 0 0 0,-9 22-64 0 0,-2 30-8 0 0,-3-48 125 0 0,-1 31-203 0 0,-10 32 295 0 0,10 43-190 0 0,-18-81 82 0 0,0-40-13 0 0,4-42 96 0 0,7-13-234 0 0,0 1-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1-1 0 0 0,-1 1-1 0 0,-1 1 51 0 0,0-2 114 0 0,2 0 0 0 0,-3 0 0 0 0,1 0 1 0 0,1-1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1-1 0 0 0,1 0-114 0 0,-15 0 158 0 0,-97 8-218 0 0,81-3 59 0 0,-1-1-1 0 0,2-2 1 0 0,-1-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-22-6 1 0 0,4-3-9 0 0,-2 3 0 0 0,2 2 0 0 0,-1 2 0 0 0,-22 2 9 0 0,-111 0 332 0 0,138 4-330 0 0,1-1-1 0 0,-2-3 1 0 0,1-2-1 0 0,0-1 1 0 0,-8-6-2 0 0,23 8-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-20 4 18 0 0,-143 29 64 0 0,-4-12-136 0 0,-46-9 152 0 0,171-12-80 0 0,-91 0 11 0 0,-34-16 42 0 0,101 16-53 0 0,-23-12 80 0 0,22-12-176 0 0,-85-17 224 0 0,57 22-196 0 0,62 6 192 0 0,-62-4-124 0 0,51 11 0 0 0,45 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="78758.085">3766 836 13560 0 0,'0'0'306'0'0,"-12"-2"752"0"0,-24-5-12 0 0,35 7-11 0 0,-8-6 1119 0 0,9 5 2052 0 0,65 4-3188 0 0,30-6 262 0 0,160 30 512 0 0,-136-20-1336 0 0,154 25-663 0 0,-48 8 353 0 0,-6-7 891 0 0,-124-30-445 0 0,-76-3-541 0 0,-1-1 0 0 0,1 0 0 0 0,-1-2 1 0 0,1 0-1 0 0,-1-1 0 0 0,10-4-51 0 0,72-34-278 0 0,-97 41 89 0 0,-3 1-156 0 0,3 0-611 0 0,0 1-1432 0 0,-2-2-4991 0 0,-1 1-504 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="79175.854">5363 556 6448 0 0,'0'0'498'0'0,"1"-1"-28"0"0,30-3 10100 0 0,24 22-6654 0 0,-34-9-3356 0 0,3 1 0 0 0,-2 1 1 0 0,0 1-1 0 0,-2 1 0 0 0,1 0 0 0 0,5 6-560 0 0,59 53 264 0 0,-77-62-125 0 0,-1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,-2 0 1 0 0,0-1-1 0 0,1 1 1 0 0,2 12-139 0 0,-5-12 187 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-3 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0-1-1 0 0,-3 0 1 0 0,2 0-1 0 0,-2 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,-1-1-1 0 0,0 0 1 0 0,-4 7-188 0 0,-25 28 165 0 0,-33-7 587 0 0,-89-22 352 0 0,124-18-1542 0 0,-23 5-2761 0 0,47 0 2491 0 0,-28 11-2399 0 0,17-3-3298 0 0,4 1-1217 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37346.914">6693 824 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,21-14-8855 0 0,-15 9 1888 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37618.204">7066 866 10592 0 0,'-13'-11'818'0'0,"10"7"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37903.659">7413 780 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,4 0-232 0 0,0 0-5476 0 0,-5 0-2114 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38875.93">7776 866 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-9-13 464 0 0,13-39 1231 0 0,1 44-2463 0 0,-2 2 0 0 0,3 0 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-5-189 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 4-113 0 0,1-4 41 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,2 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-14-143 0 0,-13 31-62 0 0,1 0-1 0 0,-2 0 1 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-3-1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-1-43 0 0,3 1 32 0 0,1 9 23 0 0,-11 19 200 0 0,4-27-96 0 0,-6 4-695 0 0,12-7-611 0 0,9-10-5710 0 0,-6 6 446 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="44618.988">8058 509 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 21-45 0 0,-12-24-3788 0 0,3 8 1039 0 0,3 80 1637 0 0,7 80-1221 0 0,-14-82-1606 0 0,0-78-341 0 0,-2-3-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53832.509">8358 549 2760 0 0,'4'8'1828'0'0,"4"19"4892"0"0,4 25-3444 0 0,3 99 1947 0 0,-12-78-3937 0 0,-6-35-4508 0 0,3-35 1701 0 0,-4 5-229 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54557.219">8411 866 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,8-37 5734 0 0,5-11-521 0 0,-17 19-3279 0 0,10 9-1202 0 0,9-35 1 0 0,-13 54-738 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,3 0-93 0 0,1-2 95 0 0,-5 3-21 0 0,27 0-60 0 0,1 13-14 0 0,-5 8 0 0 0,-20-12 0 0 0,10 22 0 0 0,20 71 514 0 0,-20-50 356 0 0,5-17-278 0 0,-18-34-517 0 0,4 3 98 0 0,-2-2-141 0 0,-1-1 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,3-1 0 0 0,-1 1-1 0 0,-2-1 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-28-4233 0 0,-22 31 2840 0 0,0 1-164 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56701.452">9196 603 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-38-6 1747 0 0,40 9-1667 0 0,7-2 170 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-3-1 0 0 0,1 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,3 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 40-483 0 0,18 3 618 0 0,16 11 378 0 0,10 4-513 0 0,15-4 1899 0 0,26-10-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 1 0 0 0,-22-9 0 0 0,-2 2 0 0 0,0-5-64 0 0,30-21-5497 0 0,-31 15 3530 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57367.528">9460 926 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-16 649 0 0,-9 18-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 19 784 0 0,-16 13 56 0 0,6-31-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="64361.857">9731 596 1840 0 0,'0'5'396'0'0,"0"-3"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 70 1352 0 0,-5-52-2105 0 0,-9 61 686 0 0,-2-6-314 0 0,3 65-530 0 0,6-108-273 0 0,-3-11 0 0 0,-6-11-45 0 0,4-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-2-14-1557 0 0,1-1 195 0 0,-2 0-70 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="69762.645">9697 598 1376 0 0,'4'6'367'0'0,"-4"-5"1002"0"0,0-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,2 0 1 0 0,-2 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,9-7 51 0 0,33-22 1588 0 0,-29 23-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,1 1-1 0 0,-2-1 1 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,1 2 108 0 0,2 1-1 0 0,-1 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,1-1-1 0 0,-2 0 0 0 0,0 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,2-1-1 0 0,-3 1 0 0 0,0 1 0 0 0,1-1 1 0 0,0 6-108 0 0,9 26 435 0 0,0 56 787 0 0,-11-79-980 0 0,0-12-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1-56 0 0,-43 35 929 0 0,42-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-2 0 1 0 0,3 0 0 0 0,-2 0 0 0 0,0-1-1 0 0,1 1 1 0 0,0 0 0 0 0,-2-1 0 0 0,1 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,2 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-3-1 0 0 0,3 0 0 0 0,-3 0 0 0 0,1 0 0 0 0,2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-3-4 0 0 0,5-16-5381 0 0,0 15-2125 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70961.788">10171 338 0 0 0,'-12'11'0'0'0,"7"-14"140"0"0,2 3 2586 0 0,3 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 29 3000 0 0,-14 30-1947 0 0,1 48 181 0 0,4 2 624 0 0,-6-40-881 0 0,9 37-1316 0 0,-11-26-173 0 0,8-42 0 0 0,14 3-2476 0 0,-12-39 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,2 1-1 0 0,-2-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-2 0-1 0 0,2-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="71766.961">10154 754 4376 0 0,'0'0'199'0'0,"9"-10"1918"0"0,-5-3 1016 0 0,11-9 683 0 0,-6-13-1297 0 0,-2-1-472 0 0,5 29-1272 0 0,-9 6-743 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-3-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 20 598 0 0,-25-15-674 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,2 7-227 0 0,6 89 608 0 0,-7-64-165 0 0,-1-10 997 0 0,27-2-1275 0 0,-6-26-165 0 0,7-1 0 0 0,12-10-60 0 0,-19 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73476.329">10779 632 2760 0 0,'0'1'207'0'0,"0"43"6763"0"0,0-43-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 12-344 0 0,-2 0 0 0 0,0 0 1 0 0,-2 1-1 0 0,0 0 1 0 0,-1-2-1 0 0,-2 11-1278 0 0,-12 60 616 0 0,0-17 973 0 0,14 37-2158 0 0,1-84 962 0 0,-2-25-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="74025.376">10843 625 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,57-24 1867 0 0,-54 26-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,-2 0 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,-2 0 0 0 0,3 1-156 0 0,-2 0 96 0 0,3 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-2 1-1 0 0,2 1 1 0 0,-1-2-1 0 0,0 1 1 0 0,0 1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,2 1-95 0 0,-2-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 4-94 0 0,-43 57 1952 0 0,47-65-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128695.154">5890 1434 4144 0 0,'0'0'319'0'0,"-7"7"1871"0"0,2-2 3495 0 0,-27-2-688 0 0,1-4-2621 0 0,2-15 488 0 0,-17 8-1852 0 0,-8-2 1272 0 0,-24-14-812 0 0,3 6-939 0 0,0 1 998 0 0,-5 0-1171 0 0,-9 11-360 0 0,-116 12 1824 0 0,110 7-1887 0 0,39-8 230 0 0,-34-9-256 0 0,8-6 82 0 0,13 7 87 0 0,24 3-80 0 0,-75-13 0 0 0,51-2 0 0 0,-9 6 0 0 0,50 2 0 0 0,13 5-60 0 0,11 2-440 0 0,5 5-11674 0 0,-1-4 3997 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129337.391">4416 1113 8288 0 0,'0'2'227'0'0,"-1"-1"0"0"0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,2 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,0 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-3 0 0 0 0,2-1 0 0 0,0 1-227 0 0,-20 1 2894 0 0,14 2-2512 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,2 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,2 1 0 0 0,-7 5-381 0 0,-3 3 422 0 0,-15 13 408 0 0,-37 32 222 0 0,17-4-867 0 0,47-30 92 0 0,2-22-266 0 0,0-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-2-1-1 0 0,3 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1-11 0 0,26 11 26 0 0,95 20-304 0 0,-47-10-3852 0 0,-21 7-1623 0 0,-39-15 3707 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="133691.162">6028 3653 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-10 0 710 0 0,-68 11 2232 0 0,-103-9 113 0 0,76-16-2111 0 0,101 12-1711 0 0,-1 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,2 1-1 0 0,-3-1 1 0 0,2 1 0 0 0,-1 0-1 0 0,0 0-7 0 0,0 0 3 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-2 0 1 0 0,3 0 0 0 0,-1 0 0 0 0,-4-1-3 0 0,-4-1 53 0 0,-56 15 746 0 0,-5-31-422 0 0,-46 18 95 0 0,21 17-267 0 0,-3-26 255 0 0,19 7-262 0 0,-6-6 515 0 0,25 23-785 0 0,-8-10 316 0 0,71-3-237 0 0,0-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,2 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 0 1 0 0,2 0-1 0 0,2 0 0 0 0,-2 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,0 5-384 0 0,1 0-2483 0 0,-1-5 1589 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="134078.302">4789 3399 12384 0 0,'-13'-11'1277'0'0,"-2"9"-438"0"0,-16 9 3998 0 0,10 3-3431 0 0,-23 13 690 0 0,-50 37-1014 0 0,26-28 402 0 0,6 19-1322 0 0,35-24-154 0 0,-10 15 872 0 0,34-40-855 0 0,2 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1-2 0 0 0,-2 2 0 0 0,2-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-2-1 0 0,1 3-23 0 0,37 38 389 0 0,-28-35-394 0 0,0 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0-1 0 0 0,0-1 1 0 0,1 1-1 0 0,0-2 0 0 0,0 0 0 0 0,0-1 1 0 0,0-1-1 0 0,6 0 4 0 0,-6 0-173 0 0,104 17-1371 0 0,-42 3-4118 0 0,-58-15-1845 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136187.119">3947 2767 2760 0 0,'9'14'125'0'0,"-23"-7"1798"0"0,-7 9-59 0 0,17-9 428 0 0,-27 5 4862 0 0,31-12-6578 0 0,0 0-15 0 0,0 0-34 0 0,-1 2 119 0 0,0-1-159 0 0,1-1 2989 0 0,56-15-1901 0 0,11 8-396 0 0,21 3-749 0 0,-23 1 156 0 0,41-1 469 0 0,22-4-497 0 0,-4-3-454 0 0,55-3 952 0 0,-52 8-543 0 0,-51-4-402 0 0,53-8 402 0 0,-69 7-745 0 0,3 11 112 0 0,-33-6 120 0 0,16 4 0 0 0,6-13 444 0 0,-25 4-280 0 0,14 0-164 0 0,-25 4 0 0 0,-6 6 0 0 0,19 6-1208 0 0,-28-4 877 0 0,8 3-1583 0 0,6 12-3659 0 0,-9-10 3847 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136591.973">5461 2323 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,9 22 9129 0 0,24-6-7935 0 0,-18-11-2328 0 0,61 29 1337 0 0,-60-23-2420 0 0,-7-6 346 0 0,2 0 1 0 0,-1 1-1 0 0,0 1 1 0 0,-2 0-1 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,4 7-255 0 0,7 66 1080 0 0,-27-5-224 0 0,-12-27-856 0 0,-27-2 327 0 0,-29-11 1242 0 0,8-14-2553 0 0,39-23-3117 0 0,24-1 2058 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="139663.33">12060 2826 8288 0 0,'11'-45'864'0'0,"-13"42"-720"0"0,4-9 1811 0 0,0 9 5703 0 0,63-2-3242 0 0,-25 5-4222 0 0,80 2 1838 0 0,5 8-1085 0 0,276-13 1101 0 0,-174-1-1030 0 0,-76 8-540 0 0,41-1-45 0 0,11-13 803 0 0,-45-20-1236 0 0,-153 28-64 0 0,-5 2-273 0 0,24-10-2694 0 0,-22 10 2502 0 0,8 0-15 0 0,-5 4-3511 0 0,0 2-4432 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="140326.574">13849 2403 8288 0 0,'0'0'638'0'0,"0"1"-414"0"0,-2 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,7 6 488 0 0,69 15 2067 0 0,-42-15-2223 0 0,51 23 954 0 0,-53-9-1577 0 0,43 37 370 0 0,-19 1-375 0 0,30 32 240 0 0,-83-87-712 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 0 0 0,2 1 1 0 0,-3 0-1 0 0,2-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-23 0 0,-5 4 44 0 0,0 0 1 0 0,0-2-1 0 0,-1 2 0 0 0,0-1 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,0-1-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-2-1 0 0 0,1 0-44 0 0,-27 11 59 0 0,0-3-1 0 0,0-1 1 0 0,-1-1 0 0 0,-1-3-1 0 0,1-1 1 0 0,-18-1-59 0 0,30-4-59 0 0,-75-9-1395 0 0,89 3-1171 0 0,11 5 1267 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151416.768">14974 2518 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-12 7 790 0 0,-14 10 150 0 0,-49 20 1099 0 0,6-4-1196 0 0,66-31-1165 0 0,-13 9 158 0 0,0 0 0 0 0,1 1-1 0 0,0 0 1 0 0,1 1 0 0 0,1 0 0 0 0,1 2 0 0 0,-1 0 0 0 0,1 0-1 0 0,-6 11-202 0 0,15-21 65 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,3 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 0 1 0 0,1 1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 1-64 0 0,1 1 108 0 0,1 0 0 0 0,-1 1-1 0 0,2-2 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,1 0-1 0 0,-1-2 1 0 0,1 2 0 0 0,0-1-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,-1 0-1 0 0,10 2-107 0 0,-5-2 42 0 0,-1-1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 0 0 0 0,9-2-41 0 0,23-18-4007 0 0,-37 14-3607 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="152065.555">15162 2850 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-4-9 655 0 0,4 3-930 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 2 0 0 0,2-2 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 2 0 0 0,1-2 0 0 0,0 1 0 0 0,2-1-345 0 0,-4 2 74 0 0,-1 0 0 0 0,-1 0-1 0 0,2 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,2 1-1 0 0,-2-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 1-1 0 0,1-1 1 0 0,-3 0 0 0 0,2 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 2-73 0 0,2 4 95 0 0,-1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 9-95 0 0,-13 68 1049 0 0,12-80-938 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-2-2-1 0 0,1 2 0 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0-1-111 0 0,1-3 23 0 0,0 0 0 0 0,2 0 0 0 0,-3 0 1 0 0,2-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-3 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-2-1-24 0 0,0-1-63 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 2 1 0 0,-1-2-1 0 0,2 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,0-1-1 0 0,2 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,1-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 1 1 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-6 63 0 0,7-22-2404 0 0,-5 16 1056 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153048.506">15674 2532 0 0 0,'-4'-6'-1709'0'0,"2"-5"9298"0"0,3 10 1867 0 0,-1 12-7849 0 0,4 99 2619 0 0,-7-24-3124 0 0,7 9 60 0 0,-9 39-1060 0 0,14-66-102 0 0,-6-62-68 0 0,-2-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153375.191">15651 2744 2304 0 0,'0'0'464'0'0,"4"-7"3648"0"0,-3 4 1786 0 0,28-40-750 0 0,12 4-2447 0 0,4 12-1313 0 0,-23 31-788 0 0,-20-4-482 0 0,0 1-42 0 0,3 2-30 0 0,0 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 0 0 0,-1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 1-46 0 0,24 85 1079 0 0,-14-64-711 0 0,-11-13-53 0 0,21 62 642 0 0,0-36-721 0 0,12-28-183 0 0,38-39-1154 0 0,-28-3-4448 0 0,-32 22 3543 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160253.303">16421 2358 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,6 2 583 0 0,-2-7-849 0 0,-4 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 15-2962 0 0,1 58 539 0 0,-6 67 472 0 0,-7 14 1084 0 0,10 76-784 0 0,10-186-592 0 0,2-24-84 0 0,12-17 3 0 0,-15-9-156 0 0,1 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 0 0 0,-3 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,3-3-35 0 0,49-39 80 0 0,-43 34-172 0 0,-8 8-92 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,-1-2 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1-3 184 0 0,2 0-1288 0 0,-1-8-6336 0 0,-4 11 565 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160816.746">16425 2573 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,62-5 2910 0 0,-44 4-3513 0 0,6 0-489 0 0,-9 4-4783 0 0,-5 1-1037 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="165875.957">16937 2595 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,4 5 4769 0 0,0 0-4077 0 0,-1-1-1648 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 2-394 0 0,-6 178 4855 0 0,1-66-3199 0 0,0-89-1224 0 0,6-10-3265 0 0,-1-13 1400 0 0,0-7-5540 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="166400.987">16975 2823 456 0 0,'2'-10'295'0'0,"-1"8"1230"0"0,6-14 4652 0 0,-6 15-4821 0 0,8-15 3233 0 0,-3 6-3731 0 0,20-33 2412 0 0,-24 41-3133 0 0,-1-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-137 0 0,40 1 1322 0 0,-39 1-1262 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-3 1-1 0 0,2-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 2-59 0 0,22 18 91 0 0,-8 2-240 0 0,-17-24-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167273.982">17464 2886 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 7-605 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 0 1 0 0,2 0-1 0 0,0 1 0 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 2-1 0 0,0-2 0 0 0,2 1 0 0 0,-3-1 0 0 0,2 1 0 0 0,2-3-329 0 0,12-26 1366 0 0,21-3-185 0 0,-35 35-1119 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,3 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,2 2-62 0 0,46 62 531 0 0,-45-51-291 0 0,2-2-1 0 0,-3 2 1 0 0,1 1 0 0 0,-1-1-1 0 0,-2 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-2 10-239 0 0,-7 39 0 0 0,-13-23 1095 0 0,1-43-406 0 0,14 1-606 0 0,1 1-72 0 0,-1 0 0 0 0,1-1 0 0 0,0 1-1 0 0,-1-1 1 0 0,1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,0 0 0 0 0,-3-2-11 0 0,2 0-209 0 0,2 1 0 0 0,-2 0-1 0 0,1-1 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-5 209 0 0,0-20-4042 0 0,2 15-3529 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167927.933">17974 2281 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,3 8 590 0 0,12 64 2596 0 0,-22 143-2669 0 0,-1-73 14 0 0,8 82-1117 0 0,4-174 0 0 0,-2-45-165 0 0,0-4-698 0 0,-2-1-315 0 0,1-1-1352 0 0,2-5-5157 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="189572.02">18272 2801 3568 0 0,'22'-10'1553'0'0,"-7"-6"1718"0"0,-2 11-2487 0 0,42-31 3450 0 0,-26 9-3218 0 0,35-42-474 0 0,-53 46-542 0 0,-8 15 0 0 0,-6-1 0 0 0,2 6-7 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,3 1 1 0 0,-5 0 6 0 0,0 2 11 0 0,-1-1 1 0 0,1 2-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 2 1 0 0,1-1-1 0 0,0 1 1 0 0,-4 5-12 0 0,-14 24 272 0 0,-7 53 161 0 0,28-82-291 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,0-1 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,2-1 0 0 0,-2 0-1 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,2-1-142 0 0,-2-1 13 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 1 0 0,1-1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,3 0-13 0 0,68-24-2033 0 0,-62 16 586 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190134.967">18742 2525 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-1 1-172 0 0,-17 52 5027 0 0,10-27-3083 0 0,-7 32 478 0 0,12-49-2198 0 0,1 2 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,2 6-320 0 0,-2 25 797 0 0,-1-36-713 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-2 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,5 3-83 0 0,-7-7 16 0 0,0 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-2 0 1 0 0,1-1-1 0 0,1-2-15 0 0,6-4 20 0 0,19-32 87 0 0,13-38-97 0 0,-36 71-49 0 0,0 1 0 0 0,-1-1-1 0 0,0-1 1 0 0,1 1 0 0 0,-3-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,-1-5 39 0 0,-4-22-1383 0 0,4 35 837 0 0,-1 0-1200 0 0,-6-5-4721 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192408.343">17375 2358 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,2-1-292 0 0,4-4-365 0 0,3-2-1 0 0,-2 1 1 0 0,-1-1 0 0 0,3-1-1 0 0,-4 1 1 0 0,1-1 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0-363 0 0,50-75 852 0 0,-40 66-781 0 0,-1 15-61 0 0,-11 6 2 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 2-11 0 0,2 2-4 0 0,7 24 57 0 0,1-3-53 0 0,6 0-1856 0 0,-10-23-4807 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="211829.387">8050 2582 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-12-2-24 0 0,8 2 8851 0 0,1 5-9133 0 0,-9 14-17 0 0,7-16-769 0 0,4-2-3236 0 0,1-1-1404 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-211952.654">20797 2883 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-8 0-423 0 0,2-2-329 0 0,4 2-272 0 0,-1-3-398 0 0,1-1-3749 0 0,-3-8 2451 0 0,4 10-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212149.586">20514 2615 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-14-3 2088 0 0,-5-4-821 0 0,17 7-1285 0 0,-13 3 543 0 0,-34 27 578 0 0,-5 47-1009 0 0,54-69-646 0 0,-2 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,3 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,3 0 0 0 0,-2-1 0 0 0,1 2-74 0 0,27 23 398 0 0,-29-29-397 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 0 1 0 0,-1 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,2-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,2-1-1 0 0,7 1-134 0 0,-8-1-167 0 0,0 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-2-1 0 0,-2 1 1 0 0,2 0 301 0 0,-5 2-105 0 0,15-8-1239 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205932.193">21011 2655 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,6 8 1656 0 0,-5-6-2461 0 0,1 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,-1 2-229 0 0,2 71 2716 0 0,19 156 1049 0 0,-30-72-3749 0 0,-1-90-16 0 0,-2 20 0 0 0,13-85-64 0 0,1-3-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205389.214">21041 2728 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,4-7 616 0 0,22-27 2026 0 0,-4 17-2035 0 0,-19 16-1214 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-3-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,3 1 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,3 0 0 0 0,-1 0-84 0 0,3 5 138 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,2 1 0 0 0,-4 0 0 0 0,2-1 0 0 0,-1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,-4 7-137 0 0,5-12 22 0 0,0 1-1 0 0,-1-2 0 0 0,1 1 1 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,-2 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 0-21 0 0,-38 9 162 0 0,36-10-192 0 0,3 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0 0 0 0,1-1-1 0 0,-5-1 30 0 0,-13-31-3512 0 0,17 22 1769 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-204187.105">21512 2476 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203902.979">21492 2452 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203901.979">21477 2556 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203439.752">21444 2367 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,4 11 2392 0 0,14 78 1583 0 0,-17 33-1639 0 0,9 43-192 0 0,13-21-2656 0 0,-26-126 0 0 0,-1-3-337 0 0,3-13-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202468.889">21481 2780 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-2-17 3737 0 0,5-3 4077 0 0,8-22-4186 0 0,8 2-1366 0 0,-1 19-2142 0 0,-10 19-211 0 0,-8 7 222 0 0,20-9 1281 0 0,9 11-1444 0 0,-26 1-105 0 0,47 31-8 0 0,-24-3 744 0 0,-11-4-56 0 0,7 34-96 0 0,-14-20-16 0 0,3 12 191 0 0,0-18-526 0 0,-1-4-59 0 0,-2-16-12 0 0,-6-13-90 0 0,17 3 16 0 0,18-2-96 0 0,-8-4-141 0 0,-28 2-596 0 0,28-10-4249 0 0,-15 4 1073 0 0,-8 2 1923 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201801.05">22089 2582 1376 0 0,'-16'6'65'0'0,"12"-5"277"0"0,4-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-6 11 5285 0 0,12 44-3424 0 0,-9-9-2068 0 0,-2 46 541 0 0,-5-51-877 0 0,6 2-432 0 0,5 22-1088 0 0,8 8 915 0 0,-3-3-416 0 0,-3-58-545 0 0,-5 18 164 0 0,-3-11-45 0 0,3-18-557 0 0,2-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-4 0-797 0 0,2 0-5332 0 0,2 0 728 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201246.613">22042 2631 456 0 0,'34'-10'12581'0'0,"-22"4"-11549"0"0,16 5 3076 0 0,-2-5-1928 0 0,31 39 262 0 0,-20 0-1426 0 0,-11 18-48 0 0,-9-18-336 0 0,-17-29-440 0 0,-3 27-53 0 0,-7-10-60 0 0,-9-8 791 0 0,18-11-867 0 0,0-1 1 0 0,-2 1-1 0 0,3-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 0-1 0 0,1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-2-1-1 0 0,1 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-2-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,-2 1-3 0 0,-37-21-1713 0 0,14-1-2008 0 0,23 15 1827 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190828.747">19149 2549 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,3 14 1120 0 0,0 35 395 0 0,1 68 75 0 0,4-39-2940 0 0,4 7-252 0 0,-4-12-192 0 0,0-37-12 0 0,-8-34-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="191215.919">19164 2707 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,4-14 2209 0 0,12-3-1077 0 0,32-21 345 0 0,-19 31-1146 0 0,-5 21-314 0 0,-19-11-177 0 0,-1 1 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0-37 0 0,-1-4 176 0 0,9 11 413 0 0,-9-12-998 0 0,11 6-4069 0 0,-12-7 3075 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="199554.903">19491 3003 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,7-4 224 0 0,-5 3 3136 0 0,10-10-3493 0 0,-10 8-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174270.903">19894 2655 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 12 8138 0 0,-3 35-5693 0 0,3-49-1919 0 0,-3 16 1214 0 0,-1 77 988 0 0,4-93-2320 0 0,0-2-72 0 0,0 7 75 0 0,-5 26-43 0 0,-2 43-122 0 0,7-73-45 0 0,0 0-235 0 0,0 0-3512 0 0,0-3-1706 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173620.241">19879 2794 5296 0 0,'5'7'472'0'0,"-5"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-22 1372 0 0,0 20-1542 0 0,0 0-40 0 0,6-28 954 0 0,-5 29-1144 0 0,13-27 1755 0 0,4 10-1413 0 0,-16 17-538 0 0,-2 1 0 0 0,0 0-6 0 0,15-2 374 0 0,-9 3-368 0 0,-3-1-159 0 0,-2 0 0 0 0,1 0-1 0 0,1 0 1 0 0,-3 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 0 0 0 0,3 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,0 0 0 0 0,2 0-1 0 0,-3 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,2 1 0 0 0,-2-1-1 0 0,1 1-24 0 0,14 59 908 0 0,-11-27-544 0 0,-5-11-78 0 0,1-22-204 0 0,0 21 170 0 0,1-19-204 0 0,2 5-36 0 0,1-1-1 0 0,0 1 42 0 0,3-4 13 0 0,-4-3-58 0 0,1 0 1 0 0,-1 0 0 0 0,-1-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,3 1 0 0 0,-1-1 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,2-3-9 0 0,35-22-3222 0 0,-34 21-430 0 0,-4 5 1775 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="-165827.57">13990 3494 920 0 0,'0'0'411'0'0,"0"0"1389"0"0,0 0 609 0 0,0 0 119 0 0,0 0-215 0 0,0 0-1014 0 0,0 0-445 0 0,0 0-87 0 0,0 0-46 0 0,0 0-109 0 0,0 0-48 0 0,0 0-10 0 0,0 0 0 0 0,0 0 11 0 0,-15-2 1750 0 0,-7-1-885 0 0,-1 0-1 0 0,1 2 1 0 0,-1 0-1 0 0,1 1 1 0 0,-14 2-1430 0 0,-40 9 1057 0 0,-26-10-2 0 0,32-4-630 0 0,-85 0 196 0 0,35-7-298 0 0,38-9 8 0 0,68 15-305 0 0,0 1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 1 0 0 0,1 0 0 0 0,-3 0 0 0 0,1 2 0 0 0,2 0 0 0 0,-1 0-1 0 0,-5 2-25 0 0,-46 12 22 0 0,13-6 31 0 0,11-13 11 0 0,-79-2 64 0 0,57 27-128 0 0,-21 1 0 0 0,46-21 0 0 0,-11-5 0 0 0,-23 7 0 0 0,39 3 0 0 0,-13-12 0 0 0,-3-24 0 0 0,-7 28 0 0 0,4-3 0 0 0,35 3-632 0 0,15 1 769 0 0,-1 1-984 0 0,3 0-6440 0 0,6-2 5260 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-62540.216">6177 235 9240 0 0,'0'0'208'0'0,"0"0"33"0"0,0 0 14 0 0,0 0 69 0 0,0 0 284 0 0,0 0 120 0 0,0 0 28 0 0,0 0-30 0 0,0 0-139 0 0,0 0-62 0 0,0 16 1654 0 0,-7 120 2954 0 0,-3 15-3081 0 0,9 57-343 0 0,9 147 170 0 0,2-197-1465 0 0,-10-127-531 0 0,0-29-556 0 0,0-4-270 0 0,-4-25-3089 0 0,1 16 1904 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-50190.827">6144 270 3224 0 0,'0'0'387'0'0,"0"0"414"0"0,0 0 183 0 0,0 0 37 0 0,-12-2 2900 0 0,3 0 1482 0 0,5 5 686 0 0,21 7-5649 0 0,85-9 731 0 0,-34-11-391 0 0,69 6-160 0 0,50-5-302 0 0,-70-3-104 0 0,26 7 148 0 0,-7 3 150 0 0,-12 2-320 0 0,25 3-48 0 0,-27 4 171 0 0,65 15 58 0 0,-60-9 92 0 0,8-9 14 0 0,-8-11-479 0 0,-47 2 68 0 0,-61 2-39 0 0,0 2-1 0 0,1 0 1 0 0,-1 1 0 0 0,0 1-1 0 0,1 1 1 0 0,10 2-29 0 0,38 5 0 0 0,32-5 0 0 0,-14 0 0 0 0,-7-1 0 0 0,-38 7 0 0 0,48-4 0 0 0,51-8 0 0 0,-99-1 0 0 0,44 5 0 0 0,-71 1 5 0 0,0 0 0 0 0,0-1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-2-1 0 0 0,6-1-5 0 0,65-5 19 0 0,97 21-8 0 0,-107-7 95 0 0,20-6-31 0 0,-17-10-11 0 0,96 1 0 0 0,-82 2 0 0 0,8 1-64 0 0,-46-2 53 0 0,38-1-42 0 0,-45 9-11 0 0,59-4 0 0 0,20 0 0 0 0,-35 16 0 0 0,207-10 0 0 0,-131-19 0 0 0,-86 11 0 0 0,41-1 0 0 0,-28 11 0 0 0,-35 3 0 0 0,28-6 64 0 0,-4-6 128 0 0,62 5-192 0 0,-110 4 0 0 0,0-2 0 0 0,-26-2 0 0 0,-2 0-12 0 0,-5 0-53 0 0,-1 0-170 0 0,0 0-576 0 0,0 0-247 0 0,0 0-49 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-49193.598">11691 188 5928 0 0,'0'0'266'0'0,"0"0"1"0"0,0 1-171 0 0,0 4 92 0 0,0-4 732 0 0,-2 15 4758 0 0,4 13-1191 0 0,8 34 169 0 0,-13-10-3447 0 0,-4 116 1305 0 0,2-59-2021 0 0,0-8-60 0 0,3 50 591 0 0,9-33-728 0 0,-3-89-284 0 0,-3 2 204 0 0,-1-31-157 0 0,0-1 6 0 0,0 0-26 0 0,0 0-98 0 0,0 0-9 0 0,0 0 4 0 0,0 0 0 0 0,0 0-43 0 0,0 0-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0-98 0 0,0 0-410 0 0,0 0-182 0 0,0 0-42 0 0,0 0-73 0 0,0 0-285 0 0,0 0-126 0 0,0 0-983 0 0,0 0-3823 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-48911.614">11676 1067 456 0 0,'0'0'1737'0'0,"0"0"207"0"0,0 0 88 0 0,0 0-76 0 0,0 0-381 0 0,0 0-174 0 0,0 0-32 0 0,0 0-62 0 0,0 0-231 0 0,0 2-99 0 0,0 74 4474 0 0,5-45-4150 0 0,0 17 250 0 0,-3 2-1349 0 0,-4-22-20 0 0,2-20-172 0 0,0 4 904 0 0,0-12-2338 0 0,0 3-8055 0 0,0-3 3197 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-46458.211">11701 1295 3224 0 0,'-11'8'2653'0'0,"-43"18"4634"0"0,52-26-6665 0 0,0 0 33 0 0,-48-6 3329 0 0,-36 0 217 0 0,54 7-3372 0 0,-81-2 683 0 0,48-20 54 0 0,32 11-1308 0 0,14 5-82 0 0,2 1 1 0 0,-1 1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 2 0 0 0,1 0 1 0 0,-12 2-177 0 0,-15-1 177 0 0,-42-8 419 0 0,14-3-51 0 0,-62 6 350 0 0,26 11-662 0 0,16 3-169 0 0,12-3-64 0 0,-16-14 140 0 0,-62 6 320 0 0,49 2-460 0 0,7-13 83 0 0,18 0-30 0 0,32 6-53 0 0,-40 1 0 0 0,-64 5 0 0 0,-21-4 0 0 0,80 1 0 0 0,-1 5 0 0 0,-46-4 0 0 0,8-5 0 0 0,-146 7 0 0 0,198 4 0 0 0,-38-8 117 0 0,10-8 118 0 0,49 8-410 0 0,-108 8 326 0 0,104-8-162 0 0,-88-1 37 0 0,3 9-289 0 0,9 5 263 0 0,-37-1 208 0 0,67-1-413 0 0,-52-4 194 0 0,39-6 11 0 0,-39 21 344 0 0,77-4-608 0 0,-67 3 160 0 0,77-14 104 0 0,-38-3 968 0 0,15-10-1140 0 0,13 10-113 0 0,25 9 214 0 0,-43-4 71 0 0,74-6-97 0 0,25 2 121 0 0,4-1-4216 0 0,4 0-5767 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-41895.864">6310 2480 5264 0 0,'3'0'1129'0'0,"7"0"-2200"0"0,-6 0 4901 0 0,-3 1 4833 0 0,7 40-6741 0 0,-8 52 512 0 0,-8 20-998 0 0,16 99 1044 0 0,7-73-1600 0 0,-3-44-128 0 0,3 47-792 0 0,-8-68 515 0 0,-7-35 182 0 0,-5-14 138 0 0,0-15-1692 0 0,5-10-2271 0 0,2-7 1285 0 0,-1-2-408 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-39644.648">6271 2483 456 0 0,'0'0'1548'0'0,"0"0"185"0"0,0 0 82 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-42 0 0,0 0-140 0 0,0 0-57 0 0,0 0-16 0 0,0 0-1 0 0,0 0 12 0 0,0 0 2 0 0,0 0-1 0 0,0 0-47 0 0,0 0-202 0 0,0 0-92 0 0,3 0-11 0 0,51-7 2042 0 0,49 2 147 0 0,70 4-222 0 0,-24 10-1432 0 0,-19-15-175 0 0,143-11 402 0 0,-122-6-820 0 0,-55 7 18 0 0,-56 9-382 0 0,1 2 1 0 0,0 2-1 0 0,32 1 7 0 0,65 2 256 0 0,-92 0-256 0 0,45 0 181 0 0,-23 10-106 0 0,7-4 1 0 0,-3-2 68 0 0,57-1-1 0 0,-81 0-90 0 0,84-4 144 0 0,193-7-122 0 0,-259 11-75 0 0,45 7 0 0 0,21-7 0 0 0,-68 4 0 0 0,-4-2 0 0 0,58-5 0 0 0,16 0 0 0 0,-66 11 0 0 0,-23-4 64 0 0,66-18 0 0 0,-41 1-64 0 0,55-2-67 0 0,43 22 54 0 0,-96-11 13 0 0,-45-2 11 0 0,4 1-1 0 0,-4 1 1 0 0,1 1 0 0 0,0 1-1 0 0,26 4-10 0 0,10-2 11 0 0,79-6-74 0 0,-52-2 30 0 0,49 17 33 0 0,15-2 152 0 0,-92-3-152 0 0,-24-6-172 0 0,45 4 160 0 0,12-5 12 0 0,-28 0 0 0 0,-8-3 0 0 0,-24 3 0 0 0,2 0-16 0 0,-36 0-61 0 0,-2 0-6 0 0,0 0-138 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1739 0 0,0 0-6757 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-38736.343">11284 2434 1376 0 0,'0'0'65'0'0,"0"0"341"0"0,0 0 1404 0 0,0 0 611 0 0,9 0 3921 0 0,-6 1-6029 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 2-313 0 0,6 60 2731 0 0,20 118-151 0 0,-16-99-1558 0 0,-15 39 98 0 0,14 23 148 0 0,-4-75-785 0 0,-4-28-243 0 0,-2 25 129 0 0,1 21 111 0 0,-1-55-253 0 0,0-32-205 0 0,0-1-106 0 0,0 0-8 0 0,-19 20-828 0 0,19-20 767 0 0,-11 16-1455 0 0,10-15 1350 0 0,1-1-81 0 0,0 0-40 0 0,0 0-5 0 0,0 0-101 0 0,0 0-426 0 0,0 0-185 0 0,0 0-37 0 0,0 0-102 0 0,0 0-386 0 0,0 0-166 0 0,0 0-32 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36969.387">11366 3435 3224 0 0,'-7'11'5642'0'0,"-8"13"-878"0"0,15-22-3930 0 0,-1-1-138 0 0,-34 27 3385 0 0,-35-14 128 0 0,36-12-2861 0 0,-136 22 765 0 0,115-14-1621 0 0,-105-3 1168 0 0,22-23-712 0 0,-139 2-243 0 0,154 17-482 0 0,-32 1 141 0 0,51-5-364 0 0,-187 8 0 0 0,182 3 0 0 0,-294-7 0 0 0,223 1 228 0 0,-59-31 541 0 0,131 17-750 0 0,-63-3-19 0 0,119 6 0 0 0,28 6 0 0 0,0-2 0 0 0,-1-1 0 0 0,1 0 0 0 0,1-1 0 0 0,-8-5 0 0 0,19 7 0 0 0,-39-13 0 0 0,-2 3 0 0 0,1 2 0 0 0,-1 3 0 0 0,0 1 0 0 0,-15 4 0 0 0,-28 5 0 0 0,29 4 0 0 0,-88-8 0 0 0,88-2 0 0 0,-78 7 0 0 0,51 10-21 0 0,3-3-5 0 0,-33 0-287 0 0,87-4 334 0 0,-12-2 286 0 0,-77-10-307 0 0,31-8-103 0 0,3 11-9 0 0,55 6 23 0 0,-4-3 89 0 0,-11 13 0 0 0,-58 5 73 0 0,53-9-143 0 0,4-2 403 0 0,5-9-333 0 0,18 4 0 0 0,-17-4-32 0 0,48 2-137 0 0,-2 8-3011 0 0,2-5 1857 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1488.941">14464 2155 3224 0 0,'0'0'389'0'0,"0"0"426"0"0,0 0 185 0 0,0 0 37 0 0,0 0-41 0 0,0 0-211 0 0,9 14 2921 0 0,0 1-2586 0 0,-8-14-544 0 0,-1 0 0 0 0,15 143 6159 0 0,-23 6-3759 0 0,6-40-1768 0 0,4 57 608 0 0,2 44-811 0 0,23 103 755 0 0,-12-178-1237 0 0,-8 21-2562 0 0,-7-166-744 0 0,0-6-6530 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="854.454">14458 2113 3224 0 0,'-4'-1'-2321'0'0,"1"-2"3355"0"0,-6-4 11775 0 0,12 5-10726 0 0,-2 1-1175 0 0,-1 1-164 0 0,12-2 590 0 0,120 14 3826 0 0,139-5-1952 0 0,-1 0-2760 0 0,-77-11 16 0 0,-45-9 16 0 0,47-10 88 0 0,-26 6-187 0 0,42 3-162 0 0,-33 3-75 0 0,36-4 144 0 0,-6 2-149 0 0,-47 3-22 0 0,67-6-205 0 0,-7 10 211 0 0,58 5 714 0 0,-30 8-953 0 0,41 9-59 0 0,-169-3 482 0 0,5-10-635 0 0,-9 1 267 0 0,85 19 74 0 0,-31-3-13 0 0,22 0-88 0 0,18-10 152 0 0,12-10-64 0 0,-79-3 0 0 0,-43-4 0 0 0,171-3 0 0 0,-119 7 0 0 0,78 2 0 0 0,-145 11 0 0 0,74-3 0 0 0,-11 0 0 0 0,-61 7 0 0 0,59 6 0 0 0,-90-9 0 0 0,58 0 0 0 0,39 0 0 0 0,9 2 0 0 0,-75-7 400 0 0,-8 1-480 0 0,77-11 133 0 0,-14 1-106 0 0,-107 3 53 0 0,60-1-64 0 0,-22-4 64 0 0,-21 2 11 0 0,75 1 375 0 0,-67-14-452 0 0,-28 10 108 0 0,36-4-95 0 0,-41 10 53 0 0,-28 19-245 0 0,-2-16 238 0 0,2-3 7 0 0,-2 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-2 1 1 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,2-1 0 0 0,10 59 0 0 0,0-26 0 0 0,-12 4 0 0 0,18 3 0 0 0,-22 2 0 0 0,7-25 0 0 0,0-9 0 0 0,-3 0 0 0 0,1 1 0 0 0,0-2 0 0 0,-1 2 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-2 5 0 0 0,-9 79-11 0 0,-9-3-42 0 0,17-3 53 0 0,10 36 0 0 0,0-59 0 0 0,-4-7 12 0 0,0-50 4 0 0,0 38 108 0 0,-35 61-44 0 0,22-58-80 0 0,4-36 0 0 0,-3 21 0 0 0,8 31 0 0 0,13-30 0 0 0,-9 3 0 0 0,-7-25 0 0 0,4 1 0 0 0,-2 27 99 0 0,0-27 95 0 0,-7 12-174 0 0,3-7 27 0 0,8-7-47 0 0,6-3 0 0 0,1 0 0 0 0,-7-1 0 0 0,6-3-20 0 0,-4-2-73 0 0,-3-1 7 0 0,-3 0-3 0 0,2 0-9 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1-1 0 0,-2 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1-1 0 0,2 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 98 0 0,5-6-6888 0 0,-4 2-1987 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6517.426">14541 3603 7688 0 0,'0'0'349'0'0,"0"0"-2"0"0,0 0-90 0 0,0 0 455 0 0,0 0 227 0 0,0 0 42 0 0,15 5 4082 0 0,56-12-625 0 0,3 6-2566 0 0,-15 4-1407 0 0,127-3 623 0 0,-14 5-464 0 0,-49 11 788 0 0,28-5-770 0 0,177-35 656 0 0,-205 24-914 0 0,-66 3-169 0 0,136-13 21 0 0,-22-2-119 0 0,-98 21-53 0 0,11 4 128 0 0,-32-7-192 0 0,49 5-8 0 0,55-2 144 0 0,-63 4-136 0 0,11 0 32 0 0,-71-10 64 0 0,12-3-335 0 0,11 4 142 0 0,19 7 97 0 0,-3-8 168 0 0,82-14-96 0 0,-82 5-8 0 0,10-4-240 0 0,-13 16 64 0 0,36-15 96 0 0,-7-1 167 0 0,32-2-62 0 0,-74 12-25 0 0,113-18-57 0 0,-101 9-318 0 0,108 4 639 0 0,43-2-696 0 0,-30 21 1344 0 0,-62-6-976 0 0,-16-2 0 0 0,-7-3 0 0 0,18 7 200 0 0,-61 2-40 0 0,209 5-64 0 0,-28-10 203 0 0,-167-10-246 0 0,72 13 139 0 0,135-7-128 0 0,-152-6 428 0 0,-2-5 0 0 0,2-7-492 0 0,33-2 0 0 0,157-22-11 0 0,-185 22-42 0 0,15 1 53 0 0,-48 13 0 0 0,-80 1 0 0 0,0 2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 1 0 0 0,19 5 0 0 0,74 6 0 0 0,15-3 0 0 0,60 0 0 0 0,-109-9 0 0 0,-48-6 0 0 0,10-1 0 0 0,38-7 0 0 0,-21 6 0 0 0,-47 7 0 0 0,-6 0 0 0 0,5 0-16 0 0,-10 0-68 0 0,-2 0-32 0 0,16 3-689 0 0,-21 1-1817 0 0,-8 5-1623 0 0,-26 7 1843 0 0,-7-5-20 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">232 662 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="310.099">601 678 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-8 10039 0 0,4 3-11103 0 0,-2 0-133 0 0,2-1-129 0 0,0 6-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="684.255">972 620 11976 0 0,'-1'5'296'0'0,"-4"5"4551"0"0,3-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1921.293">1299 703 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,3-22-839 0 0,-6 31-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-13 79 971 0 0,11-78-904 0 0,2-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,5-16-522 0 0,2-30 325 0 0,-7 45 218 0 0,0 1 13 0 0,6-4-260 0 0,0 7-230 0 0,-4 3 347 0 0,-12 35 365 0 0,9-39-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-10-12-214 0 0,20-43 40 0 0,0 47 757 0 0,-8 7-562 0 0,-2 1-34 0 0,12 15 96 0 0,-21 51 294 0 0,9-64 48 0 0,0-2-24 0 0,-11 10 14 0 0,10-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 1 0 0,-2-1-1 0 0,2 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-2 1-12 0 0,0-1-1 0 0,1 0 1 0 0,0-1-1 0 0,-2 1 0 0 0,3 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-2-1 0 0,0 2 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-2-1 0 0,1 2 0 0 0,0-3 1 0 0,15-19-798 0 0,-5 23 705 0 0,11 18 39 0 0,-20-15 64 0 0,1 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 2 0 0 0,1-1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,2 1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,-2-2 0 0 0,1 3-10 0 0,1-5 84 0 0,-4 18 237 0 0,-19-10-89 0 0,22-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,5-11-3857 0 0,1 13-3207 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8390.611">1575 419 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,7 58 3341 0 0,1-35-2076 0 0,-3 53 1115 0 0,0 16 113 0 0,-1-14-1404 0 0,-1 52 981 0 0,-4-3-1688 0 0,1-58-1417 0 0,-2-33 962 0 0,-6-27-2248 0 0,2-6-5035 0 0,6-10 5419 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8997.239">1515 555 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0-1 240 0 0,14-33 2722 0 0,-14 32-3180 0 0,14-14 1008 0 0,22-26 674 0 0,-34 37-2057 0 0,2 2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-2 0 0 0 0,2 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,1 3 1 0 0,-1-2 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 1-137 0 0,64 19 1009 0 0,-49 14 55 0 0,-5-17-600 0 0,21 46 1448 0 0,-22 2-2113 0 0,-14-61 230 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,2 0 0 0 0,-2-1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 0 0 0,-1 1-29 0 0,3-3 5 0 0,-8 22 399 0 0,0-11-337 0 0,8-8-104 0 0,-3-1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 37 0 0,-32-1 653 0 0,-8-25-4978 0 0,33 19 2334 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11709.08">2821 384 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 48 1154 0 0,-12 24 2052 0 0,-2 34 1755 0 0,2 52-2463 0 0,5-55-962 0 0,-4 32-1172 0 0,7-140-851 0 0,0-2-91 0 0,0 0-16 0 0,0 12-2832 0 0,-2 12-2556 0 0,0-23 1622 0 0,2-1-894 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12315.019">2838 442 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,12-7 8 0 0,2-4 772 0 0,-13 10-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2 0 0 0 0,3 0 0 0 0,-3 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0-250 0 0,7 4 395 0 0,1 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 1 1 0 0,3 4-396 0 0,-5-7 170 0 0,-1 1 5 0 0,-1 2-1 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,-2 0 1 0 0,1 2-1 0 0,-1-2 1 0 0,-1 1-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 1 0 0,-1 2-1 0 0,1 1-174 0 0,-2 35 278 0 0,-1-42-199 0 0,1-2 0 0 0,-1 2 1 0 0,0-1-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,-1-1 1 0 0,3 0-1 0 0,-2 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 1 1 0 0,1-2-1 0 0,-2 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 2-79 0 0,-2 0 4 0 0,0-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,2-1 0 0 0,-3 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,2 0 0 0 0,-3-1 0 0 0,1 0 0 0 0,-2-1-4 0 0,-52-44-4198 0 0,52 41-3651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10346.212">2092 79 3680 0 0,'-5'48'613'0'0,"1"-10"6816"0"0,-7 24-4591 0 0,8 16-23 0 0,3-13-297 0 0,4 4-1604 0 0,-8 95 2 0 0,7-78 200 0 0,0-18-716 0 0,3-41-126 0 0,-6-20-115 0 0,-4 0-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10997.838">2022 653 1376 0 0,'4'-21'2159'0'0,"4"1"4223"0"0,4-7-3735 0 0,-1 7-1523 0 0,10-17 1153 0 0,5 13 523 0 0,-5 1-1591 0 0,22-16 135 0 0,-42 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,0-2 0 0 0,0 2 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 2-1 0 0,3-2 0 0 0,-1 1 1 0 0,-2-1-1 0 0,3 1 0 0 0,-2-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 1 0 0,0 1-51 0 0,2 3 27 0 0,2 1 1 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 1-1 0 0,2-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,0 1-1 0 0,0-2 1 0 0,0 2 0 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 6-27 0 0,9 30 368 0 0,28 121 1443 0 0,-19-125-1634 0 0,1-14-84 0 0,-14-24-77 0 0,-4-1-29 0 0,0-1-1 0 0,0 1 1 0 0,-2-1 0 0 0,3 0 0 0 0,1 1 0 0 0,-3-1 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,3 0 0 0 0,-1 1 0 0 0,-2-1 0 0 0,0 0 0 0 0,1-1-1 0 0,0 1 1 0 0,1-1 13 0 0,35-28-350 0 0,20-13-3834 0 0,-52 37 2533 0 0,4 3-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="32289.342">1 257 6448 0 0,'7'21'6309'0'0,"-7"-18"-6682"0"0,4 55 3514 0 0,7 84-847 0 0,-1-43-690 0 0,-6-11-929 0 0,12 133 737 0 0,-26 32 57 0 0,6-177-1337 0 0,-2-47-256 0 0,6-13-955 0 0,0-13-4480 0 0,0-3-582 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35199.426">12 288 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,16-37 6274 0 0,-16 46-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,11-3 291 0 0,68-19 828 0 0,-37 5-729 0 0,13-3 96 0 0,45 11 370 0 0,-55 8-222 0 0,38 2-1079 0 0,-18-6 16 0 0,34-21 451 0 0,-28 17 1144 0 0,57-1-1448 0 0,4 21 224 0 0,-51-21-645 0 0,-27 1 1538 0 0,5-1-1123 0 0,-33 8-292 0 0,47-1 264 0 0,-22-5 20 0 0,50-26 70 0 0,10 18-205 0 0,12 9 34 0 0,-62-3 219 0 0,21-7-424 0 0,-5 13 192 0 0,-8 5 584 0 0,40 1-1352 0 0,-6 10 736 0 0,1 4 1017 0 0,-31-9-298 0 0,-11 0-1239 0 0,25-4 520 0 0,13 3 64 0 0,12 29 75 0 0,-57-10-166 0 0,15-1 523 0 0,-5-7-840 0 0,-20-7 749 0 0,-6-3-675 0 0,23 7 487 0 0,69-11-197 0 0,-20 20 0 0 0,-38-15-20 0 0,-43-2 0 0 0,-10-5 0 0 0,22 17 0 0 0,-35-3 0 0 0,4 6 0 0 0,12 24 64 0 0,-4 27 0 0 0,-8 24-64 0 0,-3 30-8 0 0,-2-49 125 0 0,-2 32-203 0 0,-8 33 295 0 0,8 45-190 0 0,-16-84 82 0 0,0-42-13 0 0,3-44 96 0 0,8-12-234 0 0,-1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,1-2-1 0 0,-2 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1-1 0 0 0,0 1-1 0 0,-2 1 51 0 0,0-1 114 0 0,2-1 0 0 0,-2 0 0 0 0,0 0 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 0 1 0 0,0 0-1 0 0,-2-1 0 0 0,1 0-114 0 0,-14 0 158 0 0,-91 8-218 0 0,76-3 59 0 0,0-1-1 0 0,1-2 1 0 0,-1-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-21-6 1 0 0,5-4-9 0 0,-3 4 0 0 0,2 2 0 0 0,-1 2 0 0 0,-20 2 9 0 0,-105-1 332 0 0,130 5-330 0 0,1-1-1 0 0,-2-3 1 0 0,1-2-1 0 0,0-1 1 0 0,-8-7-2 0 0,22 9-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-18 4 18 0 0,-136 31 64 0 0,-3-14-136 0 0,-43-8 152 0 0,160-13-80 0 0,-85 0 11 0 0,-32-17 42 0 0,95 17-53 0 0,-21-12 80 0 0,20-13-176 0 0,-80-18 224 0 0,53 24-196 0 0,59 5 192 0 0,-58-3-124 0 0,48 10 0 0 0,42 15-499 0 0,31-8 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="78758.085">3545 867 13560 0 0,'0'0'306'0'0,"-11"-2"752"0"0,-23-5-12 0 0,33 7-11 0 0,-8-6 1119 0 0,9 5 2052 0 0,61 4-3188 0 0,29-6 262 0 0,150 31 512 0 0,-128-21-1336 0 0,145 26-663 0 0,-45 9 353 0 0,-6-8 891 0 0,-117-31-445 0 0,-71-3-541 0 0,-1-1 0 0 0,1 0 0 0 0,-1-2 1 0 0,1 0-1 0 0,-1-1 0 0 0,9-5-51 0 0,68-34-278 0 0,-91 42 89 0 0,-3 1-156 0 0,3 0-611 0 0,0 1-1432 0 0,-2-2-4991 0 0,-1 1-504 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="79175.854">5048 577 6448 0 0,'0'0'498'0'0,"1"-1"-28"0"0,28-3 10100 0 0,23 22-6654 0 0,-32-8-3356 0 0,2 0 0 0 0,-1 1 1 0 0,0 2-1 0 0,-2 0 0 0 0,0 1 0 0 0,6 6-560 0 0,55 54 264 0 0,-73-63-125 0 0,0 0-1 0 0,0 0 1 0 0,-1 2-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 0 1 0 0,3 13-139 0 0,-5-12 187 0 0,-2-1 1 0 0,1 0-1 0 0,1 1 1 0 0,-3 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-3-1 1 0 0,2 1-1 0 0,-1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,-1 0-1 0 0,1-1 1 0 0,-5 8-188 0 0,-23 29 165 0 0,-31-8 587 0 0,-84-22 352 0 0,117-19-1542 0 0,-22 5-2761 0 0,45 0 2491 0 0,-27 12-2399 0 0,16-4-3298 0 0,4 2-1217 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37346.914">6300 855 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,19-15-8855 0 0,-13 10 1888 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37618.204">6651 898 10592 0 0,'-12'-11'818'0'0,"9"7"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 1 1568 0 0,12-2-8082 0 0,-4 4-1569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37903.659">6978 809 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,3 0-232 0 0,1 0-5476 0 0,-5 0-2114 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="38875.93">7319 898 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-8-13 464 0 0,12-41 1231 0 0,0 46-2463 0 0,-1 1 0 0 0,3 1 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,6 8 88 0 0,-5-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-2-2 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 5-113 0 0,1-5 41 0 0,2-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,1-2 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1-2 0 0 0,1 2 0 0 0,-2 0 0 0 0,2 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-16-143 0 0,-13 33-62 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 1 1 0 0,1-1 0 0 0,0 0 0 0 0,0-1-1 0 0,1 2 1 0 0,-3-1 0 0 0,1 1 0 0 0,1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,-1-1-43 0 0,4 1 32 0 0,1 9 23 0 0,-11 20 200 0 0,4-28-96 0 0,-6 4-695 0 0,12-7-611 0 0,8-10-5710 0 0,-6 6 446 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="44618.988">7585 528 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-2-3 4251 0 0,12 22-45 0 0,-12-25-3788 0 0,2 9 1039 0 0,4 82 1637 0 0,6 83-1221 0 0,-13-84-1606 0 0,0-82-341 0 0,-2-3-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="53832.509">7867 570 2760 0 0,'4'8'1828'0'0,"3"20"4892"0"0,5 26-3444 0 0,2 102 1947 0 0,-11-80-3937 0 0,-6-36-4508 0 0,3-37 1701 0 0,-4 5-229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="54557.219">7917 898 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,8-38 5734 0 0,4-12-521 0 0,-16 20-3279 0 0,10 9-1202 0 0,8-36 1 0 0,-12 56-738 0 0,0-1 0 0 0,-1 1-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-2 1 0 0 0,2-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,4 0-93 0 0,1-2 95 0 0,-5 3-21 0 0,25 0-60 0 0,1 13-14 0 0,-4 9 0 0 0,-20-13 0 0 0,10 24 0 0 0,19 72 514 0 0,-18-51 356 0 0,3-17-278 0 0,-16-36-517 0 0,4 3 98 0 0,-2-2-141 0 0,-2-1 0 0 0,1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2-1 0 0 0,0 1-1 0 0,-2-1 1 0 0,2 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 0-32 0 0,23-3-185 0 0,-6-29-4233 0 0,-20 32 2840 0 0,0 1-164 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="56701.452">8656 626 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-3 102 0 0,-1 3-405 0 0,2 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-10-2-143 0 0,-36-6 1747 0 0,37 9-1667 0 0,7-2 170 0 0,0 0 0 0 0,-1 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 1-1 0 0,-3-1 0 0 0,1 1 0 0 0,0 0 1 0 0,2 0-1 0 0,-3 1 0 0 0,3-1 0 0 0,-1 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-32 42-483 0 0,18 2 618 0 0,14 12 378 0 0,9 5-513 0 0,15-5 1899 0 0,24-10-1734 0 0,-11-19-165 0 0,-18-20 0 0 0,14 1 0 0 0,-20-9 0 0 0,-3 3 0 0 0,1-6-64 0 0,27-22-5497 0 0,-28 15 3530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="57367.528">8904 961 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-8 907 0 0,12-15 649 0 0,-10 17-2004 0 0,-2 5 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 20 784 0 0,-16 13 56 0 0,6-32-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="64361.857">9160 618 1840 0 0,'0'5'396'0'0,"0"-2"991"0"0,0-3 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,6 17 886 0 0,5 74 1352 0 0,-4-55-2105 0 0,-9 64 686 0 0,-2-7-314 0 0,3 68-530 0 0,6-113-273 0 0,-3-10 0 0 0,-6-12-45 0 0,4-24-194 0 0,0-2-94 0 0,0 0-19 0 0,-2-15-1557 0 0,1 0 195 0 0,-1-1-70 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="69762.645">9128 620 1376 0 0,'3'7'367'0'0,"-3"-6"1002"0"0,0-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,2 0 1 0 0,-2 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,8-7 51 0 0,32-24 1588 0 0,-28 25-1245 0 0,-10 4-294 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,1 1-100 0 0,1 2 108 0 0,2 2-1 0 0,-2-1 0 0 0,0-1 0 0 0,0 2 1 0 0,0-1-1 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 0 0 0,-1 1 1 0 0,3-2-1 0 0,-3 1 0 0 0,0 1 0 0 0,1 0 1 0 0,0 5-108 0 0,8 27 435 0 0,1 59 787 0 0,-11-82-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,0-2-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,0 1-56 0 0,-40 37 929 0 0,39-37-879 0 0,1-1-45 0 0,1 0-1 0 0,-2 0 1 0 0,3 0 0 0 0,-2 0 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-2-1 0 0 0,1 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,-1-1 1 0 0,0 0 0 0 0,2 0 0 0 0,-2 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1 0 0 0,2 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-5 0 0,-3-1 0 0 0,0-1 0 0 0,1 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,1-2 0 0 0,0 2 0 0 0,3 0 0 0 0,-4-1 0 0 0,3 0 0 0 0,-3 0 0 0 0,2 0 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-3-4 0 0 0,5-17-5381 0 0,0 16-2125 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="70961.788">9574 351 0 0 0,'-12'11'0'0'0,"8"-14"140"0"0,1 3 2586 0 0,3 0 5496 0 0,14 21-7158 0 0,-13-20-552 0 0,7 30 3000 0 0,-12 31-1947 0 0,0 50 181 0 0,4 2 624 0 0,-6-41-881 0 0,9 38-1316 0 0,-10-27-173 0 0,7-44 0 0 0,13 4-2476 0 0,-11-41 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1 0 0 0,2 1-1 0 0,-2-1 1 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1-2-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,0-1 1 0 0,0 1 0 0 0,-2 0-1 0 0,2-1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="71766.961">9558 782 4376 0 0,'0'0'199'0'0,"8"-10"1918"0"0,-4-4 1016 0 0,10-8 683 0 0,-6-15-1297 0 0,-1 0-472 0 0,4 30-1272 0 0,-8 6-743 0 0,-2 0 0 0 0,1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,2 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,0 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 2-33 0 0,4-1 304 0 0,20 20 598 0 0,-23-14-674 0 0,1-1-1 0 0,-2 0 1 0 0,1 2 0 0 0,-1-2-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-2-1 0 0,2 7-227 0 0,5 93 608 0 0,-6-66-165 0 0,-1-11 997 0 0,25-2-1275 0 0,-6-27-165 0 0,8-1 0 0 0,10-10-60 0 0,-17 0-2985 0 0,-17 9-1180 0 0,-6 1 2595 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="73476.329">10146 656 2760 0 0,'0'1'207'0'0,"0"44"6763"0"0,0-44-5925 0 0,0-1-21 0 0,2 9 598 0 0,2 11-344 0 0,-3 1 0 0 0,1 0 1 0 0,-2 1-1 0 0,0-1 1 0 0,-1-1-1 0 0,-1 11-1278 0 0,-13 63 616 0 0,1-19 973 0 0,13 40-2158 0 0,1-89 962 0 0,-1-24-377 0 0,1-2-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="74025.376">10206 648 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-2-81 0 0,53-23 1867 0 0,-50 26-2559 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,2 1 0 0 0,-2 0 0 0 0,-1 1 0 0 0,2-1-1 0 0,0 1 1 0 0,-2 0 0 0 0,2 1-156 0 0,-1 1 96 0 0,3-1-1 0 0,-3 0 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,-1 2-1 0 0,2 0 1 0 0,-1-2-1 0 0,0 1 1 0 0,-1 1-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 1-95 0 0,-2-1 94 0 0,0 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-2-1 0 0,0 1 1 0 0,0 0 0 0 0,0 2 0 0 0,-1-2-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0-1 0 0 0,-4 5-94 0 0,-40 58 1952 0 0,44-67-2012 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-2-1 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0-3 59 0 0,2 5-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128695.154">5544 1488 4144 0 0,'0'0'319'0'0,"-6"7"1871"0"0,1-2 3495 0 0,-25-2-688 0 0,1-4-2621 0 0,1-15 488 0 0,-15 7-1852 0 0,-8-1 1272 0 0,-22-15-812 0 0,2 6-939 0 0,0 2 998 0 0,-4-1-1171 0 0,-9 12-360 0 0,-109 12 1824 0 0,104 8-1887 0 0,36-9 230 0 0,-31-9-256 0 0,6-7 82 0 0,13 8 87 0 0,23 3-80 0 0,-71-13 0 0 0,48-3 0 0 0,-8 7 0 0 0,46 1 0 0 0,13 6-60 0 0,11 2-440 0 0,4 6-11674 0 0,-1-5 3997 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129337.391">4157 1155 8288 0 0,'0'2'227'0'0,"-1"-1"0"0"0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,2 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,0 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-3 0 0 0 0,2-1 0 0 0,0 1-227 0 0,-19 1 2894 0 0,14 2-2512 0 0,-1 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,1 1 0 0 0,-7 5-381 0 0,-2 4 422 0 0,-14 13 408 0 0,-35 33 222 0 0,16-4-867 0 0,44-31 92 0 0,2-23-266 0 0,0-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,-1 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-2-1-1 0 0,3 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-11 0 0,24 11 26 0 0,90 21-304 0 0,-44-10-3852 0 0,-20 7-1623 0 0,-37-15 3707 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="133691.162">5674 3790 6448 0 0,'0'0'141'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 50 0 0,0 0 161 0 0,0 0 76 0 0,0 0 15 0 0,0 0 9 0 0,0 0 34 0 0,0 0 20 0 0,0 0 2 0 0,0 0 73 0 0,0 0 308 0 0,0 0 135 0 0,0 0 27 0 0,0 0-38 0 0,0 0-189 0 0,0 0-85 0 0,-9 0 710 0 0,-65 11 2232 0 0,-96-9 113 0 0,71-16-2111 0 0,95 12-1711 0 0,0-1 0 0 0,0 2-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,1 1-1 0 0,-3-1 1 0 0,2 1 0 0 0,0 0-1 0 0,-1 0-7 0 0,0 0 3 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,-2-1 1 0 0,3 1 0 0 0,0 0 0 0 0,-5-1-3 0 0,-3-1 53 0 0,-53 16 746 0 0,-5-33-422 0 0,-42 19 95 0 0,18 18-267 0 0,-2-28 255 0 0,18 8-262 0 0,-6-6 515 0 0,24 23-785 0 0,-8-10 316 0 0,67-3-237 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-2 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 2 1 0 0,0-2-1 0 0,-1 1 0 0 0,2 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 0 0 0,-1 0-7 0 0,0 0-480 0 0,0-1-257 0 0,0 0-51 0 0,0 0-42 0 0,0 0-130 0 0,0 6-384 0 0,1-1-2483 0 0,-1-5 1589 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="134078.302">4508 3526 12384 0 0,'-12'-11'1277'0'0,"-3"9"-438"0"0,-14 9 3998 0 0,9 3-3431 0 0,-21 14 690 0 0,-47 38-1014 0 0,24-28 402 0 0,5 19-1322 0 0,34-25-154 0 0,-10 15 872 0 0,32-41-855 0 0,2 1 0 0 0,-1 1 0 0 0,0 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1-1 0 0,1 2 1 0 0,-1-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,0 1 1 0 0,0-2 0 0 0,0 1 0 0 0,1-2 0 0 0,-2 2 0 0 0,1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-2-1 0 0,0 3-23 0 0,36 40 389 0 0,-27-37-394 0 0,0 0 1 0 0,2 1-1 0 0,-1-2 0 0 0,0-1 0 0 0,0-1 1 0 0,1 2-1 0 0,0-3 0 0 0,1 0 0 0 0,-1-1 1 0 0,0-1-1 0 0,6 0 4 0 0,-6 0-173 0 0,98 18-1371 0 0,-40 3-4118 0 0,-54-16-1845 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136187.119">3715 2871 2760 0 0,'9'14'125'0'0,"-22"-7"1798"0"0,-7 10-59 0 0,16-10 428 0 0,-25 6 4862 0 0,29-13-6578 0 0,0 0-15 0 0,0 0-34 0 0,-1 2 119 0 0,0-1-159 0 0,1-1 2989 0 0,53-16-1901 0 0,10 9-396 0 0,20 3-749 0 0,-22 1 156 0 0,38-2 469 0 0,22-3-497 0 0,-4-3-454 0 0,51-4 952 0 0,-48 9-543 0 0,-49-4-402 0 0,51-9 402 0 0,-66 8-745 0 0,3 11 112 0 0,-30-7 120 0 0,14 5 0 0 0,6-13 444 0 0,-24 3-280 0 0,14 1-164 0 0,-24 4 0 0 0,-6 6 0 0 0,19 6-1208 0 0,-27-4 877 0 0,7 3-1583 0 0,6 13-3659 0 0,-8-11 3847 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="136591.973">5140 2410 920 0 0,'0'7'67'0'0,"0"-1"355"0"0,0-5 1704 0 0,9 23 9129 0 0,22-6-7935 0 0,-17-12-2328 0 0,57 30 1337 0 0,-55-23-2420 0 0,-8-7 346 0 0,2 0 1 0 0,0 2-1 0 0,-1 0 1 0 0,-1 0-1 0 0,-1 2 1 0 0,2-1-1 0 0,-3 0 1 0 0,2 2-1 0 0,3 6-255 0 0,7 69 1080 0 0,-25-5-224 0 0,-12-28-856 0 0,-26-2 327 0 0,-26-12 1242 0 0,7-14-2553 0 0,37-24-3117 0 0,22-1 2058 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="139663.3298">11352 2932 8288 0 0,'10'-47'864'0'0,"-12"44"-720"0"0,4-10 1811 0 0,0 10 5703 0 0,59-2-3242 0 0,-23 5-4222 0 0,75 2 1838 0 0,4 9-1085 0 0,261-14 1101 0 0,-164-2-1030 0 0,-72 10-540 0 0,38-2-45 0 0,11-14 803 0 0,-42-20-1236 0 0,-144 29-64 0 0,-5 2-273 0 0,22-10-2694 0 0,-20 10 2502 0 0,8 0-15 0 0,-6 4-3511 0 0,1 2-4432 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="140326.574">13036 2493 8288 0 0,'0'0'638'0'0,"0"1"-414"0"0,-2 2-28 0 0,2-3 686 0 0,0 0 288 0 0,0 0 57 0 0,0 0-50 0 0,0 0-255 0 0,0 0-112 0 0,0 0-18 0 0,6 6 488 0 0,66 16 2067 0 0,-40-16-2223 0 0,48 24 954 0 0,-50-9-1577 0 0,41 38 370 0 0,-19 1-375 0 0,29 34 240 0 0,-78-91-712 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0 1-1 0 0,1 0 1 0 0,-1-1-1 0 0,-1 0 0 0 0,2 1 1 0 0,-3 0-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 2-23 0 0,-5 3 44 0 0,0 0 1 0 0,1-1-1 0 0,-2 1 0 0 0,1-1 0 0 0,-1-1 1 0 0,0 2-1 0 0,0-2 0 0 0,-1-1 0 0 0,0 2 0 0 0,-1-2 1 0 0,1-1-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,-1-2 0 0 0,0 0-44 0 0,-25 11 59 0 0,1-2-1 0 0,-1-2 1 0 0,-1-1 0 0 0,-1-2-1 0 0,2-2 1 0 0,-18-1-59 0 0,28-4-59 0 0,-70-9-1395 0 0,84 2-1171 0 0,10 6 1267 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="151416.768">14095 2612 3224 0 0,'0'0'355'0'0,"0"0"279"0"0,0 0 125 0 0,0 0 29 0 0,0 0 0 0 0,0 0-16 0 0,0 0-4 0 0,0 0 0 0 0,0 0-50 0 0,0 0-207 0 0,0 0-95 0 0,0 0-21 0 0,0 0-14 0 0,0 0-44 0 0,0 0-17 0 0,0 0-6 0 0,0 0 8 0 0,0 0 45 0 0,-12 7 790 0 0,-12 11 150 0 0,-47 20 1099 0 0,6-3-1196 0 0,62-33-1165 0 0,-12 9 158 0 0,0 1 0 0 0,1 0-1 0 0,0 1 1 0 0,1 0 0 0 0,1 0 0 0 0,0 3 0 0 0,0 0 0 0 0,1-1-1 0 0,-6 12-202 0 0,14-22 65 0 0,0 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 2 1 0 0,3-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 0 1 0 0,1 2-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0 0-64 0 0,1 1 108 0 0,1 1 0 0 0,-1 0-1 0 0,1-2 1 0 0,0 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,2 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0-2 1 0 0,1 2 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-2 0 0 0,0 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 0-1 0 0,9 2-107 0 0,-5-1 42 0 0,-1-2-1 0 0,1-1 0 0 0,0 0 0 0 0,-1-1 1 0 0,1 0-1 0 0,1-1 0 0 0,-2 0 0 0 0,9-3-41 0 0,21-17-4007 0 0,-34 13-3607 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="152065.555">14272 2957 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-96 0 0,0 0 287 0 0,0 0 142 0 0,0 0 27 0 0,0 0-27 0 0,-4-10 655 0 0,4 4-930 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-2 3 0 0 0,1-2 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,-1 0 0 0 0,2-1 0 0 0,0 1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 0 0 0,2-1-345 0 0,-5 2 74 0 0,0 0 0 0 0,-1 0-1 0 0,2 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,2 2-1 0 0,-2-1 1 0 0,0 1 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 1-1 0 0,1-1 1 0 0,-4 0 0 0 0,3 1-1 0 0,0-1 1 0 0,-1 2 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,1-1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,0 2-73 0 0,2 5 95 0 0,-1-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,0 0 0 0 0,-2-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1 8-95 0 0,-12 72 1049 0 0,11-84-938 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1-2-1 0 0,0 2 0 0 0,0-1 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-111 0 0,1-3 23 0 0,0 0 0 0 0,3 0 0 0 0,-4 0 1 0 0,2-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-24 0 0,-1-1-63 0 0,-1-1 1 0 0,1 1-1 0 0,1-1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 2 1 0 0,0-2-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,2 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,-2-1-1 0 0,1 1 1 0 0,1-2-1 0 0,0 2 1 0 0,0 0-1 0 0,0-6 63 0 0,6-24-2404 0 0,-4 18 1056 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153048.506">14753 2627 0 0 0,'-3'-7'-1709'0'0,"1"-4"9298"0"0,3 10 1867 0 0,-1 12-7849 0 0,4 104 2619 0 0,-7-26-3124 0 0,6 9 60 0 0,-7 41-1060 0 0,12-68-102 0 0,-5-65-68 0 0,-2-5-286 0 0,-1-1-130 0 0,0 0-27 0 0,0 0-212 0 0,0 0-857 0 0,0 0-373 0 0,0-1-79 0 0,3-1-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="153375.191">14732 2847 2304 0 0,'0'0'464'0'0,"4"-8"3648"0"0,-3 5 1786 0 0,26-41-750 0 0,11 3-2447 0 0,5 13-1313 0 0,-23 32-788 0 0,-18-4-482 0 0,0 1-42 0 0,3 2-30 0 0,0 2 0 0 0,-1-2 1 0 0,1 1-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,-1 2-1 0 0,2-2 0 0 0,-1 1 1 0 0,-2 0-1 0 0,1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,-1 1-46 0 0,24 89 1079 0 0,-14-67-711 0 0,-10-14-53 0 0,20 65 642 0 0,0-37-721 0 0,11-30-183 0 0,35-40-1154 0 0,-25-3-4448 0 0,-31 23 3543 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160253.3029">15457 2446 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-119 0 0,0 0 199 0 0,0 0 103 0 0,0 0 17 0 0,0 0 13 0 0,0 0 30 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-3 0 0,0 0-10 0 0,0 0-3 0 0,0 0 0 0 0,0 0-14 0 0,0 0-56 0 0,0 0-30 0 0,0 0-5 0 0,0 0-5 0 0,0 0-28 0 0,0 0-7 0 0,0 0-6 0 0,0 0-14 0 0,0 0-55 0 0,0 0-20 0 0,0 0-7 0 0,5 2 583 0 0,-1-7-849 0 0,-4 4 60 0 0,0 1 17 0 0,0 0-12 0 0,0 0-2 0 0,1 5 2437 0 0,-2 16-2962 0 0,1 60 539 0 0,-6 69 472 0 0,-6 15 1084 0 0,9 79-784 0 0,10-193-592 0 0,1-25-84 0 0,12-18 3 0 0,-14-9-156 0 0,0 0 0 0 0,-1-1 0 0 0,2 0 0 0 0,-2 0 0 0 0,0-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-2-1 0 0 0,2 0 0 0 0,-2 1 0 0 0,1-1 0 0 0,3-3-35 0 0,45-41 80 0 0,-40 36-172 0 0,-7 7-92 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-2 0 0 0,-2-1 0 0 0,3 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,2-4 184 0 0,2 1-1288 0 0,-2-9-6336 0 0,-3 12 565 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="160816.746">15460 2669 8120 0 0,'0'0'366'0'0,"0"0"1"0"0,0 0-66 0 0,0 0 591 0 0,0 0 284 0 0,0 0 59 0 0,0 0-42 0 0,1 0-222 0 0,59-5 2910 0 0,-43 4-3513 0 0,7 0-489 0 0,-9 4-4783 0 0,-5 1-1037 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="165875.957">15942 2692 920 0 0,'0'0'324'0'0,"0"0"1025"0"0,4 5 4769 0 0,0 0-4077 0 0,-1 0-1648 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 2 1 0 0,0 1-394 0 0,-6 185 4855 0 0,1-69-3199 0 0,1-92-1224 0 0,4-10-3265 0 0,0-14 1400 0 0,0-7-5540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="166400.987">15978 2929 456 0 0,'2'-11'295'0'0,"-1"9"1230"0"0,5-14 4652 0 0,-5 15-4821 0 0,8-16 3233 0 0,-3 7-3731 0 0,18-35 2412 0 0,-22 43-3133 0 0,-1-1-1 0 0,1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 1 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 1 0 0,2 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 0-137 0 0,38 1 1322 0 0,-38 1-1262 0 0,2 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0 1 0 0,-3 1-1 0 0,2-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 1-1 0 0,1 1-59 0 0,20 19 91 0 0,-7 2-240 0 0,-16-25-597 0 0,-1-1-214 0 0,0 0-813 0 0,0 0-3268 0 0,0 0-1396 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167273.982">16438 2994 11976 0 0,'0'0'266'0'0,"-1"-11"668"0"0,0 6-605 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-2-1 1 0 0,2 1-1 0 0,0 1 0 0 0,2-1 0 0 0,-2 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,1 3-1 0 0,0-2 0 0 0,2 1 0 0 0,-3-1 0 0 0,2 1 0 0 0,2-4-329 0 0,11-26 1366 0 0,20-3-185 0 0,-33 36-1119 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,3 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,1 2-62 0 0,45 65 531 0 0,-44-54-291 0 0,3-1-1 0 0,-3 1 1 0 0,1 2 0 0 0,-2-2-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 1-1 0 0,-2 10-239 0 0,-6 40 0 0 0,-13-23 1095 0 0,1-46-406 0 0,13 2-606 0 0,2 1-72 0 0,-2 0 0 0 0,1-1 0 0 0,1 1-1 0 0,-2-1 1 0 0,1-1 0 0 0,2 1 0 0 0,-3-1 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-2-2-11 0 0,1 0-209 0 0,2 1 0 0 0,-2-1-1 0 0,2 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1-2 0 0 0,0 2-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,0-6 209 0 0,0-20-4042 0 0,2 15-3529 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="167927.933">16918 2366 1376 0 0,'0'0'367'0'0,"0"0"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,0 0-28 0 0,0 0-86 0 0,0 0-38 0 0,0 0-8 0 0,0 0-41 0 0,0 0-161 0 0,0 0-68 0 0,0 0-18 0 0,3 9 590 0 0,11 65 2596 0 0,-20 149-2669 0 0,-2-75 14 0 0,8 84-1117 0 0,4-180 0 0 0,-2-47-165 0 0,0-4-698 0 0,-2-1-315 0 0,1-1-1352 0 0,1-5-5157 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="189572.02">17199 2906 3568 0 0,'21'-11'1553'0'0,"-7"-5"1718"0"0,-2 11-2487 0 0,40-33 3450 0 0,-25 10-3218 0 0,33-43-474 0 0,-49 47-542 0 0,-9 16 0 0 0,-4-2 0 0 0,1 7-7 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 2 0 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,3 0 0 0 0,-2 0 0 0 0,-1 1 0 0 0,1 0 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,-1 1 1 0 0,1-2-1 0 0,-1 2 0 0 0,0-1 0 0 0,2 1 1 0 0,-5 0 6 0 0,1 3 11 0 0,-2-2 1 0 0,1 2-1 0 0,0-1 1 0 0,0 1-1 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 2 1 0 0,0-1-1 0 0,0 2 1 0 0,-3 4-12 0 0,-14 25 272 0 0,-6 56 161 0 0,26-86-291 0 0,1 0-1 0 0,-1 1 1 0 0,2 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0-1 0 0 0,0 2 0 0 0,1-2-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-2 1 1 0 0,3-1 0 0 0,-1 0-1 0 0,0-1 1 0 0,1 2 0 0 0,-1-2 0 0 0,1 0-1 0 0,0 0 1 0 0,2-1 0 0 0,-3 0-1 0 0,2 1 1 0 0,1-1 0 0 0,-2 0 0 0 0,2-1-1 0 0,-1 1 1 0 0,1-1-142 0 0,-1-1 13 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,0-1 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-2 0 0 0,2 1-13 0 0,65-24-2033 0 0,-59 15 586 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190134.967">17641 2619 6048 0 0,'0'0'273'0'0,"0"0"-5"0"0,-1 1-172 0 0,-16 54 5027 0 0,10-28-3083 0 0,-7 34 478 0 0,11-52-2198 0 0,1 2 0 0 0,0 2 0 0 0,1-2 0 0 0,0 1-1 0 0,1-1 1 0 0,0 0 0 0 0,1 1 0 0 0,2 6-320 0 0,-2 25 797 0 0,-1-37-713 0 0,1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,1-2-1 0 0,-2 1 1 0 0,2-2 0 0 0,1 1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,6 3-83 0 0,-7-7 16 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 1 0 0,1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,-2-1 0 0 0,2 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 0 0 0,-2 0 1 0 0,1-1-1 0 0,1-2-15 0 0,5-5 20 0 0,18-32 87 0 0,13-40-97 0 0,-34 74-49 0 0,0 0 0 0 0,-1 0-1 0 0,-1-1 1 0 0,2 0 0 0 0,-3 0-1 0 0,1 1 1 0 0,-1-2 0 0 0,0 1-1 0 0,0 0 1 0 0,-1-6 39 0 0,-4-22-1383 0 0,4 36 837 0 0,-1 0-1200 0 0,-6-5-4721 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192408.343">16355 2446 3224 0 0,'0'0'143'0'0,"0"0"258"0"0,0 0 983 0 0,0 0 432 0 0,0 0 82 0 0,0 0-92 0 0,0 0-468 0 0,0 0-200 0 0,0 0-40 0 0,0 0-78 0 0,1-1-292 0 0,5-4-365 0 0,3-2-1 0 0,-3 0 1 0 0,0 0 0 0 0,2-1-1 0 0,-3 1 1 0 0,1-2 0 0 0,-1 1-1 0 0,0 0 1 0 0,1-1-363 0 0,46-77 852 0 0,-37 69-781 0 0,-1 15-61 0 0,-10 6 2 0 0,-1 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,-1 1 0 0 0,1 1-1 0 0,0-2 1 0 0,0 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,-2-1-1 0 0,1 2-11 0 0,2 3-4 0 0,7 24 57 0 0,0-3-53 0 0,6 0-1856 0 0,-9-24-4807 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="211829.3868">7577 2679 7256 0 0,'0'0'330'0'0,"0"0"-7"0"0,-11-2-24 0 0,7 2 8851 0 0,1 5-9133 0 0,-8 14-17 0 0,6-15-769 0 0,4-3-3236 0 0,1-1-1404 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-211952.6539">19576 2991 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,0 0-50 0 0,0 0 614 0 0,0 0 288 0 0,0 0 57 0 0,0 0-53 0 0,0 0-253 0 0,0 0-115 0 0,0 0-20 0 0,0 0-112 0 0,-8 0-423 0 0,2-2-329 0 0,4 2-272 0 0,0-3-398 0 0,0-1-3749 0 0,-3-9 2451 0 0,4 11-14 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-212149.5859">19309 2713 920 0 0,'0'0'288'0'0,"0"0"873"0"0,0 0 383 0 0,0 0 79 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-32 0 0,0 0-104 0 0,0 0-46 0 0,0 0-10 0 0,-13-3 2088 0 0,-5-5-821 0 0,16 8-1285 0 0,-12 4 543 0 0,-32 27 578 0 0,-5 49-1009 0 0,51-72-646 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 2 0 0 0,1-2 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,3 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 2 0 0 0,0-2 0 0 0,3 0 0 0 0,-3-1 0 0 0,2 3-74 0 0,25 23 398 0 0,-27-30-397 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,2-1-1 0 0,6 1-134 0 0,-7-1-167 0 0,-1 0-1 0 0,1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-3-1 0 0,-2 2 1 0 0,1 0 301 0 0,-4 2-105 0 0,14-8-1239 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205932.193">19777 2754 1376 0 0,'0'0'65'0'0,"0"0"253"0"0,0 0 1036 0 0,0 0 454 0 0,0 0 89 0 0,0 0-99 0 0,0 0-502 0 0,0 0-220 0 0,0 0-42 0 0,6 9 1656 0 0,-5-7-2461 0 0,0 1 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 2 0 0 0,-1-2 1 0 0,0 0-1 0 0,-1 2-229 0 0,2 74 2716 0 0,18 162 1049 0 0,-28-75-3749 0 0,-1-94-16 0 0,-3 22 0 0 0,13-89-64 0 0,1-3-273 0 0,0-2-138 0 0,0 0-33 0 0,0 0-169 0 0,0 0-696 0 0,0 0-311 0 0,0 0-63 0 0,0 0 48 0 0,0 0 252 0 0,0 0 109 0 0,0 0-360 0 0,0 0-1612 0 0,0 0-692 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-205389.214">19805 2830 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,0 0-143 0 0,0 0 329 0 0,0 0 174 0 0,0 0 40 0 0,0 0-17 0 0,0 0-87 0 0,4-7 616 0 0,20-28 2026 0 0,-3 17-2035 0 0,-18 17-1214 0 0,-2-1 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-3-1 0 0 0,1 1 0 0 0,0-2 0 0 0,1 2 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,2 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,0 0-84 0 0,3 5 138 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,-1 2 0 0 0,1-2 0 0 0,-1 1 1 0 0,1 0-1 0 0,-3 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,2 0 0 0 0,-4 0 0 0 0,2 0 0 0 0,-1 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-2 0 0 0,-1 1 1 0 0,0 1-1 0 0,0-1 0 0 0,0-1 0 0 0,-4 8-137 0 0,5-13 22 0 0,0 1-1 0 0,-1-2 0 0 0,1 1 1 0 0,-1 0-1 0 0,-1 1 1 0 0,2-1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0-1 1 0 0,-2 1-1 0 0,1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1-1 1 0 0,-2 0-1 0 0,1-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0-21 0 0,-36 10 162 0 0,35-11-192 0 0,2 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1-1-1 0 0,-4-1 30 0 0,-13-33-3512 0 0,16 24 1769 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-204187.105">20249 2569 2760 0 0,'0'0'120'0'0,"0"0"32"0"0,0 0-152 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 120 0 0,0 0-8 0 0,0 0 0 0 0,0 0-1000 0 0,0 0-200 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203902.979">20230 2544 2240 0 0,'0'0'0'0'0,"0"0"96"0"0,0 0-24 0 0,0 0-8 0 0,0 0-64 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203901.979">20216 2652 864 0 0,'0'0'0'0'0,"0"0"0"0"0,0 0 0 0 0,0 0 72 0 0,0 0-72 0 0,0 0 0 0 0,0 0 0 0 0,0 0-368 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-203439.752">20185 2456 5040 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 13 0 0,0 0 43 0 0,0 0 137 0 0,0 0 60 0 0,0 0 7 0 0,0 0 22 0 0,0 0 69 0 0,0 0 32 0 0,0 0 4 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,3 11 2392 0 0,14 81 1583 0 0,-16 35-1639 0 0,9 44-192 0 0,11-22-2656 0 0,-24-130 0 0 0,0-3-337 0 0,2-14-1422 0 0,1-2-638 0 0,0 0-130 0 0,0 0-28 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-202468.8889">20219 2884 920 0 0,'0'-6'80'0'0,"0"0"65"0"0,-2-18 3737 0 0,5-3 4077 0 0,8-23-4186 0 0,7 2-1366 0 0,-2 20-2142 0 0,-8 20-211 0 0,-8 7 222 0 0,19-10 1281 0 0,8 13-1444 0 0,-24 0-105 0 0,44 32-8 0 0,-22-3 744 0 0,-11-4-56 0 0,6 35-96 0 0,-12-20-16 0 0,2 12 191 0 0,1-19-526 0 0,-2-4-59 0 0,-1-16-12 0 0,-7-14-90 0 0,17 3 16 0 0,17-2-96 0 0,-8-4-141 0 0,-26 2-596 0 0,27-11-4249 0 0,-15 5 1073 0 0,-8 2 1923 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201801.05">20792 2679 1376 0 0,'-15'6'65'0'0,"11"-5"277"0"0,4-1 1138 0 0,0 0 500 0 0,0 0 99 0 0,-6 11 5285 0 0,12 46-3424 0 0,-9-9-2068 0 0,-2 47 541 0 0,-4-52-877 0 0,5 2-432 0 0,5 22-1088 0 0,8 9 915 0 0,-4-4-416 0 0,-2-59-545 0 0,-5 18 164 0 0,-3-11-45 0 0,4-19-557 0 0,1-1-39 0 0,0 0 65 0 0,0 0 152 0 0,0 0-451 0 0,-4 0-797 0 0,2 0-5332 0 0,2 0 728 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-201246.613">20747 2729 456 0 0,'32'-10'12581'0'0,"-20"4"-11549"0"0,14 5 3076 0 0,-1-5-1928 0 0,28 40 262 0 0,-18 0-1426 0 0,-10 19-48 0 0,-9-19-336 0 0,-16-30-440 0 0,-3 28-53 0 0,-7-10-60 0 0,-8-8 791 0 0,17-12-867 0 0,1-1 1 0 0,-3 1-1 0 0,3-1 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 1 1 0 0,2-1 0 0 0,-3 0-1 0 0,1 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,1 2 1 0 0,-2-2 0 0 0,2 0-1 0 0,-1 0 1 0 0,0-2-1 0 0,-2 2-3 0 0,-35-21-1713 0 0,14-2-2008 0 0,21 16 1827 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190828.747">18024 2644 3680 0 0,'0'0'284'0'0,"0"0"75"0"0,0 0 1008 0 0,0 0 464 0 0,0 0 90 0 0,0 0-127 0 0,3 15 1120 0 0,0 36 395 0 0,1 70 75 0 0,3-40-2940 0 0,5 7-252 0 0,-5-12-192 0 0,1-39-12 0 0,-8-35-53 0 0,0-2-166 0 0,0 0-558 0 0,0 0-239 0 0,0 0-1104 0 0,0 0-4234 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="191215.919">18038 2808 12528 0 0,'0'0'281'0'0,"0"0"40"0"0,0 0 22 0 0,0 0-39 0 0,0 0-107 0 0,4-14 2209 0 0,11-4-1077 0 0,30-21 345 0 0,-17 31-1146 0 0,-6 23-314 0 0,-17-12-177 0 0,-1 1 0 0 0,1 0-1 0 0,-2 2 1 0 0,2-2 0 0 0,-1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-37 0 0,-1-3 176 0 0,9 10 413 0 0,-9-12-998 0 0,10 6-4069 0 0,-11-7 3075 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="199554.903">18346 3115 5096 0 0,'0'0'108'0'0,"0"0"17"0"0,0 0 14 0 0,0 0 77 0 0,0 0 257 0 0,0 0 115 0 0,0 0 20 0 0,0 0 8 0 0,0 0 7 0 0,0 0 1 0 0,0 0 0 0 0,0 0-19 0 0,0 0-77 0 0,0 0-31 0 0,0 0-7 0 0,0 0-42 0 0,0 0-170 0 0,0 0-76 0 0,0 0-12 0 0,0 0 13 0 0,7-4 224 0 0,-5 3 3136 0 0,9-10-3493 0 0,-9 8-76 0 0,-1 6-128 0 0,-1-1-240 0 0,0-2-71 0 0,0 0-1004 0 0,0 0-3980 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-174270.903">18726 2754 2096 0 0,'0'0'99'0'0,"0"0"35"0"0,0 0 110 0 0,0 0 48 0 0,0 0 11 0 0,0 0-11 0 0,0 4-485 0 0,0 13 8138 0 0,-3 36-5693 0 0,3-51-1919 0 0,-3 17 1214 0 0,-1 79 988 0 0,4-96-2320 0 0,0-2-72 0 0,0 8 75 0 0,-5 26-43 0 0,-1 45-122 0 0,6-76-45 0 0,0 0-235 0 0,0 0-3512 0 0,0-3-1706 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-173620.241">18711 2899 5296 0 0,'5'7'472'0'0,"-5"-1"-294"0"0,0-5 493 0 0,0-1 202 0 0,0 0 30 0 0,0 0-18 0 0,0 0-105 0 0,0-23 1372 0 0,0 21-1542 0 0,0 0-40 0 0,6-29 954 0 0,-5 30-1144 0 0,12-28 1755 0 0,4 10-1413 0 0,-15 18-538 0 0,-2 1 0 0 0,0 0-6 0 0,14-2 374 0 0,-8 3-368 0 0,-4-1-159 0 0,-1 0 0 0 0,1 0-1 0 0,1 0 1 0 0,-3 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-2 0 0 0 0,3 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,0 0 0 0 0,2 1-1 0 0,-3-1 1 0 0,1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,2 1 0 0 0,-2-1-1 0 0,1 1-24 0 0,13 61 908 0 0,-10-27-544 0 0,-5-12-78 0 0,1-23-204 0 0,0 21 170 0 0,1-18-204 0 0,2 4-36 0 0,1-1-1 0 0,-1 1 42 0 0,4-3 13 0 0,-4-4-58 0 0,1 0 1 0 0,-2 0 0 0 0,0-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,3 1 0 0 0,-2-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-3 1 0 0 0,2-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0-1 0 0,1 0 1 0 0,2-3-9 0 0,33-23-3222 0 0,-33 21-430 0 0,-3 6 1775 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="-165827.57">13168 3625 920 0 0,'0'0'411'0'0,"0"0"1389"0"0,0 0 609 0 0,0 0 119 0 0,0 0-215 0 0,0 0-1014 0 0,0 0-445 0 0,0 0-87 0 0,0 0-46 0 0,0 0-109 0 0,0 0-48 0 0,0 0-10 0 0,0 0 0 0 0,0 0 11 0 0,-14-2 1750 0 0,-6-1-885 0 0,-2-1-1 0 0,1 3 1 0 0,0 0-1 0 0,0 1 1 0 0,-13 2-1430 0 0,-38 10 1057 0 0,-24-11-2 0 0,30-4-630 0 0,-79 0 196 0 0,32-8-298 0 0,35-8 8 0 0,65 14-305 0 0,0 2-1 0 0,0 0 1 0 0,0 1 0 0 0,0 1 0 0 0,0 0 0 0 0,-2 0 0 0 0,1 2 0 0 0,2 0 0 0 0,-1 0-1 0 0,-5 2-25 0 0,-43 13 22 0 0,12-7 31 0 0,10-13 11 0 0,-74-2 64 0 0,54 28-128 0 0,-20 0 0 0 0,43-21 0 0 0,-10-5 0 0 0,-22 7 0 0 0,37 4 0 0 0,-12-14 0 0 0,-3-24 0 0 0,-7 29 0 0 0,4-3 0 0 0,33 3-632 0 0,14 1 769 0 0,-1 1-984 0 0,3 0-6440 0 0,6-2 5260 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-62540.216">5814 244 9240 0 0,'0'0'208'0'0,"0"0"33"0"0,0 0 14 0 0,0 0 69 0 0,0 0 284 0 0,0 0 120 0 0,0 0 28 0 0,0 0-30 0 0,0 0-139 0 0,0 0-62 0 0,0 16 1654 0 0,-6 125 2954 0 0,-4 16-3081 0 0,9 59-343 0 0,9 152 170 0 0,1-204-1465 0 0,-9-132-531 0 0,0-30-556 0 0,0-4-270 0 0,-4-26-3089 0 0,2 17 1904 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-50190.827">5783 280 3224 0 0,'0'0'387'0'0,"0"0"414"0"0,0 0 183 0 0,0 0 37 0 0,-11-2 2900 0 0,2 0 1482 0 0,6 5 686 0 0,19 7-5649 0 0,80-9 731 0 0,-32-11-391 0 0,65 6-160 0 0,47-5-302 0 0,-66-4-104 0 0,24 8 148 0 0,-6 3 150 0 0,-11 2-320 0 0,23 3-48 0 0,-25 4 171 0 0,61 16 58 0 0,-56-9 92 0 0,7-10 14 0 0,-8-12-479 0 0,-43 3 68 0 0,-58 2-39 0 0,-1 2-1 0 0,2 0 1 0 0,-1 1 0 0 0,0 1-1 0 0,1 1 1 0 0,9 2-29 0 0,36 6 0 0 0,30-6 0 0 0,-13 0 0 0 0,-6-1 0 0 0,-37 7 0 0 0,46-3 0 0 0,48-9 0 0 0,-94-1 0 0 0,42 5 0 0 0,-67 1 5 0 0,1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,2 0 0 0 0,-3-1 0 0 0,6-1-5 0 0,61-6 19 0 0,91 23-8 0 0,-100-8 95 0 0,18-6-31 0 0,-15-10-11 0 0,90 0 0 0 0,-78 3 0 0 0,8 1-64 0 0,-43-2 53 0 0,36-2-42 0 0,-43 10-11 0 0,56-4 0 0 0,19 0 0 0 0,-34 16 0 0 0,196-10 0 0 0,-124-19 0 0 0,-80 11 0 0 0,37-2 0 0 0,-25 13 0 0 0,-33 2 0 0 0,26-6 64 0 0,-4-6 128 0 0,58 5-192 0 0,-103 4 0 0 0,0-2 0 0 0,-24-2 0 0 0,-3 0-12 0 0,-4 0-53 0 0,-1 0-170 0 0,0 0-576 0 0,0 0-247 0 0,0 0-49 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-49193.598">11004 195 5928 0 0,'0'0'266'0'0,"0"0"1"0"0,0 1-171 0 0,0 4 92 0 0,0-4 732 0 0,-1 16 4758 0 0,2 13-1191 0 0,9 35 169 0 0,-13-10-3447 0 0,-4 121 1305 0 0,3-62-2021 0 0,-1-8-60 0 0,3 51 591 0 0,9-33-728 0 0,-4-93-284 0 0,-2 2 204 0 0,-1-32-157 0 0,0-1 6 0 0,0 0-26 0 0,0 0-98 0 0,0 0-9 0 0,0 0 4 0 0,0 0 0 0 0,0 0-43 0 0,0 0-179 0 0,0 0-82 0 0,0 0-15 0 0,0 0-98 0 0,0 0-410 0 0,0 0-182 0 0,0 0-42 0 0,0 0-73 0 0,0 0-285 0 0,0 0-126 0 0,0 0-983 0 0,0 0-3823 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-48911.614">10990 1107 456 0 0,'0'0'1737'0'0,"0"0"207"0"0,0 0 88 0 0,0 0-76 0 0,0 0-381 0 0,0 0-174 0 0,0 0-32 0 0,0 0-62 0 0,0 0-231 0 0,0 2-99 0 0,0 77 4474 0 0,5-47-4150 0 0,0 18 250 0 0,-3 2-1349 0 0,-4-23-20 0 0,2-21-172 0 0,0 4 904 0 0,0-12-2338 0 0,0 4-8055 0 0,0-4 3197 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-46458.2109">11014 1343 3224 0 0,'-11'9'2653'0'0,"-39"18"4634"0"0,48-27-6665 0 0,0 0 33 0 0,-45-7 3329 0 0,-34 1 217 0 0,51 7-3372 0 0,-77-2 683 0 0,46-21 54 0 0,30 12-1308 0 0,13 5-82 0 0,2 1 1 0 0,-1 1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 2 0 0 0,0 0 1 0 0,-12 2-177 0 0,-13-1 177 0 0,-40-9 419 0 0,13-2-51 0 0,-58 6 350 0 0,25 11-662 0 0,14 3-169 0 0,12-2-64 0 0,-15-16 140 0 0,-59 7 320 0 0,46 2-460 0 0,7-13 83 0 0,17 0-30 0 0,31 5-53 0 0,-39 2 0 0 0,-60 5 0 0 0,-19-4 0 0 0,74 1 0 0 0,0 5 0 0 0,-43-4 0 0 0,7-5 0 0 0,-138 7 0 0 0,187 4 0 0 0,-35-8 117 0 0,8-9 118 0 0,47 9-410 0 0,-102 8 326 0 0,98-8-162 0 0,-83-1 37 0 0,3 9-289 0 0,9 5 263 0 0,-36 0 208 0 0,64-2-413 0 0,-49-4 194 0 0,36-6 11 0 0,-36 22 344 0 0,72-5-608 0 0,-63 4 160 0 0,73-15 104 0 0,-36-3 968 0 0,14-11-1140 0 0,12 11-113 0 0,24 10 214 0 0,-41-5 71 0 0,70-6-97 0 0,24 2 121 0 0,3-1-4216 0 0,4 0-5767 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-41895.864">5939 2573 5264 0 0,'3'0'1129'0'0,"7"0"-2200"0"0,-7 0 4901 0 0,-2 1 4833 0 0,7 41-6741 0 0,-8 55 512 0 0,-8 20-998 0 0,16 103 1044 0 0,6-76-1600 0 0,-3-45-128 0 0,3 48-792 0 0,-7-70 515 0 0,-7-37 182 0 0,-5-14 138 0 0,1-15-1692 0 0,4-11-2271 0 0,2-8 1285 0 0,-2-1-408 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-39644.648">5903 2576 456 0 0,'0'0'1548'0'0,"0"0"185"0"0,0 0 82 0 0,0 0-101 0 0,0 0-459 0 0,0 0-204 0 0,0 0-41 0 0,0 0-42 0 0,0 0-140 0 0,0 0-57 0 0,0 0-16 0 0,0 0-1 0 0,0 0 12 0 0,0 0 2 0 0,0 0-1 0 0,0 0-47 0 0,0 0-202 0 0,0 0-92 0 0,3 0-11 0 0,47-7 2042 0 0,47 1 147 0 0,66 5-222 0 0,-23 11-1432 0 0,-17-16-175 0 0,134-12 402 0 0,-115-6-820 0 0,-52 7 18 0 0,-52 10-382 0 0,0 2 1 0 0,1 2-1 0 0,30 1 7 0 0,61 2 256 0 0,-87 0-256 0 0,43 0 181 0 0,-22 10-106 0 0,6-4 1 0 0,-2-1 68 0 0,53-2-1 0 0,-75 0-90 0 0,78-4 144 0 0,182-8-122 0 0,-244 13-75 0 0,42 6 0 0 0,21-7 0 0 0,-65 4 0 0 0,-4-2 0 0 0,55-5 0 0 0,16 0 0 0 0,-63 12 0 0 0,-22-5 64 0 0,62-18 0 0 0,-38 0-64 0 0,52-1-67 0 0,40 22 54 0 0,-90-11 13 0 0,-43-2 11 0 0,4 1-1 0 0,-3 1 1 0 0,0 1 0 0 0,1 1-1 0 0,23 4-10 0 0,11-2 11 0 0,73-6-74 0 0,-48-2 30 0 0,46 17 33 0 0,14-1 152 0 0,-87-4-152 0 0,-22-6-172 0 0,42 4 160 0 0,11-5 12 0 0,-26 0 0 0 0,-8-3 0 0 0,-22 3 0 0 0,2 0-16 0 0,-34 0-61 0 0,-2 0-6 0 0,0 0-138 0 0,0 0-595 0 0,0 0-264 0 0,0 0-1739 0 0,0 0-6757 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-38736.343">10621 2525 1376 0 0,'0'0'65'0'0,"0"0"341"0"0,0 0 1404 0 0,0 0 611 0 0,9 0 3921 0 0,-6 1-6029 0 0,-2 0 0 0 0,2-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 3-313 0 0,6 61 2731 0 0,18 123-151 0 0,-14-103-1558 0 0,-15 40 98 0 0,13 25 148 0 0,-3-79-785 0 0,-4-28-243 0 0,-2 26 129 0 0,1 21 111 0 0,-1-57-253 0 0,0-33-205 0 0,0-1-106 0 0,0 0-8 0 0,-18 21-828 0 0,18-21 767 0 0,-11 16-1455 0 0,10-14 1350 0 0,1-2-81 0 0,0 0-40 0 0,0 0-5 0 0,0 0-101 0 0,0 0-426 0 0,0 0-185 0 0,0 0-37 0 0,0 0-102 0 0,0 0-386 0 0,0 0-166 0 0,0 0-32 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36969.387">10698 3563 3224 0 0,'-6'12'5642'0'0,"-8"13"-878"0"0,14-23-3930 0 0,-1-1-138 0 0,-32 28 3385 0 0,-33-15 128 0 0,34-11-2861 0 0,-128 21 765 0 0,108-13-1621 0 0,-98-4 1168 0 0,20-24-712 0 0,-131 3-243 0 0,145 17-482 0 0,-30 1 141 0 0,48-5-364 0 0,-175 8 0 0 0,170 4 0 0 0,-276-8 0 0 0,209 1 228 0 0,-55-32 541 0 0,124 18-750 0 0,-60-4-19 0 0,112 7 0 0 0,26 6 0 0 0,0-2 0 0 0,0-1 0 0 0,0 0 0 0 0,2-2 0 0 0,-8-4 0 0 0,17 7 0 0 0,-36-14 0 0 0,-2 4 0 0 0,1 1 0 0 0,-1 4 0 0 0,1 1 0 0 0,-15 4 0 0 0,-27 5 0 0 0,28 4 0 0 0,-83-8 0 0 0,83-2 0 0 0,-73 7 0 0 0,47 10-21 0 0,4-2-5 0 0,-32-1-287 0 0,82-4 334 0 0,-11-2 286 0 0,-73-10-307 0 0,30-8-103 0 0,2 11-9 0 0,52 6 23 0 0,-3-3 89 0 0,-11 13 0 0 0,-55 6 73 0 0,51-10-143 0 0,3-2 403 0 0,5-9-333 0 0,16 4 0 0 0,-15-4-32 0 0,45 2-137 0 0,-2 9-3011 0 0,2-6 1857 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1488.941">13615 2236 3224 0 0,'0'0'389'0'0,"0"0"426"0"0,0 0 185 0 0,0 0 37 0 0,0 0-41 0 0,0 0-211 0 0,8 14 2921 0 0,0 2-2586 0 0,-7-15-544 0 0,-1 0 0 0 0,15 148 6159 0 0,-23 7-3759 0 0,6-42-1768 0 0,4 59 608 0 0,2 46-811 0 0,21 107 755 0 0,-11-185-1237 0 0,-7 22-2562 0 0,-7-173-744 0 0,0-5-6530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="854.454">13609 2192 3224 0 0,'-4'-1'-2321'0'0,"1"-2"3355"0"0,-5-4 11775 0 0,11 5-10726 0 0,-2 1-1175 0 0,-1 1-164 0 0,11-3 590 0 0,113 16 3826 0 0,131-6-1952 0 0,-1 0-2760 0 0,-72-11 16 0 0,-43-9 16 0 0,45-11 88 0 0,-25 6-187 0 0,40 4-162 0 0,-32 2-75 0 0,35-3 144 0 0,-7 1-149 0 0,-43 4-22 0 0,62-7-205 0 0,-6 11 211 0 0,55 5 714 0 0,-29 8-953 0 0,39 10-59 0 0,-159-4 482 0 0,5-9-635 0 0,-9 0 267 0 0,80 20 74 0 0,-29-4-13 0 0,21 1-88 0 0,16-11 152 0 0,12-10-64 0 0,-74-3 0 0 0,-41-4 0 0 0,161-3 0 0 0,-112 7 0 0 0,73 2 0 0 0,-136 11 0 0 0,70-3 0 0 0,-11 0 0 0 0,-57 8 0 0 0,55 6 0 0 0,-84-10 0 0 0,54 1 0 0 0,37-1 0 0 0,9 2 0 0 0,-72-6 400 0 0,-6 0-480 0 0,72-11 133 0 0,-14 1-106 0 0,-100 3 53 0 0,56-1-64 0 0,-20-5 64 0 0,-20 3 11 0 0,70 1 375 0 0,-62-14-452 0 0,-27 9 108 0 0,34-3-95 0 0,-39 10 53 0 0,-26 20-245 0 0,-2-17 238 0 0,2-3 7 0 0,-2 0 0 0 0,2 1-1 0 0,0-1 1 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1-1 0 0,-2 1 1 0 0,2-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 2 0 0 0,0-2-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,2-1 0 0 0,9 61 0 0 0,0-27 0 0 0,-11 4 0 0 0,17 4 0 0 0,-20 2 0 0 0,5-27 0 0 0,1-9 0 0 0,-3 1 0 0 0,1 0 0 0 0,0-2 0 0 0,-1 3 0 0 0,0-2 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,-2 5 0 0 0,-8 83-11 0 0,-9-4-42 0 0,17-3 53 0 0,8 38 0 0 0,1-62 0 0 0,-4-7 12 0 0,0-51 4 0 0,-1 38 108 0 0,-32 64-44 0 0,21-60-80 0 0,3-38 0 0 0,-2 23 0 0 0,7 31 0 0 0,13-31 0 0 0,-10 4 0 0 0,-5-27 0 0 0,3 1 0 0 0,-2 29 99 0 0,0-29 95 0 0,-6 13-174 0 0,2-7 27 0 0,8-8-47 0 0,6-3 0 0 0,0 1 0 0 0,-6-2 0 0 0,6-3-20 0 0,-4-2-73 0 0,-3-1 7 0 0,-3 0-3 0 0,2 0-9 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1-1-1 0 0,2 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,2 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 98 0 0,5-6-6888 0 0,-4 1-1987 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6517.426">13687 3738 7688 0 0,'0'0'349'0'0,"0"0"-2"0"0,0 0-90 0 0,0 0 455 0 0,0 0 227 0 0,0 0 42 0 0,14 5 4082 0 0,53-12-625 0 0,3 6-2566 0 0,-15 4-1407 0 0,120-3 623 0 0,-13 5-464 0 0,-46 12 788 0 0,26-6-770 0 0,167-36 656 0 0,-193 25-914 0 0,-63 3-169 0 0,129-13 21 0 0,-21-3-119 0 0,-92 23-53 0 0,10 3 128 0 0,-30-7-192 0 0,46 6-8 0 0,51-3 144 0 0,-58 5-136 0 0,10-1 32 0 0,-67-10 64 0 0,11-3-335 0 0,11 4 142 0 0,18 8 97 0 0,-4-9 168 0 0,78-14-96 0 0,-77 4-8 0 0,9-3-240 0 0,-12 16 64 0 0,34-15 96 0 0,-7-2 167 0 0,31-1-62 0 0,-71 12-25 0 0,107-19-57 0 0,-95 10-318 0 0,102 4 639 0 0,40-2-696 0 0,-28 21 1344 0 0,-58-6-976 0 0,-16-1 0 0 0,-6-4 0 0 0,17 7 200 0 0,-58 2-40 0 0,197 6-64 0 0,-26-11 203 0 0,-157-10-246 0 0,67 14 139 0 0,128-8-128 0 0,-144-6 428 0 0,-2-6 0 0 0,3-6-492 0 0,30-3 0 0 0,148-22-11 0 0,-173 22-42 0 0,13 1 53 0 0,-45 14 0 0 0,-76 1 0 0 0,1 2 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 1 0 0 0,19 6 0 0 0,69 5 0 0 0,15-2 0 0 0,55-1 0 0 0,-101-9 0 0 0,-46-6 0 0 0,9-1 0 0 0,36-8 0 0 0,-19 7 0 0 0,-45 7 0 0 0,-5 0 0 0 0,4 0-16 0 0,-9 0-68 0 0,-2 0-32 0 0,15 3-689 0 0,-20 1-1817 0 0,-7 5-1623 0 0,-25 8 1843 0 0,-6-6-20 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2485,33 +2478,33 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2378 755 2760 0 0,'0'0'531'0'0,"0"0"1186"0"0,0 0 519 0 0,0 0 106 0 0,0 0-166 0 0,0 0-792 0 0,0 0-346 0 0,0 0-70 0 0,0 0-47 0 0,0 0-163 0 0,0 0-71 0 0,0 0-14 0 0,0 0 10 0 0,0 0 42 0 0,0 0 13 0 0,0 9 699 0 0,-6 115 2364 0 0,12 23-1865 0 0,5 116-247 0 0,5-21-814 0 0,-13-49-319 0 0,-18-69 500 0 0,22-94-2539 0 0,-7-29 905 0 0,0-1-60 0 0,0 0-15 0 0,0 0-116 0 0,0 0-476 0 0,0 0-209 0 0,2 0-39 0 0,8-2-10 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2597.859">2201 671 4144 0 0,'0'0'319'0'0,"0"0"23"0"0,0 0 881 0 0,5-5 1496 0 0,-1 3 846 0 0,51-23 2209 0 0,17 20-278 0 0,131-4-967 0 0,-119-1-3873 0 0,6-1-272 0 0,115-9 368 0 0,-47 17-373 0 0,-155 3-377 0 0,61 0 316 0 0,0-2-1 0 0,57-11-317 0 0,32-5 240 0 0,43-10-96 0 0,-55 18-73 0 0,-46 6 277 0 0,28 2-231 0 0,84-12 51 0 0,-37 4-88 0 0,-38 17-27 0 0,-61-1-42 0 0,-46-3 14 0 0,-3-2 0 0 0,2 0-1 0 0,1-2 1 0 0,-3 0 0 0 0,22-4-25 0 0,54-3 73 0 0,20 5 130 0 0,-76 3-371 0 0,59-10 88 0 0,53-22 197 0 0,-59 14-106 0 0,-38 12 42 0 0,123 8-170 0 0,-93-2 117 0 0,-27 5 64 0 0,92-3-64 0 0,47 5 0 0 0,-59-1 0 0 0,61-9 0 0 0,-58 10-64 0 0,2 0 75 0 0,-46 1 31 0 0,58-2-95 0 0,49 3 53 0 0,-38 11-160 0 0,-63-14 107 0 0,1-2-22 0 0,-11 7 11 0 0,40-9 53 0 0,-61 5-42 0 0,94-6-339 0 0,-20 6 280 0 0,38-3 32 0 0,-132-3 80 0 0,123 4 0 0 0,-32-15 177 0 0,-2-3-378 0 0,-20 15 201 0 0,-24-12 0 0 0,-47 2 46 0 0,1 1 0 0 0,1 4-1 0 0,12 1-45 0 0,81-2-5 0 0,22 1-127 0 0,-39-6 284 0 0,103-7-13 0 0,61 8-422 0 0,-153-1 407 0 0,12-3 201 0 0,-121 18-371 0 0,-30-5-57 0 0,9 0-101 0 0,-4 1 124 0 0,31 8 64 0 0,-8-1 16 0 0,-10 9 0 0 0,-8-1 0 0 0,2 23 0 0 0,-7 4 0 0 0,-10 7 0 0 0,-5 9 257 0 0,0-14-154 0 0,8 21 193 0 0,-11 31-376 0 0,1-10-72 0 0,-6-5 152 0 0,0 49 64 0 0,3-29-64 0 0,4-12 64 0 0,12-28-53 0 0,-7-3 42 0 0,2-2-53 0 0,-5 25 75 0 0,0-36 31 0 0,2-11-84 0 0,1-28 20 0 0,8-2-31 0 0,-1 1-11 0 0,1 11-21 0 0,-4-16-85 0 0,0-2-15 0 0,0 0 1 0 0,-2 1-73 0 0,-5 4-309 0 0,4-4-135 0 0,3-1-31 0 0,-3 3-3225 0 0,3-3 2170 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4154.481">10638 1795 456 0 0,'0'0'1935'0'0,"0"0"230"0"0,0 0 105 0 0,7 0 2569 0 0,-16 0 1235 0 0,8 0-5318 0 0,-8 0 604 0 0,-39 0 319 0 0,-4 3 418 0 0,5 4-841 0 0,-1-1-398 0 0,-138-19 1481 0 0,-4 0-1024 0 0,62 19-770 0 0,56 5-530 0 0,-155 22 160 0 0,47-25 530 0 0,-121-4-273 0 0,35 7-305 0 0,21-8 282 0 0,86-17-409 0 0,-67 12 0 0 0,-473 81 0 0 0,638-72 12 0 0,2-4 1 0 0,-2-2-1 0 0,1-3 1 0 0,1-4-1 0 0,-2-1 1 0 0,-43-11-13 0 0,-163-33 117 0 0,67 22-117 0 0,54 16 89 0 0,-93 6-89 0 0,-183-10-97 0 0,271 30 97 0 0,-190-30 0 0 0,74-8 0 0 0,151 14 11 0 0,-83 4 138 0 0,-105 7-149 0 0,204 3 0 0 0,-33-10 0 0 0,-59 7 45 0 0,79 4-26 0 0,1 6-322 0 0,-201 14 758 0 0,224-18-455 0 0,-135-5 344 0 0,20 8-365 0 0,113-3-99 0 0,-32 5 109 0 0,52-15 11 0 0,41-1 0 0 0,-29 1 0 0 0,-58 10-368 0 0,57 4-707 0 0,42-6-1382 0 0,17-4 988 0 0,1 0-298 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8166.184">1945 1805 2760 0 0,'7'31'2136'0'0,"-7"-30"-1553"0"0,0-1-342 0 0,0 0-148 0 0,36 15 2680 0 0,-35-15-2055 0 0,-1 0 30 0 0,0 0 117 0 0,0 0 51 0 0,0 0 11 0 0,0 0-21 0 0,0 0-87 0 0,0 0-34 0 0,0 0-7 0 0,0 0-4 0 0,0 0-6 0 0,0 0-7 0 0,0 0-1 0 0,0 0-33 0 0,0 0-140 0 0,0 0-62 0 0,-14 6 796 0 0,-37 1 55 0 0,-18 10 107 0 0,-28-10 121 0 0,-63 7-11 0 0,36 2-921 0 0,44-16-416 0 0,23-4-63 0 0,-70-16 422 0 0,96 14-425 0 0,-1 1-1 0 0,1 2 0 0 0,-1 0 1 0 0,0 3-1 0 0,-3 1-189 0 0,13-1 26 0 0,-65-1-15 0 0,-67 41-11 0 0,74-38 0 0 0,-26-1 0 0 0,74-4 0 0 0,9-6-11 0 0,1-1-554 0 0,20 9 409 0 0,-9-10-997 0 0,6-3-1235 0 0,-1-3-4013 0 0,5 15 1126 0 0,-3-5-1271 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8769.491">500 1677 4144 0 0,'-4'0'371'0'0,"-37"10"5674"0"0,10-4 1575 0 0,10 1-6482 0 0,-55 24 2093 0 0,-60 53-822 0 0,21 26-2088 0 0,46-16 366 0 0,68-90-645 0 0,0-1 1 0 0,1 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,2 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-2-2 1 0 0,3 1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,2 0-42 0 0,9 8 113 0 0,1-1 0 0 0,0-1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1-1-1 0 0,2-2 1 0 0,-2 2 0 0 0,2-2 0 0 0,15 2-113 0 0,41 7 53 0 0,35-4-769 0 0,-107-9-139 0 0,-1 0-1079 0 0,2 1-4291 0 0,6 2-1841 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11563.093">11079 614 1376 0 0,'0'0'65'0'0,"0"0"-6"0"0,-2 2 265 0 0,2 0 1296 0 0,-11 5 9233 0 0,7-5-11305 0 0,-1 2 8571 0 0,9-3-7501 0 0,-1-1-153 0 0,-3 0-1 0 0,0 0-25 0 0,9-1 177 0 0,145-26 2488 0 0,188-22-951 0 0,-156 24-1665 0 0,-105 16-280 0 0,68 5-144 0 0,-70 7 3 0 0,11 1 63 0 0,78 2 73 0 0,-113-15-234 0 0,-53 4 49 0 0,0 3-3067 0 0,-2 2-3310 0 0,0 0 4316 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12290.505">12486 202 13104 0 0,'0'0'297'0'0,"0"0"39"0"0,0 0 19 0 0,0 0-34 0 0,0 0-126 0 0,0 0 250 0 0,0 0 130 0 0,0 0 29 0 0,0 0-13 0 0,10 6 913 0 0,44 14 1575 0 0,40 15-91 0 0,-84-31-2871 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 1 1 0 0,1-2-1 0 0,-1 2 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1 1 0 0 0,4 3-117 0 0,18 47 400 0 0,-21-13-62 0 0,0-8 43 0 0,-1 11 309 0 0,-33 10 92 0 0,12-39-673 0 0,-2-2 0 0 0,2-1 0 0 0,-3 0 0 0 0,2-1 0 0 0,-19 14-109 0 0,18-20 53 0 0,2 0 1 0 0,-3-1-1 0 0,2 0 0 0 0,-3-1 1 0 0,2-1-1 0 0,-16 6-53 0 0,-12-12-351 0 0,38-4-332 0 0,1-1-1543 0 0,3 3-4239 0 0,-2 1-1953 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="90996.656">13715 1177 920 0 0,'0'0'304'0'0,"0"0"941"0"0,0 0 414 0 0,0-1 1565 0 0,6-8-1987 0 0,38-68 3794 0 0,-40 70-4715 0 0,-1 1 1 0 0,3 0-1 0 0,-1 2 1 0 0,0-2-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0-316 0 0,-4 4 87 0 0,2-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-3 0 1 0 0,3 1 0 0 0,-3 1-1 0 0,3-1 1 0 0,-2 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,-1 1-1 0 0,1-2 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0-86 0 0,9 24 477 0 0,-2-1 0 0 0,-1-1 0 0 0,-1 3 0 0 0,0-1-1 0 0,-1 27-476 0 0,-10 54 1538 0 0,5-106-1494 0 0,0 1 1 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-2 0-1 0 0,2-2 1 0 0,-2 1 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-2-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1-45 0 0,-3 1 47 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,2-1-1 0 0,-2 1 1 0 0,-1-2-47 0 0,-3-3-7 0 0,3 0-1 0 0,-2 0 0 0 0,0-1 1 0 0,2 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1-3 0 0 0,1 2 1 0 0,0-1-1 0 0,1 0 1 0 0,2 1-1 0 0,-5-12 8 0 0,5 15-502 0 0,3 0 0 0 0,-1-2 0 0 0,0 2 0 0 0,0 0-1 0 0,-1 0 1 0 0,2-1 0 0 0,2 2 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,0-1 502 0 0,7-10-7366 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="91897.027">14272 887 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-132 0 0,0 0-646 0 0,0 0-278 0 0,2-1-58 0 0,11-8 2229 0 0,-12 9-2573 0 0,-1 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-13 0 0,0 0-49 0 0,9 5 828 0 0,-6-1-1148 0 0,-1 0 0 0 0,-1 1 0 0 0,0-2 1 0 0,1 1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 1 0 0,-1-2-140 0 0,-2 25 426 0 0,-16 192 876 0 0,19-145-1182 0 0,0-75-384 0 0,0 4 981 0 0,0 1-1983 0 0,0 6-3464 0 0,0-12 2540 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="92647.981">14298 1084 920 0 0,'0'1'67'0'0,"0"3"290"0"0,0-3 1430 0 0,0-1 622 0 0,0 0 119 0 0,0 0-204 0 0,0 0-970 0 0,0 0-423 0 0,0 0-88 0 0,5-22 1733 0 0,-5 21-2071 0 0,1 0-229 0 0,11-16 61 0 0,-9 15-136 0 0,2-4 690 0 0,30-29 1892 0 0,5 12-882 0 0,-34 22-1876 0 0,-2 1 0 0 0,-1 0 0 0 0,2-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,2 1 1 0 0,-1 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-25 0 0,20 33 1472 0 0,-3 10-864 0 0,-18-17-608 0 0,10 11 0 0 0,-8-4 72 0 0,-4-33 299 0 0,0-2 117 0 0,20 14 597 0 0,5-2-1750 0 0,-24-11 404 0 0,18-8-493 0 0,13-20-1947 0 0,-19 2-3478 0 0,-11 17-300 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="93989.379">15129 951 456 0 0,'0'0'1413'0'0,"0"0"159"0"0,0 0 76 0 0,0 0-140 0 0,0 0-647 0 0,0 0-278 0 0,0 0-58 0 0,0-7 1476 0 0,-1 6 4407 0 0,-8 1-5892 0 0,-1 0-1 0 0,1 1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,2 0 1 0 0,-2 1-1 0 0,2 0 0 0 0,-1 0 1 0 0,-1 1-1 0 0,3 0 0 0 0,-8 5-515 0 0,-7 4 424 0 0,16-11-374 0 0,3 0 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 1 0 0,3 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-2 1 1 0 0,2 1-1 0 0,0-1 0 0 0,-2 3-50 0 0,-13 42 264 0 0,15 2-125 0 0,3-41-85 0 0,0-1 0 0 0,1 0 1 0 0,1 1-1 0 0,-2-1 0 0 0,3 2 1 0 0,-1-2-1 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-2-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,7 8-54 0 0,-9-13-18 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,2 0 1 0 0,-1 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,3 0 18 0 0,37-6-3249 0 0,-38 2 1306 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95267.643">15520 504 920 0 0,'0'0'341'0'0,"0"0"1098"0"0,0 0 480 0 0,0 0 96 0 0,0 0-104 0 0,0 0-531 0 0,0 0-237 0 0,2 2-45 0 0,1 14 790 0 0,-3-15-1129 0 0,0-1-20 0 0,0 2-30 0 0,0 127 4843 0 0,-5-35-3927 0 0,-2 118 184 0 0,4-54-1385 0 0,3-131-472 0 0,0 4-118 0 0,0-8-6313 0 0,0-23 4748 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95643.07">15536 641 920 0 0,'12'-7'6425'0'0,"13"-16"3843"0"0,22 3-5971 0 0,-39 17-3958 0 0,-2 1 0 0 0,3 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1 0 0 0 0,2 1 0 0 0,-1-1-1 0 0,0 2 1 0 0,8 0-339 0 0,33 11 773 0 0,-12-1-4595 0 0,-27-11-1695 0 0,-2 0-1564 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98550.722">15959 855 920 0 0,'0'0'241'0'0,"0"0"678"0"0,0 0 296 0 0,0 0 58 0 0,0 0-53 0 0,0 0-254 0 0,0 0-114 0 0,0 0-20 0 0,0 0-22 0 0,0 0-70 0 0,0 0-32 0 0,0 26 3129 0 0,-12 227 4156 0 0,15-96-6298 0 0,1-94-1707 0 0,-4-62-70 0 0,0-1-160 0 0,0 0-685 0 0,0-7-2761 0 0,0-3-3454 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98832.077">15985 600 7976 0 0,'0'14'364'0'0,"0"-10"-8"0"0,0 3-212 0 0,0-1-7 0 0,0-5 574 0 0,0-1 238 0 0,0 10 1235 0 0,0-9 2609 0 0,1-1-5097 0 0,2-8-870 0 0,0 5-3805 0 0,-3 3 790 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="100011.114">16350 1170 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-6 6 0 0,-6-41 6095 0 0,15 10-2868 0 0,29-7-2391 0 0,-14 27 397 0 0,-20 17-1428 0 0,-2-1 1 0 0,2 1-1 0 0,-2 0 0 0 0,2 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 2 0 0 0,0-2 0 0 0,0 1 0 0 0,-2 0 0 0 0,3-1 0 0 0,-2 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 3-36 0 0,11 79 216 0 0,-23 14 176 0 0,-6-61 1491 0 0,17-37-1877 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,3 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,1 0 0 0 0,-2 0-6 0 0,-16-8 9 0 0,-33-34 46 0 0,29-17-327 0 0,20 55 112 0 0,1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-2 1 0 0 0,3 1 1 0 0,0-2 160 0 0,25-36-6577 0 0,-18 32 179 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="112707.469">13508 852 6192 0 0,'0'0'133'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 66 0 0,0 0 226 0 0,1-22 6285 0 0,-2-20-2539 0 0,-10 23-3101 0 0,-40-44-120 0 0,-15 21-726 0 0,43 36-73 0 0,-19 9 54 0 0,-21 21-89 0 0,25 30-88 0 0,12 9-64 0 0,14 25 80 0 0,8-63 60 0 0,3 2 0 0 0,1 0 0 0 0,0-1 0 0 0,3 0 0 0 0,0 1 0 0 0,4 9-140 0 0,7 89 1072 0 0,-3-56-1705 0 0,3 4-463 0 0,-12-61-34 0 0,-2-9-5836 0 0,0-3 1152 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="113106.261">13171 1024 11952 0 0,'0'0'546'0'0,"0"0"-10"0"0,6-5-322 0 0,1 1 384 0 0,2 0 1 0 0,-1 0 0 0 0,0 1 0 0 0,-1 1-1 0 0,3-1 1 0 0,-2 1 0 0 0,0 0 0 0 0,1 1-1 0 0,0 0 1 0 0,-1 1-599 0 0,17-4 579 0 0,19 8 986 0 0,1-1-980 0 0,-18 0-2039 0 0,-8-2-3511 0 0,-3-1-1716 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119095.651">16840 961 920 0 0,'0'0'215'0'0,"0"0"565"0"0,0 0 246 0 0,0 0 50 0 0,0 0-38 0 0,0 0-207 0 0,0 0-88 0 0,-11-18 1465 0 0,11 18-2144 0 0,-5-8 120 0 0,5 3-161 0 0,0 4 46 0 0,0 1 50 0 0,0 0 7 0 0,0 0-4 0 0,-1-6-39 0 0,0 6 8497 0 0,-12 47-6476 0 0,7 50 348 0 0,2-26-1794 0 0,10 69 1307 0 0,-6-53-1940 0 0,2-74 372 0 0,-2 1-4686 0 0,0-14 2473 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119948.343">16818 1177 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-112 0 0,0 0 219 0 0,8-5 2204 0 0,12-19-38 0 0,-19 23-2011 0 0,-1-21 3079 0 0,2 8-2359 0 0,15-36 1842 0 0,9 20-1982 0 0,8 5 8 0 0,-27 24-1121 0 0,-4 2 6 0 0,-1-1 0 0 0,-1 0-1 0 0,2 0 1 0 0,0 1 0 0 0,-2 0-1 0 0,2-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0 3-22 0 0,12 9-263 0 0,-12-10 258 0 0,2 0 0 0 0,-2 0 1 0 0,2 1-1 0 0,-2-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,-2 0 0 0 0,3 0 0 0 0,-2 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 1 5 0 0,6 19 825 0 0,9 56 291 0 0,-4-48-1116 0 0,1-11 562 0 0,12-21 72 0 0,-21-2-761 0 0,2-1 1 0 0,-2 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-2 1 0 0,2 1-1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,2-2 127 0 0,3-1-1228 0 0,19-12-4345 0 0,-24 16 3808 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121219.819">17515 497 3224 0 0,'-3'12'2653'0'0,"-1"28"1684"0"0,-8-2-951 0 0,8 30-459 0 0,-3 41-127 0 0,5 43-152 0 0,1-90-2024 0 0,4 1 194 0 0,-3-3 190 0 0,-11 26-96 0 0,0 82-482 0 0,5-147-526 0 0,4-19 68 0 0,2-2-108 0 0,0 0-10 0 0,0 0 8 0 0,0 0-167 0 0,0 0-710 0 0,-1-10-2894 0 0,-2-3-3509 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121883.773">17515 545 11024 0 0,'0'0'248'0'0,"0"0"34"0"0,0 0 22 0 0,0 0-29 0 0,2 1-54 0 0,47 5 5667 0 0,-2 8-4316 0 0,2 8 205 0 0,4 19-391 0 0,-19-5-436 0 0,-12-5-482 0 0,31 66 576 0 0,-30-42-556 0 0,2 40 243 0 0,-24-76-582 0 0,1-1 1 0 0,-2 0-1 0 0,-2 0 1 0 0,2 1-1 0 0,-3-1 1 0 0,0-1-1 0 0,-1 4-149 0 0,-16 97 744 0 0,-2-15 79 0 0,14-81-656 0 0,4-14-103 0 0,3 1 0 0 0,-2 0 0 0 0,0-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-2 1-1 0 0,2-1 1 0 0,-1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,-6 6-64 0 0,5-8 14 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2-1 1 0 0,2 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,-1 0-14 0 0,-39-13-1612 0 0,40 10 372 0 0,3 2 9 0 0,2-6-3128 0 0,-2-6 2299 0 0,5 11-11 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122684.061">18190 504 6968 0 0,'0'0'316'0'0,"0"0"-3"0"0,0 0-49 0 0,0 0 543 0 0,0 0 258 0 0,0 0 50 0 0,3 11 2997 0 0,-3 29-882 0 0,-3 13-957 0 0,-28 118 1538 0 0,-1 73-1086 0 0,20-110-1413 0 0,7-16-1045 0 0,5-61-214 0 0,0-49-2118 0 0,-2-6-5266 0 0,1-2 4284 0 0,4-10-3949 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="123499.345">18254 521 1376 0 0,'0'0'455'0'0,"0"0"1373"0"0,0 0 605 0 0,0 0 119 0 0,0 0-232 0 0,0 0-1087 0 0,0 0-473 0 0,0 0-96 0 0,0 0-7 0 0,0 0 58 0 0,0 0 21 0 0,0 0 7 0 0,0 0-22 0 0,2 0-96 0 0,37-7 3303 0 0,-36 7-3725 0 0,1-1 0 0 0,0 1 0 0 0,-2 0 0 0 0,3 0 1 0 0,-3 0-1 0 0,3 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,3 1-203 0 0,2 1 237 0 0,80 37 1652 0 0,-78-33-1701 0 0,-1 0 1 0 0,1 1-1 0 0,-2 0 0 0 0,0 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,3 6-188 0 0,-7-11 45 0 0,26 88 375 0 0,-29-87-406 0 0,0-1 0 0 0,0 1 1 0 0,0 1-1 0 0,0-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1-1 0 0 0,0 2 1 0 0,-2-1-1 0 0,3 0 0 0 0,-2 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,-1 2-14 0 0,-2-1 56 0 0,0 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,1-2 0 0 0,-1 1 0 0 0,-4 1-56 0 0,-17 6 176 0 0,16-11-196 0 0,42 13-457 0 0,-22-11 473 0 0,0 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,1 0-1 0 0,-2 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 1 0 0,2 1-1 0 0,-1-1 1 0 0,-1 1-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 3 4 0 0,-20 89 137 0 0,13-81 1 0 0,-2 0-1 0 0,2-1 0 0 0,-1-1 0 0 0,-2-1 0 0 0,0 1 0 0 0,-6 7-137 0 0,-11 12 332 0 0,-37 37 176 0 0,33-50-504 0 0,-9-41-3300 0 0,36 16 1814 0 0,0-2-56 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="126421.51">12877 1852 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-2 10-158 0 0,1-10 318 0 0,1 0 203 0 0,-4-17 4327 0 0,11-83 858 0 0,9-12-4362 0 0,-12-51-443 0 0,-5 31-346 0 0,14-65-590 0 0,-7 43 735 0 0,2-19-741 0 0,-5-30-100 0 0,19-21 802 0 0,17 49-1204 0 0,-9 58 526 0 0,-19 94-375 0 0,14-24 96 0 0,-11 33 0 0 0,-8 11 11 0 0,2-3 42 0 0,7 5-120 0 0,159 32 118 0 0,-80-21-51 0 0,24 0 0 0 0,93 29 0 0 0,-39-11 13 0 0,-60-8 12 0 0,3-5 1 0 0,96-1-26 0 0,379-33 619 0 0,-259-2-286 0 0,211-3 704 0 0,-127 2-1079 0 0,361 34 539 0 0,-131-24-461 0 0,-399-3-36 0 0,-42 6 0 0 0,-27 0-89 0 0,235 2 178 0 0,41 56-89 0 0,-162-18-53 0 0,-197-27 106 0 0,-79 12-53 0 0,-13-11 0 0 0,0 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1 4 0 0 0,-2 27 0 0 0,-14 132 0 0 0,-16 51 0 0 0,-11 72 0 0 0,-8 64 0 0 0,18-179 0 0 0,19-106 0 0 0,-35 106 0 0 0,25-88 0 0 0,-1 10 0 0 0,16-49 0 0 0,-11 31 0 0 0,-12-22 0 0 0,28-51 0 0 0,-18 9 0 0 0,-2-1 0 0 0,-62 12 0 0 0,23-22-89 0 0,-290-1 178 0 0,137 0-89 0 0,-134-16 0 0 0,31-4 0 0 0,-369 8-364 0 0,360 23 728 0 0,-73-30-364 0 0,122 7-488 0 0,157 6 351 0 0,-262 9-206 0 0,276-2 409 0 0,-2-6 0 0 0,-62-9-66 0 0,-99-18 67 0 0,-54 0 57 0 0,97 19-596 0 0,-20-13 472 0 0,172 14 141 0 0,-173-19 66 0 0,111 7-414 0 0,-223-34 751 0 0,243 44-712 0 0,67 2-1600 0 0,29 7-7788 0 0,17 0 569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128916.561">12562 1607 1376 0 0,'1'0'379'0'0,"1"0"-255"0"0,3-1 1065 0 0,20-34 2596 0 0,-20 27-3929 0 0,-2-24 6888 0 0,-3 31-6157 0 0,-15 1 1265 0 0,-42 24 2723 0 0,-109 14-187 0 0,83-25-3294 0 0,-1-5 0 0 0,-1-4 0 0 0,1-3 0 0 0,-2-5-1094 0 0,-38-3 693 0 0,-205-33-271 0 0,244 27-246 0 0,-6 6 42 0 0,-25-2-111 0 0,78 27-215 0 0,36-17-45 0 0,-6-3-2 0 0,6 1-5493 0 0,2 1 3616 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129317.678">11445 1369 12496 0 0,'0'0'572'0'0,"-8"4"186"0"0,-107 25 4653 0 0,-38 33-21 0 0,-1 45-3631 0 0,107-44-1578 0 0,32-15 21 0 0,14-47-198 0 0,0 2 21 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 1 0 0,0 1-26 0 0,34 53 343 0 0,17-18 88 0 0,24-1-135 0 0,111 32-1529 0 0,-164-63-94 0 0,-2-4-65 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2223 771 2760 0 0,'0'0'531'0'0,"0"0"1186"0"0,0 0 519 0 0,0 0 106 0 0,0 0-166 0 0,0 0-792 0 0,0 0-346 0 0,0 0-70 0 0,0 0-47 0 0,0 0-163 0 0,0 0-71 0 0,0 0-14 0 0,0 0 10 0 0,0 0 42 0 0,0 0 13 0 0,0 9 699 0 0,-6 118 2364 0 0,12 23-1865 0 0,4 118-247 0 0,5-20-814 0 0,-12-51-319 0 0,-17-71 500 0 0,20-95-2539 0 0,-6-30 905 0 0,0-1-60 0 0,0 0-15 0 0,0 0-116 0 0,0 0-476 0 0,0 0-209 0 0,2 0-39 0 0,8-2-10 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2597.859">2057 685 4144 0 0,'0'0'319'0'0,"0"0"23"0"0,0 0 881 0 0,5-5 1496 0 0,-1 3 846 0 0,47-23 2209 0 0,17 19-278 0 0,121-3-967 0 0,-110-1-3873 0 0,5-1-272 0 0,108-10 368 0 0,-45 18-373 0 0,-144 3-377 0 0,57 0 316 0 0,0-2-1 0 0,53-11-317 0 0,30-5 240 0 0,40-11-96 0 0,-51 19-73 0 0,-43 6 277 0 0,26 2-231 0 0,78-13 51 0 0,-34 5-88 0 0,-36 17-27 0 0,-56-1-42 0 0,-44-3 14 0 0,-2-1 0 0 0,1-1-1 0 0,1-2 1 0 0,-2-1 0 0 0,20-3-25 0 0,51-3 73 0 0,18 5 130 0 0,-71 3-371 0 0,56-10 88 0 0,49-23 197 0 0,-56 15-106 0 0,-34 12 42 0 0,114 8-170 0 0,-87-2 117 0 0,-25 5 64 0 0,86-3-64 0 0,44 5 0 0 0,-55-1 0 0 0,57-9 0 0 0,-54 10-64 0 0,1 0 75 0 0,-42 2 31 0 0,54-3-95 0 0,45 3 53 0 0,-35 11-160 0 0,-59-14 107 0 0,1-1-22 0 0,-10 6 11 0 0,37-9 53 0 0,-56 5-42 0 0,87-6-339 0 0,-19 6 280 0 0,36-3 32 0 0,-124-3 80 0 0,116 4 0 0 0,-31-15 177 0 0,-1-3-378 0 0,-19 15 201 0 0,-23-12 0 0 0,-43 2 46 0 0,1 0 0 0 0,0 5-1 0 0,12 1-45 0 0,75-2-5 0 0,21 1-127 0 0,-36-6 284 0 0,95-7-13 0 0,58 7-422 0 0,-143 0 407 0 0,11-3 201 0 0,-113 18-371 0 0,-28-5-57 0 0,8 0-101 0 0,-3 1 124 0 0,28 8 64 0 0,-7 0 16 0 0,-9 8 0 0 0,-8-1 0 0 0,2 24 0 0 0,-6 4 0 0 0,-10 7 0 0 0,-4 10 257 0 0,-1-16-154 0 0,8 23 193 0 0,-10 31-376 0 0,0-10-72 0 0,-5-5 152 0 0,0 49 64 0 0,3-28-64 0 0,4-13 64 0 0,11-29-53 0 0,-7-3 42 0 0,2-2-53 0 0,-4 26 75 0 0,-1-37 31 0 0,2-11-84 0 0,2-29 20 0 0,6-2-31 0 0,0 1-11 0 0,1 12-21 0 0,-4-17-85 0 0,0-2-15 0 0,0 0 1 0 0,-2 1-73 0 0,-5 4-309 0 0,5-4-135 0 0,2-1-31 0 0,-3 3-3225 0 0,3-3 2170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4154.481">9944 1833 456 0 0,'0'0'1935'0'0,"0"0"230"0"0,0 0 105 0 0,6 0 2569 0 0,-14 0 1235 0 0,7 0-5318 0 0,-8 0 604 0 0,-35 0 319 0 0,-5 3 418 0 0,5 4-841 0 0,-1-1-398 0 0,-129-19 1481 0 0,-3 0-1024 0 0,57 19-770 0 0,53 5-530 0 0,-145 23 160 0 0,43-26 530 0 0,-112-4-273 0 0,32 7-305 0 0,20-8 282 0 0,81-17-409 0 0,-64 12 0 0 0,-441 83 0 0 0,596-74 12 0 0,2-4 1 0 0,-2-2-1 0 0,1-3 1 0 0,1-4-1 0 0,-2-1 1 0 0,-41-12-13 0 0,-151-33 117 0 0,62 23-117 0 0,50 15 89 0 0,-86 7-89 0 0,-171-10-97 0 0,252 30 97 0 0,-176-30 0 0 0,68-9 0 0 0,142 15 11 0 0,-78 4 138 0 0,-98 7-149 0 0,190 3 0 0 0,-30-10 0 0 0,-56 7 45 0 0,75 4-26 0 0,0 6-322 0 0,-188 15 758 0 0,210-19-455 0 0,-126-5 344 0 0,18 8-365 0 0,106-3-99 0 0,-30 5 109 0 0,49-15 11 0 0,38-1 0 0 0,-27 1 0 0 0,-55 10-368 0 0,54 4-707 0 0,39-6-1382 0 0,16-4 988 0 0,1 0-298 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8166.184">1818 1843 2760 0 0,'7'32'2136'0'0,"-7"-31"-1553"0"0,0-1-342 0 0,0 0-148 0 0,33 15 2680 0 0,-32-15-2055 0 0,-1 0 30 0 0,0 0 117 0 0,0 0 51 0 0,0 0 11 0 0,0 0-21 0 0,0 0-87 0 0,0 0-34 0 0,0 0-7 0 0,0 0-4 0 0,0 0-6 0 0,0 0-7 0 0,0 0-1 0 0,0 0-33 0 0,0 0-140 0 0,0 0-62 0 0,-13 6 796 0 0,-35 2 55 0 0,-16 9 107 0 0,-27-10 121 0 0,-58 7-11 0 0,33 3-921 0 0,41-17-416 0 0,22-4-63 0 0,-66-17 422 0 0,90 15-425 0 0,-1 1-1 0 0,1 2 0 0 0,-1 0 1 0 0,0 3-1 0 0,-2 1-189 0 0,11-1 26 0 0,-60-1-15 0 0,-63 42-11 0 0,69-39 0 0 0,-24-1 0 0 0,69-4 0 0 0,9-7-11 0 0,0 0-554 0 0,19 9 409 0 0,-8-10-997 0 0,5-3-1235 0 0,0-4-4013 0 0,4 16 1126 0 0,-3-5-1271 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="8769.491">467 1713 4144 0 0,'-3'0'371'0'0,"-36"10"5674"0"0,10-4 1575 0 0,10 1-6482 0 0,-52 25 2093 0 0,-56 53-822 0 0,19 28-2088 0 0,44-17 366 0 0,63-92-645 0 0,0-1 1 0 0,1 0-1 0 0,-2 1 1 0 0,1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,2 1-1 0 0,-2-1 1 0 0,2 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-2 1 0 0,3 1-1 0 0,-1 1 1 0 0,-1-1-1 0 0,2 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,3 0-42 0 0,8 8 113 0 0,1-1 0 0 0,0 0 0 0 0,0-1 0 0 0,1-1 0 0 0,-1-1-1 0 0,2-2 1 0 0,-2 2 0 0 0,2-2 0 0 0,14 2-113 0 0,38 8 53 0 0,33-5-769 0 0,-100-9-139 0 0,-1 0-1079 0 0,2 1-4291 0 0,5 2-1841 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11563.093">10356 627 1376 0 0,'0'0'65'0'0,"0"0"-6"0"0,-2 2 265 0 0,2 0 1296 0 0,-10 5 9233 0 0,6-5-11305 0 0,-1 2 8571 0 0,9-3-7501 0 0,-1-1-153 0 0,-3 0-1 0 0,0 0-25 0 0,8-1 177 0 0,136-26 2488 0 0,176-23-951 0 0,-146 24-1665 0 0,-99 17-280 0 0,65 5-144 0 0,-66 7 3 0 0,10 1 63 0 0,73 2 73 0 0,-106-15-234 0 0,-49 4 49 0 0,0 3-3067 0 0,-2 2-3310 0 0,0 0 4316 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12290.5049">11671 206 13104 0 0,'0'0'297'0'0,"0"0"39"0"0,0 0 19 0 0,0 0-34 0 0,0 0-126 0 0,0 0 250 0 0,0 0 130 0 0,0 0 29 0 0,0 0-13 0 0,9 6 913 0 0,42 15 1575 0 0,37 15-91 0 0,-79-32-2871 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 1 1 0 0,0-2-1 0 0,0 2 0 0 0,-2 2 0 0 0,1-2 0 0 0,0 1 0 0 0,-2 1 0 0 0,5 3-117 0 0,16 49 400 0 0,-20-14-62 0 0,1-9 43 0 0,-2 12 309 0 0,-30 11 92 0 0,11-41-673 0 0,-2-1 0 0 0,2-2 0 0 0,-3 0 0 0 0,2 0 0 0 0,-18 13-109 0 0,17-20 53 0 0,2 1 1 0 0,-3-2-1 0 0,2 0 0 0 0,-3-1 1 0 0,2-1-1 0 0,-14 7-53 0 0,-13-13-351 0 0,37-4-332 0 0,0-2-1543 0 0,3 4-4239 0 0,-1 1-1953 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="90996.656">12820 1202 920 0 0,'0'0'304'0'0,"0"0"941"0"0,0 0 414 0 0,0-1 1565 0 0,5-8-1987 0 0,37-70 3794 0 0,-39 72-4715 0 0,0 1 1 0 0,3 0-1 0 0,-2 2 1 0 0,1-3-1 0 0,0 2 1 0 0,-1 0-1 0 0,2 0 1 0 0,1 0-1 0 0,-2 1 1 0 0,2 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,-1 1 1 0 0,2 0-1 0 0,-2 0-316 0 0,-3 4 87 0 0,2-1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,2 0-1 0 0,-4 0 1 0 0,4 1 0 0 0,-3 1-1 0 0,3-1 1 0 0,-3 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,2 1 1 0 0,-2-1 0 0 0,2 1-1 0 0,-3 0 1 0 0,2 0-1 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,-1 2-1 0 0,0-3 1 0 0,1 2-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0-86 0 0,8 25 477 0 0,-1-2 0 0 0,-2 0 0 0 0,0 2 0 0 0,0 0-1 0 0,-2 27-476 0 0,-8 55 1538 0 0,4-108-1494 0 0,0 1 1 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,-1-1-1 0 0,1-2 1 0 0,-2 1 0 0 0,2 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-2-1-1 0 0,2 0 1 0 0,-2 0 0 0 0,2 0 0 0 0,-2 0 0 0 0,1-1-45 0 0,-3 1 47 0 0,1-1 0 0 0,-2 0-1 0 0,2 0 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,0 0 0 0 0,1-2-1 0 0,-2 2 1 0 0,0-2-47 0 0,-4-3-7 0 0,4 0-1 0 0,-3 0 0 0 0,1-1 1 0 0,1-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0-3 0 0 0,0 1 1 0 0,1 0-1 0 0,0 0 1 0 0,2 1-1 0 0,-4-13 8 0 0,4 16-502 0 0,3 0 0 0 0,-1-2 0 0 0,0 2 0 0 0,0 0-1 0 0,-1-1 1 0 0,2 0 0 0 0,2 2 0 0 0,-2-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1-1 0 0,2 0 1 0 0,-2 1 0 0 0,1-1 502 0 0,7-10-7366 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="91897.027">13340 906 456 0 0,'0'0'1836'0'0,"0"0"219"0"0,0 0 96 0 0,0 0-132 0 0,0 0-646 0 0,0 0-278 0 0,2-1-58 0 0,10-8 2229 0 0,-11 9-2573 0 0,-1 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-13 0 0,0 0-49 0 0,9 5 828 0 0,-6-1-1148 0 0,-2 0 0 0 0,0 1 0 0 0,0-2 1 0 0,1 1-1 0 0,-1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 1 0 0,-1-2-140 0 0,-2 26 426 0 0,-14 195 876 0 0,17-147-1182 0 0,0-77-384 0 0,0 4 981 0 0,0 1-1983 0 0,0 7-3464 0 0,0-13 2540 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="92647.981">13365 1107 920 0 0,'0'1'67'0'0,"0"3"290"0"0,0-3 1430 0 0,0-1 622 0 0,0 0 119 0 0,0 0-204 0 0,0 0-970 0 0,0 0-423 0 0,0 0-88 0 0,4-22 1733 0 0,-4 21-2071 0 0,1 0-229 0 0,11-17 61 0 0,-10 16-136 0 0,3-4 690 0 0,28-30 1892 0 0,4 13-882 0 0,-31 22-1876 0 0,-3 1 0 0 0,0 0 0 0 0,2-1-1 0 0,-1 1 1 0 0,-1 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,2 1 1 0 0,-1 0 0 0 0,-2 1 0 0 0,3-1 0 0 0,-1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-25 0 0,18 34 1472 0 0,-2 10-864 0 0,-17-18-608 0 0,9 12 0 0 0,-7-4 72 0 0,-4-34 299 0 0,0-2 117 0 0,18 14 597 0 0,6-1-1750 0 0,-23-12 404 0 0,16-8-493 0 0,13-21-1947 0 0,-18 2-3478 0 0,-10 18-300 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="93989.379">14141 971 456 0 0,'0'0'1413'0'0,"0"0"159"0"0,0 0 76 0 0,0 0-140 0 0,0 0-647 0 0,0 0-278 0 0,0 0-58 0 0,0-7 1476 0 0,0 6 4407 0 0,-9 1-5892 0 0,0 0-1 0 0,0 1 0 0 0,0 1 1 0 0,1-1-1 0 0,-2 1 0 0 0,3 0 1 0 0,-3 1-1 0 0,3 0 0 0 0,-1 0 1 0 0,-2 1-1 0 0,4 1 0 0 0,-8 4-515 0 0,-7 4 424 0 0,15-11-374 0 0,4 0 0 0 0,-2 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 2-1 0 0,1-2 0 0 0,-2 1 1 0 0,2 1-1 0 0,0-1 0 0 0,-1 3-50 0 0,-13 43 264 0 0,14 2-125 0 0,3-42-85 0 0,0 0 0 0 0,0-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,3 2 1 0 0,-1-1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,1-2-1 0 0,0 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,8 8-54 0 0,-10-13-18 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,0 1 0 0 0,0-2 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 0 0 0 0,2 0 18 0 0,35-6-3249 0 0,-35 2 1306 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95267.643">14507 515 920 0 0,'0'0'341'0'0,"0"0"1098"0"0,0 0 480 0 0,0 0 96 0 0,0 0-104 0 0,0 0-531 0 0,0 0-237 0 0,2 2-45 0 0,1 14 790 0 0,-3-15-1129 0 0,0-1-20 0 0,0 2-30 0 0,0 130 4843 0 0,-5-36-3927 0 0,-2 120 184 0 0,5-54-1385 0 0,2-135-472 0 0,0 5-118 0 0,0-9-6313 0 0,0-23 4748 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="95643.07">14522 655 920 0 0,'11'-8'6425'0'0,"12"-15"3843"0"0,21 3-5971 0 0,-36 16-3958 0 0,-3 2 0 0 0,4 0-1 0 0,-2 0 1 0 0,1 1 0 0 0,-2 0 0 0 0,3 1 0 0 0,-2-1-1 0 0,1 2 1 0 0,7 0-339 0 0,31 12 773 0 0,-12-2-4595 0 0,-25-11-1695 0 0,-1 0-1564 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98550.722">14917 873 920 0 0,'0'0'241'0'0,"0"0"678"0"0,0 0 296 0 0,0 0 58 0 0,0 0-53 0 0,0 0-254 0 0,0 0-114 0 0,0 0-20 0 0,0 0-22 0 0,0 0-70 0 0,0 0-32 0 0,0 27 3129 0 0,-11 231 4156 0 0,14-98-6298 0 0,1-95-1707 0 0,-4-64-70 0 0,0-1-160 0 0,0 0-685 0 0,0-7-2761 0 0,0-4-3454 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="98832.077">14942 613 7976 0 0,'0'14'364'0'0,"0"-10"-8"0"0,0 3-212 0 0,0-1-7 0 0,0-5 574 0 0,0-1 238 0 0,0 11 1235 0 0,0-10 2609 0 0,1-1-5097 0 0,1-9-870 0 0,1 6-3805 0 0,-3 3 790 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="100011.114">15283 1195 8288 0 0,'0'0'190'0'0,"0"0"28"0"0,0 0 7 0 0,0-6 6 0 0,-6-42 6095 0 0,15 10-2868 0 0,26-7-2391 0 0,-12 28 397 0 0,-20 17-1428 0 0,-1-1 1 0 0,2 1-1 0 0,-2 0 0 0 0,1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-2 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,-2 0 0 0 0,3-1 0 0 0,-2 1 0 0 0,1 1 0 0 0,-2-1 0 0 0,1 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-2 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 3-36 0 0,10 81 216 0 0,-21 14 176 0 0,-6-62 1491 0 0,16-38-1877 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,3 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,-2 1 0 0 0,2-1 0 0 0,1 0 0 0 0,-2 0-6 0 0,-15-8 9 0 0,-30-35 46 0 0,26-17-327 0 0,19 56 112 0 0,1-1-1 0 0,1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1-1 0 0 0,-2 0 0 0 0,2 2 1 0 0,1-2 160 0 0,23-37-6577 0 0,-16 33 179 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="112707.469">12626 870 6192 0 0,'0'0'133'0'0,"0"0"23"0"0,0 0 13 0 0,0 0 66 0 0,0 0 226 0 0,1-22 6285 0 0,-2-21-2539 0 0,-9 23-3101 0 0,-38-44-120 0 0,-13 21-726 0 0,39 37-73 0 0,-17 9 54 0 0,-20 22-89 0 0,23 30-88 0 0,12 9-64 0 0,13 26 80 0 0,7-65 60 0 0,3 3 0 0 0,1 0 0 0 0,0-2 0 0 0,3 1 0 0 0,0 0 0 0 0,3 10-140 0 0,8 91 1072 0 0,-4-58-1705 0 0,3 5-463 0 0,-11-63-34 0 0,-2-9-5836 0 0,0-3 1152 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="113106.261">12311 1046 11952 0 0,'0'0'546'0'0,"0"0"-10"0"0,6-5-322 0 0,0 0 384 0 0,3 1 1 0 0,-2 0 0 0 0,1 1 0 0 0,-2 1-1 0 0,4-1 1 0 0,-3 1 0 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0 1-599 0 0,15-4 579 0 0,18 8 986 0 0,2-1-980 0 0,-18 0-2039 0 0,-7-2-3511 0 0,-4-1-1716 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119095.651">15741 981 920 0 0,'0'0'215'0'0,"0"0"565"0"0,0 0 246 0 0,0 0 50 0 0,0 0-38 0 0,0 0-207 0 0,0 0-88 0 0,-11-18 1465 0 0,11 18-2144 0 0,-4-8 120 0 0,4 3-161 0 0,0 4 46 0 0,0 1 50 0 0,0 0 7 0 0,0 0-4 0 0,-1-6-39 0 0,0 6 8497 0 0,-11 48-6476 0 0,6 51 348 0 0,2-27-1794 0 0,10 71 1307 0 0,-6-54-1940 0 0,2-76 372 0 0,-2 1-4686 0 0,0-14 2473 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="119948.343">15720 1202 6360 0 0,'0'0'290'0'0,"0"0"-3"0"0,0 0-112 0 0,0 0 219 0 0,8-5 2204 0 0,10-20-38 0 0,-17 24-2011 0 0,-1-21 3079 0 0,2 8-2359 0 0,14-38 1842 0 0,8 22-1982 0 0,8 4 8 0 0,-25 25-1121 0 0,-4 2 6 0 0,-2-1 0 0 0,0 0-1 0 0,2 0 1 0 0,0 1 0 0 0,-2 0-1 0 0,2-1 1 0 0,-1 1-1 0 0,-2 0 1 0 0,3 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,1 2 1 0 0,-1-2 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0 3-22 0 0,11 9-263 0 0,-11-10 258 0 0,2 0 0 0 0,-2 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 2 0 0 0,0 0 5 0 0,6 19 825 0 0,8 58 291 0 0,-4-49-1116 0 0,1-12 562 0 0,12-21 72 0 0,-20-2-761 0 0,1-1 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 0 0 0,-2-2 1 0 0,1 1-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-2 127 0 0,4-1-1228 0 0,17-13-4345 0 0,-22 17 3808 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121219.819">16372 508 3224 0 0,'-3'12'2653'0'0,"-1"29"1684"0"0,-7-3-951 0 0,7 32-459 0 0,-2 41-127 0 0,4 44-152 0 0,1-91-2024 0 0,4 0 194 0 0,-3-3 190 0 0,-11 27-96 0 0,1 84-482 0 0,4-151-526 0 0,5-19 68 0 0,1-2-108 0 0,0 0-10 0 0,0 0 8 0 0,0 0-167 0 0,0 0-710 0 0,-1-10-2894 0 0,-2-3-3509 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="121883.773">16372 557 11024 0 0,'0'0'248'0'0,"0"0"34"0"0,0 0 22 0 0,0 0-29 0 0,2 1-54 0 0,43 5 5667 0 0,-1 8-4316 0 0,2 8 205 0 0,4 20-391 0 0,-19-5-436 0 0,-10-5-482 0 0,29 67 576 0 0,-29-43-556 0 0,2 41 243 0 0,-22-78-582 0 0,1 0 1 0 0,-2-1-1 0 0,-2 1 1 0 0,2 0-1 0 0,-2-1 1 0 0,-1 0-1 0 0,-1 3-149 0 0,-15 100 744 0 0,-1-16 79 0 0,12-83-656 0 0,5-14-103 0 0,2 2 0 0 0,-2-1 0 0 0,0-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1-1 0 0 0,-3 2-1 0 0,2-2 1 0 0,0-1 0 0 0,-2 1 0 0 0,1-1-1 0 0,-1 0 1 0 0,-5 7-64 0 0,4-9 14 0 0,1 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,-3-1 1 0 0,3 0-1 0 0,-2 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,0 0-14 0 0,-37-13-1612 0 0,38 10 372 0 0,2 2 9 0 0,2-6-3128 0 0,-1-7 2299 0 0,4 12-11 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122684.061">17003 515 6968 0 0,'0'0'316'0'0,"0"0"-3"0"0,0 0-49 0 0,0 0 543 0 0,0 0 258 0 0,0 0 50 0 0,2 11 2997 0 0,-2 30-882 0 0,-2 13-957 0 0,-27 120 1538 0 0,-1 76-1086 0 0,19-113-1413 0 0,6-17-1045 0 0,5-62-214 0 0,0-50-2118 0 0,-2-6-5266 0 0,1-2 4284 0 0,4-10-3949 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="123499.345">17062 532 1376 0 0,'0'0'455'0'0,"0"0"1373"0"0,0 0 605 0 0,0 0 119 0 0,0 0-232 0 0,0 0-1087 0 0,0 0-473 0 0,0 0-96 0 0,0 0-7 0 0,0 0 58 0 0,0 0 21 0 0,0 0 7 0 0,0 0-22 0 0,2 0-96 0 0,35-7 3303 0 0,-34 7-3725 0 0,0-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,3 0 1 0 0,-4 0-1 0 0,4 1 0 0 0,-1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,4 1-203 0 0,1 1 237 0 0,76 38 1652 0 0,-74-34-1701 0 0,-1 0 1 0 0,2 2-1 0 0,-3-1 0 0 0,1 0 0 0 0,-1 1 1 0 0,0 0-1 0 0,-1 1 0 0 0,4 5-188 0 0,-7-11 45 0 0,24 90 375 0 0,-27-89-406 0 0,0-1 0 0 0,0 1 1 0 0,0 2-1 0 0,0-2 0 0 0,-1-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1-1 0 0 0,0 2 1 0 0,-2-1-1 0 0,4 1 0 0 0,-3-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,0 2-14 0 0,-3-1 56 0 0,0 2 0 0 0,1-2 0 0 0,-2 1 0 0 0,2-2 1 0 0,-2 0-1 0 0,0 0 0 0 0,0-2 0 0 0,0 1 0 0 0,-4 1-56 0 0,-16 6 176 0 0,15-11-196 0 0,39 14-457 0 0,-20-12 473 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-2-1 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,-2-1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 4 4 0 0,-19 90 137 0 0,13-83 1 0 0,-3 0-1 0 0,3 0 0 0 0,-2-2 0 0 0,-1-1 0 0 0,0 2 0 0 0,-6 6-137 0 0,-11 13 332 0 0,-33 37 176 0 0,30-50-504 0 0,-9-43-3300 0 0,34 17 1814 0 0,1-2-56 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="126421.51">12036 1891 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-1 10-158 0 0,0-10 318 0 0,1 0 203 0 0,-4-17 4327 0 0,10-85 858 0 0,9-12-4362 0 0,-11-53-443 0 0,-5 32-346 0 0,13-66-590 0 0,-6 44 735 0 0,1-20-741 0 0,-4-30-100 0 0,18-22 802 0 0,15 50-1204 0 0,-8 60 526 0 0,-17 96-375 0 0,12-25 96 0 0,-10 33 0 0 0,-7 12 11 0 0,1-3 42 0 0,7 5-120 0 0,149 33 118 0 0,-75-22-51 0 0,22 0 0 0 0,87 30 0 0 0,-36-11 13 0 0,-56-9 12 0 0,2-5 1 0 0,90 0-26 0 0,355-35 619 0 0,-243-1-286 0 0,198-4 704 0 0,-119 3-1079 0 0,337 34 539 0 0,-122-24-461 0 0,-373-4-36 0 0,-39 7 0 0 0,-26 0-89 0 0,220 2 178 0 0,39 57-89 0 0,-152-18-53 0 0,-184-28 106 0 0,-74 12-53 0 0,-13-11 0 0 0,1 1 0 0 0,-2 0 0 0 0,2-1 0 0 0,-1 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1 5 0 0 0,-1 26 0 0 0,-14 136 0 0 0,-15 52 0 0 0,-10 73 0 0 0,-8 65 0 0 0,18-182 0 0 0,17-108 0 0 0,-33 107 0 0 0,24-89 0 0 0,-2 10 0 0 0,16-50 0 0 0,-10 32 0 0 0,-12-23 0 0 0,26-52 0 0 0,-16 10 0 0 0,-3-2 0 0 0,-57 13 0 0 0,21-23-89 0 0,-270-1 178 0 0,127 0-89 0 0,-125-16 0 0 0,29-4 0 0 0,-345 7-364 0 0,336 25 728 0 0,-67-32-364 0 0,113 8-488 0 0,147 6 351 0 0,-245 9-206 0 0,258-1 409 0 0,-1-7 0 0 0,-59-10-66 0 0,-92-17 67 0 0,-51-1 57 0 0,91 20-596 0 0,-18-13 472 0 0,160 14 141 0 0,-162-20 66 0 0,104 8-414 0 0,-208-36 751 0 0,227 46-712 0 0,62 2-1600 0 0,28 7-7788 0 0,15 0 569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="128916.561">11742 1641 1376 0 0,'1'0'379'0'0,"1"0"-255"0"0,3-1 1065 0 0,18-35 2596 0 0,-18 28-3929 0 0,-3-25 6888 0 0,-2 32-6157 0 0,-14 1 1265 0 0,-39 25 2723 0 0,-102 14-187 0 0,77-26-3294 0 0,0-5 0 0 0,-2-4 0 0 0,2-3 0 0 0,-3-5-1094 0 0,-34-3 693 0 0,-193-34-271 0 0,229 28-246 0 0,-6 6 42 0 0,-24-2-111 0 0,74 27-215 0 0,33-17-45 0 0,-6-3-2 0 0,6 1-5493 0 0,2 1 3616 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="129317.678">10698 1398 12496 0 0,'0'0'572'0'0,"-8"4"186"0"0,-99 26 4653 0 0,-36 33-21 0 0,-1 46-3631 0 0,100-44-1578 0 0,30-16 21 0 0,13-48-198 0 0,0 2 21 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0 0-1 0 0,2 0 1 0 0,0 1-26 0 0,32 54 343 0 0,15-18 88 0 0,23-1-135 0 0,104 32-1529 0 0,-153-64-94 0 0,-3-4-65 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2542,7 +2535,7 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">27 6 1208 0 0,'-4'-6'289'0'0,"3"6"8094"0"0,-2 14-7238 0 0,2-13-680 0 0,1 17 1541 0 0,-4 22-206 0 0,4-15-1476 0 0,-1 29 1078 0 0,-6 27 73 0 0,1 5-627 0 0,6-84-1179 0 0,0-2-137 0 0,0 0-767 0 0,0 0-3063 0 0,0 0-1315 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 6 1208 0 0,'0'-6'289'0'0,"0"6"8094"0"0,0 14-7238 0 0,0-12-680 0 0,0 16 1541 0 0,0 23-206 0 0,0-15-1476 0 0,-1 30 1078 0 0,1 28 73 0 0,0 5-627 0 0,0-87-1179 0 0,0-2-137 0 0,0 0-767 0 0,0 0-3063 0 0,0 0-1315 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2573,7 +2566,7 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 3 3224 0 0,'14'10'573'0'0,"-13"-10"782"0"0,-1 0 461 0 0,0 0 82 0 0,11-3 3130 0 0,-10-1-4221 0 0,1-2-3150 0 0,-2 6 1465 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 3 3224 0 0,'2'10'573'0'0,"-2"-10"782"0"0,0 0 461 0 0,0 0 82 0 0,1-3 3130 0 0,0-1-4221 0 0,-1-2-3150 0 0,0 6 1465 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2870,26 +2863,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.73046875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="37.265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="3" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="90.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2897,13 +2890,13 @@
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43557</v>
       </c>
@@ -2911,26 +2904,26 @@
         <v>0.3125</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="4">
         <v>0.3263888888888889</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="4">
         <v>0.36805555555555558</v>
@@ -2938,881 +2931,883 @@
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4">
-        <v>0.4548611111111111</v>
-      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="4">
-        <v>0.46527777777777773</v>
+        <v>0.4548611111111111</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="4">
-        <v>0.47222222222222227</v>
+        <v>0.46527777777777773</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="4">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="4">
         <v>0.59027777777777779</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4">
-        <v>0.66319444444444442</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4">
-        <v>0.66666666666666663</v>
+        <v>0.66319444444444442</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4">
-        <v>0.68402777777777779</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4">
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="4">
         <v>0.6875</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>43558</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B19" s="4">
         <v>0.3125</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4">
+      <c r="C19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4">
-        <v>0.375</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4">
-        <v>0.4201388888888889</v>
+        <v>0.375</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4">
-        <v>0.52777777777777779</v>
+        <v>0.4201388888888889</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="4">
         <v>0.55208333333333337</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="2"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D27" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="4">
-        <v>0.59375</v>
-      </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="4">
-        <v>0.61458333333333337</v>
+        <v>0.59375</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+        <v>83</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="4">
-        <v>0.66666666666666663</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="4">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>43559</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.3125</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="3">
-        <v>43559</v>
-      </c>
-      <c r="B32" s="4">
-        <v>0.3125</v>
-      </c>
-      <c r="C32" s="2" t="s">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="4">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="2"/>
-      <c r="B33" s="4">
-        <v>0.3263888888888889</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="4">
-        <v>0.41666666666666669</v>
-      </c>
+      <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="4">
-        <v>0.44097222222222227</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="4">
-        <v>0.52777777777777779</v>
+        <v>0.44097222222222227</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="4">
-        <v>0.54166666666666663</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="4">
-        <v>0.5625</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="4">
-        <v>0.67361111111111116</v>
+        <v>0.5625</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="4">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="4">
         <v>0.69444444444444453</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A42" s="3">
+      <c r="C42" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>43560</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B43" s="4">
         <v>0.3125</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" s="2"/>
-      <c r="B43" s="4">
-        <v>0.34722222222222227</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="4">
-        <v>0.39583333333333331</v>
+        <v>0.34722222222222227</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="4">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="4">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" s="3">
+      <c r="C46" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
         <v>43563</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B47" s="4">
         <v>0.3125</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A47" s="2"/>
-      <c r="B47" s="4">
-        <v>0.31944444444444448</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="4">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="4">
         <v>0.375</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A49" s="2"/>
-      <c r="B49" s="4"/>
       <c r="C49" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="2" t="s">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="4">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="4">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" s="2"/>
-      <c r="B51" s="4">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A53" s="2"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="2" t="s">
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A54" s="2"/>
-      <c r="B54" s="4">
-        <v>0.61805555555555558</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A56" s="2"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A57" s="2"/>
-      <c r="B57" s="4">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D57" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="4">
         <v>0.68055555555555547</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A59" s="3">
+      <c r="C59" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
         <v>43564</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B60" s="4">
         <v>0.3125</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="B61" s="4">
-        <v>0.34375</v>
-      </c>
+      <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="4">
-        <v>0.4201388888888889</v>
+        <v>0.34375</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="4">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B64" s="4">
+      <c r="C64" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B65" s="4">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B65" s="4"/>
       <c r="C65" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B66" s="7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="C66" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="7">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D66" s="2" t="s">
+      <c r="C67" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="7">
+        <v>0.6875</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="7">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>43565</v>
+      </c>
+      <c r="B70" s="7">
+        <v>0.3125</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="7">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B67" s="7">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="7">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="7">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C77" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="7">
         <v>0.6875</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A68" s="3"/>
-      <c r="B68" s="7">
-        <v>0.70138888888888884</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A69" s="3">
-        <v>43565</v>
-      </c>
-      <c r="B69" s="7">
+      <c r="C78" s="2" t="str">
+        <f>+C88</f>
+        <v>Alanyse Critère 7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="8">
+        <v>43566</v>
+      </c>
+      <c r="B79" s="7">
         <v>0.3125</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B70" s="7">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="C79" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B82" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B71" s="7">
-        <v>0.375</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B72" s="7">
-        <v>0.43402777777777773</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B73" s="7">
-        <v>0.4513888888888889</v>
-      </c>
-      <c r="C73" s="2" t="s">
+    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B84" s="7">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="7">
+        <v>0.625</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="7">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C74" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C75" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C76" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B77" s="7">
-        <v>0.6875</v>
-      </c>
-      <c r="C77" s="2" t="str">
-        <f>+C87</f>
-        <v>Alanyse Critère 7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A78" s="8">
-        <v>43566</v>
-      </c>
-      <c r="B78" s="7">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="8">
+        <v>43567</v>
+      </c>
+      <c r="B88" s="7">
         <v>0.3125</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B79" s="7">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B80" s="7">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B81" s="7">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C82" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B83" s="7">
-        <v>0.56944444444444442</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B84" s="7">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C84" s="2" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="7">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="8">
+        <v>43570</v>
+      </c>
+      <c r="B91" s="7">
+        <v>0.3125</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B85" s="7">
-        <v>0.625</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B86" s="7">
-        <v>0.65277777777777779</v>
-      </c>
-      <c r="C86" s="2" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B95" s="7">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="7">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A87" s="8">
-        <v>43567</v>
-      </c>
-      <c r="B87" s="7">
-        <v>0.3125</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B88" s="7">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B89" s="7">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A90" s="8">
-        <v>43570</v>
-      </c>
-      <c r="B90" s="7">
-        <v>0.3125</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C91" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B92" s="7">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C92" s="2" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B93" s="7">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B94" s="7">
-        <v>0.4861111111111111</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B95" s="7">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C96" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C97" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C98" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A99" s="8">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="8">
         <v>43571</v>
       </c>
-      <c r="B99" s="7">
+      <c r="B100" s="7">
         <v>0.3125</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B100" s="7">
+      <c r="C100" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B101" s="7">
         <v>0.4861111111111111</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B101" s="7">
+      <c r="C101" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="7">
         <v>0.52777777777777779</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B102" s="7"/>
-      <c r="C102" s="2" t="s">
-        <v>118</v>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="7"/>
+      <c r="C103" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D52" r:id="rId1" xr:uid="{3ABE7781-7A63-49E3-B7D9-7A926D777280}"/>
+    <hyperlink ref="D53" r:id="rId1"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3821,193 +3816,194 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="49.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="49.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.1328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1328125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="49.3984375" style="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="49.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="C16" s="2"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -4017,26 +4013,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405881BC-250B-44EF-9833-781DFFD746B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView zoomScale="72" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="103.265625" customWidth="1"/>
+    <col min="1" max="1" width="103.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added resume. Modified logbook, documentation
</commit_message>
<xml_diff>
--- a/JournalDeBord.xlsx
+++ b/JournalDeBord.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_5EE694708D43841AFD7FF13BEC4929CF749799F7" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{178BFD60-2C96-4E93-A763-6EAFB600B878}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13680" windowHeight="9435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal De Bord" sheetId="1" r:id="rId1"/>
     <sheet name="Question" sheetId="2" r:id="rId2"/>
     <sheet name="Dessin" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="123">
   <si>
     <t>Documentation</t>
   </si>
@@ -356,9 +357,6 @@
     <t>Logiciel pour recuperer tout le code et le transformer en PDF ?</t>
   </si>
   <si>
-    <t>Added IMG</t>
-  </si>
-  <si>
     <t>Debugging</t>
   </si>
   <si>
@@ -399,13 +397,25 @@
   </si>
   <si>
     <t>Réponse Q11</t>
+  </si>
+  <si>
+    <t>Passage V1</t>
+  </si>
+  <si>
+    <t>Ajouter l'image au site</t>
+  </si>
+  <si>
+    <t>Commentaire code</t>
+  </si>
+  <si>
+    <t>Compte admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +439,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -438,7 +455,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -446,12 +463,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -477,8 +533,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -503,15 +564,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>241290</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>23707</xdr:rowOff>
+      <xdr:colOff>173251</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>91203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4220370</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>153517</xdr:rowOff>
+      <xdr:colOff>2321120</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>51252</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -528,8 +589,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="241290" y="1109557"/>
-            <a:ext cx="3979080" cy="491760"/>
+            <a:off x="173251" y="805578"/>
+            <a:ext cx="2147869" cy="317237"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -568,15 +629,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>184140</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>157057</xdr:rowOff>
+      <xdr:colOff>142402</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>45388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4163220</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>105892</xdr:rowOff>
+      <xdr:colOff>2290271</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>3885</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -593,8 +654,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="184140" y="2147782"/>
-            <a:ext cx="3979080" cy="491760"/>
+            <a:off x="142402" y="1474138"/>
+            <a:ext cx="2147869" cy="315685"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -633,15 +694,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1572856</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>110415</xdr:rowOff>
+      <xdr:colOff>892018</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>15005</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>59183</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>13995</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4470936</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>60361</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -658,8 +719,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="1572856" y="2101140"/>
-            <a:ext cx="6625440" cy="627480"/>
+            <a:off x="892018" y="1443755"/>
+            <a:ext cx="3578918" cy="402544"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -698,15 +759,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2472840</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>158835</xdr:rowOff>
+      <xdr:colOff>1377821</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>46546</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4275360</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>140430</xdr:rowOff>
+      <xdr:colOff>2350803</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>26384</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -723,8 +784,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="2472840" y="2149560"/>
-            <a:ext cx="1802520" cy="524520"/>
+            <a:off x="1377821" y="1475296"/>
+            <a:ext cx="972982" cy="337026"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -763,15 +824,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>231766</xdr:colOff>
+      <xdr:colOff>168110</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>85620</xdr:rowOff>
+      <xdr:rowOff>85622</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>210653</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>61620</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4552698</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>107728</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -788,8 +849,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="231766" y="266595"/>
-            <a:ext cx="8118000" cy="1423800"/>
+            <a:off x="168110" y="264217"/>
+            <a:ext cx="4384588" cy="915074"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -828,15 +889,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4541400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>50010</xdr:rowOff>
+      <xdr:colOff>2494408</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>37909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>374647</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>124230</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6286500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15832</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -853,8 +914,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="4541400" y="1859760"/>
-            <a:ext cx="7020360" cy="798120"/>
+            <a:off x="2494408" y="1288067"/>
+            <a:ext cx="3792092" cy="513703"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -893,15 +954,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7263720</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>113580</xdr:rowOff>
+      <xdr:colOff>3963889</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133404</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7273440</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>48165</xdr:rowOff>
+      <xdr:colOff>3969136</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28536</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -918,8 +979,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7263720" y="2285280"/>
-            <a:ext cx="9720" cy="115560"/>
+            <a:off x="3963889" y="1562154"/>
+            <a:ext cx="5247" cy="73727"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -958,15 +1019,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7254000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>29700</xdr:rowOff>
+      <xdr:colOff>3958643</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>78763</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7264800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>34740</xdr:rowOff>
+      <xdr:colOff>3964472</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>82047</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -983,8 +1044,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7254000" y="2201400"/>
-            <a:ext cx="10800" cy="5040"/>
+            <a:off x="3958643" y="1507513"/>
+            <a:ext cx="5829" cy="3284"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1023,15 +1084,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7317360</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>169470</xdr:rowOff>
+      <xdr:colOff>3992844</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7561</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7320240</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>108375</xdr:rowOff>
+      <xdr:colOff>3994398</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>84102</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1048,8 +1109,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7317360" y="1255320"/>
-            <a:ext cx="2880" cy="119880"/>
+            <a:off x="3992844" y="900531"/>
+            <a:ext cx="1554" cy="76541"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1088,15 +1149,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7293240</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>67230</xdr:rowOff>
+      <xdr:colOff>3979824</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>119556</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7293600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>71190</xdr:rowOff>
+      <xdr:colOff>3980019</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>122135</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1113,8 +1174,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7293240" y="1153080"/>
-            <a:ext cx="360" cy="3960"/>
+            <a:off x="3979824" y="833931"/>
+            <a:ext cx="195" cy="2579"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1153,15 +1214,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4528800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>166125</xdr:rowOff>
+      <xdr:colOff>2487607</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>121720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4727160</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>18015</xdr:rowOff>
+      <xdr:colOff>2594679</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>79323</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1178,8 +1239,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="4528800" y="1432950"/>
-            <a:ext cx="198360" cy="213840"/>
+            <a:off x="2487607" y="1014690"/>
+            <a:ext cx="107072" cy="136196"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1217,16 +1278,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>71047</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>148935</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5763802</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>46137</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85087</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>180255</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5771381</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66539</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1243,8 +1304,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10496160" y="8654760"/>
-            <a:ext cx="14040" cy="31320"/>
+            <a:off x="5763802" y="6323979"/>
+            <a:ext cx="7579" cy="20402"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1282,16 +1343,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>192607</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>31470</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5418098</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>30864</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>662047</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5671497</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>116740</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1308,8 +1369,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="9855720" y="8356320"/>
-            <a:ext cx="469440" cy="410760"/>
+            <a:off x="5418098" y="6129338"/>
+            <a:ext cx="253399" cy="265244"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1347,16 +1408,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190207</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>170790</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5828123</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>122632</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>328087</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5902550</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>160595</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1373,8 +1434,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10615320" y="8495640"/>
-            <a:ext cx="137880" cy="338760"/>
+            <a:off x="5828123" y="6221106"/>
+            <a:ext cx="74427" cy="217331"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1412,16 +1473,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>595207</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>170790</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6046737</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>122632</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>712207</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6109892</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>122134</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1438,8 +1499,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="11020320" y="8495640"/>
-            <a:ext cx="117000" cy="279720"/>
+            <a:off x="6046737" y="6221106"/>
+            <a:ext cx="63155" cy="178870"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1477,16 +1538,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>379567</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>90150</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5930337</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>70101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>504487</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>23040</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5997767</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>80464</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1503,8 +1564,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10804680" y="8415000"/>
-            <a:ext cx="124920" cy="294840"/>
+            <a:off x="5930337" y="6168575"/>
+            <a:ext cx="67430" cy="189731"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1543,15 +1604,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>87840</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>69750</xdr:rowOff>
+      <xdr:colOff>142922</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>138529</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>69487</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>69615</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5351639</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>48553</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -1568,8 +1629,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="87840" y="2965350"/>
-            <a:ext cx="9644760" cy="5972040"/>
+            <a:off x="142922" y="2649665"/>
+            <a:ext cx="5208717" cy="3856096"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1635,33 +1696,33 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">246 704 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">638 721 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-3-9 10039 0 0,4 4-11103 0 0,-2-1-133 0 0,2 1-129 0 0,0 5-468 0 0,0 1-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">1033 663 11976 0 0,'-1'4'296'0'0,"-5"6"4551"0"0,4-6-506 0 0,1-2-3562 0 0,0 2-7280 0 0,1-4-277 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">1380 745 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-4 7070 0 0,2-6-6507 0 0,4-23-839 0 0,-7 32-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-14 79 971 0 0,13-78-904 0 0,1-2-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,4-16-522 0 0,3-28 325 0 0,-7 43 218 0 0,0 1 13 0 0,7-4-260 0 0,-1 7-230 0 0,-4 2 347 0 0,-12 35 365 0 0,9-38-139 0 0,1-2-27 0 0,0 0-161 0 0,0 0-194 0 0,-11-12-214 0 0,22-43 40 0 0,-1 48 757 0 0,-8 6-562 0 0,-2 1-34 0 0,14 15 96 0 0,-24 51 294 0 0,10-64 48 0 0,0-2-24 0 0,-12 10 14 0 0,11-10-266 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-12 0 0,-1-2-1 0 0,1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-4 1 0 0,16-18-798 0 0,-5 23 705 0 0,11 17 39 0 0,-21-13 64 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 2-10 0 0,2-5 84 0 0,-5 17 237 0 0,-20-9-89 0 0,24-9-144 0 0,1 0 0 0 0,-7-10-1050 0 0,4-10-3857 0 0,2 11-3207 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">1674 462 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 7 198 0 0,8 57 3341 0 0,0-33-2076 0 0,-3 51 1115 0 0,1 17 113 0 0,-2-14-1404 0 0,-1 51 981 0 0,-4-3-1688 0 0,1-58-1417 0 0,-2-32 962 0 0,-7-28-2248 0 0,3-5-5035 0 0,6-10 5419 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">1610 597 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,1-1 240 0 0,13-32 2722 0 0,-14 31-3180 0 0,15-15 1008 0 0,23-24 674 0 0,-35 36-2057 0 0,1 2 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,1-1 1 0 0,-1 1 0 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 1-137 0 0,67 19 1009 0 0,-52 14 55 0 0,-5-18-600 0 0,22 47 1448 0 0,-23 2-2113 0 0,-15-60 230 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 1-29 0 0,3-3 5 0 0,-9 22 399 0 0,1-11-337 0 0,7-8-104 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 37 0 0,-35-1 653 0 0,-7-25-4978 0 0,34 19 2334 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">2998 427 7488 0 0,'0'0'166'0'0,"0"7"236"0"0,4 48 1154 0 0,-12 24 2052 0 0,-3 33 1755 0 0,3 52-2463 0 0,4-54-962 0 0,-3 31-1172 0 0,7-139-851 0 0,0-2-91 0 0,0 0-16 0 0,0 11-2832 0 0,-3 13-2556 0 0,2-23 1622 0 0,1-1-894 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">3016 485 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,13-7 8 0 0,2-4 772 0 0,-14 10-801 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-250 0 0,8 4 395 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,3 4-396 0 0,-6-7 170 0 0,-1 1 5 0 0,0 1-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 2-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1 2-174 0 0,-2 34 278 0 0,-1-41-199 0 0,1-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,0 2 1 0 0,0-2-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 2-79 0 0,-1 0 4 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-4-1-4 0 0,-53-44-4198 0 0,55 42-3651 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">2224 124 3680 0 0,'-6'48'613'0'0,"1"-10"6816"0"0,-6 24-4591 0 0,8 16-23 0 0,2-14-297 0 0,6 4-1604 0 0,-9 95 2 0 0,7-77 200 0 0,1-18-716 0 0,2-41-126 0 0,-6-21-115 0 0,-4 1-1048 0 0,2 4-4224 0 0,2-11 3723 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">2149 694 1376 0 0,'5'-20'2159'0'0,"2"0"4223"0"0,7-6-3735 0 0,-3 6-1523 0 0,12-17 1153 0 0,4 12 523 0 0,-4 3-1591 0 0,22-17 135 0 0,-44 38-1294 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,0-1 0 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-51 0 0,3 3 27 0 0,1 1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,0-1-1 0 0,0 7-27 0 0,10 30 368 0 0,29 120 1443 0 0,-20-124-1634 0 0,1-14-84 0 0,-14-23-77 0 0,-5-2-29 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 13 0 0,40-28-350 0 0,19-12-3834 0 0,-54 36 2533 0 0,3 3-12 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">1 302 6448 0 0,'7'21'6309'0'0,"-7"-18"-6682"0"0,4 54 3514 0 0,8 84-847 0 0,-2-43-690 0 0,-5-10-929 0 0,13 132 737 0 0,-29 31 57 0 0,6-175-1337 0 0,-1-48-256 0 0,5-13-955 0 0,1-11-4480 0 0,0-4-582 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">12 333 6248 0 0,'0'13'190'0'0,"0"-24"349"0"0,18-38 6274 0 0,-18 47-6115 0 0,0 2-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,12-3 291 0 0,71-18 828 0 0,-38 5-729 0 0,12-5 96 0 0,51 12 370 0 0,-61 8-222 0 0,43 2-1079 0 0,-22-6 16 0 0,37-20 451 0 0,-30 15 1144 0 0,61 1-1448 0 0,4 19 224 0 0,-53-19-645 0 0,-30-1 1538 0 0,6 0-1123 0 0,-36 8-292 0 0,52 0 264 0 0,-26-6 20 0 0,55-26 70 0 0,10 18-205 0 0,13 9 34 0 0,-66-4 219 0 0,22-5-424 0 0,-4 12 192 0 0,-11 5 584 0 0,44 1-1352 0 0,-7 9 736 0 0,1 6 1017 0 0,-32-10-298 0 0,-12 0-1239 0 0,26-4 520 0 0,15 3 64 0 0,12 29 75 0 0,-61-11-166 0 0,15 1 523 0 0,-3-9-840 0 0,-22-6 749 0 0,-6-3-675 0 0,24 6 487 0 0,73-9-197 0 0,-21 19 0 0 0,-41-15-20 0 0,-44-2 0 0 0,-13-5 0 0 0,25 17 0 0 0,-38-3 0 0 0,5 6 0 0 0,13 23 64 0 0,-5 27 0 0 0,-8 24-64 0 0,-5 32-8 0 0,1-51 125 0 0,-4 32-203 0 0,-8 34 295 0 0,8 43-190 0 0,-17-83 82 0 0,-1-41-13 0 0,6-44 96 0 0,6-12-234 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0-1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,-1 2 51 0 0,0-3 114 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,-1 0-114 0 0,-14 0 158 0 0,-97 8-218 0 0,81-3 59 0 0,0-1-1 0 0,0-2 1 0 0,0-1 0 0 0,0-2-1 0 0,0-1 1 0 0,-22-6 1 0 0,4-4-9 0 0,-1 3 0 0 0,0 3 0 0 0,0 2 0 0 0,-22 2 9 0 0,-111 0 332 0 0,138 4-330 0 0,0-1-1 0 0,0-3 1 0 0,0-2-1 0 0,0-1 1 0 0,-8-7-2 0 0,23 9-18 0 0,-1 2 0 0 0,1 1 0 0 0,-1 1 0 0 0,-20 4 18 0 0,-143 30 64 0 0,-3-12-136 0 0,-48-9 152 0 0,172-13-80 0 0,-92 0 11 0 0,-33-17 42 0 0,101 17-53 0 0,-23-13 80 0 0,22-11-176 0 0,-85-18 224 0 0,57 22-196 0 0,62 6 192 0 0,-62-3-124 0 0,51 11 0 0 0,45 13-499 0 0,33-7 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">6695 896 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,3 2 218 0 0,0-1 5134 0 0,22-14-8855 0 0,-18 9 1888 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">7069 940 10592 0 0,'-13'-13'818'0'0,"10"9"-344"0"0,3 3 530 0 0,0 1 290 0 0,0 0 61 0 0,0-5 606 0 0,1 2 1568 0 0,13-3-8082 0 0,-5 4-1569 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">7416 850 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,1 0-6 0 0,5 0-232 0 0,-2 0-5476 0 0,-4 0-2114 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">7778 940 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-7-15 464 0 0,10-38 1231 0 0,1 45-2463 0 0,0 1 0 0 0,2 1 52 0 0,-5 5 215 0 0,-1 1 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,7 8 88 0 0,-6-4-189 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,-1 0 0 0 0,-1 3-113 0 0,3-4 41 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 1 0 0,0-1-42 0 0,-9-17 194 0 0,25-16-143 0 0,-13 33-62 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 11 0 0,0-2-43 0 0,3 2 32 0 0,1 10 23 0 0,-10 18 200 0 0,3-27-96 0 0,-7 4-695 0 0,14-7-611 0 0,7-10-5710 0 0,-6 6 446 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">8061 571 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,3 7-221 0 0,-1-3 4251 0 0,11 22-45 0 0,-12-25-3788 0 0,3 8 1039 0 0,3 83 1637 0 0,7 83-1221 0 0,-14-86-1606 0 0,0-79-341 0 0,-2-4-56 0 0,1-5-228 0 0,1-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">8361 612 2760 0 0,'4'8'1828'0'0,"4"20"4892"0"0,5 25-3444 0 0,1 103 1947 0 0,-11-80-3937 0 0,-6-37-4508 0 0,3-36 1701 0 0,-4 6-229 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">8414 940 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0-1-181 0 0,9-39 5734 0 0,3-11-521 0 0,-16 20-3279 0 0,11 10-1202 0 0,8-37 1 0 0,-14 56-738 0 0,1-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2-1 0 0,-1 2 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,3 0-93 0 0,2-2 95 0 0,-4 3-21 0 0,26 0-60 0 0,1 14-14 0 0,-5 7 0 0 0,-20-12 0 0 0,10 23 0 0 0,19 74 514 0 0,-19-52 356 0 0,6-19-278 0 0,-20-34-517 0 0,7 3 98 0 0,-5-1-141 0 0,0-2 0 0 0,0 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1-1 0 0 0,1 0-32 0 0,23-3-185 0 0,-5-29-4233 0 0,-22 32 2840 0 0,0 1-164 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">9199 668 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-2 102 0 0,-1 2-405 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 1-82 0 0,-11-2-143 0 0,-39-6 1747 0 0,43 9-1667 0 0,4-2 170 0 0,0 0 0 0 0,0 1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 1 1 0 0,1-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,-1 0-107 0 0,-34 42-483 0 0,18 2 618 0 0,16 12 378 0 0,10 4-513 0 0,15-4 1899 0 0,26-11-1734 0 0,-12-18-165 0 0,-19-19 0 0 0,15 0 0 0 0,-22-9 0 0 0,-2 2 0 0 0,0-5-64 0 0,30-22-5497 0 0,-31 16 3530 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">9463 1001 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-7 907 0 0,12-17 649 0 0,-9 19-2004 0 0,-3 4 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,10 20 784 0 0,-16 13 56 0 0,6-32-836 0 0,0-1 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">9734 660 1840 0 0,'0'6'396'0'0,"0"-4"991"0"0,0-2 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-4 2 2724 0 0,7 1-2482 0 0,-2-3-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,7 17 886 0 0,5 73 1352 0 0,-5-54-2105 0 0,-9 63 686 0 0,-2-6-314 0 0,3 67-530 0 0,6-112-273 0 0,-3-10 0 0 0,-5-13-45 0 0,3-23-194 0 0,0-2-94 0 0,0 0-19 0 0,-3-14-1557 0 0,2-1 195 0 0,-3-2-70 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">9700 663 1376 0 0,'4'6'367'0'0,"-3"-5"1002"0"0,-1-1 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-133 0 0,9-7 51 0 0,33-23 1588 0 0,-29 24-1245 0 0,-11 4-294 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1 1-100 0 0,2 2 108 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 0 0 0,0 2 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,-1 2 0 0 0,1-2 1 0 0,0 6-108 0 0,9 27 435 0 0,0 58 787 0 0,-11-81-980 0 0,0-13-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 0 0 0,0 0-56 0 0,-44 35 929 0 0,43-35-879 0 0,1-1-45 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0-5 0 0,-3-2 0 0 0,0 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-5 0 0 0,4-15-5381 0 0,0 15-2125 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">10175 394 0 0 0,'-12'12'0'0'0,"6"-15"140"0"0,4 3 2586 0 0,2 0 5496 0 0,15 20-7158 0 0,-14-19-552 0 0,8 30 3000 0 0,-14 31-1947 0 0,1 50 181 0 0,4 1 624 0 0,-7-41-881 0 0,11 38-1316 0 0,-12-26-173 0 0,8-43 0 0 0,14 2-2476 0 0,-12-40 2128 0 0,-2-2 173 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 1-1 0 0,-1-1 1 0 0,0 1 175 0 0,-1-1-2221 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">10157 824 4376 0 0,'0'0'199'0'0,"10"-11"1918"0"0,-6-2 1016 0 0,11-10 683 0 0,-6-13-1297 0 0,-2-1-472 0 0,5 29-1272 0 0,-10 7-743 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,2 1-33 0 0,5 0 304 0 0,21 22 598 0 0,-25-17-674 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 0-1 0 0,2 6-227 0 0,6 92 608 0 0,-7-65-165 0 0,-1-12 997 0 0,27-1-1275 0 0,-6-27-165 0 0,7-1 0 0 0,12-10-60 0 0,-19 1-2985 0 0,-17 8-1180 0 0,-7 1 2595 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27">10783 697 2760 0 0,'0'1'207'0'0,"0"45"6763"0"0,0-45-5925 0 0,0-1-21 0 0,2 8 598 0 0,2 13-344 0 0,-2 0 0 0 0,0-1 1 0 0,-2 2-1 0 0,0-1 1 0 0,-1 0-1 0 0,-2 9-1278 0 0,-12 63 616 0 0,0-18 973 0 0,13 38-2158 0 0,3-86 962 0 0,-3-26-377 0 0,2-1-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28">10847 690 3224 0 0,'-2'-5'1144'0'0,"5"-6"9068"0"0,-2 6-10979 0 0,0 4 1696 0 0,1-1-81 0 0,57-25 1867 0 0,-54 27-2559 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 1 0 0 0,2 0-156 0 0,-1 0 96 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 2-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1-95 0 0,-1-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,-4 5-94 0 0,-43 58 1952 0 0,47-67-2012 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0-1 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0-2-1 0 0,0 2 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 1 0 0,-1-2 59 0 0,3 4-75 0 0,-8-6-2618 0 0,5-2 1170 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">133 475 12696 0 0,'0'0'289'0'0,"0"0"40"0"0,0 0 21 0 0,0 0-45 0 0,0 0-17 0 0,0 0 663 0 0,0 0 305 0 0,0 0 65 0 0,0 0-144 0 0,0 0-658 0 0,0 0-287 0 0,0 0-59 0 0,0 0-54 0 0,0 0-181 0 0,0 0-76 0 0,0 0-20 0 0,0 0-48 0 0,0 0-197 0 0,0 0-86 0 0,0 0-1146 0 0,0 0-4503 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1">345 486 6912 0 0,'0'0'528'0'0,"0"0"-150"0"0,0 0 637 0 0,-1-1 198 0 0,-1-5 10039 0 0,2 2-11103 0 0,-1-1-133 0 0,1 1-129 0 0,0 4-468 0 0,0 0-177 0 0,0 0-770 0 0,0 0-3111 0 0,0 0-1333 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2">558 448 11976 0 0,'0'3'296'0'0,"-4"3"4551"0"0,3-3-506 0 0,1-2-3562 0 0,-1 2-7280 0 0,1-3-277 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3">745 501 13328 0 0,'0'0'298'0'0,"0"0"46"0"0,0 0 24 0 0,0 0-38 0 0,0 0-129 0 0,0 0 272 0 0,1-2 7070 0 0,1-5-6507 0 0,1-14-839 0 0,-3 20-358 0 0,0 1-21 0 0,0 0 46 0 0,0 0 202 0 0,0 1 87 0 0,-7 51 971 0 0,6-51-904 0 0,1-1-57 0 0,0 0-17 0 0,0 0-10 0 0,0 0-21 0 0,0 0 36 0 0,0 0 17 0 0,0 0-40 0 0,2-10-522 0 0,2-19 325 0 0,-4 28 218 0 0,0 1 13 0 0,4-2-260 0 0,-1 4-230 0 0,-2 1 347 0 0,-6 23 365 0 0,4-25-139 0 0,1-1-27 0 0,0 0-161 0 0,0 0-194 0 0,-6-7-214 0 0,12-29 40 0 0,0 31 757 0 0,-5 5-562 0 0,-1 0-34 0 0,7 9 96 0 0,-12 34 294 0 0,5-41 48 0 0,0-2-24 0 0,-7 6 14 0 0,7-6-266 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,-1 2-12 0 0,0-2-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 1 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1-3 1 0 0,10-12-798 0 0,-4 16 705 0 0,6 10 39 0 0,-10-8 64 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 2-10 0 0,1-3 84 0 0,-3 11 237 0 0,-10-6-89 0 0,12-6-144 0 0,1 0 0 0 0,-3-7-1050 0 0,1-6-3857 0 0,1 7-3207 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4">904 317 7800 0 0,'0'0'174'0'0,"0"0"29"0"0,0 5 198 0 0,4 36 3341 0 0,1-21-2076 0 0,-3 34 1115 0 0,2 10 113 0 0,-2-8-1404 0 0,-1 32 981 0 0,-1-1-1688 0 0,0-38-1417 0 0,-1-21 962 0 0,-4-18-2248 0 0,2-4-5035 0 0,3-6 5419 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5">870 405 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-49 0 0,0 0 491 0 0,0-1 240 0 0,8-20 2722 0 0,-8 19-3180 0 0,8-9 1008 0 0,12-15 674 0 0,-18 22-2057 0 0,0 2 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,2 0-137 0 0,35 12 1009 0 0,-28 9 55 0 0,-2-11-600 0 0,11 31 1448 0 0,-11 0-2113 0 0,-9-38 230 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1-29 0 0,1-2 5 0 0,-5 14 399 0 0,0-7-337 0 0,5-5-104 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-2 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 37 0 0,-20-1 653 0 0,-3-17-4978 0 0,18 13 2334 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6">1619 294 7488 0 0,'0'0'166'0'0,"0"5"236"0"0,2 31 1154 0 0,-6 15 2052 0 0,-2 22 1755 0 0,1 34-2463 0 0,3-36-962 0 0,-2 21-1172 0 0,4-90-851 0 0,0-2-91 0 0,0 0-16 0 0,0 7-2832 0 0,-1 8-2556 0 0,0-14 1622 0 0,1-1-894 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7">1628 332 9848 0 0,'0'0'222'0'0,"0"0"30"0"0,0 0 19 0 0,7-5 8 0 0,2-2 772 0 0,-9 7-801 0 0,1-2 0 0 0,0 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0-250 0 0,4 3 395 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1 1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 2 1 0 0,1 2-396 0 0,-4-5 170 0 0,1 1 5 0 0,-1 0-1 0 0,0 1 0 0 0,0-1 1 0 0,0 2-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1-174 0 0,-1 22 278 0 0,-1-26-199 0 0,1-1 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,1 0-1 0 0,-2 0 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1-79 0 0,-1 0 4 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-2 0 0 0,1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-2 0 0 0,-1 0-4 0 0,-29-28-4198 0 0,30 26-3651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8">1201 97 3680 0 0,'-3'31'613'0'0,"0"-6"6816"0"0,-3 15-4591 0 0,4 11-23 0 0,2-9-297 0 0,3 2-1604 0 0,-6 62 2 0 0,5-50 200 0 0,0-11-716 0 0,1-28-126 0 0,-3-13-115 0 0,-2 1-1048 0 0,1 2-4224 0 0,1-7 3723 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9">1160 468 1376 0 0,'3'-13'2159'0'0,"1"0"4223"0"0,4-4-3735 0 0,-3 4-1523 0 0,8-11 1153 0 0,1 8 523 0 0,-1 1-1591 0 0,11-10 135 0 0,-23 24-1294 0 0,-1 1 1 0 0,1-1-1 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0 0-51 0 0,1 2 27 0 0,2 1 1 0 0,-2 0-1 0 0,1 1 1 0 0,0-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,0 1 1 0 0,-1-2 0 0 0,0 1-1 0 0,0 1 1 0 0,1-2-1 0 0,-1 5-27 0 0,5 20 368 0 0,16 78 1443 0 0,-10-81-1634 0 0,-1-9-84 0 0,-6-15-77 0 0,-4-2-29 0 0,1 0-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1-2 0 0 0,1 2 0 0 0,0-2-1 0 0,-1 2 1 0 0,1-2 13 0 0,21-17-350 0 0,11-8-3834 0 0,-30 23 2533 0 0,2 2-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10">1 213 6448 0 0,'4'13'6309'0'0,"-4"-11"-6682"0"0,2 36 3514 0 0,4 53-847 0 0,0-27-690 0 0,-3-6-929 0 0,6 85 737 0 0,-15 20 57 0 0,4-113-1337 0 0,-2-32-256 0 0,4-8-955 0 0,0-8-4480 0 0,0-2-582 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11">7 233 6248 0 0,'0'8'190'0'0,"0"-15"349"0"0,10-25 6274 0 0,-10 31-6115 0 0,0 1-34 0 0,0 0-135 0 0,0 0-60 0 0,0 0-12 0 0,0 0-15 0 0,6-2 291 0 0,39-12 828 0 0,-21 4-729 0 0,7-4 96 0 0,27 8 370 0 0,-32 6-222 0 0,22 0-1079 0 0,-11-3 16 0 0,20-13 451 0 0,-17 9 1144 0 0,34 2-1448 0 0,1 11 224 0 0,-28-12-645 0 0,-16 0 1538 0 0,3-1-1123 0 0,-20 6-292 0 0,29 0 264 0 0,-14-5 20 0 0,29-16 70 0 0,6 12-205 0 0,6 5 34 0 0,-35-2 219 0 0,12-3-424 0 0,-2 7 192 0 0,-6 4 584 0 0,24 0-1352 0 0,-4 6 736 0 0,0 4 1017 0 0,-17-6-298 0 0,-6-1-1239 0 0,13-2 520 0 0,9 2 64 0 0,6 19 75 0 0,-32-7-166 0 0,7 0 523 0 0,-1-6-840 0 0,-12-3 749 0 0,-4-3-675 0 0,14 5 487 0 0,39-7-197 0 0,-11 13 0 0 0,-23-9-20 0 0,-23-2 0 0 0,-7-4 0 0 0,13 12 0 0 0,-20-2 0 0 0,2 3 0 0 0,8 16 64 0 0,-3 17 0 0 0,-5 16-64 0 0,-2 21-8 0 0,0-34 125 0 0,-2 22-203 0 0,-4 21 295 0 0,4 29-190 0 0,-9-55 82 0 0,0-26-13 0 0,3-29 96 0 0,2-8-234 0 0,1 1-1 0 0,0-2 1 0 0,0 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-2 0 1 0 0,2 0 0 0 0,-1 0-1 0 0,-1 2 51 0 0,0-3 114 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,-1-2-1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1-114 0 0,-8-1 158 0 0,-52 6-218 0 0,44-3 59 0 0,-1 0-1 0 0,1-1 1 0 0,-1-1 0 0 0,1-1-1 0 0,-1-1 1 0 0,-11-4 1 0 0,2-3-9 0 0,-1 3 0 0 0,1 1 0 0 0,-1 2 0 0 0,-12 1 9 0 0,-59 0 332 0 0,74 3-330 0 0,0-1-1 0 0,0-2 1 0 0,0-2-1 0 0,0 1 1 0 0,-4-6-2 0 0,12 6-18 0 0,-1 2 0 0 0,1 0 0 0 0,0 1 0 0 0,-11 3 18 0 0,-78 19 64 0 0,-1-7-136 0 0,-26-7 152 0 0,93-8-80 0 0,-50 0 11 0 0,-17-11 42 0 0,54 11-53 0 0,-13-8 80 0 0,13-8-176 0 0,-47-11 224 0 0,32 13-196 0 0,32 5 192 0 0,-32-2-124 0 0,26 7 0 0 0,26 9-499 0 0,16-5 309 0 0,2 0-9 0 0,0 0-85 0 0,0 0-352 0 0,0 0-151 0 0,0 0-27 0 0,0 0-202 0 0,0 0-812 0 0,0 0-343 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14">3614 600 11720 0 0,'0'0'532'0'0,"0"0"-4"0"0,2 1 218 0 0,0 0 5134 0 0,11-10-8855 0 0,-9 7 1888 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="15">3816 628 10592 0 0,'-7'-8'818'0'0,"6"5"-344"0"0,1 3 530 0 0,0 0 290 0 0,0 0 61 0 0,0-4 606 0 0,0 2 1568 0 0,8-1-8082 0 0,-3 1-1569 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16">4004 570 11976 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 15 0 0,0 0-26 0 0,0 0-59 0 0,0 0 490 0 0,0 0 240 0 0,0 0 43 0 0,0 0-1 0 0,0 0-42 0 0,0 0-11 0 0,0 0-6 0 0,3 0-232 0 0,-1 0-5476 0 0,-2 0-2114 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17">4199 628 1376 0 0,'0'0'415'0'0,"0"0"1203"0"0,0 0 529 0 0,0 0 106 0 0,0 0-174 0 0,0 0-807 0 0,0 0-360 0 0,0 0-72 0 0,0 0-72 0 0,-4-9 464 0 0,6-26 1231 0 0,0 30-2463 0 0,0 0 0 0 0,1 1 52 0 0,-2 4 215 0 0,-1 0 78 0 0,0 0 9 0 0,0 0-24 0 0,0 0-116 0 0,4 5 88 0 0,-4-2-189 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-1 2 0 0 0,0-3 0 0 0,-1 1 0 0 0,0 2-113 0 0,1-2 41 0 0,1-2 0 0 0,0 2 0 0 0,-1-2 0 0 0,1 2 1 0 0,0-2-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-2 1 0 0 0,2-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-2 0 0 0 0,2-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0 0 1 0 0,0-2-42 0 0,-5-10 194 0 0,14-11-143 0 0,-8 22-62 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,2 1 0 0 0,-2-1-1 0 0,1 2 1 0 0,0-2 0 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,-1 1 11 0 0,1-2-43 0 0,1 1 32 0 0,1 7 23 0 0,-6 12 200 0 0,2-18-96 0 0,-4 2-695 0 0,8-4-611 0 0,4-6-5710 0 0,-4 3 446 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="18">4352 388 6560 0 0,'0'0'298'0'0,"0"0"-3"0"0,1 5-221 0 0,0-3 4251 0 0,6 15-45 0 0,-6-16-3788 0 0,1 5 1039 0 0,2 54 1637 0 0,3 54-1221 0 0,-7-56-1606 0 0,0-52-341 0 0,-1-2-56 0 0,1-3-228 0 0,0-1-73 0 0,0 0-10 0 0,0 0-249 0 0,0 0-1040 0 0,0 0-440 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="19">4514 415 2760 0 0,'2'5'1828'0'0,"2"13"4892"0"0,3 17-3444 0 0,1 66 1947 0 0,-7-51-3937 0 0,-2-25-4508 0 0,1-23 1701 0 0,-2 4-229 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="20">4542 628 6248 0 0,'0'0'282'0'0,"0"0"-2"0"0,0 0-181 0 0,5-26 5734 0 0,2-8-521 0 0,-10 14-3279 0 0,7 7-1202 0 0,4-25 1 0 0,-7 36-738 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 2 1 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,2 1-93 0 0,1-2 95 0 0,-3 2-21 0 0,15 0-60 0 0,0 9-14 0 0,-2 4 0 0 0,-12-7 0 0 0,7 15 0 0 0,9 48 514 0 0,-10-34 356 0 0,3-12-278 0 0,-10-22-517 0 0,3 1 98 0 0,-2 0-141 0 0,-1-1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1-1 0 0,1 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,2 1-32 0 0,11-3-185 0 0,-2-18-4233 0 0,-12 20 2840 0 0,0 1-164 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="21">4966 451 1376 0 0,'0'0'65'0'0,"0"0"158"0"0,0 0 638 0 0,0 0 277 0 0,0 0 56 0 0,0 0-54 0 0,0 0-277 0 0,0 0-119 0 0,0 0-28 0 0,0 0-99 0 0,0 0-329 0 0,0 0 112 0 0,0 0 89 0 0,0 0 21 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,1-1 102 0 0,-1 1-405 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1-82 0 0,-6-2-143 0 0,-21-3 1747 0 0,23 5-1667 0 0,3-1 170 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,2 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0 0-107 0 0,-19 27-483 0 0,9 2 618 0 0,10 7 378 0 0,4 3-513 0 0,9-2 1899 0 0,14-8-1734 0 0,-6-11-165 0 0,-11-13 0 0 0,8 0 0 0 0,-11-6 0 0 0,-2 2 0 0 0,0-4-64 0 0,17-14-5497 0 0,-18 11 3530 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="22">5108 668 3680 0 0,'0'0'284'0'0,"0"0"103"0"0,0 0 1126 0 0,0 0 513 0 0,0 0 101 0 0,0 0-166 0 0,0 0-759 0 0,0 0-333 0 0,0 0-65 0 0,0 0-75 0 0,0 0-243 0 0,1-4 907 0 0,6-12 649 0 0,-5 13-2004 0 0,-1 2 164 0 0,-1 1 104 0 0,0 0 22 0 0,0 0-26 0 0,0 0-132 0 0,0 0-61 0 0,0 0-12 0 0,0 0 3 0 0,0 0 16 0 0,5 13 784 0 0,-8 9 56 0 0,3-22-836 0 0,0 0 10 0 0,0 0-41 0 0,0 0-176 0 0,0 0-27 0 0,0 0 8 0 0,0 0 2 0 0,0 0 0 0 0,0 0 0 0 0,0 0-56 0 0,0 0-234 0 0,0 0-101 0 0,0 0-889 0 0,0 0-3668 0 0,0 0-1566 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="23">5255 446 1840 0 0,'0'4'396'0'0,"0"-3"991"0"0,0-1 433 0 0,0 0 89 0 0,0 0-127 0 0,0 0-576 0 0,-2 1 2724 0 0,3 1-2482 0 0,0-2-958 0 0,-1 0-3 0 0,0 0-16 0 0,0 0-75 0 0,0 0-39 0 0,0 0-5 0 0,0 0-6 0 0,0 0-30 0 0,0 0-18 0 0,4 12 886 0 0,2 46 1352 0 0,-2-34-2105 0 0,-5 40 686 0 0,-1-3-314 0 0,1 43-530 0 0,4-73-273 0 0,-2-6 0 0 0,-3-9-45 0 0,2-15-194 0 0,0-1-94 0 0,0 0-19 0 0,-1-9-1557 0 0,0 0 195 0 0,-1-2-70 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="24">5236 448 1376 0 0,'3'4'367'0'0,"-3"-4"1002"0"0,0 0 440 0 0,0 0 88 0 0,0 0-1763 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0-133 0 0,5-3 51 0 0,18-16 1588 0 0,-16 15-1245 0 0,-6 4-294 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0 0-100 0 0,2 2 108 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 4-108 0 0,5 18 435 0 0,0 37 787 0 0,-6-53-980 0 0,0-8-186 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0-1 0 0 0,0 0 0 0 0,0 2 0 0 0,0-2 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0-56 0 0,-24 23 929 0 0,23-22-879 0 0,1-2-45 0 0,0 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-2 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1-5 0 0,-1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,0-4 0 0 0,2-10-5381 0 0,0 10-2125 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="25">5493 273 0 0 0,'-7'8'0'0'0,"4"-10"140"0"0,2 2 2586 0 0,1 0 5496 0 0,8 13-7158 0 0,-7-13-552 0 0,4 20 3000 0 0,-8 21-1947 0 0,1 32 181 0 0,2 0 624 0 0,-4-26-881 0 0,6 25-1316 0 0,-6-17-173 0 0,4-29 0 0 0,7 2-2476 0 0,-6-26 2128 0 0,-1-1 173 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,-1-1-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,0 0-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 1 175 0 0,-1-1-2221 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26">5483 553 4376 0 0,'0'0'199'0'0,"6"-7"1918"0"0,-4-2 1016 0 0,6-6 683 0 0,-3-8-1297 0 0,-2-1-472 0 0,4 18-1272 0 0,-6 6-743 0 0,0-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1 0-33 0 0,3 0 304 0 0,11 15 598 0 0,-13-11-674 0 0,0-1-1 0 0,-1 1 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,-2-1 1 0 0,1 0-1 0 0,1 4-227 0 0,3 60 608 0 0,-4-42-165 0 0,-1-8 997 0 0,16-1-1275 0 0,-5-17-165 0 0,5-1 0 0 0,6-7-60 0 0,-10 1-2985 0 0,-9 6-1180 0 0,-4 0 2595 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="27">5821 470 2760 0 0,'0'1'207'0'0,"0"29"6763"0"0,0-30-5925 0 0,0 0-21 0 0,1 6 598 0 0,1 7-344 0 0,-1 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,-2 5-1278 0 0,-6 42 616 0 0,0-12 973 0 0,7 24-2158 0 0,2-55 962 0 0,-3-18-377 0 0,2 0-672 0 0,0 0-294 0 0,0 0-834 0 0,0 0-3260 0 0,0 0-1393 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="28">5856 466 3224 0 0,'-2'-4'1144'0'0,"4"-3"9068"0"0,-1 4-10979 0 0,-1 2 1696 0 0,1 0-81 0 0,31-17 1867 0 0,-29 18-2559 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 1-156 0 0,0-1 96 0 0,0 1-1 0 0,0 0 0 0 0,0-1 1 0 0,-1 2-1 0 0,1-2 1 0 0,-1 1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1-95 0 0,-1-1 94 0 0,1 0 0 0 0,-2 0 0 0 0,1-1-1 0 0,0 2 1 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,-2 4-94 0 0,-23 37 1952 0 0,25-43-2012 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,0 0-1 0 0,-1-1 0 0 0,0 0 1 0 0,1 1-1 0 0,0 0 0 0 0,0-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0-1 1 0 0,-1 0 59 0 0,2 2-75 0 0,-4-4-2618 0 0,2-1 1170 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1692,7 +1753,7 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 10136 0 0,'0'0'224'0'0,"0"0"40"0"0,0 0 16 0 0,0 0 8 0 0,0 0-288 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 672 0 0,0 0 88 0 0,0 9 8 0 0,0-9 8 0 0,0 0-424 0 0,0 0-80 0 0,0 0-16 0 0,0 0-8 0 0,0 0-1016 0 0,0 0-208 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 10136 0 0,'0'0'224'0'0,"0"0"40"0"0,0 0 16 0 0,0 0 8 0 0,0 0-288 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 672 0 0,0 0 88 0 0,0 6 8 0 0,0-6 8 0 0,0 0-424 0 0,0 0-80 0 0,0 0-16 0 0,0 0-8 0 0,0 0-1016 0 0,0 0-208 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1724,7 +1785,7 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">170 617 2760 0 0,'-22'-8'3128'0'0,"16"-1"-821"0"0,-31-61 5175 0 0,-4-49-4528 0 0,19 36-2212 0 0,-1 5-684 0 0,12 38 1037 0 0,3 9-46 0 0,8-12-1018 0 0,16 29 738 0 0,31-3 95 0 0,18-8-285 0 0,21 11 18 0 0,41-6 553 0 0,-102 9-836 0 0,25-13-4 0 0,8 13-300 0 0,11 18-3179 0 0,-62-7 1586 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">92 402 2760 0 0,'-12'-5'3128'0'0,"9"-1"-821"0"0,-17-40 5175 0 0,-2-31-4528 0 0,10 23-2212 0 0,-1 3-684 0 0,7 25 1037 0 0,2 6-46 0 0,4-8-1018 0 0,9 18 738 0 0,16-1 95 0 0,10-5-285 0 0,12 7 18 0 0,21-4 553 0 0,-54 6-836 0 0,13-9-4 0 0,4 9-300 0 0,6 12-3179 0 0,-33-5 1586 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1755,7 +1816,7 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">38 1 16096 0 0,'0'0'365'0'0,"0"0"56"0"0,-7 12 546 0 0,0-3 6082 0 0,3-1-4429 0 0,-3 13-3843 0 0,6-18 1887 0 0,-10 29-320 0 0,10-31-280 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-22 0 0,0 0-119 0 0,0-8-220 0 0,2-18-184 0 0,0 13-1091 0 0,-2 0-4490 0 0,0 13-914 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">21 1 16096 0 0,'0'0'365'0'0,"0"0"56"0"0,-4 8 546 0 0,0-2 6082 0 0,2-1-4429 0 0,-2 9-3843 0 0,3-12 1887 0 0,-4 18-320 0 0,4-19-280 0 0,1-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-22 0 0,0 0-119 0 0,0-5-220 0 0,1-12-184 0 0,0 8-1091 0 0,-1 1-4490 0 0,0 8-914 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1786,10 +1847,10 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">139 53 9728 0 0,'-3'29'446'0'0,"2"-23"-10"0"0,1-6-110 0 0,-7 21 5217 0 0,-4 39-376 0 0,-11 67-1014 0 0,-9 218-706 0 0,15-150-2342 0 0,10-97-825 0 0,-9 103-24 0 0,11-172-383 0 0,3-28-26 0 0,1-1-8 0 0,0 0-161 0 0,0 0-650 0 0,1-25-9059 0 0,3 6 1774 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="639.092">110 193 11776 0 0,'6'-17'1280'0'0,"0"-3"2430"0"0,2 2 2588 0 0,2 8-5875 0 0,-3 4 86 0 0,1-3-282 0 0,0 3 0 0 0,0-1 0 0 0,0 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,2 2 1 0 0,-1-1-1 0 0,0 0 0 0 0,1 1 1 0 0,9-2-228 0 0,42 10 628 0 0,-56-3-593 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 3-36 0 0,10 8 14 0 0,30 35 450 0 0,-14 3 1116 0 0,-2 60-1568 0 0,-28-101 95 0 0,0 0-1 0 0,0 0 0 0 0,-1 2 1 0 0,-1-2-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 2 1 0 0,-1-1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-7 8-106 0 0,7-11 49 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,-1 1 1 0 0,1-2-1 0 0,-1 0 0 0 0,0-1 1 0 0,-3 2-50 0 0,-52 13 153 0 0,56-17-165 0 0,63-9 9 0 0,-45 9 6 0 0,-5-2-28 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 2-1 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,3 2 25 0 0,-1 0-62 0 0,-1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 2 1 0 0,0-2-1 0 0,0 3 62 0 0,5 55 641 0 0,-9-58-617 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 1 1 0 0,-1-2 0 0 0,0 1 0 0 0,-2 3-24 0 0,-6 8 0 0 0,-1 1 0 0 0,0-2 0 0 0,-2-1 0 0 0,1 1 0 0 0,-2-2 0 0 0,0 0 0 0 0,-13 9 0 0 0,8-9 0 0 0,-1-2 0 0 0,-1 1 0 0 0,0-2 0 0 0,0-1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-8-1 0 0 0,-74 23-80 0 0,17-6-16 0 0,86-25 358 0 0,-7 1-2469 0 0,5-10-7469 0 0,4 0 1106 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1210.204">893 1 14456 0 0,'0'0'330'0'0,"0"0"45"0"0,0 0 18 0 0,0 0-42 0 0,0 1-75 0 0,-3 74 6166 0 0,-5-10-4114 0 0,-18 145 1352 0 0,-4 59-2060 0 0,-11 15-805 0 0,7-76-674 0 0,26-181-350 0 0,8-26 82 0 0,-11-12-1918 0 0,6-8-4504 0 0,5 15 4273 0 0,-2-9-6349 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1636.656">935 118 1376 0 0,'7'-37'68'0'0,"7"3"5954"0"0,-5 13 1686 0 0,-8 20-7576 0 0,-1-2 0 0 0,0 2 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0-1 0 0,0 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 1-132 0 0,0 0 58 0 0,0 1 33 0 0,0-1-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,-1 1 1 0 0,0-1 0 0 0,1 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,2 0-91 0 0,2 0 102 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,0 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,-1 0-1 0 0,1 1 1 0 0,2 4-103 0 0,6 12 174 0 0,-10-14-111 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,1-1 1 0 0,-1 0 0 0 0,3 1-63 0 0,34 22 581 0 0,7 34 291 0 0,-42-31-651 0 0,-1-2-1 0 0,-2 3 0 0 0,0-1 1 0 0,-2-1-1 0 0,-2 1 1 0 0,0 0-1 0 0,-2-1 1 0 0,-1 1-1 0 0,-8 28-220 0 0,6-21 236 0 0,-2 1 0 0 0,-1-3 0 0 0,-1 2 0 0 0,-5 5-236 0 0,-23 56 424 0 0,30-83-365 0 0,1 2 31 0 0,-1 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-9 7-90 0 0,14-15 26 0 0,0 0-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0-1 1 0 0,-8 2-26 0 0,-115 9 33 0 0,-7-28-1057 0 0,71-9-4105 0 0,60 15 3206 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">75 35 9728 0 0,'-2'18'446'0'0,"2"-14"-10"0"0,0-4-110 0 0,-4 14 5217 0 0,-2 24-376 0 0,-6 44-1014 0 0,-4 140-706 0 0,7-96-2342 0 0,6-63-825 0 0,-5 67-24 0 0,5-111-383 0 0,3-19-26 0 0,0 0-8 0 0,0 0-161 0 0,0 0-650 0 0,0-16-9059 0 0,3 4 1774 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="639.092">59 125 11776 0 0,'4'-11'1280'0'0,"-1"-2"2430"0"0,1 1 2588 0 0,2 6-5875 0 0,-3 2 86 0 0,2-2-282 0 0,-1 2 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,6-1-228 0 0,21 7 628 0 0,-29-2-593 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1 0 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,-1 1-1 0 0,1 0 0 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,0 0 0 0 0,-1-1 1 0 0,1 3-36 0 0,6 4 14 0 0,16 24 450 0 0,-8 1 1116 0 0,-1 39-1568 0 0,-15-66 95 0 0,0 1-1 0 0,0 0 0 0 0,0 1 1 0 0,-2-1-1 0 0,1-1 1 0 0,0 0-1 0 0,-1 2 1 0 0,0-2-1 0 0,0 1 1 0 0,-1-1-1 0 0,0 0 1 0 0,1 0-1 0 0,-5 6-106 0 0,5-8 49 0 0,-1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,0 1-1 0 0,-1-1 0 0 0,0 2 1 0 0,0-2-1 0 0,0-1 0 0 0,-1 1 1 0 0,-1 0-50 0 0,-28 9 153 0 0,31-11-165 0 0,33-6 9 0 0,-24 6 6 0 0,-3-1-28 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,3 1 25 0 0,-2 0-62 0 0,1 0 1 0 0,-2 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1 1 1 0 0,-1-2-1 0 0,0 3 62 0 0,3 35 641 0 0,-5-38-617 0 0,-1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 1 1 0 0,0-2 0 0 0,-1 1 0 0 0,-1 2-24 0 0,-3 5 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,-7 5 0 0 0,4-5 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-2 0 0 0,-1 0 0 0 0,1 0 0 0 0,-5-1 0 0 0,-39 15-80 0 0,8-4-16 0 0,47-16 358 0 0,-4 1-2469 0 0,3-7-7469 0 0,2 0 1106 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1210.204">482 1 14456 0 0,'0'0'330'0'0,"0"0"45"0"0,0 0 18 0 0,0 0-42 0 0,0 1-75 0 0,-2 47 6166 0 0,-2-6-4114 0 0,-10 93 1352 0 0,-2 39-2060 0 0,-6 9-805 0 0,3-49-674 0 0,15-117-350 0 0,4-16 82 0 0,-6-8-1918 0 0,3-6-4504 0 0,3 11 4273 0 0,-1-7-6349 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1636.656">505 76 1376 0 0,'3'-23'68'0'0,"5"1"5954"0"0,-3 8 1686 0 0,-5 13-7576 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1-1 0 0,0-1 1 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 1 1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1 0 0 0,-1 0-132 0 0,1 1 58 0 0,-1 0 33 0 0,1 0-1 0 0,-1-1 1 0 0,0 2 0 0 0,1-2-1 0 0,-1 1 1 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,2 0-91 0 0,1 0 102 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 2-1 0 0,1-1 1 0 0,-1-1-1 0 0,1 2 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,-1 0-1 0 0,2 0 1 0 0,0 3-103 0 0,3 8 174 0 0,-5-9-111 0 0,1-1 0 0 0,0 1 0 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,2-1 0 0 0,-1-1 0 0 0,0 2-1 0 0,1-2 1 0 0,-1 1 0 0 0,2 0-63 0 0,18 14 581 0 0,4 23 291 0 0,-23-21-651 0 0,0-1-1 0 0,-2 2 0 0 0,1-1 1 0 0,-2 0-1 0 0,0 0 1 0 0,-1 1-1 0 0,0-2 1 0 0,-2 2-1 0 0,-3 17-220 0 0,3-13 236 0 0,-2 0 0 0 0,1-1 0 0 0,-2 1 0 0 0,-2 3-236 0 0,-12 36 424 0 0,15-53-365 0 0,1 1 31 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,-1-2 0 0 0,1 0 0 0 0,-1 0 0 0 0,-5 5-90 0 0,7-10 26 0 0,1 0-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,-4 1-26 0 0,-63 6 33 0 0,-3-18-1057 0 0,39-6-4105 0 0,31 10 3206 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1820,8 +1881,8 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">100 9 3224 0 0,'0'0'457'0'0,"0"0"711"0"0,0 0 311 0 0,0 0 66 0 0,0 0-146 0 0,0 0-671 0 0,0 0-295 0 0,0 0-60 0 0,0 0 9 0 0,0 0 83 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,0 0 102 0 0,0 0 22 0 0,0 15 1235 0 0,-10 56 4955 0 0,4 27-4234 0 0,17 6-97 0 0,-9-47-1040 0 0,-3-30-1012 0 0,0 49-267 0 0,-5 178 1877 0 0,1-162-1879 0 0,6-83-48 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,0-2 0 0 0,-1 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-4 5 0 0 0,-11 13-801 0 0,-7-13-6747 0 0,18-17-982 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="412.914">107 89 2304 0 0,'0'-2'167'0'0,"8"-15"2093"0"0,18-21 9580 0 0,0 22-10365 0 0,-22 13-1240 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 1 0 0 0,0 0 0 0 0,0 0 0 0 0,3 2-235 0 0,-2-1 218 0 0,-1 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,3 6-217 0 0,5 8 528 0 0,-7-11-392 0 0,1 1-1 0 0,-2 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,0 1 1 0 0,0 0-1 0 0,0 3-135 0 0,-3 108 1604 0 0,-35-43-855 0 0,31-73-713 0 0,-1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,1 1-1 0 0,-1-2 0 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 1 0 0,1-1-1 0 0,-1 1 0 0 0,0-1-35 0 0,1-1-135 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-2 0 0 0 0,2 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1-1 0 0 0,-1 0 0 0 0,-4-4 136 0 0,6 5-520 0 0,1-1-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 0 0 0 0,-1 1 0 0 0,1-2 521 0 0,-5-26-2538 0 0,5 6-19 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">44 6 3224 0 0,'0'0'457'0'0,"0"0"711"0"0,0 0 311 0 0,0 0 66 0 0,0 0-146 0 0,0 0-671 0 0,0 0-295 0 0,0 0-60 0 0,0 0 9 0 0,0 0 83 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,0 0-220 0 0,0 0 164 0 0,0 0 102 0 0,0 0 22 0 0,0 9 1235 0 0,-5 37 4955 0 0,3 17-4234 0 0,7 3-97 0 0,-5-29-1040 0 0,0-20-1012 0 0,0 32-267 0 0,-3 113 1877 0 0,1-103-1879 0 0,2-53-48 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 3 0 0 0,-5 8-801 0 0,-4-8-6747 0 0,9-11-982 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="412.914">47 57 2304 0 0,'0'-1'167'0'0,"3"-10"2093"0"0,8-14 9580 0 0,1 15-10365 0 0,-11 8-1240 0 0,2 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 1 0 0 0,0 0 0 0 0,2 0-235 0 0,-2 1 218 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 1 0 0 0,-1-1 1 0 0,2 1-1 0 0,-2-1 0 0 0,1 1 1 0 0,0 0-1 0 0,-1 0 0 0 0,3 3-217 0 0,1 6 528 0 0,-3-8-392 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 3-135 0 0,-1 69 1604 0 0,-15-28-855 0 0,13-46-713 0 0,0 0-1 0 0,0-1 0 0 0,-1 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 0 1 0 0,-1-1-1 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0-1-1 0 0,0 0 0 0 0,0 0-35 0 0,0 0-135 0 0,0 0-1 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,2 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-1 1 0 0 0,-1-3 136 0 0,2 3-520 0 0,1-1-1 0 0,-1 1 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 0 0 0,-1-2 0 0 0,2 1 0 0 0,-1 1 1 0 0,0-2-1 0 0,0 1 0 0 0,1 1 0 0 0,-1-2 521 0 0,-2-17-2538 0 0,3 5-19 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1852,8 +1913,8 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">67 103 10592 0 0,'0'0'818'0'0,"-3"11"2010"0"0,-12 34 2029 0 0,4 26-1721 0 0,0 16-649 0 0,-5 120 1221 0 0,12-83-2576 0 0,4 9-475 0 0,-3-115-1193 0 0,2-17-68 0 0,1-1-32 0 0,0 0-79 0 0,0 0-314 0 0,-2-14-8176 0 0,1 7 1651 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="332.092">71 93 11520 0 0,'5'-11'1224'0'0,"26"-25"6290"0"0,34 0-4470 0 0,-62 34-2967 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 1 1 0 0,1-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,-1 2 0 0 0,1-2 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,2 2-77 0 0,4 16 316 0 0,0-2 0 0 0,-1 2 0 0 0,-1-1 0 0 0,-1 1 0 0 0,-1 0-1 0 0,-1 0 1 0 0,-1 1 0 0 0,0-1 0 0 0,-2 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,-2 5-316 0 0,2-14 99 0 0,0 1 1 0 0,-1-2-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 0-1 0 0,-1-1 1 0 0,0 1-1 0 0,-1-1 1 0 0,-3 6-100 0 0,5-12 18 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-2 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0 0 0 0,-1 0-18 0 0,-2-1-59 0 0,0 1 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,0 0 0 0 0,-7-4 59 0 0,-47-33-3704 0 0,55 31 957 0 0,5-2-5943 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">32 66 10592 0 0,'0'0'818'0'0,"-2"7"2010"0"0,-5 21 2029 0 0,2 17-1721 0 0,0 11-649 0 0,-3 76 1221 0 0,6-53-2576 0 0,2 5-475 0 0,-1-72-1193 0 0,0-12-68 0 0,1 0-32 0 0,0 0-79 0 0,0 0-314 0 0,-1-8-8176 0 0,1 3 1651 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="332.092">34 59 11520 0 0,'2'-7'1224'0'0,"13"-16"6290"0"0,15 0-4470 0 0,-28 22-2967 0 0,0 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 2 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 2 0 0 0,0-2 0 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 2-77 0 0,2 9 316 0 0,-1-1 0 0 0,1 1 0 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 0 0 0 0,-2 4-316 0 0,2-9 99 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,-1 0-1 0 0,-1 0 1 0 0,0 4-100 0 0,1-8 18 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0-18 0 0,-2 0-59 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-4-1 59 0 0,-22-22-3704 0 0,26 20 957 0 0,3-2-5943 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1884,8 +1945,8 @@
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">142 9 3224 0 0,'-2'-8'1623'0'0,"2"7"4003"0"0,-1 1 5780 0 0,-3 43-9766 0 0,-7 15-232 0 0,-4 47-776 0 0,7 16-182 0 0,-7 72 1156 0 0,16-178-1404 0 0,-2 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,-1 0 1 0 0,-5 14-202 0 0,9 65 272 0 0,-1-86-248 0 0,1-7-103 0 0,0-1-12 0 0,0 0-71 0 0,0 0-341 0 0,-19-4-7577 0 0,14-3 457 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="423.109">0 616 2304 0 0,'0'0'101'0'0,"6"-13"5654"0"0,-2 2-935 0 0,1-13-218 0 0,24-24-1523 0 0,28-18-965 0 0,0 8-1362 0 0,-55 56-723 0 0,-1 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,0 1 1 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0-1 0 0,-1-1 1 0 0,1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1-1 0 0 0,2 2-29 0 0,3 1 86 0 0,0 1-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,-1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-2 0-1 0 0,3 9-85 0 0,-8 82 1468 0 0,-2-80-1328 0 0,-4 13 188 0 0,1 0 0 0 0,2 1 1 0 0,1 0-1 0 0,2 0 0 0 0,1 18-328 0 0,17-53-374 0 0,15-39-3517 0 0,-22 27 1623 0 0,-1 4-436 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">77 6 3224 0 0,'-1'-5'1623'0'0,"1"4"4003"0"0,-1 1 5780 0 0,-1 28-9766 0 0,-4 10-232 0 0,-2 30-776 0 0,4 11-182 0 0,-5 47 1156 0 0,10-116-1404 0 0,-2 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,-3 9-202 0 0,5 42 272 0 0,0-56-248 0 0,0-4-103 0 0,0-1-12 0 0,0 0-71 0 0,0 0-341 0 0,-11-3-7577 0 0,9-1 457 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="423.109">0 401 2304 0 0,'0'0'101'0'0,"3"-8"5654"0"0,-1 1-935 0 0,1-9-218 0 0,13-15-1523 0 0,15-12-965 0 0,-1 5-1362 0 0,-29 37-723 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-1-1-1 0 0,0 2 1 0 0,0-2 0 0 0,0 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 1 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,1 2-29 0 0,2 1 86 0 0,0 0-1 0 0,-1 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0 0 0 0,0 2-1 0 0,-1-2 1 0 0,1 1-1 0 0,-1-1 1 0 0,0 2-1 0 0,0-1 1 0 0,0 0 0 0 0,-1 0-1 0 0,2 6-85 0 0,-5 54 1468 0 0,-1-53-1328 0 0,-2 9 188 0 0,1 0 0 0 0,1 0 1 0 0,0 1-1 0 0,1-1 0 0 0,1 12-328 0 0,9-34-374 0 0,9-26-3517 0 0,-13 18 1623 0 0,0 3-436 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1921,251 +1982,251 @@
       <inkml:brushProperty name="color" value="#E71224"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">22570 6625 0 0 0,'0'0'580'0'0,"0"0"-64"0"0,0 0 47 0 0,0 0-35 0 0,0 0-254 0 0,0 0-107 0 0,0 0-27 0 0,0 0 51 0 0,0 0 229 0 0,0 0 100 0 0,0 3 21 0 0,3 12 472 0 0,-3-13-554 0 0,0-2-3 0 0,0 0-54 0 0,0 0-223 0 0,0 0-98 0 0,0 0 51 0 0,0 0 272 0 0,0 0 95 0 0,0 0 12 0 0,0 0 1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 2 0 0 0,0 7 0 0 0,0-8 0 0 0,0-1 0 0 0,0 0 36 0 0,0 0 150 0 0,0 0 66 0 0,0 0 18 0 0,0 0-29 0 0,0 6 436 0 0,2 53 2189 0 0,-4 64-643 0 0,-8-38-852 0 0,-7 70-1718 0 0,15-52-165 0 0,1-95 90 0 0,0 1-403 0 0,1 9-2730 0 0,-4-30-1033 0 0,-1 3-2741 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="208.461">22566 6684 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,7-4-112 0 0,1 1 125 0 0,-2 1 1 0 0,1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,0 1-346 0 0,45 71 1246 0 0,-49-67-1102 0 0,1 0-1 0 0,-1 0 1 0 0,-1 1-1 0 0,1-1 1 0 0,-2 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,0-1-1 0 0,0 1 1 0 0,-1 1-1 0 0,0-1 1 0 0,0-2 0 0 0,0 1-1 0 0,-2 2 1 0 0,1-2-1 0 0,-1 2-143 0 0,2-3 57 0 0,-1-2 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,-2-2 0 0 0,2 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,-1-2 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,-2-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,2-1 1 0 0,-3 0 0 0 0,2 0 0 0 0,-2-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,0 0-57 0 0,-91-6-816 0 0,62-15-3738 0 0,27 13 2908 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55956.919">24026 16033 456 0 0,'22'-42'0'0'0,"-7"27"2824"0"0,-6 4 664 0 0,-8 11-2678 0 0,-1 0 44 0 0,0 0 11 0 0,0 0 6 0 0,0 0 21 0 0,0 0 85 0 0,0 0 42 0 0,0 0 5 0 0,0 0-70 0 0,3-22 2411 0 0,-17 3-1851 0 0,13 17-1397 0 0,-1-1 0 0 0,-1 1 1 0 0,2 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,1-2-1 0 0,-1 2 0 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,1-1 1 0 0,-2 1-1 0 0,2-1 0 0 0,0 1 1 0 0,-2 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,0 0 0 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 0-1 0 0,2 1 0 0 0,-2 0-117 0 0,-3 2 139 0 0,0 0 0 0 0,0 0 0 0 0,0 1-1 0 0,1 0 1 0 0,0 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,0 0 0 0 0,1 1-1 0 0,-1 0 1 0 0,-3 6-139 0 0,-18 35 224 0 0,-6 47 448 0 0,32 5 696 0 0,1-96-1368 0 0,0 1-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,2 1 1 0 0,-2-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0 0 0 0 0,1-1 1 0 0,-1 0-1 0 0,0 0 0 0 0,1 0 1 0 0,0 0 0 0 0,-2-1 16 0 0,1 0 1 0 0,1-1-1 0 0,-2 0 0 0 0,1 0 1 0 0,0 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-2 0-1 0 0,1-1 0 0 0,1-1 1 0 0,-1 2-1 0 0,1-1 0 0 0,-1 0 1 0 0,1 0-1 0 0,0-1 0 0 0,-2 1 1 0 0,2 0-1 0 0,0-1 0 0 0,0 0-16 0 0,4 0-124 0 0,-1 0-1 0 0,2 0 0 0 0,-1-1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0-1 1 0 0,1-1-1 0 0,-2 0 0 0 0,2 0 0 0 0,-2-2 0 0 0,2 1 0 0 0,-2 0 125 0 0,12-6-613 0 0,19-16-2912 0 0,-19 11 1494 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55516.919">24367 15714 5984 0 0,'3'-43'472'0'0,"-2"2"5162"0"0,-1 39-3819 0 0,0 2-663 0 0,0 0-288 0 0,0 0-58 0 0,0 0-20 0 0,0 0-61 0 0,0 0-21 0 0,0 0-7 0 0,-8 5 1975 0 0,-17 111 1356 0 0,-27 213-3264 0 0,28-146-640 0 0,8-28-1060 0 0,15-138-1236 0 0,1-12-5747 0 0,0-5 911 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55296.919">24312 15896 9216 0 0,'0'0'706'0'0,"0"0"-114"0"0,4-5 3675 0 0,19-10 1993 0 0,16 4-3644 0 0,12-4-1858 0 0,4 19-1979 0 0,-50 6-2143 0 0,-2-1 1389 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-66366.92">23037 15459 6304 0 0,'14'-1'822'0'0,"-14"0"-83"0"0,0 1 249 0 0,0 0 48 0 0,0 0-31 0 0,0 0-170 0 0,0 0-71 0 0,0 0-17 0 0,0 0-27 0 0,0 0-102 0 0,0 0-46 0 0,0 0-10 0 0,0 0-16 0 0,0 0-57 0 0,0 0-29 0 0,0 0-4 0 0,0 0 48 0 0,0 0 202 0 0,0 0 87 0 0,0 0 20 0 0,0 0-70 0 0,0 0-308 0 0,-1-1-137 0 0,-48-67 1234 0 0,-30 3 383 0 0,74 62-1902 0 0,-2 0 0 0 0,1 1 1 0 0,2-1-1 0 0,-3 0 0 0 0,1 2 1 0 0,1-1-1 0 0,-2 1 0 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 1 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0 1 1 0 0,-1 1-1 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 1 0 0,1 1-1 0 0,-1 0 0 0 0,2 1 1 0 0,-7 2-14 0 0,-28 33 373 0 0,8 1-682 0 0,-13 59 985 0 0,27-17-666 0 0,-1 45 460 0 0,16 10-108 0 0,13-13-298 0 0,19 16-7518 0 0,-26-132 13 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-66056.919">22584 15862 11976 0 0,'0'0'546'0'0,"4"-11"204"0"0,14 5 2195 0 0,36-9 2019 0 0,25-2-3091 0 0,-37 20-1743 0 0,0 1 0 0 0,-1 0 1 0 0,27 9-131 0 0,-21 1-3223 0 0,-33-10 2016 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-65316.919">23086 16078 920 0 0,'1'-3'80'0'0,"-1"2"-114"0"0,9-21 1775 0 0,19-25 8599 0 0,-13 37-9435 0 0,-2 2-70 0 0,-11 6-714 0 0,0 1 1 0 0,1 0-1 0 0,-1-2 1 0 0,-1 1 0 0 0,2 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 1 0 0,1 1 0 0 0,1 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1-1 0 0,-1 0 1 0 0,2 0 0 0 0,-2 0-1 0 0,0 0 1 0 0,1 0-1 0 0,1 2-121 0 0,30 31 1528 0 0,-17 31 812 0 0,-18-57-2114 0 0,0-1 0 0 0,-1 3 0 0 0,-1-2 0 0 0,1 0 0 0 0,0 1 0 0 0,-2-1 0 0 0,1 0 0 0 0,1 0 0 0 0,-3-1 0 0 0,1 0-226 0 0,-1-3 108 0 0,2 1 0 0 0,-1 0-1 0 0,0-1 1 0 0,-1-1 0 0 0,0 1 0 0 0,1-1-1 0 0,-2 0 1 0 0,2-1 0 0 0,-2 1 0 0 0,2-1-1 0 0,-2 0 1 0 0,0 1 0 0 0,1-1-1 0 0,0-1 1 0 0,-6 1-108 0 0,6-3-56 0 0,2 1 0 0 0,-1-1-1 0 0,0 0 1 0 0,-1 0 0 0 0,2-1-1 0 0,-1 0 1 0 0,0 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,0 0 0 0 0,0 0-1 0 0,2-1 1 0 0,-2 1 0 0 0,1-1-1 0 0,0 0 1 0 0,0 0 0 0 0,1-2-1 0 0,0 2 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 0 0 0 0,1 1 0 0 0,-2-1-1 0 0,2-1 1 0 0,-1 2 0 0 0,1-2-1 0 0,0 1 1 0 0,0-2 56 0 0,1-36-2485 0 0,3 23 635 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-57246.919">23427 15892 9616 0 0,'0'0'216'0'0,"0"0"32"0"0,1-2 12 0 0,9-23 16 0 0,8-32 4156 0 0,-18 55-3764 0 0,0 2 151 0 0,0 0 69 0 0,0 0 10 0 0,0 0-48 0 0,0 0-216 0 0,0 0-98 0 0,0 0-22 0 0,-8 62 3070 0 0,4-6-2456 0 0,-12 163 920 0 0,16-150-2048 0 0,-1-23-64 0 0,1-45-273 0 0,0-1-138 0 0,0 0-33 0 0,0 0-217 0 0,0-8-2919 0 0,1-4 1541 0 0,2-1-9 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-56836.919">23370 16043 10136 0 0,'0'0'42'0'0,"0"1"-1"0"0,0-1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,0-1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 0-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,2 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0-1-1 0 0,0 1 1 0 0,0 0 0 0 0,0-2 0 0 0,0 2 0 0 0,0 0-1 0 0,0-1 1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-42 0 0,30-34 4246 0 0,11 4-1699 0 0,-37 26-2345 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-2 0 0 0 0,2 1 0 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 0 0 0,2 0-202 0 0,29 19 1351 0 0,-32-12-1230 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 2 0 0 0,-1-2 0 0 0,-1 1 0 0 0,2 5-121 0 0,23 82 144 0 0,-16 2-545 0 0,-19-81-269 0 0,5-10-1904 0 0,0-4-3466 0 0,0 0-762 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45426.919">24658 16075 456 0 0,'10'-3'13004'0'0,"-5"12"-6955"0"0,-9 20-4332 0 0,2-13-273 0 0,7 100-283 0 0,-3-75-2968 0 0,0 0-3416 0 0,-2-41-2002 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-45206.919">24739 15707 5984 0 0,'0'0'273'0'0,"0"0"-5"0"0,0 0 121 0 0,0 0 1143 0 0,0 0 514 0 0,0 0 104 0 0,0 0-119 0 0,0 0-596 0 0,0 0-261 0 0,0 0-49 0 0,0 0-98 0 0,0 0-392 0 0,0 0-171 0 0,0 0-31 0 0,0 0-64 0 0,0 0-1670 0 0,0 0-5837 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44826.919">24879 16349 11232 0 0,'0'-5'1016'0'0,"-18"-78"3747"0"0,28 13-109 0 0,-7 62-4545 0 0,0-1 0 0 0,0 2 0 0 0,1-1 0 0 0,-2 2 0 0 0,3-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,2-1 0 0 0,0 0 0 0 0,-2 3 0 0 0,2-1 0 0 0,3-1-109 0 0,-7 3 0 0 0,0 1 0 0 0,0 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,2 0 0 0 0,14 40 10 0 0,-16-31 52 0 0,-7 49 1898 0 0,-34 28-1744 0 0,35-85-173 0 0,1 0 0 0 0,0-1 0 0 0,0 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1 0 0 0,-2 0 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-2 0 0 0,-2 2-1 0 0,2-1 1 0 0,-1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,2 0 0 0 0,-5-1-43 0 0,3-1-36 0 0,-2 1 0 0 0,1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,0-2 0 0 0,1 1 0 0 0,0-1-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1-1 0 0 0,2 0-1 0 0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,1 0-1 0 0,1-1 1 0 0,-2 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 0-1 0 0,1-1 1 0 0,0 1 0 0 0,0-4 36 0 0,5-34-2989 0 0,1 24 1539 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-43876.919">25282 16126 456 0 0,'0'0'83'0'0,"0"0"42"0"0,0 0 131 0 0,0 0 32 0 0,0 0 0 0 0,0 0 49 0 0,0 0 209 0 0,0 0 94 0 0,0 0 21 0 0,0 0-5 0 0,0 0-33 0 0,0 0-14 0 0,0 0-1 0 0,0 0-74 0 0,0 0-307 0 0,0 0-135 0 0,0-1-36 0 0,9-37 684 0 0,-1-5 547 0 0,-5 18-691 0 0,-3-25 2561 0 0,0 49-2790 0 0,0 1 1 0 0,0 0 0 0 0,0 7 8134 0 0,-3 26-7718 0 0,-11 125 1476 0 0,0-85-2207 0 0,14-64-53 0 0,0-4-32 0 0,0-3-137 0 0,0-2-71 0 0,0 0-16 0 0,0 0-147 0 0,0 0-589 0 0,0 0-257 0 0,0 0-51 0 0,0 0-35 0 0,0 0-102 0 0,2 15-5517 0 0,-2-15 5738 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-43576.919">25288 16167 8952 0 0,'0'0'406'0'0,"0"0"-4"0"0,0 0-140 0 0,0 0 368 0 0,0 0 187 0 0,0 0 42 0 0,-6-6 963 0 0,5 2-1582 0 0,1-1 1 0 0,0-1-1 0 0,1 2 0 0 0,-1-1 1 0 0,0 0-1 0 0,1 0 0 0 0,1-1 0 0 0,-1 1 1 0 0,1 1-1 0 0,-1-1 0 0 0,1 0 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 2 0 0 0,0-2 0 0 0,-1 1 1 0 0,1 2-1 0 0,1-2 0 0 0,-1 0 0 0 0,4-3-240 0 0,-6 6 154 0 0,0 0-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,1-1 1 0 0,-2 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,1 0 1 0 0,-2 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-2 0 1 0 0,1 1-1 0 0,-1-1-153 0 0,7 4 222 0 0,18 14-38 0 0,-4 10-184 0 0,-20-24 130 0 0,0 0-1 0 0,-1 0 1 0 0,2 0-1 0 0,-2 0 0 0 0,0-1 1 0 0,0 2-1 0 0,-1-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 4-130 0 0,2 34 130 0 0,3-18-130 0 0,0-20-97 0 0,22-10-2811 0 0,-19 1 1087 0 0,1-3-377 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-1576.986">22100 6526 4608 0 0,'0'0'353'0'0,"5"10"155"0"0,-3-6 2425 0 0,9 28 3145 0 0,-9-10-3733 0 0,-11 23 1085 0 0,0 15-1742 0 0,3-7-736 0 0,11 43-312 0 0,-9-16-640 0 0,8-23 0 0 0,-16-9 0 0 0,12-43-9 0 0,0 0-146 0 0,0 0-4162 0 0,0-5-2729 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-759.69">22086 6825 8720 0 0,'0'0'398'0'0,"0"0"-3"0"0,4-4 272 0 0,0 2 2425 0 0,9-13-1132 0 0,7 6-314 0 0,-19 9-1141 0 0,9-11 879 0 0,27-21 835 0 0,9 16-867 0 0,-45 16-985 0 0,7-2 305 0 0,40 13-1282 0 0,-38-4 625 0 0,-8 28 186 0 0,-5 2 15 0 0,-1-9 170 0 0,-3 12-74 0 0,5-39-411 0 0,2-1-12 0 0,0 0 37 0 0,3 10 308 0 0,15 9-12 0 0,-17-18-372 0 0,7 17-262 0 0,-2 9-1153 0 0,-5-26 785 0 0,-1-1-831 0 0,0 0-363 0 0,0 0-70 0 0,0 0-17 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2740.813">21637 6653 2304 0 0,'2'0'473'0'0,"3"-1"1939"0"0,-5 7 6695 0 0,-1-1-5123 0 0,2 2-5610 0 0,-4 32 3901 0 0,5 2 62 0 0,5 57-84 0 0,6 4-1147 0 0,-3-11 156 0 0,-10 11-32 0 0,-10 12-700 0 0,12-100-583 0 0,-2-13-216 0 0,0-1-65 0 0,0-3-2 0 0,2-34-3313 0 0,-6 25 1834 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-2395.418">21658 6677 6912 0 0,'-11'-8'528'0'0,"28"-1"-128"0"0,7-10 4668 0 0,33 17 409 0 0,-53 2-5324 0 0,0 0-1 0 0,0 0 1 0 0,0 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,-2 0 1 0 0,2 2 0 0 0,0-2 0 0 0,0 0 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 0 0 0 0,1 2-153 0 0,33 70 2062 0 0,-23 7-1603 0 0,-14-3 1130 0 0,0-72-1534 0 0,-3 0 1 0 0,2 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,-2-1 1 0 0,1 0-1 0 0,-1 1 0 0 0,2-2 0 0 0,-1 1 1 0 0,-2 0-1 0 0,1 1 0 0 0,-1-2 0 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 0 0 0,-1 1-55 0 0,-25 6 67 0 0,30-11-206 0 0,-2 0-58 0 0,-2 0-1 0 0,3-1 1 0 0,-3 1 0 0 0,2-1-1 0 0,0 0 1 0 0,-2 0-1 0 0,2-1 1 0 0,0 1 0 0 0,0-2-1 0 0,-1 1 1 0 0,1 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,2-2-1 0 0,-1 1 1 0 0,0-1-1 0 0,-1-1 198 0 0,-5-5-5692 0 0,-5-1-1767 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="75099.81">3322 14611 7488 0 0,'0'2'340'0'0,"-6"99"3520"0"0,12 113 4791 0 0,-5 32-4784 0 0,6-63-3019 0 0,4-73-648 0 0,1-66-288 0 0,-12-42-387 0 0,0-2-33 0 0,0 0-192 0 0,0 0-790 0 0,0-5-352 0 0,2-20-70 0 0,-2-4-7 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="75669.811">3370 14709 8288 0 0,'-4'17'381'0'0,"3"-14"-6"0"0,9-35-227 0 0,-7 16 279 0 0,2 0 0 0 0,0 1-1 0 0,-1-1 1 0 0,2 1 0 0 0,1-1 0 0 0,0 2 0 0 0,1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,0 2 0 0 0,7-7-427 0 0,-10 13 230 0 0,1-2 0 0 0,0 2 1 0 0,1 0-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,-1 0-1 0 0,2 0 0 0 0,0 1 1 0 0,-1 0-1 0 0,2 1 0 0 0,1 0-230 0 0,54-2 1008 0 0,-57 5-919 0 0,0 1 0 0 0,-1 1 0 0 0,1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 2 0 0 0,-2 0 0 0 0,1 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1 0-1 0 0,-2 2 1 0 0,4 2-89 0 0,2 5 277 0 0,-2 0 1 0 0,-1 0-1 0 0,1-1 0 0 0,-1 2 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 8-277 0 0,10 86 608 0 0,-11-95-471 0 0,-1-2-1 0 0,1 2 1 0 0,-2 0-1 0 0,0-2 1 0 0,1 0-1 0 0,-3 1 1 0 0,1 0 0 0 0,-1 1-1 0 0,-2-4 1 0 0,1 3-1 0 0,0-1 1 0 0,-2 1-1 0 0,0-3 1 0 0,-1 2-1 0 0,0 1-136 0 0,-1-5 0 0 0,2-1 0 0 0,-2-1 0 0 0,-1 0 0 0 0,3 1 0 0 0,-3-2 0 0 0,1 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,-1 0 0 0 0,0-2 0 0 0,1-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,-4 0 0 0 0,-11 8 0 0 0,-27 0 0 0 0,42-13-8 0 0,0 0 1 0 0,0-1-1 0 0,0 0 0 0 0,1-1 0 0 0,-1-1 0 0 0,0 1 1 0 0,2-1-1 0 0,-2 1 0 0 0,2-1 0 0 0,-1-2 0 0 0,0 1 1 0 0,3-1-1 0 0,-4-1 8 0 0,-25-49-411 0 0,31 56 334 0 0,3 1 10 0 0,0 0 3 0 0,0 0 0 0 0,12 5-105 0 0,-7-1 109 0 0,2 0 0 0 0,-1-1 0 0 0,-2 2 0 0 0,3 1 0 0 0,-2-1 0 0 0,-1 1-1 0 0,1-1 1 0 0,0 1 0 0 0,0 1 0 0 0,-2-1 0 0 0,1 1 0 0 0,0 2 60 0 0,17 22-246 0 0,41 56 1336 0 0,-38-53-896 0 0,1-3 0 0 0,0 1 1 0 0,3-2-1 0 0,8 6-194 0 0,-16-15-3 0 0,73 46-2666 0 0,-77-58 1330 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="85949.811">4158 15263 920 0 0,'0'0'327'0'0,"0"0"1035"0"0,0 9 2340 0 0,-1-6-656 0 0,-1 23 2742 0 0,7-12-4840 0 0,-3-12-526 0 0,-2-2-26 0 0,0 0 12 0 0,0 0 68 0 0,0 0 32 0 0,1 1 4 0 0,45 6 1536 0 0,-7-3-1138 0 0,19-63-236 0 0,28-34 437 0 0,-47 21-618 0 0,-18 7-757 0 0,-21 63 329 0 0,1 0-31 0 0,-1 0 1 0 0,1-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0 1-1 0 0,0-2 1 0 0,0 1-1 0 0,-1 0 0 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,-1 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,0 1 1 0 0,0-1-1 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,-2 1 1 0 0,2-1-1 0 0,-1 0 1 0 0,1 1-1 0 0,-1-2 1 0 0,-1 2-1 0 0,2 0 0 0 0,0-1 1 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1-34 0 0,-6 0 41 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 1 0 0 0,3 0-1 0 0,-3 0 1 0 0,1 0 0 0 0,1 2-1 0 0,-1-1 1 0 0,1 0 0 0 0,0 1-1 0 0,-3 0-40 0 0,-21 14 98 0 0,22-14-115 0 0,-1-1 0 0 0,1 2 0 0 0,0 0 0 0 0,2 1-1 0 0,-2 0 1 0 0,0 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,0 1 0 0 0,2-3 0 0 0,-3 5 17 0 0,-17 42 618 0 0,15 24-194 0 0,26 33-1082 0 0,-14-101 704 0 0,1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,2 1 1 0 0,1 0 0 0 0,-2-1 0 0 0,1-2-1 0 0,0 2 1 0 0,1-1 0 0 0,0 0 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1-1-1 0 0,2-1 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 0-1 0 0,0-2 1 0 0,-1 1 0 0 0,2 0 0 0 0,-2 0-1 0 0,2-2 1 0 0,2 1-47 0 0,40-6-792 0 0,-50 5 622 0 0,2 0-1 0 0,-2 2 1 0 0,1-2-1 0 0,-1 0 1 0 0,1 0-1 0 0,1 0 1 0 0,-2 0-1 0 0,1 0 1 0 0,0-2-1 0 0,-1 2 1 0 0,2 0-1 0 0,-1-1 1 0 0,-1 0-1 0 0,0 1 1 0 0,2-1-1 0 0,-2 1 1 0 0,1-1-1 0 0,-1 0 1 0 0,0 0-1 0 0,2 0 1 0 0,-2 0-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-2 170 0 0,13-10-5654 0 0,-3 8-1513 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="87029.81">4991 14903 1376 0 0,'0'0'65'0'0,"0"0"287"0"0,0 0 1184 0 0,0 0 522 0 0,0 0 100 0 0,0 0-171 0 0,0-16 1609 0 0,17-85 4054 0 0,-9 72-6749 0 0,-8 26-797 0 0,0-4-41 0 0,0 6-160 0 0,0 1-19 0 0,0 0 92 0 0,0 0 344 0 0,0 0 154 0 0,0 0 34 0 0,0 0-97 0 0,0 0-403 0 0,0 0-59 0 0,0 0 127 0 0,0 0 15 0 0,0 0 21 0 0,0 0 128 0 0,0 1 59 0 0,-8 71 675 0 0,-14 52-478 0 0,10-30-496 0 0,1 80 642 0 0,10 80-1033 0 0,-2-173 1100 0 0,-5-20-1141 0 0,8-59 208 0 0,-6 0-1960 0 0,5-1 0 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="87299.81">4974 15018 12696 0 0,'11'-13'1376'0'0,"38"6"1778"0"0,13-3 1363 0 0,2 1-3125 0 0,3 22-1540 0 0,-44-6-2470 0 0,-17-1-4791 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="204899.81">6074 15361 8288 0 0,'13'-33'1072'0'0,"27"-2"4316"0"0,-36 34-5186 0 0,1 0 1 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1-1 0 0,-1 2 1 0 0,2-1 0 0 0,-2 2 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-3 0 0 0 0,2 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1-1 0 0,1-1 1 0 0,-2 2 0 0 0,1 2-203 0 0,3 3 280 0 0,-1 1 1 0 0,0 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,0 1 0 0 0,-1-2 1 0 0,0 8-281 0 0,-1-11 347 0 0,2-5-303 0 0,-1 0 0 0 0,0-2 0 0 0,-1 2 0 0 0,1-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1 1-44 0 0,1 0 8 0 0,-1-2 0 0 0,2 0-1 0 0,-2 0 1 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-2 1 0 0 0,2-1 0 0 0,0 0-1 0 0,-2 0 1 0 0,2-1 0 0 0,-1 1-1 0 0,-1 0 1 0 0,1 0 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,0 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,2-1-1 0 0,0 0 1 0 0,-2 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-2-2-8 0 0,-3-3-53 0 0,0 1 0 0 0,1-1 0 0 0,1-2 0 0 0,-2 1 0 0 0,2 0 0 0 0,-1 0 1 0 0,1-2-1 0 0,0 2 0 0 0,1-1 0 0 0,-1-1 0 0 0,1 1 0 0 0,1-1 0 0 0,0-1 0 0 0,-3-5 53 0 0,5 11-246 0 0,-1-3 1 0 0,2 1 0 0 0,-1 0 0 0 0,1-1-1 0 0,1 0 1 0 0,-1 1 0 0 0,1 1-1 0 0,-1-2 1 0 0,1 0 0 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,1 1-1 0 0,0-2 1 0 0,-1 2 0 0 0,1-2 245 0 0,11-26-3579 0 0,-5 17-2927 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="203719.8109">5482 15129 3224 0 0,'0'-2'240'0'0,"0"-1"25"0"0,0 2 855 0 0,0 1 359 0 0,0 0 66 0 0,0 0-81 0 0,0 0-397 0 0,0 0-178 0 0,0 0-32 0 0,0 0-13 0 0,0 0-24 0 0,0 0-10 0 0,0 0-2 0 0,0 0-18 0 0,0 0-74 0 0,5 30 1869 0 0,-12 148 1427 0 0,-6 4-2668 0 0,8-90-1106 0 0,5-91-198 0 0,0 19-364 0 0,0-20 191 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,0 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-1 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 134 0 0,3-14-2091 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="204089.8109">5498 15266 8288 0 0,'3'9'2948'0'0,"4"-25"1960"0"0,-2 6-5020 0 0,30-38 3418 0 0,17-6-299 0 0,-49 52-2908 0 0,0 1 0 0 0,0-2 0 0 0,1 2 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,1 0 1 0 0,1 1-1 0 0,-1-1 0 0 0,0 1 0 0 0,2 0 0 0 0,-3 0 0 0 0,2 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 0 0 0,0 0 0 0 0,1 2 0 0 0,-1-2 0 0 0,1 1 0 0 0,-1 0-99 0 0,22 31 274 0 0,19 33 16 0 0,-2-8-146 0 0,-12-20 0 0 0,-25-26-597 0 0,-3-10-3304 0 0,-2-2 2223 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35574.03">18789 6660 11888 0 0,'0'0'266'0'0,"0"0"44"0"0,0 0 14 0 0,1 10 69 0 0,-2 75 4760 0 0,-6-15-2346 0 0,7-31-2146 0 0,-1-35-594 0 0,-3 29-145 0 0,2-22-10 0 0,1-9-188 0 0,1-2-789 0 0,0 0-344 0 0,0 0-65 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-35139.5208">19054 6663 2304 0 0,'-3'1'3435'0'0,"8"5"13324"0"0,-3-4-18570 0 0,12 97 5563 0 0,0 27-2624 0 0,-5-51-1128 0 0,-7-66-133 0 0,-1-8-563 0 0,-1-1-257 0 0,0 0-922 0 0,0 0-3642 0 0,0 0-1564 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-34747.75">19072 6791 1840 0 0,'0'0'83'0'0,"0"0"373"0"0,0 0 1526 0 0,0 0 670 0 0,0 0 131 0 0,3-1 950 0 0,8-6-2192 0 0,8-24 2196 0 0,-3 12-2845 0 0,-14 14-638 0 0,2 1-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,0-1-1 0 0,1 1 1 0 0,0 0-1 0 0,1 1 1 0 0,-1 0-1 0 0,0 0 1 0 0,0 1-1 0 0,2-1 1 0 0,-1 0-1 0 0,-1 1 1 0 0,6-2-254 0 0,20 16 16 0 0,-24-8-15 0 0,45 51 773 0 0,-46-47-785 0 0,-4-7-105 0 0,13 4-2683 0 0,-14-5 751 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44644.387">18129 6475 3224 0 0,'-1'0'2310'0'0,"0"1"10093"0"0,0 0-11285 0 0,1 2-3278 0 0,-15 170 7048 0 0,-9 34-3120 0 0,19-148-1645 0 0,7 49-583 0 0,1-101 325 0 0,-3-7-3458 0 0,0 0 1850 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-44417.2638">18062 6551 13824 0 0,'0'0'314'0'0,"0"0"46"0"0,0 0 22 0 0,0 0-50 0 0,2 0-220 0 0,56 3 3130 0 0,53 24-834 0 0,-55-20-4427 0 0,-54-7-69 0 0,5 0-4147 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-36024.581">18390 6897 2304 0 0,'0'0'348'0'0,"0"0"620"0"0,-8-5 2737 0 0,3-54-382 0 0,5 58-2754 0 0,-8-17 2487 0 0,3-42 2906 0 0,6 54-5754 0 0,-1 1-1 0 0,3 1 0 0 0,-2-2 1 0 0,1 1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 1 1 0 0,0-2-1 0 0,-1 1 1 0 0,1 1-1 0 0,0-1 1 0 0,1 1-1 0 0,-1 1 1 0 0,1-1-1 0 0,1-2-207 0 0,-3 4-36 0 0,2-1 14 0 0,-1 0-1 0 0,0 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1 0 0 0,-1 1 1 0 0,0-1-1 0 0,1-1 0 0 0,0 2 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 1 0 0,0 0-1 0 0,3 0 23 0 0,-4 0 21 0 0,1 0 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 2 0 0 0,2-1 1 0 0,-1 0-1 0 0,-1 1 0 0 0,1 0 1 0 0,-1 0-1 0 0,2 0 0 0 0,-2 0 1 0 0,2 1-1 0 0,-3 0 0 0 0,1-1 1 0 0,2 2-1 0 0,-2 0 0 0 0,1-2 1 0 0,-1 1-1 0 0,-1 1 0 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 0 0 0,2 0-21 0 0,0 5 5 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 2 1 0 0,0-1-1 0 0,0 0 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-2 5-5 0 0,2-4 151 0 0,-1 0 1 0 0,-1 1-1 0 0,0 0 1 0 0,-1-1-1 0 0,0 0 1 0 0,2 1-1 0 0,-3-1 1 0 0,0 1-1 0 0,0-3 1 0 0,-1 2-1 0 0,0 0 1 0 0,1-1-1 0 0,-4 3-151 0 0,6-7 28 0 0,-1-1-1 0 0,0 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 0-1 0 0,0-1 1 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 2 1 0 0,-1-2-1 0 0,0-1 0 0 0,0 1 1 0 0,1-1-1 0 0,-2 0 1 0 0,2 1-1 0 0,-1-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,1 0-1 0 0,-2-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,0 0 1 0 0,0 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,0-1 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 0 1 0 0,-1 0-1 0 0,1-1-27 0 0,-4-2-27 0 0,1-3-1 0 0,1 2 0 0 0,-2-1 1 0 0,2 0-1 0 0,0-1 0 0 0,-1-1 1 0 0,1 1-1 0 0,1 0 1 0 0,0-2-1 0 0,0 3 0 0 0,1-1 1 0 0,-1-1-1 0 0,1-1 1 0 0,1 0 27 0 0,-5-55-3584 0 0,10 58 2142 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33796.383">19417 6891 456 0 0,'0'0'2349'0'0,"0"0"293"0"0,0 0 128 0 0,0 0-221 0 0,0 0-1013 0 0,0 0-448 0 0,0 0-89 0 0,0 0-30 0 0,5 7 1768 0 0,-2-4-2425 0 0,1-1 0 0 0,-1-1 0 0 0,0 2 0 0 0,0-1 0 0 0,1-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,2 0 0 0 0,-3 0 0 0 0,3 0 0 0 0,-1-1 0 0 0,-1 1 0 0 0,2-1 0 0 0,0 0-312 0 0,56-6 2120 0 0,4-21-1296 0 0,-5-17-672 0 0,-23 0 656 0 0,-15-26-516 0 0,-36 14-160 0 0,13 53-153 0 0,0 1-1 0 0,0 0 1 0 0,0-1 0 0 0,-1 2-1 0 0,1-1 1 0 0,0 0-1 0 0,0-1 1 0 0,-1 1 0 0 0,1 0-1 0 0,-2 0 1 0 0,2 0-1 0 0,0 0 1 0 0,-1 1 0 0 0,-1-1-1 0 0,2 1 1 0 0,-1-1-1 0 0,0 1 1 0 0,0 1 0 0 0,-1-1-1 0 0,1 0 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 1 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,0-1 1 0 0,1 1 0 0 0,0 0-1 0 0,0 0 1 0 0,0 1-1 0 0,-1-1 1 0 0,0 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,1-1-1 0 0,-4 2 22 0 0,-3 4 44 0 0,2 2 0 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 1 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,2 2 0 0 0,-5 8-44 0 0,1-3 32 0 0,0 4-32 0 0,1 1 0 0 0,0-3 0 0 0,2 2 0 0 0,-1 1 0 0 0,4-1 0 0 0,-3 8 0 0 0,4-20 8 0 0,1-1 0 0 0,0 1 0 0 0,0-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0-1 0 0 0,0 0-1 0 0,2 0 1 0 0,-2-1 0 0 0,1 1 0 0 0,0-1 0 0 0,4 8-8 0 0,10 4 88 0 0,42-11-2149 0 0,-21-14-6089 0 0,-22 2 1076 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-33464.079">19893 6888 13824 0 0,'0'0'314'0'0,"-7"7"872"0"0,1 11-891 0 0,5-12 1764 0 0,-1-4 3765 0 0,8-3-5807 0 0,8-6-1723 0 0,-6 1-236 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-28557.543">18833 6421 4144 0 0,'0'0'319'0'0,"0"0"295"0"0,0 0 2022 0 0,0 0 904 0 0,0 0 185 0 0,0 0-408 0 0,0 0-1846 0 0,0 0-815 0 0,0 0-161 0 0,0 0-25 0 0,0 0 16 0 0,0 0 8 0 0,0 0 2 0 0,0 0-64 0 0,0 0-1313 0 0,0 0-4508 0 0,0 0-1916 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-19052.7189">20155 6627 10136 0 0,'0'0'464'0'0,"0"0"-10"0"0,-3 6 160 0 0,3-4 8708 0 0,20 88-4943 0 0,-16 5-3675 0 0,-13-10-98 0 0,9-77-623 0 0,0-7-63 0 0,0-1-165 0 0,0 0-726 0 0,0 0-316 0 0,0 0-65 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-9426.743">20428 6509 920 0 0,'1'-1'67'0'0,"0"-4"143"0"0,0 5 814 0 0,-1 0 355 0 0,0 0 70 0 0,0 0 5373 0 0,0 4-3378 0 0,0 18-2234 0 0,12 166 4151 0 0,-9-33-3309 0 0,0-105-1683 0 0,0-31-1984 0 0,-1-2-3835 0 0,-2-17 3608 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-8994.302">20428 6677 3224 0 0,'0'7'527'0'0,"10"-32"8375"0"0,7-1-6343 0 0,-15 23-2627 0 0,0-2 178 0 0,1 0 0 0 0,0 1 0 0 0,-2 0 0 0 0,3 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 1 0 0,2 0-1 0 0,-1 1 0 0 0,0 0 0 0 0,-1 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,1-1 0 0 0,-3 1 0 0 0,2-1 0 0 0,-1 1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,1 0-110 0 0,19 32 453 0 0,1 11 891 0 0,-18-26-1051 0 0,0 58 781 0 0,9 8 131 0 0,-6-38-1044 0 0,9-14-3885 0 0,-18-30 1631 0 0,-1-2-17 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7909.834">21028 6612 2760 0 0,'0'0'395'0'0,"0"0"617"0"0,0 0 274 0 0,0 0 53 0 0,0 0-86 0 0,0 0-380 0 0,0 0-163 0 0,0 0-36 0 0,0 0-28 0 0,0 0-85 0 0,6 0 260 0 0,-5-1 2703 0 0,-1 0-3426 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1-1 0 0,1 0 1 0 0,-2 0 0 0 0,1-1 0 0 0,1 1 0 0 0,-1 0-1 0 0,0 0 1 0 0,0-1 0 0 0,0 1 0 0 0,0 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,-1 1 0 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 0 0 0 0,0 1 0 0 0,-1 0-1 0 0,1-1 1 0 0,0 1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0-1-1 0 0,0 1 1 0 0,-1 0 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1-1 0 0,1 0 1 0 0,-1 0 0 0 0,-2 1 0 0 0,2-1 0 0 0,0 1-1 0 0,0-1 1 0 0,-1 1-98 0 0,-10 0 483 0 0,-30 7 677 0 0,-1 20-16 0 0,40-25-1069 0 0,-2 1-1 0 0,2-2 0 0 0,1 2 0 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 1 1 0 0,1-2-1 0 0,0 1 0 0 0,0 1 0 0 0,1-1 1 0 0,-1 1-1 0 0,1 1 0 0 0,0-2 1 0 0,0 0-1 0 0,0 1 0 0 0,1 0 0 0 0,0 0 1 0 0,-1 1-1 0 0,2-1 0 0 0,-1 0 1 0 0,0 0-1 0 0,1-1 0 0 0,0 0 0 0 0,0 1 1 0 0,0 0-1 0 0,-1-1 0 0 0,4 4-74 0 0,27 86 784 0 0,-18-66-634 0 0,-11-22-112 0 0,2-1 0 0 0,-2 0 1 0 0,1 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 0 0 0,0 0 1 0 0,0-1-1 0 0,0 1 0 0 0,1 0 0 0 0,1-1-38 0 0,-3-1-114 0 0,-1 0 0 0 0,2-1 0 0 0,-1 0-1 0 0,2 0 1 0 0,-2 0 0 0 0,1 1 0 0 0,0-2-1 0 0,-1 1 1 0 0,2-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0-1 0 0,1-1 1 0 0,-1 0 0 0 0,1 0 0 0 0,-3 0-1 0 0,3 0 1 0 0,-1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,2-1 114 0 0,5-1-2547 0 0,0-4-5195 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-7043.897">21275 6949 7112 0 0,'15'0'324'0'0,"-11"0"-4"0"0,-4 0-94 0 0,0 0 380 0 0,0 0 186 0 0,0 0 37 0 0,0 0 35 0 0,0 0 107 0 0,0 0 42 0 0,0 0 10 0 0,0 0-26 0 0,0 0-112 0 0,0 0-49 0 0,0 0-11 0 0,0 0-58 0 0,0 0-240 0 0,0 0-102 0 0,0 0-17 0 0,0 0-25 0 0,0 0-82 0 0,0 0-40 0 0,0 0-5 0 0,0 0-26 0 0,0 0-108 0 0,0 0-42 0 0,1-19-240 0 0,15 1 132 0 0,-16 17-8 0 0,0 1 88 0 0,0 0 35 0 0,0 0-18 0 0,-1 1-1 0 0,-1 0-1 0 0,2-1 0 0 0,-1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 0 0 0,1 0 0 0 0,0 0 1 0 0,-2 0-1 0 0,2 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 0 0 0,0 0 1 0 0,0 1-1 0 0,0-1 0 0 0,0 0 1 0 0,0 1-1 0 0,2-1 0 0 0,-2 0 0 0 0,0 0 1 0 0,1 0-1 0 0,-1 0-67 0 0,1 1-279 0 0,-1-2-186 0 0,0 0-42 0 0,0 0-209 0 0,0 0-857 0 0,0 0-379 0 0,0 0-80 0 0,0 0-14 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2101.423">20162 6276 13304 0 0,'0'0'605'0'0,"0"0"-9"0"0,0-1-381 0 0,-2-3-42 0 0,1 2 600 0 0,1 2 260 0 0,0 0 45 0 0,0 0-26 0 0,0 0-144 0 0,0 0-63 0 0,-4 21 1994 0 0,14-14-5523 0 0,-8-7-4821 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122096.968">3851 803 6448 0 0,'0'0'297'0'0,"0"0"-9"0"0,0 0-120 0 0,0 0 193 0 0,-4-8 582 0 0,-46-23 3117 0 0,23 18-1623 0 0,-47-16-841 0 0,62 26-1311 0 0,3 1-1 0 0,-2 1 0 0 0,-1-2 1 0 0,1 3-1 0 0,1 0 0 0 0,-1 0 1 0 0,0 2-1 0 0,0 0 0 0 0,1 0 1 0 0,-1 0-1 0 0,1 1 0 0 0,0-1 1 0 0,-1 2-1 0 0,2 1 0 0 0,-11 5-284 0 0,16-8 41 0 0,0 0 0 0 0,1 0-1 0 0,0 1 1 0 0,-1-1-1 0 0,2 1 1 0 0,-1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,1 2-1 0 0,-2-2 1 0 0,2 0-1 0 0,1 0 1 0 0,-2 1 0 0 0,1 0-1 0 0,0 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-2 0 0 0 0,2 1-1 0 0,0-1 1 0 0,1-1-1 0 0,-1 2 1 0 0,1 0 0 0 0,-1-1-1 0 0,1 0 1 0 0,1 0-1 0 0,-1 2-40 0 0,6 9 100 0 0,0-1 0 0 0,1 0 0 0 0,1-2 0 0 0,0 2 0 0 0,0-2 0 0 0,2 1 0 0 0,-2-2 0 0 0,4 0 0 0 0,-3 0 0 0 0,3-1 0 0 0,-2-1 0 0 0,2 1 0 0 0,0-1-100 0 0,-7-6 32 0 0,68 83-590 0 0,-61-69 602 0 0,0 1 1 0 0,-3-1-1 0 0,2 2 1 0 0,-3-1 0 0 0,1 0-1 0 0,-2 3 1 0 0,-1 0-1 0 0,0-2 1 0 0,0 1-1 0 0,-3 2 1 0 0,0-3 0 0 0,0 3-1 0 0,-2-2 1 0 0,0 2-1 0 0,-1 0 1 0 0,-3 19-45 0 0,0-26 91 0 0,1-2 1 0 0,0 2-1 0 0,-2-2 1 0 0,0 0-1 0 0,-2 0 1 0 0,1 0-1 0 0,0 1 1 0 0,-2-1-1 0 0,0-1 1 0 0,0-1-1 0 0,-3 4-91 0 0,7-10 67 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 0 0 0 0,-2 0 0 0 0,2-1 1 0 0,-1 1-1 0 0,-1-1 0 0 0,1-1 0 0 0,-1 2 0 0 0,2-2 0 0 0,-3 0 0 0 0,1 0 0 0 0,0-1 0 0 0,1-1 0 0 0,-2 1 0 0 0,1 0 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1 0 0 0 0,2-1 0 0 0,-1 1 1 0 0,-6-2-68 0 0,7 0 4 0 0,-2 0 0 0 0,0 0 0 0 0,3-2 0 0 0,-3 1 0 0 0,1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,1-1 0 0 0,-2 0 0 0 0,2 0 1 0 0,-1 0-1 0 0,0-5-4 0 0,-2 0-603 0 0,0 1 1 0 0,2 0-1 0 0,0-3 0 0 0,-1 1 1 0 0,2-1-1 0 0,0 1 1 0 0,1 1-1 0 0,-1-4 603 0 0,-4-12-1535 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="122485.17">3743 532 13680 0 0,'0'0'306'0'0,"-5"7"421"0"0,-1 7-534 0 0,-2-1-1 0 0,2 2 1 0 0,2-2-1 0 0,-2 2 1 0 0,2-1 0 0 0,0 1-1 0 0,1 0 1 0 0,-1 12-193 0 0,0-4 459 0 0,-10 64 963 0 0,3 2 0 0 0,5 0 0 0 0,3-2 0 0 0,5 59-1422 0 0,-11 66 1773 0 0,-6-13-700 0 0,0 109-1515 0 0,17-246-1557 0 0,-1-34 952 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="142634.009">4193 1572 9